<commit_message>
more fine tunning of dvp and pp associations
</commit_message>
<xml_diff>
--- a/Structural.xlsx
+++ b/Structural.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA3FFFE-7AE2-4722-A706-8CE32F50373D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A7F894-0262-4828-97F6-09DE7A4F6104}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
@@ -126,12 +126,12 @@
     <definedName name="ia_dams_dsegroup_b1">Stock!$L$153:$V$153</definedName>
     <definedName name="ia_g1_tg1">Stock!$K$123:$N$125</definedName>
     <definedName name="ia_k2_mlsb1">Stock!$L$168:$V$207</definedName>
-    <definedName name="ia_offs_dsegroup_b1">Stock!$L$155</definedName>
+    <definedName name="ia_offs_dsegroup">Stock!$L$155</definedName>
     <definedName name="ia_ppk2g1_rlsb1">Stock!$L$214:$V$273</definedName>
     <definedName name="ia_ppk5_lsb0">Stock!$L$280:$Q$299</definedName>
     <definedName name="ia_prepost_b1">Stock!$L$159:$V$159</definedName>
     <definedName name="ia_r1type_fi">Stock!#REF!</definedName>
-    <definedName name="ia_sire_dsegroup_b1">Stock!$L$152</definedName>
+    <definedName name="ia_sire_dsegroup">Stock!$L$152</definedName>
     <definedName name="ia_yatf_dsegroup_b1">Stock!$L$154:$V$154</definedName>
     <definedName name="labour_period_len" localSheetId="0">General!$I$65</definedName>
     <definedName name="pastures" localSheetId="0">General!$I$55:$K$55</definedName>
@@ -578,6 +578,30 @@
           <t xml:space="preserve">
 If early lambing then use # of foetuses
 If late lambing use number of lambs</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I154" authorId="0" shapeId="0" xr:uid="{4480F7C9-AFC2-4EF1-9DB3-141549F180B2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Michael Young (21512438):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+not counted in dse stuff. They are accounted for by dam. If this changes will need to add them to code.</t>
         </r>
       </text>
     </comment>
@@ -3645,6 +3669,12 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="47" xfId="3" applyBorder="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="25" xfId="3" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="25" xfId="3" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="38" xfId="12" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3661,6 +3691,24 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="22" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="8" borderId="43" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="8" borderId="44" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="8" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="8" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="8" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="8" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="43" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3689,36 +3737,12 @@
     <xf numFmtId="0" fontId="13" fillId="8" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="8" borderId="43" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="8" borderId="44" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="8" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="8" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="8" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="8" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="12" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="23" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="25" xfId="3" applyFont="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="25" xfId="3" applyFont="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -4903,19 +4927,19 @@
       <c r="I18" s="31">
         <v>2</v>
       </c>
-      <c r="J18" s="171" t="s">
+      <c r="J18" s="173" t="s">
         <v>70</v>
       </c>
-      <c r="K18" s="172"/>
-      <c r="L18" s="172"/>
-      <c r="M18" s="172"/>
-      <c r="N18" s="172"/>
-      <c r="O18" s="172"/>
-      <c r="P18" s="172"/>
-      <c r="Q18" s="172"/>
-      <c r="R18" s="172"/>
-      <c r="S18" s="172"/>
-      <c r="T18" s="173"/>
+      <c r="K18" s="174"/>
+      <c r="L18" s="174"/>
+      <c r="M18" s="174"/>
+      <c r="N18" s="174"/>
+      <c r="O18" s="174"/>
+      <c r="P18" s="174"/>
+      <c r="Q18" s="174"/>
+      <c r="R18" s="174"/>
+      <c r="S18" s="174"/>
+      <c r="T18" s="175"/>
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
       <c r="W18" s="2"/>
@@ -5008,19 +5032,19 @@
       <c r="I21" s="23">
         <v>1</v>
       </c>
-      <c r="J21" s="174" t="s">
+      <c r="J21" s="176" t="s">
         <v>35</v>
       </c>
-      <c r="K21" s="175"/>
-      <c r="L21" s="175"/>
-      <c r="M21" s="175"/>
-      <c r="N21" s="175"/>
-      <c r="O21" s="175"/>
-      <c r="P21" s="175"/>
-      <c r="Q21" s="175"/>
-      <c r="R21" s="175"/>
-      <c r="S21" s="175"/>
-      <c r="T21" s="175"/>
+      <c r="K21" s="177"/>
+      <c r="L21" s="177"/>
+      <c r="M21" s="177"/>
+      <c r="N21" s="177"/>
+      <c r="O21" s="177"/>
+      <c r="P21" s="177"/>
+      <c r="Q21" s="177"/>
+      <c r="R21" s="177"/>
+      <c r="S21" s="177"/>
+      <c r="T21" s="177"/>
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
       <c r="W21" s="2"/>
@@ -7214,8 +7238,8 @@
   </sheetPr>
   <dimension ref="A1:AE384"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A332" workbookViewId="0">
-      <selection activeCell="N349" sqref="N349"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="K161" sqref="K161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.35"/>
@@ -7872,19 +7896,19 @@
       <c r="I18" s="31">
         <v>2</v>
       </c>
-      <c r="J18" s="171" t="s">
+      <c r="J18" s="173" t="s">
         <v>70</v>
       </c>
-      <c r="K18" s="172"/>
-      <c r="L18" s="172"/>
-      <c r="M18" s="172"/>
-      <c r="N18" s="172"/>
-      <c r="O18" s="172"/>
-      <c r="P18" s="172"/>
-      <c r="Q18" s="172"/>
-      <c r="R18" s="172"/>
-      <c r="S18" s="172"/>
-      <c r="T18" s="173"/>
+      <c r="K18" s="174"/>
+      <c r="L18" s="174"/>
+      <c r="M18" s="174"/>
+      <c r="N18" s="174"/>
+      <c r="O18" s="174"/>
+      <c r="P18" s="174"/>
+      <c r="Q18" s="174"/>
+      <c r="R18" s="174"/>
+      <c r="S18" s="174"/>
+      <c r="T18" s="175"/>
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
       <c r="W18" s="2"/>
@@ -7977,19 +8001,19 @@
       <c r="I21" s="23">
         <v>1</v>
       </c>
-      <c r="J21" s="174" t="s">
+      <c r="J21" s="176" t="s">
         <v>35</v>
       </c>
-      <c r="K21" s="175"/>
-      <c r="L21" s="175"/>
-      <c r="M21" s="175"/>
-      <c r="N21" s="175"/>
-      <c r="O21" s="175"/>
-      <c r="P21" s="175"/>
-      <c r="Q21" s="175"/>
-      <c r="R21" s="175"/>
-      <c r="S21" s="175"/>
-      <c r="T21" s="175"/>
+      <c r="K21" s="177"/>
+      <c r="L21" s="177"/>
+      <c r="M21" s="177"/>
+      <c r="N21" s="177"/>
+      <c r="O21" s="177"/>
+      <c r="P21" s="177"/>
+      <c r="Q21" s="177"/>
+      <c r="R21" s="177"/>
+      <c r="S21" s="177"/>
+      <c r="T21" s="177"/>
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
       <c r="W21" s="2"/>
@@ -9377,7 +9401,7 @@
         <v>169</v>
       </c>
       <c r="I61" s="31">
-        <v>-19</v>
+        <v>-18</v>
       </c>
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
@@ -9411,7 +9435,7 @@
         <v>170</v>
       </c>
       <c r="I62" s="31">
-        <v>-18</v>
+        <v>-17</v>
       </c>
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
@@ -22337,14 +22361,14 @@
         <v>4</v>
       </c>
       <c r="Q323" s="126"/>
-      <c r="R323" s="185" t="s">
+      <c r="R323" s="178" t="s">
         <v>167</v>
       </c>
-      <c r="S323" s="186"/>
-      <c r="T323" s="186"/>
-      <c r="U323" s="186"/>
-      <c r="V323" s="186"/>
-      <c r="W323" s="187"/>
+      <c r="S323" s="179"/>
+      <c r="T323" s="179"/>
+      <c r="U323" s="179"/>
+      <c r="V323" s="179"/>
+      <c r="W323" s="180"/>
       <c r="X323" s="4"/>
       <c r="Y323" s="16"/>
       <c r="Z323" s="1"/>
@@ -22382,12 +22406,12 @@
         <v>1</v>
       </c>
       <c r="Q324" s="2"/>
-      <c r="R324" s="188"/>
-      <c r="S324" s="189"/>
-      <c r="T324" s="189"/>
-      <c r="U324" s="189"/>
-      <c r="V324" s="189"/>
-      <c r="W324" s="190"/>
+      <c r="R324" s="181"/>
+      <c r="S324" s="182"/>
+      <c r="T324" s="182"/>
+      <c r="U324" s="182"/>
+      <c r="V324" s="182"/>
+      <c r="W324" s="183"/>
       <c r="X324" s="4"/>
       <c r="Y324" s="16"/>
       <c r="Z324" s="1"/>
@@ -22425,12 +22449,12 @@
         <v>1</v>
       </c>
       <c r="Q325" s="2"/>
-      <c r="R325" s="188"/>
-      <c r="S325" s="189"/>
-      <c r="T325" s="189"/>
-      <c r="U325" s="189"/>
-      <c r="V325" s="189"/>
-      <c r="W325" s="190"/>
+      <c r="R325" s="181"/>
+      <c r="S325" s="182"/>
+      <c r="T325" s="182"/>
+      <c r="U325" s="182"/>
+      <c r="V325" s="182"/>
+      <c r="W325" s="183"/>
       <c r="X325" s="4"/>
       <c r="Y325" s="16"/>
       <c r="Z325" s="1"/>
@@ -23368,14 +23392,14 @@
       <c r="F347" s="5"/>
       <c r="G347" s="4"/>
       <c r="H347" s="2"/>
-      <c r="I347" s="193"/>
-      <c r="J347" s="194" t="s">
+      <c r="I347" s="171"/>
+      <c r="J347" s="172" t="s">
         <v>295</v>
       </c>
-      <c r="K347" s="194" t="s">
+      <c r="K347" s="172" t="s">
         <v>296</v>
       </c>
-      <c r="L347" s="194" t="s">
+      <c r="L347" s="172" t="s">
         <v>297</v>
       </c>
       <c r="M347" s="2"/>
@@ -23406,7 +23430,7 @@
       <c r="H348" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="I348" s="193"/>
+      <c r="I348" s="171"/>
       <c r="J348" s="31">
         <v>1</v>
       </c>
@@ -23442,10 +23466,10 @@
       <c r="F349" s="5"/>
       <c r="G349" s="4"/>
       <c r="H349" s="2"/>
-      <c r="I349" s="193"/>
-      <c r="J349" s="194"/>
-      <c r="K349" s="194"/>
-      <c r="L349" s="194"/>
+      <c r="I349" s="171"/>
+      <c r="J349" s="172"/>
+      <c r="K349" s="172"/>
+      <c r="L349" s="172"/>
       <c r="M349" s="2"/>
       <c r="N349" s="2"/>
       <c r="O349" s="2"/>
@@ -23909,13 +23933,13 @@
       <c r="N360" s="2"/>
       <c r="O360" s="2"/>
       <c r="P360" s="2"/>
-      <c r="Q360" s="176"/>
-      <c r="R360" s="177"/>
-      <c r="S360" s="177"/>
-      <c r="T360" s="177"/>
-      <c r="U360" s="177"/>
-      <c r="V360" s="177"/>
-      <c r="W360" s="178"/>
+      <c r="Q360" s="184"/>
+      <c r="R360" s="185"/>
+      <c r="S360" s="185"/>
+      <c r="T360" s="185"/>
+      <c r="U360" s="185"/>
+      <c r="V360" s="185"/>
+      <c r="W360" s="186"/>
       <c r="X360" s="4"/>
       <c r="Y360" s="16"/>
       <c r="Z360" s="1"/>
@@ -23956,13 +23980,13 @@
       <c r="N361" s="2"/>
       <c r="O361" s="2"/>
       <c r="P361" s="2"/>
-      <c r="Q361" s="179"/>
-      <c r="R361" s="180"/>
-      <c r="S361" s="180"/>
-      <c r="T361" s="180"/>
-      <c r="U361" s="180"/>
-      <c r="V361" s="180"/>
-      <c r="W361" s="181"/>
+      <c r="Q361" s="187"/>
+      <c r="R361" s="188"/>
+      <c r="S361" s="188"/>
+      <c r="T361" s="188"/>
+      <c r="U361" s="188"/>
+      <c r="V361" s="188"/>
+      <c r="W361" s="189"/>
       <c r="X361" s="4"/>
       <c r="Y361" s="16"/>
       <c r="Z361" s="1"/>
@@ -24001,13 +24025,13 @@
       <c r="N362" s="2"/>
       <c r="O362" s="2"/>
       <c r="P362" s="2"/>
-      <c r="Q362" s="179"/>
-      <c r="R362" s="180"/>
-      <c r="S362" s="180"/>
-      <c r="T362" s="180"/>
-      <c r="U362" s="180"/>
-      <c r="V362" s="180"/>
-      <c r="W362" s="181"/>
+      <c r="Q362" s="187"/>
+      <c r="R362" s="188"/>
+      <c r="S362" s="188"/>
+      <c r="T362" s="188"/>
+      <c r="U362" s="188"/>
+      <c r="V362" s="188"/>
+      <c r="W362" s="189"/>
       <c r="X362" s="4"/>
       <c r="Y362" s="16"/>
       <c r="Z362" s="1"/>
@@ -24036,13 +24060,13 @@
       <c r="N363" s="2"/>
       <c r="O363" s="2"/>
       <c r="P363" s="2"/>
-      <c r="Q363" s="182"/>
-      <c r="R363" s="183"/>
-      <c r="S363" s="183"/>
-      <c r="T363" s="183"/>
-      <c r="U363" s="183"/>
-      <c r="V363" s="183"/>
-      <c r="W363" s="184"/>
+      <c r="Q363" s="190"/>
+      <c r="R363" s="191"/>
+      <c r="S363" s="191"/>
+      <c r="T363" s="191"/>
+      <c r="U363" s="191"/>
+      <c r="V363" s="191"/>
+      <c r="W363" s="192"/>
       <c r="X363" s="4"/>
       <c r="Y363" s="16"/>
       <c r="Z363" s="1"/>
@@ -25623,23 +25647,23 @@
       <c r="I18" s="31">
         <v>1</v>
       </c>
-      <c r="J18" s="191" t="s">
+      <c r="J18" s="193" t="s">
         <v>22</v>
       </c>
-      <c r="K18" s="191"/>
-      <c r="L18" s="191"/>
-      <c r="M18" s="191"/>
-      <c r="N18" s="191"/>
-      <c r="O18" s="191"/>
-      <c r="P18" s="191"/>
-      <c r="Q18" s="191"/>
-      <c r="R18" s="191"/>
-      <c r="S18" s="191"/>
-      <c r="T18" s="191"/>
-      <c r="U18" s="191"/>
-      <c r="V18" s="191"/>
-      <c r="W18" s="191"/>
-      <c r="X18" s="191"/>
+      <c r="K18" s="193"/>
+      <c r="L18" s="193"/>
+      <c r="M18" s="193"/>
+      <c r="N18" s="193"/>
+      <c r="O18" s="193"/>
+      <c r="P18" s="193"/>
+      <c r="Q18" s="193"/>
+      <c r="R18" s="193"/>
+      <c r="S18" s="193"/>
+      <c r="T18" s="193"/>
+      <c r="U18" s="193"/>
+      <c r="V18" s="193"/>
+      <c r="W18" s="193"/>
+      <c r="X18" s="193"/>
       <c r="Y18" s="2"/>
       <c r="Z18" s="4"/>
       <c r="AA18" s="16"/>
@@ -25734,23 +25758,23 @@
       <c r="I21" s="23">
         <v>1</v>
       </c>
-      <c r="J21" s="174" t="s">
+      <c r="J21" s="176" t="s">
         <v>34</v>
       </c>
-      <c r="K21" s="175"/>
-      <c r="L21" s="175"/>
-      <c r="M21" s="175"/>
-      <c r="N21" s="175"/>
-      <c r="O21" s="175"/>
-      <c r="P21" s="175"/>
-      <c r="Q21" s="175"/>
-      <c r="R21" s="175"/>
-      <c r="S21" s="175"/>
-      <c r="T21" s="175"/>
-      <c r="U21" s="175"/>
-      <c r="V21" s="175"/>
-      <c r="W21" s="175"/>
-      <c r="X21" s="192"/>
+      <c r="K21" s="177"/>
+      <c r="L21" s="177"/>
+      <c r="M21" s="177"/>
+      <c r="N21" s="177"/>
+      <c r="O21" s="177"/>
+      <c r="P21" s="177"/>
+      <c r="Q21" s="177"/>
+      <c r="R21" s="177"/>
+      <c r="S21" s="177"/>
+      <c r="T21" s="177"/>
+      <c r="U21" s="177"/>
+      <c r="V21" s="177"/>
+      <c r="W21" s="177"/>
+      <c r="X21" s="194"/>
       <c r="Y21" s="2"/>
       <c r="Z21" s="4"/>
       <c r="AA21" s="16"/>

</xml_diff>

<commit_message>
fix error in n_fvp_prior calc. testing with only 3 dvps and comparing againts old verison (pre season stuff)
</commit_message>
<xml_diff>
--- a/Structural.xlsx
+++ b/Structural.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A7F894-0262-4828-97F6-09DE7A4F6104}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E468F5-4896-44AE-9DB3-758555493430}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -30,18 +30,18 @@
     <definedName name="grazing_int" localSheetId="0">General!$I$58:$L$58</definedName>
     <definedName name="i_a0_pos">Stock!$I$52</definedName>
     <definedName name="i_a1_pos">Stock!$I$53</definedName>
-    <definedName name="i_adjp_cfw_initial_w0">Stock!$K$369</definedName>
-    <definedName name="i_adjp_cfw_initial_w1">Stock!$P$369:$P$371</definedName>
-    <definedName name="i_adjp_cfw_initial_w3">Stock!$V$369:$V$371</definedName>
-    <definedName name="i_adjp_fd_initial_w0">Stock!$L$369</definedName>
-    <definedName name="i_adjp_fd_initial_w1">Stock!$Q$369:$Q$371</definedName>
-    <definedName name="i_adjp_fd_initial_w3">Stock!$U$369:$U$371</definedName>
-    <definedName name="i_adjp_fl_initial_w0">Stock!$M$369</definedName>
-    <definedName name="i_adjp_fl_initial_w1">Stock!$R$369:$R$371</definedName>
-    <definedName name="i_adjp_fl_initial_w3">Stock!$W$369:$W$371</definedName>
-    <definedName name="i_adjp_lw_initial_w0">Stock!$J$369</definedName>
-    <definedName name="i_adjp_lw_initial_w1">Stock!$O$369:$O$371</definedName>
-    <definedName name="i_adjp_lw_initial_w3">Stock!$T$369:$T$371</definedName>
+    <definedName name="i_adjp_cfw_initial_w0">Stock!$K$364</definedName>
+    <definedName name="i_adjp_cfw_initial_w1">Stock!$P$364:$P$366</definedName>
+    <definedName name="i_adjp_cfw_initial_w3">Stock!$V$364:$V$366</definedName>
+    <definedName name="i_adjp_fd_initial_w0">Stock!$L$364</definedName>
+    <definedName name="i_adjp_fd_initial_w1">Stock!$Q$364:$Q$366</definedName>
+    <definedName name="i_adjp_fd_initial_w3">Stock!$U$364:$U$366</definedName>
+    <definedName name="i_adjp_fl_initial_w0">Stock!$M$364</definedName>
+    <definedName name="i_adjp_fl_initial_w1">Stock!$R$364:$R$366</definedName>
+    <definedName name="i_adjp_fl_initial_w3">Stock!$W$364:$W$366</definedName>
+    <definedName name="i_adjp_lw_initial_w0">Stock!$J$364</definedName>
+    <definedName name="i_adjp_lw_initial_w1">Stock!$O$364:$O$366</definedName>
+    <definedName name="i_adjp_lw_initial_w3">Stock!$T$364:$T$366</definedName>
     <definedName name="i_age_max">Stock!$I$71</definedName>
     <definedName name="i_age_max_offs">Stock!$I$72</definedName>
     <definedName name="i_b0_pos">Stock!$I$54</definedName>
@@ -112,7 +112,7 @@
     <definedName name="i_progeny_w2_len">Stock!$O$320</definedName>
     <definedName name="i_sim_periods_year">Stock!$I$70</definedName>
     <definedName name="i_transfer_exists_tg1">Stock!$K$127:$N$129</definedName>
-    <definedName name="i_w_idx_sire">OFFSET(Stock!$I$369,0,0,Stock!$J$320,1)</definedName>
+    <definedName name="i_w_idx_sire">OFFSET(Stock!$I$364,0,0,Stock!$J$320,1)</definedName>
     <definedName name="i_w_pos">Stock!$I$65</definedName>
     <definedName name="i_w_start_len1" localSheetId="1">Stock!$L$321</definedName>
     <definedName name="i_w_start_len3">Stock!$P$321</definedName>
@@ -1122,60 +1122,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="J358" authorId="0" shapeId="0" xr:uid="{693A6FF1-2DB9-4B79-B819-60CE71AB1300}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Michael Young (21512438):</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-#this is only the v type axis. it is expanded to full v axis in code.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H361" authorId="0" shapeId="0" xr:uid="{67EB845D-0B2A-4F06-A743-CE82E4536FB1}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Michael Young (21512438):</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-condensing happens at prejoining. </t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="292">
   <si>
     <t>Controls for this worksheet</t>
   </si>
@@ -2016,25 +1968,7 @@
     <t>R type</t>
   </si>
   <si>
-    <t>How many fvps occur in each dvp</t>
-  </si>
-  <si>
-    <t>DVP0</t>
-  </si>
-  <si>
-    <t>DVP1</t>
-  </si>
-  <si>
-    <t>DVP2</t>
-  </si>
-  <si>
-    <t>DVP3</t>
-  </si>
-  <si>
     <t>Dams FVP/DVP</t>
-  </si>
-  <si>
-    <t>Number of fvps since condenseing</t>
   </si>
   <si>
     <t>LW</t>
@@ -3252,7 +3186,7 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="195">
+  <cellXfs count="189">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="25" xfId="3">
@@ -3709,24 +3643,6 @@
     </xf>
     <xf numFmtId="0" fontId="28" fillId="8" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="43" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="44" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -7236,10 +7152,10 @@
   <sheetPr codeName="Sheet1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AE384"/>
+  <dimension ref="A1:AE379"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="K161" sqref="K161"/>
+    <sheetView tabSelected="1" topLeftCell="A328" workbookViewId="0">
+      <selection activeCell="J356" sqref="J356"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.35"/>
@@ -21786,7 +21702,7 @@
       <c r="A308" s="1"/>
       <c r="B308" s="33"/>
       <c r="C308" s="76">
-        <f>INT(MAX($C$319:$D$373))+1</f>
+        <f>INT(MAX($C$319:$D$368))+1</f>
         <v>5</v>
       </c>
       <c r="D308" s="3"/>
@@ -22227,7 +22143,7 @@
       <c r="K320" s="2"/>
       <c r="L320" s="132">
         <f>i_w_start_len1*i_n1_len^L323</f>
-        <v>243</v>
+        <v>81</v>
       </c>
       <c r="M320" s="2"/>
       <c r="N320" s="127" t="s">
@@ -22238,7 +22154,7 @@
       </c>
       <c r="P320" s="132">
         <f>i_w_start_len3*i_n3_len^P323</f>
-        <v>243</v>
+        <v>81</v>
       </c>
       <c r="Q320" s="2"/>
       <c r="R320" s="2"/>
@@ -22351,14 +22267,14 @@
       <c r="K323" s="2"/>
       <c r="L323" s="132">
         <f>COUNTIF(J341:O341,TRUE)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M323" s="2"/>
       <c r="N323" s="2"/>
       <c r="O323" s="2"/>
       <c r="P323" s="132">
         <f>COUNTIF(J353:M353,TRUE)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q323" s="126"/>
       <c r="R323" s="178" t="s">
@@ -22516,13 +22432,13 @@
       <c r="H327" s="2"/>
       <c r="I327" s="56"/>
       <c r="J327" s="2" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="K327" s="2" t="s">
         <v>115</v>
       </c>
       <c r="L327" s="2" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="M327" s="2" t="s">
         <v>115</v>
@@ -22530,7 +22446,7 @@
       <c r="N327" s="2"/>
       <c r="O327" s="2"/>
       <c r="P327" s="2" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="Q327" s="2" t="s">
         <v>115</v>
@@ -22990,7 +22906,7 @@
       <c r="F338" s="5"/>
       <c r="G338" s="4"/>
       <c r="H338" s="107" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="I338" s="2"/>
       <c r="J338" s="2"/>
@@ -23017,7 +22933,7 @@
       <c r="A339" s="1"/>
       <c r="B339" s="33"/>
       <c r="C339" s="76">
-        <f t="shared" ref="C339:C364" si="44">INT($C$309)+3</f>
+        <f t="shared" ref="C339:C359" si="44">INT($C$309)+3</f>
         <v>4</v>
       </c>
       <c r="D339" s="4"/>
@@ -23091,7 +23007,7 @@
       </c>
       <c r="P340" s="2"/>
       <c r="Q340" s="2" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="R340" s="2"/>
       <c r="S340" s="2"/>
@@ -23123,7 +23039,7 @@
         <v>264</v>
       </c>
       <c r="J341" s="31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K341" s="31" t="b">
         <v>1</v>
@@ -23143,7 +23059,7 @@
       <c r="P341" s="2"/>
       <c r="Q341" s="31">
         <f>K342</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R341" s="2"/>
       <c r="S341" s="2"/>
@@ -23166,32 +23082,32 @@
       <c r="F342" s="5"/>
       <c r="G342" s="4"/>
       <c r="H342" s="2" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="I342" s="2"/>
       <c r="J342" s="132">
         <f>COUNTIF($J$341:J341,TRUE)-1</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="K342" s="132">
         <f>COUNTIF($J$341:K341,TRUE)-1</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L342" s="132">
         <f>COUNTIF($J$341:L341,TRUE)-1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M342" s="132">
         <f>COUNTIF($J$341:M341,TRUE)-1</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N342" s="132">
         <f>COUNTIF($J$341:N341,TRUE)-1</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O342" s="132">
         <f>COUNTIF($J$341:O341,TRUE)-1</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P342" s="2"/>
       <c r="Q342" s="2"/>
@@ -23225,7 +23141,7 @@
         <v>264</v>
       </c>
       <c r="J343" s="31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K343" s="31" t="b">
         <v>1</v>
@@ -23265,7 +23181,7 @@
       <c r="F344" s="5"/>
       <c r="G344" s="4"/>
       <c r="H344" s="2" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="I344" s="2"/>
       <c r="J344" s="31" t="b">
@@ -23394,13 +23310,13 @@
       <c r="H347" s="2"/>
       <c r="I347" s="171"/>
       <c r="J347" s="172" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="K347" s="172" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="L347" s="172" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="M347" s="2"/>
       <c r="N347" s="2"/>
@@ -23428,17 +23344,20 @@
       <c r="F348" s="5"/>
       <c r="G348" s="4"/>
       <c r="H348" s="2" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="I348" s="171"/>
       <c r="J348" s="31">
-        <v>1</v>
+        <f>K342</f>
+        <v>0</v>
       </c>
       <c r="K348" s="31">
+        <f t="shared" ref="K348" si="45">L342</f>
+        <v>1</v>
+      </c>
+      <c r="L348" s="31">
+        <f>M342</f>
         <v>2</v>
-      </c>
-      <c r="L348" s="31">
-        <v>3</v>
       </c>
       <c r="M348" s="2"/>
       <c r="N348" s="2"/>
@@ -23499,7 +23418,7 @@
       <c r="F350" s="5"/>
       <c r="G350" s="4"/>
       <c r="H350" s="107" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="I350" s="2"/>
       <c r="J350" s="2"/>
@@ -23539,13 +23458,13 @@
         <v>266</v>
       </c>
       <c r="K351" s="2" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="L351" s="2" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="M351" s="2" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="N351" s="2"/>
       <c r="O351" s="2"/>
@@ -23592,7 +23511,7 @@
       <c r="O352" s="2"/>
       <c r="P352" s="2"/>
       <c r="Q352" s="2" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="R352" s="2"/>
       <c r="S352" s="2"/>
@@ -23624,7 +23543,7 @@
         <v>264</v>
       </c>
       <c r="J353" s="31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K353" s="31" t="b">
         <v>1</v>
@@ -23640,7 +23559,7 @@
       <c r="P353" s="2"/>
       <c r="Q353" s="31">
         <f>K354</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R353" s="2"/>
       <c r="S353" s="2"/>
@@ -23663,24 +23582,24 @@
       <c r="F354" s="5"/>
       <c r="G354" s="4"/>
       <c r="H354" s="2" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="I354" s="2"/>
       <c r="J354" s="132">
         <f>COUNTIF($J$353:J353,TRUE)-1</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="K354" s="132">
         <f>COUNTIF($J$353:K353,TRUE)-1</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L354" s="132">
         <f>COUNTIF($J$353:L353,TRUE)-1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M354" s="132">
         <f>COUNTIF($J$353:M353,TRUE)-1</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N354" s="2"/>
       <c r="O354" s="2"/>
@@ -23716,7 +23635,7 @@
         <v>264</v>
       </c>
       <c r="J355" s="31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K355" s="31" t="b">
         <v>1</v>
@@ -23820,34 +23739,26 @@
       </c>
       <c r="D358" s="4"/>
       <c r="E358" s="5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F358" s="5"/>
       <c r="G358" s="4"/>
       <c r="H358" s="2"/>
       <c r="I358" s="2"/>
-      <c r="J358" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="K358" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="L358" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="M358" s="2" t="s">
-        <v>276</v>
-      </c>
+      <c r="J358" s="2"/>
+      <c r="K358" s="2"/>
+      <c r="L358" s="2"/>
+      <c r="M358" s="2"/>
       <c r="N358" s="2"/>
       <c r="O358" s="2"/>
       <c r="P358" s="2"/>
-      <c r="Q358" s="2"/>
-      <c r="R358" s="2"/>
-      <c r="S358" s="2"/>
-      <c r="T358" s="2"/>
-      <c r="U358" s="2"/>
-      <c r="V358" s="2"/>
-      <c r="W358" s="2"/>
+      <c r="Q358" s="184"/>
+      <c r="R358" s="185"/>
+      <c r="S358" s="185"/>
+      <c r="T358" s="185"/>
+      <c r="U358" s="185"/>
+      <c r="V358" s="185"/>
+      <c r="W358" s="186"/>
       <c r="X358" s="4"/>
       <c r="Y358" s="16"/>
       <c r="Z358" s="1"/>
@@ -23863,28 +23774,16 @@
       </c>
       <c r="D359" s="4"/>
       <c r="E359" s="5">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F359" s="5"/>
       <c r="G359" s="4"/>
-      <c r="H359" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="I359" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="J359" s="31">
-        <v>1</v>
-      </c>
-      <c r="K359" s="31">
-        <v>1</v>
-      </c>
-      <c r="L359" s="31">
-        <v>1</v>
-      </c>
-      <c r="M359" s="31">
-        <v>2</v>
-      </c>
+      <c r="H359" s="2"/>
+      <c r="I359" s="2"/>
+      <c r="J359" s="2"/>
+      <c r="K359" s="2"/>
+      <c r="L359" s="2"/>
+      <c r="M359" s="2"/>
       <c r="N359" s="2"/>
       <c r="O359" s="2"/>
       <c r="P359" s="2"/>
@@ -23901,315 +23800,359 @@
       <c r="AA359" s="1"/>
       <c r="AB359" s="1"/>
     </row>
-    <row r="360" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:28" s="155" customFormat="1" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A360" s="1"/>
       <c r="B360" s="33"/>
       <c r="C360" s="76">
-        <f t="shared" si="44"/>
-        <v>4</v>
+        <f>INT($C$309)+3.005</f>
+        <v>4.0049999999999999</v>
       </c>
       <c r="D360" s="4"/>
-      <c r="E360" s="5">
+      <c r="E360" s="4"/>
+      <c r="F360" s="4"/>
+      <c r="G360" s="4"/>
+      <c r="H360" s="86"/>
+      <c r="I360" s="86"/>
+      <c r="J360" s="86"/>
+      <c r="K360" s="86"/>
+      <c r="L360" s="86"/>
+      <c r="M360" s="86"/>
+      <c r="N360" s="86"/>
+      <c r="O360" s="86"/>
+      <c r="P360" s="86"/>
+      <c r="Q360" s="86"/>
+      <c r="R360" s="86"/>
+      <c r="S360" s="86"/>
+      <c r="T360" s="86"/>
+      <c r="U360" s="86"/>
+      <c r="V360" s="86"/>
+      <c r="W360" s="86"/>
+      <c r="X360" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F360" s="5"/>
-      <c r="G360" s="4"/>
-      <c r="H360" s="2"/>
-      <c r="I360" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="J360" s="31">
-        <v>1</v>
-      </c>
-      <c r="K360" s="31">
-        <v>1</v>
-      </c>
-      <c r="L360" s="31">
-        <v>1</v>
-      </c>
-      <c r="M360" s="31">
-        <v>2</v>
-      </c>
-      <c r="N360" s="2"/>
-      <c r="O360" s="2"/>
-      <c r="P360" s="2"/>
-      <c r="Q360" s="184"/>
-      <c r="R360" s="185"/>
-      <c r="S360" s="185"/>
-      <c r="T360" s="185"/>
-      <c r="U360" s="185"/>
-      <c r="V360" s="185"/>
-      <c r="W360" s="186"/>
-      <c r="X360" s="4"/>
       <c r="Y360" s="16"/>
       <c r="Z360" s="1"/>
       <c r="AA360" s="1"/>
       <c r="AB360" s="1"/>
     </row>
-    <row r="361" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:28" s="102" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A361" s="1"/>
       <c r="B361" s="33"/>
       <c r="C361" s="76">
-        <f t="shared" si="44"/>
-        <v>4</v>
-      </c>
-      <c r="D361" s="4"/>
-      <c r="E361" s="5">
-        <v>4</v>
-      </c>
-      <c r="F361" s="5"/>
+        <f>INT($C$309)+2.005</f>
+        <v>3.0049999999999999</v>
+      </c>
+      <c r="D361" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E361" s="4"/>
+      <c r="F361" s="4"/>
       <c r="G361" s="4"/>
-      <c r="H361" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="I361" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="J361" s="31">
-        <v>0</v>
-      </c>
-      <c r="K361" s="31">
-        <v>1</v>
-      </c>
-      <c r="L361" s="31">
-        <v>2</v>
-      </c>
-      <c r="M361" s="31">
-        <v>2</v>
-      </c>
-      <c r="N361" s="2"/>
-      <c r="O361" s="2"/>
-      <c r="P361" s="2"/>
-      <c r="Q361" s="187"/>
-      <c r="R361" s="188"/>
-      <c r="S361" s="188"/>
-      <c r="T361" s="188"/>
-      <c r="U361" s="188"/>
-      <c r="V361" s="188"/>
-      <c r="W361" s="189"/>
+      <c r="H361" s="98"/>
+      <c r="I361" s="98"/>
+      <c r="J361" s="98"/>
+      <c r="K361" s="98"/>
+      <c r="L361" s="98"/>
+      <c r="M361" s="98"/>
+      <c r="N361" s="98"/>
+      <c r="O361" s="98"/>
+      <c r="P361" s="98"/>
+      <c r="Q361" s="98"/>
+      <c r="R361" s="98"/>
+      <c r="S361" s="98"/>
+      <c r="T361" s="98"/>
+      <c r="U361" s="98"/>
+      <c r="V361" s="98"/>
+      <c r="W361" s="98"/>
       <c r="X361" s="4"/>
       <c r="Y361" s="16"/>
       <c r="Z361" s="1"/>
       <c r="AA361" s="1"/>
       <c r="AB361" s="1"/>
     </row>
-    <row r="362" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:28" s="102" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A362" s="1"/>
       <c r="B362" s="33"/>
       <c r="C362" s="76">
-        <f t="shared" si="44"/>
-        <v>4</v>
+        <f>INT($C$309)+2</f>
+        <v>3</v>
       </c>
       <c r="D362" s="4"/>
-      <c r="E362" s="5">
-        <v>5</v>
-      </c>
+      <c r="E362" s="5"/>
       <c r="F362" s="5"/>
       <c r="G362" s="4"/>
-      <c r="H362" s="2"/>
-      <c r="I362" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="J362" s="31">
-        <v>0</v>
-      </c>
-      <c r="K362" s="31">
-        <v>1</v>
-      </c>
-      <c r="L362" s="31">
-        <v>2</v>
-      </c>
-      <c r="M362" s="31">
-        <v>2</v>
-      </c>
+      <c r="H362" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="I362" s="149"/>
+      <c r="J362" s="107" t="s">
+        <v>75</v>
+      </c>
+      <c r="K362" s="107"/>
+      <c r="L362" s="107"/>
+      <c r="M362" s="107"/>
       <c r="N362" s="2"/>
-      <c r="O362" s="2"/>
+      <c r="O362" s="107" t="s">
+        <v>76</v>
+      </c>
       <c r="P362" s="2"/>
-      <c r="Q362" s="187"/>
-      <c r="R362" s="188"/>
-      <c r="S362" s="188"/>
-      <c r="T362" s="188"/>
-      <c r="U362" s="188"/>
-      <c r="V362" s="188"/>
-      <c r="W362" s="189"/>
+      <c r="Q362" s="2"/>
+      <c r="R362" s="2"/>
+      <c r="S362" s="2"/>
+      <c r="T362" s="107" t="s">
+        <v>78</v>
+      </c>
+      <c r="U362" s="2"/>
+      <c r="V362" s="2"/>
+      <c r="W362" s="2"/>
       <c r="X362" s="4"/>
       <c r="Y362" s="16"/>
       <c r="Z362" s="1"/>
       <c r="AA362" s="1"/>
       <c r="AB362" s="1"/>
     </row>
-    <row r="363" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A363" s="1"/>
       <c r="B363" s="33"/>
-      <c r="C363" s="76">
-        <f t="shared" si="44"/>
-        <v>4</v>
-      </c>
+      <c r="C363" s="76"/>
       <c r="D363" s="4"/>
-      <c r="E363" s="5">
-        <v>6</v>
-      </c>
+      <c r="E363" s="5"/>
       <c r="F363" s="5"/>
       <c r="G363" s="4"/>
       <c r="H363" s="2"/>
-      <c r="I363" s="2"/>
-      <c r="J363" s="2"/>
-      <c r="K363" s="2"/>
-      <c r="L363" s="2"/>
-      <c r="M363" s="2"/>
+      <c r="I363" s="149"/>
+      <c r="J363" s="107" t="s">
+        <v>273</v>
+      </c>
+      <c r="K363" s="107" t="s">
+        <v>274</v>
+      </c>
+      <c r="L363" s="107" t="s">
+        <v>275</v>
+      </c>
+      <c r="M363" s="107" t="s">
+        <v>276</v>
+      </c>
       <c r="N363" s="2"/>
-      <c r="O363" s="2"/>
-      <c r="P363" s="2"/>
-      <c r="Q363" s="190"/>
-      <c r="R363" s="191"/>
-      <c r="S363" s="191"/>
-      <c r="T363" s="191"/>
-      <c r="U363" s="191"/>
-      <c r="V363" s="191"/>
-      <c r="W363" s="192"/>
+      <c r="O363" s="107" t="s">
+        <v>273</v>
+      </c>
+      <c r="P363" s="107" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q363" s="107" t="s">
+        <v>275</v>
+      </c>
+      <c r="R363" s="107" t="s">
+        <v>276</v>
+      </c>
+      <c r="S363" s="2"/>
+      <c r="T363" s="107" t="s">
+        <v>273</v>
+      </c>
+      <c r="U363" s="107" t="s">
+        <v>274</v>
+      </c>
+      <c r="V363" s="107" t="s">
+        <v>275</v>
+      </c>
+      <c r="W363" s="107" t="s">
+        <v>276</v>
+      </c>
       <c r="X363" s="4"/>
       <c r="Y363" s="16"/>
       <c r="Z363" s="1"/>
       <c r="AA363" s="1"/>
       <c r="AB363" s="1"/>
     </row>
-    <row r="364" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:28" s="102" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A364" s="1"/>
       <c r="B364" s="33"/>
       <c r="C364" s="76">
-        <f t="shared" si="44"/>
-        <v>4</v>
+        <f>INT($C$309)+2</f>
+        <v>3</v>
       </c>
       <c r="D364" s="4"/>
       <c r="E364" s="5">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F364" s="5"/>
       <c r="G364" s="4"/>
-      <c r="H364" s="2"/>
-      <c r="I364" s="2"/>
-      <c r="J364" s="2"/>
-      <c r="K364" s="2"/>
-      <c r="L364" s="2"/>
-      <c r="M364" s="2"/>
+      <c r="H364" s="61" t="s">
+        <v>283</v>
+      </c>
+      <c r="I364" s="149"/>
+      <c r="J364" s="162">
+        <v>0</v>
+      </c>
+      <c r="K364" s="106">
+        <v>0</v>
+      </c>
+      <c r="L364" s="106">
+        <v>0</v>
+      </c>
+      <c r="M364" s="106">
+        <v>0</v>
+      </c>
       <c r="N364" s="2"/>
-      <c r="O364" s="2"/>
-      <c r="P364" s="2"/>
-      <c r="Q364" s="2"/>
-      <c r="R364" s="2"/>
+      <c r="O364" s="106">
+        <v>0</v>
+      </c>
+      <c r="P364" s="106">
+        <v>0</v>
+      </c>
+      <c r="Q364" s="106">
+        <v>0</v>
+      </c>
+      <c r="R364" s="106">
+        <v>0</v>
+      </c>
       <c r="S364" s="2"/>
-      <c r="T364" s="2"/>
-      <c r="U364" s="2"/>
-      <c r="V364" s="2"/>
-      <c r="W364" s="2"/>
+      <c r="T364" s="106">
+        <v>0</v>
+      </c>
+      <c r="U364" s="106">
+        <v>0</v>
+      </c>
+      <c r="V364" s="106">
+        <v>0</v>
+      </c>
+      <c r="W364" s="106">
+        <v>0</v>
+      </c>
       <c r="X364" s="4"/>
       <c r="Y364" s="16"/>
       <c r="Z364" s="1"/>
       <c r="AA364" s="1"/>
       <c r="AB364" s="1"/>
     </row>
-    <row r="365" spans="1:28" s="155" customFormat="1" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:28" s="130" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A365" s="1"/>
       <c r="B365" s="33"/>
       <c r="C365" s="76">
-        <f>INT($C$309)+3.005</f>
-        <v>4.0049999999999999</v>
+        <f>INT($C$309)+2</f>
+        <v>3</v>
       </c>
       <c r="D365" s="4"/>
-      <c r="E365" s="4"/>
-      <c r="F365" s="4"/>
+      <c r="E365" s="5">
+        <v>27</v>
+      </c>
+      <c r="F365" s="5"/>
       <c r="G365" s="4"/>
-      <c r="H365" s="86"/>
-      <c r="I365" s="86"/>
-      <c r="J365" s="86"/>
-      <c r="K365" s="86"/>
-      <c r="L365" s="86"/>
-      <c r="M365" s="86"/>
-      <c r="N365" s="86"/>
-      <c r="O365" s="86"/>
-      <c r="P365" s="86"/>
-      <c r="Q365" s="86"/>
-      <c r="R365" s="86"/>
-      <c r="S365" s="86"/>
-      <c r="T365" s="86"/>
-      <c r="U365" s="86"/>
-      <c r="V365" s="86"/>
-      <c r="W365" s="86"/>
-      <c r="X365" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="H365" s="61" t="s">
+        <v>284</v>
+      </c>
+      <c r="I365" s="149"/>
+      <c r="J365" s="149"/>
+      <c r="K365" s="2"/>
+      <c r="L365" s="107"/>
+      <c r="M365" s="2"/>
+      <c r="N365" s="2"/>
+      <c r="O365" s="32">
+        <v>0.15</v>
+      </c>
+      <c r="P365" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="Q365" s="32">
+        <v>0.05</v>
+      </c>
+      <c r="R365" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="S365" s="2"/>
+      <c r="T365" s="32">
+        <v>0.15</v>
+      </c>
+      <c r="U365" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="V365" s="32">
+        <v>0.05</v>
+      </c>
+      <c r="W365" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="X365" s="4"/>
       <c r="Y365" s="16"/>
       <c r="Z365" s="1"/>
       <c r="AA365" s="1"/>
       <c r="AB365" s="1"/>
     </row>
-    <row r="366" spans="1:28" s="102" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:28" s="130" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A366" s="1"/>
       <c r="B366" s="33"/>
       <c r="C366" s="76">
-        <f>INT($C$309)+2.005</f>
-        <v>3.0049999999999999</v>
-      </c>
-      <c r="D366" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E366" s="4"/>
-      <c r="F366" s="4"/>
+        <f>INT($C$309)+2</f>
+        <v>3</v>
+      </c>
+      <c r="D366" s="4"/>
+      <c r="E366" s="5">
+        <v>54</v>
+      </c>
+      <c r="F366" s="5"/>
       <c r="G366" s="4"/>
-      <c r="H366" s="98"/>
-      <c r="I366" s="98"/>
-      <c r="J366" s="98"/>
-      <c r="K366" s="98"/>
-      <c r="L366" s="98"/>
-      <c r="M366" s="98"/>
-      <c r="N366" s="98"/>
-      <c r="O366" s="98"/>
-      <c r="P366" s="98"/>
-      <c r="Q366" s="98"/>
-      <c r="R366" s="98"/>
-      <c r="S366" s="98"/>
-      <c r="T366" s="98"/>
-      <c r="U366" s="98"/>
-      <c r="V366" s="98"/>
-      <c r="W366" s="98"/>
+      <c r="H366" s="61" t="s">
+        <v>285</v>
+      </c>
+      <c r="I366" s="149"/>
+      <c r="J366" s="149"/>
+      <c r="K366" s="2"/>
+      <c r="L366" s="107"/>
+      <c r="M366" s="2"/>
+      <c r="N366" s="2"/>
+      <c r="O366" s="32">
+        <v>-0.15</v>
+      </c>
+      <c r="P366" s="32">
+        <v>-0.1</v>
+      </c>
+      <c r="Q366" s="32">
+        <v>-0.05</v>
+      </c>
+      <c r="R366" s="32">
+        <v>-0.1</v>
+      </c>
+      <c r="S366" s="2"/>
+      <c r="T366" s="32">
+        <v>-0.15</v>
+      </c>
+      <c r="U366" s="32">
+        <v>-0.1</v>
+      </c>
+      <c r="V366" s="32">
+        <v>-0.05</v>
+      </c>
+      <c r="W366" s="32">
+        <v>-0.1</v>
+      </c>
       <c r="X366" s="4"/>
       <c r="Y366" s="16"/>
       <c r="Z366" s="1"/>
       <c r="AA366" s="1"/>
       <c r="AB366" s="1"/>
     </row>
-    <row r="367" spans="1:28" s="102" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A367" s="1"/>
       <c r="B367" s="33"/>
-      <c r="C367" s="76">
-        <f>INT($C$309)+2</f>
-        <v>3</v>
-      </c>
+      <c r="C367" s="76"/>
       <c r="D367" s="4"/>
       <c r="E367" s="5"/>
       <c r="F367" s="5"/>
       <c r="G367" s="4"/>
-      <c r="H367" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="I367" s="149"/>
-      <c r="J367" s="107" t="s">
-        <v>75</v>
-      </c>
-      <c r="K367" s="107"/>
+      <c r="H367" s="168"/>
+      <c r="I367" s="167"/>
+      <c r="J367" s="2"/>
+      <c r="K367" s="2"/>
       <c r="L367" s="107"/>
-      <c r="M367" s="107"/>
+      <c r="M367" s="2"/>
       <c r="N367" s="2"/>
-      <c r="O367" s="107" t="s">
-        <v>76</v>
-      </c>
+      <c r="O367" s="2"/>
       <c r="P367" s="2"/>
       <c r="Q367" s="2"/>
       <c r="R367" s="2"/>
       <c r="S367" s="2"/>
-      <c r="T367" s="107" t="s">
-        <v>78</v>
-      </c>
+      <c r="T367" s="2"/>
       <c r="U367" s="2"/>
       <c r="V367" s="2"/>
       <c r="W367" s="2"/>
@@ -24219,400 +24162,299 @@
       <c r="AA367" s="1"/>
       <c r="AB367" s="1"/>
     </row>
-    <row r="368" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:28" s="102" customFormat="1" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
       <c r="A368" s="1"/>
       <c r="B368" s="33"/>
-      <c r="C368" s="76"/>
+      <c r="C368" s="76">
+        <f>INT($C$309)+3.005</f>
+        <v>4.0049999999999999</v>
+      </c>
       <c r="D368" s="4"/>
-      <c r="E368" s="5"/>
-      <c r="F368" s="5"/>
+      <c r="E368" s="4"/>
+      <c r="F368" s="4"/>
       <c r="G368" s="4"/>
-      <c r="H368" s="2"/>
-      <c r="I368" s="149"/>
-      <c r="J368" s="107" t="s">
-        <v>279</v>
-      </c>
-      <c r="K368" s="107" t="s">
-        <v>280</v>
-      </c>
-      <c r="L368" s="107" t="s">
-        <v>281</v>
-      </c>
-      <c r="M368" s="107" t="s">
-        <v>282</v>
-      </c>
-      <c r="N368" s="2"/>
-      <c r="O368" s="107" t="s">
-        <v>279</v>
-      </c>
-      <c r="P368" s="107" t="s">
-        <v>280</v>
-      </c>
-      <c r="Q368" s="107" t="s">
-        <v>281</v>
-      </c>
-      <c r="R368" s="107" t="s">
-        <v>282</v>
-      </c>
-      <c r="S368" s="2"/>
-      <c r="T368" s="107" t="s">
-        <v>279</v>
-      </c>
-      <c r="U368" s="107" t="s">
-        <v>280</v>
-      </c>
-      <c r="V368" s="107" t="s">
-        <v>281</v>
-      </c>
-      <c r="W368" s="107" t="s">
-        <v>282</v>
-      </c>
-      <c r="X368" s="4"/>
+      <c r="H368" s="4"/>
+      <c r="I368" s="4"/>
+      <c r="J368" s="4"/>
+      <c r="K368" s="4"/>
+      <c r="L368" s="4"/>
+      <c r="M368" s="4"/>
+      <c r="N368" s="4"/>
+      <c r="O368" s="4"/>
+      <c r="P368" s="4"/>
+      <c r="Q368" s="4"/>
+      <c r="R368" s="4"/>
+      <c r="S368" s="4"/>
+      <c r="T368" s="4"/>
+      <c r="U368" s="4"/>
+      <c r="V368" s="4"/>
+      <c r="W368" s="4"/>
+      <c r="X368" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="Y368" s="16"/>
       <c r="Z368" s="1"/>
       <c r="AA368" s="1"/>
       <c r="AB368" s="1"/>
     </row>
-    <row r="369" spans="1:28" s="102" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:28" s="142" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A369" s="1"/>
       <c r="B369" s="33"/>
       <c r="C369" s="76">
-        <f>INT($C$309)+2</f>
-        <v>3</v>
+        <f>INT($C$309)+2.005</f>
+        <v>3.0049999999999999</v>
       </c>
       <c r="D369" s="4"/>
-      <c r="E369" s="5">
-        <v>0</v>
-      </c>
-      <c r="F369" s="5"/>
+      <c r="E369" s="4"/>
+      <c r="F369" s="4"/>
       <c r="G369" s="4"/>
-      <c r="H369" s="61" t="s">
-        <v>289</v>
-      </c>
-      <c r="I369" s="149"/>
-      <c r="J369" s="162">
-        <v>0</v>
-      </c>
-      <c r="K369" s="106">
-        <v>0</v>
-      </c>
-      <c r="L369" s="106">
-        <v>0</v>
-      </c>
-      <c r="M369" s="106">
-        <v>0</v>
-      </c>
-      <c r="N369" s="2"/>
-      <c r="O369" s="106">
-        <v>0</v>
-      </c>
-      <c r="P369" s="106">
-        <v>0</v>
-      </c>
-      <c r="Q369" s="106">
-        <v>0</v>
-      </c>
-      <c r="R369" s="106">
-        <v>0</v>
-      </c>
-      <c r="S369" s="2"/>
-      <c r="T369" s="106">
-        <v>0</v>
-      </c>
-      <c r="U369" s="106">
-        <v>0</v>
-      </c>
-      <c r="V369" s="106">
-        <v>0</v>
-      </c>
-      <c r="W369" s="106">
-        <v>0</v>
-      </c>
+      <c r="H369" s="4"/>
+      <c r="I369" s="4"/>
+      <c r="J369" s="4"/>
+      <c r="K369" s="4"/>
+      <c r="L369" s="4"/>
+      <c r="M369" s="4"/>
+      <c r="N369" s="4"/>
+      <c r="O369" s="4"/>
+      <c r="P369" s="4"/>
+      <c r="Q369" s="4"/>
+      <c r="R369" s="4"/>
+      <c r="S369" s="4"/>
+      <c r="T369" s="4"/>
+      <c r="U369" s="4"/>
+      <c r="V369" s="4"/>
+      <c r="W369" s="4"/>
       <c r="X369" s="4"/>
       <c r="Y369" s="16"/>
       <c r="Z369" s="1"/>
       <c r="AA369" s="1"/>
       <c r="AB369" s="1"/>
     </row>
-    <row r="370" spans="1:28" s="130" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:28" s="142" customFormat="1" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A370" s="1"/>
-      <c r="B370" s="33"/>
-      <c r="C370" s="76">
-        <f>INT($C$309)+2</f>
-        <v>3</v>
-      </c>
-      <c r="D370" s="4"/>
-      <c r="E370" s="5">
-        <v>27</v>
-      </c>
-      <c r="F370" s="5"/>
-      <c r="G370" s="4"/>
-      <c r="H370" s="61" t="s">
-        <v>290</v>
-      </c>
-      <c r="I370" s="149"/>
-      <c r="J370" s="149"/>
-      <c r="K370" s="2"/>
-      <c r="L370" s="107"/>
-      <c r="M370" s="2"/>
-      <c r="N370" s="2"/>
-      <c r="O370" s="32">
-        <v>0.15</v>
-      </c>
-      <c r="P370" s="32">
-        <v>0.1</v>
-      </c>
-      <c r="Q370" s="32">
-        <v>0.05</v>
-      </c>
-      <c r="R370" s="32">
-        <v>0.1</v>
-      </c>
-      <c r="S370" s="2"/>
-      <c r="T370" s="32">
-        <v>0.15</v>
-      </c>
-      <c r="U370" s="32">
-        <v>0.1</v>
-      </c>
-      <c r="V370" s="32">
-        <v>0.05</v>
-      </c>
-      <c r="W370" s="32">
-        <v>0.1</v>
-      </c>
-      <c r="X370" s="4"/>
-      <c r="Y370" s="16"/>
+      <c r="B370" s="35"/>
+      <c r="C370" s="79">
+        <f>INT($C$309)+1.005</f>
+        <v>2.0049999999999999</v>
+      </c>
+      <c r="D370" s="17"/>
+      <c r="E370" s="17"/>
+      <c r="F370" s="17"/>
+      <c r="G370" s="17"/>
+      <c r="H370" s="17"/>
+      <c r="I370" s="17"/>
+      <c r="J370" s="17"/>
+      <c r="K370" s="17"/>
+      <c r="L370" s="17"/>
+      <c r="M370" s="17"/>
+      <c r="N370" s="17"/>
+      <c r="O370" s="17"/>
+      <c r="P370" s="17"/>
+      <c r="Q370" s="17"/>
+      <c r="R370" s="17"/>
+      <c r="S370" s="17"/>
+      <c r="T370" s="17"/>
+      <c r="U370" s="17"/>
+      <c r="V370" s="17"/>
+      <c r="W370" s="17"/>
+      <c r="X370" s="17"/>
+      <c r="Y370" s="18" t="s">
+        <v>1</v>
+      </c>
       <c r="Z370" s="1"/>
       <c r="AA370" s="1"/>
       <c r="AB370" s="1"/>
     </row>
-    <row r="371" spans="1:28" s="130" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:28" s="142" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A371" s="1"/>
-      <c r="B371" s="33"/>
-      <c r="C371" s="76">
-        <f>INT($C$309)+2</f>
-        <v>3</v>
-      </c>
-      <c r="D371" s="4"/>
-      <c r="E371" s="5">
-        <v>54</v>
-      </c>
-      <c r="F371" s="5"/>
-      <c r="G371" s="4"/>
-      <c r="H371" s="61" t="s">
-        <v>291</v>
-      </c>
-      <c r="I371" s="149"/>
-      <c r="J371" s="149"/>
-      <c r="K371" s="2"/>
-      <c r="L371" s="107"/>
-      <c r="M371" s="2"/>
-      <c r="N371" s="2"/>
-      <c r="O371" s="32">
-        <v>-0.15</v>
-      </c>
-      <c r="P371" s="32">
-        <v>-0.1</v>
-      </c>
-      <c r="Q371" s="32">
-        <v>-0.05</v>
-      </c>
-      <c r="R371" s="32">
-        <v>-0.1</v>
-      </c>
-      <c r="S371" s="2"/>
-      <c r="T371" s="32">
-        <v>-0.15</v>
-      </c>
-      <c r="U371" s="32">
-        <v>-0.1</v>
-      </c>
-      <c r="V371" s="32">
-        <v>-0.05</v>
-      </c>
-      <c r="W371" s="32">
-        <v>-0.1</v>
-      </c>
-      <c r="X371" s="4"/>
-      <c r="Y371" s="16"/>
+      <c r="B371" s="19"/>
+      <c r="C371" s="80">
+        <f>INT($C$309)+0.005</f>
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="D371" s="19"/>
+      <c r="E371" s="19"/>
+      <c r="F371" s="19"/>
+      <c r="G371" s="19"/>
+      <c r="H371" s="19"/>
+      <c r="I371" s="19"/>
+      <c r="J371" s="19"/>
+      <c r="K371" s="19"/>
+      <c r="L371" s="19"/>
+      <c r="M371" s="19"/>
+      <c r="N371" s="19"/>
+      <c r="O371" s="19"/>
+      <c r="P371" s="19"/>
+      <c r="Q371" s="19"/>
+      <c r="R371" s="19"/>
+      <c r="S371" s="19"/>
+      <c r="T371" s="19"/>
+      <c r="U371" s="19"/>
+      <c r="V371" s="19"/>
+      <c r="W371" s="19"/>
+      <c r="X371" s="19"/>
+      <c r="Y371" s="19"/>
       <c r="Z371" s="1"/>
       <c r="AA371" s="1"/>
       <c r="AB371" s="1"/>
     </row>
-    <row r="372" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A372" s="1"/>
-      <c r="B372" s="33"/>
-      <c r="C372" s="76"/>
-      <c r="D372" s="4"/>
-      <c r="E372" s="5"/>
-      <c r="F372" s="5"/>
-      <c r="G372" s="4"/>
-      <c r="H372" s="168"/>
-      <c r="I372" s="167"/>
-      <c r="J372" s="2"/>
-      <c r="K372" s="2"/>
-      <c r="L372" s="107"/>
-      <c r="M372" s="2"/>
-      <c r="N372" s="2"/>
-      <c r="O372" s="2"/>
-      <c r="P372" s="2"/>
-      <c r="Q372" s="2"/>
-      <c r="R372" s="2"/>
-      <c r="S372" s="2"/>
-      <c r="T372" s="2"/>
-      <c r="U372" s="2"/>
-      <c r="V372" s="2"/>
-      <c r="W372" s="2"/>
-      <c r="X372" s="4"/>
-      <c r="Y372" s="16"/>
+      <c r="B372" s="1"/>
+      <c r="C372" s="76">
+        <f>INT($C$309)+2</f>
+        <v>3</v>
+      </c>
+      <c r="D372" s="1"/>
+      <c r="E372" s="1"/>
+      <c r="F372" s="1"/>
+      <c r="G372" s="1"/>
+      <c r="H372" s="1"/>
+      <c r="I372" s="1"/>
+      <c r="J372" s="1"/>
+      <c r="K372" s="1"/>
+      <c r="L372" s="1"/>
+      <c r="M372" s="1"/>
+      <c r="N372" s="1"/>
+      <c r="O372" s="1"/>
+      <c r="P372" s="1"/>
+      <c r="Q372" s="1"/>
+      <c r="R372" s="1"/>
+      <c r="S372" s="1"/>
+      <c r="T372" s="1"/>
+      <c r="U372" s="1"/>
+      <c r="V372" s="1"/>
+      <c r="W372" s="1"/>
+      <c r="X372" s="1"/>
+      <c r="Y372" s="1"/>
       <c r="Z372" s="1"/>
       <c r="AA372" s="1"/>
       <c r="AB372" s="1"/>
     </row>
-    <row r="373" spans="1:28" s="102" customFormat="1" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A373" s="1"/>
-      <c r="B373" s="33"/>
-      <c r="C373" s="76">
-        <f>INT($C$309)+3.005</f>
-        <v>4.0049999999999999</v>
-      </c>
-      <c r="D373" s="4"/>
-      <c r="E373" s="4"/>
-      <c r="F373" s="4"/>
-      <c r="G373" s="4"/>
-      <c r="H373" s="4"/>
-      <c r="I373" s="4"/>
-      <c r="J373" s="4"/>
-      <c r="K373" s="4"/>
-      <c r="L373" s="4"/>
-      <c r="M373" s="4"/>
-      <c r="N373" s="4"/>
-      <c r="O373" s="4"/>
-      <c r="P373" s="4"/>
-      <c r="Q373" s="4"/>
-      <c r="R373" s="4"/>
-      <c r="S373" s="4"/>
-      <c r="T373" s="4"/>
-      <c r="U373" s="4"/>
-      <c r="V373" s="4"/>
-      <c r="W373" s="4"/>
-      <c r="X373" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y373" s="16"/>
+      <c r="B373" s="1"/>
+      <c r="C373" s="69"/>
+      <c r="D373" s="1"/>
+      <c r="E373" s="1"/>
+      <c r="F373" s="1"/>
+      <c r="G373" s="1"/>
+      <c r="H373" s="1"/>
+      <c r="I373" s="1"/>
+      <c r="J373" s="1"/>
+      <c r="K373" s="1"/>
+      <c r="L373" s="1"/>
+      <c r="M373" s="1"/>
+      <c r="N373" s="1"/>
+      <c r="O373" s="1"/>
+      <c r="P373" s="1"/>
+      <c r="Q373" s="1"/>
+      <c r="R373" s="1"/>
+      <c r="S373" s="1"/>
+      <c r="T373" s="1"/>
+      <c r="U373" s="1"/>
+      <c r="V373" s="1"/>
+      <c r="W373" s="1"/>
+      <c r="X373" s="1"/>
+      <c r="Y373" s="1"/>
       <c r="Z373" s="1"/>
       <c r="AA373" s="1"/>
       <c r="AB373" s="1"/>
     </row>
-    <row r="374" spans="1:28" s="142" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A374" s="1"/>
-      <c r="B374" s="33"/>
-      <c r="C374" s="76">
-        <f>INT($C$309)+2.005</f>
-        <v>3.0049999999999999</v>
-      </c>
-      <c r="D374" s="4"/>
-      <c r="E374" s="4"/>
-      <c r="F374" s="4"/>
-      <c r="G374" s="4"/>
-      <c r="H374" s="4"/>
-      <c r="I374" s="4"/>
-      <c r="J374" s="4"/>
-      <c r="K374" s="4"/>
-      <c r="L374" s="4"/>
-      <c r="M374" s="4"/>
-      <c r="N374" s="4"/>
-      <c r="O374" s="4"/>
-      <c r="P374" s="4"/>
-      <c r="Q374" s="4"/>
-      <c r="R374" s="4"/>
-      <c r="S374" s="4"/>
-      <c r="T374" s="4"/>
-      <c r="U374" s="4"/>
-      <c r="V374" s="4"/>
-      <c r="W374" s="4"/>
-      <c r="X374" s="4"/>
-      <c r="Y374" s="16"/>
+      <c r="B374" s="1"/>
+      <c r="C374" s="69"/>
+      <c r="D374" s="1"/>
+      <c r="E374" s="1"/>
+      <c r="F374" s="1"/>
+      <c r="G374" s="1"/>
+      <c r="H374" s="1"/>
+      <c r="I374" s="1"/>
+      <c r="J374" s="1"/>
+      <c r="K374" s="1"/>
+      <c r="L374" s="1"/>
+      <c r="M374" s="1"/>
+      <c r="N374" s="1"/>
+      <c r="O374" s="1"/>
+      <c r="P374" s="1"/>
+      <c r="Q374" s="1"/>
+      <c r="R374" s="1"/>
+      <c r="S374" s="1"/>
+      <c r="T374" s="1"/>
+      <c r="U374" s="1"/>
+      <c r="V374" s="1"/>
+      <c r="W374" s="1"/>
+      <c r="X374" s="1"/>
+      <c r="Y374" s="1"/>
       <c r="Z374" s="1"/>
       <c r="AA374" s="1"/>
       <c r="AB374" s="1"/>
     </row>
-    <row r="375" spans="1:28" s="142" customFormat="1" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A375" s="1"/>
-      <c r="B375" s="35"/>
-      <c r="C375" s="79">
-        <f>INT($C$309)+1.005</f>
-        <v>2.0049999999999999</v>
-      </c>
-      <c r="D375" s="17"/>
-      <c r="E375" s="17"/>
-      <c r="F375" s="17"/>
-      <c r="G375" s="17"/>
-      <c r="H375" s="17"/>
-      <c r="I375" s="17"/>
-      <c r="J375" s="17"/>
-      <c r="K375" s="17"/>
-      <c r="L375" s="17"/>
-      <c r="M375" s="17"/>
-      <c r="N375" s="17"/>
-      <c r="O375" s="17"/>
-      <c r="P375" s="17"/>
-      <c r="Q375" s="17"/>
-      <c r="R375" s="17"/>
-      <c r="S375" s="17"/>
-      <c r="T375" s="17"/>
-      <c r="U375" s="17"/>
-      <c r="V375" s="17"/>
-      <c r="W375" s="17"/>
-      <c r="X375" s="17"/>
-      <c r="Y375" s="18" t="s">
-        <v>1</v>
-      </c>
+      <c r="B375" s="1"/>
+      <c r="C375" s="69"/>
+      <c r="D375" s="1"/>
+      <c r="E375" s="1"/>
+      <c r="F375" s="1"/>
+      <c r="G375" s="1"/>
+      <c r="H375" s="1"/>
+      <c r="I375" s="1"/>
+      <c r="J375" s="1"/>
+      <c r="K375" s="1"/>
+      <c r="L375" s="1"/>
+      <c r="M375" s="1"/>
+      <c r="N375" s="1"/>
+      <c r="O375" s="1"/>
+      <c r="P375" s="1"/>
+      <c r="Q375" s="1"/>
+      <c r="R375" s="1"/>
+      <c r="S375" s="1"/>
+      <c r="T375" s="1"/>
+      <c r="U375" s="1"/>
+      <c r="V375" s="1"/>
+      <c r="W375" s="1"/>
+      <c r="X375" s="1"/>
+      <c r="Y375" s="1"/>
       <c r="Z375" s="1"/>
       <c r="AA375" s="1"/>
       <c r="AB375" s="1"/>
     </row>
-    <row r="376" spans="1:28" s="142" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A376" s="1"/>
-      <c r="B376" s="19"/>
-      <c r="C376" s="80">
-        <f>INT($C$309)+0.005</f>
-        <v>1.0049999999999999</v>
-      </c>
-      <c r="D376" s="19"/>
-      <c r="E376" s="19"/>
-      <c r="F376" s="19"/>
-      <c r="G376" s="19"/>
-      <c r="H376" s="19"/>
-      <c r="I376" s="19"/>
-      <c r="J376" s="19"/>
-      <c r="K376" s="19"/>
-      <c r="L376" s="19"/>
-      <c r="M376" s="19"/>
-      <c r="N376" s="19"/>
-      <c r="O376" s="19"/>
-      <c r="P376" s="19"/>
-      <c r="Q376" s="19"/>
-      <c r="R376" s="19"/>
-      <c r="S376" s="19"/>
-      <c r="T376" s="19"/>
-      <c r="U376" s="19"/>
-      <c r="V376" s="19"/>
-      <c r="W376" s="19"/>
-      <c r="X376" s="19"/>
-      <c r="Y376" s="19"/>
+      <c r="B376" s="1"/>
+      <c r="C376" s="69"/>
+      <c r="D376" s="1"/>
+      <c r="E376" s="1"/>
+      <c r="F376" s="1"/>
+      <c r="G376" s="1"/>
+      <c r="H376" s="1"/>
+      <c r="I376" s="1"/>
+      <c r="J376" s="1"/>
+      <c r="K376" s="1"/>
+      <c r="L376" s="1"/>
+      <c r="M376" s="1"/>
+      <c r="N376" s="1"/>
+      <c r="O376" s="1"/>
+      <c r="P376" s="1"/>
+      <c r="Q376" s="1"/>
+      <c r="R376" s="1"/>
+      <c r="S376" s="1"/>
+      <c r="T376" s="1"/>
+      <c r="U376" s="1"/>
+      <c r="V376" s="1"/>
+      <c r="W376" s="1"/>
+      <c r="X376" s="1"/>
+      <c r="Y376" s="1"/>
       <c r="Z376" s="1"/>
       <c r="AA376" s="1"/>
       <c r="AB376" s="1"/>
     </row>
-    <row r="377" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A377" s="1"/>
       <c r="B377" s="1"/>
-      <c r="C377" s="76">
-        <f>INT($C$309)+2</f>
-        <v>3</v>
-      </c>
+      <c r="C377" s="69"/>
       <c r="D377" s="1"/>
       <c r="E377" s="1"/>
       <c r="F377" s="1"/>
@@ -24670,157 +24512,7 @@
       <c r="AB378" s="1"/>
     </row>
     <row r="379" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A379" s="1"/>
-      <c r="B379" s="1"/>
-      <c r="C379" s="69"/>
-      <c r="D379" s="1"/>
-      <c r="E379" s="1"/>
-      <c r="F379" s="1"/>
-      <c r="G379" s="1"/>
-      <c r="H379" s="1"/>
-      <c r="I379" s="1"/>
-      <c r="J379" s="1"/>
-      <c r="K379" s="1"/>
-      <c r="L379" s="1"/>
-      <c r="M379" s="1"/>
-      <c r="N379" s="1"/>
-      <c r="O379" s="1"/>
-      <c r="P379" s="1"/>
-      <c r="Q379" s="1"/>
-      <c r="R379" s="1"/>
-      <c r="S379" s="1"/>
-      <c r="T379" s="1"/>
-      <c r="U379" s="1"/>
-      <c r="V379" s="1"/>
-      <c r="W379" s="1"/>
-      <c r="X379" s="1"/>
-      <c r="Y379" s="1"/>
-      <c r="Z379" s="1"/>
-      <c r="AA379" s="1"/>
-      <c r="AB379" s="1"/>
-    </row>
-    <row r="380" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A380" s="1"/>
-      <c r="B380" s="1"/>
-      <c r="C380" s="69"/>
-      <c r="D380" s="1"/>
-      <c r="E380" s="1"/>
-      <c r="F380" s="1"/>
-      <c r="G380" s="1"/>
-      <c r="H380" s="1"/>
-      <c r="I380" s="1"/>
-      <c r="J380" s="1"/>
-      <c r="K380" s="1"/>
-      <c r="L380" s="1"/>
-      <c r="M380" s="1"/>
-      <c r="N380" s="1"/>
-      <c r="O380" s="1"/>
-      <c r="P380" s="1"/>
-      <c r="Q380" s="1"/>
-      <c r="R380" s="1"/>
-      <c r="S380" s="1"/>
-      <c r="T380" s="1"/>
-      <c r="U380" s="1"/>
-      <c r="V380" s="1"/>
-      <c r="W380" s="1"/>
-      <c r="X380" s="1"/>
-      <c r="Y380" s="1"/>
-      <c r="Z380" s="1"/>
-      <c r="AA380" s="1"/>
-      <c r="AB380" s="1"/>
-    </row>
-    <row r="381" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A381" s="1"/>
-      <c r="B381" s="1"/>
-      <c r="C381" s="69"/>
-      <c r="D381" s="1"/>
-      <c r="E381" s="1"/>
-      <c r="F381" s="1"/>
-      <c r="G381" s="1"/>
-      <c r="H381" s="1"/>
-      <c r="I381" s="1"/>
-      <c r="J381" s="1"/>
-      <c r="K381" s="1"/>
-      <c r="L381" s="1"/>
-      <c r="M381" s="1"/>
-      <c r="N381" s="1"/>
-      <c r="O381" s="1"/>
-      <c r="P381" s="1"/>
-      <c r="Q381" s="1"/>
-      <c r="R381" s="1"/>
-      <c r="S381" s="1"/>
-      <c r="T381" s="1"/>
-      <c r="U381" s="1"/>
-      <c r="V381" s="1"/>
-      <c r="W381" s="1"/>
-      <c r="X381" s="1"/>
-      <c r="Y381" s="1"/>
-      <c r="Z381" s="1"/>
-      <c r="AA381" s="1"/>
-      <c r="AB381" s="1"/>
-    </row>
-    <row r="382" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A382" s="1"/>
-      <c r="B382" s="1"/>
-      <c r="C382" s="69"/>
-      <c r="D382" s="1"/>
-      <c r="E382" s="1"/>
-      <c r="F382" s="1"/>
-      <c r="G382" s="1"/>
-      <c r="H382" s="1"/>
-      <c r="I382" s="1"/>
-      <c r="J382" s="1"/>
-      <c r="K382" s="1"/>
-      <c r="L382" s="1"/>
-      <c r="M382" s="1"/>
-      <c r="N382" s="1"/>
-      <c r="O382" s="1"/>
-      <c r="P382" s="1"/>
-      <c r="Q382" s="1"/>
-      <c r="R382" s="1"/>
-      <c r="S382" s="1"/>
-      <c r="T382" s="1"/>
-      <c r="U382" s="1"/>
-      <c r="V382" s="1"/>
-      <c r="W382" s="1"/>
-      <c r="X382" s="1"/>
-      <c r="Y382" s="1"/>
-      <c r="Z382" s="1"/>
-      <c r="AA382" s="1"/>
-      <c r="AB382" s="1"/>
-    </row>
-    <row r="383" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A383" s="1"/>
-      <c r="B383" s="1"/>
-      <c r="C383" s="69"/>
-      <c r="D383" s="1"/>
-      <c r="E383" s="1"/>
-      <c r="F383" s="1"/>
-      <c r="G383" s="1"/>
-      <c r="H383" s="1"/>
-      <c r="I383" s="1"/>
-      <c r="J383" s="1"/>
-      <c r="K383" s="1"/>
-      <c r="L383" s="1"/>
-      <c r="M383" s="1"/>
-      <c r="N383" s="1"/>
-      <c r="O383" s="1"/>
-      <c r="P383" s="1"/>
-      <c r="Q383" s="1"/>
-      <c r="R383" s="1"/>
-      <c r="S383" s="1"/>
-      <c r="T383" s="1"/>
-      <c r="U383" s="1"/>
-      <c r="V383" s="1"/>
-      <c r="W383" s="1"/>
-      <c r="X383" s="1"/>
-      <c r="Y383" s="1"/>
-      <c r="Z383" s="1"/>
-      <c r="AA383" s="1"/>
-      <c r="AB383" s="1"/>
-    </row>
-    <row r="384" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="C384" s="75" t="s">
+      <c r="C379" s="75" t="s">
         <v>4</v>
       </c>
     </row>
@@ -24829,110 +24521,110 @@
     <mergeCell ref="J18:T18"/>
     <mergeCell ref="J21:T21"/>
     <mergeCell ref="R323:W325"/>
-    <mergeCell ref="Q360:W363"/>
+    <mergeCell ref="Q358:W358"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
-  <conditionalFormatting sqref="I369:J371 I367:I368">
+  <conditionalFormatting sqref="I364:J366 I362:I363">
     <cfRule type="expression" dxfId="20" priority="75">
-      <formula>($E367&gt;=I$320)</formula>
+      <formula>($E362&gt;=I$320)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O369:O371">
+  <conditionalFormatting sqref="O364:O366">
     <cfRule type="expression" dxfId="19" priority="76">
-      <formula>($E369&gt;=L$320)</formula>
+      <formula>($E364&gt;=L$320)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T369:T371">
+  <conditionalFormatting sqref="T364:T366">
     <cfRule type="expression" dxfId="18" priority="83">
-      <formula>($E369&gt;=P$320)</formula>
+      <formula>($E364&gt;=P$320)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P371">
+  <conditionalFormatting sqref="P366">
     <cfRule type="expression" dxfId="17" priority="149">
       <formula>(#REF!&gt;=L$320)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q371 U371">
+  <conditionalFormatting sqref="Q366 U366">
     <cfRule type="expression" dxfId="16" priority="150">
       <formula>(#REF!&gt;=L$320)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R371">
+  <conditionalFormatting sqref="R366">
     <cfRule type="expression" dxfId="15" priority="152">
       <formula>(#REF!&gt;=L$320)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W371">
+  <conditionalFormatting sqref="W366">
     <cfRule type="expression" dxfId="14" priority="153">
       <formula>(#REF!&gt;=P$320)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V371">
+  <conditionalFormatting sqref="V366">
     <cfRule type="expression" dxfId="13" priority="154">
       <formula>(#REF!&gt;=P$320)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P370">
+  <conditionalFormatting sqref="P365">
     <cfRule type="expression" dxfId="12" priority="155">
       <formula>(#REF!&gt;=L$320)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q370 U370">
+  <conditionalFormatting sqref="Q365 U365">
     <cfRule type="expression" dxfId="11" priority="156">
       <formula>(#REF!&gt;=L$320)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R370">
+  <conditionalFormatting sqref="R365">
     <cfRule type="expression" dxfId="10" priority="158">
       <formula>(#REF!&gt;=L$320)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W370">
+  <conditionalFormatting sqref="W365">
     <cfRule type="expression" dxfId="9" priority="159">
       <formula>(#REF!&gt;=P$320)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V370">
+  <conditionalFormatting sqref="V365">
     <cfRule type="expression" dxfId="8" priority="160">
       <formula>(#REF!&gt;=P$320)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K369">
+  <conditionalFormatting sqref="K364">
     <cfRule type="expression" dxfId="7" priority="161">
       <formula>(#REF!&gt;=J$320)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M369">
+  <conditionalFormatting sqref="M364">
     <cfRule type="expression" dxfId="6" priority="162">
       <formula>(#REF!&gt;=J$320)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L369">
+  <conditionalFormatting sqref="L364">
     <cfRule type="expression" dxfId="5" priority="163">
       <formula>(#REF!&gt;=J$320)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P369">
+  <conditionalFormatting sqref="P364">
     <cfRule type="expression" dxfId="4" priority="164">
       <formula>(#REF!&gt;=L$320)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q369 U369">
+  <conditionalFormatting sqref="Q364 U364">
     <cfRule type="expression" dxfId="3" priority="165">
       <formula>(#REF!&gt;=L$320)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R369">
+  <conditionalFormatting sqref="R364">
     <cfRule type="expression" dxfId="2" priority="167">
       <formula>(#REF!&gt;=L$320)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W369">
+  <conditionalFormatting sqref="W364">
     <cfRule type="expression" dxfId="1" priority="168">
       <formula>(#REF!&gt;=P$320)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V369">
+  <conditionalFormatting sqref="V364">
     <cfRule type="expression" dxfId="0" priority="169">
       <formula>(#REF!&gt;=P$320)</formula>
     </cfRule>
@@ -25647,23 +25339,23 @@
       <c r="I18" s="31">
         <v>1</v>
       </c>
-      <c r="J18" s="193" t="s">
+      <c r="J18" s="187" t="s">
         <v>22</v>
       </c>
-      <c r="K18" s="193"/>
-      <c r="L18" s="193"/>
-      <c r="M18" s="193"/>
-      <c r="N18" s="193"/>
-      <c r="O18" s="193"/>
-      <c r="P18" s="193"/>
-      <c r="Q18" s="193"/>
-      <c r="R18" s="193"/>
-      <c r="S18" s="193"/>
-      <c r="T18" s="193"/>
-      <c r="U18" s="193"/>
-      <c r="V18" s="193"/>
-      <c r="W18" s="193"/>
-      <c r="X18" s="193"/>
+      <c r="K18" s="187"/>
+      <c r="L18" s="187"/>
+      <c r="M18" s="187"/>
+      <c r="N18" s="187"/>
+      <c r="O18" s="187"/>
+      <c r="P18" s="187"/>
+      <c r="Q18" s="187"/>
+      <c r="R18" s="187"/>
+      <c r="S18" s="187"/>
+      <c r="T18" s="187"/>
+      <c r="U18" s="187"/>
+      <c r="V18" s="187"/>
+      <c r="W18" s="187"/>
+      <c r="X18" s="187"/>
       <c r="Y18" s="2"/>
       <c r="Z18" s="4"/>
       <c r="AA18" s="16"/>
@@ -25774,7 +25466,7 @@
       <c r="U21" s="177"/>
       <c r="V21" s="177"/>
       <c r="W21" s="177"/>
-      <c r="X21" s="194"/>
+      <c r="X21" s="188"/>
       <c r="Y21" s="2"/>
       <c r="Z21" s="4"/>
       <c r="AA21" s="16"/>

</xml_diff>

<commit_message>
trying to workout problem with season dvp
</commit_message>
<xml_diff>
--- a/Structural.xlsx
+++ b/Structural.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F28DCB02-6784-4FEA-ADE5-E4C2F6D23E9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D6001E-D633-409F-9121-754C71F1DAC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -55,7 +55,7 @@
     <definedName name="i_d_pos">Stock!$I$56</definedName>
     <definedName name="i_date_assetvalue" localSheetId="0">General!$I$67</definedName>
     <definedName name="i_density_n0">Stock!$K$328</definedName>
-    <definedName name="i_density_n1">Stock!$M$328:$M$330</definedName>
+    <definedName name="i_density_n1">Stock!$M$328:$M$329</definedName>
     <definedName name="i_density_n3">Stock!$Q$328:$Q$330</definedName>
     <definedName name="i_dvp_mask_f1">Stock!$J$343:$O$343</definedName>
     <definedName name="i_dvp_mask_f3">Stock!$J$355:$M$355</definedName>
@@ -105,7 +105,7 @@
     <definedName name="i_n3_matrix_len">Stock!$P$326</definedName>
     <definedName name="i_numbers_min_b1">Stock!$L$163:$V$163</definedName>
     <definedName name="i_nut_spread_n0">Stock!$J$328</definedName>
-    <definedName name="i_nut_spread_n1">Stock!$L$328:$L$330</definedName>
+    <definedName name="i_nut_spread_n1">Stock!$L$328:$L$329</definedName>
     <definedName name="i_nut_spread_n3">Stock!$P$328:$P$330</definedName>
     <definedName name="i_p_pos">Stock!$I$64</definedName>
     <definedName name="i_prejoin_offset">Stock!$I$74</definedName>
@@ -7154,7 +7154,7 @@
   </sheetPr>
   <dimension ref="A1:AE379"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A319" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A316" workbookViewId="0">
       <selection activeCell="N342" sqref="N342"/>
     </sheetView>
   </sheetViews>
@@ -22143,7 +22143,7 @@
       <c r="K320" s="2"/>
       <c r="L320" s="132">
         <f>i_w_start_len1*i_n1_len^L323</f>
-        <v>243</v>
+        <v>48</v>
       </c>
       <c r="M320" s="2"/>
       <c r="N320" s="127" t="s">
@@ -22228,7 +22228,7 @@
       </c>
       <c r="K322" s="126"/>
       <c r="L322" s="31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M322" s="126"/>
       <c r="N322" s="2"/>
@@ -22581,10 +22581,10 @@
       </c>
       <c r="J330" s="54"/>
       <c r="K330" s="54"/>
-      <c r="L330" s="31">
+      <c r="L330" s="54">
         <v>-1</v>
       </c>
-      <c r="M330" s="31">
+      <c r="M330" s="54">
         <v>1.5</v>
       </c>
       <c r="N330" s="2"/>
@@ -23039,7 +23039,7 @@
         <v>264</v>
       </c>
       <c r="J341" s="31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K341" s="31" t="b">
         <v>1</v>
@@ -23051,7 +23051,7 @@
         <v>1</v>
       </c>
       <c r="N341" s="31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O341" s="31" t="b">
         <v>0</v>
@@ -23086,20 +23086,16 @@
       </c>
       <c r="I342" s="2"/>
       <c r="J342" s="132">
-        <f>COUNTIF($J$341:J341,TRUE)-1</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K342" s="132">
-        <f>COUNTIF($J$341:K341,TRUE)-1</f>
         <v>0</v>
       </c>
       <c r="L342" s="132">
-        <f>COUNTIF($J$341:L341,TRUE)-1</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M342" s="132">
-        <f>COUNTIF($J$341:M341,TRUE)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N342" s="132">
         <f>COUNTIF($J$341:N341,TRUE)-1</f>
@@ -23141,7 +23137,7 @@
         <v>264</v>
       </c>
       <c r="J343" s="31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K343" s="31" t="b">
         <v>1</v>
@@ -23353,11 +23349,11 @@
       </c>
       <c r="K348" s="31">
         <f t="shared" ref="K348" si="45">L342</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L348" s="31">
         <f>M342</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M348" s="2"/>
       <c r="N348" s="2"/>

</xml_diff>

<commit_message>
Lw distributing updates. Mask dvps before weaning.
</commit_message>
<xml_diff>
--- a/Structural.xlsx
+++ b/Structural.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D6001E-D633-409F-9121-754C71F1DAC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC8D2B4-8F1B-4C40-9B7A-A91DA7F6E9BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -3186,7 +3186,7 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="189">
+  <cellXfs count="190">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="25" xfId="3">
@@ -3659,6 +3659,9 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="23" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="8" borderId="25" xfId="3" applyNumberFormat="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -7154,8 +7157,8 @@
   </sheetPr>
   <dimension ref="A1:AE379"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A316" workbookViewId="0">
-      <selection activeCell="N342" sqref="N342"/>
+    <sheetView tabSelected="1" topLeftCell="A319" workbookViewId="0">
+      <selection activeCell="O344" sqref="O344"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.35"/>
@@ -22143,7 +22146,7 @@
       <c r="K320" s="2"/>
       <c r="L320" s="132">
         <f>i_w_start_len1*i_n1_len^L323</f>
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="M320" s="2"/>
       <c r="N320" s="127" t="s">
@@ -22267,7 +22270,7 @@
       <c r="K323" s="2"/>
       <c r="L323" s="132">
         <f>COUNTIF(J341:O341,TRUE)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M323" s="2"/>
       <c r="N323" s="2"/>
@@ -23039,7 +23042,7 @@
         <v>264</v>
       </c>
       <c r="J341" s="31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K341" s="31" t="b">
         <v>1</v>
@@ -23086,24 +23089,28 @@
       </c>
       <c r="I342" s="2"/>
       <c r="J342" s="132">
-        <v>1</v>
+        <f>COUNTIF($J$341:J341,TRUE)-1</f>
+        <v>-1</v>
       </c>
       <c r="K342" s="132">
+        <f>COUNTIF($J$341:K341,TRUE)-1</f>
         <v>0</v>
       </c>
       <c r="L342" s="132">
+        <f>COUNTIF($J$341:L341,TRUE)-1</f>
+        <v>1</v>
+      </c>
+      <c r="M342" s="132">
+        <f>COUNTIF($J$341:M341,TRUE)-1</f>
         <v>2</v>
-      </c>
-      <c r="M342" s="132">
-        <v>3</v>
       </c>
       <c r="N342" s="132">
         <f>COUNTIF($J$341:N341,TRUE)-1</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O342" s="132">
         <f>COUNTIF($J$341:O341,TRUE)-1</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P342" s="2"/>
       <c r="Q342" s="2"/>
@@ -23137,7 +23144,7 @@
         <v>264</v>
       </c>
       <c r="J343" s="31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K343" s="31" t="b">
         <v>1</v>
@@ -23237,7 +23244,9 @@
       <c r="O345" s="166">
         <v>43784</v>
       </c>
-      <c r="P345" s="2"/>
+      <c r="P345" s="189">
+        <v>43784</v>
+      </c>
       <c r="Q345" s="2"/>
       <c r="R345" s="2"/>
       <c r="S345" s="2"/>
@@ -23274,9 +23283,11 @@
       <c r="M346" s="2"/>
       <c r="N346" s="2"/>
       <c r="O346" s="166">
+        <v>43818</v>
+      </c>
+      <c r="P346" s="189">
         <v>43480</v>
       </c>
-      <c r="P346" s="2"/>
       <c r="Q346" s="2"/>
       <c r="R346" s="2"/>
       <c r="S346" s="2"/>
@@ -23349,11 +23360,11 @@
       </c>
       <c r="K348" s="31">
         <f t="shared" ref="K348" si="45">L342</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L348" s="31">
         <f>M342</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M348" s="2"/>
       <c r="N348" s="2"/>

</xml_diff>

<commit_message>
Tidy up pasture variable names and comments
</commit_message>
<xml_diff>
--- a/Structural.xlsx
+++ b/Structural.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F28DCB02-6784-4FEA-ADE5-E4C2F6D23E9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9009EBE-3316-4969-85AD-3B4E47FE101C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView minimized="1" xWindow="225" yWindow="240" windowWidth="28305" windowHeight="14595" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -92,9 +92,7 @@
     <definedName name="i_mul_g2c0">Stock!$P$111:$R$114</definedName>
     <definedName name="i_mul_g3c0">Stock!$P$116:$R$119</definedName>
     <definedName name="i_n_fvp_period0">Stock!$J$323</definedName>
-    <definedName name="i_n_fvps_vi1">Stock!#REF!</definedName>
     <definedName name="i_n_pos">Stock!$I$63</definedName>
-    <definedName name="i_n_prior_fvps_vi1">Stock!#REF!</definedName>
     <definedName name="i_n_r1type">Stock!$L$213</definedName>
     <definedName name="i_n0_len">Stock!$J$322</definedName>
     <definedName name="i_n0_matrix_len">Stock!$J$326</definedName>
@@ -130,7 +128,6 @@
     <definedName name="ia_ppk2g1_rlsb1">Stock!$L$214:$V$273</definedName>
     <definedName name="ia_ppk5_lsb0">Stock!$L$280:$Q$299</definedName>
     <definedName name="ia_prepost_b1">Stock!$L$159:$V$159</definedName>
-    <definedName name="ia_r1type_fi">Stock!#REF!</definedName>
     <definedName name="ia_sire_dsegroup">Stock!$L$152</definedName>
     <definedName name="ia_yatf_dsegroup_b1">Stock!$L$154:$V$154</definedName>
     <definedName name="labour_period_len" localSheetId="0">General!$I$65</definedName>
@@ -159,7 +156,7 @@
     <definedName name="ZA.WidthCol" localSheetId="2">Admin!$L$26</definedName>
     <definedName name="ZA.ZoomSheet" localSheetId="2">Admin!$O$26</definedName>
   </definedNames>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -589,7 +586,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Michael Young (21512438):</t>
         </r>
@@ -598,7 +595,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 not counted in dse stuff. They are accounted for by dam. If this changes will need to add them to code.</t>
@@ -866,7 +863,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Michael Young (21512438):</t>
         </r>
@@ -875,7 +872,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 This is a user defined date. See just below.</t>
@@ -890,7 +887,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Michael Young (21512438):</t>
         </r>
@@ -899,7 +896,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 fvp type when LW is condensed back to the starting number (eg 3). This fvp must also be a dvp. Typically this is prejoining.</t>
@@ -914,7 +911,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Michael Young (21512438):</t>
         </r>
@@ -923,7 +920,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 is the fvp being included in the model?</t>
@@ -938,7 +935,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Michael Young (21512438):</t>
         </r>
@@ -947,7 +944,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 FVP type is only relevant for the fvps that are included. It must start at 0 and icrement by 1 for each active fvp.</t>
@@ -962,7 +959,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Michael Young (21512438):</t>
         </r>
@@ -971,7 +968,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 is the fvp also a dvp?</t>
@@ -986,7 +983,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Michael Young (21512438):</t>
         </r>
@@ -995,7 +992,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 reproduction dvps. Used in the ppk2g1 cluster input above.</t>
@@ -1034,7 +1031,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Michael Young (21512438):</t>
         </r>
@@ -1043,7 +1040,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 fvp type when LW is condensed back to the starting number (eg 3). This fvp must also be a dvp. Typically this is prejoining.</t>
@@ -1058,7 +1055,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Michael Young (21512438):</t>
         </r>
@@ -1067,7 +1064,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 is the fvp being included in the model?</t>
@@ -1082,7 +1079,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Michael Young (21512438):</t>
         </r>
@@ -1091,7 +1088,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 FVP type is only relevant for the fvps that are included. It must start at 0 and icrement by 1 for each active fvp.</t>
@@ -1106,7 +1103,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Michael Young (21512438):</t>
         </r>
@@ -1115,7 +1112,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 is the fvp also a dvp?</t>
@@ -2035,7 +2032,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2232,19 +2229,6 @@
       <color rgb="FF0000FF"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="35">
@@ -4187,25 +4171,25 @@
       <selection activeCell="L63" sqref="L63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" style="155" customWidth="1"/>
-    <col min="2" max="2" width="2.7265625" style="155" customWidth="1"/>
-    <col min="3" max="3" width="4.7265625" style="155" customWidth="1" outlineLevel="2"/>
-    <col min="4" max="4" width="1.7265625" style="155" customWidth="1"/>
-    <col min="5" max="6" width="9.7265625" style="155" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="1.7265625" style="155" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="37.26953125" style="155" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7265625" style="155" customWidth="1"/>
-    <col min="10" max="23" width="10.81640625" style="155" customWidth="1"/>
-    <col min="24" max="24" width="1.7265625" style="155" customWidth="1"/>
-    <col min="25" max="26" width="4.7265625" style="155" customWidth="1"/>
-    <col min="27" max="27" width="8.7265625" style="155"/>
-    <col min="28" max="28" width="46.1796875" style="155" customWidth="1"/>
-    <col min="29" max="16384" width="8.7265625" style="155"/>
+    <col min="1" max="1" width="4.7109375" style="155" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" style="155" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" style="155" customWidth="1" outlineLevel="2"/>
+    <col min="4" max="4" width="1.7109375" style="155" customWidth="1"/>
+    <col min="5" max="6" width="9.7109375" style="155" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="1.7109375" style="155" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="37.28515625" style="155" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="155" customWidth="1"/>
+    <col min="10" max="23" width="10.85546875" style="155" customWidth="1"/>
+    <col min="24" max="24" width="1.7109375" style="155" customWidth="1"/>
+    <col min="25" max="26" width="4.7109375" style="155" customWidth="1"/>
+    <col min="27" max="27" width="8.7109375" style="155"/>
+    <col min="28" max="28" width="46.140625" style="155" customWidth="1"/>
+    <col min="29" max="16384" width="8.7109375" style="155"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="69"/>
@@ -4235,7 +4219,7 @@
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
     </row>
-    <row r="2" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="70">
@@ -4268,7 +4252,7 @@
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
     </row>
-    <row r="3" spans="1:28" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:28" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="20"/>
       <c r="C3" s="71">
@@ -4301,7 +4285,7 @@
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
     </row>
-    <row r="4" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="34" t="s">
         <v>21</v>
@@ -4336,7 +4320,7 @@
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
     </row>
-    <row r="5" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="33"/>
       <c r="C5" s="70">
@@ -4407,7 +4391,7 @@
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
     </row>
-    <row r="6" spans="1:28" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="33"/>
       <c r="C6" s="70">
@@ -4445,7 +4429,7 @@
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
     </row>
-    <row r="7" spans="1:28" ht="20.149999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="33"/>
       <c r="C7" s="70">
@@ -4484,7 +4468,7 @@
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
     </row>
-    <row r="8" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="33"/>
       <c r="C8" s="70">
@@ -4517,7 +4501,7 @@
       <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
     </row>
-    <row r="9" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="33"/>
       <c r="C9" s="70">
@@ -4550,7 +4534,7 @@
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
     </row>
-    <row r="10" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="33"/>
       <c r="C10" s="70">
@@ -4583,7 +4567,7 @@
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
     </row>
-    <row r="11" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="33"/>
       <c r="C11" s="70">
@@ -4616,7 +4600,7 @@
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
     </row>
-    <row r="12" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="33"/>
       <c r="C12" s="70">
@@ -4653,7 +4637,7 @@
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
     </row>
-    <row r="13" spans="1:28" ht="11.5" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:28" ht="11.45" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="33" t="s">
         <v>20</v>
@@ -4688,7 +4672,7 @@
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
     </row>
-    <row r="14" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="33"/>
       <c r="C14" s="70">
@@ -4721,7 +4705,7 @@
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
     </row>
-    <row r="15" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="33"/>
       <c r="C15" s="70">
@@ -4754,7 +4738,7 @@
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
     </row>
-    <row r="16" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="33" t="s">
         <v>19</v>
@@ -4791,7 +4775,7 @@
       <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>
     </row>
-    <row r="17" spans="1:28" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:28" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="33"/>
       <c r="C17" s="70">
@@ -4826,7 +4810,7 @@
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
     </row>
-    <row r="18" spans="1:28" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:28" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="33"/>
       <c r="C18" s="70">
@@ -4865,7 +4849,7 @@
       <c r="AA18" s="1"/>
       <c r="AB18" s="1"/>
     </row>
-    <row r="19" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="33"/>
       <c r="C19" s="70">
@@ -4898,7 +4882,7 @@
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
     </row>
-    <row r="20" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="33"/>
       <c r="C20" s="70">
@@ -4931,7 +4915,7 @@
       <c r="AA20" s="1"/>
       <c r="AB20" s="1"/>
     </row>
-    <row r="21" spans="1:28" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:28" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="33"/>
       <c r="C21" s="70">
@@ -4970,7 +4954,7 @@
       <c r="AA21" s="1"/>
       <c r="AB21" s="1"/>
     </row>
-    <row r="22" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="33"/>
       <c r="C22" s="70">
@@ -5003,7 +4987,7 @@
       <c r="AA22" s="1"/>
       <c r="AB22" s="1"/>
     </row>
-    <row r="23" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="33"/>
       <c r="C23" s="70">
@@ -5036,7 +5020,7 @@
       <c r="AA23" s="1"/>
       <c r="AB23" s="1"/>
     </row>
-    <row r="24" spans="1:28" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="33"/>
       <c r="C24" s="70">
@@ -5071,7 +5055,7 @@
       <c r="AA24" s="1"/>
       <c r="AB24" s="1"/>
     </row>
-    <row r="25" spans="1:28" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="33"/>
       <c r="C25" s="70">
@@ -5106,7 +5090,7 @@
       <c r="AA25" s="1"/>
       <c r="AB25" s="1"/>
     </row>
-    <row r="26" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="33"/>
       <c r="C26" s="70">
@@ -5153,7 +5137,7 @@
       <c r="AA26" s="1"/>
       <c r="AB26" s="1"/>
     </row>
-    <row r="27" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="33"/>
       <c r="C27" s="70">
@@ -5190,7 +5174,7 @@
       <c r="AA27" s="1"/>
       <c r="AB27" s="1"/>
     </row>
-    <row r="28" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="33"/>
       <c r="C28" s="70">
@@ -5227,7 +5211,7 @@
       <c r="AA28" s="1"/>
       <c r="AB28" s="1"/>
     </row>
-    <row r="29" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="33"/>
       <c r="C29" s="70">
@@ -5264,7 +5248,7 @@
       <c r="AA29" s="1"/>
       <c r="AB29" s="1"/>
     </row>
-    <row r="30" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="33"/>
       <c r="C30" s="70">
@@ -5301,7 +5285,7 @@
       <c r="AA30" s="1"/>
       <c r="AB30" s="1"/>
     </row>
-    <row r="31" spans="1:28" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="33"/>
       <c r="C31" s="70">
@@ -5336,7 +5320,7 @@
       <c r="AA31" s="1"/>
       <c r="AB31" s="1"/>
     </row>
-    <row r="32" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="33"/>
       <c r="C32" s="70">
@@ -5369,7 +5353,7 @@
       <c r="AA32" s="1"/>
       <c r="AB32" s="1"/>
     </row>
-    <row r="33" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="35"/>
       <c r="C33" s="73">
@@ -5404,7 +5388,7 @@
       <c r="AA33" s="1"/>
       <c r="AB33" s="1"/>
     </row>
-    <row r="34" spans="1:28" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:28" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="19"/>
       <c r="C34" s="74">
@@ -5437,7 +5421,7 @@
       <c r="AA34" s="1"/>
       <c r="AB34" s="1"/>
     </row>
-    <row r="35" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="70">
@@ -5470,7 +5454,7 @@
       <c r="AA35" s="1"/>
       <c r="AB35" s="1"/>
     </row>
-    <row r="36" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="76">
@@ -5503,7 +5487,7 @@
       <c r="AA36" s="1"/>
       <c r="AB36" s="1"/>
     </row>
-    <row r="37" spans="1:28" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:28" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="20"/>
       <c r="C37" s="77">
@@ -5536,7 +5520,7 @@
       <c r="AA37" s="1"/>
       <c r="AB37" s="1"/>
     </row>
-    <row r="38" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="34" t="s">
         <v>21</v>
@@ -5571,7 +5555,7 @@
       <c r="AA38" s="1"/>
       <c r="AB38" s="1"/>
     </row>
-    <row r="39" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="33"/>
       <c r="C39" s="76">
@@ -5604,7 +5588,7 @@
       <c r="AA39" s="1"/>
       <c r="AB39" s="1"/>
     </row>
-    <row r="40" spans="1:28" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="33"/>
       <c r="C40" s="76">
@@ -5641,7 +5625,7 @@
       <c r="AA40" s="1"/>
       <c r="AB40" s="1"/>
     </row>
-    <row r="41" spans="1:28" ht="20.149999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:28" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="33"/>
       <c r="C41" s="76">
@@ -5680,7 +5664,7 @@
       <c r="AA41" s="1"/>
       <c r="AB41" s="1"/>
     </row>
-    <row r="42" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="33"/>
       <c r="C42" s="76">
@@ -5713,7 +5697,7 @@
       <c r="AA42" s="1"/>
       <c r="AB42" s="1"/>
     </row>
-    <row r="43" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="33"/>
       <c r="C43" s="76">
@@ -5746,7 +5730,7 @@
       <c r="AA43" s="1"/>
       <c r="AB43" s="1"/>
     </row>
-    <row r="44" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="33"/>
       <c r="C44" s="76">
@@ -5779,7 +5763,7 @@
       <c r="AA44" s="1"/>
       <c r="AB44" s="1"/>
     </row>
-    <row r="45" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="33"/>
       <c r="C45" s="76">
@@ -5812,7 +5796,7 @@
       <c r="AA45" s="1"/>
       <c r="AB45" s="1"/>
     </row>
-    <row r="46" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="33"/>
       <c r="C46" s="76">
@@ -5845,7 +5829,7 @@
       <c r="AA46" s="1"/>
       <c r="AB46" s="1"/>
     </row>
-    <row r="47" spans="1:28" ht="11.5" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:28" ht="11.45" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="33" t="s">
         <v>20</v>
@@ -5880,7 +5864,7 @@
       <c r="AA47" s="1"/>
       <c r="AB47" s="1"/>
     </row>
-    <row r="48" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="33"/>
       <c r="C48" s="76">
@@ -5913,7 +5897,7 @@
       <c r="AA48" s="1"/>
       <c r="AB48" s="1"/>
     </row>
-    <row r="49" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="33" t="s">
         <v>19</v>
@@ -5950,7 +5934,7 @@
       <c r="AA49" s="1"/>
       <c r="AB49" s="1"/>
     </row>
-    <row r="50" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="33"/>
       <c r="C50" s="76">
@@ -5985,7 +5969,7 @@
       <c r="AA50" s="1"/>
       <c r="AB50" s="1"/>
     </row>
-    <row r="51" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="33"/>
       <c r="C51" s="76"/>
@@ -6023,7 +6007,7 @@
       <c r="AA51" s="1"/>
       <c r="AB51" s="1"/>
     </row>
-    <row r="52" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="33"/>
       <c r="C52" s="76"/>
@@ -6053,7 +6037,7 @@
       <c r="AA52" s="1"/>
       <c r="AB52" s="1"/>
     </row>
-    <row r="53" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="33"/>
       <c r="C53" s="76"/>
@@ -6089,7 +6073,7 @@
       <c r="AA53" s="1"/>
       <c r="AB53" s="1"/>
     </row>
-    <row r="54" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="33"/>
       <c r="C54" s="76"/>
@@ -6119,7 +6103,7 @@
       <c r="AA54" s="1"/>
       <c r="AB54" s="1"/>
     </row>
-    <row r="55" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="33"/>
       <c r="C55" s="76"/>
@@ -6157,7 +6141,7 @@
       <c r="AA55" s="1"/>
       <c r="AB55" s="1"/>
     </row>
-    <row r="56" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="33"/>
       <c r="C56" s="76"/>
@@ -6195,7 +6179,7 @@
       <c r="AA56" s="1"/>
       <c r="AB56" s="1"/>
     </row>
-    <row r="57" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="33"/>
       <c r="C57" s="76"/>
@@ -6231,7 +6215,7 @@
       <c r="AA57" s="1"/>
       <c r="AB57" s="1"/>
     </row>
-    <row r="58" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="33"/>
       <c r="C58" s="76"/>
@@ -6271,7 +6255,7 @@
       <c r="AA58" s="1"/>
       <c r="AB58" s="1"/>
     </row>
-    <row r="59" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="33"/>
       <c r="C59" s="76"/>
@@ -6309,7 +6293,7 @@
       <c r="AA59" s="1"/>
       <c r="AB59" s="1"/>
     </row>
-    <row r="60" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="33"/>
       <c r="C60" s="76"/>
@@ -6339,7 +6323,7 @@
       <c r="AA60" s="1"/>
       <c r="AB60" s="1"/>
     </row>
-    <row r="61" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="33"/>
       <c r="C61" s="76"/>
@@ -6379,7 +6363,7 @@
       <c r="AA61" s="1"/>
       <c r="AB61" s="1"/>
     </row>
-    <row r="62" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="33"/>
       <c r="C62" s="76"/>
@@ -6409,7 +6393,7 @@
       <c r="AA62" s="1"/>
       <c r="AB62" s="1"/>
     </row>
-    <row r="63" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="33"/>
       <c r="C63" s="76"/>
@@ -6443,7 +6427,7 @@
       <c r="AA63" s="1"/>
       <c r="AB63" s="1"/>
     </row>
-    <row r="64" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="33"/>
       <c r="C64" s="76"/>
@@ -6473,7 +6457,7 @@
       <c r="AA64" s="1"/>
       <c r="AB64" s="1"/>
     </row>
-    <row r="65" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="33"/>
       <c r="C65" s="76"/>
@@ -6507,7 +6491,7 @@
       <c r="AA65" s="1"/>
       <c r="AB65" s="1"/>
     </row>
-    <row r="66" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="33"/>
       <c r="C66" s="76"/>
@@ -6537,7 +6521,7 @@
       <c r="AA66" s="1"/>
       <c r="AB66" s="1"/>
     </row>
-    <row r="67" spans="1:46" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:46" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="33"/>
       <c r="C67" s="76">
@@ -6593,7 +6577,7 @@
       <c r="AS67" s="1"/>
       <c r="AT67" s="1"/>
     </row>
-    <row r="68" spans="1:46" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:46" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="33"/>
       <c r="C68" s="76"/>
@@ -6654,7 +6638,7 @@
       <c r="AS68" s="1"/>
       <c r="AT68" s="1"/>
     </row>
-    <row r="69" spans="1:46" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:46" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="33"/>
       <c r="C69" s="76"/>
@@ -6701,7 +6685,7 @@
       <c r="AS69" s="1"/>
       <c r="AT69" s="1"/>
     </row>
-    <row r="70" spans="1:46" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:46" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="33"/>
       <c r="C70" s="76"/>
@@ -6748,7 +6732,7 @@
       <c r="AS70" s="1"/>
       <c r="AT70" s="1"/>
     </row>
-    <row r="71" spans="1:46" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:46" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="33"/>
       <c r="C71" s="76">
@@ -6783,7 +6767,7 @@
       <c r="AA71" s="1"/>
       <c r="AB71" s="1"/>
     </row>
-    <row r="72" spans="1:46" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:46" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="33"/>
       <c r="C72" s="76">
@@ -6816,7 +6800,7 @@
       <c r="AA72" s="1"/>
       <c r="AB72" s="1"/>
     </row>
-    <row r="73" spans="1:46" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:46" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="35"/>
       <c r="C73" s="79">
@@ -6851,7 +6835,7 @@
       <c r="AA73" s="1"/>
       <c r="AB73" s="1"/>
     </row>
-    <row r="74" spans="1:46" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:46" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="19"/>
       <c r="C74" s="80">
@@ -6884,7 +6868,7 @@
       <c r="AA74" s="1"/>
       <c r="AB74" s="1"/>
     </row>
-    <row r="75" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="76">
@@ -6917,7 +6901,7 @@
       <c r="AA75" s="1"/>
       <c r="AB75" s="1"/>
     </row>
-    <row r="76" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="76">
@@ -6950,7 +6934,7 @@
       <c r="AA76" s="1"/>
       <c r="AB76" s="1"/>
     </row>
-    <row r="77" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="69"/>
@@ -6980,7 +6964,7 @@
       <c r="AA77" s="1"/>
       <c r="AB77" s="1"/>
     </row>
-    <row r="78" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="69"/>
@@ -7010,7 +6994,7 @@
       <c r="AA78" s="1"/>
       <c r="AB78" s="1"/>
     </row>
-    <row r="79" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="69"/>
@@ -7040,7 +7024,7 @@
       <c r="AA79" s="1"/>
       <c r="AB79" s="1"/>
     </row>
-    <row r="80" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="69"/>
@@ -7070,7 +7054,7 @@
       <c r="AA80" s="1"/>
       <c r="AB80" s="1"/>
     </row>
-    <row r="81" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="69"/>
@@ -7100,7 +7084,7 @@
       <c r="AA81" s="1"/>
       <c r="AB81" s="1"/>
     </row>
-    <row r="82" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="69"/>
@@ -7130,7 +7114,7 @@
       <c r="AA82" s="1"/>
       <c r="AB82" s="1"/>
     </row>
-    <row r="83" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C83" s="75" t="s">
         <v>4</v>
       </c>
@@ -7154,27 +7138,27 @@
   </sheetPr>
   <dimension ref="A1:AE379"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A319" workbookViewId="0">
-      <selection activeCell="N342" sqref="N342"/>
+    <sheetView tabSelected="1" topLeftCell="A311" workbookViewId="0">
+      <selection activeCell="Q341" sqref="Q341"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" customWidth="1"/>
-    <col min="2" max="2" width="2.7265625" customWidth="1"/>
-    <col min="3" max="3" width="4.7265625" customWidth="1" outlineLevel="2"/>
-    <col min="4" max="4" width="1.7265625" customWidth="1"/>
-    <col min="5" max="6" width="9.7265625" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="1.7265625" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="37.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7265625" customWidth="1"/>
-    <col min="10" max="23" width="10.81640625" customWidth="1"/>
-    <col min="24" max="24" width="1.7265625" customWidth="1"/>
-    <col min="25" max="26" width="4.7265625" customWidth="1"/>
-    <col min="28" max="28" width="46.1796875" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="4" max="4" width="1.7109375" customWidth="1"/>
+    <col min="5" max="6" width="9.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="1.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" customWidth="1"/>
+    <col min="10" max="23" width="10.85546875" customWidth="1"/>
+    <col min="24" max="24" width="1.7109375" customWidth="1"/>
+    <col min="25" max="26" width="4.7109375" customWidth="1"/>
+    <col min="28" max="28" width="46.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="69"/>
@@ -7204,7 +7188,7 @@
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
     </row>
-    <row r="2" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="70">
@@ -7237,7 +7221,7 @@
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
     </row>
-    <row r="3" spans="1:28" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:28" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="20"/>
       <c r="C3" s="71">
@@ -7270,7 +7254,7 @@
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
     </row>
-    <row r="4" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="34" t="s">
         <v>21</v>
@@ -7305,7 +7289,7 @@
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
     </row>
-    <row r="5" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="33"/>
       <c r="C5" s="70">
@@ -7376,7 +7360,7 @@
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
     </row>
-    <row r="6" spans="1:28" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="33"/>
       <c r="C6" s="70">
@@ -7414,7 +7398,7 @@
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
     </row>
-    <row r="7" spans="1:28" ht="20.149999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="33"/>
       <c r="C7" s="70">
@@ -7453,7 +7437,7 @@
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
     </row>
-    <row r="8" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="33"/>
       <c r="C8" s="70">
@@ -7486,7 +7470,7 @@
       <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
     </row>
-    <row r="9" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="33"/>
       <c r="C9" s="70">
@@ -7519,7 +7503,7 @@
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
     </row>
-    <row r="10" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="33"/>
       <c r="C10" s="70">
@@ -7552,7 +7536,7 @@
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
     </row>
-    <row r="11" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="33"/>
       <c r="C11" s="70">
@@ -7585,7 +7569,7 @@
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
     </row>
-    <row r="12" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="33"/>
       <c r="C12" s="70">
@@ -7622,7 +7606,7 @@
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
     </row>
-    <row r="13" spans="1:28" ht="11.5" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:28" ht="11.45" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="33" t="s">
         <v>20</v>
@@ -7657,7 +7641,7 @@
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
     </row>
-    <row r="14" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="33"/>
       <c r="C14" s="70">
@@ -7690,7 +7674,7 @@
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
     </row>
-    <row r="15" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="33"/>
       <c r="C15" s="70">
@@ -7723,7 +7707,7 @@
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
     </row>
-    <row r="16" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="33" t="s">
         <v>19</v>
@@ -7760,7 +7744,7 @@
       <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>
     </row>
-    <row r="17" spans="1:28" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:28" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="33"/>
       <c r="C17" s="70">
@@ -7795,7 +7779,7 @@
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
     </row>
-    <row r="18" spans="1:28" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:28" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="33"/>
       <c r="C18" s="70">
@@ -7834,7 +7818,7 @@
       <c r="AA18" s="1"/>
       <c r="AB18" s="1"/>
     </row>
-    <row r="19" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="33"/>
       <c r="C19" s="70">
@@ -7867,7 +7851,7 @@
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
     </row>
-    <row r="20" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="33"/>
       <c r="C20" s="70">
@@ -7900,7 +7884,7 @@
       <c r="AA20" s="1"/>
       <c r="AB20" s="1"/>
     </row>
-    <row r="21" spans="1:28" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:28" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="33"/>
       <c r="C21" s="70">
@@ -7939,7 +7923,7 @@
       <c r="AA21" s="1"/>
       <c r="AB21" s="1"/>
     </row>
-    <row r="22" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="33"/>
       <c r="C22" s="70">
@@ -7972,7 +7956,7 @@
       <c r="AA22" s="1"/>
       <c r="AB22" s="1"/>
     </row>
-    <row r="23" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="33"/>
       <c r="C23" s="70">
@@ -8005,7 +7989,7 @@
       <c r="AA23" s="1"/>
       <c r="AB23" s="1"/>
     </row>
-    <row r="24" spans="1:28" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="33"/>
       <c r="C24" s="70">
@@ -8040,7 +8024,7 @@
       <c r="AA24" s="1"/>
       <c r="AB24" s="1"/>
     </row>
-    <row r="25" spans="1:28" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="33"/>
       <c r="C25" s="70">
@@ -8075,7 +8059,7 @@
       <c r="AA25" s="1"/>
       <c r="AB25" s="1"/>
     </row>
-    <row r="26" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="33"/>
       <c r="C26" s="70">
@@ -8122,7 +8106,7 @@
       <c r="AA26" s="1"/>
       <c r="AB26" s="1"/>
     </row>
-    <row r="27" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="33"/>
       <c r="C27" s="70">
@@ -8159,7 +8143,7 @@
       <c r="AA27" s="1"/>
       <c r="AB27" s="1"/>
     </row>
-    <row r="28" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="33"/>
       <c r="C28" s="70">
@@ -8196,7 +8180,7 @@
       <c r="AA28" s="1"/>
       <c r="AB28" s="1"/>
     </row>
-    <row r="29" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="33"/>
       <c r="C29" s="70">
@@ -8233,7 +8217,7 @@
       <c r="AA29" s="1"/>
       <c r="AB29" s="1"/>
     </row>
-    <row r="30" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="33"/>
       <c r="C30" s="70">
@@ -8270,7 +8254,7 @@
       <c r="AA30" s="1"/>
       <c r="AB30" s="1"/>
     </row>
-    <row r="31" spans="1:28" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="33"/>
       <c r="C31" s="70">
@@ -8305,7 +8289,7 @@
       <c r="AA31" s="1"/>
       <c r="AB31" s="1"/>
     </row>
-    <row r="32" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="33"/>
       <c r="C32" s="70">
@@ -8338,7 +8322,7 @@
       <c r="AA32" s="1"/>
       <c r="AB32" s="1"/>
     </row>
-    <row r="33" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="35"/>
       <c r="C33" s="73">
@@ -8373,7 +8357,7 @@
       <c r="AA33" s="1"/>
       <c r="AB33" s="1"/>
     </row>
-    <row r="34" spans="1:28" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:28" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="19"/>
       <c r="C34" s="74">
@@ -8406,7 +8390,7 @@
       <c r="AA34" s="1"/>
       <c r="AB34" s="1"/>
     </row>
-    <row r="35" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="70">
@@ -8439,7 +8423,7 @@
       <c r="AA35" s="1"/>
       <c r="AB35" s="1"/>
     </row>
-    <row r="36" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="76">
@@ -8472,7 +8456,7 @@
       <c r="AA36" s="1"/>
       <c r="AB36" s="1"/>
     </row>
-    <row r="37" spans="1:28" s="142" customFormat="1" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:28" s="142" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="20"/>
       <c r="C37" s="77">
@@ -8505,7 +8489,7 @@
       <c r="AA37" s="1"/>
       <c r="AB37" s="1"/>
     </row>
-    <row r="38" spans="1:28" s="142" customFormat="1" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:28" s="142" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="34" t="s">
         <v>21</v>
@@ -8540,7 +8524,7 @@
       <c r="AA38" s="1"/>
       <c r="AB38" s="1"/>
     </row>
-    <row r="39" spans="1:28" s="142" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:28" s="142" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="33"/>
       <c r="C39" s="76">
@@ -8573,7 +8557,7 @@
       <c r="AA39" s="1"/>
       <c r="AB39" s="1"/>
     </row>
-    <row r="40" spans="1:28" s="142" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:28" s="142" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="33"/>
       <c r="C40" s="76">
@@ -8610,7 +8594,7 @@
       <c r="AA40" s="1"/>
       <c r="AB40" s="1"/>
     </row>
-    <row r="41" spans="1:28" s="142" customFormat="1" ht="20.149999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:28" s="142" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="33"/>
       <c r="C41" s="76">
@@ -8649,7 +8633,7 @@
       <c r="AA41" s="1"/>
       <c r="AB41" s="1"/>
     </row>
-    <row r="42" spans="1:28" s="142" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:28" s="142" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="33"/>
       <c r="C42" s="76">
@@ -8682,7 +8666,7 @@
       <c r="AA42" s="1"/>
       <c r="AB42" s="1"/>
     </row>
-    <row r="43" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="33"/>
       <c r="C43" s="76">
@@ -8715,7 +8699,7 @@
       <c r="AA43" s="1"/>
       <c r="AB43" s="1"/>
     </row>
-    <row r="44" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="33"/>
       <c r="C44" s="76">
@@ -8748,7 +8732,7 @@
       <c r="AA44" s="1"/>
       <c r="AB44" s="1"/>
     </row>
-    <row r="45" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="33"/>
       <c r="C45" s="76">
@@ -8781,7 +8765,7 @@
       <c r="AA45" s="1"/>
       <c r="AB45" s="1"/>
     </row>
-    <row r="46" spans="1:28" s="142" customFormat="1" ht="28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:28" s="142" customFormat="1" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="33"/>
       <c r="C46" s="76">
@@ -8824,7 +8808,7 @@
       <c r="AA46" s="1"/>
       <c r="AB46" s="1"/>
     </row>
-    <row r="47" spans="1:28" s="142" customFormat="1" ht="11.5" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:28" s="142" customFormat="1" ht="11.45" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="33" t="s">
         <v>20</v>
@@ -8859,7 +8843,7 @@
       <c r="AA47" s="1"/>
       <c r="AB47" s="1"/>
     </row>
-    <row r="48" spans="1:28" s="142" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:28" s="142" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="33"/>
       <c r="C48" s="76">
@@ -8892,7 +8876,7 @@
       <c r="AA48" s="1"/>
       <c r="AB48" s="1"/>
     </row>
-    <row r="49" spans="1:28" s="142" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:28" s="142" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="33" t="s">
         <v>19</v>
@@ -8929,7 +8913,7 @@
       <c r="AA49" s="1"/>
       <c r="AB49" s="1"/>
     </row>
-    <row r="50" spans="1:28" s="142" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:28" s="142" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="33"/>
       <c r="C50" s="76">
@@ -8964,7 +8948,7 @@
       <c r="AA50" s="1"/>
       <c r="AB50" s="1"/>
     </row>
-    <row r="51" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="33"/>
       <c r="C51" s="76">
@@ -8999,7 +8983,7 @@
       <c r="AA51" s="1"/>
       <c r="AB51" s="1"/>
     </row>
-    <row r="52" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="33"/>
       <c r="C52" s="76"/>
@@ -9033,7 +9017,7 @@
       <c r="AA52" s="1"/>
       <c r="AB52" s="1"/>
     </row>
-    <row r="53" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="33"/>
       <c r="C53" s="76"/>
@@ -9067,7 +9051,7 @@
       <c r="AA53" s="1"/>
       <c r="AB53" s="1"/>
     </row>
-    <row r="54" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="33"/>
       <c r="C54" s="76"/>
@@ -9101,7 +9085,7 @@
       <c r="AA54" s="1"/>
       <c r="AB54" s="1"/>
     </row>
-    <row r="55" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="33"/>
       <c r="C55" s="76"/>
@@ -9135,7 +9119,7 @@
       <c r="AA55" s="1"/>
       <c r="AB55" s="1"/>
     </row>
-    <row r="56" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="33"/>
       <c r="C56" s="76"/>
@@ -9169,7 +9153,7 @@
       <c r="AA56" s="1"/>
       <c r="AB56" s="1"/>
     </row>
-    <row r="57" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="33"/>
       <c r="C57" s="76"/>
@@ -9203,7 +9187,7 @@
       <c r="AA57" s="1"/>
       <c r="AB57" s="1"/>
     </row>
-    <row r="58" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="33"/>
       <c r="C58" s="76"/>
@@ -9237,7 +9221,7 @@
       <c r="AA58" s="1"/>
       <c r="AB58" s="1"/>
     </row>
-    <row r="59" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="33"/>
       <c r="C59" s="76"/>
@@ -9271,7 +9255,7 @@
       <c r="AA59" s="1"/>
       <c r="AB59" s="1"/>
     </row>
-    <row r="60" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="33"/>
       <c r="C60" s="76"/>
@@ -9305,7 +9289,7 @@
       <c r="AA60" s="1"/>
       <c r="AB60" s="1"/>
     </row>
-    <row r="61" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="33"/>
       <c r="C61" s="76"/>
@@ -9339,7 +9323,7 @@
       <c r="AA61" s="1"/>
       <c r="AB61" s="1"/>
     </row>
-    <row r="62" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="33"/>
       <c r="C62" s="76"/>
@@ -9373,7 +9357,7 @@
       <c r="AA62" s="1"/>
       <c r="AB62" s="1"/>
     </row>
-    <row r="63" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="33"/>
       <c r="C63" s="76"/>
@@ -9407,7 +9391,7 @@
       <c r="AA63" s="1"/>
       <c r="AB63" s="1"/>
     </row>
-    <row r="64" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="33"/>
       <c r="C64" s="76"/>
@@ -9441,7 +9425,7 @@
       <c r="AA64" s="1"/>
       <c r="AB64" s="1"/>
     </row>
-    <row r="65" spans="1:28" s="113" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:28" s="113" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="33"/>
       <c r="C65" s="76">
@@ -9480,7 +9464,7 @@
       <c r="AA65" s="1"/>
       <c r="AB65" s="1"/>
     </row>
-    <row r="66" spans="1:28" s="105" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:28" s="105" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="33"/>
       <c r="C66" s="76">
@@ -9517,7 +9501,7 @@
       <c r="AA66" s="1"/>
       <c r="AB66" s="1"/>
     </row>
-    <row r="67" spans="1:28" s="105" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:28" s="105" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="33"/>
       <c r="C67" s="76">
@@ -9554,7 +9538,7 @@
       <c r="AA67" s="1"/>
       <c r="AB67" s="1"/>
     </row>
-    <row r="68" spans="1:28" s="129" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:28" s="129" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="33"/>
       <c r="C68" s="76">
@@ -9591,7 +9575,7 @@
       <c r="AA68" s="1"/>
       <c r="AB68" s="1"/>
     </row>
-    <row r="69" spans="1:28" s="145" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:28" s="145" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="33"/>
       <c r="C69" s="76">
@@ -9624,7 +9608,7 @@
       <c r="AA69" s="1"/>
       <c r="AB69" s="1"/>
     </row>
-    <row r="70" spans="1:28" s="109" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:28" s="109" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="33"/>
       <c r="C70" s="76">
@@ -9661,7 +9645,7 @@
       <c r="AA70" s="1"/>
       <c r="AB70" s="1"/>
     </row>
-    <row r="71" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="33"/>
       <c r="C71" s="76">
@@ -9702,7 +9686,7 @@
       <c r="AA71" s="1"/>
       <c r="AB71" s="1"/>
     </row>
-    <row r="72" spans="1:28" s="154" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:28" s="154" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="33"/>
       <c r="C72" s="76">
@@ -9741,7 +9725,7 @@
       <c r="AA72" s="1"/>
       <c r="AB72" s="1"/>
     </row>
-    <row r="73" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="33"/>
       <c r="C73" s="76"/>
@@ -9771,7 +9755,7 @@
       <c r="AA73" s="1"/>
       <c r="AB73" s="1"/>
     </row>
-    <row r="74" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="33"/>
       <c r="C74" s="76"/>
@@ -9807,7 +9791,7 @@
       <c r="AA74" s="1"/>
       <c r="AB74" s="1"/>
     </row>
-    <row r="75" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="33"/>
       <c r="C75" s="76"/>
@@ -9837,7 +9821,7 @@
       <c r="AA75" s="1"/>
       <c r="AB75" s="1"/>
     </row>
-    <row r="76" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="33"/>
       <c r="C76" s="76">
@@ -9872,7 +9856,7 @@
       <c r="AA76" s="1"/>
       <c r="AB76" s="1"/>
     </row>
-    <row r="77" spans="1:28" s="101" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:28" s="101" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="33"/>
       <c r="C77" s="76">
@@ -9913,7 +9897,7 @@
       <c r="AA77" s="1"/>
       <c r="AB77" s="1"/>
     </row>
-    <row r="78" spans="1:28" s="101" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:28" s="101" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="33"/>
       <c r="C78" s="76">
@@ -9954,7 +9938,7 @@
       <c r="AA78" s="1"/>
       <c r="AB78" s="1"/>
     </row>
-    <row r="79" spans="1:28" s="101" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:28" s="101" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="33"/>
       <c r="C79" s="76">
@@ -9987,7 +9971,7 @@
       <c r="AA79" s="1"/>
       <c r="AB79" s="1"/>
     </row>
-    <row r="80" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="33"/>
       <c r="C80" s="76">
@@ -10024,7 +10008,7 @@
       <c r="AA80" s="1"/>
       <c r="AB80" s="1"/>
     </row>
-    <row r="81" spans="1:28" s="152" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:28" s="152" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="33"/>
       <c r="C81" s="76">
@@ -10057,7 +10041,7 @@
       <c r="AA81" s="1"/>
       <c r="AB81" s="1"/>
     </row>
-    <row r="82" spans="1:28" s="101" customFormat="1" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:28" s="101" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="33"/>
       <c r="C82" s="76">
@@ -10092,7 +10076,7 @@
       <c r="AA82" s="1"/>
       <c r="AB82" s="1"/>
     </row>
-    <row r="83" spans="1:28" s="101" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:28" s="101" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="33"/>
       <c r="C83" s="76">
@@ -10125,7 +10109,7 @@
       <c r="AA83" s="1"/>
       <c r="AB83" s="1"/>
     </row>
-    <row r="84" spans="1:28" s="101" customFormat="1" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:28" s="101" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="35"/>
       <c r="C84" s="79">
@@ -10160,7 +10144,7 @@
       <c r="AA84" s="1"/>
       <c r="AB84" s="1"/>
     </row>
-    <row r="85" spans="1:28" s="101" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:28" s="101" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="19"/>
       <c r="C85" s="80">
@@ -10193,7 +10177,7 @@
       <c r="AA85" s="1"/>
       <c r="AB85" s="1"/>
     </row>
-    <row r="86" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="76">
@@ -10226,7 +10210,7 @@
       <c r="AA86" s="1"/>
       <c r="AB86" s="1"/>
     </row>
-    <row r="87" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="76">
@@ -10259,7 +10243,7 @@
       <c r="AA87" s="1"/>
       <c r="AB87" s="1"/>
     </row>
-    <row r="88" spans="1:28" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:28" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="1"/>
       <c r="B88" s="20"/>
       <c r="C88" s="77">
@@ -10292,7 +10276,7 @@
       <c r="AA88" s="1"/>
       <c r="AB88" s="1"/>
     </row>
-    <row r="89" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="34" t="s">
         <v>21</v>
@@ -10327,7 +10311,7 @@
       <c r="AA89" s="1"/>
       <c r="AB89" s="1"/>
     </row>
-    <row r="90" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="33"/>
       <c r="C90" s="76">
@@ -10360,7 +10344,7 @@
       <c r="AA90" s="1"/>
       <c r="AB90" s="1"/>
     </row>
-    <row r="91" spans="1:28" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="33"/>
       <c r="C91" s="76">
@@ -10397,7 +10381,7 @@
       <c r="AA91" s="1"/>
       <c r="AB91" s="1"/>
     </row>
-    <row r="92" spans="1:28" ht="20.149999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:28" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="33"/>
       <c r="C92" s="76">
@@ -10436,7 +10420,7 @@
       <c r="AA92" s="1"/>
       <c r="AB92" s="1"/>
     </row>
-    <row r="93" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="33"/>
       <c r="C93" s="76">
@@ -10469,7 +10453,7 @@
       <c r="AA93" s="1"/>
       <c r="AB93" s="1"/>
     </row>
-    <row r="94" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="33"/>
       <c r="C94" s="76">
@@ -10502,7 +10486,7 @@
       <c r="AA94" s="1"/>
       <c r="AB94" s="1"/>
     </row>
-    <row r="95" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="33"/>
       <c r="C95" s="76">
@@ -10535,7 +10519,7 @@
       <c r="AA95" s="1"/>
       <c r="AB95" s="1"/>
     </row>
-    <row r="96" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="33"/>
       <c r="C96" s="76">
@@ -10574,7 +10558,7 @@
       <c r="AA96" s="1"/>
       <c r="AB96" s="1"/>
     </row>
-    <row r="97" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="33"/>
       <c r="C97" s="76">
@@ -10623,7 +10607,7 @@
       <c r="AA97" s="1"/>
       <c r="AB97" s="1"/>
     </row>
-    <row r="98" spans="1:28" ht="11.5" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:28" ht="11.45" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="33" t="s">
         <v>20</v>
@@ -10658,7 +10642,7 @@
       <c r="AA98" s="1"/>
       <c r="AB98" s="1"/>
     </row>
-    <row r="99" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="33"/>
       <c r="C99" s="76">
@@ -10691,7 +10675,7 @@
       <c r="AA99" s="1"/>
       <c r="AB99" s="1"/>
     </row>
-    <row r="100" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="33" t="s">
         <v>19</v>
@@ -10728,7 +10712,7 @@
       <c r="AA100" s="1"/>
       <c r="AB100" s="1"/>
     </row>
-    <row r="101" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="33"/>
       <c r="C101" s="76">
@@ -10763,7 +10747,7 @@
       <c r="AA101" s="1"/>
       <c r="AB101" s="1"/>
     </row>
-    <row r="102" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="33"/>
       <c r="C102" s="76">
@@ -10816,7 +10800,7 @@
       <c r="AA102" s="1"/>
       <c r="AB102" s="1"/>
     </row>
-    <row r="103" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="33"/>
       <c r="C103" s="76">
@@ -10867,7 +10851,7 @@
       <c r="AA103" s="1"/>
       <c r="AB103" s="1"/>
     </row>
-    <row r="104" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="33"/>
       <c r="C104" s="76">
@@ -10918,7 +10902,7 @@
       <c r="AA104" s="1"/>
       <c r="AB104" s="1"/>
     </row>
-    <row r="105" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="33"/>
       <c r="C105" s="76">
@@ -10951,7 +10935,7 @@
       <c r="AA105" s="1"/>
       <c r="AB105" s="1"/>
     </row>
-    <row r="106" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="33"/>
       <c r="C106" s="76">
@@ -11002,7 +10986,7 @@
       <c r="AA106" s="1"/>
       <c r="AB106" s="1"/>
     </row>
-    <row r="107" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="33"/>
       <c r="C107" s="76">
@@ -11051,7 +11035,7 @@
       <c r="AA107" s="1"/>
       <c r="AB107" s="1"/>
     </row>
-    <row r="108" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="33"/>
       <c r="C108" s="76">
@@ -11100,7 +11084,7 @@
       <c r="AA108" s="1"/>
       <c r="AB108" s="1"/>
     </row>
-    <row r="109" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="33"/>
       <c r="C109" s="76">
@@ -11149,7 +11133,7 @@
       <c r="AA109" s="1"/>
       <c r="AB109" s="1"/>
     </row>
-    <row r="110" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="33"/>
       <c r="C110" s="76">
@@ -11182,7 +11166,7 @@
       <c r="AA110" s="1"/>
       <c r="AB110" s="1"/>
     </row>
-    <row r="111" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111" s="33"/>
       <c r="C111" s="76">
@@ -11233,7 +11217,7 @@
       <c r="AA111" s="1"/>
       <c r="AB111" s="1"/>
     </row>
-    <row r="112" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="33"/>
       <c r="C112" s="76">
@@ -11282,7 +11266,7 @@
       <c r="AA112" s="1"/>
       <c r="AB112" s="1"/>
     </row>
-    <row r="113" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="33"/>
       <c r="C113" s="76">
@@ -11331,7 +11315,7 @@
       <c r="AA113" s="1"/>
       <c r="AB113" s="1"/>
     </row>
-    <row r="114" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="33"/>
       <c r="C114" s="76">
@@ -11380,7 +11364,7 @@
       <c r="AA114" s="1"/>
       <c r="AB114" s="1"/>
     </row>
-    <row r="115" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="33"/>
       <c r="C115" s="76">
@@ -11413,7 +11397,7 @@
       <c r="AA115" s="1"/>
       <c r="AB115" s="1"/>
     </row>
-    <row r="116" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="33"/>
       <c r="C116" s="76">
@@ -11464,7 +11448,7 @@
       <c r="AA116" s="1"/>
       <c r="AB116" s="1"/>
     </row>
-    <row r="117" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="33"/>
       <c r="C117" s="76">
@@ -11513,7 +11497,7 @@
       <c r="AA117" s="1"/>
       <c r="AB117" s="1"/>
     </row>
-    <row r="118" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="33"/>
       <c r="C118" s="76">
@@ -11562,7 +11546,7 @@
       <c r="AA118" s="1"/>
       <c r="AB118" s="1"/>
     </row>
-    <row r="119" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="33"/>
       <c r="C119" s="76">
@@ -11611,7 +11595,7 @@
       <c r="AA119" s="1"/>
       <c r="AB119" s="1"/>
     </row>
-    <row r="120" spans="1:28" s="151" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:28" s="151" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="33"/>
       <c r="C120" s="76">
@@ -11644,7 +11628,7 @@
       <c r="AA120" s="1"/>
       <c r="AB120" s="1"/>
     </row>
-    <row r="121" spans="1:28" s="151" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:28" s="151" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="33"/>
       <c r="C121" s="76">
@@ -11679,7 +11663,7 @@
       <c r="AA121" s="1"/>
       <c r="AB121" s="1"/>
     </row>
-    <row r="122" spans="1:28" s="151" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:28" s="151" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="33"/>
       <c r="C122" s="76">
@@ -11720,7 +11704,7 @@
       <c r="AA122" s="1"/>
       <c r="AB122" s="1"/>
     </row>
-    <row r="123" spans="1:28" s="151" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:28" s="151" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
       <c r="B123" s="33"/>
       <c r="C123" s="76">
@@ -11768,7 +11752,7 @@
       <c r="AA123" s="1"/>
       <c r="AB123" s="1"/>
     </row>
-    <row r="124" spans="1:28" s="151" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:28" s="151" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
       <c r="B124" s="33"/>
       <c r="C124" s="76">
@@ -11814,7 +11798,7 @@
       <c r="AA124" s="1"/>
       <c r="AB124" s="1"/>
     </row>
-    <row r="125" spans="1:28" s="151" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:28" s="151" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="B125" s="33"/>
       <c r="C125" s="76">
@@ -11857,7 +11841,7 @@
       <c r="AA125" s="1"/>
       <c r="AB125" s="1"/>
     </row>
-    <row r="126" spans="1:28" s="151" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:28" s="151" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
       <c r="B126" s="33"/>
       <c r="C126" s="76">
@@ -11890,7 +11874,7 @@
       <c r="AA126" s="1"/>
       <c r="AB126" s="1"/>
     </row>
-    <row r="127" spans="1:28" s="151" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:28" s="151" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="B127" s="33"/>
       <c r="C127" s="76">
@@ -11937,7 +11921,7 @@
       <c r="AA127" s="1"/>
       <c r="AB127" s="1"/>
     </row>
-    <row r="128" spans="1:28" s="151" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:28" s="151" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
       <c r="B128" s="33"/>
       <c r="C128" s="76">
@@ -11982,7 +11966,7 @@
       <c r="AA128" s="1"/>
       <c r="AB128" s="1"/>
     </row>
-    <row r="129" spans="1:28" s="151" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:28" s="151" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
       <c r="B129" s="33"/>
       <c r="C129" s="76">
@@ -12025,7 +12009,7 @@
       <c r="AA129" s="1"/>
       <c r="AB129" s="1"/>
     </row>
-    <row r="130" spans="1:28" s="151" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:28" s="151" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="B130" s="33"/>
       <c r="C130" s="76">
@@ -12058,7 +12042,7 @@
       <c r="AA130" s="1"/>
       <c r="AB130" s="1"/>
     </row>
-    <row r="131" spans="1:28" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131" s="33"/>
       <c r="C131" s="76">
@@ -12093,7 +12077,7 @@
       <c r="AA131" s="1"/>
       <c r="AB131" s="1"/>
     </row>
-    <row r="132" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="33"/>
       <c r="C132" s="76">
@@ -12126,7 +12110,7 @@
       <c r="AA132" s="1"/>
       <c r="AB132" s="1"/>
     </row>
-    <row r="133" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" s="35"/>
       <c r="C133" s="79">
@@ -12161,7 +12145,7 @@
       <c r="AA133" s="1"/>
       <c r="AB133" s="1"/>
     </row>
-    <row r="134" spans="1:28" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:28" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134" s="19"/>
       <c r="C134" s="80">
@@ -12194,7 +12178,7 @@
       <c r="AA134" s="1"/>
       <c r="AB134" s="1"/>
     </row>
-    <row r="135" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="76">
@@ -12227,7 +12211,7 @@
       <c r="AA135" s="1"/>
       <c r="AB135" s="1"/>
     </row>
-    <row r="136" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="76">
@@ -12260,7 +12244,7 @@
       <c r="AA136" s="1"/>
       <c r="AB136" s="1"/>
     </row>
-    <row r="137" spans="1:28" s="99" customFormat="1" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:28" s="99" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="1"/>
       <c r="B137" s="20"/>
       <c r="C137" s="77">
@@ -12293,7 +12277,7 @@
       <c r="AA137" s="1"/>
       <c r="AB137" s="1"/>
     </row>
-    <row r="138" spans="1:28" s="99" customFormat="1" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:28" s="99" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
       <c r="B138" s="34" t="s">
         <v>21</v>
@@ -12328,7 +12312,7 @@
       <c r="AA138" s="1"/>
       <c r="AB138" s="1"/>
     </row>
-    <row r="139" spans="1:28" s="99" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:28" s="99" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
       <c r="B139" s="33"/>
       <c r="C139" s="76">
@@ -12361,7 +12345,7 @@
       <c r="AA139" s="1"/>
       <c r="AB139" s="1"/>
     </row>
-    <row r="140" spans="1:28" s="99" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:28" s="99" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
       <c r="B140" s="33"/>
       <c r="C140" s="76">
@@ -12398,7 +12382,7 @@
       <c r="AA140" s="1"/>
       <c r="AB140" s="1"/>
     </row>
-    <row r="141" spans="1:28" s="99" customFormat="1" ht="20.149999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:28" s="99" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
       <c r="B141" s="33"/>
       <c r="C141" s="76">
@@ -12437,7 +12421,7 @@
       <c r="AA141" s="1"/>
       <c r="AB141" s="1"/>
     </row>
-    <row r="142" spans="1:28" s="99" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:28" s="99" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
       <c r="B142" s="33"/>
       <c r="C142" s="76">
@@ -12470,7 +12454,7 @@
       <c r="AA142" s="1"/>
       <c r="AB142" s="1"/>
     </row>
-    <row r="143" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
       <c r="B143" s="33"/>
       <c r="C143" s="76">
@@ -12503,7 +12487,7 @@
       <c r="AA143" s="1"/>
       <c r="AB143" s="1"/>
     </row>
-    <row r="144" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
       <c r="B144" s="33"/>
       <c r="C144" s="76">
@@ -12538,7 +12522,7 @@
       <c r="AA144" s="1"/>
       <c r="AB144" s="1"/>
     </row>
-    <row r="145" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
       <c r="B145" s="33"/>
       <c r="C145" s="76">
@@ -12573,7 +12557,7 @@
       <c r="AA145" s="1"/>
       <c r="AB145" s="1"/>
     </row>
-    <row r="146" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
       <c r="B146" s="33"/>
       <c r="C146" s="76">
@@ -12628,7 +12612,7 @@
       <c r="AA146" s="1"/>
       <c r="AB146" s="1"/>
     </row>
-    <row r="147" spans="1:28" s="99" customFormat="1" ht="11.5" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:28" s="99" customFormat="1" ht="11.45" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
       <c r="B147" s="33" t="s">
         <v>20</v>
@@ -12663,7 +12647,7 @@
       <c r="AA147" s="1"/>
       <c r="AB147" s="1"/>
     </row>
-    <row r="148" spans="1:28" s="99" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:28" s="99" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
       <c r="B148" s="33"/>
       <c r="C148" s="76">
@@ -12718,7 +12702,7 @@
       <c r="AA148" s="1"/>
       <c r="AB148" s="1"/>
     </row>
-    <row r="149" spans="1:28" s="99" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:28" s="99" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
       <c r="B149" s="33" t="s">
         <v>19</v>
@@ -12755,7 +12739,7 @@
       <c r="AA149" s="1"/>
       <c r="AB149" s="1"/>
     </row>
-    <row r="150" spans="1:28" s="99" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:28" s="99" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
       <c r="B150" s="33"/>
       <c r="C150" s="76">
@@ -12790,7 +12774,7 @@
       <c r="AA150" s="1"/>
       <c r="AB150" s="1"/>
     </row>
-    <row r="151" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
       <c r="B151" s="33"/>
       <c r="C151" s="76">
@@ -12825,7 +12809,7 @@
       <c r="AA151" s="1"/>
       <c r="AB151" s="1"/>
     </row>
-    <row r="152" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
       <c r="B152" s="33"/>
       <c r="C152" s="76">
@@ -12864,7 +12848,7 @@
       <c r="AA152" s="1"/>
       <c r="AB152" s="1"/>
     </row>
-    <row r="153" spans="1:28" s="99" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:28" s="99" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A153" s="1"/>
       <c r="B153" s="33"/>
       <c r="C153" s="76">
@@ -12923,7 +12907,7 @@
       <c r="AA153" s="1"/>
       <c r="AB153" s="1"/>
     </row>
-    <row r="154" spans="1:28" s="99" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:28" s="99" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A154" s="1"/>
       <c r="B154" s="33"/>
       <c r="C154" s="76">
@@ -12980,7 +12964,7 @@
       <c r="AA154" s="1"/>
       <c r="AB154" s="1"/>
     </row>
-    <row r="155" spans="1:28" s="99" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:28" s="99" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
       <c r="B155" s="33"/>
       <c r="C155" s="76">
@@ -13017,7 +13001,7 @@
       <c r="AA155" s="1"/>
       <c r="AB155" s="1"/>
     </row>
-    <row r="156" spans="1:28" s="99" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:28" s="99" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A156" s="1"/>
       <c r="B156" s="33"/>
       <c r="C156" s="76">
@@ -13074,7 +13058,7 @@
       <c r="AA156" s="1"/>
       <c r="AB156" s="1"/>
     </row>
-    <row r="157" spans="1:28" s="150" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:28" s="150" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
       <c r="B157" s="33"/>
       <c r="C157" s="76">
@@ -13133,7 +13117,7 @@
       <c r="AA157" s="1"/>
       <c r="AB157" s="1"/>
     </row>
-    <row r="158" spans="1:28" s="124" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:28" s="124" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
       <c r="B158" s="33"/>
       <c r="C158" s="76">
@@ -13190,7 +13174,7 @@
       <c r="AA158" s="1"/>
       <c r="AB158" s="1"/>
     </row>
-    <row r="159" spans="1:28" s="124" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:28" s="124" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A159" s="1"/>
       <c r="B159" s="33"/>
       <c r="C159" s="76">
@@ -13247,7 +13231,7 @@
       <c r="AA159" s="1"/>
       <c r="AB159" s="1"/>
     </row>
-    <row r="160" spans="1:28" s="99" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:28" s="99" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
       <c r="B160" s="33"/>
       <c r="C160" s="76">
@@ -13304,7 +13288,7 @@
       <c r="AA160" s="1"/>
       <c r="AB160" s="1"/>
     </row>
-    <row r="161" spans="1:31" s="99" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:31" s="99" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A161" s="1"/>
       <c r="B161" s="33"/>
       <c r="C161" s="76">
@@ -13361,7 +13345,7 @@
       <c r="AA161" s="1"/>
       <c r="AB161" s="1"/>
     </row>
-    <row r="162" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A162" s="1"/>
       <c r="B162" s="33"/>
       <c r="C162" s="76">
@@ -13421,7 +13405,7 @@
       <c r="AD162" s="130"/>
       <c r="AE162" s="130"/>
     </row>
-    <row r="163" spans="1:31" s="146" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:31" s="146" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A163" s="1"/>
       <c r="B163" s="33"/>
       <c r="C163" s="76">
@@ -13478,7 +13462,7 @@
       <c r="AA163" s="1"/>
       <c r="AB163" s="1"/>
     </row>
-    <row r="164" spans="1:31" s="113" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:31" s="113" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A164" s="1"/>
       <c r="B164" s="33"/>
       <c r="C164" s="76">
@@ -13514,7 +13498,7 @@
       <c r="AD164" s="130"/>
       <c r="AE164" s="130"/>
     </row>
-    <row r="165" spans="1:31" s="113" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:31" s="113" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A165" s="1"/>
       <c r="B165" s="33"/>
       <c r="C165" s="76">
@@ -13577,7 +13561,7 @@
       <c r="AD165" s="130"/>
       <c r="AE165" s="130"/>
     </row>
-    <row r="166" spans="1:31" s="113" customFormat="1" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:31" s="113" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A166" s="1"/>
       <c r="B166" s="33"/>
       <c r="C166" s="76">
@@ -13615,7 +13599,7 @@
       <c r="AD166" s="130"/>
       <c r="AE166" s="130"/>
     </row>
-    <row r="167" spans="1:31" s="112" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:31" s="112" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A167" s="1"/>
       <c r="B167" s="33"/>
       <c r="C167" s="76">
@@ -13669,7 +13653,7 @@
       <c r="AD167" s="130"/>
       <c r="AE167" s="130"/>
     </row>
-    <row r="168" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A168" s="1"/>
       <c r="B168" s="33"/>
       <c r="C168" s="76">
@@ -13732,7 +13716,7 @@
       <c r="AA168" s="1"/>
       <c r="AB168" s="1"/>
     </row>
-    <row r="169" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A169" s="1"/>
       <c r="B169" s="33"/>
       <c r="C169" s="76">
@@ -13793,7 +13777,7 @@
       <c r="AA169" s="1"/>
       <c r="AB169" s="1"/>
     </row>
-    <row r="170" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A170" s="1"/>
       <c r="B170" s="33"/>
       <c r="C170" s="76">
@@ -13852,7 +13836,7 @@
       <c r="AA170" s="1"/>
       <c r="AB170" s="1"/>
     </row>
-    <row r="171" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A171" s="1"/>
       <c r="B171" s="33"/>
       <c r="C171" s="76">
@@ -13911,7 +13895,7 @@
       <c r="AA171" s="1"/>
       <c r="AB171" s="1"/>
     </row>
-    <row r="172" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A172" s="1"/>
       <c r="B172" s="33"/>
       <c r="C172" s="76">
@@ -13970,7 +13954,7 @@
       <c r="AA172" s="1"/>
       <c r="AB172" s="1"/>
     </row>
-    <row r="173" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A173" s="1"/>
       <c r="B173" s="33"/>
       <c r="C173" s="76">
@@ -14031,7 +14015,7 @@
       <c r="AA173" s="1"/>
       <c r="AB173" s="1"/>
     </row>
-    <row r="174" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A174" s="1"/>
       <c r="B174" s="33"/>
       <c r="C174" s="76">
@@ -14092,7 +14076,7 @@
       <c r="AA174" s="1"/>
       <c r="AB174" s="1"/>
     </row>
-    <row r="175" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A175" s="1"/>
       <c r="B175" s="33"/>
       <c r="C175" s="76">
@@ -14151,7 +14135,7 @@
       <c r="AA175" s="1"/>
       <c r="AB175" s="1"/>
     </row>
-    <row r="176" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A176" s="1"/>
       <c r="B176" s="33"/>
       <c r="C176" s="76">
@@ -14210,7 +14194,7 @@
       <c r="AA176" s="1"/>
       <c r="AB176" s="1"/>
     </row>
-    <row r="177" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A177" s="1"/>
       <c r="B177" s="33"/>
       <c r="C177" s="76">
@@ -14269,7 +14253,7 @@
       <c r="AA177" s="1"/>
       <c r="AB177" s="1"/>
     </row>
-    <row r="178" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A178" s="1"/>
       <c r="B178" s="33"/>
       <c r="C178" s="76">
@@ -14330,7 +14314,7 @@
       <c r="AA178" s="1"/>
       <c r="AB178" s="1"/>
     </row>
-    <row r="179" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A179" s="1"/>
       <c r="B179" s="33"/>
       <c r="C179" s="76">
@@ -14391,7 +14375,7 @@
       <c r="AA179" s="1"/>
       <c r="AB179" s="1"/>
     </row>
-    <row r="180" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A180" s="1"/>
       <c r="B180" s="33"/>
       <c r="C180" s="76">
@@ -14450,7 +14434,7 @@
       <c r="AA180" s="1"/>
       <c r="AB180" s="1"/>
     </row>
-    <row r="181" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A181" s="1"/>
       <c r="B181" s="33"/>
       <c r="C181" s="76">
@@ -14507,7 +14491,7 @@
       <c r="AA181" s="1"/>
       <c r="AB181" s="1"/>
     </row>
-    <row r="182" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A182" s="1"/>
       <c r="B182" s="33"/>
       <c r="C182" s="76">
@@ -14566,7 +14550,7 @@
       <c r="AA182" s="1"/>
       <c r="AB182" s="1"/>
     </row>
-    <row r="183" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A183" s="1"/>
       <c r="B183" s="33"/>
       <c r="C183" s="76">
@@ -14627,7 +14611,7 @@
       <c r="AA183" s="1"/>
       <c r="AB183" s="1"/>
     </row>
-    <row r="184" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A184" s="1"/>
       <c r="B184" s="33"/>
       <c r="C184" s="76">
@@ -14688,7 +14672,7 @@
       <c r="AA184" s="1"/>
       <c r="AB184" s="1"/>
     </row>
-    <row r="185" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A185" s="1"/>
       <c r="B185" s="33"/>
       <c r="C185" s="76">
@@ -14747,7 +14731,7 @@
       <c r="AA185" s="1"/>
       <c r="AB185" s="1"/>
     </row>
-    <row r="186" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A186" s="1"/>
       <c r="B186" s="33"/>
       <c r="C186" s="76">
@@ -14806,7 +14790,7 @@
       <c r="AA186" s="1"/>
       <c r="AB186" s="1"/>
     </row>
-    <row r="187" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A187" s="1"/>
       <c r="B187" s="33"/>
       <c r="C187" s="76">
@@ -14865,7 +14849,7 @@
       <c r="AA187" s="1"/>
       <c r="AB187" s="1"/>
     </row>
-    <row r="188" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A188" s="1"/>
       <c r="B188" s="33"/>
       <c r="C188" s="76">
@@ -14928,7 +14912,7 @@
       <c r="AA188" s="1"/>
       <c r="AB188" s="1"/>
     </row>
-    <row r="189" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A189" s="1"/>
       <c r="B189" s="33"/>
       <c r="C189" s="76">
@@ -14987,7 +14971,7 @@
       <c r="AA189" s="1"/>
       <c r="AB189" s="1"/>
     </row>
-    <row r="190" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A190" s="1"/>
       <c r="B190" s="33"/>
       <c r="C190" s="76">
@@ -15044,7 +15028,7 @@
       <c r="AA190" s="1"/>
       <c r="AB190" s="1"/>
     </row>
-    <row r="191" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A191" s="1"/>
       <c r="B191" s="33"/>
       <c r="C191" s="76">
@@ -15101,7 +15085,7 @@
       <c r="AA191" s="1"/>
       <c r="AB191" s="1"/>
     </row>
-    <row r="192" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A192" s="1"/>
       <c r="B192" s="33"/>
       <c r="C192" s="76">
@@ -15158,7 +15142,7 @@
       <c r="AA192" s="1"/>
       <c r="AB192" s="1"/>
     </row>
-    <row r="193" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A193" s="1"/>
       <c r="B193" s="33"/>
       <c r="C193" s="76">
@@ -15217,7 +15201,7 @@
       <c r="AA193" s="1"/>
       <c r="AB193" s="1"/>
     </row>
-    <row r="194" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A194" s="1"/>
       <c r="B194" s="33"/>
       <c r="C194" s="76">
@@ -15274,7 +15258,7 @@
       <c r="AA194" s="1"/>
       <c r="AB194" s="1"/>
     </row>
-    <row r="195" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A195" s="1"/>
       <c r="B195" s="33"/>
       <c r="C195" s="76">
@@ -15331,7 +15315,7 @@
       <c r="AA195" s="1"/>
       <c r="AB195" s="1"/>
     </row>
-    <row r="196" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A196" s="1"/>
       <c r="B196" s="33"/>
       <c r="C196" s="76">
@@ -15388,7 +15372,7 @@
       <c r="AA196" s="1"/>
       <c r="AB196" s="1"/>
     </row>
-    <row r="197" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A197" s="1"/>
       <c r="B197" s="33"/>
       <c r="C197" s="76">
@@ -15445,7 +15429,7 @@
       <c r="AA197" s="1"/>
       <c r="AB197" s="1"/>
     </row>
-    <row r="198" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A198" s="1"/>
       <c r="B198" s="33"/>
       <c r="C198" s="76">
@@ -15504,7 +15488,7 @@
       <c r="AA198" s="1"/>
       <c r="AB198" s="1"/>
     </row>
-    <row r="199" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A199" s="1"/>
       <c r="B199" s="33"/>
       <c r="C199" s="76">
@@ -15561,7 +15545,7 @@
       <c r="AA199" s="1"/>
       <c r="AB199" s="1"/>
     </row>
-    <row r="200" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A200" s="1"/>
       <c r="B200" s="33"/>
       <c r="C200" s="76">
@@ -15618,7 +15602,7 @@
       <c r="AA200" s="1"/>
       <c r="AB200" s="1"/>
     </row>
-    <row r="201" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A201" s="1"/>
       <c r="B201" s="33"/>
       <c r="C201" s="76">
@@ -15675,7 +15659,7 @@
       <c r="AA201" s="1"/>
       <c r="AB201" s="1"/>
     </row>
-    <row r="202" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A202" s="1"/>
       <c r="B202" s="33"/>
       <c r="C202" s="76">
@@ -15732,7 +15716,7 @@
       <c r="AA202" s="1"/>
       <c r="AB202" s="1"/>
     </row>
-    <row r="203" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A203" s="1"/>
       <c r="B203" s="33"/>
       <c r="C203" s="76">
@@ -15791,7 +15775,7 @@
       <c r="AA203" s="1"/>
       <c r="AB203" s="1"/>
     </row>
-    <row r="204" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A204" s="1"/>
       <c r="B204" s="33"/>
       <c r="C204" s="76">
@@ -15848,7 +15832,7 @@
       <c r="AA204" s="1"/>
       <c r="AB204" s="1"/>
     </row>
-    <row r="205" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A205" s="1"/>
       <c r="B205" s="33"/>
       <c r="C205" s="76">
@@ -15905,7 +15889,7 @@
       <c r="AA205" s="1"/>
       <c r="AB205" s="1"/>
     </row>
-    <row r="206" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A206" s="1"/>
       <c r="B206" s="33"/>
       <c r="C206" s="76">
@@ -15962,7 +15946,7 @@
       <c r="AA206" s="1"/>
       <c r="AB206" s="1"/>
     </row>
-    <row r="207" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A207" s="1"/>
       <c r="B207" s="33"/>
       <c r="C207" s="76">
@@ -16019,7 +16003,7 @@
       <c r="AA207" s="1"/>
       <c r="AB207" s="1"/>
     </row>
-    <row r="208" spans="1:30" s="113" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:30" s="113" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A208" s="1"/>
       <c r="B208" s="33"/>
       <c r="C208" s="76">
@@ -16054,7 +16038,7 @@
       <c r="AC208" s="130"/>
       <c r="AD208" s="130"/>
     </row>
-    <row r="209" spans="1:28" s="133" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:28" s="133" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A209" s="1"/>
       <c r="B209" s="33"/>
       <c r="C209" s="76">
@@ -16114,7 +16098,7 @@
       <c r="AA209" s="1"/>
       <c r="AB209" s="1"/>
     </row>
-    <row r="210" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A210" s="1"/>
       <c r="B210" s="33"/>
       <c r="C210" s="76">
@@ -16184,7 +16168,7 @@
       <c r="AA210" s="1"/>
       <c r="AB210" s="1"/>
     </row>
-    <row r="211" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A211" s="1"/>
       <c r="B211" s="33"/>
       <c r="C211" s="76">
@@ -16254,7 +16238,7 @@
       <c r="AA211" s="1"/>
       <c r="AB211" s="1"/>
     </row>
-    <row r="212" spans="1:28" s="133" customFormat="1" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:28" s="133" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A212" s="1"/>
       <c r="B212" s="33"/>
       <c r="C212" s="76">
@@ -16289,7 +16273,7 @@
       <c r="AA212" s="1"/>
       <c r="AB212" s="1"/>
     </row>
-    <row r="213" spans="1:28" s="133" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:28" s="133" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A213" s="1"/>
       <c r="B213" s="33"/>
       <c r="C213" s="76">
@@ -16340,7 +16324,7 @@
       <c r="AA213" s="1"/>
       <c r="AB213" s="1"/>
     </row>
-    <row r="214" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A214" s="1"/>
       <c r="B214" s="33"/>
       <c r="C214" s="76">
@@ -16403,7 +16387,7 @@
       <c r="AA214" s="1"/>
       <c r="AB214" s="1"/>
     </row>
-    <row r="215" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A215" s="1"/>
       <c r="B215" s="33"/>
       <c r="C215" s="76">
@@ -16466,7 +16450,7 @@
       <c r="AA215" s="1"/>
       <c r="AB215" s="1"/>
     </row>
-    <row r="216" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A216" s="1"/>
       <c r="B216" s="33"/>
       <c r="C216" s="76">
@@ -16523,7 +16507,7 @@
       <c r="AA216" s="1"/>
       <c r="AB216" s="1"/>
     </row>
-    <row r="217" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A217" s="1"/>
       <c r="B217" s="33"/>
       <c r="C217" s="76">
@@ -16582,7 +16566,7 @@
       <c r="AA217" s="1"/>
       <c r="AB217" s="1"/>
     </row>
-    <row r="218" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A218" s="1"/>
       <c r="B218" s="33"/>
       <c r="C218" s="76">
@@ -16641,7 +16625,7 @@
       <c r="AA218" s="1"/>
       <c r="AB218" s="1"/>
     </row>
-    <row r="219" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A219" s="1"/>
       <c r="B219" s="33"/>
       <c r="C219" s="76">
@@ -16702,7 +16686,7 @@
       <c r="AA219" s="1"/>
       <c r="AB219" s="1"/>
     </row>
-    <row r="220" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A220" s="1"/>
       <c r="B220" s="33"/>
       <c r="C220" s="76">
@@ -16763,7 +16747,7 @@
       <c r="AA220" s="1"/>
       <c r="AB220" s="1"/>
     </row>
-    <row r="221" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A221" s="1"/>
       <c r="B221" s="33"/>
       <c r="C221" s="76">
@@ -16820,7 +16804,7 @@
       <c r="AA221" s="1"/>
       <c r="AB221" s="1"/>
     </row>
-    <row r="222" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A222" s="1"/>
       <c r="B222" s="33"/>
       <c r="C222" s="76">
@@ -16877,7 +16861,7 @@
       <c r="AA222" s="1"/>
       <c r="AB222" s="1"/>
     </row>
-    <row r="223" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A223" s="1"/>
       <c r="B223" s="33"/>
       <c r="C223" s="76">
@@ -16934,7 +16918,7 @@
       <c r="AA223" s="1"/>
       <c r="AB223" s="1"/>
     </row>
-    <row r="224" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A224" s="1"/>
       <c r="B224" s="33"/>
       <c r="C224" s="76">
@@ -16993,7 +16977,7 @@
       <c r="AA224" s="1"/>
       <c r="AB224" s="1"/>
     </row>
-    <row r="225" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A225" s="1"/>
       <c r="B225" s="33"/>
       <c r="C225" s="76">
@@ -17052,7 +17036,7 @@
       <c r="AA225" s="1"/>
       <c r="AB225" s="1"/>
     </row>
-    <row r="226" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A226" s="1"/>
       <c r="B226" s="33"/>
       <c r="C226" s="76">
@@ -17109,7 +17093,7 @@
       <c r="AA226" s="1"/>
       <c r="AB226" s="1"/>
     </row>
-    <row r="227" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A227" s="1"/>
       <c r="B227" s="33"/>
       <c r="C227" s="76">
@@ -17166,7 +17150,7 @@
       <c r="AA227" s="1"/>
       <c r="AB227" s="1"/>
     </row>
-    <row r="228" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A228" s="1"/>
       <c r="B228" s="33"/>
       <c r="C228" s="76">
@@ -17223,7 +17207,7 @@
       <c r="AA228" s="1"/>
       <c r="AB228" s="1"/>
     </row>
-    <row r="229" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A229" s="1"/>
       <c r="B229" s="33"/>
       <c r="C229" s="76">
@@ -17282,7 +17266,7 @@
       <c r="AA229" s="1"/>
       <c r="AB229" s="1"/>
     </row>
-    <row r="230" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A230" s="1"/>
       <c r="B230" s="33"/>
       <c r="C230" s="76">
@@ -17341,7 +17325,7 @@
       <c r="AA230" s="1"/>
       <c r="AB230" s="1"/>
     </row>
-    <row r="231" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A231" s="1"/>
       <c r="B231" s="33"/>
       <c r="C231" s="76">
@@ -17398,7 +17382,7 @@
       <c r="AA231" s="1"/>
       <c r="AB231" s="1"/>
     </row>
-    <row r="232" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A232" s="1"/>
       <c r="B232" s="33"/>
       <c r="C232" s="76">
@@ -17455,7 +17439,7 @@
       <c r="AA232" s="1"/>
       <c r="AB232" s="1"/>
     </row>
-    <row r="233" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A233" s="1"/>
       <c r="B233" s="33"/>
       <c r="C233" s="76">
@@ -17512,7 +17496,7 @@
       <c r="AA233" s="1"/>
       <c r="AB233" s="1"/>
     </row>
-    <row r="234" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A234" s="1"/>
       <c r="B234" s="33"/>
       <c r="C234" s="76">
@@ -17582,7 +17566,7 @@
       <c r="AA234" s="1"/>
       <c r="AB234" s="1"/>
     </row>
-    <row r="235" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A235" s="1"/>
       <c r="B235" s="33"/>
       <c r="C235" s="76">
@@ -17649,7 +17633,7 @@
       <c r="AA235" s="1"/>
       <c r="AB235" s="1"/>
     </row>
-    <row r="236" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A236" s="1"/>
       <c r="B236" s="33"/>
       <c r="C236" s="76">
@@ -17712,7 +17696,7 @@
       <c r="AA236" s="1"/>
       <c r="AB236" s="1"/>
     </row>
-    <row r="237" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A237" s="1"/>
       <c r="B237" s="33"/>
       <c r="C237" s="76">
@@ -17775,7 +17759,7 @@
       <c r="AA237" s="1"/>
       <c r="AB237" s="1"/>
     </row>
-    <row r="238" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A238" s="1"/>
       <c r="B238" s="33"/>
       <c r="C238" s="76">
@@ -17842,7 +17826,7 @@
       <c r="AA238" s="1"/>
       <c r="AB238" s="1"/>
     </row>
-    <row r="239" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A239" s="1"/>
       <c r="B239" s="33"/>
       <c r="C239" s="76">
@@ -17911,7 +17895,7 @@
       <c r="AA239" s="1"/>
       <c r="AB239" s="1"/>
     </row>
-    <row r="240" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A240" s="1"/>
       <c r="B240" s="33"/>
       <c r="C240" s="76">
@@ -17978,7 +17962,7 @@
       <c r="AA240" s="1"/>
       <c r="AB240" s="1"/>
     </row>
-    <row r="241" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A241" s="1"/>
       <c r="B241" s="33"/>
       <c r="C241" s="76">
@@ -18045,7 +18029,7 @@
       <c r="AA241" s="1"/>
       <c r="AB241" s="1"/>
     </row>
-    <row r="242" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A242" s="1"/>
       <c r="B242" s="33"/>
       <c r="C242" s="76">
@@ -18112,7 +18096,7 @@
       <c r="AA242" s="1"/>
       <c r="AB242" s="1"/>
     </row>
-    <row r="243" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A243" s="1"/>
       <c r="B243" s="33"/>
       <c r="C243" s="76">
@@ -18179,7 +18163,7 @@
       <c r="AA243" s="1"/>
       <c r="AB243" s="1"/>
     </row>
-    <row r="244" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A244" s="1"/>
       <c r="B244" s="33"/>
       <c r="C244" s="76">
@@ -18248,7 +18232,7 @@
       <c r="AA244" s="1"/>
       <c r="AB244" s="1"/>
     </row>
-    <row r="245" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A245" s="1"/>
       <c r="B245" s="33"/>
       <c r="C245" s="76">
@@ -18315,7 +18299,7 @@
       <c r="AA245" s="1"/>
       <c r="AB245" s="1"/>
     </row>
-    <row r="246" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A246" s="1"/>
       <c r="B246" s="33"/>
       <c r="C246" s="76">
@@ -18382,7 +18366,7 @@
       <c r="AA246" s="1"/>
       <c r="AB246" s="1"/>
     </row>
-    <row r="247" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A247" s="1"/>
       <c r="B247" s="33"/>
       <c r="C247" s="76">
@@ -18449,7 +18433,7 @@
       <c r="AA247" s="1"/>
       <c r="AB247" s="1"/>
     </row>
-    <row r="248" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A248" s="1"/>
       <c r="B248" s="33"/>
       <c r="C248" s="76">
@@ -18516,7 +18500,7 @@
       <c r="AA248" s="1"/>
       <c r="AB248" s="1"/>
     </row>
-    <row r="249" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A249" s="1"/>
       <c r="B249" s="33"/>
       <c r="C249" s="76">
@@ -18585,7 +18569,7 @@
       <c r="AA249" s="1"/>
       <c r="AB249" s="1"/>
     </row>
-    <row r="250" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A250" s="1"/>
       <c r="B250" s="33"/>
       <c r="C250" s="76">
@@ -18652,7 +18636,7 @@
       <c r="AA250" s="1"/>
       <c r="AB250" s="1"/>
     </row>
-    <row r="251" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A251" s="1"/>
       <c r="B251" s="33"/>
       <c r="C251" s="76">
@@ -18719,7 +18703,7 @@
       <c r="AA251" s="1"/>
       <c r="AB251" s="1"/>
     </row>
-    <row r="252" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A252" s="1"/>
       <c r="B252" s="33"/>
       <c r="C252" s="76">
@@ -18786,7 +18770,7 @@
       <c r="AA252" s="1"/>
       <c r="AB252" s="1"/>
     </row>
-    <row r="253" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A253" s="1"/>
       <c r="B253" s="33"/>
       <c r="C253" s="76">
@@ -18853,7 +18837,7 @@
       <c r="AA253" s="1"/>
       <c r="AB253" s="1"/>
     </row>
-    <row r="254" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A254" s="1"/>
       <c r="B254" s="33"/>
       <c r="C254" s="76">
@@ -18914,7 +18898,7 @@
       <c r="AA254" s="1"/>
       <c r="AB254" s="1"/>
     </row>
-    <row r="255" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A255" s="1"/>
       <c r="B255" s="33"/>
       <c r="C255" s="76">
@@ -18971,7 +18955,7 @@
       <c r="AA255" s="1"/>
       <c r="AB255" s="1"/>
     </row>
-    <row r="256" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A256" s="1"/>
       <c r="B256" s="33"/>
       <c r="C256" s="76">
@@ -19028,7 +19012,7 @@
       <c r="AA256" s="1"/>
       <c r="AB256" s="1"/>
     </row>
-    <row r="257" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A257" s="1"/>
       <c r="B257" s="33"/>
       <c r="C257" s="76">
@@ -19085,7 +19069,7 @@
       <c r="AA257" s="1"/>
       <c r="AB257" s="1"/>
     </row>
-    <row r="258" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A258" s="1"/>
       <c r="B258" s="33"/>
       <c r="C258" s="76">
@@ -19142,7 +19126,7 @@
       <c r="AA258" s="1"/>
       <c r="AB258" s="1"/>
     </row>
-    <row r="259" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A259" s="1"/>
       <c r="B259" s="33"/>
       <c r="C259" s="76">
@@ -19211,7 +19195,7 @@
       <c r="AA259" s="1"/>
       <c r="AB259" s="1"/>
     </row>
-    <row r="260" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A260" s="1"/>
       <c r="B260" s="33"/>
       <c r="C260" s="76">
@@ -19278,7 +19262,7 @@
       <c r="AA260" s="1"/>
       <c r="AB260" s="1"/>
     </row>
-    <row r="261" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A261" s="1"/>
       <c r="B261" s="33"/>
       <c r="C261" s="76">
@@ -19345,7 +19329,7 @@
       <c r="AA261" s="1"/>
       <c r="AB261" s="1"/>
     </row>
-    <row r="262" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A262" s="1"/>
       <c r="B262" s="33"/>
       <c r="C262" s="76">
@@ -19412,7 +19396,7 @@
       <c r="AA262" s="1"/>
       <c r="AB262" s="1"/>
     </row>
-    <row r="263" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A263" s="1"/>
       <c r="B263" s="33"/>
       <c r="C263" s="76">
@@ -19479,7 +19463,7 @@
       <c r="AA263" s="1"/>
       <c r="AB263" s="1"/>
     </row>
-    <row r="264" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A264" s="1"/>
       <c r="B264" s="33"/>
       <c r="C264" s="76">
@@ -19538,7 +19522,7 @@
       <c r="AA264" s="1"/>
       <c r="AB264" s="1"/>
     </row>
-    <row r="265" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A265" s="1"/>
       <c r="B265" s="33"/>
       <c r="C265" s="76">
@@ -19600,7 +19584,7 @@
       <c r="AA265" s="1"/>
       <c r="AB265" s="1"/>
     </row>
-    <row r="266" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A266" s="1"/>
       <c r="B266" s="33"/>
       <c r="C266" s="76">
@@ -19661,7 +19645,7 @@
       <c r="AA266" s="1"/>
       <c r="AB266" s="1"/>
     </row>
-    <row r="267" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A267" s="1"/>
       <c r="B267" s="33"/>
       <c r="C267" s="76">
@@ -19721,7 +19705,7 @@
       <c r="AA267" s="1"/>
       <c r="AB267" s="1"/>
     </row>
-    <row r="268" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A268" s="1"/>
       <c r="B268" s="33"/>
       <c r="C268" s="76">
@@ -19788,7 +19772,7 @@
       <c r="AA268" s="1"/>
       <c r="AB268" s="1"/>
     </row>
-    <row r="269" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A269" s="1"/>
       <c r="B269" s="33"/>
       <c r="C269" s="76">
@@ -19853,7 +19837,7 @@
       <c r="AA269" s="1"/>
       <c r="AB269" s="1"/>
     </row>
-    <row r="270" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A270" s="1"/>
       <c r="B270" s="33"/>
       <c r="C270" s="76">
@@ -19915,7 +19899,7 @@
       <c r="AA270" s="1"/>
       <c r="AB270" s="1"/>
     </row>
-    <row r="271" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A271" s="1"/>
       <c r="B271" s="33"/>
       <c r="C271" s="76">
@@ -19975,7 +19959,7 @@
       <c r="AA271" s="1"/>
       <c r="AB271" s="1"/>
     </row>
-    <row r="272" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A272" s="1"/>
       <c r="B272" s="33"/>
       <c r="C272" s="76">
@@ -20032,7 +20016,7 @@
       <c r="AA272" s="1"/>
       <c r="AB272" s="1"/>
     </row>
-    <row r="273" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A273" s="1"/>
       <c r="B273" s="33"/>
       <c r="C273" s="76">
@@ -20099,7 +20083,7 @@
       <c r="AA273" s="1"/>
       <c r="AB273" s="1"/>
     </row>
-    <row r="274" spans="1:28" s="133" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:28" s="133" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A274" s="1"/>
       <c r="B274" s="33"/>
       <c r="C274" s="76">
@@ -20132,7 +20116,7 @@
       <c r="AA274" s="1"/>
       <c r="AB274" s="1"/>
     </row>
-    <row r="275" spans="1:28" s="133" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:28" s="133" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A275" s="1"/>
       <c r="B275" s="33"/>
       <c r="C275" s="76">
@@ -20188,7 +20172,7 @@
       <c r="AA275" s="1"/>
       <c r="AB275" s="1"/>
     </row>
-    <row r="276" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A276" s="1"/>
       <c r="B276" s="33"/>
       <c r="C276" s="76">
@@ -20241,7 +20225,7 @@
       <c r="AA276" s="1"/>
       <c r="AB276" s="1"/>
     </row>
-    <row r="277" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A277" s="1"/>
       <c r="B277" s="33"/>
       <c r="C277" s="76">
@@ -20294,7 +20278,7 @@
       <c r="AA277" s="1"/>
       <c r="AB277" s="1"/>
     </row>
-    <row r="278" spans="1:28" s="133" customFormat="1" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:28" s="133" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A278" s="1"/>
       <c r="B278" s="33"/>
       <c r="C278" s="76">
@@ -20329,7 +20313,7 @@
       <c r="AA278" s="1"/>
       <c r="AB278" s="1"/>
     </row>
-    <row r="279" spans="1:28" s="133" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:28" s="133" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A279" s="1"/>
       <c r="B279" s="33"/>
       <c r="C279" s="76">
@@ -20379,7 +20363,7 @@
       <c r="AA279" s="1"/>
       <c r="AB279" s="1"/>
     </row>
-    <row r="280" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A280" s="1"/>
       <c r="B280" s="33"/>
       <c r="C280" s="76">
@@ -20437,7 +20421,7 @@
       <c r="AA280" s="1"/>
       <c r="AB280" s="1"/>
     </row>
-    <row r="281" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A281" s="1"/>
       <c r="B281" s="33"/>
       <c r="C281" s="76">
@@ -20495,7 +20479,7 @@
       <c r="AA281" s="1"/>
       <c r="AB281" s="1"/>
     </row>
-    <row r="282" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A282" s="1"/>
       <c r="B282" s="33"/>
       <c r="C282" s="76">
@@ -20548,7 +20532,7 @@
       <c r="AA282" s="1"/>
       <c r="AB282" s="1"/>
     </row>
-    <row r="283" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A283" s="1"/>
       <c r="B283" s="33"/>
       <c r="C283" s="76">
@@ -20600,7 +20584,7 @@
       <c r="AA283" s="1"/>
       <c r="AB283" s="1"/>
     </row>
-    <row r="284" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A284" s="1"/>
       <c r="B284" s="33"/>
       <c r="C284" s="76">
@@ -20655,7 +20639,7 @@
       <c r="AA284" s="1"/>
       <c r="AB284" s="1"/>
     </row>
-    <row r="285" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A285" s="1"/>
       <c r="B285" s="33"/>
       <c r="C285" s="76">
@@ -20709,7 +20693,7 @@
       <c r="AA285" s="1"/>
       <c r="AB285" s="1"/>
     </row>
-    <row r="286" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A286" s="1"/>
       <c r="B286" s="33"/>
       <c r="C286" s="76">
@@ -20763,7 +20747,7 @@
       <c r="AA286" s="1"/>
       <c r="AB286" s="1"/>
     </row>
-    <row r="287" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A287" s="1"/>
       <c r="B287" s="33"/>
       <c r="C287" s="76">
@@ -20813,7 +20797,7 @@
       <c r="AA287" s="1"/>
       <c r="AB287" s="1"/>
     </row>
-    <row r="288" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A288" s="1"/>
       <c r="B288" s="33"/>
       <c r="C288" s="76">
@@ -20863,7 +20847,7 @@
       <c r="AA288" s="1"/>
       <c r="AB288" s="1"/>
     </row>
-    <row r="289" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A289" s="1"/>
       <c r="B289" s="33"/>
       <c r="C289" s="76">
@@ -20916,7 +20900,7 @@
       <c r="AA289" s="1"/>
       <c r="AB289" s="1"/>
     </row>
-    <row r="290" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A290" s="1"/>
       <c r="B290" s="33"/>
       <c r="C290" s="76">
@@ -20970,7 +20954,7 @@
       <c r="AA290" s="1"/>
       <c r="AB290" s="1"/>
     </row>
-    <row r="291" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A291" s="1"/>
       <c r="B291" s="33"/>
       <c r="C291" s="76">
@@ -21024,7 +21008,7 @@
       <c r="AA291" s="1"/>
       <c r="AB291" s="1"/>
     </row>
-    <row r="292" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A292" s="1"/>
       <c r="B292" s="33"/>
       <c r="C292" s="76">
@@ -21074,7 +21058,7 @@
       <c r="AA292" s="1"/>
       <c r="AB292" s="1"/>
     </row>
-    <row r="293" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A293" s="1"/>
       <c r="B293" s="33"/>
       <c r="C293" s="76">
@@ -21124,7 +21108,7 @@
       <c r="AA293" s="1"/>
       <c r="AB293" s="1"/>
     </row>
-    <row r="294" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A294" s="1"/>
       <c r="B294" s="33"/>
       <c r="C294" s="76">
@@ -21177,7 +21161,7 @@
       <c r="AA294" s="1"/>
       <c r="AB294" s="1"/>
     </row>
-    <row r="295" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A295" s="1"/>
       <c r="B295" s="33"/>
       <c r="C295" s="76">
@@ -21229,7 +21213,7 @@
       <c r="AA295" s="1"/>
       <c r="AB295" s="1"/>
     </row>
-    <row r="296" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A296" s="1"/>
       <c r="B296" s="33"/>
       <c r="C296" s="76">
@@ -21281,7 +21265,7 @@
       <c r="AA296" s="1"/>
       <c r="AB296" s="1"/>
     </row>
-    <row r="297" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A297" s="1"/>
       <c r="B297" s="33"/>
       <c r="C297" s="76">
@@ -21330,7 +21314,7 @@
       <c r="AA297" s="1"/>
       <c r="AB297" s="1"/>
     </row>
-    <row r="298" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A298" s="1"/>
       <c r="B298" s="33"/>
       <c r="C298" s="76">
@@ -21377,7 +21361,7 @@
       <c r="AA298" s="1"/>
       <c r="AB298" s="1"/>
     </row>
-    <row r="299" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A299" s="1"/>
       <c r="B299" s="33"/>
       <c r="C299" s="76">
@@ -21430,7 +21414,7 @@
       <c r="AA299" s="1"/>
       <c r="AB299" s="1"/>
     </row>
-    <row r="300" spans="1:28" s="133" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:28" s="133" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A300" s="1"/>
       <c r="B300" s="33"/>
       <c r="C300" s="76">
@@ -21463,7 +21447,7 @@
       <c r="AA300" s="1"/>
       <c r="AB300" s="1"/>
     </row>
-    <row r="301" spans="1:28" s="99" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:28" s="99" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A301" s="1"/>
       <c r="B301" s="33"/>
       <c r="C301" s="76">
@@ -21496,7 +21480,7 @@
       <c r="AA301" s="1"/>
       <c r="AB301" s="1"/>
     </row>
-    <row r="302" spans="1:28" s="99" customFormat="1" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:28" s="99" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A302" s="1"/>
       <c r="B302" s="35"/>
       <c r="C302" s="79">
@@ -21531,7 +21515,7 @@
       <c r="AA302" s="1"/>
       <c r="AB302" s="1"/>
     </row>
-    <row r="303" spans="1:28" s="99" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:28" s="99" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A303" s="1"/>
       <c r="B303" s="19"/>
       <c r="C303" s="80">
@@ -21564,7 +21548,7 @@
       <c r="AA303" s="1"/>
       <c r="AB303" s="1"/>
     </row>
-    <row r="304" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A304" s="1"/>
       <c r="B304" s="1"/>
       <c r="C304" s="76">
@@ -21597,7 +21581,7 @@
       <c r="AA304" s="1"/>
       <c r="AB304" s="1"/>
     </row>
-    <row r="305" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A305" s="1"/>
       <c r="B305" s="1"/>
       <c r="C305" s="76">
@@ -21630,7 +21614,7 @@
       <c r="AA305" s="1"/>
       <c r="AB305" s="1"/>
     </row>
-    <row r="306" spans="1:28" s="101" customFormat="1" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="306" spans="1:28" s="101" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A306" s="1"/>
       <c r="B306" s="20"/>
       <c r="C306" s="77">
@@ -21663,7 +21647,7 @@
       <c r="AA306" s="1"/>
       <c r="AB306" s="1"/>
     </row>
-    <row r="307" spans="1:28" s="101" customFormat="1" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:28" s="101" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A307" s="1"/>
       <c r="B307" s="34" t="s">
         <v>21</v>
@@ -21698,7 +21682,7 @@
       <c r="AA307" s="1"/>
       <c r="AB307" s="1"/>
     </row>
-    <row r="308" spans="1:28" s="101" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:28" s="101" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A308" s="1"/>
       <c r="B308" s="33"/>
       <c r="C308" s="76">
@@ -21731,7 +21715,7 @@
       <c r="AA308" s="1"/>
       <c r="AB308" s="1"/>
     </row>
-    <row r="309" spans="1:28" s="101" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:28" s="101" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A309" s="1"/>
       <c r="B309" s="33"/>
       <c r="C309" s="76">
@@ -21768,7 +21752,7 @@
       <c r="AA309" s="1"/>
       <c r="AB309" s="1"/>
     </row>
-    <row r="310" spans="1:28" s="101" customFormat="1" ht="20.149999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:28" s="101" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A310" s="1"/>
       <c r="B310" s="33"/>
       <c r="C310" s="76">
@@ -21807,7 +21791,7 @@
       <c r="AA310" s="1"/>
       <c r="AB310" s="1"/>
     </row>
-    <row r="311" spans="1:28" s="101" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:28" s="101" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A311" s="1"/>
       <c r="B311" s="33"/>
       <c r="C311" s="76">
@@ -21840,7 +21824,7 @@
       <c r="AA311" s="1"/>
       <c r="AB311" s="1"/>
     </row>
-    <row r="312" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A312" s="1"/>
       <c r="B312" s="33"/>
       <c r="C312" s="76">
@@ -21873,7 +21857,7 @@
       <c r="AA312" s="1"/>
       <c r="AB312" s="1"/>
     </row>
-    <row r="313" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A313" s="1"/>
       <c r="B313" s="33"/>
       <c r="C313" s="76">
@@ -21906,7 +21890,7 @@
       <c r="AA313" s="1"/>
       <c r="AB313" s="1"/>
     </row>
-    <row r="314" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A314" s="1"/>
       <c r="B314" s="33"/>
       <c r="C314" s="76">
@@ -21939,7 +21923,7 @@
       <c r="AA314" s="1"/>
       <c r="AB314" s="1"/>
     </row>
-    <row r="315" spans="1:28" s="101" customFormat="1" ht="28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:28" s="101" customFormat="1" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A315" s="1"/>
       <c r="B315" s="33"/>
       <c r="C315" s="76">
@@ -21982,7 +21966,7 @@
       <c r="AA315" s="1"/>
       <c r="AB315" s="1"/>
     </row>
-    <row r="316" spans="1:28" s="101" customFormat="1" ht="11.5" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:28" s="101" customFormat="1" ht="11.45" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A316" s="1"/>
       <c r="B316" s="33" t="s">
         <v>20</v>
@@ -22017,7 +22001,7 @@
       <c r="AA316" s="1"/>
       <c r="AB316" s="1"/>
     </row>
-    <row r="317" spans="1:28" s="101" customFormat="1" ht="13" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:28" s="101" customFormat="1" ht="12.95" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A317" s="1"/>
       <c r="B317" s="33"/>
       <c r="C317" s="76">
@@ -22050,7 +22034,7 @@
       <c r="AA317" s="1"/>
       <c r="AB317" s="1"/>
     </row>
-    <row r="318" spans="1:28" s="101" customFormat="1" ht="8.5" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:28" s="101" customFormat="1" ht="8.4499999999999993" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A318" s="1"/>
       <c r="B318" s="33" t="s">
         <v>19</v>
@@ -22087,7 +22071,7 @@
       <c r="AA318" s="1"/>
       <c r="AB318" s="1"/>
     </row>
-    <row r="319" spans="1:28" s="101" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:28" s="101" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A319" s="1"/>
       <c r="B319" s="33"/>
       <c r="C319" s="76">
@@ -22122,7 +22106,7 @@
       <c r="AA319" s="1"/>
       <c r="AB319" s="1"/>
     </row>
-    <row r="320" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A320" s="1"/>
       <c r="B320" s="33"/>
       <c r="C320" s="76">
@@ -22169,7 +22153,7 @@
       <c r="AA320" s="1"/>
       <c r="AB320" s="1"/>
     </row>
-    <row r="321" spans="1:31" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:31" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A321" s="1"/>
       <c r="B321" s="33"/>
       <c r="C321" s="76"/>
@@ -22208,7 +22192,7 @@
       <c r="AA321" s="1"/>
       <c r="AB321" s="1"/>
     </row>
-    <row r="322" spans="1:31" s="101" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:31" s="101" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A322" s="1"/>
       <c r="B322" s="33"/>
       <c r="C322" s="76">
@@ -22249,7 +22233,7 @@
       <c r="AA322" s="1"/>
       <c r="AB322" s="1"/>
     </row>
-    <row r="323" spans="1:31" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:31" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A323" s="1"/>
       <c r="B323" s="33"/>
       <c r="C323" s="76"/>
@@ -22291,7 +22275,7 @@
       <c r="AA323" s="1"/>
       <c r="AB323" s="1"/>
     </row>
-    <row r="324" spans="1:31" s="101" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:31" s="101" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A324" s="1"/>
       <c r="B324" s="33"/>
       <c r="C324" s="76">
@@ -22334,7 +22318,7 @@
       <c r="AA324" s="1"/>
       <c r="AB324" s="1"/>
     </row>
-    <row r="325" spans="1:31" s="111" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:31" s="111" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A325" s="1"/>
       <c r="B325" s="33"/>
       <c r="C325" s="76">
@@ -22377,7 +22361,7 @@
       <c r="AA325" s="1"/>
       <c r="AB325" s="1"/>
     </row>
-    <row r="326" spans="1:31" s="131" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:31" s="131" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A326" s="1"/>
       <c r="B326" s="33"/>
       <c r="C326" s="76">
@@ -22418,7 +22402,7 @@
       <c r="AA326" s="1"/>
       <c r="AB326" s="1"/>
     </row>
-    <row r="327" spans="1:31" s="125" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:31" s="125" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A327" s="1"/>
       <c r="B327" s="33"/>
       <c r="C327" s="76">
@@ -22466,7 +22450,7 @@
       <c r="AD327" s="130"/>
       <c r="AE327" s="130"/>
     </row>
-    <row r="328" spans="1:31" s="111" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:31" s="111" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A328" s="1"/>
       <c r="B328" s="33"/>
       <c r="C328" s="76">
@@ -22517,7 +22501,7 @@
       <c r="AA328" s="1"/>
       <c r="AB328" s="1"/>
     </row>
-    <row r="329" spans="1:31" s="111" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:31" s="111" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A329" s="1"/>
       <c r="B329" s="33"/>
       <c r="C329" s="76">
@@ -22562,7 +22546,7 @@
       <c r="AA329" s="1"/>
       <c r="AB329" s="1"/>
     </row>
-    <row r="330" spans="1:31" s="111" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:31" s="111" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A330" s="1"/>
       <c r="B330" s="33"/>
       <c r="C330" s="76">
@@ -22607,7 +22591,7 @@
       <c r="AA330" s="1"/>
       <c r="AB330" s="1"/>
     </row>
-    <row r="331" spans="1:31" s="111" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:31" s="111" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A331" s="1"/>
       <c r="B331" s="33"/>
       <c r="C331" s="76">
@@ -22652,7 +22636,7 @@
       <c r="AA331" s="1"/>
       <c r="AB331" s="1"/>
     </row>
-    <row r="332" spans="1:31" s="111" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:31" s="111" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A332" s="1"/>
       <c r="B332" s="33"/>
       <c r="C332" s="76">
@@ -22697,7 +22681,7 @@
       <c r="AA332" s="1"/>
       <c r="AB332" s="1"/>
     </row>
-    <row r="333" spans="1:31" s="111" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:31" s="111" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A333" s="1"/>
       <c r="B333" s="33"/>
       <c r="C333" s="76">
@@ -22742,7 +22726,7 @@
       <c r="AA333" s="1"/>
       <c r="AB333" s="1"/>
     </row>
-    <row r="334" spans="1:31" s="111" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:31" s="111" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A334" s="1"/>
       <c r="B334" s="33"/>
       <c r="C334" s="76">
@@ -22783,7 +22767,7 @@
       <c r="AA334" s="1"/>
       <c r="AB334" s="1"/>
     </row>
-    <row r="335" spans="1:31" s="111" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:31" s="111" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A335" s="1"/>
       <c r="B335" s="33"/>
       <c r="C335" s="76">
@@ -22824,7 +22808,7 @@
       <c r="AA335" s="1"/>
       <c r="AB335" s="1"/>
     </row>
-    <row r="336" spans="1:31" s="101" customFormat="1" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:31" s="101" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A336" s="1"/>
       <c r="B336" s="33"/>
       <c r="C336" s="76">
@@ -22859,7 +22843,7 @@
       <c r="AA336" s="1"/>
       <c r="AB336" s="1"/>
     </row>
-    <row r="337" spans="1:28" s="155" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:28" s="155" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A337" s="1"/>
       <c r="B337" s="33"/>
       <c r="C337" s="76">
@@ -22894,7 +22878,7 @@
       <c r="AA337" s="1"/>
       <c r="AB337" s="1"/>
     </row>
-    <row r="338" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A338" s="1"/>
       <c r="B338" s="33"/>
       <c r="C338" s="76">
@@ -22929,7 +22913,7 @@
       <c r="AA338" s="1"/>
       <c r="AB338" s="1"/>
     </row>
-    <row r="339" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A339" s="1"/>
       <c r="B339" s="33"/>
       <c r="C339" s="76">
@@ -22974,7 +22958,7 @@
       <c r="AA339" s="1"/>
       <c r="AB339" s="1"/>
     </row>
-    <row r="340" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A340" s="1"/>
       <c r="B340" s="33"/>
       <c r="C340" s="76">
@@ -23021,7 +23005,7 @@
       <c r="AA340" s="1"/>
       <c r="AB340" s="1"/>
     </row>
-    <row r="341" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A341" s="1"/>
       <c r="B341" s="33"/>
       <c r="C341" s="76">
@@ -23073,7 +23057,7 @@
       <c r="AA341" s="1"/>
       <c r="AB341" s="1"/>
     </row>
-    <row r="342" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A342" s="1"/>
       <c r="B342" s="33"/>
       <c r="C342" s="76"/>
@@ -23123,7 +23107,7 @@
       <c r="AA342" s="1"/>
       <c r="AB342" s="1"/>
     </row>
-    <row r="343" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A343" s="1"/>
       <c r="B343" s="33"/>
       <c r="C343" s="76">
@@ -23172,7 +23156,7 @@
       <c r="AA343" s="1"/>
       <c r="AB343" s="1"/>
     </row>
-    <row r="344" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A344" s="1"/>
       <c r="B344" s="33"/>
       <c r="C344" s="76"/>
@@ -23216,7 +23200,7 @@
       <c r="AA344" s="1"/>
       <c r="AB344" s="1"/>
     </row>
-    <row r="345" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A345" s="1"/>
       <c r="B345" s="33"/>
       <c r="C345" s="76">
@@ -23255,7 +23239,7 @@
       <c r="AA345" s="1"/>
       <c r="AB345" s="1"/>
     </row>
-    <row r="346" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A346" s="1"/>
       <c r="B346" s="33"/>
       <c r="C346" s="76">
@@ -23294,7 +23278,7 @@
       <c r="AA346" s="1"/>
       <c r="AB346" s="1"/>
     </row>
-    <row r="347" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A347" s="1"/>
       <c r="B347" s="33"/>
       <c r="C347" s="76">
@@ -23335,7 +23319,7 @@
       <c r="AA347" s="1"/>
       <c r="AB347" s="1"/>
     </row>
-    <row r="348" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A348" s="1"/>
       <c r="B348" s="33"/>
       <c r="C348" s="76"/>
@@ -23376,7 +23360,7 @@
       <c r="AA348" s="1"/>
       <c r="AB348" s="1"/>
     </row>
-    <row r="349" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A349" s="1"/>
       <c r="B349" s="33"/>
       <c r="C349" s="76"/>
@@ -23406,7 +23390,7 @@
       <c r="AA349" s="1"/>
       <c r="AB349" s="1"/>
     </row>
-    <row r="350" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A350" s="1"/>
       <c r="B350" s="33"/>
       <c r="C350" s="76">
@@ -23441,7 +23425,7 @@
       <c r="AA350" s="1"/>
       <c r="AB350" s="1"/>
     </row>
-    <row r="351" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A351" s="1"/>
       <c r="B351" s="33"/>
       <c r="C351" s="76">
@@ -23482,7 +23466,7 @@
       <c r="AA351" s="1"/>
       <c r="AB351" s="1"/>
     </row>
-    <row r="352" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A352" s="1"/>
       <c r="B352" s="33"/>
       <c r="C352" s="76">
@@ -23525,7 +23509,7 @@
       <c r="AA352" s="1"/>
       <c r="AB352" s="1"/>
     </row>
-    <row r="353" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A353" s="1"/>
       <c r="B353" s="33"/>
       <c r="C353" s="76">
@@ -23573,7 +23557,7 @@
       <c r="AA353" s="1"/>
       <c r="AB353" s="1"/>
     </row>
-    <row r="354" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A354" s="1"/>
       <c r="B354" s="33"/>
       <c r="C354" s="76"/>
@@ -23617,7 +23601,7 @@
       <c r="AA354" s="1"/>
       <c r="AB354" s="1"/>
     </row>
-    <row r="355" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A355" s="1"/>
       <c r="B355" s="33"/>
       <c r="C355" s="76">
@@ -23662,7 +23646,7 @@
       <c r="AA355" s="1"/>
       <c r="AB355" s="1"/>
     </row>
-    <row r="356" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A356" s="1"/>
       <c r="B356" s="33"/>
       <c r="C356" s="76">
@@ -23695,7 +23679,7 @@
       <c r="AA356" s="1"/>
       <c r="AB356" s="1"/>
     </row>
-    <row r="357" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A357" s="1"/>
       <c r="B357" s="33"/>
       <c r="C357" s="76">
@@ -23730,7 +23714,7 @@
       <c r="AA357" s="1"/>
       <c r="AB357" s="1"/>
     </row>
-    <row r="358" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A358" s="1"/>
       <c r="B358" s="33"/>
       <c r="C358" s="76">
@@ -23765,7 +23749,7 @@
       <c r="AA358" s="1"/>
       <c r="AB358" s="1"/>
     </row>
-    <row r="359" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A359" s="1"/>
       <c r="B359" s="33"/>
       <c r="C359" s="76">
@@ -23800,7 +23784,7 @@
       <c r="AA359" s="1"/>
       <c r="AB359" s="1"/>
     </row>
-    <row r="360" spans="1:28" s="155" customFormat="1" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:28" s="155" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A360" s="1"/>
       <c r="B360" s="33"/>
       <c r="C360" s="76">
@@ -23835,7 +23819,7 @@
       <c r="AA360" s="1"/>
       <c r="AB360" s="1"/>
     </row>
-    <row r="361" spans="1:28" s="102" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:28" s="102" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A361" s="1"/>
       <c r="B361" s="33"/>
       <c r="C361" s="76">
@@ -23870,7 +23854,7 @@
       <c r="AA361" s="1"/>
       <c r="AB361" s="1"/>
     </row>
-    <row r="362" spans="1:28" s="102" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:28" s="102" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A362" s="1"/>
       <c r="B362" s="33"/>
       <c r="C362" s="76">
@@ -23911,7 +23895,7 @@
       <c r="AA362" s="1"/>
       <c r="AB362" s="1"/>
     </row>
-    <row r="363" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A363" s="1"/>
       <c r="B363" s="33"/>
       <c r="C363" s="76"/>
@@ -23965,7 +23949,7 @@
       <c r="AA363" s="1"/>
       <c r="AB363" s="1"/>
     </row>
-    <row r="364" spans="1:28" s="102" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:28" s="102" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A364" s="1"/>
       <c r="B364" s="33"/>
       <c r="C364" s="76">
@@ -24026,7 +24010,7 @@
       <c r="AA364" s="1"/>
       <c r="AB364" s="1"/>
     </row>
-    <row r="365" spans="1:28" s="130" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:28" s="130" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A365" s="1"/>
       <c r="B365" s="33"/>
       <c r="C365" s="76">
@@ -24079,7 +24063,7 @@
       <c r="AA365" s="1"/>
       <c r="AB365" s="1"/>
     </row>
-    <row r="366" spans="1:28" s="130" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:28" s="130" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A366" s="1"/>
       <c r="B366" s="33"/>
       <c r="C366" s="76">
@@ -24132,7 +24116,7 @@
       <c r="AA366" s="1"/>
       <c r="AB366" s="1"/>
     </row>
-    <row r="367" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A367" s="1"/>
       <c r="B367" s="33"/>
       <c r="C367" s="76"/>
@@ -24162,7 +24146,7 @@
       <c r="AA367" s="1"/>
       <c r="AB367" s="1"/>
     </row>
-    <row r="368" spans="1:28" s="102" customFormat="1" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:28" s="102" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A368" s="1"/>
       <c r="B368" s="33"/>
       <c r="C368" s="76">
@@ -24197,7 +24181,7 @@
       <c r="AA368" s="1"/>
       <c r="AB368" s="1"/>
     </row>
-    <row r="369" spans="1:28" s="142" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:28" s="142" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A369" s="1"/>
       <c r="B369" s="33"/>
       <c r="C369" s="76">
@@ -24230,7 +24214,7 @@
       <c r="AA369" s="1"/>
       <c r="AB369" s="1"/>
     </row>
-    <row r="370" spans="1:28" s="142" customFormat="1" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:28" s="142" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A370" s="1"/>
       <c r="B370" s="35"/>
       <c r="C370" s="79">
@@ -24265,7 +24249,7 @@
       <c r="AA370" s="1"/>
       <c r="AB370" s="1"/>
     </row>
-    <row r="371" spans="1:28" s="142" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:28" s="142" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A371" s="1"/>
       <c r="B371" s="19"/>
       <c r="C371" s="80">
@@ -24298,7 +24282,7 @@
       <c r="AA371" s="1"/>
       <c r="AB371" s="1"/>
     </row>
-    <row r="372" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A372" s="1"/>
       <c r="B372" s="1"/>
       <c r="C372" s="76">
@@ -24331,7 +24315,7 @@
       <c r="AA372" s="1"/>
       <c r="AB372" s="1"/>
     </row>
-    <row r="373" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A373" s="1"/>
       <c r="B373" s="1"/>
       <c r="C373" s="69"/>
@@ -24361,7 +24345,7 @@
       <c r="AA373" s="1"/>
       <c r="AB373" s="1"/>
     </row>
-    <row r="374" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A374" s="1"/>
       <c r="B374" s="1"/>
       <c r="C374" s="69"/>
@@ -24391,7 +24375,7 @@
       <c r="AA374" s="1"/>
       <c r="AB374" s="1"/>
     </row>
-    <row r="375" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A375" s="1"/>
       <c r="B375" s="1"/>
       <c r="C375" s="69"/>
@@ -24421,7 +24405,7 @@
       <c r="AA375" s="1"/>
       <c r="AB375" s="1"/>
     </row>
-    <row r="376" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A376" s="1"/>
       <c r="B376" s="1"/>
       <c r="C376" s="69"/>
@@ -24451,7 +24435,7 @@
       <c r="AA376" s="1"/>
       <c r="AB376" s="1"/>
     </row>
-    <row r="377" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A377" s="1"/>
       <c r="B377" s="1"/>
       <c r="C377" s="69"/>
@@ -24481,7 +24465,7 @@
       <c r="AA377" s="1"/>
       <c r="AB377" s="1"/>
     </row>
-    <row r="378" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A378" s="1"/>
       <c r="B378" s="1"/>
       <c r="C378" s="69"/>
@@ -24511,7 +24495,7 @@
       <c r="AA378" s="1"/>
       <c r="AB378" s="1"/>
     </row>
-    <row r="379" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C379" s="75" t="s">
         <v>4</v>
       </c>
@@ -24646,22 +24630,22 @@
       <selection activeCell="U37" sqref="U37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" customWidth="1"/>
-    <col min="2" max="2" width="2.7265625" customWidth="1"/>
-    <col min="3" max="3" width="4.7265625" customWidth="1" outlineLevel="2"/>
-    <col min="4" max="4" width="1.7265625" customWidth="1"/>
-    <col min="5" max="6" width="9.1796875" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="1.7265625" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="15.7265625" customWidth="1"/>
-    <col min="12" max="12" width="9.1796875" customWidth="1"/>
-    <col min="26" max="26" width="1.7265625" customWidth="1"/>
-    <col min="27" max="28" width="4.7265625" customWidth="1"/>
-    <col min="30" max="30" width="46.1796875" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="4" max="4" width="1.7109375" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="1.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" customWidth="1"/>
+    <col min="26" max="26" width="1.7109375" customWidth="1"/>
+    <col min="27" max="28" width="4.7109375" customWidth="1"/>
+    <col min="30" max="30" width="46.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="69"/>
@@ -24693,7 +24677,7 @@
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
     </row>
-    <row r="2" spans="1:30" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="70">
@@ -24728,7 +24712,7 @@
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
-    <row r="3" spans="1:30" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:30" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="20"/>
       <c r="C3" s="71">
@@ -24763,7 +24747,7 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
     </row>
-    <row r="4" spans="1:30" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="34" t="s">
         <v>21</v>
@@ -24800,7 +24784,7 @@
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
     </row>
-    <row r="5" spans="1:30" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:30" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="33"/>
       <c r="C5" s="70">
@@ -24877,7 +24861,7 @@
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" spans="1:30" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="33"/>
       <c r="C6" s="70">
@@ -24917,7 +24901,7 @@
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
     </row>
-    <row r="7" spans="1:30" ht="20.149999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:30" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="33"/>
       <c r="C7" s="70">
@@ -24958,7 +24942,7 @@
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
     </row>
-    <row r="8" spans="1:30" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="33"/>
       <c r="C8" s="70">
@@ -24993,7 +24977,7 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
     </row>
-    <row r="9" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="33"/>
       <c r="C9" s="70">
@@ -25028,7 +25012,7 @@
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
     </row>
-    <row r="10" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="33"/>
       <c r="C10" s="70">
@@ -25063,7 +25047,7 @@
       <c r="AC10" s="1"/>
       <c r="AD10" s="1"/>
     </row>
-    <row r="11" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="33"/>
       <c r="C11" s="70">
@@ -25098,7 +25082,7 @@
       <c r="AC11" s="1"/>
       <c r="AD11" s="1"/>
     </row>
-    <row r="12" spans="1:30" ht="28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:30" ht="30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="33"/>
       <c r="C12" s="70">
@@ -25137,7 +25121,7 @@
       <c r="AC12" s="1"/>
       <c r="AD12" s="1"/>
     </row>
-    <row r="13" spans="1:30" ht="11.5" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:30" ht="11.45" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="33" t="s">
         <v>20</v>
@@ -25174,7 +25158,7 @@
       <c r="AC13" s="1"/>
       <c r="AD13" s="1"/>
     </row>
-    <row r="14" spans="1:30" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:30" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="33"/>
       <c r="C14" s="70">
@@ -25209,7 +25193,7 @@
       <c r="AC14" s="1"/>
       <c r="AD14" s="1"/>
     </row>
-    <row r="15" spans="1:30" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:30" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="33" t="s">
         <v>19</v>
@@ -25248,7 +25232,7 @@
       <c r="AC15" s="1"/>
       <c r="AD15" s="1"/>
     </row>
-    <row r="16" spans="1:30" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="33"/>
       <c r="C16" s="70">
@@ -25285,7 +25269,7 @@
       <c r="AC16" s="1"/>
       <c r="AD16" s="1"/>
     </row>
-    <row r="17" spans="1:30" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="33"/>
       <c r="C17" s="70">
@@ -25322,7 +25306,7 @@
       <c r="AC17" s="1"/>
       <c r="AD17" s="1"/>
     </row>
-    <row r="18" spans="1:30" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:30" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="33"/>
       <c r="C18" s="70">
@@ -25363,7 +25347,7 @@
       <c r="AC18" s="1"/>
       <c r="AD18" s="1"/>
     </row>
-    <row r="19" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="33"/>
       <c r="C19" s="70">
@@ -25398,7 +25382,7 @@
       <c r="AC19" s="1"/>
       <c r="AD19" s="1"/>
     </row>
-    <row r="20" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="33"/>
       <c r="C20" s="70">
@@ -25433,7 +25417,7 @@
       <c r="AC20" s="1"/>
       <c r="AD20" s="1"/>
     </row>
-    <row r="21" spans="1:30" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:30" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="33"/>
       <c r="C21" s="70">
@@ -25474,7 +25458,7 @@
       <c r="AC21" s="1"/>
       <c r="AD21" s="1"/>
     </row>
-    <row r="22" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="33"/>
       <c r="C22" s="70">
@@ -25509,7 +25493,7 @@
       <c r="AC22" s="1"/>
       <c r="AD22" s="1"/>
     </row>
-    <row r="23" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="33"/>
       <c r="C23" s="70">
@@ -25544,7 +25528,7 @@
       <c r="AC23" s="1"/>
       <c r="AD23" s="1"/>
     </row>
-    <row r="24" spans="1:30" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="33"/>
       <c r="C24" s="70">
@@ -25581,7 +25565,7 @@
       <c r="AC24" s="1"/>
       <c r="AD24" s="1"/>
     </row>
-    <row r="25" spans="1:30" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="33"/>
       <c r="C25" s="70">
@@ -25618,7 +25602,7 @@
       <c r="AC25" s="1"/>
       <c r="AD25" s="1"/>
     </row>
-    <row r="26" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="33"/>
       <c r="C26" s="70">
@@ -25667,7 +25651,7 @@
       <c r="AC26" s="1"/>
       <c r="AD26" s="1"/>
     </row>
-    <row r="27" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="33"/>
       <c r="C27" s="70">
@@ -25706,7 +25690,7 @@
       <c r="AC27" s="1"/>
       <c r="AD27" s="1"/>
     </row>
-    <row r="28" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="33"/>
       <c r="C28" s="70">
@@ -25745,7 +25729,7 @@
       <c r="AC28" s="1"/>
       <c r="AD28" s="1"/>
     </row>
-    <row r="29" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="33"/>
       <c r="C29" s="70">
@@ -25784,7 +25768,7 @@
       <c r="AC29" s="1"/>
       <c r="AD29" s="1"/>
     </row>
-    <row r="30" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="33"/>
       <c r="C30" s="70">
@@ -25823,7 +25807,7 @@
       <c r="AC30" s="1"/>
       <c r="AD30" s="1"/>
     </row>
-    <row r="31" spans="1:30" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="33"/>
       <c r="C31" s="70">
@@ -25860,7 +25844,7 @@
       <c r="AC31" s="1"/>
       <c r="AD31" s="1"/>
     </row>
-    <row r="32" spans="1:30" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="33"/>
       <c r="C32" s="70">
@@ -25897,7 +25881,7 @@
       <c r="AC32" s="1"/>
       <c r="AD32" s="1"/>
     </row>
-    <row r="33" spans="1:30" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:30" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="33"/>
       <c r="C33" s="70">
@@ -25958,7 +25942,7 @@
       <c r="AC33" s="1"/>
       <c r="AD33" s="1"/>
     </row>
-    <row r="34" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="33"/>
       <c r="C34" s="70">
@@ -26023,7 +26007,7 @@
       <c r="AC34" s="1"/>
       <c r="AD34" s="1"/>
     </row>
-    <row r="35" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="33"/>
       <c r="C35" s="70">
@@ -26058,7 +26042,7 @@
       <c r="AC35" s="1"/>
       <c r="AD35" s="1"/>
     </row>
-    <row r="36" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="33"/>
       <c r="C36" s="70">
@@ -26093,7 +26077,7 @@
       <c r="AC36" s="1"/>
       <c r="AD36" s="1"/>
     </row>
-    <row r="37" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="33"/>
       <c r="C37" s="70">
@@ -26128,7 +26112,7 @@
       <c r="AC37" s="1"/>
       <c r="AD37" s="1"/>
     </row>
-    <row r="38" spans="1:30" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="33"/>
       <c r="C38" s="70">
@@ -26165,7 +26149,7 @@
       <c r="AC38" s="1"/>
       <c r="AD38" s="1"/>
     </row>
-    <row r="39" spans="1:30" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="33"/>
       <c r="C39" s="70">
@@ -26200,7 +26184,7 @@
       <c r="AC39" s="1"/>
       <c r="AD39" s="1"/>
     </row>
-    <row r="40" spans="1:30" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="35"/>
       <c r="C40" s="73">
@@ -26237,7 +26221,7 @@
       <c r="AC40" s="1"/>
       <c r="AD40" s="1"/>
     </row>
-    <row r="41" spans="1:30" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:30" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="19"/>
       <c r="C41" s="74">
@@ -26272,7 +26256,7 @@
       <c r="AC41" s="1"/>
       <c r="AD41" s="1"/>
     </row>
-    <row r="42" spans="1:30" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="70">
@@ -26307,7 +26291,7 @@
       <c r="AC42" s="1"/>
       <c r="AD42" s="1"/>
     </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="69"/>
@@ -26339,7 +26323,7 @@
       <c r="AC43" s="1"/>
       <c r="AD43" s="1"/>
     </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="69"/>
@@ -26371,7 +26355,7 @@
       <c r="AC44" s="1"/>
       <c r="AD44" s="1"/>
     </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="69"/>
@@ -26403,7 +26387,7 @@
       <c r="AC45" s="1"/>
       <c r="AD45" s="1"/>
     </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="69"/>
@@ -26435,7 +26419,7 @@
       <c r="AC46" s="1"/>
       <c r="AD46" s="1"/>
     </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="69"/>
@@ -26467,7 +26451,7 @@
       <c r="AC47" s="1"/>
       <c r="AD47" s="1"/>
     </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="69"/>
@@ -26499,7 +26483,7 @@
       <c r="AC48" s="1"/>
       <c r="AD48" s="1"/>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C49" s="75" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
few mods to reduce memory of param keys.
</commit_message>
<xml_diff>
--- a/Structural.xlsx
+++ b/Structural.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC8D2B4-8F1B-4C40-9B7A-A91DA7F6E9BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C8E2AF-A616-4EC6-BEBC-DECA72AA4C21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="30150" yWindow="450" windowWidth="24675" windowHeight="12840" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -55,7 +55,7 @@
     <definedName name="i_d_pos">Stock!$I$56</definedName>
     <definedName name="i_date_assetvalue" localSheetId="0">General!$I$67</definedName>
     <definedName name="i_density_n0">Stock!$K$328</definedName>
-    <definedName name="i_density_n1">Stock!$M$328:$M$329</definedName>
+    <definedName name="i_density_n1">Stock!$M$328:$M$330</definedName>
     <definedName name="i_density_n3">Stock!$Q$328:$Q$330</definedName>
     <definedName name="i_dvp_mask_f1">Stock!$J$343:$O$343</definedName>
     <definedName name="i_dvp_mask_f3">Stock!$J$355:$M$355</definedName>
@@ -105,7 +105,7 @@
     <definedName name="i_n3_matrix_len">Stock!$P$326</definedName>
     <definedName name="i_numbers_min_b1">Stock!$L$163:$V$163</definedName>
     <definedName name="i_nut_spread_n0">Stock!$J$328</definedName>
-    <definedName name="i_nut_spread_n1">Stock!$L$328:$L$329</definedName>
+    <definedName name="i_nut_spread_n1">Stock!$L$328:$L$330</definedName>
     <definedName name="i_nut_spread_n3">Stock!$P$328:$P$330</definedName>
     <definedName name="i_p_pos">Stock!$I$64</definedName>
     <definedName name="i_prejoin_offset">Stock!$I$74</definedName>
@@ -1905,18 +1905,6 @@
     <t>sheep pools</t>
   </si>
   <si>
-    <t>pool0</t>
-  </si>
-  <si>
-    <t>pool1</t>
-  </si>
-  <si>
-    <t>pool2</t>
-  </si>
-  <si>
-    <t>pool3</t>
-  </si>
-  <si>
     <t>FVP0</t>
   </si>
   <si>
@@ -2026,6 +2014,18 @@
   </si>
   <si>
     <t>R2</t>
+  </si>
+  <si>
+    <t>ev0</t>
+  </si>
+  <si>
+    <t>ev1</t>
+  </si>
+  <si>
+    <t>ev2</t>
+  </si>
+  <si>
+    <t>ev3</t>
   </si>
 </sst>
 </file>
@@ -4186,8 +4186,8 @@
   </sheetPr>
   <dimension ref="A1:AT83"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="L63" sqref="L63"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="I61" sqref="I61:L61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.35"/>
@@ -6354,16 +6354,16 @@
         <v>250</v>
       </c>
       <c r="I61" s="108" t="s">
-        <v>251</v>
+        <v>288</v>
       </c>
       <c r="J61" s="108" t="s">
-        <v>252</v>
+        <v>289</v>
       </c>
       <c r="K61" s="108" t="s">
-        <v>253</v>
+        <v>290</v>
       </c>
       <c r="L61" s="108" t="s">
-        <v>254</v>
+        <v>291</v>
       </c>
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
@@ -7157,8 +7157,8 @@
   </sheetPr>
   <dimension ref="A1:AE379"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A319" workbookViewId="0">
-      <selection activeCell="O344" sqref="O344"/>
+    <sheetView tabSelected="1" topLeftCell="A336" workbookViewId="0">
+      <selection activeCell="M343" sqref="M343:N343"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.35"/>
@@ -16307,7 +16307,7 @@
         <v>134</v>
       </c>
       <c r="I213" s="55" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="J213" s="55" t="s">
         <v>116</v>
@@ -22146,7 +22146,7 @@
       <c r="K320" s="2"/>
       <c r="L320" s="132">
         <f>i_w_start_len1*i_n1_len^L323</f>
-        <v>24</v>
+        <v>243</v>
       </c>
       <c r="M320" s="2"/>
       <c r="N320" s="127" t="s">
@@ -22231,7 +22231,7 @@
       </c>
       <c r="K322" s="126"/>
       <c r="L322" s="31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M322" s="126"/>
       <c r="N322" s="2"/>
@@ -22270,7 +22270,7 @@
       <c r="K323" s="2"/>
       <c r="L323" s="132">
         <f>COUNTIF(J341:O341,TRUE)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M323" s="2"/>
       <c r="N323" s="2"/>
@@ -22435,13 +22435,13 @@
       <c r="H327" s="2"/>
       <c r="I327" s="56"/>
       <c r="J327" s="2" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="K327" s="2" t="s">
         <v>115</v>
       </c>
       <c r="L327" s="2" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="M327" s="2" t="s">
         <v>115</v>
@@ -22449,7 +22449,7 @@
       <c r="N327" s="2"/>
       <c r="O327" s="2"/>
       <c r="P327" s="2" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="Q327" s="2" t="s">
         <v>115</v>
@@ -22584,10 +22584,10 @@
       </c>
       <c r="J330" s="54"/>
       <c r="K330" s="54"/>
-      <c r="L330" s="54">
+      <c r="L330" s="31">
         <v>-1</v>
       </c>
-      <c r="M330" s="54">
+      <c r="M330" s="31">
         <v>1.5</v>
       </c>
       <c r="N330" s="2"/>
@@ -22909,7 +22909,7 @@
       <c r="F338" s="5"/>
       <c r="G338" s="4"/>
       <c r="H338" s="107" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="I338" s="2"/>
       <c r="J338" s="2"/>
@@ -22946,22 +22946,22 @@
       <c r="H339" s="2"/>
       <c r="I339" s="2"/>
       <c r="J339" s="2" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="K339" s="2" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="L339" s="2" t="s">
         <v>101</v>
       </c>
       <c r="M339" s="2" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="N339" s="2" t="s">
         <v>102</v>
       </c>
       <c r="O339" s="2" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="P339" s="2"/>
       <c r="Q339" s="2"/>
@@ -22991,26 +22991,26 @@
       <c r="H340" s="2"/>
       <c r="I340" s="2"/>
       <c r="J340" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="K340" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="L340" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="M340" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="N340" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="K340" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="L340" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="M340" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="N340" s="2" t="s">
-        <v>259</v>
-      </c>
       <c r="O340" s="2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="P340" s="2"/>
       <c r="Q340" s="2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="R340" s="2"/>
       <c r="S340" s="2"/>
@@ -23036,10 +23036,10 @@
       <c r="F341" s="5"/>
       <c r="G341" s="4"/>
       <c r="H341" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="I341" s="2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="J341" s="31" t="b">
         <v>0</v>
@@ -23054,7 +23054,7 @@
         <v>1</v>
       </c>
       <c r="N341" s="31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O341" s="31" t="b">
         <v>0</v>
@@ -23085,7 +23085,7 @@
       <c r="F342" s="5"/>
       <c r="G342" s="4"/>
       <c r="H342" s="2" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="I342" s="2"/>
       <c r="J342" s="132">
@@ -23106,11 +23106,11 @@
       </c>
       <c r="N342" s="132">
         <f>COUNTIF($J$341:N341,TRUE)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O342" s="132">
         <f>COUNTIF($J$341:O341,TRUE)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P342" s="2"/>
       <c r="Q342" s="2"/>
@@ -23138,10 +23138,10 @@
       <c r="F343" s="5"/>
       <c r="G343" s="4"/>
       <c r="H343" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="I343" s="2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="J343" s="31" t="b">
         <v>0</v>
@@ -23156,7 +23156,7 @@
         <v>1</v>
       </c>
       <c r="N343" s="31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O343" s="31" t="b">
         <v>0</v>
@@ -23184,7 +23184,7 @@
       <c r="F344" s="5"/>
       <c r="G344" s="4"/>
       <c r="H344" s="2" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="I344" s="2"/>
       <c r="J344" s="31" t="b">
@@ -23231,10 +23231,10 @@
       <c r="F345" s="5"/>
       <c r="G345" s="4"/>
       <c r="H345" s="2" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="I345" s="2" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="J345" s="2"/>
       <c r="K345" s="2"/>
@@ -23244,9 +23244,7 @@
       <c r="O345" s="166">
         <v>43784</v>
       </c>
-      <c r="P345" s="189">
-        <v>43784</v>
-      </c>
+      <c r="P345" s="189"/>
       <c r="Q345" s="2"/>
       <c r="R345" s="2"/>
       <c r="S345" s="2"/>
@@ -23275,7 +23273,7 @@
       <c r="G346" s="4"/>
       <c r="H346" s="2"/>
       <c r="I346" s="2" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="J346" s="2"/>
       <c r="K346" s="2"/>
@@ -23283,11 +23281,9 @@
       <c r="M346" s="2"/>
       <c r="N346" s="2"/>
       <c r="O346" s="166">
-        <v>43818</v>
-      </c>
-      <c r="P346" s="189">
         <v>43480</v>
       </c>
+      <c r="P346" s="189"/>
       <c r="Q346" s="2"/>
       <c r="R346" s="2"/>
       <c r="S346" s="2"/>
@@ -23317,13 +23313,13 @@
       <c r="H347" s="2"/>
       <c r="I347" s="171"/>
       <c r="J347" s="172" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="K347" s="172" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="L347" s="172" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="M347" s="2"/>
       <c r="N347" s="2"/>
@@ -23351,7 +23347,7 @@
       <c r="F348" s="5"/>
       <c r="G348" s="4"/>
       <c r="H348" s="2" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="I348" s="171"/>
       <c r="J348" s="31">
@@ -23425,7 +23421,7 @@
       <c r="F350" s="5"/>
       <c r="G350" s="4"/>
       <c r="H350" s="107" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="I350" s="2"/>
       <c r="J350" s="2"/>
@@ -23462,16 +23458,16 @@
       <c r="H351" s="2"/>
       <c r="I351" s="2"/>
       <c r="J351" s="2" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="K351" s="2" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="L351" s="2" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="M351" s="2" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="N351" s="2"/>
       <c r="O351" s="2"/>
@@ -23503,22 +23499,22 @@
       <c r="H352" s="2"/>
       <c r="I352" s="2"/>
       <c r="J352" s="2" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="K352" s="2" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="L352" s="2" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="M352" s="2" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="N352" s="2"/>
       <c r="O352" s="2"/>
       <c r="P352" s="2"/>
       <c r="Q352" s="2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="R352" s="2"/>
       <c r="S352" s="2"/>
@@ -23544,10 +23540,10 @@
       <c r="F353" s="5"/>
       <c r="G353" s="4"/>
       <c r="H353" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="I353" s="2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="J353" s="31" t="b">
         <v>0</v>
@@ -23589,7 +23585,7 @@
       <c r="F354" s="5"/>
       <c r="G354" s="4"/>
       <c r="H354" s="2" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="I354" s="2"/>
       <c r="J354" s="132">
@@ -23636,10 +23632,10 @@
       <c r="F355" s="5"/>
       <c r="G355" s="4"/>
       <c r="H355" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="I355" s="2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="J355" s="31" t="b">
         <v>0</v>
@@ -23929,42 +23925,42 @@
       <c r="H363" s="2"/>
       <c r="I363" s="149"/>
       <c r="J363" s="107" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="K363" s="107" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="L363" s="107" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="M363" s="107" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="N363" s="2"/>
       <c r="O363" s="107" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="P363" s="107" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="Q363" s="107" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="R363" s="107" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="S363" s="2"/>
       <c r="T363" s="107" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="U363" s="107" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="V363" s="107" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="W363" s="107" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="X363" s="4"/>
       <c r="Y363" s="16"/>
@@ -23986,7 +23982,7 @@
       <c r="F364" s="5"/>
       <c r="G364" s="4"/>
       <c r="H364" s="61" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="I364" s="149"/>
       <c r="J364" s="162">
@@ -24047,7 +24043,7 @@
       <c r="F365" s="5"/>
       <c r="G365" s="4"/>
       <c r="H365" s="61" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="I365" s="149"/>
       <c r="J365" s="149"/>
@@ -24100,7 +24096,7 @@
       <c r="F366" s="5"/>
       <c r="G366" s="4"/>
       <c r="H366" s="61" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="I366" s="149"/>
       <c r="J366" s="149"/>

</xml_diff>

<commit_message>
make xl param name changes again (lost when i merged with master)
</commit_message>
<xml_diff>
--- a/Structural.xlsx
+++ b/Structural.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9009EBE-3316-4969-85AD-3B4E47FE101C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A2AA69-6822-4750-A892-1A4AE9B63071}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="225" yWindow="240" windowWidth="28305" windowHeight="14595" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -1902,18 +1902,6 @@
     <t>sheep pools</t>
   </si>
   <si>
-    <t>pool0</t>
-  </si>
-  <si>
-    <t>pool1</t>
-  </si>
-  <si>
-    <t>pool2</t>
-  </si>
-  <si>
-    <t>pool3</t>
-  </si>
-  <si>
     <t>FVP0</t>
   </si>
   <si>
@@ -2023,6 +2011,18 @@
   </si>
   <si>
     <t>R2</t>
+  </si>
+  <si>
+    <t>ev0</t>
+  </si>
+  <si>
+    <t>ev1</t>
+  </si>
+  <si>
+    <t>ev2</t>
+  </si>
+  <si>
+    <t>ev3</t>
   </si>
 </sst>
 </file>
@@ -4167,8 +4167,8 @@
   </sheetPr>
   <dimension ref="A1:AT83"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="L63" sqref="L63"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="I61" sqref="I61:L61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -6335,16 +6335,16 @@
         <v>250</v>
       </c>
       <c r="I61" s="108" t="s">
-        <v>251</v>
+        <v>288</v>
       </c>
       <c r="J61" s="108" t="s">
-        <v>252</v>
+        <v>289</v>
       </c>
       <c r="K61" s="108" t="s">
-        <v>253</v>
+        <v>290</v>
       </c>
       <c r="L61" s="108" t="s">
-        <v>254</v>
+        <v>291</v>
       </c>
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
@@ -7138,7 +7138,7 @@
   </sheetPr>
   <dimension ref="A1:AE379"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A311" workbookViewId="0">
+    <sheetView topLeftCell="A323" workbookViewId="0">
       <selection activeCell="Q341" sqref="Q341"/>
     </sheetView>
   </sheetViews>
@@ -16288,7 +16288,7 @@
         <v>134</v>
       </c>
       <c r="I213" s="55" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="J213" s="55" t="s">
         <v>116</v>
@@ -22416,13 +22416,13 @@
       <c r="H327" s="2"/>
       <c r="I327" s="56"/>
       <c r="J327" s="2" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="K327" s="2" t="s">
         <v>115</v>
       </c>
       <c r="L327" s="2" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="M327" s="2" t="s">
         <v>115</v>
@@ -22430,7 +22430,7 @@
       <c r="N327" s="2"/>
       <c r="O327" s="2"/>
       <c r="P327" s="2" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="Q327" s="2" t="s">
         <v>115</v>
@@ -22890,7 +22890,7 @@
       <c r="F338" s="5"/>
       <c r="G338" s="4"/>
       <c r="H338" s="107" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="I338" s="2"/>
       <c r="J338" s="2"/>
@@ -22927,22 +22927,22 @@
       <c r="H339" s="2"/>
       <c r="I339" s="2"/>
       <c r="J339" s="2" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="K339" s="2" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="L339" s="2" t="s">
         <v>101</v>
       </c>
       <c r="M339" s="2" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="N339" s="2" t="s">
         <v>102</v>
       </c>
       <c r="O339" s="2" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="P339" s="2"/>
       <c r="Q339" s="2"/>
@@ -22972,26 +22972,26 @@
       <c r="H340" s="2"/>
       <c r="I340" s="2"/>
       <c r="J340" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="K340" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="L340" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="M340" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="N340" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="K340" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="L340" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="M340" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="N340" s="2" t="s">
-        <v>259</v>
-      </c>
       <c r="O340" s="2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="P340" s="2"/>
       <c r="Q340" s="2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="R340" s="2"/>
       <c r="S340" s="2"/>
@@ -23017,10 +23017,10 @@
       <c r="F341" s="5"/>
       <c r="G341" s="4"/>
       <c r="H341" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="I341" s="2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="J341" s="31" t="b">
         <v>0</v>
@@ -23066,7 +23066,7 @@
       <c r="F342" s="5"/>
       <c r="G342" s="4"/>
       <c r="H342" s="2" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="I342" s="2"/>
       <c r="J342" s="132">
@@ -23119,10 +23119,10 @@
       <c r="F343" s="5"/>
       <c r="G343" s="4"/>
       <c r="H343" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="I343" s="2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="J343" s="31" t="b">
         <v>0</v>
@@ -23165,7 +23165,7 @@
       <c r="F344" s="5"/>
       <c r="G344" s="4"/>
       <c r="H344" s="2" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="I344" s="2"/>
       <c r="J344" s="31" t="b">
@@ -23212,10 +23212,10 @@
       <c r="F345" s="5"/>
       <c r="G345" s="4"/>
       <c r="H345" s="2" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="I345" s="2" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="J345" s="2"/>
       <c r="K345" s="2"/>
@@ -23254,7 +23254,7 @@
       <c r="G346" s="4"/>
       <c r="H346" s="2"/>
       <c r="I346" s="2" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="J346" s="2"/>
       <c r="K346" s="2"/>
@@ -23294,13 +23294,13 @@
       <c r="H347" s="2"/>
       <c r="I347" s="171"/>
       <c r="J347" s="172" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="K347" s="172" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="L347" s="172" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="M347" s="2"/>
       <c r="N347" s="2"/>
@@ -23328,7 +23328,7 @@
       <c r="F348" s="5"/>
       <c r="G348" s="4"/>
       <c r="H348" s="2" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="I348" s="171"/>
       <c r="J348" s="31">
@@ -23402,7 +23402,7 @@
       <c r="F350" s="5"/>
       <c r="G350" s="4"/>
       <c r="H350" s="107" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="I350" s="2"/>
       <c r="J350" s="2"/>
@@ -23439,16 +23439,16 @@
       <c r="H351" s="2"/>
       <c r="I351" s="2"/>
       <c r="J351" s="2" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="K351" s="2" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="L351" s="2" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="M351" s="2" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="N351" s="2"/>
       <c r="O351" s="2"/>
@@ -23480,22 +23480,22 @@
       <c r="H352" s="2"/>
       <c r="I352" s="2"/>
       <c r="J352" s="2" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="K352" s="2" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="L352" s="2" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="M352" s="2" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="N352" s="2"/>
       <c r="O352" s="2"/>
       <c r="P352" s="2"/>
       <c r="Q352" s="2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="R352" s="2"/>
       <c r="S352" s="2"/>
@@ -23521,10 +23521,10 @@
       <c r="F353" s="5"/>
       <c r="G353" s="4"/>
       <c r="H353" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="I353" s="2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="J353" s="31" t="b">
         <v>0</v>
@@ -23566,7 +23566,7 @@
       <c r="F354" s="5"/>
       <c r="G354" s="4"/>
       <c r="H354" s="2" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="I354" s="2"/>
       <c r="J354" s="132">
@@ -23613,10 +23613,10 @@
       <c r="F355" s="5"/>
       <c r="G355" s="4"/>
       <c r="H355" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="I355" s="2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="J355" s="31" t="b">
         <v>0</v>
@@ -23906,42 +23906,42 @@
       <c r="H363" s="2"/>
       <c r="I363" s="149"/>
       <c r="J363" s="107" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="K363" s="107" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="L363" s="107" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="M363" s="107" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="N363" s="2"/>
       <c r="O363" s="107" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="P363" s="107" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="Q363" s="107" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="R363" s="107" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="S363" s="2"/>
       <c r="T363" s="107" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="U363" s="107" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="V363" s="107" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="W363" s="107" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="X363" s="4"/>
       <c r="Y363" s="16"/>
@@ -23963,7 +23963,7 @@
       <c r="F364" s="5"/>
       <c r="G364" s="4"/>
       <c r="H364" s="61" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="I364" s="149"/>
       <c r="J364" s="162">
@@ -24024,7 +24024,7 @@
       <c r="F365" s="5"/>
       <c r="G365" s="4"/>
       <c r="H365" s="61" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="I365" s="149"/>
       <c r="J365" s="149"/>
@@ -24077,7 +24077,7 @@
       <c r="F366" s="5"/>
       <c r="G366" s="4"/>
       <c r="H366" s="61" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="I366" s="149"/>
       <c r="J366" s="149"/>

</xml_diff>

<commit_message>
un important xl changes
</commit_message>
<xml_diff>
--- a/Structural.xlsx
+++ b/Structural.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A2AA69-6822-4750-A892-1A4AE9B63071}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7FED8A1-3120-4969-8A8F-3CF5A6A6407E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -4167,7 +4167,7 @@
   </sheetPr>
   <dimension ref="A1:AT83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="I61" sqref="I61:L61"/>
     </sheetView>
   </sheetViews>
@@ -7138,8 +7138,8 @@
   </sheetPr>
   <dimension ref="A1:AE379"/>
   <sheetViews>
-    <sheetView topLeftCell="A323" workbookViewId="0">
-      <selection activeCell="Q341" sqref="Q341"/>
+    <sheetView tabSelected="1" topLeftCell="A323" workbookViewId="0">
+      <selection activeCell="O341" sqref="N341:O341"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -22127,7 +22127,7 @@
       <c r="K320" s="2"/>
       <c r="L320" s="132">
         <f>i_w_start_len1*i_n1_len^L323</f>
-        <v>243</v>
+        <v>81</v>
       </c>
       <c r="M320" s="2"/>
       <c r="N320" s="127" t="s">
@@ -22251,7 +22251,7 @@
       <c r="K323" s="2"/>
       <c r="L323" s="132">
         <f>COUNTIF(J341:O341,TRUE)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M323" s="2"/>
       <c r="N323" s="2"/>
@@ -23035,7 +23035,7 @@
         <v>1</v>
       </c>
       <c r="N341" s="31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O341" s="31" t="b">
         <v>0</v>
@@ -23087,11 +23087,11 @@
       </c>
       <c r="N342" s="132">
         <f>COUNTIF($J$341:N341,TRUE)-1</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O342" s="132">
         <f>COUNTIF($J$341:O341,TRUE)-1</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P342" s="2"/>
       <c r="Q342" s="2"/>

</xml_diff>

<commit_message>
tidy lw dist stuff and comment change to structure.xl
</commit_message>
<xml_diff>
--- a/Structural.xlsx
+++ b/Structural.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3BBF6A-521B-46DF-A619-A42367226690}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2371F758-829D-4EDF-B2BF-E47173A73BB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -899,7 +899,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-fvp type when LW is condensed back to the starting number (eg 3). This fvp must also be a dvp. Typically this is prejoining.</t>
+fvp type when LW is condensed back to the starting number (eg 3). This fvp must also be a dvp. Currently this must be prejoining (lw_dist doesn’t handle them to be different).</t>
         </r>
       </text>
     </comment>
@@ -7139,7 +7139,7 @@
   <dimension ref="A1:AE379"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A326" workbookViewId="0">
-      <selection activeCell="O341" sqref="N341:O341"/>
+      <selection activeCell="R349" sqref="R349"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.35"/>
@@ -22127,7 +22127,7 @@
       <c r="K320" s="2"/>
       <c r="L320" s="132">
         <f>i_w_start_len1*i_n1_len^L323</f>
-        <v>81</v>
+        <v>243</v>
       </c>
       <c r="M320" s="2"/>
       <c r="N320" s="127" t="s">
@@ -22251,7 +22251,7 @@
       <c r="K323" s="2"/>
       <c r="L323" s="132">
         <f>COUNTIF(J341:O341,TRUE)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M323" s="2"/>
       <c r="N323" s="2"/>
@@ -23035,7 +23035,7 @@
         <v>1</v>
       </c>
       <c r="N341" s="31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O341" s="31" t="b">
         <v>0</v>
@@ -23087,11 +23087,11 @@
       </c>
       <c r="N342" s="132">
         <f>COUNTIF($J$341:N341,TRUE)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O342" s="132">
         <f>COUNTIF($J$341:O341,TRUE)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P342" s="2"/>
       <c r="Q342" s="2"/>

</xml_diff>

<commit_message>
fix stubble error. and comment change in Structural.xlsx
</commit_message>
<xml_diff>
--- a/Structural.xlsx
+++ b/Structural.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Michael\Work\AFO - local\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2371F758-829D-4EDF-B2BF-E47173A73BB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA57DD8-866E-4F62-8D78-43FE5C34F4FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -899,7 +899,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-fvp type when LW is condensed back to the starting number (eg 3). This fvp must also be a dvp. Currently this must be prejoining (lw_dist doesn’t handle them to be different).</t>
+fvp type when LW is condensed back to the starting number (eg 3). This fvp must also be a dvp. ATM this must be equal to prejoining (if you want to change this lw_distribution will need modification)</t>
         </r>
       </text>
     </comment>
@@ -4171,25 +4171,25 @@
       <selection activeCell="I61" sqref="I61:L61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" style="155" customWidth="1"/>
-    <col min="2" max="2" width="2.7265625" style="155" customWidth="1"/>
-    <col min="3" max="3" width="4.7265625" style="155" customWidth="1" outlineLevel="2"/>
-    <col min="4" max="4" width="1.7265625" style="155" customWidth="1"/>
-    <col min="5" max="6" width="9.7265625" style="155" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="1.7265625" style="155" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="37.26953125" style="155" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7265625" style="155" customWidth="1"/>
-    <col min="10" max="23" width="10.81640625" style="155" customWidth="1"/>
-    <col min="24" max="24" width="1.7265625" style="155" customWidth="1"/>
-    <col min="25" max="26" width="4.7265625" style="155" customWidth="1"/>
-    <col min="27" max="27" width="8.7265625" style="155"/>
-    <col min="28" max="28" width="46.1796875" style="155" customWidth="1"/>
-    <col min="29" max="16384" width="8.7265625" style="155"/>
+    <col min="1" max="1" width="4.6640625" style="155" customWidth="1"/>
+    <col min="2" max="2" width="2.6640625" style="155" customWidth="1"/>
+    <col min="3" max="3" width="4.6640625" style="155" customWidth="1" outlineLevel="2"/>
+    <col min="4" max="4" width="1.6640625" style="155" customWidth="1"/>
+    <col min="5" max="6" width="9.6640625" style="155" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="1.6640625" style="155" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="37.33203125" style="155" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" style="155" customWidth="1"/>
+    <col min="10" max="23" width="10.88671875" style="155" customWidth="1"/>
+    <col min="24" max="24" width="1.6640625" style="155" customWidth="1"/>
+    <col min="25" max="26" width="4.6640625" style="155" customWidth="1"/>
+    <col min="27" max="27" width="8.6640625" style="155"/>
+    <col min="28" max="28" width="46.109375" style="155" customWidth="1"/>
+    <col min="29" max="16384" width="8.6640625" style="155"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="69"/>
@@ -4219,7 +4219,7 @@
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
     </row>
-    <row r="2" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="70">
@@ -4252,7 +4252,7 @@
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
     </row>
-    <row r="3" spans="1:28" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:28" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="20"/>
       <c r="C3" s="71">
@@ -4285,7 +4285,7 @@
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
     </row>
-    <row r="4" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="34" t="s">
         <v>21</v>
@@ -4320,7 +4320,7 @@
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
     </row>
-    <row r="5" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="33"/>
       <c r="C5" s="70">
@@ -4391,7 +4391,7 @@
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
     </row>
-    <row r="6" spans="1:28" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="33"/>
       <c r="C6" s="70">
@@ -4429,7 +4429,7 @@
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
     </row>
-    <row r="7" spans="1:28" ht="20.149999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="33"/>
       <c r="C7" s="70">
@@ -4468,7 +4468,7 @@
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
     </row>
-    <row r="8" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="33"/>
       <c r="C8" s="70">
@@ -4501,7 +4501,7 @@
       <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
     </row>
-    <row r="9" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="33"/>
       <c r="C9" s="70">
@@ -4534,7 +4534,7 @@
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
     </row>
-    <row r="10" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="33"/>
       <c r="C10" s="70">
@@ -4567,7 +4567,7 @@
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
     </row>
-    <row r="11" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="33"/>
       <c r="C11" s="70">
@@ -4600,7 +4600,7 @@
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
     </row>
-    <row r="12" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="33"/>
       <c r="C12" s="70">
@@ -4637,7 +4637,7 @@
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
     </row>
-    <row r="13" spans="1:28" ht="11.5" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:28" ht="11.4" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="33" t="s">
         <v>20</v>
@@ -4672,7 +4672,7 @@
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
     </row>
-    <row r="14" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="33"/>
       <c r="C14" s="70">
@@ -4705,7 +4705,7 @@
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
     </row>
-    <row r="15" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="33"/>
       <c r="C15" s="70">
@@ -4738,7 +4738,7 @@
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
     </row>
-    <row r="16" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="33" t="s">
         <v>19</v>
@@ -4775,7 +4775,7 @@
       <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>
     </row>
-    <row r="17" spans="1:28" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:28" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="33"/>
       <c r="C17" s="70">
@@ -4810,7 +4810,7 @@
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
     </row>
-    <row r="18" spans="1:28" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:28" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="33"/>
       <c r="C18" s="70">
@@ -4849,7 +4849,7 @@
       <c r="AA18" s="1"/>
       <c r="AB18" s="1"/>
     </row>
-    <row r="19" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="33"/>
       <c r="C19" s="70">
@@ -4882,7 +4882,7 @@
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
     </row>
-    <row r="20" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="33"/>
       <c r="C20" s="70">
@@ -4915,7 +4915,7 @@
       <c r="AA20" s="1"/>
       <c r="AB20" s="1"/>
     </row>
-    <row r="21" spans="1:28" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:28" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="33"/>
       <c r="C21" s="70">
@@ -4954,7 +4954,7 @@
       <c r="AA21" s="1"/>
       <c r="AB21" s="1"/>
     </row>
-    <row r="22" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="33"/>
       <c r="C22" s="70">
@@ -4987,7 +4987,7 @@
       <c r="AA22" s="1"/>
       <c r="AB22" s="1"/>
     </row>
-    <row r="23" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="33"/>
       <c r="C23" s="70">
@@ -5020,7 +5020,7 @@
       <c r="AA23" s="1"/>
       <c r="AB23" s="1"/>
     </row>
-    <row r="24" spans="1:28" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="33"/>
       <c r="C24" s="70">
@@ -5055,7 +5055,7 @@
       <c r="AA24" s="1"/>
       <c r="AB24" s="1"/>
     </row>
-    <row r="25" spans="1:28" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="33"/>
       <c r="C25" s="70">
@@ -5090,7 +5090,7 @@
       <c r="AA25" s="1"/>
       <c r="AB25" s="1"/>
     </row>
-    <row r="26" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="33"/>
       <c r="C26" s="70">
@@ -5137,7 +5137,7 @@
       <c r="AA26" s="1"/>
       <c r="AB26" s="1"/>
     </row>
-    <row r="27" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="33"/>
       <c r="C27" s="70">
@@ -5174,7 +5174,7 @@
       <c r="AA27" s="1"/>
       <c r="AB27" s="1"/>
     </row>
-    <row r="28" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="33"/>
       <c r="C28" s="70">
@@ -5211,7 +5211,7 @@
       <c r="AA28" s="1"/>
       <c r="AB28" s="1"/>
     </row>
-    <row r="29" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="33"/>
       <c r="C29" s="70">
@@ -5248,7 +5248,7 @@
       <c r="AA29" s="1"/>
       <c r="AB29" s="1"/>
     </row>
-    <row r="30" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="33"/>
       <c r="C30" s="70">
@@ -5285,7 +5285,7 @@
       <c r="AA30" s="1"/>
       <c r="AB30" s="1"/>
     </row>
-    <row r="31" spans="1:28" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="33"/>
       <c r="C31" s="70">
@@ -5320,7 +5320,7 @@
       <c r="AA31" s="1"/>
       <c r="AB31" s="1"/>
     </row>
-    <row r="32" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="33"/>
       <c r="C32" s="70">
@@ -5353,7 +5353,7 @@
       <c r="AA32" s="1"/>
       <c r="AB32" s="1"/>
     </row>
-    <row r="33" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="35"/>
       <c r="C33" s="73">
@@ -5388,7 +5388,7 @@
       <c r="AA33" s="1"/>
       <c r="AB33" s="1"/>
     </row>
-    <row r="34" spans="1:28" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:28" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="19"/>
       <c r="C34" s="74">
@@ -5421,7 +5421,7 @@
       <c r="AA34" s="1"/>
       <c r="AB34" s="1"/>
     </row>
-    <row r="35" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="70">
@@ -5454,7 +5454,7 @@
       <c r="AA35" s="1"/>
       <c r="AB35" s="1"/>
     </row>
-    <row r="36" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="76">
@@ -5487,7 +5487,7 @@
       <c r="AA36" s="1"/>
       <c r="AB36" s="1"/>
     </row>
-    <row r="37" spans="1:28" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:28" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
       <c r="B37" s="20"/>
       <c r="C37" s="77">
@@ -5520,7 +5520,7 @@
       <c r="AA37" s="1"/>
       <c r="AB37" s="1"/>
     </row>
-    <row r="38" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="34" t="s">
         <v>21</v>
@@ -5555,7 +5555,7 @@
       <c r="AA38" s="1"/>
       <c r="AB38" s="1"/>
     </row>
-    <row r="39" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="33"/>
       <c r="C39" s="76">
@@ -5588,7 +5588,7 @@
       <c r="AA39" s="1"/>
       <c r="AB39" s="1"/>
     </row>
-    <row r="40" spans="1:28" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="33"/>
       <c r="C40" s="76">
@@ -5625,7 +5625,7 @@
       <c r="AA40" s="1"/>
       <c r="AB40" s="1"/>
     </row>
-    <row r="41" spans="1:28" ht="20.149999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:28" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="33"/>
       <c r="C41" s="76">
@@ -5664,7 +5664,7 @@
       <c r="AA41" s="1"/>
       <c r="AB41" s="1"/>
     </row>
-    <row r="42" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="33"/>
       <c r="C42" s="76">
@@ -5697,7 +5697,7 @@
       <c r="AA42" s="1"/>
       <c r="AB42" s="1"/>
     </row>
-    <row r="43" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="33"/>
       <c r="C43" s="76">
@@ -5730,7 +5730,7 @@
       <c r="AA43" s="1"/>
       <c r="AB43" s="1"/>
     </row>
-    <row r="44" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="33"/>
       <c r="C44" s="76">
@@ -5763,7 +5763,7 @@
       <c r="AA44" s="1"/>
       <c r="AB44" s="1"/>
     </row>
-    <row r="45" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="33"/>
       <c r="C45" s="76">
@@ -5796,7 +5796,7 @@
       <c r="AA45" s="1"/>
       <c r="AB45" s="1"/>
     </row>
-    <row r="46" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="33"/>
       <c r="C46" s="76">
@@ -5829,7 +5829,7 @@
       <c r="AA46" s="1"/>
       <c r="AB46" s="1"/>
     </row>
-    <row r="47" spans="1:28" ht="11.5" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:28" ht="11.4" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="33" t="s">
         <v>20</v>
@@ -5864,7 +5864,7 @@
       <c r="AA47" s="1"/>
       <c r="AB47" s="1"/>
     </row>
-    <row r="48" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="33"/>
       <c r="C48" s="76">
@@ -5897,7 +5897,7 @@
       <c r="AA48" s="1"/>
       <c r="AB48" s="1"/>
     </row>
-    <row r="49" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="33" t="s">
         <v>19</v>
@@ -5934,7 +5934,7 @@
       <c r="AA49" s="1"/>
       <c r="AB49" s="1"/>
     </row>
-    <row r="50" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="33"/>
       <c r="C50" s="76">
@@ -5969,7 +5969,7 @@
       <c r="AA50" s="1"/>
       <c r="AB50" s="1"/>
     </row>
-    <row r="51" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="33"/>
       <c r="C51" s="76"/>
@@ -6007,7 +6007,7 @@
       <c r="AA51" s="1"/>
       <c r="AB51" s="1"/>
     </row>
-    <row r="52" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="33"/>
       <c r="C52" s="76"/>
@@ -6037,7 +6037,7 @@
       <c r="AA52" s="1"/>
       <c r="AB52" s="1"/>
     </row>
-    <row r="53" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="33"/>
       <c r="C53" s="76"/>
@@ -6073,7 +6073,7 @@
       <c r="AA53" s="1"/>
       <c r="AB53" s="1"/>
     </row>
-    <row r="54" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="33"/>
       <c r="C54" s="76"/>
@@ -6103,7 +6103,7 @@
       <c r="AA54" s="1"/>
       <c r="AB54" s="1"/>
     </row>
-    <row r="55" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" s="33"/>
       <c r="C55" s="76"/>
@@ -6141,7 +6141,7 @@
       <c r="AA55" s="1"/>
       <c r="AB55" s="1"/>
     </row>
-    <row r="56" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="33"/>
       <c r="C56" s="76"/>
@@ -6179,7 +6179,7 @@
       <c r="AA56" s="1"/>
       <c r="AB56" s="1"/>
     </row>
-    <row r="57" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="33"/>
       <c r="C57" s="76"/>
@@ -6215,7 +6215,7 @@
       <c r="AA57" s="1"/>
       <c r="AB57" s="1"/>
     </row>
-    <row r="58" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
       <c r="B58" s="33"/>
       <c r="C58" s="76"/>
@@ -6255,7 +6255,7 @@
       <c r="AA58" s="1"/>
       <c r="AB58" s="1"/>
     </row>
-    <row r="59" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
       <c r="B59" s="33"/>
       <c r="C59" s="76"/>
@@ -6293,7 +6293,7 @@
       <c r="AA59" s="1"/>
       <c r="AB59" s="1"/>
     </row>
-    <row r="60" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
       <c r="B60" s="33"/>
       <c r="C60" s="76"/>
@@ -6323,7 +6323,7 @@
       <c r="AA60" s="1"/>
       <c r="AB60" s="1"/>
     </row>
-    <row r="61" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="B61" s="33"/>
       <c r="C61" s="76"/>
@@ -6363,7 +6363,7 @@
       <c r="AA61" s="1"/>
       <c r="AB61" s="1"/>
     </row>
-    <row r="62" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="33"/>
       <c r="C62" s="76"/>
@@ -6393,7 +6393,7 @@
       <c r="AA62" s="1"/>
       <c r="AB62" s="1"/>
     </row>
-    <row r="63" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
       <c r="B63" s="33"/>
       <c r="C63" s="76"/>
@@ -6427,7 +6427,7 @@
       <c r="AA63" s="1"/>
       <c r="AB63" s="1"/>
     </row>
-    <row r="64" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
       <c r="B64" s="33"/>
       <c r="C64" s="76"/>
@@ -6457,7 +6457,7 @@
       <c r="AA64" s="1"/>
       <c r="AB64" s="1"/>
     </row>
-    <row r="65" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
       <c r="B65" s="33"/>
       <c r="C65" s="76"/>
@@ -6491,7 +6491,7 @@
       <c r="AA65" s="1"/>
       <c r="AB65" s="1"/>
     </row>
-    <row r="66" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A66" s="1"/>
       <c r="B66" s="33"/>
       <c r="C66" s="76"/>
@@ -6521,7 +6521,7 @@
       <c r="AA66" s="1"/>
       <c r="AB66" s="1"/>
     </row>
-    <row r="67" spans="1:46" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:46" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A67" s="1"/>
       <c r="B67" s="33"/>
       <c r="C67" s="76">
@@ -6577,7 +6577,7 @@
       <c r="AS67" s="1"/>
       <c r="AT67" s="1"/>
     </row>
-    <row r="68" spans="1:46" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:46" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
       <c r="B68" s="33"/>
       <c r="C68" s="76"/>
@@ -6638,7 +6638,7 @@
       <c r="AS68" s="1"/>
       <c r="AT68" s="1"/>
     </row>
-    <row r="69" spans="1:46" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:46" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A69" s="1"/>
       <c r="B69" s="33"/>
       <c r="C69" s="76"/>
@@ -6685,7 +6685,7 @@
       <c r="AS69" s="1"/>
       <c r="AT69" s="1"/>
     </row>
-    <row r="70" spans="1:46" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:46" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A70" s="1"/>
       <c r="B70" s="33"/>
       <c r="C70" s="76"/>
@@ -6732,7 +6732,7 @@
       <c r="AS70" s="1"/>
       <c r="AT70" s="1"/>
     </row>
-    <row r="71" spans="1:46" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:46" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A71" s="1"/>
       <c r="B71" s="33"/>
       <c r="C71" s="76">
@@ -6767,7 +6767,7 @@
       <c r="AA71" s="1"/>
       <c r="AB71" s="1"/>
     </row>
-    <row r="72" spans="1:46" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:46" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
       <c r="B72" s="33"/>
       <c r="C72" s="76">
@@ -6800,7 +6800,7 @@
       <c r="AA72" s="1"/>
       <c r="AB72" s="1"/>
     </row>
-    <row r="73" spans="1:46" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:46" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
       <c r="B73" s="35"/>
       <c r="C73" s="79">
@@ -6835,7 +6835,7 @@
       <c r="AA73" s="1"/>
       <c r="AB73" s="1"/>
     </row>
-    <row r="74" spans="1:46" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:46" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1"/>
       <c r="B74" s="19"/>
       <c r="C74" s="80">
@@ -6868,7 +6868,7 @@
       <c r="AA74" s="1"/>
       <c r="AB74" s="1"/>
     </row>
-    <row r="75" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="76">
@@ -6901,7 +6901,7 @@
       <c r="AA75" s="1"/>
       <c r="AB75" s="1"/>
     </row>
-    <row r="76" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="76">
@@ -6934,7 +6934,7 @@
       <c r="AA76" s="1"/>
       <c r="AB76" s="1"/>
     </row>
-    <row r="77" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="69"/>
@@ -6964,7 +6964,7 @@
       <c r="AA77" s="1"/>
       <c r="AB77" s="1"/>
     </row>
-    <row r="78" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="69"/>
@@ -6994,7 +6994,7 @@
       <c r="AA78" s="1"/>
       <c r="AB78" s="1"/>
     </row>
-    <row r="79" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="69"/>
@@ -7024,7 +7024,7 @@
       <c r="AA79" s="1"/>
       <c r="AB79" s="1"/>
     </row>
-    <row r="80" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="69"/>
@@ -7054,7 +7054,7 @@
       <c r="AA80" s="1"/>
       <c r="AB80" s="1"/>
     </row>
-    <row r="81" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="69"/>
@@ -7084,7 +7084,7 @@
       <c r="AA81" s="1"/>
       <c r="AB81" s="1"/>
     </row>
-    <row r="82" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="69"/>
@@ -7114,7 +7114,7 @@
       <c r="AA82" s="1"/>
       <c r="AB82" s="1"/>
     </row>
-    <row r="83" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:28" x14ac:dyDescent="0.3">
       <c r="C83" s="75" t="s">
         <v>4</v>
       </c>
@@ -7138,27 +7138,27 @@
   </sheetPr>
   <dimension ref="A1:AE379"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A326" workbookViewId="0">
-      <selection activeCell="R349" sqref="R349"/>
+    <sheetView tabSelected="1" topLeftCell="H322" workbookViewId="0">
+      <selection activeCell="Q340" sqref="Q340"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" customWidth="1"/>
-    <col min="2" max="2" width="2.7265625" customWidth="1"/>
-    <col min="3" max="3" width="4.7265625" customWidth="1" outlineLevel="2"/>
-    <col min="4" max="4" width="1.7265625" customWidth="1"/>
-    <col min="5" max="6" width="9.7265625" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="1.7265625" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="37.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7265625" customWidth="1"/>
-    <col min="10" max="23" width="10.81640625" customWidth="1"/>
-    <col min="24" max="24" width="1.7265625" customWidth="1"/>
-    <col min="25" max="26" width="4.7265625" customWidth="1"/>
-    <col min="28" max="28" width="46.1796875" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="2.6640625" customWidth="1"/>
+    <col min="3" max="3" width="4.6640625" customWidth="1" outlineLevel="2"/>
+    <col min="4" max="4" width="1.6640625" customWidth="1"/>
+    <col min="5" max="6" width="9.6640625" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="1.6640625" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" customWidth="1"/>
+    <col min="10" max="23" width="10.88671875" customWidth="1"/>
+    <col min="24" max="24" width="1.6640625" customWidth="1"/>
+    <col min="25" max="26" width="4.6640625" customWidth="1"/>
+    <col min="28" max="28" width="46.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="69"/>
@@ -7188,7 +7188,7 @@
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
     </row>
-    <row r="2" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="70">
@@ -7221,7 +7221,7 @@
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
     </row>
-    <row r="3" spans="1:28" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:28" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="20"/>
       <c r="C3" s="71">
@@ -7254,7 +7254,7 @@
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
     </row>
-    <row r="4" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="34" t="s">
         <v>21</v>
@@ -7289,7 +7289,7 @@
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
     </row>
-    <row r="5" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="33"/>
       <c r="C5" s="70">
@@ -7360,7 +7360,7 @@
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
     </row>
-    <row r="6" spans="1:28" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="33"/>
       <c r="C6" s="70">
@@ -7398,7 +7398,7 @@
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
     </row>
-    <row r="7" spans="1:28" ht="20.149999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="33"/>
       <c r="C7" s="70">
@@ -7437,7 +7437,7 @@
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
     </row>
-    <row r="8" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="33"/>
       <c r="C8" s="70">
@@ -7470,7 +7470,7 @@
       <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
     </row>
-    <row r="9" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="33"/>
       <c r="C9" s="70">
@@ -7503,7 +7503,7 @@
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
     </row>
-    <row r="10" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="33"/>
       <c r="C10" s="70">
@@ -7536,7 +7536,7 @@
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
     </row>
-    <row r="11" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="33"/>
       <c r="C11" s="70">
@@ -7569,7 +7569,7 @@
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
     </row>
-    <row r="12" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="33"/>
       <c r="C12" s="70">
@@ -7606,7 +7606,7 @@
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
     </row>
-    <row r="13" spans="1:28" ht="11.5" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:28" ht="11.4" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="33" t="s">
         <v>20</v>
@@ -7641,7 +7641,7 @@
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
     </row>
-    <row r="14" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="33"/>
       <c r="C14" s="70">
@@ -7674,7 +7674,7 @@
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
     </row>
-    <row r="15" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="33"/>
       <c r="C15" s="70">
@@ -7707,7 +7707,7 @@
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
     </row>
-    <row r="16" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="33" t="s">
         <v>19</v>
@@ -7744,7 +7744,7 @@
       <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>
     </row>
-    <row r="17" spans="1:28" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:28" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="33"/>
       <c r="C17" s="70">
@@ -7779,7 +7779,7 @@
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
     </row>
-    <row r="18" spans="1:28" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:28" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="33"/>
       <c r="C18" s="70">
@@ -7818,7 +7818,7 @@
       <c r="AA18" s="1"/>
       <c r="AB18" s="1"/>
     </row>
-    <row r="19" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="33"/>
       <c r="C19" s="70">
@@ -7851,7 +7851,7 @@
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
     </row>
-    <row r="20" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="33"/>
       <c r="C20" s="70">
@@ -7884,7 +7884,7 @@
       <c r="AA20" s="1"/>
       <c r="AB20" s="1"/>
     </row>
-    <row r="21" spans="1:28" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:28" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="33"/>
       <c r="C21" s="70">
@@ -7923,7 +7923,7 @@
       <c r="AA21" s="1"/>
       <c r="AB21" s="1"/>
     </row>
-    <row r="22" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="33"/>
       <c r="C22" s="70">
@@ -7956,7 +7956,7 @@
       <c r="AA22" s="1"/>
       <c r="AB22" s="1"/>
     </row>
-    <row r="23" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="33"/>
       <c r="C23" s="70">
@@ -7989,7 +7989,7 @@
       <c r="AA23" s="1"/>
       <c r="AB23" s="1"/>
     </row>
-    <row r="24" spans="1:28" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="33"/>
       <c r="C24" s="70">
@@ -8024,7 +8024,7 @@
       <c r="AA24" s="1"/>
       <c r="AB24" s="1"/>
     </row>
-    <row r="25" spans="1:28" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="33"/>
       <c r="C25" s="70">
@@ -8059,7 +8059,7 @@
       <c r="AA25" s="1"/>
       <c r="AB25" s="1"/>
     </row>
-    <row r="26" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="33"/>
       <c r="C26" s="70">
@@ -8106,7 +8106,7 @@
       <c r="AA26" s="1"/>
       <c r="AB26" s="1"/>
     </row>
-    <row r="27" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="33"/>
       <c r="C27" s="70">
@@ -8143,7 +8143,7 @@
       <c r="AA27" s="1"/>
       <c r="AB27" s="1"/>
     </row>
-    <row r="28" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="33"/>
       <c r="C28" s="70">
@@ -8180,7 +8180,7 @@
       <c r="AA28" s="1"/>
       <c r="AB28" s="1"/>
     </row>
-    <row r="29" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="33"/>
       <c r="C29" s="70">
@@ -8217,7 +8217,7 @@
       <c r="AA29" s="1"/>
       <c r="AB29" s="1"/>
     </row>
-    <row r="30" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="33"/>
       <c r="C30" s="70">
@@ -8254,7 +8254,7 @@
       <c r="AA30" s="1"/>
       <c r="AB30" s="1"/>
     </row>
-    <row r="31" spans="1:28" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="33"/>
       <c r="C31" s="70">
@@ -8289,7 +8289,7 @@
       <c r="AA31" s="1"/>
       <c r="AB31" s="1"/>
     </row>
-    <row r="32" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="33"/>
       <c r="C32" s="70">
@@ -8322,7 +8322,7 @@
       <c r="AA32" s="1"/>
       <c r="AB32" s="1"/>
     </row>
-    <row r="33" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="35"/>
       <c r="C33" s="73">
@@ -8357,7 +8357,7 @@
       <c r="AA33" s="1"/>
       <c r="AB33" s="1"/>
     </row>
-    <row r="34" spans="1:28" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:28" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="19"/>
       <c r="C34" s="74">
@@ -8390,7 +8390,7 @@
       <c r="AA34" s="1"/>
       <c r="AB34" s="1"/>
     </row>
-    <row r="35" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="70">
@@ -8423,7 +8423,7 @@
       <c r="AA35" s="1"/>
       <c r="AB35" s="1"/>
     </row>
-    <row r="36" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="76">
@@ -8456,7 +8456,7 @@
       <c r="AA36" s="1"/>
       <c r="AB36" s="1"/>
     </row>
-    <row r="37" spans="1:28" s="142" customFormat="1" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:28" s="142" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
       <c r="B37" s="20"/>
       <c r="C37" s="77">
@@ -8489,7 +8489,7 @@
       <c r="AA37" s="1"/>
       <c r="AB37" s="1"/>
     </row>
-    <row r="38" spans="1:28" s="142" customFormat="1" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:28" s="142" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="34" t="s">
         <v>21</v>
@@ -8524,7 +8524,7 @@
       <c r="AA38" s="1"/>
       <c r="AB38" s="1"/>
     </row>
-    <row r="39" spans="1:28" s="142" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:28" s="142" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="33"/>
       <c r="C39" s="76">
@@ -8557,7 +8557,7 @@
       <c r="AA39" s="1"/>
       <c r="AB39" s="1"/>
     </row>
-    <row r="40" spans="1:28" s="142" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:28" s="142" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="33"/>
       <c r="C40" s="76">
@@ -8594,7 +8594,7 @@
       <c r="AA40" s="1"/>
       <c r="AB40" s="1"/>
     </row>
-    <row r="41" spans="1:28" s="142" customFormat="1" ht="20.149999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:28" s="142" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="33"/>
       <c r="C41" s="76">
@@ -8633,7 +8633,7 @@
       <c r="AA41" s="1"/>
       <c r="AB41" s="1"/>
     </row>
-    <row r="42" spans="1:28" s="142" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:28" s="142" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="33"/>
       <c r="C42" s="76">
@@ -8666,7 +8666,7 @@
       <c r="AA42" s="1"/>
       <c r="AB42" s="1"/>
     </row>
-    <row r="43" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="33"/>
       <c r="C43" s="76">
@@ -8699,7 +8699,7 @@
       <c r="AA43" s="1"/>
       <c r="AB43" s="1"/>
     </row>
-    <row r="44" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="33"/>
       <c r="C44" s="76">
@@ -8732,7 +8732,7 @@
       <c r="AA44" s="1"/>
       <c r="AB44" s="1"/>
     </row>
-    <row r="45" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="33"/>
       <c r="C45" s="76">
@@ -8765,7 +8765,7 @@
       <c r="AA45" s="1"/>
       <c r="AB45" s="1"/>
     </row>
-    <row r="46" spans="1:28" s="142" customFormat="1" ht="28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:28" s="142" customFormat="1" ht="27.6" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="33"/>
       <c r="C46" s="76">
@@ -8808,7 +8808,7 @@
       <c r="AA46" s="1"/>
       <c r="AB46" s="1"/>
     </row>
-    <row r="47" spans="1:28" s="142" customFormat="1" ht="11.5" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:28" s="142" customFormat="1" ht="11.4" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="33" t="s">
         <v>20</v>
@@ -8843,7 +8843,7 @@
       <c r="AA47" s="1"/>
       <c r="AB47" s="1"/>
     </row>
-    <row r="48" spans="1:28" s="142" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:28" s="142" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="33"/>
       <c r="C48" s="76">
@@ -8876,7 +8876,7 @@
       <c r="AA48" s="1"/>
       <c r="AB48" s="1"/>
     </row>
-    <row r="49" spans="1:28" s="142" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:28" s="142" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="33" t="s">
         <v>19</v>
@@ -8913,7 +8913,7 @@
       <c r="AA49" s="1"/>
       <c r="AB49" s="1"/>
     </row>
-    <row r="50" spans="1:28" s="142" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:28" s="142" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="33"/>
       <c r="C50" s="76">
@@ -8948,7 +8948,7 @@
       <c r="AA50" s="1"/>
       <c r="AB50" s="1"/>
     </row>
-    <row r="51" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="33"/>
       <c r="C51" s="76">
@@ -8983,7 +8983,7 @@
       <c r="AA51" s="1"/>
       <c r="AB51" s="1"/>
     </row>
-    <row r="52" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="33"/>
       <c r="C52" s="76"/>
@@ -9017,7 +9017,7 @@
       <c r="AA52" s="1"/>
       <c r="AB52" s="1"/>
     </row>
-    <row r="53" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="33"/>
       <c r="C53" s="76"/>
@@ -9051,7 +9051,7 @@
       <c r="AA53" s="1"/>
       <c r="AB53" s="1"/>
     </row>
-    <row r="54" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="33"/>
       <c r="C54" s="76"/>
@@ -9085,7 +9085,7 @@
       <c r="AA54" s="1"/>
       <c r="AB54" s="1"/>
     </row>
-    <row r="55" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" s="33"/>
       <c r="C55" s="76"/>
@@ -9119,7 +9119,7 @@
       <c r="AA55" s="1"/>
       <c r="AB55" s="1"/>
     </row>
-    <row r="56" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="33"/>
       <c r="C56" s="76"/>
@@ -9153,7 +9153,7 @@
       <c r="AA56" s="1"/>
       <c r="AB56" s="1"/>
     </row>
-    <row r="57" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="33"/>
       <c r="C57" s="76"/>
@@ -9187,7 +9187,7 @@
       <c r="AA57" s="1"/>
       <c r="AB57" s="1"/>
     </row>
-    <row r="58" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
       <c r="B58" s="33"/>
       <c r="C58" s="76"/>
@@ -9221,7 +9221,7 @@
       <c r="AA58" s="1"/>
       <c r="AB58" s="1"/>
     </row>
-    <row r="59" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
       <c r="B59" s="33"/>
       <c r="C59" s="76"/>
@@ -9255,7 +9255,7 @@
       <c r="AA59" s="1"/>
       <c r="AB59" s="1"/>
     </row>
-    <row r="60" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
       <c r="B60" s="33"/>
       <c r="C60" s="76"/>
@@ -9289,7 +9289,7 @@
       <c r="AA60" s="1"/>
       <c r="AB60" s="1"/>
     </row>
-    <row r="61" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="B61" s="33"/>
       <c r="C61" s="76"/>
@@ -9323,7 +9323,7 @@
       <c r="AA61" s="1"/>
       <c r="AB61" s="1"/>
     </row>
-    <row r="62" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="33"/>
       <c r="C62" s="76"/>
@@ -9357,7 +9357,7 @@
       <c r="AA62" s="1"/>
       <c r="AB62" s="1"/>
     </row>
-    <row r="63" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
       <c r="B63" s="33"/>
       <c r="C63" s="76"/>
@@ -9391,7 +9391,7 @@
       <c r="AA63" s="1"/>
       <c r="AB63" s="1"/>
     </row>
-    <row r="64" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
       <c r="B64" s="33"/>
       <c r="C64" s="76"/>
@@ -9425,7 +9425,7 @@
       <c r="AA64" s="1"/>
       <c r="AB64" s="1"/>
     </row>
-    <row r="65" spans="1:28" s="113" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:28" s="113" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
       <c r="B65" s="33"/>
       <c r="C65" s="76">
@@ -9464,7 +9464,7 @@
       <c r="AA65" s="1"/>
       <c r="AB65" s="1"/>
     </row>
-    <row r="66" spans="1:28" s="105" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:28" s="105" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A66" s="1"/>
       <c r="B66" s="33"/>
       <c r="C66" s="76">
@@ -9501,7 +9501,7 @@
       <c r="AA66" s="1"/>
       <c r="AB66" s="1"/>
     </row>
-    <row r="67" spans="1:28" s="105" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:28" s="105" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A67" s="1"/>
       <c r="B67" s="33"/>
       <c r="C67" s="76">
@@ -9538,7 +9538,7 @@
       <c r="AA67" s="1"/>
       <c r="AB67" s="1"/>
     </row>
-    <row r="68" spans="1:28" s="129" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:28" s="129" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
       <c r="B68" s="33"/>
       <c r="C68" s="76">
@@ -9575,7 +9575,7 @@
       <c r="AA68" s="1"/>
       <c r="AB68" s="1"/>
     </row>
-    <row r="69" spans="1:28" s="145" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:28" s="145" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A69" s="1"/>
       <c r="B69" s="33"/>
       <c r="C69" s="76">
@@ -9608,7 +9608,7 @@
       <c r="AA69" s="1"/>
       <c r="AB69" s="1"/>
     </row>
-    <row r="70" spans="1:28" s="109" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:28" s="109" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A70" s="1"/>
       <c r="B70" s="33"/>
       <c r="C70" s="76">
@@ -9645,7 +9645,7 @@
       <c r="AA70" s="1"/>
       <c r="AB70" s="1"/>
     </row>
-    <row r="71" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A71" s="1"/>
       <c r="B71" s="33"/>
       <c r="C71" s="76">
@@ -9686,7 +9686,7 @@
       <c r="AA71" s="1"/>
       <c r="AB71" s="1"/>
     </row>
-    <row r="72" spans="1:28" s="154" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:28" s="154" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
       <c r="B72" s="33"/>
       <c r="C72" s="76">
@@ -9725,7 +9725,7 @@
       <c r="AA72" s="1"/>
       <c r="AB72" s="1"/>
     </row>
-    <row r="73" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
       <c r="B73" s="33"/>
       <c r="C73" s="76"/>
@@ -9755,7 +9755,7 @@
       <c r="AA73" s="1"/>
       <c r="AB73" s="1"/>
     </row>
-    <row r="74" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A74" s="1"/>
       <c r="B74" s="33"/>
       <c r="C74" s="76"/>
@@ -9791,7 +9791,7 @@
       <c r="AA74" s="1"/>
       <c r="AB74" s="1"/>
     </row>
-    <row r="75" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A75" s="1"/>
       <c r="B75" s="33"/>
       <c r="C75" s="76"/>
@@ -9821,7 +9821,7 @@
       <c r="AA75" s="1"/>
       <c r="AB75" s="1"/>
     </row>
-    <row r="76" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A76" s="1"/>
       <c r="B76" s="33"/>
       <c r="C76" s="76">
@@ -9856,7 +9856,7 @@
       <c r="AA76" s="1"/>
       <c r="AB76" s="1"/>
     </row>
-    <row r="77" spans="1:28" s="101" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:28" s="101" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A77" s="1"/>
       <c r="B77" s="33"/>
       <c r="C77" s="76">
@@ -9897,7 +9897,7 @@
       <c r="AA77" s="1"/>
       <c r="AB77" s="1"/>
     </row>
-    <row r="78" spans="1:28" s="101" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:28" s="101" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A78" s="1"/>
       <c r="B78" s="33"/>
       <c r="C78" s="76">
@@ -9938,7 +9938,7 @@
       <c r="AA78" s="1"/>
       <c r="AB78" s="1"/>
     </row>
-    <row r="79" spans="1:28" s="101" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:28" s="101" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A79" s="1"/>
       <c r="B79" s="33"/>
       <c r="C79" s="76">
@@ -9971,7 +9971,7 @@
       <c r="AA79" s="1"/>
       <c r="AB79" s="1"/>
     </row>
-    <row r="80" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A80" s="1"/>
       <c r="B80" s="33"/>
       <c r="C80" s="76">
@@ -10008,7 +10008,7 @@
       <c r="AA80" s="1"/>
       <c r="AB80" s="1"/>
     </row>
-    <row r="81" spans="1:28" s="152" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:28" s="152" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A81" s="1"/>
       <c r="B81" s="33"/>
       <c r="C81" s="76">
@@ -10041,7 +10041,7 @@
       <c r="AA81" s="1"/>
       <c r="AB81" s="1"/>
     </row>
-    <row r="82" spans="1:28" s="101" customFormat="1" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:28" s="101" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A82" s="1"/>
       <c r="B82" s="33"/>
       <c r="C82" s="76">
@@ -10076,7 +10076,7 @@
       <c r="AA82" s="1"/>
       <c r="AB82" s="1"/>
     </row>
-    <row r="83" spans="1:28" s="101" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:28" s="101" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A83" s="1"/>
       <c r="B83" s="33"/>
       <c r="C83" s="76">
@@ -10109,7 +10109,7 @@
       <c r="AA83" s="1"/>
       <c r="AB83" s="1"/>
     </row>
-    <row r="84" spans="1:28" s="101" customFormat="1" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:28" s="101" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A84" s="1"/>
       <c r="B84" s="35"/>
       <c r="C84" s="79">
@@ -10144,7 +10144,7 @@
       <c r="AA84" s="1"/>
       <c r="AB84" s="1"/>
     </row>
-    <row r="85" spans="1:28" s="101" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:28" s="101" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="1"/>
       <c r="B85" s="19"/>
       <c r="C85" s="80">
@@ -10177,7 +10177,7 @@
       <c r="AA85" s="1"/>
       <c r="AB85" s="1"/>
     </row>
-    <row r="86" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="76">
@@ -10210,7 +10210,7 @@
       <c r="AA86" s="1"/>
       <c r="AB86" s="1"/>
     </row>
-    <row r="87" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="76">
@@ -10243,7 +10243,7 @@
       <c r="AA87" s="1"/>
       <c r="AB87" s="1"/>
     </row>
-    <row r="88" spans="1:28" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:28" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="1"/>
       <c r="B88" s="20"/>
       <c r="C88" s="77">
@@ -10276,7 +10276,7 @@
       <c r="AA88" s="1"/>
       <c r="AB88" s="1"/>
     </row>
-    <row r="89" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A89" s="1"/>
       <c r="B89" s="34" t="s">
         <v>21</v>
@@ -10311,7 +10311,7 @@
       <c r="AA89" s="1"/>
       <c r="AB89" s="1"/>
     </row>
-    <row r="90" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.3">
       <c r="A90" s="1"/>
       <c r="B90" s="33"/>
       <c r="C90" s="76">
@@ -10344,7 +10344,7 @@
       <c r="AA90" s="1"/>
       <c r="AB90" s="1"/>
     </row>
-    <row r="91" spans="1:28" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="1"/>
       <c r="B91" s="33"/>
       <c r="C91" s="76">
@@ -10381,7 +10381,7 @@
       <c r="AA91" s="1"/>
       <c r="AB91" s="1"/>
     </row>
-    <row r="92" spans="1:28" ht="20.149999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:28" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A92" s="1"/>
       <c r="B92" s="33"/>
       <c r="C92" s="76">
@@ -10420,7 +10420,7 @@
       <c r="AA92" s="1"/>
       <c r="AB92" s="1"/>
     </row>
-    <row r="93" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A93" s="1"/>
       <c r="B93" s="33"/>
       <c r="C93" s="76">
@@ -10453,7 +10453,7 @@
       <c r="AA93" s="1"/>
       <c r="AB93" s="1"/>
     </row>
-    <row r="94" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A94" s="1"/>
       <c r="B94" s="33"/>
       <c r="C94" s="76">
@@ -10486,7 +10486,7 @@
       <c r="AA94" s="1"/>
       <c r="AB94" s="1"/>
     </row>
-    <row r="95" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A95" s="1"/>
       <c r="B95" s="33"/>
       <c r="C95" s="76">
@@ -10519,7 +10519,7 @@
       <c r="AA95" s="1"/>
       <c r="AB95" s="1"/>
     </row>
-    <row r="96" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A96" s="1"/>
       <c r="B96" s="33"/>
       <c r="C96" s="76">
@@ -10558,7 +10558,7 @@
       <c r="AA96" s="1"/>
       <c r="AB96" s="1"/>
     </row>
-    <row r="97" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A97" s="1"/>
       <c r="B97" s="33"/>
       <c r="C97" s="76">
@@ -10607,7 +10607,7 @@
       <c r="AA97" s="1"/>
       <c r="AB97" s="1"/>
     </row>
-    <row r="98" spans="1:28" ht="11.5" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:28" ht="11.4" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A98" s="1"/>
       <c r="B98" s="33" t="s">
         <v>20</v>
@@ -10642,7 +10642,7 @@
       <c r="AA98" s="1"/>
       <c r="AB98" s="1"/>
     </row>
-    <row r="99" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.3">
       <c r="A99" s="1"/>
       <c r="B99" s="33"/>
       <c r="C99" s="76">
@@ -10675,7 +10675,7 @@
       <c r="AA99" s="1"/>
       <c r="AB99" s="1"/>
     </row>
-    <row r="100" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.3">
       <c r="A100" s="1"/>
       <c r="B100" s="33" t="s">
         <v>19</v>
@@ -10712,7 +10712,7 @@
       <c r="AA100" s="1"/>
       <c r="AB100" s="1"/>
     </row>
-    <row r="101" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A101" s="1"/>
       <c r="B101" s="33"/>
       <c r="C101" s="76">
@@ -10747,7 +10747,7 @@
       <c r="AA101" s="1"/>
       <c r="AB101" s="1"/>
     </row>
-    <row r="102" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A102" s="1"/>
       <c r="B102" s="33"/>
       <c r="C102" s="76">
@@ -10800,7 +10800,7 @@
       <c r="AA102" s="1"/>
       <c r="AB102" s="1"/>
     </row>
-    <row r="103" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A103" s="1"/>
       <c r="B103" s="33"/>
       <c r="C103" s="76">
@@ -10851,7 +10851,7 @@
       <c r="AA103" s="1"/>
       <c r="AB103" s="1"/>
     </row>
-    <row r="104" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A104" s="1"/>
       <c r="B104" s="33"/>
       <c r="C104" s="76">
@@ -10902,7 +10902,7 @@
       <c r="AA104" s="1"/>
       <c r="AB104" s="1"/>
     </row>
-    <row r="105" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A105" s="1"/>
       <c r="B105" s="33"/>
       <c r="C105" s="76">
@@ -10935,7 +10935,7 @@
       <c r="AA105" s="1"/>
       <c r="AB105" s="1"/>
     </row>
-    <row r="106" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A106" s="1"/>
       <c r="B106" s="33"/>
       <c r="C106" s="76">
@@ -10986,7 +10986,7 @@
       <c r="AA106" s="1"/>
       <c r="AB106" s="1"/>
     </row>
-    <row r="107" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A107" s="1"/>
       <c r="B107" s="33"/>
       <c r="C107" s="76">
@@ -11035,7 +11035,7 @@
       <c r="AA107" s="1"/>
       <c r="AB107" s="1"/>
     </row>
-    <row r="108" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A108" s="1"/>
       <c r="B108" s="33"/>
       <c r="C108" s="76">
@@ -11084,7 +11084,7 @@
       <c r="AA108" s="1"/>
       <c r="AB108" s="1"/>
     </row>
-    <row r="109" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A109" s="1"/>
       <c r="B109" s="33"/>
       <c r="C109" s="76">
@@ -11133,7 +11133,7 @@
       <c r="AA109" s="1"/>
       <c r="AB109" s="1"/>
     </row>
-    <row r="110" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A110" s="1"/>
       <c r="B110" s="33"/>
       <c r="C110" s="76">
@@ -11166,7 +11166,7 @@
       <c r="AA110" s="1"/>
       <c r="AB110" s="1"/>
     </row>
-    <row r="111" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A111" s="1"/>
       <c r="B111" s="33"/>
       <c r="C111" s="76">
@@ -11217,7 +11217,7 @@
       <c r="AA111" s="1"/>
       <c r="AB111" s="1"/>
     </row>
-    <row r="112" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A112" s="1"/>
       <c r="B112" s="33"/>
       <c r="C112" s="76">
@@ -11266,7 +11266,7 @@
       <c r="AA112" s="1"/>
       <c r="AB112" s="1"/>
     </row>
-    <row r="113" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A113" s="1"/>
       <c r="B113" s="33"/>
       <c r="C113" s="76">
@@ -11315,7 +11315,7 @@
       <c r="AA113" s="1"/>
       <c r="AB113" s="1"/>
     </row>
-    <row r="114" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A114" s="1"/>
       <c r="B114" s="33"/>
       <c r="C114" s="76">
@@ -11364,7 +11364,7 @@
       <c r="AA114" s="1"/>
       <c r="AB114" s="1"/>
     </row>
-    <row r="115" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A115" s="1"/>
       <c r="B115" s="33"/>
       <c r="C115" s="76">
@@ -11397,7 +11397,7 @@
       <c r="AA115" s="1"/>
       <c r="AB115" s="1"/>
     </row>
-    <row r="116" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A116" s="1"/>
       <c r="B116" s="33"/>
       <c r="C116" s="76">
@@ -11448,7 +11448,7 @@
       <c r="AA116" s="1"/>
       <c r="AB116" s="1"/>
     </row>
-    <row r="117" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A117" s="1"/>
       <c r="B117" s="33"/>
       <c r="C117" s="76">
@@ -11497,7 +11497,7 @@
       <c r="AA117" s="1"/>
       <c r="AB117" s="1"/>
     </row>
-    <row r="118" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A118" s="1"/>
       <c r="B118" s="33"/>
       <c r="C118" s="76">
@@ -11546,7 +11546,7 @@
       <c r="AA118" s="1"/>
       <c r="AB118" s="1"/>
     </row>
-    <row r="119" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A119" s="1"/>
       <c r="B119" s="33"/>
       <c r="C119" s="76">
@@ -11595,7 +11595,7 @@
       <c r="AA119" s="1"/>
       <c r="AB119" s="1"/>
     </row>
-    <row r="120" spans="1:28" s="151" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:28" s="151" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A120" s="1"/>
       <c r="B120" s="33"/>
       <c r="C120" s="76">
@@ -11628,7 +11628,7 @@
       <c r="AA120" s="1"/>
       <c r="AB120" s="1"/>
     </row>
-    <row r="121" spans="1:28" s="151" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:28" s="151" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A121" s="1"/>
       <c r="B121" s="33"/>
       <c r="C121" s="76">
@@ -11663,7 +11663,7 @@
       <c r="AA121" s="1"/>
       <c r="AB121" s="1"/>
     </row>
-    <row r="122" spans="1:28" s="151" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:28" s="151" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A122" s="1"/>
       <c r="B122" s="33"/>
       <c r="C122" s="76">
@@ -11704,7 +11704,7 @@
       <c r="AA122" s="1"/>
       <c r="AB122" s="1"/>
     </row>
-    <row r="123" spans="1:28" s="151" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:28" s="151" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A123" s="1"/>
       <c r="B123" s="33"/>
       <c r="C123" s="76">
@@ -11752,7 +11752,7 @@
       <c r="AA123" s="1"/>
       <c r="AB123" s="1"/>
     </row>
-    <row r="124" spans="1:28" s="151" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:28" s="151" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A124" s="1"/>
       <c r="B124" s="33"/>
       <c r="C124" s="76">
@@ -11798,7 +11798,7 @@
       <c r="AA124" s="1"/>
       <c r="AB124" s="1"/>
     </row>
-    <row r="125" spans="1:28" s="151" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:28" s="151" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A125" s="1"/>
       <c r="B125" s="33"/>
       <c r="C125" s="76">
@@ -11841,7 +11841,7 @@
       <c r="AA125" s="1"/>
       <c r="AB125" s="1"/>
     </row>
-    <row r="126" spans="1:28" s="151" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:28" s="151" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A126" s="1"/>
       <c r="B126" s="33"/>
       <c r="C126" s="76">
@@ -11874,7 +11874,7 @@
       <c r="AA126" s="1"/>
       <c r="AB126" s="1"/>
     </row>
-    <row r="127" spans="1:28" s="151" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:28" s="151" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A127" s="1"/>
       <c r="B127" s="33"/>
       <c r="C127" s="76">
@@ -11921,7 +11921,7 @@
       <c r="AA127" s="1"/>
       <c r="AB127" s="1"/>
     </row>
-    <row r="128" spans="1:28" s="151" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:28" s="151" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A128" s="1"/>
       <c r="B128" s="33"/>
       <c r="C128" s="76">
@@ -11966,7 +11966,7 @@
       <c r="AA128" s="1"/>
       <c r="AB128" s="1"/>
     </row>
-    <row r="129" spans="1:28" s="151" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:28" s="151" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A129" s="1"/>
       <c r="B129" s="33"/>
       <c r="C129" s="76">
@@ -12009,7 +12009,7 @@
       <c r="AA129" s="1"/>
       <c r="AB129" s="1"/>
     </row>
-    <row r="130" spans="1:28" s="151" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:28" s="151" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A130" s="1"/>
       <c r="B130" s="33"/>
       <c r="C130" s="76">
@@ -12042,7 +12042,7 @@
       <c r="AA130" s="1"/>
       <c r="AB130" s="1"/>
     </row>
-    <row r="131" spans="1:28" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A131" s="1"/>
       <c r="B131" s="33"/>
       <c r="C131" s="76">
@@ -12077,7 +12077,7 @@
       <c r="AA131" s="1"/>
       <c r="AB131" s="1"/>
     </row>
-    <row r="132" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A132" s="1"/>
       <c r="B132" s="33"/>
       <c r="C132" s="76">
@@ -12110,7 +12110,7 @@
       <c r="AA132" s="1"/>
       <c r="AB132" s="1"/>
     </row>
-    <row r="133" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A133" s="1"/>
       <c r="B133" s="35"/>
       <c r="C133" s="79">
@@ -12145,7 +12145,7 @@
       <c r="AA133" s="1"/>
       <c r="AB133" s="1"/>
     </row>
-    <row r="134" spans="1:28" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:28" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="1"/>
       <c r="B134" s="19"/>
       <c r="C134" s="80">
@@ -12178,7 +12178,7 @@
       <c r="AA134" s="1"/>
       <c r="AB134" s="1"/>
     </row>
-    <row r="135" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="76">
@@ -12211,7 +12211,7 @@
       <c r="AA135" s="1"/>
       <c r="AB135" s="1"/>
     </row>
-    <row r="136" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="76">
@@ -12244,7 +12244,7 @@
       <c r="AA136" s="1"/>
       <c r="AB136" s="1"/>
     </row>
-    <row r="137" spans="1:28" s="99" customFormat="1" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:28" s="99" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A137" s="1"/>
       <c r="B137" s="20"/>
       <c r="C137" s="77">
@@ -12277,7 +12277,7 @@
       <c r="AA137" s="1"/>
       <c r="AB137" s="1"/>
     </row>
-    <row r="138" spans="1:28" s="99" customFormat="1" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:28" s="99" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A138" s="1"/>
       <c r="B138" s="34" t="s">
         <v>21</v>
@@ -12312,7 +12312,7 @@
       <c r="AA138" s="1"/>
       <c r="AB138" s="1"/>
     </row>
-    <row r="139" spans="1:28" s="99" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:28" s="99" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.3">
       <c r="A139" s="1"/>
       <c r="B139" s="33"/>
       <c r="C139" s="76">
@@ -12345,7 +12345,7 @@
       <c r="AA139" s="1"/>
       <c r="AB139" s="1"/>
     </row>
-    <row r="140" spans="1:28" s="99" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:28" s="99" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="1"/>
       <c r="B140" s="33"/>
       <c r="C140" s="76">
@@ -12382,7 +12382,7 @@
       <c r="AA140" s="1"/>
       <c r="AB140" s="1"/>
     </row>
-    <row r="141" spans="1:28" s="99" customFormat="1" ht="20.149999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:28" s="99" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A141" s="1"/>
       <c r="B141" s="33"/>
       <c r="C141" s="76">
@@ -12421,7 +12421,7 @@
       <c r="AA141" s="1"/>
       <c r="AB141" s="1"/>
     </row>
-    <row r="142" spans="1:28" s="99" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:28" s="99" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A142" s="1"/>
       <c r="B142" s="33"/>
       <c r="C142" s="76">
@@ -12454,7 +12454,7 @@
       <c r="AA142" s="1"/>
       <c r="AB142" s="1"/>
     </row>
-    <row r="143" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A143" s="1"/>
       <c r="B143" s="33"/>
       <c r="C143" s="76">
@@ -12487,7 +12487,7 @@
       <c r="AA143" s="1"/>
       <c r="AB143" s="1"/>
     </row>
-    <row r="144" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A144" s="1"/>
       <c r="B144" s="33"/>
       <c r="C144" s="76">
@@ -12522,7 +12522,7 @@
       <c r="AA144" s="1"/>
       <c r="AB144" s="1"/>
     </row>
-    <row r="145" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A145" s="1"/>
       <c r="B145" s="33"/>
       <c r="C145" s="76">
@@ -12557,7 +12557,7 @@
       <c r="AA145" s="1"/>
       <c r="AB145" s="1"/>
     </row>
-    <row r="146" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A146" s="1"/>
       <c r="B146" s="33"/>
       <c r="C146" s="76">
@@ -12612,7 +12612,7 @@
       <c r="AA146" s="1"/>
       <c r="AB146" s="1"/>
     </row>
-    <row r="147" spans="1:28" s="99" customFormat="1" ht="11.5" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:28" s="99" customFormat="1" ht="11.4" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A147" s="1"/>
       <c r="B147" s="33" t="s">
         <v>20</v>
@@ -12647,7 +12647,7 @@
       <c r="AA147" s="1"/>
       <c r="AB147" s="1"/>
     </row>
-    <row r="148" spans="1:28" s="99" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:28" s="99" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.3">
       <c r="A148" s="1"/>
       <c r="B148" s="33"/>
       <c r="C148" s="76">
@@ -12702,7 +12702,7 @@
       <c r="AA148" s="1"/>
       <c r="AB148" s="1"/>
     </row>
-    <row r="149" spans="1:28" s="99" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:28" s="99" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.3">
       <c r="A149" s="1"/>
       <c r="B149" s="33" t="s">
         <v>19</v>
@@ -12739,7 +12739,7 @@
       <c r="AA149" s="1"/>
       <c r="AB149" s="1"/>
     </row>
-    <row r="150" spans="1:28" s="99" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:28" s="99" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A150" s="1"/>
       <c r="B150" s="33"/>
       <c r="C150" s="76">
@@ -12774,7 +12774,7 @@
       <c r="AA150" s="1"/>
       <c r="AB150" s="1"/>
     </row>
-    <row r="151" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A151" s="1"/>
       <c r="B151" s="33"/>
       <c r="C151" s="76">
@@ -12809,7 +12809,7 @@
       <c r="AA151" s="1"/>
       <c r="AB151" s="1"/>
     </row>
-    <row r="152" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A152" s="1"/>
       <c r="B152" s="33"/>
       <c r="C152" s="76">
@@ -12848,7 +12848,7 @@
       <c r="AA152" s="1"/>
       <c r="AB152" s="1"/>
     </row>
-    <row r="153" spans="1:28" s="99" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:28" s="99" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A153" s="1"/>
       <c r="B153" s="33"/>
       <c r="C153" s="76">
@@ -12907,7 +12907,7 @@
       <c r="AA153" s="1"/>
       <c r="AB153" s="1"/>
     </row>
-    <row r="154" spans="1:28" s="99" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:28" s="99" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A154" s="1"/>
       <c r="B154" s="33"/>
       <c r="C154" s="76">
@@ -12964,7 +12964,7 @@
       <c r="AA154" s="1"/>
       <c r="AB154" s="1"/>
     </row>
-    <row r="155" spans="1:28" s="99" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:28" s="99" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A155" s="1"/>
       <c r="B155" s="33"/>
       <c r="C155" s="76">
@@ -13001,7 +13001,7 @@
       <c r="AA155" s="1"/>
       <c r="AB155" s="1"/>
     </row>
-    <row r="156" spans="1:28" s="99" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:28" s="99" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A156" s="1"/>
       <c r="B156" s="33"/>
       <c r="C156" s="76">
@@ -13058,7 +13058,7 @@
       <c r="AA156" s="1"/>
       <c r="AB156" s="1"/>
     </row>
-    <row r="157" spans="1:28" s="150" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:28" s="150" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A157" s="1"/>
       <c r="B157" s="33"/>
       <c r="C157" s="76">
@@ -13117,7 +13117,7 @@
       <c r="AA157" s="1"/>
       <c r="AB157" s="1"/>
     </row>
-    <row r="158" spans="1:28" s="124" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:28" s="124" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A158" s="1"/>
       <c r="B158" s="33"/>
       <c r="C158" s="76">
@@ -13174,7 +13174,7 @@
       <c r="AA158" s="1"/>
       <c r="AB158" s="1"/>
     </row>
-    <row r="159" spans="1:28" s="124" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:28" s="124" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A159" s="1"/>
       <c r="B159" s="33"/>
       <c r="C159" s="76">
@@ -13231,7 +13231,7 @@
       <c r="AA159" s="1"/>
       <c r="AB159" s="1"/>
     </row>
-    <row r="160" spans="1:28" s="99" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:28" s="99" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A160" s="1"/>
       <c r="B160" s="33"/>
       <c r="C160" s="76">
@@ -13288,7 +13288,7 @@
       <c r="AA160" s="1"/>
       <c r="AB160" s="1"/>
     </row>
-    <row r="161" spans="1:31" s="99" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:31" s="99" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A161" s="1"/>
       <c r="B161" s="33"/>
       <c r="C161" s="76">
@@ -13345,7 +13345,7 @@
       <c r="AA161" s="1"/>
       <c r="AB161" s="1"/>
     </row>
-    <row r="162" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A162" s="1"/>
       <c r="B162" s="33"/>
       <c r="C162" s="76">
@@ -13405,7 +13405,7 @@
       <c r="AD162" s="130"/>
       <c r="AE162" s="130"/>
     </row>
-    <row r="163" spans="1:31" s="146" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:31" s="146" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A163" s="1"/>
       <c r="B163" s="33"/>
       <c r="C163" s="76">
@@ -13462,7 +13462,7 @@
       <c r="AA163" s="1"/>
       <c r="AB163" s="1"/>
     </row>
-    <row r="164" spans="1:31" s="113" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:31" s="113" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A164" s="1"/>
       <c r="B164" s="33"/>
       <c r="C164" s="76">
@@ -13498,7 +13498,7 @@
       <c r="AD164" s="130"/>
       <c r="AE164" s="130"/>
     </row>
-    <row r="165" spans="1:31" s="113" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:31" s="113" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A165" s="1"/>
       <c r="B165" s="33"/>
       <c r="C165" s="76">
@@ -13561,7 +13561,7 @@
       <c r="AD165" s="130"/>
       <c r="AE165" s="130"/>
     </row>
-    <row r="166" spans="1:31" s="113" customFormat="1" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:31" s="113" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A166" s="1"/>
       <c r="B166" s="33"/>
       <c r="C166" s="76">
@@ -13599,7 +13599,7 @@
       <c r="AD166" s="130"/>
       <c r="AE166" s="130"/>
     </row>
-    <row r="167" spans="1:31" s="112" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:31" s="112" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A167" s="1"/>
       <c r="B167" s="33"/>
       <c r="C167" s="76">
@@ -13653,7 +13653,7 @@
       <c r="AD167" s="130"/>
       <c r="AE167" s="130"/>
     </row>
-    <row r="168" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A168" s="1"/>
       <c r="B168" s="33"/>
       <c r="C168" s="76">
@@ -13716,7 +13716,7 @@
       <c r="AA168" s="1"/>
       <c r="AB168" s="1"/>
     </row>
-    <row r="169" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A169" s="1"/>
       <c r="B169" s="33"/>
       <c r="C169" s="76">
@@ -13777,7 +13777,7 @@
       <c r="AA169" s="1"/>
       <c r="AB169" s="1"/>
     </row>
-    <row r="170" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A170" s="1"/>
       <c r="B170" s="33"/>
       <c r="C170" s="76">
@@ -13836,7 +13836,7 @@
       <c r="AA170" s="1"/>
       <c r="AB170" s="1"/>
     </row>
-    <row r="171" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A171" s="1"/>
       <c r="B171" s="33"/>
       <c r="C171" s="76">
@@ -13895,7 +13895,7 @@
       <c r="AA171" s="1"/>
       <c r="AB171" s="1"/>
     </row>
-    <row r="172" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A172" s="1"/>
       <c r="B172" s="33"/>
       <c r="C172" s="76">
@@ -13954,7 +13954,7 @@
       <c r="AA172" s="1"/>
       <c r="AB172" s="1"/>
     </row>
-    <row r="173" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A173" s="1"/>
       <c r="B173" s="33"/>
       <c r="C173" s="76">
@@ -14015,7 +14015,7 @@
       <c r="AA173" s="1"/>
       <c r="AB173" s="1"/>
     </row>
-    <row r="174" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A174" s="1"/>
       <c r="B174" s="33"/>
       <c r="C174" s="76">
@@ -14076,7 +14076,7 @@
       <c r="AA174" s="1"/>
       <c r="AB174" s="1"/>
     </row>
-    <row r="175" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A175" s="1"/>
       <c r="B175" s="33"/>
       <c r="C175" s="76">
@@ -14135,7 +14135,7 @@
       <c r="AA175" s="1"/>
       <c r="AB175" s="1"/>
     </row>
-    <row r="176" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A176" s="1"/>
       <c r="B176" s="33"/>
       <c r="C176" s="76">
@@ -14194,7 +14194,7 @@
       <c r="AA176" s="1"/>
       <c r="AB176" s="1"/>
     </row>
-    <row r="177" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A177" s="1"/>
       <c r="B177" s="33"/>
       <c r="C177" s="76">
@@ -14253,7 +14253,7 @@
       <c r="AA177" s="1"/>
       <c r="AB177" s="1"/>
     </row>
-    <row r="178" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A178" s="1"/>
       <c r="B178" s="33"/>
       <c r="C178" s="76">
@@ -14314,7 +14314,7 @@
       <c r="AA178" s="1"/>
       <c r="AB178" s="1"/>
     </row>
-    <row r="179" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A179" s="1"/>
       <c r="B179" s="33"/>
       <c r="C179" s="76">
@@ -14375,7 +14375,7 @@
       <c r="AA179" s="1"/>
       <c r="AB179" s="1"/>
     </row>
-    <row r="180" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A180" s="1"/>
       <c r="B180" s="33"/>
       <c r="C180" s="76">
@@ -14434,7 +14434,7 @@
       <c r="AA180" s="1"/>
       <c r="AB180" s="1"/>
     </row>
-    <row r="181" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A181" s="1"/>
       <c r="B181" s="33"/>
       <c r="C181" s="76">
@@ -14491,7 +14491,7 @@
       <c r="AA181" s="1"/>
       <c r="AB181" s="1"/>
     </row>
-    <row r="182" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A182" s="1"/>
       <c r="B182" s="33"/>
       <c r="C182" s="76">
@@ -14550,7 +14550,7 @@
       <c r="AA182" s="1"/>
       <c r="AB182" s="1"/>
     </row>
-    <row r="183" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A183" s="1"/>
       <c r="B183" s="33"/>
       <c r="C183" s="76">
@@ -14611,7 +14611,7 @@
       <c r="AA183" s="1"/>
       <c r="AB183" s="1"/>
     </row>
-    <row r="184" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A184" s="1"/>
       <c r="B184" s="33"/>
       <c r="C184" s="76">
@@ -14672,7 +14672,7 @@
       <c r="AA184" s="1"/>
       <c r="AB184" s="1"/>
     </row>
-    <row r="185" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A185" s="1"/>
       <c r="B185" s="33"/>
       <c r="C185" s="76">
@@ -14731,7 +14731,7 @@
       <c r="AA185" s="1"/>
       <c r="AB185" s="1"/>
     </row>
-    <row r="186" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A186" s="1"/>
       <c r="B186" s="33"/>
       <c r="C186" s="76">
@@ -14790,7 +14790,7 @@
       <c r="AA186" s="1"/>
       <c r="AB186" s="1"/>
     </row>
-    <row r="187" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A187" s="1"/>
       <c r="B187" s="33"/>
       <c r="C187" s="76">
@@ -14849,7 +14849,7 @@
       <c r="AA187" s="1"/>
       <c r="AB187" s="1"/>
     </row>
-    <row r="188" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A188" s="1"/>
       <c r="B188" s="33"/>
       <c r="C188" s="76">
@@ -14912,7 +14912,7 @@
       <c r="AA188" s="1"/>
       <c r="AB188" s="1"/>
     </row>
-    <row r="189" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A189" s="1"/>
       <c r="B189" s="33"/>
       <c r="C189" s="76">
@@ -14971,7 +14971,7 @@
       <c r="AA189" s="1"/>
       <c r="AB189" s="1"/>
     </row>
-    <row r="190" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A190" s="1"/>
       <c r="B190" s="33"/>
       <c r="C190" s="76">
@@ -15028,7 +15028,7 @@
       <c r="AA190" s="1"/>
       <c r="AB190" s="1"/>
     </row>
-    <row r="191" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A191" s="1"/>
       <c r="B191" s="33"/>
       <c r="C191" s="76">
@@ -15085,7 +15085,7 @@
       <c r="AA191" s="1"/>
       <c r="AB191" s="1"/>
     </row>
-    <row r="192" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A192" s="1"/>
       <c r="B192" s="33"/>
       <c r="C192" s="76">
@@ -15142,7 +15142,7 @@
       <c r="AA192" s="1"/>
       <c r="AB192" s="1"/>
     </row>
-    <row r="193" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A193" s="1"/>
       <c r="B193" s="33"/>
       <c r="C193" s="76">
@@ -15201,7 +15201,7 @@
       <c r="AA193" s="1"/>
       <c r="AB193" s="1"/>
     </row>
-    <row r="194" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A194" s="1"/>
       <c r="B194" s="33"/>
       <c r="C194" s="76">
@@ -15258,7 +15258,7 @@
       <c r="AA194" s="1"/>
       <c r="AB194" s="1"/>
     </row>
-    <row r="195" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A195" s="1"/>
       <c r="B195" s="33"/>
       <c r="C195" s="76">
@@ -15315,7 +15315,7 @@
       <c r="AA195" s="1"/>
       <c r="AB195" s="1"/>
     </row>
-    <row r="196" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A196" s="1"/>
       <c r="B196" s="33"/>
       <c r="C196" s="76">
@@ -15372,7 +15372,7 @@
       <c r="AA196" s="1"/>
       <c r="AB196" s="1"/>
     </row>
-    <row r="197" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A197" s="1"/>
       <c r="B197" s="33"/>
       <c r="C197" s="76">
@@ -15429,7 +15429,7 @@
       <c r="AA197" s="1"/>
       <c r="AB197" s="1"/>
     </row>
-    <row r="198" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A198" s="1"/>
       <c r="B198" s="33"/>
       <c r="C198" s="76">
@@ -15488,7 +15488,7 @@
       <c r="AA198" s="1"/>
       <c r="AB198" s="1"/>
     </row>
-    <row r="199" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A199" s="1"/>
       <c r="B199" s="33"/>
       <c r="C199" s="76">
@@ -15545,7 +15545,7 @@
       <c r="AA199" s="1"/>
       <c r="AB199" s="1"/>
     </row>
-    <row r="200" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A200" s="1"/>
       <c r="B200" s="33"/>
       <c r="C200" s="76">
@@ -15602,7 +15602,7 @@
       <c r="AA200" s="1"/>
       <c r="AB200" s="1"/>
     </row>
-    <row r="201" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A201" s="1"/>
       <c r="B201" s="33"/>
       <c r="C201" s="76">
@@ -15659,7 +15659,7 @@
       <c r="AA201" s="1"/>
       <c r="AB201" s="1"/>
     </row>
-    <row r="202" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A202" s="1"/>
       <c r="B202" s="33"/>
       <c r="C202" s="76">
@@ -15716,7 +15716,7 @@
       <c r="AA202" s="1"/>
       <c r="AB202" s="1"/>
     </row>
-    <row r="203" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A203" s="1"/>
       <c r="B203" s="33"/>
       <c r="C203" s="76">
@@ -15775,7 +15775,7 @@
       <c r="AA203" s="1"/>
       <c r="AB203" s="1"/>
     </row>
-    <row r="204" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A204" s="1"/>
       <c r="B204" s="33"/>
       <c r="C204" s="76">
@@ -15832,7 +15832,7 @@
       <c r="AA204" s="1"/>
       <c r="AB204" s="1"/>
     </row>
-    <row r="205" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A205" s="1"/>
       <c r="B205" s="33"/>
       <c r="C205" s="76">
@@ -15889,7 +15889,7 @@
       <c r="AA205" s="1"/>
       <c r="AB205" s="1"/>
     </row>
-    <row r="206" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A206" s="1"/>
       <c r="B206" s="33"/>
       <c r="C206" s="76">
@@ -15946,7 +15946,7 @@
       <c r="AA206" s="1"/>
       <c r="AB206" s="1"/>
     </row>
-    <row r="207" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A207" s="1"/>
       <c r="B207" s="33"/>
       <c r="C207" s="76">
@@ -16003,7 +16003,7 @@
       <c r="AA207" s="1"/>
       <c r="AB207" s="1"/>
     </row>
-    <row r="208" spans="1:30" s="113" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:30" s="113" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A208" s="1"/>
       <c r="B208" s="33"/>
       <c r="C208" s="76">
@@ -16038,7 +16038,7 @@
       <c r="AC208" s="130"/>
       <c r="AD208" s="130"/>
     </row>
-    <row r="209" spans="1:28" s="133" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:28" s="133" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A209" s="1"/>
       <c r="B209" s="33"/>
       <c r="C209" s="76">
@@ -16098,7 +16098,7 @@
       <c r="AA209" s="1"/>
       <c r="AB209" s="1"/>
     </row>
-    <row r="210" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A210" s="1"/>
       <c r="B210" s="33"/>
       <c r="C210" s="76">
@@ -16168,7 +16168,7 @@
       <c r="AA210" s="1"/>
       <c r="AB210" s="1"/>
     </row>
-    <row r="211" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A211" s="1"/>
       <c r="B211" s="33"/>
       <c r="C211" s="76">
@@ -16238,7 +16238,7 @@
       <c r="AA211" s="1"/>
       <c r="AB211" s="1"/>
     </row>
-    <row r="212" spans="1:28" s="133" customFormat="1" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:28" s="133" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A212" s="1"/>
       <c r="B212" s="33"/>
       <c r="C212" s="76">
@@ -16273,7 +16273,7 @@
       <c r="AA212" s="1"/>
       <c r="AB212" s="1"/>
     </row>
-    <row r="213" spans="1:28" s="133" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:28" s="133" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A213" s="1"/>
       <c r="B213" s="33"/>
       <c r="C213" s="76">
@@ -16324,7 +16324,7 @@
       <c r="AA213" s="1"/>
       <c r="AB213" s="1"/>
     </row>
-    <row r="214" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A214" s="1"/>
       <c r="B214" s="33"/>
       <c r="C214" s="76">
@@ -16387,7 +16387,7 @@
       <c r="AA214" s="1"/>
       <c r="AB214" s="1"/>
     </row>
-    <row r="215" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A215" s="1"/>
       <c r="B215" s="33"/>
       <c r="C215" s="76">
@@ -16450,7 +16450,7 @@
       <c r="AA215" s="1"/>
       <c r="AB215" s="1"/>
     </row>
-    <row r="216" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A216" s="1"/>
       <c r="B216" s="33"/>
       <c r="C216" s="76">
@@ -16507,7 +16507,7 @@
       <c r="AA216" s="1"/>
       <c r="AB216" s="1"/>
     </row>
-    <row r="217" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A217" s="1"/>
       <c r="B217" s="33"/>
       <c r="C217" s="76">
@@ -16566,7 +16566,7 @@
       <c r="AA217" s="1"/>
       <c r="AB217" s="1"/>
     </row>
-    <row r="218" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A218" s="1"/>
       <c r="B218" s="33"/>
       <c r="C218" s="76">
@@ -16625,7 +16625,7 @@
       <c r="AA218" s="1"/>
       <c r="AB218" s="1"/>
     </row>
-    <row r="219" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A219" s="1"/>
       <c r="B219" s="33"/>
       <c r="C219" s="76">
@@ -16686,7 +16686,7 @@
       <c r="AA219" s="1"/>
       <c r="AB219" s="1"/>
     </row>
-    <row r="220" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A220" s="1"/>
       <c r="B220" s="33"/>
       <c r="C220" s="76">
@@ -16747,7 +16747,7 @@
       <c r="AA220" s="1"/>
       <c r="AB220" s="1"/>
     </row>
-    <row r="221" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A221" s="1"/>
       <c r="B221" s="33"/>
       <c r="C221" s="76">
@@ -16804,7 +16804,7 @@
       <c r="AA221" s="1"/>
       <c r="AB221" s="1"/>
     </row>
-    <row r="222" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A222" s="1"/>
       <c r="B222" s="33"/>
       <c r="C222" s="76">
@@ -16861,7 +16861,7 @@
       <c r="AA222" s="1"/>
       <c r="AB222" s="1"/>
     </row>
-    <row r="223" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A223" s="1"/>
       <c r="B223" s="33"/>
       <c r="C223" s="76">
@@ -16918,7 +16918,7 @@
       <c r="AA223" s="1"/>
       <c r="AB223" s="1"/>
     </row>
-    <row r="224" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A224" s="1"/>
       <c r="B224" s="33"/>
       <c r="C224" s="76">
@@ -16977,7 +16977,7 @@
       <c r="AA224" s="1"/>
       <c r="AB224" s="1"/>
     </row>
-    <row r="225" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A225" s="1"/>
       <c r="B225" s="33"/>
       <c r="C225" s="76">
@@ -17036,7 +17036,7 @@
       <c r="AA225" s="1"/>
       <c r="AB225" s="1"/>
     </row>
-    <row r="226" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A226" s="1"/>
       <c r="B226" s="33"/>
       <c r="C226" s="76">
@@ -17093,7 +17093,7 @@
       <c r="AA226" s="1"/>
       <c r="AB226" s="1"/>
     </row>
-    <row r="227" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A227" s="1"/>
       <c r="B227" s="33"/>
       <c r="C227" s="76">
@@ -17150,7 +17150,7 @@
       <c r="AA227" s="1"/>
       <c r="AB227" s="1"/>
     </row>
-    <row r="228" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A228" s="1"/>
       <c r="B228" s="33"/>
       <c r="C228" s="76">
@@ -17207,7 +17207,7 @@
       <c r="AA228" s="1"/>
       <c r="AB228" s="1"/>
     </row>
-    <row r="229" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A229" s="1"/>
       <c r="B229" s="33"/>
       <c r="C229" s="76">
@@ -17266,7 +17266,7 @@
       <c r="AA229" s="1"/>
       <c r="AB229" s="1"/>
     </row>
-    <row r="230" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A230" s="1"/>
       <c r="B230" s="33"/>
       <c r="C230" s="76">
@@ -17325,7 +17325,7 @@
       <c r="AA230" s="1"/>
       <c r="AB230" s="1"/>
     </row>
-    <row r="231" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A231" s="1"/>
       <c r="B231" s="33"/>
       <c r="C231" s="76">
@@ -17382,7 +17382,7 @@
       <c r="AA231" s="1"/>
       <c r="AB231" s="1"/>
     </row>
-    <row r="232" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A232" s="1"/>
       <c r="B232" s="33"/>
       <c r="C232" s="76">
@@ -17439,7 +17439,7 @@
       <c r="AA232" s="1"/>
       <c r="AB232" s="1"/>
     </row>
-    <row r="233" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A233" s="1"/>
       <c r="B233" s="33"/>
       <c r="C233" s="76">
@@ -17496,7 +17496,7 @@
       <c r="AA233" s="1"/>
       <c r="AB233" s="1"/>
     </row>
-    <row r="234" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A234" s="1"/>
       <c r="B234" s="33"/>
       <c r="C234" s="76">
@@ -17566,7 +17566,7 @@
       <c r="AA234" s="1"/>
       <c r="AB234" s="1"/>
     </row>
-    <row r="235" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A235" s="1"/>
       <c r="B235" s="33"/>
       <c r="C235" s="76">
@@ -17633,7 +17633,7 @@
       <c r="AA235" s="1"/>
       <c r="AB235" s="1"/>
     </row>
-    <row r="236" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A236" s="1"/>
       <c r="B236" s="33"/>
       <c r="C236" s="76">
@@ -17696,7 +17696,7 @@
       <c r="AA236" s="1"/>
       <c r="AB236" s="1"/>
     </row>
-    <row r="237" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A237" s="1"/>
       <c r="B237" s="33"/>
       <c r="C237" s="76">
@@ -17759,7 +17759,7 @@
       <c r="AA237" s="1"/>
       <c r="AB237" s="1"/>
     </row>
-    <row r="238" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A238" s="1"/>
       <c r="B238" s="33"/>
       <c r="C238" s="76">
@@ -17826,7 +17826,7 @@
       <c r="AA238" s="1"/>
       <c r="AB238" s="1"/>
     </row>
-    <row r="239" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A239" s="1"/>
       <c r="B239" s="33"/>
       <c r="C239" s="76">
@@ -17895,7 +17895,7 @@
       <c r="AA239" s="1"/>
       <c r="AB239" s="1"/>
     </row>
-    <row r="240" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A240" s="1"/>
       <c r="B240" s="33"/>
       <c r="C240" s="76">
@@ -17962,7 +17962,7 @@
       <c r="AA240" s="1"/>
       <c r="AB240" s="1"/>
     </row>
-    <row r="241" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A241" s="1"/>
       <c r="B241" s="33"/>
       <c r="C241" s="76">
@@ -18029,7 +18029,7 @@
       <c r="AA241" s="1"/>
       <c r="AB241" s="1"/>
     </row>
-    <row r="242" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A242" s="1"/>
       <c r="B242" s="33"/>
       <c r="C242" s="76">
@@ -18096,7 +18096,7 @@
       <c r="AA242" s="1"/>
       <c r="AB242" s="1"/>
     </row>
-    <row r="243" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A243" s="1"/>
       <c r="B243" s="33"/>
       <c r="C243" s="76">
@@ -18163,7 +18163,7 @@
       <c r="AA243" s="1"/>
       <c r="AB243" s="1"/>
     </row>
-    <row r="244" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A244" s="1"/>
       <c r="B244" s="33"/>
       <c r="C244" s="76">
@@ -18232,7 +18232,7 @@
       <c r="AA244" s="1"/>
       <c r="AB244" s="1"/>
     </row>
-    <row r="245" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A245" s="1"/>
       <c r="B245" s="33"/>
       <c r="C245" s="76">
@@ -18299,7 +18299,7 @@
       <c r="AA245" s="1"/>
       <c r="AB245" s="1"/>
     </row>
-    <row r="246" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A246" s="1"/>
       <c r="B246" s="33"/>
       <c r="C246" s="76">
@@ -18366,7 +18366,7 @@
       <c r="AA246" s="1"/>
       <c r="AB246" s="1"/>
     </row>
-    <row r="247" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A247" s="1"/>
       <c r="B247" s="33"/>
       <c r="C247" s="76">
@@ -18433,7 +18433,7 @@
       <c r="AA247" s="1"/>
       <c r="AB247" s="1"/>
     </row>
-    <row r="248" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A248" s="1"/>
       <c r="B248" s="33"/>
       <c r="C248" s="76">
@@ -18500,7 +18500,7 @@
       <c r="AA248" s="1"/>
       <c r="AB248" s="1"/>
     </row>
-    <row r="249" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A249" s="1"/>
       <c r="B249" s="33"/>
       <c r="C249" s="76">
@@ -18569,7 +18569,7 @@
       <c r="AA249" s="1"/>
       <c r="AB249" s="1"/>
     </row>
-    <row r="250" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A250" s="1"/>
       <c r="B250" s="33"/>
       <c r="C250" s="76">
@@ -18636,7 +18636,7 @@
       <c r="AA250" s="1"/>
       <c r="AB250" s="1"/>
     </row>
-    <row r="251" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A251" s="1"/>
       <c r="B251" s="33"/>
       <c r="C251" s="76">
@@ -18703,7 +18703,7 @@
       <c r="AA251" s="1"/>
       <c r="AB251" s="1"/>
     </row>
-    <row r="252" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A252" s="1"/>
       <c r="B252" s="33"/>
       <c r="C252" s="76">
@@ -18770,7 +18770,7 @@
       <c r="AA252" s="1"/>
       <c r="AB252" s="1"/>
     </row>
-    <row r="253" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A253" s="1"/>
       <c r="B253" s="33"/>
       <c r="C253" s="76">
@@ -18837,7 +18837,7 @@
       <c r="AA253" s="1"/>
       <c r="AB253" s="1"/>
     </row>
-    <row r="254" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A254" s="1"/>
       <c r="B254" s="33"/>
       <c r="C254" s="76">
@@ -18898,7 +18898,7 @@
       <c r="AA254" s="1"/>
       <c r="AB254" s="1"/>
     </row>
-    <row r="255" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A255" s="1"/>
       <c r="B255" s="33"/>
       <c r="C255" s="76">
@@ -18955,7 +18955,7 @@
       <c r="AA255" s="1"/>
       <c r="AB255" s="1"/>
     </row>
-    <row r="256" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A256" s="1"/>
       <c r="B256" s="33"/>
       <c r="C256" s="76">
@@ -19012,7 +19012,7 @@
       <c r="AA256" s="1"/>
       <c r="AB256" s="1"/>
     </row>
-    <row r="257" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A257" s="1"/>
       <c r="B257" s="33"/>
       <c r="C257" s="76">
@@ -19069,7 +19069,7 @@
       <c r="AA257" s="1"/>
       <c r="AB257" s="1"/>
     </row>
-    <row r="258" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A258" s="1"/>
       <c r="B258" s="33"/>
       <c r="C258" s="76">
@@ -19126,7 +19126,7 @@
       <c r="AA258" s="1"/>
       <c r="AB258" s="1"/>
     </row>
-    <row r="259" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A259" s="1"/>
       <c r="B259" s="33"/>
       <c r="C259" s="76">
@@ -19195,7 +19195,7 @@
       <c r="AA259" s="1"/>
       <c r="AB259" s="1"/>
     </row>
-    <row r="260" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A260" s="1"/>
       <c r="B260" s="33"/>
       <c r="C260" s="76">
@@ -19262,7 +19262,7 @@
       <c r="AA260" s="1"/>
       <c r="AB260" s="1"/>
     </row>
-    <row r="261" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A261" s="1"/>
       <c r="B261" s="33"/>
       <c r="C261" s="76">
@@ -19329,7 +19329,7 @@
       <c r="AA261" s="1"/>
       <c r="AB261" s="1"/>
     </row>
-    <row r="262" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A262" s="1"/>
       <c r="B262" s="33"/>
       <c r="C262" s="76">
@@ -19396,7 +19396,7 @@
       <c r="AA262" s="1"/>
       <c r="AB262" s="1"/>
     </row>
-    <row r="263" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A263" s="1"/>
       <c r="B263" s="33"/>
       <c r="C263" s="76">
@@ -19463,7 +19463,7 @@
       <c r="AA263" s="1"/>
       <c r="AB263" s="1"/>
     </row>
-    <row r="264" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A264" s="1"/>
       <c r="B264" s="33"/>
       <c r="C264" s="76">
@@ -19522,7 +19522,7 @@
       <c r="AA264" s="1"/>
       <c r="AB264" s="1"/>
     </row>
-    <row r="265" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A265" s="1"/>
       <c r="B265" s="33"/>
       <c r="C265" s="76">
@@ -19584,7 +19584,7 @@
       <c r="AA265" s="1"/>
       <c r="AB265" s="1"/>
     </row>
-    <row r="266" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A266" s="1"/>
       <c r="B266" s="33"/>
       <c r="C266" s="76">
@@ -19645,7 +19645,7 @@
       <c r="AA266" s="1"/>
       <c r="AB266" s="1"/>
     </row>
-    <row r="267" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A267" s="1"/>
       <c r="B267" s="33"/>
       <c r="C267" s="76">
@@ -19705,7 +19705,7 @@
       <c r="AA267" s="1"/>
       <c r="AB267" s="1"/>
     </row>
-    <row r="268" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A268" s="1"/>
       <c r="B268" s="33"/>
       <c r="C268" s="76">
@@ -19772,7 +19772,7 @@
       <c r="AA268" s="1"/>
       <c r="AB268" s="1"/>
     </row>
-    <row r="269" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A269" s="1"/>
       <c r="B269" s="33"/>
       <c r="C269" s="76">
@@ -19837,7 +19837,7 @@
       <c r="AA269" s="1"/>
       <c r="AB269" s="1"/>
     </row>
-    <row r="270" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A270" s="1"/>
       <c r="B270" s="33"/>
       <c r="C270" s="76">
@@ -19899,7 +19899,7 @@
       <c r="AA270" s="1"/>
       <c r="AB270" s="1"/>
     </row>
-    <row r="271" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A271" s="1"/>
       <c r="B271" s="33"/>
       <c r="C271" s="76">
@@ -19959,7 +19959,7 @@
       <c r="AA271" s="1"/>
       <c r="AB271" s="1"/>
     </row>
-    <row r="272" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A272" s="1"/>
       <c r="B272" s="33"/>
       <c r="C272" s="76">
@@ -20016,7 +20016,7 @@
       <c r="AA272" s="1"/>
       <c r="AB272" s="1"/>
     </row>
-    <row r="273" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A273" s="1"/>
       <c r="B273" s="33"/>
       <c r="C273" s="76">
@@ -20083,7 +20083,7 @@
       <c r="AA273" s="1"/>
       <c r="AB273" s="1"/>
     </row>
-    <row r="274" spans="1:28" s="133" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:28" s="133" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A274" s="1"/>
       <c r="B274" s="33"/>
       <c r="C274" s="76">
@@ -20116,7 +20116,7 @@
       <c r="AA274" s="1"/>
       <c r="AB274" s="1"/>
     </row>
-    <row r="275" spans="1:28" s="133" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:28" s="133" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A275" s="1"/>
       <c r="B275" s="33"/>
       <c r="C275" s="76">
@@ -20172,7 +20172,7 @@
       <c r="AA275" s="1"/>
       <c r="AB275" s="1"/>
     </row>
-    <row r="276" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A276" s="1"/>
       <c r="B276" s="33"/>
       <c r="C276" s="76">
@@ -20225,7 +20225,7 @@
       <c r="AA276" s="1"/>
       <c r="AB276" s="1"/>
     </row>
-    <row r="277" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A277" s="1"/>
       <c r="B277" s="33"/>
       <c r="C277" s="76">
@@ -20278,7 +20278,7 @@
       <c r="AA277" s="1"/>
       <c r="AB277" s="1"/>
     </row>
-    <row r="278" spans="1:28" s="133" customFormat="1" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:28" s="133" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A278" s="1"/>
       <c r="B278" s="33"/>
       <c r="C278" s="76">
@@ -20313,7 +20313,7 @@
       <c r="AA278" s="1"/>
       <c r="AB278" s="1"/>
     </row>
-    <row r="279" spans="1:28" s="133" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:28" s="133" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A279" s="1"/>
       <c r="B279" s="33"/>
       <c r="C279" s="76">
@@ -20363,7 +20363,7 @@
       <c r="AA279" s="1"/>
       <c r="AB279" s="1"/>
     </row>
-    <row r="280" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A280" s="1"/>
       <c r="B280" s="33"/>
       <c r="C280" s="76">
@@ -20421,7 +20421,7 @@
       <c r="AA280" s="1"/>
       <c r="AB280" s="1"/>
     </row>
-    <row r="281" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A281" s="1"/>
       <c r="B281" s="33"/>
       <c r="C281" s="76">
@@ -20479,7 +20479,7 @@
       <c r="AA281" s="1"/>
       <c r="AB281" s="1"/>
     </row>
-    <row r="282" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A282" s="1"/>
       <c r="B282" s="33"/>
       <c r="C282" s="76">
@@ -20532,7 +20532,7 @@
       <c r="AA282" s="1"/>
       <c r="AB282" s="1"/>
     </row>
-    <row r="283" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A283" s="1"/>
       <c r="B283" s="33"/>
       <c r="C283" s="76">
@@ -20584,7 +20584,7 @@
       <c r="AA283" s="1"/>
       <c r="AB283" s="1"/>
     </row>
-    <row r="284" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A284" s="1"/>
       <c r="B284" s="33"/>
       <c r="C284" s="76">
@@ -20639,7 +20639,7 @@
       <c r="AA284" s="1"/>
       <c r="AB284" s="1"/>
     </row>
-    <row r="285" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A285" s="1"/>
       <c r="B285" s="33"/>
       <c r="C285" s="76">
@@ -20693,7 +20693,7 @@
       <c r="AA285" s="1"/>
       <c r="AB285" s="1"/>
     </row>
-    <row r="286" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A286" s="1"/>
       <c r="B286" s="33"/>
       <c r="C286" s="76">
@@ -20747,7 +20747,7 @@
       <c r="AA286" s="1"/>
       <c r="AB286" s="1"/>
     </row>
-    <row r="287" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A287" s="1"/>
       <c r="B287" s="33"/>
       <c r="C287" s="76">
@@ -20797,7 +20797,7 @@
       <c r="AA287" s="1"/>
       <c r="AB287" s="1"/>
     </row>
-    <row r="288" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A288" s="1"/>
       <c r="B288" s="33"/>
       <c r="C288" s="76">
@@ -20847,7 +20847,7 @@
       <c r="AA288" s="1"/>
       <c r="AB288" s="1"/>
     </row>
-    <row r="289" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A289" s="1"/>
       <c r="B289" s="33"/>
       <c r="C289" s="76">
@@ -20900,7 +20900,7 @@
       <c r="AA289" s="1"/>
       <c r="AB289" s="1"/>
     </row>
-    <row r="290" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A290" s="1"/>
       <c r="B290" s="33"/>
       <c r="C290" s="76">
@@ -20954,7 +20954,7 @@
       <c r="AA290" s="1"/>
       <c r="AB290" s="1"/>
     </row>
-    <row r="291" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A291" s="1"/>
       <c r="B291" s="33"/>
       <c r="C291" s="76">
@@ -21008,7 +21008,7 @@
       <c r="AA291" s="1"/>
       <c r="AB291" s="1"/>
     </row>
-    <row r="292" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A292" s="1"/>
       <c r="B292" s="33"/>
       <c r="C292" s="76">
@@ -21058,7 +21058,7 @@
       <c r="AA292" s="1"/>
       <c r="AB292" s="1"/>
     </row>
-    <row r="293" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A293" s="1"/>
       <c r="B293" s="33"/>
       <c r="C293" s="76">
@@ -21108,7 +21108,7 @@
       <c r="AA293" s="1"/>
       <c r="AB293" s="1"/>
     </row>
-    <row r="294" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A294" s="1"/>
       <c r="B294" s="33"/>
       <c r="C294" s="76">
@@ -21161,7 +21161,7 @@
       <c r="AA294" s="1"/>
       <c r="AB294" s="1"/>
     </row>
-    <row r="295" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A295" s="1"/>
       <c r="B295" s="33"/>
       <c r="C295" s="76">
@@ -21213,7 +21213,7 @@
       <c r="AA295" s="1"/>
       <c r="AB295" s="1"/>
     </row>
-    <row r="296" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A296" s="1"/>
       <c r="B296" s="33"/>
       <c r="C296" s="76">
@@ -21265,7 +21265,7 @@
       <c r="AA296" s="1"/>
       <c r="AB296" s="1"/>
     </row>
-    <row r="297" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A297" s="1"/>
       <c r="B297" s="33"/>
       <c r="C297" s="76">
@@ -21314,7 +21314,7 @@
       <c r="AA297" s="1"/>
       <c r="AB297" s="1"/>
     </row>
-    <row r="298" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A298" s="1"/>
       <c r="B298" s="33"/>
       <c r="C298" s="76">
@@ -21361,7 +21361,7 @@
       <c r="AA298" s="1"/>
       <c r="AB298" s="1"/>
     </row>
-    <row r="299" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A299" s="1"/>
       <c r="B299" s="33"/>
       <c r="C299" s="76">
@@ -21414,7 +21414,7 @@
       <c r="AA299" s="1"/>
       <c r="AB299" s="1"/>
     </row>
-    <row r="300" spans="1:28" s="133" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:28" s="133" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A300" s="1"/>
       <c r="B300" s="33"/>
       <c r="C300" s="76">
@@ -21447,7 +21447,7 @@
       <c r="AA300" s="1"/>
       <c r="AB300" s="1"/>
     </row>
-    <row r="301" spans="1:28" s="99" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:28" s="99" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A301" s="1"/>
       <c r="B301" s="33"/>
       <c r="C301" s="76">
@@ -21480,7 +21480,7 @@
       <c r="AA301" s="1"/>
       <c r="AB301" s="1"/>
     </row>
-    <row r="302" spans="1:28" s="99" customFormat="1" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:28" s="99" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A302" s="1"/>
       <c r="B302" s="35"/>
       <c r="C302" s="79">
@@ -21515,7 +21515,7 @@
       <c r="AA302" s="1"/>
       <c r="AB302" s="1"/>
     </row>
-    <row r="303" spans="1:28" s="99" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:28" s="99" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A303" s="1"/>
       <c r="B303" s="19"/>
       <c r="C303" s="80">
@@ -21548,7 +21548,7 @@
       <c r="AA303" s="1"/>
       <c r="AB303" s="1"/>
     </row>
-    <row r="304" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A304" s="1"/>
       <c r="B304" s="1"/>
       <c r="C304" s="76">
@@ -21581,7 +21581,7 @@
       <c r="AA304" s="1"/>
       <c r="AB304" s="1"/>
     </row>
-    <row r="305" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A305" s="1"/>
       <c r="B305" s="1"/>
       <c r="C305" s="76">
@@ -21614,7 +21614,7 @@
       <c r="AA305" s="1"/>
       <c r="AB305" s="1"/>
     </row>
-    <row r="306" spans="1:28" s="101" customFormat="1" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="306" spans="1:28" s="101" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A306" s="1"/>
       <c r="B306" s="20"/>
       <c r="C306" s="77">
@@ -21647,7 +21647,7 @@
       <c r="AA306" s="1"/>
       <c r="AB306" s="1"/>
     </row>
-    <row r="307" spans="1:28" s="101" customFormat="1" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:28" s="101" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A307" s="1"/>
       <c r="B307" s="34" t="s">
         <v>21</v>
@@ -21682,7 +21682,7 @@
       <c r="AA307" s="1"/>
       <c r="AB307" s="1"/>
     </row>
-    <row r="308" spans="1:28" s="101" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:28" s="101" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.3">
       <c r="A308" s="1"/>
       <c r="B308" s="33"/>
       <c r="C308" s="76">
@@ -21715,7 +21715,7 @@
       <c r="AA308" s="1"/>
       <c r="AB308" s="1"/>
     </row>
-    <row r="309" spans="1:28" s="101" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:28" s="101" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A309" s="1"/>
       <c r="B309" s="33"/>
       <c r="C309" s="76">
@@ -21752,7 +21752,7 @@
       <c r="AA309" s="1"/>
       <c r="AB309" s="1"/>
     </row>
-    <row r="310" spans="1:28" s="101" customFormat="1" ht="20.149999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:28" s="101" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A310" s="1"/>
       <c r="B310" s="33"/>
       <c r="C310" s="76">
@@ -21791,7 +21791,7 @@
       <c r="AA310" s="1"/>
       <c r="AB310" s="1"/>
     </row>
-    <row r="311" spans="1:28" s="101" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:28" s="101" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A311" s="1"/>
       <c r="B311" s="33"/>
       <c r="C311" s="76">
@@ -21824,7 +21824,7 @@
       <c r="AA311" s="1"/>
       <c r="AB311" s="1"/>
     </row>
-    <row r="312" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A312" s="1"/>
       <c r="B312" s="33"/>
       <c r="C312" s="76">
@@ -21857,7 +21857,7 @@
       <c r="AA312" s="1"/>
       <c r="AB312" s="1"/>
     </row>
-    <row r="313" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A313" s="1"/>
       <c r="B313" s="33"/>
       <c r="C313" s="76">
@@ -21890,7 +21890,7 @@
       <c r="AA313" s="1"/>
       <c r="AB313" s="1"/>
     </row>
-    <row r="314" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A314" s="1"/>
       <c r="B314" s="33"/>
       <c r="C314" s="76">
@@ -21923,7 +21923,7 @@
       <c r="AA314" s="1"/>
       <c r="AB314" s="1"/>
     </row>
-    <row r="315" spans="1:28" s="101" customFormat="1" ht="28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:28" s="101" customFormat="1" ht="27.6" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A315" s="1"/>
       <c r="B315" s="33"/>
       <c r="C315" s="76">
@@ -21966,7 +21966,7 @@
       <c r="AA315" s="1"/>
       <c r="AB315" s="1"/>
     </row>
-    <row r="316" spans="1:28" s="101" customFormat="1" ht="11.5" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:28" s="101" customFormat="1" ht="11.4" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A316" s="1"/>
       <c r="B316" s="33" t="s">
         <v>20</v>
@@ -22001,7 +22001,7 @@
       <c r="AA316" s="1"/>
       <c r="AB316" s="1"/>
     </row>
-    <row r="317" spans="1:28" s="101" customFormat="1" ht="13" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:28" s="101" customFormat="1" ht="12.9" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.3">
       <c r="A317" s="1"/>
       <c r="B317" s="33"/>
       <c r="C317" s="76">
@@ -22034,7 +22034,7 @@
       <c r="AA317" s="1"/>
       <c r="AB317" s="1"/>
     </row>
-    <row r="318" spans="1:28" s="101" customFormat="1" ht="8.5" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:28" s="101" customFormat="1" ht="8.4" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.3">
       <c r="A318" s="1"/>
       <c r="B318" s="33" t="s">
         <v>19</v>
@@ -22071,7 +22071,7 @@
       <c r="AA318" s="1"/>
       <c r="AB318" s="1"/>
     </row>
-    <row r="319" spans="1:28" s="101" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:28" s="101" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A319" s="1"/>
       <c r="B319" s="33"/>
       <c r="C319" s="76">
@@ -22106,7 +22106,7 @@
       <c r="AA319" s="1"/>
       <c r="AB319" s="1"/>
     </row>
-    <row r="320" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A320" s="1"/>
       <c r="B320" s="33"/>
       <c r="C320" s="76">
@@ -22127,7 +22127,7 @@
       <c r="K320" s="2"/>
       <c r="L320" s="132">
         <f>i_w_start_len1*i_n1_len^L323</f>
-        <v>243</v>
+        <v>81</v>
       </c>
       <c r="M320" s="2"/>
       <c r="N320" s="127" t="s">
@@ -22153,7 +22153,7 @@
       <c r="AA320" s="1"/>
       <c r="AB320" s="1"/>
     </row>
-    <row r="321" spans="1:31" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:31" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A321" s="1"/>
       <c r="B321" s="33"/>
       <c r="C321" s="76"/>
@@ -22192,7 +22192,7 @@
       <c r="AA321" s="1"/>
       <c r="AB321" s="1"/>
     </row>
-    <row r="322" spans="1:31" s="101" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:31" s="101" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A322" s="1"/>
       <c r="B322" s="33"/>
       <c r="C322" s="76">
@@ -22233,7 +22233,7 @@
       <c r="AA322" s="1"/>
       <c r="AB322" s="1"/>
     </row>
-    <row r="323" spans="1:31" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:31" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A323" s="1"/>
       <c r="B323" s="33"/>
       <c r="C323" s="76"/>
@@ -22251,7 +22251,7 @@
       <c r="K323" s="2"/>
       <c r="L323" s="132">
         <f>COUNTIF(J341:O341,TRUE)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M323" s="2"/>
       <c r="N323" s="2"/>
@@ -22275,7 +22275,7 @@
       <c r="AA323" s="1"/>
       <c r="AB323" s="1"/>
     </row>
-    <row r="324" spans="1:31" s="101" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:31" s="101" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A324" s="1"/>
       <c r="B324" s="33"/>
       <c r="C324" s="76">
@@ -22318,7 +22318,7 @@
       <c r="AA324" s="1"/>
       <c r="AB324" s="1"/>
     </row>
-    <row r="325" spans="1:31" s="111" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:31" s="111" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A325" s="1"/>
       <c r="B325" s="33"/>
       <c r="C325" s="76">
@@ -22361,7 +22361,7 @@
       <c r="AA325" s="1"/>
       <c r="AB325" s="1"/>
     </row>
-    <row r="326" spans="1:31" s="131" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:31" s="131" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A326" s="1"/>
       <c r="B326" s="33"/>
       <c r="C326" s="76">
@@ -22402,7 +22402,7 @@
       <c r="AA326" s="1"/>
       <c r="AB326" s="1"/>
     </row>
-    <row r="327" spans="1:31" s="125" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:31" s="125" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A327" s="1"/>
       <c r="B327" s="33"/>
       <c r="C327" s="76">
@@ -22450,7 +22450,7 @@
       <c r="AD327" s="130"/>
       <c r="AE327" s="130"/>
     </row>
-    <row r="328" spans="1:31" s="111" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:31" s="111" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A328" s="1"/>
       <c r="B328" s="33"/>
       <c r="C328" s="76">
@@ -22501,7 +22501,7 @@
       <c r="AA328" s="1"/>
       <c r="AB328" s="1"/>
     </row>
-    <row r="329" spans="1:31" s="111" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:31" s="111" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A329" s="1"/>
       <c r="B329" s="33"/>
       <c r="C329" s="76">
@@ -22546,7 +22546,7 @@
       <c r="AA329" s="1"/>
       <c r="AB329" s="1"/>
     </row>
-    <row r="330" spans="1:31" s="111" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:31" s="111" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A330" s="1"/>
       <c r="B330" s="33"/>
       <c r="C330" s="76">
@@ -22591,7 +22591,7 @@
       <c r="AA330" s="1"/>
       <c r="AB330" s="1"/>
     </row>
-    <row r="331" spans="1:31" s="111" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:31" s="111" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A331" s="1"/>
       <c r="B331" s="33"/>
       <c r="C331" s="76">
@@ -22636,7 +22636,7 @@
       <c r="AA331" s="1"/>
       <c r="AB331" s="1"/>
     </row>
-    <row r="332" spans="1:31" s="111" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:31" s="111" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A332" s="1"/>
       <c r="B332" s="33"/>
       <c r="C332" s="76">
@@ -22681,7 +22681,7 @@
       <c r="AA332" s="1"/>
       <c r="AB332" s="1"/>
     </row>
-    <row r="333" spans="1:31" s="111" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:31" s="111" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A333" s="1"/>
       <c r="B333" s="33"/>
       <c r="C333" s="76">
@@ -22726,7 +22726,7 @@
       <c r="AA333" s="1"/>
       <c r="AB333" s="1"/>
     </row>
-    <row r="334" spans="1:31" s="111" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:31" s="111" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A334" s="1"/>
       <c r="B334" s="33"/>
       <c r="C334" s="76">
@@ -22767,7 +22767,7 @@
       <c r="AA334" s="1"/>
       <c r="AB334" s="1"/>
     </row>
-    <row r="335" spans="1:31" s="111" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:31" s="111" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A335" s="1"/>
       <c r="B335" s="33"/>
       <c r="C335" s="76">
@@ -22808,7 +22808,7 @@
       <c r="AA335" s="1"/>
       <c r="AB335" s="1"/>
     </row>
-    <row r="336" spans="1:31" s="101" customFormat="1" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:31" s="101" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A336" s="1"/>
       <c r="B336" s="33"/>
       <c r="C336" s="76">
@@ -22843,7 +22843,7 @@
       <c r="AA336" s="1"/>
       <c r="AB336" s="1"/>
     </row>
-    <row r="337" spans="1:28" s="155" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:28" s="155" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A337" s="1"/>
       <c r="B337" s="33"/>
       <c r="C337" s="76">
@@ -22878,7 +22878,7 @@
       <c r="AA337" s="1"/>
       <c r="AB337" s="1"/>
     </row>
-    <row r="338" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A338" s="1"/>
       <c r="B338" s="33"/>
       <c r="C338" s="76">
@@ -22913,7 +22913,7 @@
       <c r="AA338" s="1"/>
       <c r="AB338" s="1"/>
     </row>
-    <row r="339" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A339" s="1"/>
       <c r="B339" s="33"/>
       <c r="C339" s="76">
@@ -22958,7 +22958,7 @@
       <c r="AA339" s="1"/>
       <c r="AB339" s="1"/>
     </row>
-    <row r="340" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A340" s="1"/>
       <c r="B340" s="33"/>
       <c r="C340" s="76">
@@ -23005,7 +23005,7 @@
       <c r="AA340" s="1"/>
       <c r="AB340" s="1"/>
     </row>
-    <row r="341" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A341" s="1"/>
       <c r="B341" s="33"/>
       <c r="C341" s="76">
@@ -23035,7 +23035,7 @@
         <v>1</v>
       </c>
       <c r="N341" s="31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O341" s="31" t="b">
         <v>0</v>
@@ -23057,7 +23057,7 @@
       <c r="AA341" s="1"/>
       <c r="AB341" s="1"/>
     </row>
-    <row r="342" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A342" s="1"/>
       <c r="B342" s="33"/>
       <c r="C342" s="76"/>
@@ -23087,11 +23087,11 @@
       </c>
       <c r="N342" s="132">
         <f>COUNTIF($J$341:N341,TRUE)-1</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O342" s="132">
         <f>COUNTIF($J$341:O341,TRUE)-1</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P342" s="2"/>
       <c r="Q342" s="2"/>
@@ -23107,7 +23107,7 @@
       <c r="AA342" s="1"/>
       <c r="AB342" s="1"/>
     </row>
-    <row r="343" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A343" s="1"/>
       <c r="B343" s="33"/>
       <c r="C343" s="76">
@@ -23156,7 +23156,7 @@
       <c r="AA343" s="1"/>
       <c r="AB343" s="1"/>
     </row>
-    <row r="344" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A344" s="1"/>
       <c r="B344" s="33"/>
       <c r="C344" s="76"/>
@@ -23200,7 +23200,7 @@
       <c r="AA344" s="1"/>
       <c r="AB344" s="1"/>
     </row>
-    <row r="345" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A345" s="1"/>
       <c r="B345" s="33"/>
       <c r="C345" s="76">
@@ -23239,7 +23239,7 @@
       <c r="AA345" s="1"/>
       <c r="AB345" s="1"/>
     </row>
-    <row r="346" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A346" s="1"/>
       <c r="B346" s="33"/>
       <c r="C346" s="76">
@@ -23278,7 +23278,7 @@
       <c r="AA346" s="1"/>
       <c r="AB346" s="1"/>
     </row>
-    <row r="347" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A347" s="1"/>
       <c r="B347" s="33"/>
       <c r="C347" s="76">
@@ -23319,7 +23319,7 @@
       <c r="AA347" s="1"/>
       <c r="AB347" s="1"/>
     </row>
-    <row r="348" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A348" s="1"/>
       <c r="B348" s="33"/>
       <c r="C348" s="76"/>
@@ -23360,7 +23360,7 @@
       <c r="AA348" s="1"/>
       <c r="AB348" s="1"/>
     </row>
-    <row r="349" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A349" s="1"/>
       <c r="B349" s="33"/>
       <c r="C349" s="76"/>
@@ -23390,7 +23390,7 @@
       <c r="AA349" s="1"/>
       <c r="AB349" s="1"/>
     </row>
-    <row r="350" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A350" s="1"/>
       <c r="B350" s="33"/>
       <c r="C350" s="76">
@@ -23425,7 +23425,7 @@
       <c r="AA350" s="1"/>
       <c r="AB350" s="1"/>
     </row>
-    <row r="351" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A351" s="1"/>
       <c r="B351" s="33"/>
       <c r="C351" s="76">
@@ -23466,7 +23466,7 @@
       <c r="AA351" s="1"/>
       <c r="AB351" s="1"/>
     </row>
-    <row r="352" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A352" s="1"/>
       <c r="B352" s="33"/>
       <c r="C352" s="76">
@@ -23509,7 +23509,7 @@
       <c r="AA352" s="1"/>
       <c r="AB352" s="1"/>
     </row>
-    <row r="353" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A353" s="1"/>
       <c r="B353" s="33"/>
       <c r="C353" s="76">
@@ -23557,7 +23557,7 @@
       <c r="AA353" s="1"/>
       <c r="AB353" s="1"/>
     </row>
-    <row r="354" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A354" s="1"/>
       <c r="B354" s="33"/>
       <c r="C354" s="76"/>
@@ -23601,7 +23601,7 @@
       <c r="AA354" s="1"/>
       <c r="AB354" s="1"/>
     </row>
-    <row r="355" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A355" s="1"/>
       <c r="B355" s="33"/>
       <c r="C355" s="76">
@@ -23646,7 +23646,7 @@
       <c r="AA355" s="1"/>
       <c r="AB355" s="1"/>
     </row>
-    <row r="356" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A356" s="1"/>
       <c r="B356" s="33"/>
       <c r="C356" s="76">
@@ -23679,7 +23679,7 @@
       <c r="AA356" s="1"/>
       <c r="AB356" s="1"/>
     </row>
-    <row r="357" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A357" s="1"/>
       <c r="B357" s="33"/>
       <c r="C357" s="76">
@@ -23714,7 +23714,7 @@
       <c r="AA357" s="1"/>
       <c r="AB357" s="1"/>
     </row>
-    <row r="358" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A358" s="1"/>
       <c r="B358" s="33"/>
       <c r="C358" s="76">
@@ -23749,7 +23749,7 @@
       <c r="AA358" s="1"/>
       <c r="AB358" s="1"/>
     </row>
-    <row r="359" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:28" s="155" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A359" s="1"/>
       <c r="B359" s="33"/>
       <c r="C359" s="76">
@@ -23784,7 +23784,7 @@
       <c r="AA359" s="1"/>
       <c r="AB359" s="1"/>
     </row>
-    <row r="360" spans="1:28" s="155" customFormat="1" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:28" s="155" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A360" s="1"/>
       <c r="B360" s="33"/>
       <c r="C360" s="76">
@@ -23819,7 +23819,7 @@
       <c r="AA360" s="1"/>
       <c r="AB360" s="1"/>
     </row>
-    <row r="361" spans="1:28" s="102" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:28" s="102" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A361" s="1"/>
       <c r="B361" s="33"/>
       <c r="C361" s="76">
@@ -23854,7 +23854,7 @@
       <c r="AA361" s="1"/>
       <c r="AB361" s="1"/>
     </row>
-    <row r="362" spans="1:28" s="102" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:28" s="102" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A362" s="1"/>
       <c r="B362" s="33"/>
       <c r="C362" s="76">
@@ -23895,7 +23895,7 @@
       <c r="AA362" s="1"/>
       <c r="AB362" s="1"/>
     </row>
-    <row r="363" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A363" s="1"/>
       <c r="B363" s="33"/>
       <c r="C363" s="76"/>
@@ -23949,7 +23949,7 @@
       <c r="AA363" s="1"/>
       <c r="AB363" s="1"/>
     </row>
-    <row r="364" spans="1:28" s="102" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:28" s="102" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A364" s="1"/>
       <c r="B364" s="33"/>
       <c r="C364" s="76">
@@ -24010,7 +24010,7 @@
       <c r="AA364" s="1"/>
       <c r="AB364" s="1"/>
     </row>
-    <row r="365" spans="1:28" s="130" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:28" s="130" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A365" s="1"/>
       <c r="B365" s="33"/>
       <c r="C365" s="76">
@@ -24063,7 +24063,7 @@
       <c r="AA365" s="1"/>
       <c r="AB365" s="1"/>
     </row>
-    <row r="366" spans="1:28" s="130" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:28" s="130" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A366" s="1"/>
       <c r="B366" s="33"/>
       <c r="C366" s="76">
@@ -24116,7 +24116,7 @@
       <c r="AA366" s="1"/>
       <c r="AB366" s="1"/>
     </row>
-    <row r="367" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A367" s="1"/>
       <c r="B367" s="33"/>
       <c r="C367" s="76"/>
@@ -24146,7 +24146,7 @@
       <c r="AA367" s="1"/>
       <c r="AB367" s="1"/>
     </row>
-    <row r="368" spans="1:28" s="102" customFormat="1" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:28" s="102" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A368" s="1"/>
       <c r="B368" s="33"/>
       <c r="C368" s="76">
@@ -24181,7 +24181,7 @@
       <c r="AA368" s="1"/>
       <c r="AB368" s="1"/>
     </row>
-    <row r="369" spans="1:28" s="142" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:28" s="142" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A369" s="1"/>
       <c r="B369" s="33"/>
       <c r="C369" s="76">
@@ -24214,7 +24214,7 @@
       <c r="AA369" s="1"/>
       <c r="AB369" s="1"/>
     </row>
-    <row r="370" spans="1:28" s="142" customFormat="1" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:28" s="142" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A370" s="1"/>
       <c r="B370" s="35"/>
       <c r="C370" s="79">
@@ -24249,7 +24249,7 @@
       <c r="AA370" s="1"/>
       <c r="AB370" s="1"/>
     </row>
-    <row r="371" spans="1:28" s="142" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:28" s="142" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A371" s="1"/>
       <c r="B371" s="19"/>
       <c r="C371" s="80">
@@ -24282,7 +24282,7 @@
       <c r="AA371" s="1"/>
       <c r="AB371" s="1"/>
     </row>
-    <row r="372" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A372" s="1"/>
       <c r="B372" s="1"/>
       <c r="C372" s="76">
@@ -24315,7 +24315,7 @@
       <c r="AA372" s="1"/>
       <c r="AB372" s="1"/>
     </row>
-    <row r="373" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A373" s="1"/>
       <c r="B373" s="1"/>
       <c r="C373" s="69"/>
@@ -24345,7 +24345,7 @@
       <c r="AA373" s="1"/>
       <c r="AB373" s="1"/>
     </row>
-    <row r="374" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A374" s="1"/>
       <c r="B374" s="1"/>
       <c r="C374" s="69"/>
@@ -24375,7 +24375,7 @@
       <c r="AA374" s="1"/>
       <c r="AB374" s="1"/>
     </row>
-    <row r="375" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A375" s="1"/>
       <c r="B375" s="1"/>
       <c r="C375" s="69"/>
@@ -24405,7 +24405,7 @@
       <c r="AA375" s="1"/>
       <c r="AB375" s="1"/>
     </row>
-    <row r="376" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A376" s="1"/>
       <c r="B376" s="1"/>
       <c r="C376" s="69"/>
@@ -24435,7 +24435,7 @@
       <c r="AA376" s="1"/>
       <c r="AB376" s="1"/>
     </row>
-    <row r="377" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A377" s="1"/>
       <c r="B377" s="1"/>
       <c r="C377" s="69"/>
@@ -24465,7 +24465,7 @@
       <c r="AA377" s="1"/>
       <c r="AB377" s="1"/>
     </row>
-    <row r="378" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A378" s="1"/>
       <c r="B378" s="1"/>
       <c r="C378" s="69"/>
@@ -24495,7 +24495,7 @@
       <c r="AA378" s="1"/>
       <c r="AB378" s="1"/>
     </row>
-    <row r="379" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:28" x14ac:dyDescent="0.3">
       <c r="C379" s="75" t="s">
         <v>4</v>
       </c>
@@ -24630,22 +24630,22 @@
       <selection activeCell="U37" sqref="U37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" customWidth="1"/>
-    <col min="2" max="2" width="2.7265625" customWidth="1"/>
-    <col min="3" max="3" width="4.7265625" customWidth="1" outlineLevel="2"/>
-    <col min="4" max="4" width="1.7265625" customWidth="1"/>
-    <col min="5" max="6" width="9.1796875" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="1.7265625" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="15.7265625" customWidth="1"/>
-    <col min="12" max="12" width="9.1796875" customWidth="1"/>
-    <col min="26" max="26" width="1.7265625" customWidth="1"/>
-    <col min="27" max="28" width="4.7265625" customWidth="1"/>
-    <col min="30" max="30" width="46.1796875" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="2.6640625" customWidth="1"/>
+    <col min="3" max="3" width="4.6640625" customWidth="1" outlineLevel="2"/>
+    <col min="4" max="4" width="1.6640625" customWidth="1"/>
+    <col min="5" max="6" width="9.109375" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="1.6640625" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
+    <col min="12" max="12" width="9.109375" customWidth="1"/>
+    <col min="26" max="26" width="1.6640625" customWidth="1"/>
+    <col min="27" max="28" width="4.6640625" customWidth="1"/>
+    <col min="30" max="30" width="46.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="69"/>
@@ -24677,7 +24677,7 @@
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
     </row>
-    <row r="2" spans="1:30" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:30" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="70">
@@ -24712,7 +24712,7 @@
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
-    <row r="3" spans="1:30" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:30" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="20"/>
       <c r="C3" s="71">
@@ -24747,7 +24747,7 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
     </row>
-    <row r="4" spans="1:30" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="34" t="s">
         <v>21</v>
@@ -24784,7 +24784,7 @@
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
     </row>
-    <row r="5" spans="1:30" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:30" outlineLevel="4" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="33"/>
       <c r="C5" s="70">
@@ -24861,7 +24861,7 @@
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" spans="1:30" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="33"/>
       <c r="C6" s="70">
@@ -24901,7 +24901,7 @@
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
     </row>
-    <row r="7" spans="1:30" ht="20.149999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:30" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="33"/>
       <c r="C7" s="70">
@@ -24942,7 +24942,7 @@
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
     </row>
-    <row r="8" spans="1:30" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="33"/>
       <c r="C8" s="70">
@@ -24977,7 +24977,7 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
     </row>
-    <row r="9" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="33"/>
       <c r="C9" s="70">
@@ -25012,7 +25012,7 @@
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
     </row>
-    <row r="10" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="33"/>
       <c r="C10" s="70">
@@ -25047,7 +25047,7 @@
       <c r="AC10" s="1"/>
       <c r="AD10" s="1"/>
     </row>
-    <row r="11" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="33"/>
       <c r="C11" s="70">
@@ -25082,7 +25082,7 @@
       <c r="AC11" s="1"/>
       <c r="AD11" s="1"/>
     </row>
-    <row r="12" spans="1:30" ht="28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:30" ht="27.6" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="33"/>
       <c r="C12" s="70">
@@ -25121,7 +25121,7 @@
       <c r="AC12" s="1"/>
       <c r="AD12" s="1"/>
     </row>
-    <row r="13" spans="1:30" ht="11.5" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:30" ht="11.4" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="33" t="s">
         <v>20</v>
@@ -25158,7 +25158,7 @@
       <c r="AC13" s="1"/>
       <c r="AD13" s="1"/>
     </row>
-    <row r="14" spans="1:30" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:30" outlineLevel="4" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="33"/>
       <c r="C14" s="70">
@@ -25193,7 +25193,7 @@
       <c r="AC14" s="1"/>
       <c r="AD14" s="1"/>
     </row>
-    <row r="15" spans="1:30" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:30" outlineLevel="4" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="33" t="s">
         <v>19</v>
@@ -25232,7 +25232,7 @@
       <c r="AC15" s="1"/>
       <c r="AD15" s="1"/>
     </row>
-    <row r="16" spans="1:30" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="33"/>
       <c r="C16" s="70">
@@ -25269,7 +25269,7 @@
       <c r="AC16" s="1"/>
       <c r="AD16" s="1"/>
     </row>
-    <row r="17" spans="1:30" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:30" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="33"/>
       <c r="C17" s="70">
@@ -25306,7 +25306,7 @@
       <c r="AC17" s="1"/>
       <c r="AD17" s="1"/>
     </row>
-    <row r="18" spans="1:30" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:30" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="33"/>
       <c r="C18" s="70">
@@ -25347,7 +25347,7 @@
       <c r="AC18" s="1"/>
       <c r="AD18" s="1"/>
     </row>
-    <row r="19" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="33"/>
       <c r="C19" s="70">
@@ -25382,7 +25382,7 @@
       <c r="AC19" s="1"/>
       <c r="AD19" s="1"/>
     </row>
-    <row r="20" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="33"/>
       <c r="C20" s="70">
@@ -25417,7 +25417,7 @@
       <c r="AC20" s="1"/>
       <c r="AD20" s="1"/>
     </row>
-    <row r="21" spans="1:30" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:30" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="33"/>
       <c r="C21" s="70">
@@ -25458,7 +25458,7 @@
       <c r="AC21" s="1"/>
       <c r="AD21" s="1"/>
     </row>
-    <row r="22" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="33"/>
       <c r="C22" s="70">
@@ -25493,7 +25493,7 @@
       <c r="AC22" s="1"/>
       <c r="AD22" s="1"/>
     </row>
-    <row r="23" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="33"/>
       <c r="C23" s="70">
@@ -25528,7 +25528,7 @@
       <c r="AC23" s="1"/>
       <c r="AD23" s="1"/>
     </row>
-    <row r="24" spans="1:30" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="33"/>
       <c r="C24" s="70">
@@ -25565,7 +25565,7 @@
       <c r="AC24" s="1"/>
       <c r="AD24" s="1"/>
     </row>
-    <row r="25" spans="1:30" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="33"/>
       <c r="C25" s="70">
@@ -25602,7 +25602,7 @@
       <c r="AC25" s="1"/>
       <c r="AD25" s="1"/>
     </row>
-    <row r="26" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="33"/>
       <c r="C26" s="70">
@@ -25651,7 +25651,7 @@
       <c r="AC26" s="1"/>
       <c r="AD26" s="1"/>
     </row>
-    <row r="27" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="33"/>
       <c r="C27" s="70">
@@ -25690,7 +25690,7 @@
       <c r="AC27" s="1"/>
       <c r="AD27" s="1"/>
     </row>
-    <row r="28" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="33"/>
       <c r="C28" s="70">
@@ -25729,7 +25729,7 @@
       <c r="AC28" s="1"/>
       <c r="AD28" s="1"/>
     </row>
-    <row r="29" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="33"/>
       <c r="C29" s="70">
@@ -25768,7 +25768,7 @@
       <c r="AC29" s="1"/>
       <c r="AD29" s="1"/>
     </row>
-    <row r="30" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="33"/>
       <c r="C30" s="70">
@@ -25807,7 +25807,7 @@
       <c r="AC30" s="1"/>
       <c r="AD30" s="1"/>
     </row>
-    <row r="31" spans="1:30" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="33"/>
       <c r="C31" s="70">
@@ -25844,7 +25844,7 @@
       <c r="AC31" s="1"/>
       <c r="AD31" s="1"/>
     </row>
-    <row r="32" spans="1:30" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="33"/>
       <c r="C32" s="70">
@@ -25881,7 +25881,7 @@
       <c r="AC32" s="1"/>
       <c r="AD32" s="1"/>
     </row>
-    <row r="33" spans="1:30" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:30" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="33"/>
       <c r="C33" s="70">
@@ -25942,7 +25942,7 @@
       <c r="AC33" s="1"/>
       <c r="AD33" s="1"/>
     </row>
-    <row r="34" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="33"/>
       <c r="C34" s="70">
@@ -26007,7 +26007,7 @@
       <c r="AC34" s="1"/>
       <c r="AD34" s="1"/>
     </row>
-    <row r="35" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="33"/>
       <c r="C35" s="70">
@@ -26042,7 +26042,7 @@
       <c r="AC35" s="1"/>
       <c r="AD35" s="1"/>
     </row>
-    <row r="36" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="33"/>
       <c r="C36" s="70">
@@ -26077,7 +26077,7 @@
       <c r="AC36" s="1"/>
       <c r="AD36" s="1"/>
     </row>
-    <row r="37" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="33"/>
       <c r="C37" s="70">
@@ -26112,7 +26112,7 @@
       <c r="AC37" s="1"/>
       <c r="AD37" s="1"/>
     </row>
-    <row r="38" spans="1:30" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="33"/>
       <c r="C38" s="70">
@@ -26149,7 +26149,7 @@
       <c r="AC38" s="1"/>
       <c r="AD38" s="1"/>
     </row>
-    <row r="39" spans="1:30" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="33"/>
       <c r="C39" s="70">
@@ -26184,7 +26184,7 @@
       <c r="AC39" s="1"/>
       <c r="AD39" s="1"/>
     </row>
-    <row r="40" spans="1:30" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="35"/>
       <c r="C40" s="73">
@@ -26221,7 +26221,7 @@
       <c r="AC40" s="1"/>
       <c r="AD40" s="1"/>
     </row>
-    <row r="41" spans="1:30" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:30" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="19"/>
       <c r="C41" s="74">
@@ -26256,7 +26256,7 @@
       <c r="AC41" s="1"/>
       <c r="AD41" s="1"/>
     </row>
-    <row r="42" spans="1:30" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:30" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="70">
@@ -26291,7 +26291,7 @@
       <c r="AC42" s="1"/>
       <c r="AD42" s="1"/>
     </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="69"/>
@@ -26323,7 +26323,7 @@
       <c r="AC43" s="1"/>
       <c r="AD43" s="1"/>
     </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="69"/>
@@ -26355,7 +26355,7 @@
       <c r="AC44" s="1"/>
       <c r="AD44" s="1"/>
     </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="69"/>
@@ -26387,7 +26387,7 @@
       <c r="AC45" s="1"/>
       <c r="AD45" s="1"/>
     </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="69"/>
@@ -26419,7 +26419,7 @@
       <c r="AC46" s="1"/>
       <c r="AD46" s="1"/>
     </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="69"/>
@@ -26451,7 +26451,7 @@
       <c r="AC47" s="1"/>
       <c r="AD47" s="1"/>
     </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="69"/>
@@ -26483,7 +26483,7 @@
       <c r="AC48" s="1"/>
       <c r="AD48" s="1"/>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C49" s="75" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Change 'max' nutrition pattern to 100% of max input
</commit_message>
<xml_diff>
--- a/Structural.xlsx
+++ b/Structural.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC3F5D0-24BD-48BE-964A-2F624F4DFB95}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876BE77F-477E-4922-901A-72E8EA25B174}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="315" yWindow="450" windowWidth="28305" windowHeight="14565" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -156,7 +156,7 @@
     <definedName name="ZA.WidthCol" localSheetId="2">Admin!$L$26</definedName>
     <definedName name="ZA.ZoomSheet" localSheetId="2">Admin!$O$26</definedName>
   </definedNames>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="191029" refMode="R1C1" iterateCount="1" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -804,7 +804,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Michael Young (21512438):</t>
         </r>
@@ -813,7 +813,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 these inputs cant be changed without modifying the condense formula.</t>
@@ -828,7 +828,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Michael Young (21512438):</t>
         </r>
@@ -837,7 +837,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 these inputs can't be changed without modifying the condense formula.</t>
@@ -852,7 +852,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Michael Young (21512438):</t>
         </r>
@@ -861,7 +861,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 these inputs can't be changed without modifying the condense formula.</t>
@@ -2147,7 +2147,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2344,19 +2344,6 @@
       <color rgb="FF0000FF"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="35">
@@ -7327,7 +7314,7 @@
   <dimension ref="A1:AE379"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A316" workbookViewId="0">
-      <selection activeCell="O346" sqref="O346"/>
+      <selection activeCell="L329" sqref="L329"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -22721,7 +22708,7 @@
       <c r="J329" s="54"/>
       <c r="K329" s="54"/>
       <c r="L329" s="31">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="M329" s="31">
         <v>0.5</v>

</xml_diff>

<commit_message>
Update spreadsheets with feed supply adjustments
</commit_message>
<xml_diff>
--- a/Structural.xlsx
+++ b/Structural.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876BE77F-477E-4922-901A-72E8EA25B174}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8BC0B00-E229-475B-BBCF-417BEF2FE239}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
@@ -103,7 +103,7 @@
     <definedName name="i_n3_matrix_len">Stock!$P$326</definedName>
     <definedName name="i_numbers_min_b1">Stock!$L$163:$V$163</definedName>
     <definedName name="i_nut_spread_n0">Stock!$J$328</definedName>
-    <definedName name="i_nut_spread_n1">Stock!$L$328:$L$330</definedName>
+    <definedName name="i_nut_spread_n1">Stock!$L$328:$L$329</definedName>
     <definedName name="i_nut_spread_n3">Stock!$P$328:$P$330</definedName>
     <definedName name="i_p_pos">Stock!$I$64</definedName>
     <definedName name="i_prejoin_offset">Stock!$I$74</definedName>
@@ -156,7 +156,7 @@
     <definedName name="ZA.WidthCol" localSheetId="2">Admin!$L$26</definedName>
     <definedName name="ZA.ZoomSheet" localSheetId="2">Admin!$O$26</definedName>
   </definedNames>
-  <calcPr calcId="191029" refMode="R1C1" iterateCount="1" calcOnSave="0"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1236,7 +1236,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="294">
   <si>
     <t>Controls for this worksheet</t>
   </si>
@@ -2138,6 +2138,10 @@
   </si>
   <si>
     <t xml:space="preserve">         Therefore think about the final sale date relative to 1 Jan, rather than the age of the animal</t>
+  </si>
+  <si>
+    <t>22Mar21: Alter the initial weight &amp; wool spread for the weaners
+1: 1Apr19-Blank worksheet</t>
   </si>
 </sst>
 </file>
@@ -3285,7 +3289,7 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="190">
+  <cellXfs count="191">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="25" xfId="3">
@@ -3762,6 +3766,10 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="15" fontId="5" fillId="6" borderId="25" xfId="9" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="Accent2" xfId="33" builtinId="33" customBuiltin="1"/>
@@ -3808,7 +3816,21 @@
     <cellStyle name="Warning Text" xfId="21" builtinId="11" customBuiltin="1"/>
     <cellStyle name="WorksheetBackground" xfId="38" xr:uid="{D9586848-0E78-42E2-92FA-4C5FBD9E7440}"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="23">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -7313,8 +7335,8 @@
   </sheetPr>
   <dimension ref="A1:AE379"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A316" workbookViewId="0">
-      <selection activeCell="L329" sqref="L329"/>
+    <sheetView tabSelected="1" topLeftCell="A338" workbookViewId="0">
+      <selection activeCell="O364" sqref="O364:R366"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -7333,7 +7355,7 @@
     <col min="28" max="28" width="46.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="69"/>
@@ -7363,7 +7385,7 @@
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
     </row>
-    <row r="2" spans="1:28" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="70">
@@ -7429,7 +7451,7 @@
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
     </row>
-    <row r="4" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="34" t="s">
         <v>21</v>
@@ -7464,7 +7486,7 @@
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
     </row>
-    <row r="5" spans="1:28" hidden="1" outlineLevel="4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="33"/>
       <c r="C5" s="70">
@@ -7573,7 +7595,7 @@
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
     </row>
-    <row r="7" spans="1:28" ht="20.100000000000001" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="33"/>
       <c r="C7" s="70">
@@ -7612,7 +7634,7 @@
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
     </row>
-    <row r="8" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="33"/>
       <c r="C8" s="70">
@@ -7645,7 +7667,7 @@
       <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
     </row>
-    <row r="9" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="33"/>
       <c r="C9" s="70">
@@ -7678,7 +7700,7 @@
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
     </row>
-    <row r="10" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="33"/>
       <c r="C10" s="70">
@@ -7711,7 +7733,7 @@
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
     </row>
-    <row r="11" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="33"/>
       <c r="C11" s="70">
@@ -7744,7 +7766,7 @@
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
     </row>
-    <row r="12" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="33"/>
       <c r="C12" s="70">
@@ -7781,7 +7803,7 @@
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
     </row>
-    <row r="13" spans="1:28" ht="11.45" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" ht="11.45" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="33" t="s">
         <v>20</v>
@@ -7816,7 +7838,7 @@
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
     </row>
-    <row r="14" spans="1:28" hidden="1" outlineLevel="4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="33"/>
       <c r="C14" s="70">
@@ -7849,7 +7871,7 @@
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
     </row>
-    <row r="15" spans="1:28" hidden="1" outlineLevel="4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="33"/>
       <c r="C15" s="70">
@@ -7954,7 +7976,7 @@
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
     </row>
-    <row r="18" spans="1:28" ht="45" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="33"/>
       <c r="C18" s="70">
@@ -7993,7 +8015,7 @@
       <c r="AA18" s="1"/>
       <c r="AB18" s="1"/>
     </row>
-    <row r="19" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="33"/>
       <c r="C19" s="70">
@@ -8026,7 +8048,7 @@
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
     </row>
-    <row r="20" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="33"/>
       <c r="C20" s="70">
@@ -8059,7 +8081,7 @@
       <c r="AA20" s="1"/>
       <c r="AB20" s="1"/>
     </row>
-    <row r="21" spans="1:28" ht="45" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="33"/>
       <c r="C21" s="70">
@@ -8073,11 +8095,11 @@
       <c r="H21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I21" s="23">
-        <v>1</v>
+      <c r="I21" s="190">
+        <v>44277</v>
       </c>
       <c r="J21" s="177" t="s">
-        <v>35</v>
+        <v>293</v>
       </c>
       <c r="K21" s="178"/>
       <c r="L21" s="178"/>
@@ -8098,7 +8120,7 @@
       <c r="AA21" s="1"/>
       <c r="AB21" s="1"/>
     </row>
-    <row r="22" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="33"/>
       <c r="C22" s="70">
@@ -8131,7 +8153,7 @@
       <c r="AA22" s="1"/>
       <c r="AB22" s="1"/>
     </row>
-    <row r="23" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="33"/>
       <c r="C23" s="70">
@@ -8164,7 +8186,7 @@
       <c r="AA23" s="1"/>
       <c r="AB23" s="1"/>
     </row>
-    <row r="24" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="33"/>
       <c r="C24" s="70">
@@ -8199,7 +8221,7 @@
       <c r="AA24" s="1"/>
       <c r="AB24" s="1"/>
     </row>
-    <row r="25" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="33"/>
       <c r="C25" s="70">
@@ -8234,7 +8256,7 @@
       <c r="AA25" s="1"/>
       <c r="AB25" s="1"/>
     </row>
-    <row r="26" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="33"/>
       <c r="C26" s="70">
@@ -8281,7 +8303,7 @@
       <c r="AA26" s="1"/>
       <c r="AB26" s="1"/>
     </row>
-    <row r="27" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="33"/>
       <c r="C27" s="70">
@@ -8318,7 +8340,7 @@
       <c r="AA27" s="1"/>
       <c r="AB27" s="1"/>
     </row>
-    <row r="28" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="33"/>
       <c r="C28" s="70">
@@ -8355,7 +8377,7 @@
       <c r="AA28" s="1"/>
       <c r="AB28" s="1"/>
     </row>
-    <row r="29" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="33"/>
       <c r="C29" s="70">
@@ -8392,7 +8414,7 @@
       <c r="AA29" s="1"/>
       <c r="AB29" s="1"/>
     </row>
-    <row r="30" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="33"/>
       <c r="C30" s="70">
@@ -8429,7 +8451,7 @@
       <c r="AA30" s="1"/>
       <c r="AB30" s="1"/>
     </row>
-    <row r="31" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="33"/>
       <c r="C31" s="70">
@@ -8464,7 +8486,7 @@
       <c r="AA31" s="1"/>
       <c r="AB31" s="1"/>
     </row>
-    <row r="32" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="33"/>
       <c r="C32" s="70">
@@ -8532,7 +8554,7 @@
       <c r="AA33" s="1"/>
       <c r="AB33" s="1"/>
     </row>
-    <row r="34" spans="1:28" ht="5.0999999999999996" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="19"/>
       <c r="C34" s="74">
@@ -8565,7 +8587,7 @@
       <c r="AA34" s="1"/>
       <c r="AB34" s="1"/>
     </row>
-    <row r="35" spans="1:28" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="70">
@@ -8598,7 +8620,7 @@
       <c r="AA35" s="1"/>
       <c r="AB35" s="1"/>
     </row>
-    <row r="36" spans="1:28" s="142" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="76">
@@ -8664,7 +8686,7 @@
       <c r="AA37" s="1"/>
       <c r="AB37" s="1"/>
     </row>
-    <row r="38" spans="1:28" s="142" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:28" s="142" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="34" t="s">
         <v>21</v>
@@ -8699,7 +8721,7 @@
       <c r="AA38" s="1"/>
       <c r="AB38" s="1"/>
     </row>
-    <row r="39" spans="1:28" s="142" customFormat="1" hidden="1" outlineLevel="4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:28" s="142" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="33"/>
       <c r="C39" s="76">
@@ -8769,7 +8791,7 @@
       <c r="AA40" s="1"/>
       <c r="AB40" s="1"/>
     </row>
-    <row r="41" spans="1:28" s="142" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:28" s="142" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="33"/>
       <c r="C41" s="76">
@@ -8806,7 +8828,7 @@
       <c r="AA41" s="1"/>
       <c r="AB41" s="1"/>
     </row>
-    <row r="42" spans="1:28" s="142" customFormat="1" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:28" s="142" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="33"/>
       <c r="C42" s="76">
@@ -8839,7 +8861,7 @@
       <c r="AA42" s="1"/>
       <c r="AB42" s="1"/>
     </row>
-    <row r="43" spans="1:28" s="142" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="33"/>
       <c r="C43" s="76">
@@ -8872,7 +8894,7 @@
       <c r="AA43" s="1"/>
       <c r="AB43" s="1"/>
     </row>
-    <row r="44" spans="1:28" s="142" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="33"/>
       <c r="C44" s="76">
@@ -8905,7 +8927,7 @@
       <c r="AA44" s="1"/>
       <c r="AB44" s="1"/>
     </row>
-    <row r="45" spans="1:28" s="142" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="33"/>
       <c r="C45" s="76">
@@ -8938,7 +8960,7 @@
       <c r="AA45" s="1"/>
       <c r="AB45" s="1"/>
     </row>
-    <row r="46" spans="1:28" s="142" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:28" s="142" customFormat="1" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="33"/>
       <c r="C46" s="76">
@@ -8981,7 +9003,7 @@
       <c r="AA46" s="1"/>
       <c r="AB46" s="1"/>
     </row>
-    <row r="47" spans="1:28" s="142" customFormat="1" ht="11.45" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:28" s="142" customFormat="1" ht="11.45" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="33" t="s">
         <v>20</v>
@@ -9016,7 +9038,7 @@
       <c r="AA47" s="1"/>
       <c r="AB47" s="1"/>
     </row>
-    <row r="48" spans="1:28" s="142" customFormat="1" hidden="1" outlineLevel="4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:28" s="142" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="33"/>
       <c r="C48" s="76">
@@ -9049,7 +9071,7 @@
       <c r="AA48" s="1"/>
       <c r="AB48" s="1"/>
     </row>
-    <row r="49" spans="1:28" s="142" customFormat="1" hidden="1" outlineLevel="4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:28" s="142" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="33" t="s">
         <v>19</v>
@@ -9086,7 +9108,7 @@
       <c r="AA49" s="1"/>
       <c r="AB49" s="1"/>
     </row>
-    <row r="50" spans="1:28" s="142" customFormat="1" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:28" s="142" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="33"/>
       <c r="C50" s="76">
@@ -9121,7 +9143,7 @@
       <c r="AA50" s="1"/>
       <c r="AB50" s="1"/>
     </row>
-    <row r="51" spans="1:28" s="142" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="33"/>
       <c r="C51" s="76">
@@ -9156,7 +9178,7 @@
       <c r="AA51" s="1"/>
       <c r="AB51" s="1"/>
     </row>
-    <row r="52" spans="1:28" s="155" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="33"/>
       <c r="C52" s="76"/>
@@ -9190,7 +9212,7 @@
       <c r="AA52" s="1"/>
       <c r="AB52" s="1"/>
     </row>
-    <row r="53" spans="1:28" s="155" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="33"/>
       <c r="C53" s="76"/>
@@ -9224,7 +9246,7 @@
       <c r="AA53" s="1"/>
       <c r="AB53" s="1"/>
     </row>
-    <row r="54" spans="1:28" s="155" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="33"/>
       <c r="C54" s="76"/>
@@ -9258,7 +9280,7 @@
       <c r="AA54" s="1"/>
       <c r="AB54" s="1"/>
     </row>
-    <row r="55" spans="1:28" s="155" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="33"/>
       <c r="C55" s="76"/>
@@ -9292,7 +9314,7 @@
       <c r="AA55" s="1"/>
       <c r="AB55" s="1"/>
     </row>
-    <row r="56" spans="1:28" s="155" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="33"/>
       <c r="C56" s="76"/>
@@ -9326,7 +9348,7 @@
       <c r="AA56" s="1"/>
       <c r="AB56" s="1"/>
     </row>
-    <row r="57" spans="1:28" s="155" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="33"/>
       <c r="C57" s="76"/>
@@ -9360,7 +9382,7 @@
       <c r="AA57" s="1"/>
       <c r="AB57" s="1"/>
     </row>
-    <row r="58" spans="1:28" s="155" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="33"/>
       <c r="C58" s="76"/>
@@ -9394,7 +9416,7 @@
       <c r="AA58" s="1"/>
       <c r="AB58" s="1"/>
     </row>
-    <row r="59" spans="1:28" s="155" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="33"/>
       <c r="C59" s="76"/>
@@ -9428,7 +9450,7 @@
       <c r="AA59" s="1"/>
       <c r="AB59" s="1"/>
     </row>
-    <row r="60" spans="1:28" s="155" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="33"/>
       <c r="C60" s="76"/>
@@ -9462,7 +9484,7 @@
       <c r="AA60" s="1"/>
       <c r="AB60" s="1"/>
     </row>
-    <row r="61" spans="1:28" s="155" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="33"/>
       <c r="C61" s="76"/>
@@ -9496,7 +9518,7 @@
       <c r="AA61" s="1"/>
       <c r="AB61" s="1"/>
     </row>
-    <row r="62" spans="1:28" s="155" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="33"/>
       <c r="C62" s="76"/>
@@ -9530,7 +9552,7 @@
       <c r="AA62" s="1"/>
       <c r="AB62" s="1"/>
     </row>
-    <row r="63" spans="1:28" s="155" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="33"/>
       <c r="C63" s="76"/>
@@ -9564,7 +9586,7 @@
       <c r="AA63" s="1"/>
       <c r="AB63" s="1"/>
     </row>
-    <row r="64" spans="1:28" s="155" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="33"/>
       <c r="C64" s="76"/>
@@ -9598,7 +9620,7 @@
       <c r="AA64" s="1"/>
       <c r="AB64" s="1"/>
     </row>
-    <row r="65" spans="1:28" s="113" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:28" s="113" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="33"/>
       <c r="C65" s="76">
@@ -9637,7 +9659,7 @@
       <c r="AA65" s="1"/>
       <c r="AB65" s="1"/>
     </row>
-    <row r="66" spans="1:28" s="105" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:28" s="105" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="33"/>
       <c r="C66" s="76">
@@ -9674,7 +9696,7 @@
       <c r="AA66" s="1"/>
       <c r="AB66" s="1"/>
     </row>
-    <row r="67" spans="1:28" s="105" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:28" s="105" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="33"/>
       <c r="C67" s="76">
@@ -9711,7 +9733,7 @@
       <c r="AA67" s="1"/>
       <c r="AB67" s="1"/>
     </row>
-    <row r="68" spans="1:28" s="129" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:28" s="129" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="33"/>
       <c r="C68" s="76">
@@ -9748,7 +9770,7 @@
       <c r="AA68" s="1"/>
       <c r="AB68" s="1"/>
     </row>
-    <row r="69" spans="1:28" s="145" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:28" s="145" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="33"/>
       <c r="C69" s="76">
@@ -9781,7 +9803,7 @@
       <c r="AA69" s="1"/>
       <c r="AB69" s="1"/>
     </row>
-    <row r="70" spans="1:28" s="109" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:28" s="109" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="33"/>
       <c r="C70" s="76">
@@ -9818,7 +9840,7 @@
       <c r="AA70" s="1"/>
       <c r="AB70" s="1"/>
     </row>
-    <row r="71" spans="1:28" s="101" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="33"/>
       <c r="C71" s="76">
@@ -9859,7 +9881,7 @@
       <c r="AA71" s="1"/>
       <c r="AB71" s="1"/>
     </row>
-    <row r="72" spans="1:28" s="154" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:28" s="154" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="33"/>
       <c r="C72" s="76">
@@ -9900,7 +9922,7 @@
       <c r="AA72" s="1"/>
       <c r="AB72" s="1"/>
     </row>
-    <row r="73" spans="1:28" s="155" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="33"/>
       <c r="C73" s="76"/>
@@ -9930,7 +9952,7 @@
       <c r="AA73" s="1"/>
       <c r="AB73" s="1"/>
     </row>
-    <row r="74" spans="1:28" s="155" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="33"/>
       <c r="C74" s="76"/>
@@ -9966,7 +9988,7 @@
       <c r="AA74" s="1"/>
       <c r="AB74" s="1"/>
     </row>
-    <row r="75" spans="1:28" s="155" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:28" s="155" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="33"/>
       <c r="C75" s="76"/>
@@ -9996,7 +10018,7 @@
       <c r="AA75" s="1"/>
       <c r="AB75" s="1"/>
     </row>
-    <row r="76" spans="1:28" s="101" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="33"/>
       <c r="C76" s="76">
@@ -10031,7 +10053,7 @@
       <c r="AA76" s="1"/>
       <c r="AB76" s="1"/>
     </row>
-    <row r="77" spans="1:28" s="101" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:28" s="101" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="33"/>
       <c r="C77" s="76">
@@ -10072,7 +10094,7 @@
       <c r="AA77" s="1"/>
       <c r="AB77" s="1"/>
     </row>
-    <row r="78" spans="1:28" s="101" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:28" s="101" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="33"/>
       <c r="C78" s="76">
@@ -10113,7 +10135,7 @@
       <c r="AA78" s="1"/>
       <c r="AB78" s="1"/>
     </row>
-    <row r="79" spans="1:28" s="101" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:28" s="101" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="33"/>
       <c r="C79" s="76">
@@ -10146,7 +10168,7 @@
       <c r="AA79" s="1"/>
       <c r="AB79" s="1"/>
     </row>
-    <row r="80" spans="1:28" s="101" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="33"/>
       <c r="C80" s="76">
@@ -10183,7 +10205,7 @@
       <c r="AA80" s="1"/>
       <c r="AB80" s="1"/>
     </row>
-    <row r="81" spans="1:28" s="152" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:28" s="152" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="33"/>
       <c r="C81" s="76">
@@ -10216,7 +10238,7 @@
       <c r="AA81" s="1"/>
       <c r="AB81" s="1"/>
     </row>
-    <row r="82" spans="1:28" s="101" customFormat="1" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:28" s="101" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="33"/>
       <c r="C82" s="76">
@@ -10251,7 +10273,7 @@
       <c r="AA82" s="1"/>
       <c r="AB82" s="1"/>
     </row>
-    <row r="83" spans="1:28" s="101" customFormat="1" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:28" s="101" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="33"/>
       <c r="C83" s="76">
@@ -10319,7 +10341,7 @@
       <c r="AA84" s="1"/>
       <c r="AB84" s="1"/>
     </row>
-    <row r="85" spans="1:28" s="101" customFormat="1" ht="5.0999999999999996" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:28" s="101" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="19"/>
       <c r="C85" s="80">
@@ -10352,7 +10374,7 @@
       <c r="AA85" s="1"/>
       <c r="AB85" s="1"/>
     </row>
-    <row r="86" spans="1:28" s="101" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="76">
@@ -10385,7 +10407,7 @@
       <c r="AA86" s="1"/>
       <c r="AB86" s="1"/>
     </row>
-    <row r="87" spans="1:28" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="76">
@@ -10451,7 +10473,7 @@
       <c r="AA88" s="1"/>
       <c r="AB88" s="1"/>
     </row>
-    <row r="89" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="34" t="s">
         <v>21</v>
@@ -10486,7 +10508,7 @@
       <c r="AA89" s="1"/>
       <c r="AB89" s="1"/>
     </row>
-    <row r="90" spans="1:28" hidden="1" outlineLevel="4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="33"/>
       <c r="C90" s="76">
@@ -10556,7 +10578,7 @@
       <c r="AA91" s="1"/>
       <c r="AB91" s="1"/>
     </row>
-    <row r="92" spans="1:28" ht="20.100000000000001" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:28" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="33"/>
       <c r="C92" s="76">
@@ -10593,7 +10615,7 @@
       <c r="AA92" s="1"/>
       <c r="AB92" s="1"/>
     </row>
-    <row r="93" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="33"/>
       <c r="C93" s="76">
@@ -10626,7 +10648,7 @@
       <c r="AA93" s="1"/>
       <c r="AB93" s="1"/>
     </row>
-    <row r="94" spans="1:28" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="33"/>
       <c r="C94" s="76">
@@ -10659,7 +10681,7 @@
       <c r="AA94" s="1"/>
       <c r="AB94" s="1"/>
     </row>
-    <row r="95" spans="1:28" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="33"/>
       <c r="C95" s="76">
@@ -10692,7 +10714,7 @@
       <c r="AA95" s="1"/>
       <c r="AB95" s="1"/>
     </row>
-    <row r="96" spans="1:28" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="33"/>
       <c r="C96" s="76">
@@ -10731,7 +10753,7 @@
       <c r="AA96" s="1"/>
       <c r="AB96" s="1"/>
     </row>
-    <row r="97" spans="1:28" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="33"/>
       <c r="C97" s="76">
@@ -10780,7 +10802,7 @@
       <c r="AA97" s="1"/>
       <c r="AB97" s="1"/>
     </row>
-    <row r="98" spans="1:28" ht="11.45" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:28" ht="11.45" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="33" t="s">
         <v>20</v>
@@ -10815,7 +10837,7 @@
       <c r="AA98" s="1"/>
       <c r="AB98" s="1"/>
     </row>
-    <row r="99" spans="1:28" hidden="1" outlineLevel="4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="33"/>
       <c r="C99" s="76">
@@ -10848,7 +10870,7 @@
       <c r="AA99" s="1"/>
       <c r="AB99" s="1"/>
     </row>
-    <row r="100" spans="1:28" hidden="1" outlineLevel="4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="33" t="s">
         <v>19</v>
@@ -10885,7 +10907,7 @@
       <c r="AA100" s="1"/>
       <c r="AB100" s="1"/>
     </row>
-    <row r="101" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="33"/>
       <c r="C101" s="76">
@@ -10920,7 +10942,7 @@
       <c r="AA101" s="1"/>
       <c r="AB101" s="1"/>
     </row>
-    <row r="102" spans="1:28" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="33"/>
       <c r="C102" s="76">
@@ -10973,7 +10995,7 @@
       <c r="AA102" s="1"/>
       <c r="AB102" s="1"/>
     </row>
-    <row r="103" spans="1:28" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="33"/>
       <c r="C103" s="76">
@@ -11024,7 +11046,7 @@
       <c r="AA103" s="1"/>
       <c r="AB103" s="1"/>
     </row>
-    <row r="104" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="33"/>
       <c r="C104" s="76">
@@ -11075,7 +11097,7 @@
       <c r="AA104" s="1"/>
       <c r="AB104" s="1"/>
     </row>
-    <row r="105" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="33"/>
       <c r="C105" s="76">
@@ -11108,7 +11130,7 @@
       <c r="AA105" s="1"/>
       <c r="AB105" s="1"/>
     </row>
-    <row r="106" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="33"/>
       <c r="C106" s="76">
@@ -11159,7 +11181,7 @@
       <c r="AA106" s="1"/>
       <c r="AB106" s="1"/>
     </row>
-    <row r="107" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="33"/>
       <c r="C107" s="76">
@@ -11208,7 +11230,7 @@
       <c r="AA107" s="1"/>
       <c r="AB107" s="1"/>
     </row>
-    <row r="108" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="33"/>
       <c r="C108" s="76">
@@ -11257,7 +11279,7 @@
       <c r="AA108" s="1"/>
       <c r="AB108" s="1"/>
     </row>
-    <row r="109" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="33"/>
       <c r="C109" s="76">
@@ -11306,7 +11328,7 @@
       <c r="AA109" s="1"/>
       <c r="AB109" s="1"/>
     </row>
-    <row r="110" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="33"/>
       <c r="C110" s="76">
@@ -11339,7 +11361,7 @@
       <c r="AA110" s="1"/>
       <c r="AB110" s="1"/>
     </row>
-    <row r="111" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111" s="33"/>
       <c r="C111" s="76">
@@ -11390,7 +11412,7 @@
       <c r="AA111" s="1"/>
       <c r="AB111" s="1"/>
     </row>
-    <row r="112" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="33"/>
       <c r="C112" s="76">
@@ -11439,7 +11461,7 @@
       <c r="AA112" s="1"/>
       <c r="AB112" s="1"/>
     </row>
-    <row r="113" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="33"/>
       <c r="C113" s="76">
@@ -11488,7 +11510,7 @@
       <c r="AA113" s="1"/>
       <c r="AB113" s="1"/>
     </row>
-    <row r="114" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="33"/>
       <c r="C114" s="76">
@@ -11537,7 +11559,7 @@
       <c r="AA114" s="1"/>
       <c r="AB114" s="1"/>
     </row>
-    <row r="115" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="33"/>
       <c r="C115" s="76">
@@ -11570,7 +11592,7 @@
       <c r="AA115" s="1"/>
       <c r="AB115" s="1"/>
     </row>
-    <row r="116" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="33"/>
       <c r="C116" s="76">
@@ -11621,7 +11643,7 @@
       <c r="AA116" s="1"/>
       <c r="AB116" s="1"/>
     </row>
-    <row r="117" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="33"/>
       <c r="C117" s="76">
@@ -11670,7 +11692,7 @@
       <c r="AA117" s="1"/>
       <c r="AB117" s="1"/>
     </row>
-    <row r="118" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="33"/>
       <c r="C118" s="76">
@@ -11719,7 +11741,7 @@
       <c r="AA118" s="1"/>
       <c r="AB118" s="1"/>
     </row>
-    <row r="119" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="33"/>
       <c r="C119" s="76">
@@ -11768,7 +11790,7 @@
       <c r="AA119" s="1"/>
       <c r="AB119" s="1"/>
     </row>
-    <row r="120" spans="1:28" s="151" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:28" s="151" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="33"/>
       <c r="C120" s="76">
@@ -11801,7 +11823,7 @@
       <c r="AA120" s="1"/>
       <c r="AB120" s="1"/>
     </row>
-    <row r="121" spans="1:28" s="151" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:28" s="151" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="33"/>
       <c r="C121" s="76">
@@ -11836,7 +11858,7 @@
       <c r="AA121" s="1"/>
       <c r="AB121" s="1"/>
     </row>
-    <row r="122" spans="1:28" s="151" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:28" s="151" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="33"/>
       <c r="C122" s="76">
@@ -11877,7 +11899,7 @@
       <c r="AA122" s="1"/>
       <c r="AB122" s="1"/>
     </row>
-    <row r="123" spans="1:28" s="151" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:28" s="151" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
       <c r="B123" s="33"/>
       <c r="C123" s="76">
@@ -11925,7 +11947,7 @@
       <c r="AA123" s="1"/>
       <c r="AB123" s="1"/>
     </row>
-    <row r="124" spans="1:28" s="151" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:28" s="151" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
       <c r="B124" s="33"/>
       <c r="C124" s="76">
@@ -11971,7 +11993,7 @@
       <c r="AA124" s="1"/>
       <c r="AB124" s="1"/>
     </row>
-    <row r="125" spans="1:28" s="151" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:28" s="151" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="B125" s="33"/>
       <c r="C125" s="76">
@@ -12014,7 +12036,7 @@
       <c r="AA125" s="1"/>
       <c r="AB125" s="1"/>
     </row>
-    <row r="126" spans="1:28" s="151" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:28" s="151" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
       <c r="B126" s="33"/>
       <c r="C126" s="76">
@@ -12047,7 +12069,7 @@
       <c r="AA126" s="1"/>
       <c r="AB126" s="1"/>
     </row>
-    <row r="127" spans="1:28" s="151" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:28" s="151" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="B127" s="33"/>
       <c r="C127" s="76">
@@ -12094,7 +12116,7 @@
       <c r="AA127" s="1"/>
       <c r="AB127" s="1"/>
     </row>
-    <row r="128" spans="1:28" s="151" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:28" s="151" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
       <c r="B128" s="33"/>
       <c r="C128" s="76">
@@ -12139,7 +12161,7 @@
       <c r="AA128" s="1"/>
       <c r="AB128" s="1"/>
     </row>
-    <row r="129" spans="1:28" s="151" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:28" s="151" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
       <c r="B129" s="33"/>
       <c r="C129" s="76">
@@ -12182,7 +12204,7 @@
       <c r="AA129" s="1"/>
       <c r="AB129" s="1"/>
     </row>
-    <row r="130" spans="1:28" s="151" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:28" s="151" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="B130" s="33"/>
       <c r="C130" s="76">
@@ -12215,7 +12237,7 @@
       <c r="AA130" s="1"/>
       <c r="AB130" s="1"/>
     </row>
-    <row r="131" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131" s="33"/>
       <c r="C131" s="76">
@@ -12250,7 +12272,7 @@
       <c r="AA131" s="1"/>
       <c r="AB131" s="1"/>
     </row>
-    <row r="132" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="33"/>
       <c r="C132" s="76">
@@ -12318,7 +12340,7 @@
       <c r="AA133" s="1"/>
       <c r="AB133" s="1"/>
     </row>
-    <row r="134" spans="1:28" ht="5.0999999999999996" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:28" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134" s="19"/>
       <c r="C134" s="80">
@@ -12351,7 +12373,7 @@
       <c r="AA134" s="1"/>
       <c r="AB134" s="1"/>
     </row>
-    <row r="135" spans="1:28" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="76">
@@ -12384,7 +12406,7 @@
       <c r="AA135" s="1"/>
       <c r="AB135" s="1"/>
     </row>
-    <row r="136" spans="1:28" s="99" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="76">
@@ -12450,7 +12472,7 @@
       <c r="AA137" s="1"/>
       <c r="AB137" s="1"/>
     </row>
-    <row r="138" spans="1:28" s="99" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:28" s="99" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
       <c r="B138" s="34" t="s">
         <v>21</v>
@@ -12485,7 +12507,7 @@
       <c r="AA138" s="1"/>
       <c r="AB138" s="1"/>
     </row>
-    <row r="139" spans="1:28" s="99" customFormat="1" hidden="1" outlineLevel="4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:28" s="99" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
       <c r="B139" s="33"/>
       <c r="C139" s="76">
@@ -12555,7 +12577,7 @@
       <c r="AA140" s="1"/>
       <c r="AB140" s="1"/>
     </row>
-    <row r="141" spans="1:28" s="99" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:28" s="99" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
       <c r="B141" s="33"/>
       <c r="C141" s="76">
@@ -12592,7 +12614,7 @@
       <c r="AA141" s="1"/>
       <c r="AB141" s="1"/>
     </row>
-    <row r="142" spans="1:28" s="99" customFormat="1" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:28" s="99" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
       <c r="B142" s="33"/>
       <c r="C142" s="76">
@@ -12625,7 +12647,7 @@
       <c r="AA142" s="1"/>
       <c r="AB142" s="1"/>
     </row>
-    <row r="143" spans="1:28" s="99" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
       <c r="B143" s="33"/>
       <c r="C143" s="76">
@@ -12658,7 +12680,7 @@
       <c r="AA143" s="1"/>
       <c r="AB143" s="1"/>
     </row>
-    <row r="144" spans="1:28" s="99" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
       <c r="B144" s="33"/>
       <c r="C144" s="76">
@@ -12693,7 +12715,7 @@
       <c r="AA144" s="1"/>
       <c r="AB144" s="1"/>
     </row>
-    <row r="145" spans="1:28" s="99" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
       <c r="B145" s="33"/>
       <c r="C145" s="76">
@@ -12728,7 +12750,7 @@
       <c r="AA145" s="1"/>
       <c r="AB145" s="1"/>
     </row>
-    <row r="146" spans="1:28" s="99" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
       <c r="B146" s="33"/>
       <c r="C146" s="76">
@@ -12783,7 +12805,7 @@
       <c r="AA146" s="1"/>
       <c r="AB146" s="1"/>
     </row>
-    <row r="147" spans="1:28" s="99" customFormat="1" ht="11.45" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:28" s="99" customFormat="1" ht="11.45" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
       <c r="B147" s="33" t="s">
         <v>20</v>
@@ -12818,7 +12840,7 @@
       <c r="AA147" s="1"/>
       <c r="AB147" s="1"/>
     </row>
-    <row r="148" spans="1:28" s="99" customFormat="1" hidden="1" outlineLevel="4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:28" s="99" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
       <c r="B148" s="33"/>
       <c r="C148" s="76">
@@ -12873,7 +12895,7 @@
       <c r="AA148" s="1"/>
       <c r="AB148" s="1"/>
     </row>
-    <row r="149" spans="1:28" s="99" customFormat="1" hidden="1" outlineLevel="4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:28" s="99" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
       <c r="B149" s="33" t="s">
         <v>19</v>
@@ -12910,7 +12932,7 @@
       <c r="AA149" s="1"/>
       <c r="AB149" s="1"/>
     </row>
-    <row r="150" spans="1:28" s="99" customFormat="1" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:28" s="99" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
       <c r="B150" s="33"/>
       <c r="C150" s="76">
@@ -12945,7 +12967,7 @@
       <c r="AA150" s="1"/>
       <c r="AB150" s="1"/>
     </row>
-    <row r="151" spans="1:28" s="99" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
       <c r="B151" s="33"/>
       <c r="C151" s="76">
@@ -12980,7 +13002,7 @@
       <c r="AA151" s="1"/>
       <c r="AB151" s="1"/>
     </row>
-    <row r="152" spans="1:28" s="99" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
       <c r="B152" s="33"/>
       <c r="C152" s="76">
@@ -13019,7 +13041,7 @@
       <c r="AA152" s="1"/>
       <c r="AB152" s="1"/>
     </row>
-    <row r="153" spans="1:28" s="99" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:28" s="99" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A153" s="1"/>
       <c r="B153" s="33"/>
       <c r="C153" s="76">
@@ -13078,7 +13100,7 @@
       <c r="AA153" s="1"/>
       <c r="AB153" s="1"/>
     </row>
-    <row r="154" spans="1:28" s="99" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:28" s="99" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A154" s="1"/>
       <c r="B154" s="33"/>
       <c r="C154" s="76">
@@ -13135,7 +13157,7 @@
       <c r="AA154" s="1"/>
       <c r="AB154" s="1"/>
     </row>
-    <row r="155" spans="1:28" s="99" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:28" s="99" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
       <c r="B155" s="33"/>
       <c r="C155" s="76">
@@ -13172,7 +13194,7 @@
       <c r="AA155" s="1"/>
       <c r="AB155" s="1"/>
     </row>
-    <row r="156" spans="1:28" s="99" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:28" s="99" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A156" s="1"/>
       <c r="B156" s="33"/>
       <c r="C156" s="76">
@@ -13229,7 +13251,7 @@
       <c r="AA156" s="1"/>
       <c r="AB156" s="1"/>
     </row>
-    <row r="157" spans="1:28" s="150" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:28" s="150" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
       <c r="B157" s="33"/>
       <c r="C157" s="76">
@@ -13288,7 +13310,7 @@
       <c r="AA157" s="1"/>
       <c r="AB157" s="1"/>
     </row>
-    <row r="158" spans="1:28" s="124" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:28" s="124" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
       <c r="B158" s="33"/>
       <c r="C158" s="76">
@@ -13345,7 +13367,7 @@
       <c r="AA158" s="1"/>
       <c r="AB158" s="1"/>
     </row>
-    <row r="159" spans="1:28" s="124" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:28" s="124" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A159" s="1"/>
       <c r="B159" s="33"/>
       <c r="C159" s="76">
@@ -13402,7 +13424,7 @@
       <c r="AA159" s="1"/>
       <c r="AB159" s="1"/>
     </row>
-    <row r="160" spans="1:28" s="99" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:28" s="99" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
       <c r="B160" s="33"/>
       <c r="C160" s="76">
@@ -13459,7 +13481,7 @@
       <c r="AA160" s="1"/>
       <c r="AB160" s="1"/>
     </row>
-    <row r="161" spans="1:31" s="99" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:31" s="99" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A161" s="1"/>
       <c r="B161" s="33"/>
       <c r="C161" s="76">
@@ -13516,7 +13538,7 @@
       <c r="AA161" s="1"/>
       <c r="AB161" s="1"/>
     </row>
-    <row r="162" spans="1:31" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A162" s="1"/>
       <c r="B162" s="33"/>
       <c r="C162" s="76">
@@ -13576,7 +13598,7 @@
       <c r="AD162" s="130"/>
       <c r="AE162" s="130"/>
     </row>
-    <row r="163" spans="1:31" s="146" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:31" s="146" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A163" s="1"/>
       <c r="B163" s="33"/>
       <c r="C163" s="76">
@@ -13633,7 +13655,7 @@
       <c r="AA163" s="1"/>
       <c r="AB163" s="1"/>
     </row>
-    <row r="164" spans="1:31" s="113" customFormat="1" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:31" s="113" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A164" s="1"/>
       <c r="B164" s="33"/>
       <c r="C164" s="76">
@@ -13669,7 +13691,7 @@
       <c r="AD164" s="130"/>
       <c r="AE164" s="130"/>
     </row>
-    <row r="165" spans="1:31" s="113" customFormat="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:31" s="113" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A165" s="1"/>
       <c r="B165" s="33"/>
       <c r="C165" s="76">
@@ -13732,7 +13754,7 @@
       <c r="AD165" s="130"/>
       <c r="AE165" s="130"/>
     </row>
-    <row r="166" spans="1:31" s="113" customFormat="1" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:31" s="113" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A166" s="1"/>
       <c r="B166" s="33"/>
       <c r="C166" s="76">
@@ -13770,7 +13792,7 @@
       <c r="AD166" s="130"/>
       <c r="AE166" s="130"/>
     </row>
-    <row r="167" spans="1:31" s="112" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:31" s="112" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A167" s="1"/>
       <c r="B167" s="33"/>
       <c r="C167" s="76">
@@ -13824,7 +13846,7 @@
       <c r="AD167" s="130"/>
       <c r="AE167" s="130"/>
     </row>
-    <row r="168" spans="1:31" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A168" s="1"/>
       <c r="B168" s="33"/>
       <c r="C168" s="76">
@@ -13887,7 +13909,7 @@
       <c r="AA168" s="1"/>
       <c r="AB168" s="1"/>
     </row>
-    <row r="169" spans="1:31" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A169" s="1"/>
       <c r="B169" s="33"/>
       <c r="C169" s="76">
@@ -13948,7 +13970,7 @@
       <c r="AA169" s="1"/>
       <c r="AB169" s="1"/>
     </row>
-    <row r="170" spans="1:31" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A170" s="1"/>
       <c r="B170" s="33"/>
       <c r="C170" s="76">
@@ -14007,7 +14029,7 @@
       <c r="AA170" s="1"/>
       <c r="AB170" s="1"/>
     </row>
-    <row r="171" spans="1:31" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A171" s="1"/>
       <c r="B171" s="33"/>
       <c r="C171" s="76">
@@ -14066,7 +14088,7 @@
       <c r="AA171" s="1"/>
       <c r="AB171" s="1"/>
     </row>
-    <row r="172" spans="1:31" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A172" s="1"/>
       <c r="B172" s="33"/>
       <c r="C172" s="76">
@@ -14125,7 +14147,7 @@
       <c r="AA172" s="1"/>
       <c r="AB172" s="1"/>
     </row>
-    <row r="173" spans="1:31" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A173" s="1"/>
       <c r="B173" s="33"/>
       <c r="C173" s="76">
@@ -14186,7 +14208,7 @@
       <c r="AA173" s="1"/>
       <c r="AB173" s="1"/>
     </row>
-    <row r="174" spans="1:31" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A174" s="1"/>
       <c r="B174" s="33"/>
       <c r="C174" s="76">
@@ -14247,7 +14269,7 @@
       <c r="AA174" s="1"/>
       <c r="AB174" s="1"/>
     </row>
-    <row r="175" spans="1:31" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A175" s="1"/>
       <c r="B175" s="33"/>
       <c r="C175" s="76">
@@ -14306,7 +14328,7 @@
       <c r="AA175" s="1"/>
       <c r="AB175" s="1"/>
     </row>
-    <row r="176" spans="1:31" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:31" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A176" s="1"/>
       <c r="B176" s="33"/>
       <c r="C176" s="76">
@@ -14365,7 +14387,7 @@
       <c r="AA176" s="1"/>
       <c r="AB176" s="1"/>
     </row>
-    <row r="177" spans="1:28" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A177" s="1"/>
       <c r="B177" s="33"/>
       <c r="C177" s="76">
@@ -14424,7 +14446,7 @@
       <c r="AA177" s="1"/>
       <c r="AB177" s="1"/>
     </row>
-    <row r="178" spans="1:28" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A178" s="1"/>
       <c r="B178" s="33"/>
       <c r="C178" s="76">
@@ -14485,7 +14507,7 @@
       <c r="AA178" s="1"/>
       <c r="AB178" s="1"/>
     </row>
-    <row r="179" spans="1:28" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A179" s="1"/>
       <c r="B179" s="33"/>
       <c r="C179" s="76">
@@ -14546,7 +14568,7 @@
       <c r="AA179" s="1"/>
       <c r="AB179" s="1"/>
     </row>
-    <row r="180" spans="1:28" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A180" s="1"/>
       <c r="B180" s="33"/>
       <c r="C180" s="76">
@@ -14605,7 +14627,7 @@
       <c r="AA180" s="1"/>
       <c r="AB180" s="1"/>
     </row>
-    <row r="181" spans="1:28" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A181" s="1"/>
       <c r="B181" s="33"/>
       <c r="C181" s="76">
@@ -14662,7 +14684,7 @@
       <c r="AA181" s="1"/>
       <c r="AB181" s="1"/>
     </row>
-    <row r="182" spans="1:28" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A182" s="1"/>
       <c r="B182" s="33"/>
       <c r="C182" s="76">
@@ -14721,7 +14743,7 @@
       <c r="AA182" s="1"/>
       <c r="AB182" s="1"/>
     </row>
-    <row r="183" spans="1:28" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A183" s="1"/>
       <c r="B183" s="33"/>
       <c r="C183" s="76">
@@ -14782,7 +14804,7 @@
       <c r="AA183" s="1"/>
       <c r="AB183" s="1"/>
     </row>
-    <row r="184" spans="1:28" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A184" s="1"/>
       <c r="B184" s="33"/>
       <c r="C184" s="76">
@@ -14843,7 +14865,7 @@
       <c r="AA184" s="1"/>
       <c r="AB184" s="1"/>
     </row>
-    <row r="185" spans="1:28" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A185" s="1"/>
       <c r="B185" s="33"/>
       <c r="C185" s="76">
@@ -14902,7 +14924,7 @@
       <c r="AA185" s="1"/>
       <c r="AB185" s="1"/>
     </row>
-    <row r="186" spans="1:28" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A186" s="1"/>
       <c r="B186" s="33"/>
       <c r="C186" s="76">
@@ -14961,7 +14983,7 @@
       <c r="AA186" s="1"/>
       <c r="AB186" s="1"/>
     </row>
-    <row r="187" spans="1:28" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A187" s="1"/>
       <c r="B187" s="33"/>
       <c r="C187" s="76">
@@ -15020,7 +15042,7 @@
       <c r="AA187" s="1"/>
       <c r="AB187" s="1"/>
     </row>
-    <row r="188" spans="1:28" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A188" s="1"/>
       <c r="B188" s="33"/>
       <c r="C188" s="76">
@@ -15083,7 +15105,7 @@
       <c r="AA188" s="1"/>
       <c r="AB188" s="1"/>
     </row>
-    <row r="189" spans="1:28" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A189" s="1"/>
       <c r="B189" s="33"/>
       <c r="C189" s="76">
@@ -15142,7 +15164,7 @@
       <c r="AA189" s="1"/>
       <c r="AB189" s="1"/>
     </row>
-    <row r="190" spans="1:28" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A190" s="1"/>
       <c r="B190" s="33"/>
       <c r="C190" s="76">
@@ -15199,7 +15221,7 @@
       <c r="AA190" s="1"/>
       <c r="AB190" s="1"/>
     </row>
-    <row r="191" spans="1:28" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A191" s="1"/>
       <c r="B191" s="33"/>
       <c r="C191" s="76">
@@ -15256,7 +15278,7 @@
       <c r="AA191" s="1"/>
       <c r="AB191" s="1"/>
     </row>
-    <row r="192" spans="1:28" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:28" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A192" s="1"/>
       <c r="B192" s="33"/>
       <c r="C192" s="76">
@@ -15313,7 +15335,7 @@
       <c r="AA192" s="1"/>
       <c r="AB192" s="1"/>
     </row>
-    <row r="193" spans="1:30" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A193" s="1"/>
       <c r="B193" s="33"/>
       <c r="C193" s="76">
@@ -15372,7 +15394,7 @@
       <c r="AA193" s="1"/>
       <c r="AB193" s="1"/>
     </row>
-    <row r="194" spans="1:30" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A194" s="1"/>
       <c r="B194" s="33"/>
       <c r="C194" s="76">
@@ -15429,7 +15451,7 @@
       <c r="AA194" s="1"/>
       <c r="AB194" s="1"/>
     </row>
-    <row r="195" spans="1:30" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A195" s="1"/>
       <c r="B195" s="33"/>
       <c r="C195" s="76">
@@ -15486,7 +15508,7 @@
       <c r="AA195" s="1"/>
       <c r="AB195" s="1"/>
     </row>
-    <row r="196" spans="1:30" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A196" s="1"/>
       <c r="B196" s="33"/>
       <c r="C196" s="76">
@@ -15543,7 +15565,7 @@
       <c r="AA196" s="1"/>
       <c r="AB196" s="1"/>
     </row>
-    <row r="197" spans="1:30" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A197" s="1"/>
       <c r="B197" s="33"/>
       <c r="C197" s="76">
@@ -15600,7 +15622,7 @@
       <c r="AA197" s="1"/>
       <c r="AB197" s="1"/>
     </row>
-    <row r="198" spans="1:30" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A198" s="1"/>
       <c r="B198" s="33"/>
       <c r="C198" s="76">
@@ -15659,7 +15681,7 @@
       <c r="AA198" s="1"/>
       <c r="AB198" s="1"/>
     </row>
-    <row r="199" spans="1:30" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A199" s="1"/>
       <c r="B199" s="33"/>
       <c r="C199" s="76">
@@ -15716,7 +15738,7 @@
       <c r="AA199" s="1"/>
       <c r="AB199" s="1"/>
     </row>
-    <row r="200" spans="1:30" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A200" s="1"/>
       <c r="B200" s="33"/>
       <c r="C200" s="76">
@@ -15773,7 +15795,7 @@
       <c r="AA200" s="1"/>
       <c r="AB200" s="1"/>
     </row>
-    <row r="201" spans="1:30" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A201" s="1"/>
       <c r="B201" s="33"/>
       <c r="C201" s="76">
@@ -15830,7 +15852,7 @@
       <c r="AA201" s="1"/>
       <c r="AB201" s="1"/>
     </row>
-    <row r="202" spans="1:30" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A202" s="1"/>
       <c r="B202" s="33"/>
       <c r="C202" s="76">
@@ -15887,7 +15909,7 @@
       <c r="AA202" s="1"/>
       <c r="AB202" s="1"/>
     </row>
-    <row r="203" spans="1:30" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A203" s="1"/>
       <c r="B203" s="33"/>
       <c r="C203" s="76">
@@ -15946,7 +15968,7 @@
       <c r="AA203" s="1"/>
       <c r="AB203" s="1"/>
     </row>
-    <row r="204" spans="1:30" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A204" s="1"/>
       <c r="B204" s="33"/>
       <c r="C204" s="76">
@@ -16003,7 +16025,7 @@
       <c r="AA204" s="1"/>
       <c r="AB204" s="1"/>
     </row>
-    <row r="205" spans="1:30" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A205" s="1"/>
       <c r="B205" s="33"/>
       <c r="C205" s="76">
@@ -16060,7 +16082,7 @@
       <c r="AA205" s="1"/>
       <c r="AB205" s="1"/>
     </row>
-    <row r="206" spans="1:30" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A206" s="1"/>
       <c r="B206" s="33"/>
       <c r="C206" s="76">
@@ -16117,7 +16139,7 @@
       <c r="AA206" s="1"/>
       <c r="AB206" s="1"/>
     </row>
-    <row r="207" spans="1:30" s="112" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:30" s="112" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A207" s="1"/>
       <c r="B207" s="33"/>
       <c r="C207" s="76">
@@ -16174,7 +16196,7 @@
       <c r="AA207" s="1"/>
       <c r="AB207" s="1"/>
     </row>
-    <row r="208" spans="1:30" s="113" customFormat="1" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:30" s="113" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A208" s="1"/>
       <c r="B208" s="33"/>
       <c r="C208" s="76">
@@ -16209,7 +16231,7 @@
       <c r="AC208" s="130"/>
       <c r="AD208" s="130"/>
     </row>
-    <row r="209" spans="1:28" s="133" customFormat="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:28" s="133" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A209" s="1"/>
       <c r="B209" s="33"/>
       <c r="C209" s="76">
@@ -16269,7 +16291,7 @@
       <c r="AA209" s="1"/>
       <c r="AB209" s="1"/>
     </row>
-    <row r="210" spans="1:28" s="142" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A210" s="1"/>
       <c r="B210" s="33"/>
       <c r="C210" s="76">
@@ -16339,7 +16361,7 @@
       <c r="AA210" s="1"/>
       <c r="AB210" s="1"/>
     </row>
-    <row r="211" spans="1:28" s="142" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A211" s="1"/>
       <c r="B211" s="33"/>
       <c r="C211" s="76">
@@ -16409,7 +16431,7 @@
       <c r="AA211" s="1"/>
       <c r="AB211" s="1"/>
     </row>
-    <row r="212" spans="1:28" s="133" customFormat="1" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:28" s="133" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A212" s="1"/>
       <c r="B212" s="33"/>
       <c r="C212" s="76">
@@ -16444,7 +16466,7 @@
       <c r="AA212" s="1"/>
       <c r="AB212" s="1"/>
     </row>
-    <row r="213" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:28" s="133" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A213" s="1"/>
       <c r="B213" s="33"/>
       <c r="C213" s="76">
@@ -16495,7 +16517,7 @@
       <c r="AA213" s="1"/>
       <c r="AB213" s="1"/>
     </row>
-    <row r="214" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A214" s="1"/>
       <c r="B214" s="33"/>
       <c r="C214" s="76">
@@ -16558,7 +16580,7 @@
       <c r="AA214" s="1"/>
       <c r="AB214" s="1"/>
     </row>
-    <row r="215" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A215" s="1"/>
       <c r="B215" s="33"/>
       <c r="C215" s="76">
@@ -16621,7 +16643,7 @@
       <c r="AA215" s="1"/>
       <c r="AB215" s="1"/>
     </row>
-    <row r="216" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A216" s="1"/>
       <c r="B216" s="33"/>
       <c r="C216" s="76">
@@ -16678,7 +16700,7 @@
       <c r="AA216" s="1"/>
       <c r="AB216" s="1"/>
     </row>
-    <row r="217" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A217" s="1"/>
       <c r="B217" s="33"/>
       <c r="C217" s="76">
@@ -16737,7 +16759,7 @@
       <c r="AA217" s="1"/>
       <c r="AB217" s="1"/>
     </row>
-    <row r="218" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A218" s="1"/>
       <c r="B218" s="33"/>
       <c r="C218" s="76">
@@ -16796,7 +16818,7 @@
       <c r="AA218" s="1"/>
       <c r="AB218" s="1"/>
     </row>
-    <row r="219" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A219" s="1"/>
       <c r="B219" s="33"/>
       <c r="C219" s="76">
@@ -16857,7 +16879,7 @@
       <c r="AA219" s="1"/>
       <c r="AB219" s="1"/>
     </row>
-    <row r="220" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A220" s="1"/>
       <c r="B220" s="33"/>
       <c r="C220" s="76">
@@ -16918,7 +16940,7 @@
       <c r="AA220" s="1"/>
       <c r="AB220" s="1"/>
     </row>
-    <row r="221" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A221" s="1"/>
       <c r="B221" s="33"/>
       <c r="C221" s="76">
@@ -16975,7 +16997,7 @@
       <c r="AA221" s="1"/>
       <c r="AB221" s="1"/>
     </row>
-    <row r="222" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A222" s="1"/>
       <c r="B222" s="33"/>
       <c r="C222" s="76">
@@ -17032,7 +17054,7 @@
       <c r="AA222" s="1"/>
       <c r="AB222" s="1"/>
     </row>
-    <row r="223" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A223" s="1"/>
       <c r="B223" s="33"/>
       <c r="C223" s="76">
@@ -17089,7 +17111,7 @@
       <c r="AA223" s="1"/>
       <c r="AB223" s="1"/>
     </row>
-    <row r="224" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A224" s="1"/>
       <c r="B224" s="33"/>
       <c r="C224" s="76">
@@ -17148,7 +17170,7 @@
       <c r="AA224" s="1"/>
       <c r="AB224" s="1"/>
     </row>
-    <row r="225" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A225" s="1"/>
       <c r="B225" s="33"/>
       <c r="C225" s="76">
@@ -17207,7 +17229,7 @@
       <c r="AA225" s="1"/>
       <c r="AB225" s="1"/>
     </row>
-    <row r="226" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A226" s="1"/>
       <c r="B226" s="33"/>
       <c r="C226" s="76">
@@ -17264,7 +17286,7 @@
       <c r="AA226" s="1"/>
       <c r="AB226" s="1"/>
     </row>
-    <row r="227" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A227" s="1"/>
       <c r="B227" s="33"/>
       <c r="C227" s="76">
@@ -17321,7 +17343,7 @@
       <c r="AA227" s="1"/>
       <c r="AB227" s="1"/>
     </row>
-    <row r="228" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A228" s="1"/>
       <c r="B228" s="33"/>
       <c r="C228" s="76">
@@ -17378,7 +17400,7 @@
       <c r="AA228" s="1"/>
       <c r="AB228" s="1"/>
     </row>
-    <row r="229" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A229" s="1"/>
       <c r="B229" s="33"/>
       <c r="C229" s="76">
@@ -17437,7 +17459,7 @@
       <c r="AA229" s="1"/>
       <c r="AB229" s="1"/>
     </row>
-    <row r="230" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A230" s="1"/>
       <c r="B230" s="33"/>
       <c r="C230" s="76">
@@ -17496,7 +17518,7 @@
       <c r="AA230" s="1"/>
       <c r="AB230" s="1"/>
     </row>
-    <row r="231" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A231" s="1"/>
       <c r="B231" s="33"/>
       <c r="C231" s="76">
@@ -17553,7 +17575,7 @@
       <c r="AA231" s="1"/>
       <c r="AB231" s="1"/>
     </row>
-    <row r="232" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A232" s="1"/>
       <c r="B232" s="33"/>
       <c r="C232" s="76">
@@ -17610,7 +17632,7 @@
       <c r="AA232" s="1"/>
       <c r="AB232" s="1"/>
     </row>
-    <row r="233" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A233" s="1"/>
       <c r="B233" s="33"/>
       <c r="C233" s="76">
@@ -17667,7 +17689,7 @@
       <c r="AA233" s="1"/>
       <c r="AB233" s="1"/>
     </row>
-    <row r="234" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A234" s="1"/>
       <c r="B234" s="33"/>
       <c r="C234" s="76">
@@ -17737,7 +17759,7 @@
       <c r="AA234" s="1"/>
       <c r="AB234" s="1"/>
     </row>
-    <row r="235" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A235" s="1"/>
       <c r="B235" s="33"/>
       <c r="C235" s="76">
@@ -17804,7 +17826,7 @@
       <c r="AA235" s="1"/>
       <c r="AB235" s="1"/>
     </row>
-    <row r="236" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A236" s="1"/>
       <c r="B236" s="33"/>
       <c r="C236" s="76">
@@ -17867,7 +17889,7 @@
       <c r="AA236" s="1"/>
       <c r="AB236" s="1"/>
     </row>
-    <row r="237" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A237" s="1"/>
       <c r="B237" s="33"/>
       <c r="C237" s="76">
@@ -17930,7 +17952,7 @@
       <c r="AA237" s="1"/>
       <c r="AB237" s="1"/>
     </row>
-    <row r="238" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A238" s="1"/>
       <c r="B238" s="33"/>
       <c r="C238" s="76">
@@ -17997,7 +18019,7 @@
       <c r="AA238" s="1"/>
       <c r="AB238" s="1"/>
     </row>
-    <row r="239" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A239" s="1"/>
       <c r="B239" s="33"/>
       <c r="C239" s="76">
@@ -18066,7 +18088,7 @@
       <c r="AA239" s="1"/>
       <c r="AB239" s="1"/>
     </row>
-    <row r="240" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A240" s="1"/>
       <c r="B240" s="33"/>
       <c r="C240" s="76">
@@ -18133,7 +18155,7 @@
       <c r="AA240" s="1"/>
       <c r="AB240" s="1"/>
     </row>
-    <row r="241" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A241" s="1"/>
       <c r="B241" s="33"/>
       <c r="C241" s="76">
@@ -18200,7 +18222,7 @@
       <c r="AA241" s="1"/>
       <c r="AB241" s="1"/>
     </row>
-    <row r="242" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A242" s="1"/>
       <c r="B242" s="33"/>
       <c r="C242" s="76">
@@ -18267,7 +18289,7 @@
       <c r="AA242" s="1"/>
       <c r="AB242" s="1"/>
     </row>
-    <row r="243" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A243" s="1"/>
       <c r="B243" s="33"/>
       <c r="C243" s="76">
@@ -18334,7 +18356,7 @@
       <c r="AA243" s="1"/>
       <c r="AB243" s="1"/>
     </row>
-    <row r="244" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A244" s="1"/>
       <c r="B244" s="33"/>
       <c r="C244" s="76">
@@ -18403,7 +18425,7 @@
       <c r="AA244" s="1"/>
       <c r="AB244" s="1"/>
     </row>
-    <row r="245" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A245" s="1"/>
       <c r="B245" s="33"/>
       <c r="C245" s="76">
@@ -18470,7 +18492,7 @@
       <c r="AA245" s="1"/>
       <c r="AB245" s="1"/>
     </row>
-    <row r="246" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A246" s="1"/>
       <c r="B246" s="33"/>
       <c r="C246" s="76">
@@ -18537,7 +18559,7 @@
       <c r="AA246" s="1"/>
       <c r="AB246" s="1"/>
     </row>
-    <row r="247" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A247" s="1"/>
       <c r="B247" s="33"/>
       <c r="C247" s="76">
@@ -18604,7 +18626,7 @@
       <c r="AA247" s="1"/>
       <c r="AB247" s="1"/>
     </row>
-    <row r="248" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A248" s="1"/>
       <c r="B248" s="33"/>
       <c r="C248" s="76">
@@ -18671,7 +18693,7 @@
       <c r="AA248" s="1"/>
       <c r="AB248" s="1"/>
     </row>
-    <row r="249" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A249" s="1"/>
       <c r="B249" s="33"/>
       <c r="C249" s="76">
@@ -18740,7 +18762,7 @@
       <c r="AA249" s="1"/>
       <c r="AB249" s="1"/>
     </row>
-    <row r="250" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A250" s="1"/>
       <c r="B250" s="33"/>
       <c r="C250" s="76">
@@ -18807,7 +18829,7 @@
       <c r="AA250" s="1"/>
       <c r="AB250" s="1"/>
     </row>
-    <row r="251" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A251" s="1"/>
       <c r="B251" s="33"/>
       <c r="C251" s="76">
@@ -18874,7 +18896,7 @@
       <c r="AA251" s="1"/>
       <c r="AB251" s="1"/>
     </row>
-    <row r="252" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A252" s="1"/>
       <c r="B252" s="33"/>
       <c r="C252" s="76">
@@ -18941,7 +18963,7 @@
       <c r="AA252" s="1"/>
       <c r="AB252" s="1"/>
     </row>
-    <row r="253" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A253" s="1"/>
       <c r="B253" s="33"/>
       <c r="C253" s="76">
@@ -19008,7 +19030,7 @@
       <c r="AA253" s="1"/>
       <c r="AB253" s="1"/>
     </row>
-    <row r="254" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A254" s="1"/>
       <c r="B254" s="33"/>
       <c r="C254" s="76">
@@ -19069,7 +19091,7 @@
       <c r="AA254" s="1"/>
       <c r="AB254" s="1"/>
     </row>
-    <row r="255" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A255" s="1"/>
       <c r="B255" s="33"/>
       <c r="C255" s="76">
@@ -19126,7 +19148,7 @@
       <c r="AA255" s="1"/>
       <c r="AB255" s="1"/>
     </row>
-    <row r="256" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A256" s="1"/>
       <c r="B256" s="33"/>
       <c r="C256" s="76">
@@ -19183,7 +19205,7 @@
       <c r="AA256" s="1"/>
       <c r="AB256" s="1"/>
     </row>
-    <row r="257" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A257" s="1"/>
       <c r="B257" s="33"/>
       <c r="C257" s="76">
@@ -19240,7 +19262,7 @@
       <c r="AA257" s="1"/>
       <c r="AB257" s="1"/>
     </row>
-    <row r="258" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A258" s="1"/>
       <c r="B258" s="33"/>
       <c r="C258" s="76">
@@ -19297,7 +19319,7 @@
       <c r="AA258" s="1"/>
       <c r="AB258" s="1"/>
     </row>
-    <row r="259" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A259" s="1"/>
       <c r="B259" s="33"/>
       <c r="C259" s="76">
@@ -19366,7 +19388,7 @@
       <c r="AA259" s="1"/>
       <c r="AB259" s="1"/>
     </row>
-    <row r="260" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A260" s="1"/>
       <c r="B260" s="33"/>
       <c r="C260" s="76">
@@ -19433,7 +19455,7 @@
       <c r="AA260" s="1"/>
       <c r="AB260" s="1"/>
     </row>
-    <row r="261" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A261" s="1"/>
       <c r="B261" s="33"/>
       <c r="C261" s="76">
@@ -19500,7 +19522,7 @@
       <c r="AA261" s="1"/>
       <c r="AB261" s="1"/>
     </row>
-    <row r="262" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A262" s="1"/>
       <c r="B262" s="33"/>
       <c r="C262" s="76">
@@ -19567,7 +19589,7 @@
       <c r="AA262" s="1"/>
       <c r="AB262" s="1"/>
     </row>
-    <row r="263" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A263" s="1"/>
       <c r="B263" s="33"/>
       <c r="C263" s="76">
@@ -19634,7 +19656,7 @@
       <c r="AA263" s="1"/>
       <c r="AB263" s="1"/>
     </row>
-    <row r="264" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A264" s="1"/>
       <c r="B264" s="33"/>
       <c r="C264" s="76">
@@ -19693,7 +19715,7 @@
       <c r="AA264" s="1"/>
       <c r="AB264" s="1"/>
     </row>
-    <row r="265" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A265" s="1"/>
       <c r="B265" s="33"/>
       <c r="C265" s="76">
@@ -19755,7 +19777,7 @@
       <c r="AA265" s="1"/>
       <c r="AB265" s="1"/>
     </row>
-    <row r="266" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A266" s="1"/>
       <c r="B266" s="33"/>
       <c r="C266" s="76">
@@ -19816,7 +19838,7 @@
       <c r="AA266" s="1"/>
       <c r="AB266" s="1"/>
     </row>
-    <row r="267" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A267" s="1"/>
       <c r="B267" s="33"/>
       <c r="C267" s="76">
@@ -19876,7 +19898,7 @@
       <c r="AA267" s="1"/>
       <c r="AB267" s="1"/>
     </row>
-    <row r="268" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A268" s="1"/>
       <c r="B268" s="33"/>
       <c r="C268" s="76">
@@ -19943,7 +19965,7 @@
       <c r="AA268" s="1"/>
       <c r="AB268" s="1"/>
     </row>
-    <row r="269" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A269" s="1"/>
       <c r="B269" s="33"/>
       <c r="C269" s="76">
@@ -20008,7 +20030,7 @@
       <c r="AA269" s="1"/>
       <c r="AB269" s="1"/>
     </row>
-    <row r="270" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A270" s="1"/>
       <c r="B270" s="33"/>
       <c r="C270" s="76">
@@ -20070,7 +20092,7 @@
       <c r="AA270" s="1"/>
       <c r="AB270" s="1"/>
     </row>
-    <row r="271" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A271" s="1"/>
       <c r="B271" s="33"/>
       <c r="C271" s="76">
@@ -20130,7 +20152,7 @@
       <c r="AA271" s="1"/>
       <c r="AB271" s="1"/>
     </row>
-    <row r="272" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A272" s="1"/>
       <c r="B272" s="33"/>
       <c r="C272" s="76">
@@ -20187,7 +20209,7 @@
       <c r="AA272" s="1"/>
       <c r="AB272" s="1"/>
     </row>
-    <row r="273" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A273" s="1"/>
       <c r="B273" s="33"/>
       <c r="C273" s="76">
@@ -20254,7 +20276,7 @@
       <c r="AA273" s="1"/>
       <c r="AB273" s="1"/>
     </row>
-    <row r="274" spans="1:28" s="133" customFormat="1" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:28" s="133" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A274" s="1"/>
       <c r="B274" s="33"/>
       <c r="C274" s="76">
@@ -20287,7 +20309,7 @@
       <c r="AA274" s="1"/>
       <c r="AB274" s="1"/>
     </row>
-    <row r="275" spans="1:28" s="133" customFormat="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:28" s="133" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A275" s="1"/>
       <c r="B275" s="33"/>
       <c r="C275" s="76">
@@ -20343,7 +20365,7 @@
       <c r="AA275" s="1"/>
       <c r="AB275" s="1"/>
     </row>
-    <row r="276" spans="1:28" s="142" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A276" s="1"/>
       <c r="B276" s="33"/>
       <c r="C276" s="76">
@@ -20396,7 +20418,7 @@
       <c r="AA276" s="1"/>
       <c r="AB276" s="1"/>
     </row>
-    <row r="277" spans="1:28" s="142" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A277" s="1"/>
       <c r="B277" s="33"/>
       <c r="C277" s="76">
@@ -20449,7 +20471,7 @@
       <c r="AA277" s="1"/>
       <c r="AB277" s="1"/>
     </row>
-    <row r="278" spans="1:28" s="133" customFormat="1" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:28" s="133" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A278" s="1"/>
       <c r="B278" s="33"/>
       <c r="C278" s="76">
@@ -20484,7 +20506,7 @@
       <c r="AA278" s="1"/>
       <c r="AB278" s="1"/>
     </row>
-    <row r="279" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:28" s="133" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A279" s="1"/>
       <c r="B279" s="33"/>
       <c r="C279" s="76">
@@ -20534,7 +20556,7 @@
       <c r="AA279" s="1"/>
       <c r="AB279" s="1"/>
     </row>
-    <row r="280" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A280" s="1"/>
       <c r="B280" s="33"/>
       <c r="C280" s="76">
@@ -20592,7 +20614,7 @@
       <c r="AA280" s="1"/>
       <c r="AB280" s="1"/>
     </row>
-    <row r="281" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A281" s="1"/>
       <c r="B281" s="33"/>
       <c r="C281" s="76">
@@ -20650,7 +20672,7 @@
       <c r="AA281" s="1"/>
       <c r="AB281" s="1"/>
     </row>
-    <row r="282" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A282" s="1"/>
       <c r="B282" s="33"/>
       <c r="C282" s="76">
@@ -20703,7 +20725,7 @@
       <c r="AA282" s="1"/>
       <c r="AB282" s="1"/>
     </row>
-    <row r="283" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A283" s="1"/>
       <c r="B283" s="33"/>
       <c r="C283" s="76">
@@ -20755,7 +20777,7 @@
       <c r="AA283" s="1"/>
       <c r="AB283" s="1"/>
     </row>
-    <row r="284" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A284" s="1"/>
       <c r="B284" s="33"/>
       <c r="C284" s="76">
@@ -20810,7 +20832,7 @@
       <c r="AA284" s="1"/>
       <c r="AB284" s="1"/>
     </row>
-    <row r="285" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A285" s="1"/>
       <c r="B285" s="33"/>
       <c r="C285" s="76">
@@ -20864,7 +20886,7 @@
       <c r="AA285" s="1"/>
       <c r="AB285" s="1"/>
     </row>
-    <row r="286" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A286" s="1"/>
       <c r="B286" s="33"/>
       <c r="C286" s="76">
@@ -20918,7 +20940,7 @@
       <c r="AA286" s="1"/>
       <c r="AB286" s="1"/>
     </row>
-    <row r="287" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A287" s="1"/>
       <c r="B287" s="33"/>
       <c r="C287" s="76">
@@ -20968,7 +20990,7 @@
       <c r="AA287" s="1"/>
       <c r="AB287" s="1"/>
     </row>
-    <row r="288" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A288" s="1"/>
       <c r="B288" s="33"/>
       <c r="C288" s="76">
@@ -21018,7 +21040,7 @@
       <c r="AA288" s="1"/>
       <c r="AB288" s="1"/>
     </row>
-    <row r="289" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A289" s="1"/>
       <c r="B289" s="33"/>
       <c r="C289" s="76">
@@ -21071,7 +21093,7 @@
       <c r="AA289" s="1"/>
       <c r="AB289" s="1"/>
     </row>
-    <row r="290" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A290" s="1"/>
       <c r="B290" s="33"/>
       <c r="C290" s="76">
@@ -21125,7 +21147,7 @@
       <c r="AA290" s="1"/>
       <c r="AB290" s="1"/>
     </row>
-    <row r="291" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A291" s="1"/>
       <c r="B291" s="33"/>
       <c r="C291" s="76">
@@ -21179,7 +21201,7 @@
       <c r="AA291" s="1"/>
       <c r="AB291" s="1"/>
     </row>
-    <row r="292" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A292" s="1"/>
       <c r="B292" s="33"/>
       <c r="C292" s="76">
@@ -21229,7 +21251,7 @@
       <c r="AA292" s="1"/>
       <c r="AB292" s="1"/>
     </row>
-    <row r="293" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A293" s="1"/>
       <c r="B293" s="33"/>
       <c r="C293" s="76">
@@ -21279,7 +21301,7 @@
       <c r="AA293" s="1"/>
       <c r="AB293" s="1"/>
     </row>
-    <row r="294" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A294" s="1"/>
       <c r="B294" s="33"/>
       <c r="C294" s="76">
@@ -21332,7 +21354,7 @@
       <c r="AA294" s="1"/>
       <c r="AB294" s="1"/>
     </row>
-    <row r="295" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A295" s="1"/>
       <c r="B295" s="33"/>
       <c r="C295" s="76">
@@ -21384,7 +21406,7 @@
       <c r="AA295" s="1"/>
       <c r="AB295" s="1"/>
     </row>
-    <row r="296" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A296" s="1"/>
       <c r="B296" s="33"/>
       <c r="C296" s="76">
@@ -21436,7 +21458,7 @@
       <c r="AA296" s="1"/>
       <c r="AB296" s="1"/>
     </row>
-    <row r="297" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A297" s="1"/>
       <c r="B297" s="33"/>
       <c r="C297" s="76">
@@ -21485,7 +21507,7 @@
       <c r="AA297" s="1"/>
       <c r="AB297" s="1"/>
     </row>
-    <row r="298" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A298" s="1"/>
       <c r="B298" s="33"/>
       <c r="C298" s="76">
@@ -21532,7 +21554,7 @@
       <c r="AA298" s="1"/>
       <c r="AB298" s="1"/>
     </row>
-    <row r="299" spans="1:28" s="133" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:28" s="133" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A299" s="1"/>
       <c r="B299" s="33"/>
       <c r="C299" s="76">
@@ -21585,7 +21607,7 @@
       <c r="AA299" s="1"/>
       <c r="AB299" s="1"/>
     </row>
-    <row r="300" spans="1:28" s="133" customFormat="1" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:28" s="133" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A300" s="1"/>
       <c r="B300" s="33"/>
       <c r="C300" s="76">
@@ -21618,7 +21640,7 @@
       <c r="AA300" s="1"/>
       <c r="AB300" s="1"/>
     </row>
-    <row r="301" spans="1:28" s="99" customFormat="1" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:28" s="99" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A301" s="1"/>
       <c r="B301" s="33"/>
       <c r="C301" s="76">
@@ -21686,7 +21708,7 @@
       <c r="AA302" s="1"/>
       <c r="AB302" s="1"/>
     </row>
-    <row r="303" spans="1:28" s="99" customFormat="1" ht="5.0999999999999996" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:28" s="99" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A303" s="1"/>
       <c r="B303" s="19"/>
       <c r="C303" s="80">
@@ -21719,7 +21741,7 @@
       <c r="AA303" s="1"/>
       <c r="AB303" s="1"/>
     </row>
-    <row r="304" spans="1:28" s="99" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:28" s="99" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A304" s="1"/>
       <c r="B304" s="1"/>
       <c r="C304" s="76">
@@ -21752,7 +21774,7 @@
       <c r="AA304" s="1"/>
       <c r="AB304" s="1"/>
     </row>
-    <row r="305" spans="1:28" s="101" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:28" s="101" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A305" s="1"/>
       <c r="B305" s="1"/>
       <c r="C305" s="76">
@@ -21818,7 +21840,7 @@
       <c r="AA306" s="1"/>
       <c r="AB306" s="1"/>
     </row>
-    <row r="307" spans="1:28" s="101" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:28" s="101" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A307" s="1"/>
       <c r="B307" s="34" t="s">
         <v>21</v>
@@ -21853,7 +21875,7 @@
       <c r="AA307" s="1"/>
       <c r="AB307" s="1"/>
     </row>
-    <row r="308" spans="1:28" s="101" customFormat="1" hidden="1" outlineLevel="4" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:28" s="101" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A308" s="1"/>
       <c r="B308" s="33"/>
       <c r="C308" s="76">
@@ -22314,7 +22336,7 @@
       <c r="K320" s="2"/>
       <c r="L320" s="132">
         <f>i_w_start_len1*i_n1_len^L323</f>
-        <v>729</v>
+        <v>24</v>
       </c>
       <c r="M320" s="2"/>
       <c r="N320" s="127" t="s">
@@ -22399,7 +22421,7 @@
       </c>
       <c r="K322" s="126"/>
       <c r="L322" s="31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M322" s="126"/>
       <c r="N322" s="2"/>
@@ -22438,7 +22460,7 @@
       <c r="K323" s="2"/>
       <c r="L323" s="132">
         <f>COUNTIF(J341:O341,TRUE)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M323" s="2"/>
       <c r="N323" s="2"/>
@@ -22663,7 +22685,7 @@
         <v>1</v>
       </c>
       <c r="L328" s="31">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M328" s="31">
         <v>1</v>
@@ -22671,7 +22693,7 @@
       <c r="N328" s="2"/>
       <c r="O328" s="54"/>
       <c r="P328" s="149">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Q328" s="149">
         <v>1</v>
@@ -22708,7 +22730,7 @@
       <c r="J329" s="54"/>
       <c r="K329" s="54"/>
       <c r="L329" s="31">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="M329" s="31">
         <v>0.5</v>
@@ -22753,7 +22775,7 @@
       <c r="J330" s="54"/>
       <c r="K330" s="54"/>
       <c r="L330" s="31">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="M330" s="31">
         <v>1.5</v>
@@ -23222,10 +23244,10 @@
         <v>1</v>
       </c>
       <c r="N341" s="31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O341" s="31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P341" s="2"/>
       <c r="Q341" s="31">
@@ -23274,11 +23296,11 @@
       </c>
       <c r="N342" s="132">
         <f>COUNTIF($J$341:N341,TRUE)-1</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O342" s="132">
         <f>COUNTIF($J$341:O341,TRUE)-1</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P342" s="2"/>
       <c r="Q342" s="2"/>
@@ -24215,34 +24237,34 @@
       </c>
       <c r="I365" s="149"/>
       <c r="J365" s="149"/>
-      <c r="K365" s="2"/>
-      <c r="L365" s="107"/>
-      <c r="M365" s="2"/>
+      <c r="K365" s="149"/>
+      <c r="L365" s="149"/>
+      <c r="M365" s="149"/>
       <c r="N365" s="2"/>
       <c r="O365" s="32">
-        <v>0.15</v>
+        <v>0.4</v>
       </c>
       <c r="P365" s="32">
+        <v>0.3</v>
+      </c>
+      <c r="Q365" s="32">
         <v>0.1</v>
       </c>
-      <c r="Q365" s="32">
-        <v>0.05</v>
-      </c>
       <c r="R365" s="32">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="S365" s="2"/>
       <c r="T365" s="32">
-        <v>0.15</v>
+        <v>0.4</v>
       </c>
       <c r="U365" s="32">
+        <v>0.3</v>
+      </c>
+      <c r="V365" s="32">
         <v>0.1</v>
       </c>
-      <c r="V365" s="32">
-        <v>0.05</v>
-      </c>
       <c r="W365" s="32">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="X365" s="4"/>
       <c r="Y365" s="16"/>
@@ -24268,34 +24290,34 @@
       </c>
       <c r="I366" s="149"/>
       <c r="J366" s="149"/>
-      <c r="K366" s="2"/>
-      <c r="L366" s="107"/>
-      <c r="M366" s="2"/>
+      <c r="K366" s="149"/>
+      <c r="L366" s="149"/>
+      <c r="M366" s="149"/>
       <c r="N366" s="2"/>
       <c r="O366" s="32">
-        <v>-0.15</v>
+        <v>-0.4</v>
       </c>
       <c r="P366" s="32">
+        <v>-0.3</v>
+      </c>
+      <c r="Q366" s="32">
         <v>-0.1</v>
       </c>
-      <c r="Q366" s="32">
-        <v>-0.05</v>
-      </c>
       <c r="R366" s="32">
-        <v>-0.1</v>
+        <v>-0.3</v>
       </c>
       <c r="S366" s="2"/>
       <c r="T366" s="32">
-        <v>-0.15</v>
+        <v>-0.4</v>
       </c>
       <c r="U366" s="32">
+        <v>-0.3</v>
+      </c>
+      <c r="V366" s="32">
         <v>-0.1</v>
       </c>
-      <c r="V366" s="32">
-        <v>-0.05</v>
-      </c>
       <c r="W366" s="32">
-        <v>-0.1</v>
+        <v>-0.3</v>
       </c>
       <c r="X366" s="4"/>
       <c r="Y366" s="16"/>
@@ -24436,7 +24458,7 @@
       <c r="AA370" s="1"/>
       <c r="AB370" s="1"/>
     </row>
-    <row r="371" spans="1:28" s="142" customFormat="1" ht="5.0999999999999996" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:28" s="142" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A371" s="1"/>
       <c r="B371" s="19"/>
       <c r="C371" s="80">
@@ -24469,7 +24491,7 @@
       <c r="AA371" s="1"/>
       <c r="AB371" s="1"/>
     </row>
-    <row r="372" spans="1:28" s="142" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A372" s="1"/>
       <c r="B372" s="1"/>
       <c r="C372" s="76">
@@ -24695,109 +24717,119 @@
     <mergeCell ref="Q358:W358"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
-  <conditionalFormatting sqref="I364:J366 I362:I363">
-    <cfRule type="expression" dxfId="20" priority="75">
+  <conditionalFormatting sqref="I364:J366 I362:I363 J365:M366">
+    <cfRule type="expression" dxfId="22" priority="77">
       <formula>($E362&gt;=I$320)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O364:O366">
-    <cfRule type="expression" dxfId="19" priority="76">
+  <conditionalFormatting sqref="O364">
+    <cfRule type="expression" dxfId="21" priority="78">
       <formula>($E364&gt;=L$320)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T364:T366">
-    <cfRule type="expression" dxfId="18" priority="83">
+    <cfRule type="expression" dxfId="20" priority="85">
       <formula>($E364&gt;=P$320)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P366">
-    <cfRule type="expression" dxfId="17" priority="149">
+    <cfRule type="expression" dxfId="19" priority="151">
       <formula>(#REF!&gt;=L$320)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q366 U366">
-    <cfRule type="expression" dxfId="16" priority="150">
+    <cfRule type="expression" dxfId="18" priority="152">
       <formula>(#REF!&gt;=L$320)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R366">
-    <cfRule type="expression" dxfId="15" priority="152">
+    <cfRule type="expression" dxfId="17" priority="154">
       <formula>(#REF!&gt;=L$320)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W366">
-    <cfRule type="expression" dxfId="14" priority="153">
+    <cfRule type="expression" dxfId="16" priority="155">
       <formula>(#REF!&gt;=P$320)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V366">
-    <cfRule type="expression" dxfId="13" priority="154">
+    <cfRule type="expression" dxfId="15" priority="156">
       <formula>(#REF!&gt;=P$320)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P365">
-    <cfRule type="expression" dxfId="12" priority="155">
+    <cfRule type="expression" dxfId="14" priority="157">
       <formula>(#REF!&gt;=L$320)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q365 U365">
-    <cfRule type="expression" dxfId="11" priority="156">
+    <cfRule type="expression" dxfId="13" priority="158">
       <formula>(#REF!&gt;=L$320)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R365">
-    <cfRule type="expression" dxfId="10" priority="158">
+    <cfRule type="expression" dxfId="12" priority="160">
       <formula>(#REF!&gt;=L$320)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W365">
-    <cfRule type="expression" dxfId="9" priority="159">
+    <cfRule type="expression" dxfId="11" priority="161">
       <formula>(#REF!&gt;=P$320)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V365">
-    <cfRule type="expression" dxfId="8" priority="160">
+    <cfRule type="expression" dxfId="10" priority="162">
       <formula>(#REF!&gt;=P$320)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K364">
-    <cfRule type="expression" dxfId="7" priority="161">
+    <cfRule type="expression" dxfId="9" priority="163">
       <formula>(#REF!&gt;=J$320)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M364">
-    <cfRule type="expression" dxfId="6" priority="162">
+    <cfRule type="expression" dxfId="8" priority="164">
       <formula>(#REF!&gt;=J$320)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L364">
-    <cfRule type="expression" dxfId="5" priority="163">
+    <cfRule type="expression" dxfId="7" priority="165">
       <formula>(#REF!&gt;=J$320)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P364">
-    <cfRule type="expression" dxfId="4" priority="164">
+    <cfRule type="expression" dxfId="6" priority="166">
       <formula>(#REF!&gt;=L$320)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q364 U364">
-    <cfRule type="expression" dxfId="3" priority="165">
+    <cfRule type="expression" dxfId="5" priority="167">
       <formula>(#REF!&gt;=L$320)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R364">
-    <cfRule type="expression" dxfId="2" priority="167">
+    <cfRule type="expression" dxfId="4" priority="169">
       <formula>(#REF!&gt;=L$320)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W364">
-    <cfRule type="expression" dxfId="1" priority="168">
+    <cfRule type="expression" dxfId="3" priority="170">
       <formula>(#REF!&gt;=P$320)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V364">
-    <cfRule type="expression" dxfId="0" priority="169">
+    <cfRule type="expression" dxfId="2" priority="171">
       <formula>(#REF!&gt;=P$320)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O366">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>(#REF!&gt;=K$320)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O365">
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>(#REF!&gt;=K$320)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
prog reports and fix sire dse
</commit_message>
<xml_diff>
--- a/Structural.xlsx
+++ b/Structural.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F9AA18-5F35-4369-8658-30224DABEB8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C28B145-09C2-457C-8B3F-FFAC4BE3576D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -7000,7 +7000,7 @@
   <dimension ref="A1:AE362"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B317" workbookViewId="0">
-      <selection activeCell="P322" sqref="P322"/>
+      <selection activeCell="P323" sqref="P323"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.35"/>
@@ -22011,7 +22011,7 @@
       </c>
       <c r="P320" s="125">
         <f>i_w_start_len3*i_n3_len^P323</f>
-        <v>81</v>
+        <v>24</v>
       </c>
       <c r="Q320" s="2"/>
       <c r="R320" s="2"/>
@@ -22091,7 +22091,7 @@
       <c r="N322" s="2"/>
       <c r="O322" s="2"/>
       <c r="P322" s="31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q322" s="119"/>
       <c r="R322" s="119"/>

</xml_diff>

<commit_message>
Update spreadsheets. 3 FVPs for dams & offs. 1N for dams, 3N for Offs. Updated feed supply
</commit_message>
<xml_diff>
--- a/Structural.xlsx
+++ b/Structural.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C28B145-09C2-457C-8B3F-FFAC4BE3576D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F05337F-C246-4A1A-930A-D14752A65EB2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -142,14 +142,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -2001,7 +1993,8 @@
     <t xml:space="preserve">         Therefore think about the final sale date relative to 1 Jan, rather than the age of the animal</t>
   </si>
   <si>
-    <t>22Mar21: Alter the initial weight &amp; wool spread for the weaners
+    <t>29Mar21: Changed to FVP3, 1N for dams, 3N for Offs
+22Mar21: Alter the initial weight &amp; wool spread for the weaners
 1: 1Apr19-Blank worksheet</t>
   </si>
 </sst>
@@ -3975,25 +3968,25 @@
       <selection activeCell="C43" sqref="C43:C46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" style="147" customWidth="1"/>
-    <col min="2" max="2" width="2.7265625" style="147" customWidth="1"/>
-    <col min="3" max="3" width="4.7265625" style="147" customWidth="1" outlineLevel="2"/>
-    <col min="4" max="4" width="1.7265625" style="147" customWidth="1"/>
-    <col min="5" max="6" width="9.7265625" style="147" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="1.7265625" style="147" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="37.26953125" style="147" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7265625" style="147" customWidth="1"/>
-    <col min="10" max="23" width="10.81640625" style="147" customWidth="1"/>
-    <col min="24" max="24" width="1.7265625" style="147" customWidth="1"/>
-    <col min="25" max="26" width="4.7265625" style="147" customWidth="1"/>
-    <col min="27" max="27" width="8.7265625" style="147"/>
-    <col min="28" max="28" width="46.1796875" style="147" customWidth="1"/>
-    <col min="29" max="16384" width="8.7265625" style="147"/>
+    <col min="1" max="1" width="4.7109375" style="147" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" style="147" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" style="147" customWidth="1" outlineLevel="2"/>
+    <col min="4" max="4" width="1.7109375" style="147" customWidth="1"/>
+    <col min="5" max="6" width="9.7109375" style="147" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="1.7109375" style="147" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="37.28515625" style="147" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="147" customWidth="1"/>
+    <col min="10" max="23" width="10.85546875" style="147" customWidth="1"/>
+    <col min="24" max="24" width="1.7109375" style="147" customWidth="1"/>
+    <col min="25" max="26" width="4.7109375" style="147" customWidth="1"/>
+    <col min="27" max="27" width="8.7109375" style="147"/>
+    <col min="28" max="28" width="46.140625" style="147" customWidth="1"/>
+    <col min="29" max="16384" width="8.7109375" style="147"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="66"/>
@@ -4023,7 +4016,7 @@
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
     </row>
-    <row r="2" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="67">
@@ -4056,7 +4049,7 @@
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
     </row>
-    <row r="3" spans="1:28" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:28" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="20"/>
       <c r="C3" s="68">
@@ -4089,7 +4082,7 @@
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
     </row>
-    <row r="4" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="34" t="s">
         <v>21</v>
@@ -4124,7 +4117,7 @@
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
     </row>
-    <row r="5" spans="1:28" hidden="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:28" hidden="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="33"/>
       <c r="C5" s="67">
@@ -4195,7 +4188,7 @@
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
     </row>
-    <row r="6" spans="1:28" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="33"/>
       <c r="C6" s="67">
@@ -4233,7 +4226,7 @@
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
     </row>
-    <row r="7" spans="1:28" ht="20.149999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="33"/>
       <c r="C7" s="67">
@@ -4272,7 +4265,7 @@
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
     </row>
-    <row r="8" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="33"/>
       <c r="C8" s="67">
@@ -4305,7 +4298,7 @@
       <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
     </row>
-    <row r="9" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="33"/>
       <c r="C9" s="67">
@@ -4338,7 +4331,7 @@
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
     </row>
-    <row r="10" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="33"/>
       <c r="C10" s="67">
@@ -4371,7 +4364,7 @@
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
     </row>
-    <row r="11" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="33"/>
       <c r="C11" s="67">
@@ -4404,7 +4397,7 @@
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
     </row>
-    <row r="12" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="33"/>
       <c r="C12" s="67">
@@ -4441,7 +4434,7 @@
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
     </row>
-    <row r="13" spans="1:28" ht="11.5" hidden="1" customHeight="1" outlineLevel="3" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:28" ht="11.45" hidden="1" customHeight="1" outlineLevel="3" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="33" t="s">
         <v>20</v>
@@ -4476,7 +4469,7 @@
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
     </row>
-    <row r="14" spans="1:28" hidden="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:28" hidden="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="33"/>
       <c r="C14" s="67">
@@ -4509,7 +4502,7 @@
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
     </row>
-    <row r="15" spans="1:28" hidden="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:28" hidden="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="33"/>
       <c r="C15" s="67">
@@ -4542,7 +4535,7 @@
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
     </row>
-    <row r="16" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="33" t="s">
         <v>19</v>
@@ -4579,7 +4572,7 @@
       <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>
     </row>
-    <row r="17" spans="1:28" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:28" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="33"/>
       <c r="C17" s="67">
@@ -4614,7 +4607,7 @@
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
     </row>
-    <row r="18" spans="1:28" ht="45" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:28" ht="45" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="33"/>
       <c r="C18" s="67">
@@ -4653,7 +4646,7 @@
       <c r="AA18" s="1"/>
       <c r="AB18" s="1"/>
     </row>
-    <row r="19" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="33"/>
       <c r="C19" s="67">
@@ -4686,7 +4679,7 @@
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
     </row>
-    <row r="20" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="33"/>
       <c r="C20" s="67">
@@ -4719,7 +4712,7 @@
       <c r="AA20" s="1"/>
       <c r="AB20" s="1"/>
     </row>
-    <row r="21" spans="1:28" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:28" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="33"/>
       <c r="C21" s="67">
@@ -4758,7 +4751,7 @@
       <c r="AA21" s="1"/>
       <c r="AB21" s="1"/>
     </row>
-    <row r="22" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="33"/>
       <c r="C22" s="67">
@@ -4791,7 +4784,7 @@
       <c r="AA22" s="1"/>
       <c r="AB22" s="1"/>
     </row>
-    <row r="23" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="33"/>
       <c r="C23" s="67">
@@ -4824,7 +4817,7 @@
       <c r="AA23" s="1"/>
       <c r="AB23" s="1"/>
     </row>
-    <row r="24" spans="1:28" ht="5.15" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="33"/>
       <c r="C24" s="67">
@@ -4859,7 +4852,7 @@
       <c r="AA24" s="1"/>
       <c r="AB24" s="1"/>
     </row>
-    <row r="25" spans="1:28" ht="5.15" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="33"/>
       <c r="C25" s="67">
@@ -4894,7 +4887,7 @@
       <c r="AA25" s="1"/>
       <c r="AB25" s="1"/>
     </row>
-    <row r="26" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="33"/>
       <c r="C26" s="67">
@@ -4941,7 +4934,7 @@
       <c r="AA26" s="1"/>
       <c r="AB26" s="1"/>
     </row>
-    <row r="27" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="33"/>
       <c r="C27" s="67">
@@ -4978,7 +4971,7 @@
       <c r="AA27" s="1"/>
       <c r="AB27" s="1"/>
     </row>
-    <row r="28" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="33"/>
       <c r="C28" s="67">
@@ -5015,7 +5008,7 @@
       <c r="AA28" s="1"/>
       <c r="AB28" s="1"/>
     </row>
-    <row r="29" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="33"/>
       <c r="C29" s="67">
@@ -5052,7 +5045,7 @@
       <c r="AA29" s="1"/>
       <c r="AB29" s="1"/>
     </row>
-    <row r="30" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="33"/>
       <c r="C30" s="67">
@@ -5089,7 +5082,7 @@
       <c r="AA30" s="1"/>
       <c r="AB30" s="1"/>
     </row>
-    <row r="31" spans="1:28" ht="5.15" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="33"/>
       <c r="C31" s="67">
@@ -5124,7 +5117,7 @@
       <c r="AA31" s="1"/>
       <c r="AB31" s="1"/>
     </row>
-    <row r="32" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="33"/>
       <c r="C32" s="67">
@@ -5157,7 +5150,7 @@
       <c r="AA32" s="1"/>
       <c r="AB32" s="1"/>
     </row>
-    <row r="33" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="35"/>
       <c r="C33" s="70">
@@ -5192,7 +5185,7 @@
       <c r="AA33" s="1"/>
       <c r="AB33" s="1"/>
     </row>
-    <row r="34" spans="1:28" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:28" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="19"/>
       <c r="C34" s="71">
@@ -5225,7 +5218,7 @@
       <c r="AA34" s="1"/>
       <c r="AB34" s="1"/>
     </row>
-    <row r="35" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="67">
@@ -5258,7 +5251,7 @@
       <c r="AA35" s="1"/>
       <c r="AB35" s="1"/>
     </row>
-    <row r="36" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="73">
@@ -5291,7 +5284,7 @@
       <c r="AA36" s="1"/>
       <c r="AB36" s="1"/>
     </row>
-    <row r="37" spans="1:28" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:28" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="20"/>
       <c r="C37" s="74">
@@ -5324,7 +5317,7 @@
       <c r="AA37" s="1"/>
       <c r="AB37" s="1"/>
     </row>
-    <row r="38" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="34" t="s">
         <v>21</v>
@@ -5359,7 +5352,7 @@
       <c r="AA38" s="1"/>
       <c r="AB38" s="1"/>
     </row>
-    <row r="39" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="33"/>
       <c r="C39" s="73">
@@ -5392,7 +5385,7 @@
       <c r="AA39" s="1"/>
       <c r="AB39" s="1"/>
     </row>
-    <row r="40" spans="1:28" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="33"/>
       <c r="C40" s="73">
@@ -5429,7 +5422,7 @@
       <c r="AA40" s="1"/>
       <c r="AB40" s="1"/>
     </row>
-    <row r="41" spans="1:28" ht="20.149999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:28" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="33"/>
       <c r="C41" s="73">
@@ -5468,7 +5461,7 @@
       <c r="AA41" s="1"/>
       <c r="AB41" s="1"/>
     </row>
-    <row r="42" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="33"/>
       <c r="C42" s="73">
@@ -5501,7 +5494,7 @@
       <c r="AA42" s="1"/>
       <c r="AB42" s="1"/>
     </row>
-    <row r="43" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="33"/>
       <c r="C43" s="73">
@@ -5534,7 +5527,7 @@
       <c r="AA43" s="1"/>
       <c r="AB43" s="1"/>
     </row>
-    <row r="44" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="33"/>
       <c r="C44" s="73">
@@ -5567,7 +5560,7 @@
       <c r="AA44" s="1"/>
       <c r="AB44" s="1"/>
     </row>
-    <row r="45" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="33"/>
       <c r="C45" s="73">
@@ -5600,7 +5593,7 @@
       <c r="AA45" s="1"/>
       <c r="AB45" s="1"/>
     </row>
-    <row r="46" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="33"/>
       <c r="C46" s="73">
@@ -5633,7 +5626,7 @@
       <c r="AA46" s="1"/>
       <c r="AB46" s="1"/>
     </row>
-    <row r="47" spans="1:28" ht="11.5" customHeight="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:28" ht="11.45" customHeight="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="33" t="s">
         <v>20</v>
@@ -5668,7 +5661,7 @@
       <c r="AA47" s="1"/>
       <c r="AB47" s="1"/>
     </row>
-    <row r="48" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="33"/>
       <c r="C48" s="73">
@@ -5701,7 +5694,7 @@
       <c r="AA48" s="1"/>
       <c r="AB48" s="1"/>
     </row>
-    <row r="49" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="33" t="s">
         <v>19</v>
@@ -5738,7 +5731,7 @@
       <c r="AA49" s="1"/>
       <c r="AB49" s="1"/>
     </row>
-    <row r="50" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="33"/>
       <c r="C50" s="73">
@@ -5773,7 +5766,7 @@
       <c r="AA50" s="1"/>
       <c r="AB50" s="1"/>
     </row>
-    <row r="51" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="33"/>
       <c r="C51" s="73">
@@ -5814,7 +5807,7 @@
       <c r="AA51" s="1"/>
       <c r="AB51" s="1"/>
     </row>
-    <row r="52" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="33"/>
       <c r="C52" s="73">
@@ -5847,7 +5840,7 @@
       <c r="AA52" s="1"/>
       <c r="AB52" s="1"/>
     </row>
-    <row r="53" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="33"/>
       <c r="C53" s="73">
@@ -5886,7 +5879,7 @@
       <c r="AA53" s="1"/>
       <c r="AB53" s="1"/>
     </row>
-    <row r="54" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="33"/>
       <c r="C54" s="73">
@@ -5919,7 +5912,7 @@
       <c r="AA54" s="1"/>
       <c r="AB54" s="1"/>
     </row>
-    <row r="55" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="33"/>
       <c r="C55" s="73">
@@ -5960,7 +5953,7 @@
       <c r="AA55" s="1"/>
       <c r="AB55" s="1"/>
     </row>
-    <row r="56" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="33"/>
       <c r="C56" s="73">
@@ -6001,7 +5994,7 @@
       <c r="AA56" s="1"/>
       <c r="AB56" s="1"/>
     </row>
-    <row r="57" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="33"/>
       <c r="C57" s="73">
@@ -6040,7 +6033,7 @@
       <c r="AA57" s="1"/>
       <c r="AB57" s="1"/>
     </row>
-    <row r="58" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="33"/>
       <c r="C58" s="73">
@@ -6083,7 +6076,7 @@
       <c r="AA58" s="1"/>
       <c r="AB58" s="1"/>
     </row>
-    <row r="59" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="33"/>
       <c r="C59" s="73">
@@ -6124,7 +6117,7 @@
       <c r="AA59" s="1"/>
       <c r="AB59" s="1"/>
     </row>
-    <row r="60" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="33"/>
       <c r="C60" s="73">
@@ -6157,7 +6150,7 @@
       <c r="AA60" s="1"/>
       <c r="AB60" s="1"/>
     </row>
-    <row r="61" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="33"/>
       <c r="C61" s="73">
@@ -6200,7 +6193,7 @@
       <c r="AA61" s="1"/>
       <c r="AB61" s="1"/>
     </row>
-    <row r="62" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="33"/>
       <c r="C62" s="73">
@@ -6233,7 +6226,7 @@
       <c r="AA62" s="1"/>
       <c r="AB62" s="1"/>
     </row>
-    <row r="63" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="33"/>
       <c r="C63" s="73">
@@ -6270,7 +6263,7 @@
       <c r="AA63" s="1"/>
       <c r="AB63" s="1"/>
     </row>
-    <row r="64" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="33"/>
       <c r="C64" s="73">
@@ -6303,7 +6296,7 @@
       <c r="AA64" s="1"/>
       <c r="AB64" s="1"/>
     </row>
-    <row r="65" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="33"/>
       <c r="C65" s="73">
@@ -6340,7 +6333,7 @@
       <c r="AA65" s="1"/>
       <c r="AB65" s="1"/>
     </row>
-    <row r="66" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="33"/>
       <c r="C66" s="73">
@@ -6373,7 +6366,7 @@
       <c r="AA66" s="1"/>
       <c r="AB66" s="1"/>
     </row>
-    <row r="67" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="33"/>
       <c r="C67" s="73">
@@ -6429,7 +6422,7 @@
       <c r="AS67" s="1"/>
       <c r="AT67" s="1"/>
     </row>
-    <row r="68" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="33"/>
       <c r="C68" s="73">
@@ -6493,7 +6486,7 @@
       <c r="AS68" s="1"/>
       <c r="AT68" s="1"/>
     </row>
-    <row r="69" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="33"/>
       <c r="C69" s="73">
@@ -6543,7 +6536,7 @@
       <c r="AS69" s="1"/>
       <c r="AT69" s="1"/>
     </row>
-    <row r="70" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="33"/>
       <c r="C70" s="73">
@@ -6593,7 +6586,7 @@
       <c r="AS70" s="1"/>
       <c r="AT70" s="1"/>
     </row>
-    <row r="71" spans="1:46" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:46" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="33"/>
       <c r="C71" s="73">
@@ -6628,7 +6621,7 @@
       <c r="AA71" s="1"/>
       <c r="AB71" s="1"/>
     </row>
-    <row r="72" spans="1:46" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:46" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="33"/>
       <c r="C72" s="73">
@@ -6661,7 +6654,7 @@
       <c r="AA72" s="1"/>
       <c r="AB72" s="1"/>
     </row>
-    <row r="73" spans="1:46" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:46" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="35"/>
       <c r="C73" s="76">
@@ -6696,7 +6689,7 @@
       <c r="AA73" s="1"/>
       <c r="AB73" s="1"/>
     </row>
-    <row r="74" spans="1:46" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:46" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="19"/>
       <c r="C74" s="77">
@@ -6729,7 +6722,7 @@
       <c r="AA74" s="1"/>
       <c r="AB74" s="1"/>
     </row>
-    <row r="75" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="73">
@@ -6762,7 +6755,7 @@
       <c r="AA75" s="1"/>
       <c r="AB75" s="1"/>
     </row>
-    <row r="76" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="73">
@@ -6795,7 +6788,7 @@
       <c r="AA76" s="1"/>
       <c r="AB76" s="1"/>
     </row>
-    <row r="77" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="66"/>
@@ -6825,7 +6818,7 @@
       <c r="AA77" s="1"/>
       <c r="AB77" s="1"/>
     </row>
-    <row r="78" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="66"/>
@@ -6855,7 +6848,7 @@
       <c r="AA78" s="1"/>
       <c r="AB78" s="1"/>
     </row>
-    <row r="79" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="66"/>
@@ -6885,7 +6878,7 @@
       <c r="AA79" s="1"/>
       <c r="AB79" s="1"/>
     </row>
-    <row r="80" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="66"/>
@@ -6915,7 +6908,7 @@
       <c r="AA80" s="1"/>
       <c r="AB80" s="1"/>
     </row>
-    <row r="81" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="66"/>
@@ -6945,7 +6938,7 @@
       <c r="AA81" s="1"/>
       <c r="AB81" s="1"/>
     </row>
-    <row r="82" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="66"/>
@@ -6975,7 +6968,7 @@
       <c r="AA82" s="1"/>
       <c r="AB82" s="1"/>
     </row>
-    <row r="83" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C83" s="72" t="s">
         <v>4</v>
       </c>
@@ -6999,27 +6992,27 @@
   </sheetPr>
   <dimension ref="A1:AE362"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B317" workbookViewId="0">
-      <selection activeCell="P323" sqref="P323"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21:T21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" customWidth="1"/>
-    <col min="2" max="2" width="2.7265625" customWidth="1"/>
-    <col min="3" max="3" width="4.7265625" customWidth="1" outlineLevel="2"/>
-    <col min="4" max="4" width="1.7265625" customWidth="1"/>
-    <col min="5" max="6" width="9.7265625" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="1.7265625" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="37.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7265625" customWidth="1"/>
-    <col min="10" max="23" width="10.81640625" customWidth="1"/>
-    <col min="24" max="24" width="1.7265625" customWidth="1"/>
-    <col min="25" max="26" width="4.7265625" customWidth="1"/>
-    <col min="28" max="28" width="46.1796875" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="4" max="4" width="1.7109375" customWidth="1"/>
+    <col min="5" max="6" width="9.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="1.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" customWidth="1"/>
+    <col min="10" max="23" width="10.85546875" customWidth="1"/>
+    <col min="24" max="24" width="1.7109375" customWidth="1"/>
+    <col min="25" max="26" width="4.7109375" customWidth="1"/>
+    <col min="28" max="28" width="46.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="66"/>
@@ -7049,7 +7042,7 @@
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
     </row>
-    <row r="2" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="67">
@@ -7082,7 +7075,7 @@
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
     </row>
-    <row r="3" spans="1:28" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:28" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="20"/>
       <c r="C3" s="68">
@@ -7115,7 +7108,7 @@
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
     </row>
-    <row r="4" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="34" t="s">
         <v>21</v>
@@ -7150,7 +7143,7 @@
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
     </row>
-    <row r="5" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="33"/>
       <c r="C5" s="67">
@@ -7221,7 +7214,7 @@
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
     </row>
-    <row r="6" spans="1:28" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="33"/>
       <c r="C6" s="67">
@@ -7259,7 +7252,7 @@
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
     </row>
-    <row r="7" spans="1:28" ht="20.149999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="33"/>
       <c r="C7" s="67">
@@ -7298,7 +7291,7 @@
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
     </row>
-    <row r="8" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="33"/>
       <c r="C8" s="67">
@@ -7331,7 +7324,7 @@
       <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
     </row>
-    <row r="9" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="33"/>
       <c r="C9" s="67">
@@ -7364,7 +7357,7 @@
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
     </row>
-    <row r="10" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="33"/>
       <c r="C10" s="67">
@@ -7397,7 +7390,7 @@
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
     </row>
-    <row r="11" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="33"/>
       <c r="C11" s="67">
@@ -7430,7 +7423,7 @@
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
     </row>
-    <row r="12" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="33"/>
       <c r="C12" s="67">
@@ -7467,7 +7460,7 @@
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
     </row>
-    <row r="13" spans="1:28" ht="11.5" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:28" ht="11.45" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="33" t="s">
         <v>20</v>
@@ -7502,7 +7495,7 @@
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
     </row>
-    <row r="14" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="33"/>
       <c r="C14" s="67">
@@ -7535,7 +7528,7 @@
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
     </row>
-    <row r="15" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="33"/>
       <c r="C15" s="67">
@@ -7568,7 +7561,7 @@
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
     </row>
-    <row r="16" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="33" t="s">
         <v>19</v>
@@ -7605,7 +7598,7 @@
       <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>
     </row>
-    <row r="17" spans="1:28" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:28" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="33"/>
       <c r="C17" s="67">
@@ -7640,7 +7633,7 @@
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
     </row>
-    <row r="18" spans="1:28" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:28" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="33"/>
       <c r="C18" s="67">
@@ -7679,7 +7672,7 @@
       <c r="AA18" s="1"/>
       <c r="AB18" s="1"/>
     </row>
-    <row r="19" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="33"/>
       <c r="C19" s="67">
@@ -7712,7 +7705,7 @@
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
     </row>
-    <row r="20" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="33"/>
       <c r="C20" s="67">
@@ -7745,7 +7738,7 @@
       <c r="AA20" s="1"/>
       <c r="AB20" s="1"/>
     </row>
-    <row r="21" spans="1:28" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:28" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="33"/>
       <c r="C21" s="67">
@@ -7760,7 +7753,7 @@
         <v>17</v>
       </c>
       <c r="I21" s="161">
-        <v>44277</v>
+        <v>44284</v>
       </c>
       <c r="J21" s="165" t="s">
         <v>274</v>
@@ -7784,7 +7777,7 @@
       <c r="AA21" s="1"/>
       <c r="AB21" s="1"/>
     </row>
-    <row r="22" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="33"/>
       <c r="C22" s="67">
@@ -7817,7 +7810,7 @@
       <c r="AA22" s="1"/>
       <c r="AB22" s="1"/>
     </row>
-    <row r="23" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="33"/>
       <c r="C23" s="67">
@@ -7850,7 +7843,7 @@
       <c r="AA23" s="1"/>
       <c r="AB23" s="1"/>
     </row>
-    <row r="24" spans="1:28" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="33"/>
       <c r="C24" s="67">
@@ -7885,7 +7878,7 @@
       <c r="AA24" s="1"/>
       <c r="AB24" s="1"/>
     </row>
-    <row r="25" spans="1:28" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="33"/>
       <c r="C25" s="67">
@@ -7920,7 +7913,7 @@
       <c r="AA25" s="1"/>
       <c r="AB25" s="1"/>
     </row>
-    <row r="26" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="33"/>
       <c r="C26" s="67">
@@ -7967,7 +7960,7 @@
       <c r="AA26" s="1"/>
       <c r="AB26" s="1"/>
     </row>
-    <row r="27" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="33"/>
       <c r="C27" s="67">
@@ -8004,7 +7997,7 @@
       <c r="AA27" s="1"/>
       <c r="AB27" s="1"/>
     </row>
-    <row r="28" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="33"/>
       <c r="C28" s="67">
@@ -8041,7 +8034,7 @@
       <c r="AA28" s="1"/>
       <c r="AB28" s="1"/>
     </row>
-    <row r="29" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="33"/>
       <c r="C29" s="67">
@@ -8078,7 +8071,7 @@
       <c r="AA29" s="1"/>
       <c r="AB29" s="1"/>
     </row>
-    <row r="30" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="33"/>
       <c r="C30" s="67">
@@ -8115,7 +8108,7 @@
       <c r="AA30" s="1"/>
       <c r="AB30" s="1"/>
     </row>
-    <row r="31" spans="1:28" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="33"/>
       <c r="C31" s="67">
@@ -8150,7 +8143,7 @@
       <c r="AA31" s="1"/>
       <c r="AB31" s="1"/>
     </row>
-    <row r="32" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="33"/>
       <c r="C32" s="67">
@@ -8183,7 +8176,7 @@
       <c r="AA32" s="1"/>
       <c r="AB32" s="1"/>
     </row>
-    <row r="33" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="35"/>
       <c r="C33" s="70">
@@ -8218,7 +8211,7 @@
       <c r="AA33" s="1"/>
       <c r="AB33" s="1"/>
     </row>
-    <row r="34" spans="1:28" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:28" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="19"/>
       <c r="C34" s="71">
@@ -8251,7 +8244,7 @@
       <c r="AA34" s="1"/>
       <c r="AB34" s="1"/>
     </row>
-    <row r="35" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="67">
@@ -8284,7 +8277,7 @@
       <c r="AA35" s="1"/>
       <c r="AB35" s="1"/>
     </row>
-    <row r="36" spans="1:28" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:28" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="73">
@@ -8317,7 +8310,7 @@
       <c r="AA36" s="1"/>
       <c r="AB36" s="1"/>
     </row>
-    <row r="37" spans="1:28" s="135" customFormat="1" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:28" s="135" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="20"/>
       <c r="C37" s="74">
@@ -8350,7 +8343,7 @@
       <c r="AA37" s="1"/>
       <c r="AB37" s="1"/>
     </row>
-    <row r="38" spans="1:28" s="135" customFormat="1" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:28" s="135" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="34" t="s">
         <v>21</v>
@@ -8385,7 +8378,7 @@
       <c r="AA38" s="1"/>
       <c r="AB38" s="1"/>
     </row>
-    <row r="39" spans="1:28" s="135" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:28" s="135" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="33"/>
       <c r="C39" s="73">
@@ -8418,7 +8411,7 @@
       <c r="AA39" s="1"/>
       <c r="AB39" s="1"/>
     </row>
-    <row r="40" spans="1:28" s="135" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:28" s="135" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="33"/>
       <c r="C40" s="73">
@@ -8455,7 +8448,7 @@
       <c r="AA40" s="1"/>
       <c r="AB40" s="1"/>
     </row>
-    <row r="41" spans="1:28" s="135" customFormat="1" ht="20.149999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:28" s="135" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="33"/>
       <c r="C41" s="73">
@@ -8492,7 +8485,7 @@
       <c r="AA41" s="1"/>
       <c r="AB41" s="1"/>
     </row>
-    <row r="42" spans="1:28" s="135" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:28" s="135" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="33"/>
       <c r="C42" s="73">
@@ -8525,7 +8518,7 @@
       <c r="AA42" s="1"/>
       <c r="AB42" s="1"/>
     </row>
-    <row r="43" spans="1:28" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:28" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="33"/>
       <c r="C43" s="73">
@@ -8558,7 +8551,7 @@
       <c r="AA43" s="1"/>
       <c r="AB43" s="1"/>
     </row>
-    <row r="44" spans="1:28" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:28" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="33"/>
       <c r="C44" s="73">
@@ -8591,7 +8584,7 @@
       <c r="AA44" s="1"/>
       <c r="AB44" s="1"/>
     </row>
-    <row r="45" spans="1:28" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:28" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="33"/>
       <c r="C45" s="73">
@@ -8624,7 +8617,7 @@
       <c r="AA45" s="1"/>
       <c r="AB45" s="1"/>
     </row>
-    <row r="46" spans="1:28" s="135" customFormat="1" ht="28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:28" s="135" customFormat="1" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="33"/>
       <c r="C46" s="73">
@@ -8667,7 +8660,7 @@
       <c r="AA46" s="1"/>
       <c r="AB46" s="1"/>
     </row>
-    <row r="47" spans="1:28" s="135" customFormat="1" ht="11.5" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:28" s="135" customFormat="1" ht="11.45" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="33" t="s">
         <v>20</v>
@@ -8702,7 +8695,7 @@
       <c r="AA47" s="1"/>
       <c r="AB47" s="1"/>
     </row>
-    <row r="48" spans="1:28" s="135" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:28" s="135" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="33"/>
       <c r="C48" s="73">
@@ -8735,7 +8728,7 @@
       <c r="AA48" s="1"/>
       <c r="AB48" s="1"/>
     </row>
-    <row r="49" spans="1:28" s="135" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:28" s="135" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="33" t="s">
         <v>19</v>
@@ -8772,7 +8765,7 @@
       <c r="AA49" s="1"/>
       <c r="AB49" s="1"/>
     </row>
-    <row r="50" spans="1:28" s="135" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:28" s="135" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="33"/>
       <c r="C50" s="73">
@@ -8807,7 +8800,7 @@
       <c r="AA50" s="1"/>
       <c r="AB50" s="1"/>
     </row>
-    <row r="51" spans="1:28" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:28" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="33"/>
       <c r="C51" s="73">
@@ -8842,7 +8835,7 @@
       <c r="AA51" s="1"/>
       <c r="AB51" s="1"/>
     </row>
-    <row r="52" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="33"/>
       <c r="C52" s="73"/>
@@ -8876,7 +8869,7 @@
       <c r="AA52" s="1"/>
       <c r="AB52" s="1"/>
     </row>
-    <row r="53" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="33"/>
       <c r="C53" s="73"/>
@@ -8910,7 +8903,7 @@
       <c r="AA53" s="1"/>
       <c r="AB53" s="1"/>
     </row>
-    <row r="54" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="33"/>
       <c r="C54" s="73"/>
@@ -8944,7 +8937,7 @@
       <c r="AA54" s="1"/>
       <c r="AB54" s="1"/>
     </row>
-    <row r="55" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="33"/>
       <c r="C55" s="73"/>
@@ -8978,7 +8971,7 @@
       <c r="AA55" s="1"/>
       <c r="AB55" s="1"/>
     </row>
-    <row r="56" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="33"/>
       <c r="C56" s="73"/>
@@ -9012,7 +9005,7 @@
       <c r="AA56" s="1"/>
       <c r="AB56" s="1"/>
     </row>
-    <row r="57" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="33"/>
       <c r="C57" s="73"/>
@@ -9046,7 +9039,7 @@
       <c r="AA57" s="1"/>
       <c r="AB57" s="1"/>
     </row>
-    <row r="58" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="33"/>
       <c r="C58" s="73"/>
@@ -9080,7 +9073,7 @@
       <c r="AA58" s="1"/>
       <c r="AB58" s="1"/>
     </row>
-    <row r="59" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="33"/>
       <c r="C59" s="73"/>
@@ -9114,7 +9107,7 @@
       <c r="AA59" s="1"/>
       <c r="AB59" s="1"/>
     </row>
-    <row r="60" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="33"/>
       <c r="C60" s="73"/>
@@ -9148,7 +9141,7 @@
       <c r="AA60" s="1"/>
       <c r="AB60" s="1"/>
     </row>
-    <row r="61" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="33"/>
       <c r="C61" s="73"/>
@@ -9182,7 +9175,7 @@
       <c r="AA61" s="1"/>
       <c r="AB61" s="1"/>
     </row>
-    <row r="62" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="33"/>
       <c r="C62" s="73"/>
@@ -9216,7 +9209,7 @@
       <c r="AA62" s="1"/>
       <c r="AB62" s="1"/>
     </row>
-    <row r="63" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="33"/>
       <c r="C63" s="73"/>
@@ -9250,7 +9243,7 @@
       <c r="AA63" s="1"/>
       <c r="AB63" s="1"/>
     </row>
-    <row r="64" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="33"/>
       <c r="C64" s="73"/>
@@ -9284,7 +9277,7 @@
       <c r="AA64" s="1"/>
       <c r="AB64" s="1"/>
     </row>
-    <row r="65" spans="1:28" s="107" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:28" s="107" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="33"/>
       <c r="C65" s="73">
@@ -9323,7 +9316,7 @@
       <c r="AA65" s="1"/>
       <c r="AB65" s="1"/>
     </row>
-    <row r="66" spans="1:28" s="100" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:28" s="100" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="33"/>
       <c r="C66" s="73">
@@ -9360,7 +9353,7 @@
       <c r="AA66" s="1"/>
       <c r="AB66" s="1"/>
     </row>
-    <row r="67" spans="1:28" s="100" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:28" s="100" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="33"/>
       <c r="C67" s="73">
@@ -9397,7 +9390,7 @@
       <c r="AA67" s="1"/>
       <c r="AB67" s="1"/>
     </row>
-    <row r="68" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="33"/>
       <c r="C68" s="73">
@@ -9434,7 +9427,7 @@
       <c r="AA68" s="1"/>
       <c r="AB68" s="1"/>
     </row>
-    <row r="69" spans="1:28" s="138" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:28" s="138" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="33"/>
       <c r="C69" s="73">
@@ -9467,7 +9460,7 @@
       <c r="AA69" s="1"/>
       <c r="AB69" s="1"/>
     </row>
-    <row r="70" spans="1:28" s="103" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:28" s="103" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="33"/>
       <c r="C70" s="73">
@@ -9504,7 +9497,7 @@
       <c r="AA70" s="1"/>
       <c r="AB70" s="1"/>
     </row>
-    <row r="71" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="33"/>
       <c r="C71" s="73">
@@ -9545,7 +9538,7 @@
       <c r="AA71" s="1"/>
       <c r="AB71" s="1"/>
     </row>
-    <row r="72" spans="1:28" s="146" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:28" s="146" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="33"/>
       <c r="C72" s="73">
@@ -9586,7 +9579,7 @@
       <c r="AA72" s="1"/>
       <c r="AB72" s="1"/>
     </row>
-    <row r="73" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="33"/>
       <c r="C73" s="73"/>
@@ -9616,7 +9609,7 @@
       <c r="AA73" s="1"/>
       <c r="AB73" s="1"/>
     </row>
-    <row r="74" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="33"/>
       <c r="C74" s="73"/>
@@ -9652,7 +9645,7 @@
       <c r="AA74" s="1"/>
       <c r="AB74" s="1"/>
     </row>
-    <row r="75" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="33"/>
       <c r="C75" s="73"/>
@@ -9682,7 +9675,7 @@
       <c r="AA75" s="1"/>
       <c r="AB75" s="1"/>
     </row>
-    <row r="76" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="33"/>
       <c r="C76" s="73">
@@ -9717,7 +9710,7 @@
       <c r="AA76" s="1"/>
       <c r="AB76" s="1"/>
     </row>
-    <row r="77" spans="1:28" s="97" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:28" s="97" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="33"/>
       <c r="C77" s="73">
@@ -9758,7 +9751,7 @@
       <c r="AA77" s="1"/>
       <c r="AB77" s="1"/>
     </row>
-    <row r="78" spans="1:28" s="97" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:28" s="97" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="33"/>
       <c r="C78" s="73">
@@ -9799,7 +9792,7 @@
       <c r="AA78" s="1"/>
       <c r="AB78" s="1"/>
     </row>
-    <row r="79" spans="1:28" s="97" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:28" s="97" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="33"/>
       <c r="C79" s="73">
@@ -9832,7 +9825,7 @@
       <c r="AA79" s="1"/>
       <c r="AB79" s="1"/>
     </row>
-    <row r="80" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="33"/>
       <c r="C80" s="73">
@@ -9869,7 +9862,7 @@
       <c r="AA80" s="1"/>
       <c r="AB80" s="1"/>
     </row>
-    <row r="81" spans="1:28" s="144" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:28" s="144" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="33"/>
       <c r="C81" s="73">
@@ -9902,7 +9895,7 @@
       <c r="AA81" s="1"/>
       <c r="AB81" s="1"/>
     </row>
-    <row r="82" spans="1:28" s="97" customFormat="1" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:28" s="97" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="33"/>
       <c r="C82" s="73">
@@ -9937,7 +9930,7 @@
       <c r="AA82" s="1"/>
       <c r="AB82" s="1"/>
     </row>
-    <row r="83" spans="1:28" s="97" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:28" s="97" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="33"/>
       <c r="C83" s="73">
@@ -9970,7 +9963,7 @@
       <c r="AA83" s="1"/>
       <c r="AB83" s="1"/>
     </row>
-    <row r="84" spans="1:28" s="97" customFormat="1" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:28" s="97" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="35"/>
       <c r="C84" s="76">
@@ -10005,7 +9998,7 @@
       <c r="AA84" s="1"/>
       <c r="AB84" s="1"/>
     </row>
-    <row r="85" spans="1:28" s="97" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:28" s="97" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="19"/>
       <c r="C85" s="77">
@@ -10038,7 +10031,7 @@
       <c r="AA85" s="1"/>
       <c r="AB85" s="1"/>
     </row>
-    <row r="86" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="73">
@@ -10071,7 +10064,7 @@
       <c r="AA86" s="1"/>
       <c r="AB86" s="1"/>
     </row>
-    <row r="87" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="73">
@@ -10104,7 +10097,7 @@
       <c r="AA87" s="1"/>
       <c r="AB87" s="1"/>
     </row>
-    <row r="88" spans="1:28" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:28" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="1"/>
       <c r="B88" s="20"/>
       <c r="C88" s="74">
@@ -10137,7 +10130,7 @@
       <c r="AA88" s="1"/>
       <c r="AB88" s="1"/>
     </row>
-    <row r="89" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="34" t="s">
         <v>21</v>
@@ -10172,7 +10165,7 @@
       <c r="AA89" s="1"/>
       <c r="AB89" s="1"/>
     </row>
-    <row r="90" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="33"/>
       <c r="C90" s="73">
@@ -10205,7 +10198,7 @@
       <c r="AA90" s="1"/>
       <c r="AB90" s="1"/>
     </row>
-    <row r="91" spans="1:28" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="33"/>
       <c r="C91" s="73">
@@ -10242,7 +10235,7 @@
       <c r="AA91" s="1"/>
       <c r="AB91" s="1"/>
     </row>
-    <row r="92" spans="1:28" ht="20.149999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:28" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="33"/>
       <c r="C92" s="73">
@@ -10279,7 +10272,7 @@
       <c r="AA92" s="1"/>
       <c r="AB92" s="1"/>
     </row>
-    <row r="93" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="33"/>
       <c r="C93" s="73">
@@ -10312,7 +10305,7 @@
       <c r="AA93" s="1"/>
       <c r="AB93" s="1"/>
     </row>
-    <row r="94" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="33"/>
       <c r="C94" s="73">
@@ -10345,7 +10338,7 @@
       <c r="AA94" s="1"/>
       <c r="AB94" s="1"/>
     </row>
-    <row r="95" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="33"/>
       <c r="C95" s="73">
@@ -10378,7 +10371,7 @@
       <c r="AA95" s="1"/>
       <c r="AB95" s="1"/>
     </row>
-    <row r="96" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="33"/>
       <c r="C96" s="73">
@@ -10417,7 +10410,7 @@
       <c r="AA96" s="1"/>
       <c r="AB96" s="1"/>
     </row>
-    <row r="97" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="33"/>
       <c r="C97" s="73">
@@ -10466,7 +10459,7 @@
       <c r="AA97" s="1"/>
       <c r="AB97" s="1"/>
     </row>
-    <row r="98" spans="1:28" ht="11.5" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:28" ht="11.45" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="33" t="s">
         <v>20</v>
@@ -10501,7 +10494,7 @@
       <c r="AA98" s="1"/>
       <c r="AB98" s="1"/>
     </row>
-    <row r="99" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="33"/>
       <c r="C99" s="73">
@@ -10534,7 +10527,7 @@
       <c r="AA99" s="1"/>
       <c r="AB99" s="1"/>
     </row>
-    <row r="100" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="33" t="s">
         <v>19</v>
@@ -10571,7 +10564,7 @@
       <c r="AA100" s="1"/>
       <c r="AB100" s="1"/>
     </row>
-    <row r="101" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="33"/>
       <c r="C101" s="73">
@@ -10606,7 +10599,7 @@
       <c r="AA101" s="1"/>
       <c r="AB101" s="1"/>
     </row>
-    <row r="102" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="33"/>
       <c r="C102" s="73">
@@ -10659,7 +10652,7 @@
       <c r="AA102" s="1"/>
       <c r="AB102" s="1"/>
     </row>
-    <row r="103" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="33"/>
       <c r="C103" s="73">
@@ -10710,7 +10703,7 @@
       <c r="AA103" s="1"/>
       <c r="AB103" s="1"/>
     </row>
-    <row r="104" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="33"/>
       <c r="C104" s="73">
@@ -10761,7 +10754,7 @@
       <c r="AA104" s="1"/>
       <c r="AB104" s="1"/>
     </row>
-    <row r="105" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="33"/>
       <c r="C105" s="73">
@@ -10794,7 +10787,7 @@
       <c r="AA105" s="1"/>
       <c r="AB105" s="1"/>
     </row>
-    <row r="106" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="33"/>
       <c r="C106" s="73">
@@ -10845,7 +10838,7 @@
       <c r="AA106" s="1"/>
       <c r="AB106" s="1"/>
     </row>
-    <row r="107" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="33"/>
       <c r="C107" s="73">
@@ -10894,7 +10887,7 @@
       <c r="AA107" s="1"/>
       <c r="AB107" s="1"/>
     </row>
-    <row r="108" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="33"/>
       <c r="C108" s="73">
@@ -10943,7 +10936,7 @@
       <c r="AA108" s="1"/>
       <c r="AB108" s="1"/>
     </row>
-    <row r="109" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="33"/>
       <c r="C109" s="73">
@@ -10992,7 +10985,7 @@
       <c r="AA109" s="1"/>
       <c r="AB109" s="1"/>
     </row>
-    <row r="110" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="33"/>
       <c r="C110" s="73">
@@ -11025,7 +11018,7 @@
       <c r="AA110" s="1"/>
       <c r="AB110" s="1"/>
     </row>
-    <row r="111" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111" s="33"/>
       <c r="C111" s="73">
@@ -11076,7 +11069,7 @@
       <c r="AA111" s="1"/>
       <c r="AB111" s="1"/>
     </row>
-    <row r="112" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="33"/>
       <c r="C112" s="73">
@@ -11125,7 +11118,7 @@
       <c r="AA112" s="1"/>
       <c r="AB112" s="1"/>
     </row>
-    <row r="113" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="33"/>
       <c r="C113" s="73">
@@ -11174,7 +11167,7 @@
       <c r="AA113" s="1"/>
       <c r="AB113" s="1"/>
     </row>
-    <row r="114" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="33"/>
       <c r="C114" s="73">
@@ -11223,7 +11216,7 @@
       <c r="AA114" s="1"/>
       <c r="AB114" s="1"/>
     </row>
-    <row r="115" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="33"/>
       <c r="C115" s="73">
@@ -11256,7 +11249,7 @@
       <c r="AA115" s="1"/>
       <c r="AB115" s="1"/>
     </row>
-    <row r="116" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="33"/>
       <c r="C116" s="73">
@@ -11307,7 +11300,7 @@
       <c r="AA116" s="1"/>
       <c r="AB116" s="1"/>
     </row>
-    <row r="117" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="33"/>
       <c r="C117" s="73">
@@ -11356,7 +11349,7 @@
       <c r="AA117" s="1"/>
       <c r="AB117" s="1"/>
     </row>
-    <row r="118" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="33"/>
       <c r="C118" s="73">
@@ -11405,7 +11398,7 @@
       <c r="AA118" s="1"/>
       <c r="AB118" s="1"/>
     </row>
-    <row r="119" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="33"/>
       <c r="C119" s="73">
@@ -11454,7 +11447,7 @@
       <c r="AA119" s="1"/>
       <c r="AB119" s="1"/>
     </row>
-    <row r="120" spans="1:28" s="143" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:28" s="143" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="33"/>
       <c r="C120" s="73">
@@ -11487,7 +11480,7 @@
       <c r="AA120" s="1"/>
       <c r="AB120" s="1"/>
     </row>
-    <row r="121" spans="1:28" s="143" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:28" s="143" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="33"/>
       <c r="C121" s="73">
@@ -11522,7 +11515,7 @@
       <c r="AA121" s="1"/>
       <c r="AB121" s="1"/>
     </row>
-    <row r="122" spans="1:28" s="143" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:28" s="143" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="33"/>
       <c r="C122" s="73">
@@ -11563,7 +11556,7 @@
       <c r="AA122" s="1"/>
       <c r="AB122" s="1"/>
     </row>
-    <row r="123" spans="1:28" s="143" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:28" s="143" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
       <c r="B123" s="33"/>
       <c r="C123" s="73">
@@ -11611,7 +11604,7 @@
       <c r="AA123" s="1"/>
       <c r="AB123" s="1"/>
     </row>
-    <row r="124" spans="1:28" s="143" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:28" s="143" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
       <c r="B124" s="33"/>
       <c r="C124" s="73">
@@ -11657,7 +11650,7 @@
       <c r="AA124" s="1"/>
       <c r="AB124" s="1"/>
     </row>
-    <row r="125" spans="1:28" s="143" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:28" s="143" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="B125" s="33"/>
       <c r="C125" s="73">
@@ -11700,7 +11693,7 @@
       <c r="AA125" s="1"/>
       <c r="AB125" s="1"/>
     </row>
-    <row r="126" spans="1:28" s="143" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:28" s="143" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
       <c r="B126" s="33"/>
       <c r="C126" s="73">
@@ -11733,7 +11726,7 @@
       <c r="AA126" s="1"/>
       <c r="AB126" s="1"/>
     </row>
-    <row r="127" spans="1:28" s="143" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:28" s="143" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="B127" s="33"/>
       <c r="C127" s="73">
@@ -11780,7 +11773,7 @@
       <c r="AA127" s="1"/>
       <c r="AB127" s="1"/>
     </row>
-    <row r="128" spans="1:28" s="143" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:28" s="143" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
       <c r="B128" s="33"/>
       <c r="C128" s="73">
@@ -11825,7 +11818,7 @@
       <c r="AA128" s="1"/>
       <c r="AB128" s="1"/>
     </row>
-    <row r="129" spans="1:28" s="143" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:28" s="143" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
       <c r="B129" s="33"/>
       <c r="C129" s="73">
@@ -11868,7 +11861,7 @@
       <c r="AA129" s="1"/>
       <c r="AB129" s="1"/>
     </row>
-    <row r="130" spans="1:28" s="143" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:28" s="143" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="B130" s="33"/>
       <c r="C130" s="73">
@@ -11901,7 +11894,7 @@
       <c r="AA130" s="1"/>
       <c r="AB130" s="1"/>
     </row>
-    <row r="131" spans="1:28" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131" s="33"/>
       <c r="C131" s="73">
@@ -11936,7 +11929,7 @@
       <c r="AA131" s="1"/>
       <c r="AB131" s="1"/>
     </row>
-    <row r="132" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="33"/>
       <c r="C132" s="73">
@@ -11969,7 +11962,7 @@
       <c r="AA132" s="1"/>
       <c r="AB132" s="1"/>
     </row>
-    <row r="133" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" s="35"/>
       <c r="C133" s="76">
@@ -12004,7 +11997,7 @@
       <c r="AA133" s="1"/>
       <c r="AB133" s="1"/>
     </row>
-    <row r="134" spans="1:28" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:28" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134" s="19"/>
       <c r="C134" s="77">
@@ -12037,7 +12030,7 @@
       <c r="AA134" s="1"/>
       <c r="AB134" s="1"/>
     </row>
-    <row r="135" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="73">
@@ -12070,7 +12063,7 @@
       <c r="AA135" s="1"/>
       <c r="AB135" s="1"/>
     </row>
-    <row r="136" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="73">
@@ -12103,7 +12096,7 @@
       <c r="AA136" s="1"/>
       <c r="AB136" s="1"/>
     </row>
-    <row r="137" spans="1:28" s="95" customFormat="1" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:28" s="95" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="1"/>
       <c r="B137" s="20"/>
       <c r="C137" s="74">
@@ -12136,7 +12129,7 @@
       <c r="AA137" s="1"/>
       <c r="AB137" s="1"/>
     </row>
-    <row r="138" spans="1:28" s="95" customFormat="1" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:28" s="95" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
       <c r="B138" s="34" t="s">
         <v>21</v>
@@ -12171,7 +12164,7 @@
       <c r="AA138" s="1"/>
       <c r="AB138" s="1"/>
     </row>
-    <row r="139" spans="1:28" s="95" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:28" s="95" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
       <c r="B139" s="33"/>
       <c r="C139" s="73">
@@ -12204,7 +12197,7 @@
       <c r="AA139" s="1"/>
       <c r="AB139" s="1"/>
     </row>
-    <row r="140" spans="1:28" s="95" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:28" s="95" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
       <c r="B140" s="33"/>
       <c r="C140" s="73">
@@ -12241,7 +12234,7 @@
       <c r="AA140" s="1"/>
       <c r="AB140" s="1"/>
     </row>
-    <row r="141" spans="1:28" s="95" customFormat="1" ht="20.149999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:28" s="95" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
       <c r="B141" s="33"/>
       <c r="C141" s="73">
@@ -12278,7 +12271,7 @@
       <c r="AA141" s="1"/>
       <c r="AB141" s="1"/>
     </row>
-    <row r="142" spans="1:28" s="95" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:28" s="95" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
       <c r="B142" s="33"/>
       <c r="C142" s="73">
@@ -12311,7 +12304,7 @@
       <c r="AA142" s="1"/>
       <c r="AB142" s="1"/>
     </row>
-    <row r="143" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
       <c r="B143" s="33"/>
       <c r="C143" s="73">
@@ -12344,7 +12337,7 @@
       <c r="AA143" s="1"/>
       <c r="AB143" s="1"/>
     </row>
-    <row r="144" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
       <c r="B144" s="33"/>
       <c r="C144" s="73">
@@ -12379,7 +12372,7 @@
       <c r="AA144" s="1"/>
       <c r="AB144" s="1"/>
     </row>
-    <row r="145" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
       <c r="B145" s="33"/>
       <c r="C145" s="73">
@@ -12414,7 +12407,7 @@
       <c r="AA145" s="1"/>
       <c r="AB145" s="1"/>
     </row>
-    <row r="146" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
       <c r="B146" s="33"/>
       <c r="C146" s="73">
@@ -12469,7 +12462,7 @@
       <c r="AA146" s="1"/>
       <c r="AB146" s="1"/>
     </row>
-    <row r="147" spans="1:28" s="95" customFormat="1" ht="11.5" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:28" s="95" customFormat="1" ht="11.45" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
       <c r="B147" s="33" t="s">
         <v>20</v>
@@ -12504,7 +12497,7 @@
       <c r="AA147" s="1"/>
       <c r="AB147" s="1"/>
     </row>
-    <row r="148" spans="1:28" s="95" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:28" s="95" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
       <c r="B148" s="33"/>
       <c r="C148" s="73">
@@ -12559,7 +12552,7 @@
       <c r="AA148" s="1"/>
       <c r="AB148" s="1"/>
     </row>
-    <row r="149" spans="1:28" s="95" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:28" s="95" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
       <c r="B149" s="33" t="s">
         <v>19</v>
@@ -12596,7 +12589,7 @@
       <c r="AA149" s="1"/>
       <c r="AB149" s="1"/>
     </row>
-    <row r="150" spans="1:28" s="95" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:28" s="95" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
       <c r="B150" s="33"/>
       <c r="C150" s="73">
@@ -12631,7 +12624,7 @@
       <c r="AA150" s="1"/>
       <c r="AB150" s="1"/>
     </row>
-    <row r="151" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
       <c r="B151" s="33"/>
       <c r="C151" s="73">
@@ -12666,7 +12659,7 @@
       <c r="AA151" s="1"/>
       <c r="AB151" s="1"/>
     </row>
-    <row r="152" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
       <c r="B152" s="33"/>
       <c r="C152" s="73">
@@ -12705,7 +12698,7 @@
       <c r="AA152" s="1"/>
       <c r="AB152" s="1"/>
     </row>
-    <row r="153" spans="1:28" s="95" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:28" s="95" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A153" s="1"/>
       <c r="B153" s="33"/>
       <c r="C153" s="73">
@@ -12764,7 +12757,7 @@
       <c r="AA153" s="1"/>
       <c r="AB153" s="1"/>
     </row>
-    <row r="154" spans="1:28" s="95" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:28" s="95" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A154" s="1"/>
       <c r="B154" s="33"/>
       <c r="C154" s="73">
@@ -12821,7 +12814,7 @@
       <c r="AA154" s="1"/>
       <c r="AB154" s="1"/>
     </row>
-    <row r="155" spans="1:28" s="95" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:28" s="95" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
       <c r="B155" s="33"/>
       <c r="C155" s="73">
@@ -12858,7 +12851,7 @@
       <c r="AA155" s="1"/>
       <c r="AB155" s="1"/>
     </row>
-    <row r="156" spans="1:28" s="95" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:28" s="95" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A156" s="1"/>
       <c r="B156" s="33"/>
       <c r="C156" s="73">
@@ -12915,7 +12908,7 @@
       <c r="AA156" s="1"/>
       <c r="AB156" s="1"/>
     </row>
-    <row r="157" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
       <c r="B157" s="33"/>
       <c r="C157" s="73">
@@ -12974,7 +12967,7 @@
       <c r="AA157" s="1"/>
       <c r="AB157" s="1"/>
     </row>
-    <row r="158" spans="1:28" s="118" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:28" s="118" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
       <c r="B158" s="33"/>
       <c r="C158" s="73">
@@ -13031,7 +13024,7 @@
       <c r="AA158" s="1"/>
       <c r="AB158" s="1"/>
     </row>
-    <row r="159" spans="1:28" s="118" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:28" s="118" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A159" s="1"/>
       <c r="B159" s="33"/>
       <c r="C159" s="73">
@@ -13088,7 +13081,7 @@
       <c r="AA159" s="1"/>
       <c r="AB159" s="1"/>
     </row>
-    <row r="160" spans="1:28" s="95" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:28" s="95" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
       <c r="B160" s="33"/>
       <c r="C160" s="73">
@@ -13145,7 +13138,7 @@
       <c r="AA160" s="1"/>
       <c r="AB160" s="1"/>
     </row>
-    <row r="161" spans="1:31" s="95" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:31" s="95" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A161" s="1"/>
       <c r="B161" s="33"/>
       <c r="C161" s="73">
@@ -13202,7 +13195,7 @@
       <c r="AA161" s="1"/>
       <c r="AB161" s="1"/>
     </row>
-    <row r="162" spans="1:31" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:31" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A162" s="1"/>
       <c r="B162" s="33"/>
       <c r="C162" s="73">
@@ -13262,7 +13255,7 @@
       <c r="AD162" s="123"/>
       <c r="AE162" s="123"/>
     </row>
-    <row r="163" spans="1:31" s="139" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:31" s="139" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A163" s="1"/>
       <c r="B163" s="33"/>
       <c r="C163" s="73">
@@ -13319,7 +13312,7 @@
       <c r="AA163" s="1"/>
       <c r="AB163" s="1"/>
     </row>
-    <row r="164" spans="1:31" s="107" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:31" s="107" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A164" s="1"/>
       <c r="B164" s="33"/>
       <c r="C164" s="73">
@@ -13355,7 +13348,7 @@
       <c r="AD164" s="123"/>
       <c r="AE164" s="123"/>
     </row>
-    <row r="165" spans="1:31" s="107" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:31" s="107" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A165" s="1"/>
       <c r="B165" s="33"/>
       <c r="C165" s="73">
@@ -13418,7 +13411,7 @@
       <c r="AD165" s="123"/>
       <c r="AE165" s="123"/>
     </row>
-    <row r="166" spans="1:31" s="107" customFormat="1" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:31" s="107" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A166" s="1"/>
       <c r="B166" s="33"/>
       <c r="C166" s="73">
@@ -13456,7 +13449,7 @@
       <c r="AD166" s="123"/>
       <c r="AE166" s="123"/>
     </row>
-    <row r="167" spans="1:31" s="106" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:31" s="106" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A167" s="1"/>
       <c r="B167" s="33"/>
       <c r="C167" s="73">
@@ -13510,7 +13503,7 @@
       <c r="AD167" s="123"/>
       <c r="AE167" s="123"/>
     </row>
-    <row r="168" spans="1:31" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:31" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A168" s="1"/>
       <c r="B168" s="33"/>
       <c r="C168" s="73">
@@ -13573,7 +13566,7 @@
       <c r="AA168" s="1"/>
       <c r="AB168" s="1"/>
     </row>
-    <row r="169" spans="1:31" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:31" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A169" s="1"/>
       <c r="B169" s="33"/>
       <c r="C169" s="73">
@@ -13634,7 +13627,7 @@
       <c r="AA169" s="1"/>
       <c r="AB169" s="1"/>
     </row>
-    <row r="170" spans="1:31" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:31" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A170" s="1"/>
       <c r="B170" s="33"/>
       <c r="C170" s="73">
@@ -13693,7 +13686,7 @@
       <c r="AA170" s="1"/>
       <c r="AB170" s="1"/>
     </row>
-    <row r="171" spans="1:31" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:31" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A171" s="1"/>
       <c r="B171" s="33"/>
       <c r="C171" s="73">
@@ -13752,7 +13745,7 @@
       <c r="AA171" s="1"/>
       <c r="AB171" s="1"/>
     </row>
-    <row r="172" spans="1:31" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:31" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A172" s="1"/>
       <c r="B172" s="33"/>
       <c r="C172" s="73">
@@ -13811,7 +13804,7 @@
       <c r="AA172" s="1"/>
       <c r="AB172" s="1"/>
     </row>
-    <row r="173" spans="1:31" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:31" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A173" s="1"/>
       <c r="B173" s="33"/>
       <c r="C173" s="73">
@@ -13872,7 +13865,7 @@
       <c r="AA173" s="1"/>
       <c r="AB173" s="1"/>
     </row>
-    <row r="174" spans="1:31" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:31" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A174" s="1"/>
       <c r="B174" s="33"/>
       <c r="C174" s="73">
@@ -13933,7 +13926,7 @@
       <c r="AA174" s="1"/>
       <c r="AB174" s="1"/>
     </row>
-    <row r="175" spans="1:31" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:31" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A175" s="1"/>
       <c r="B175" s="33"/>
       <c r="C175" s="73">
@@ -13992,7 +13985,7 @@
       <c r="AA175" s="1"/>
       <c r="AB175" s="1"/>
     </row>
-    <row r="176" spans="1:31" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:31" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A176" s="1"/>
       <c r="B176" s="33"/>
       <c r="C176" s="73">
@@ -14051,7 +14044,7 @@
       <c r="AA176" s="1"/>
       <c r="AB176" s="1"/>
     </row>
-    <row r="177" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A177" s="1"/>
       <c r="B177" s="33"/>
       <c r="C177" s="73">
@@ -14110,7 +14103,7 @@
       <c r="AA177" s="1"/>
       <c r="AB177" s="1"/>
     </row>
-    <row r="178" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A178" s="1"/>
       <c r="B178" s="33"/>
       <c r="C178" s="73">
@@ -14171,7 +14164,7 @@
       <c r="AA178" s="1"/>
       <c r="AB178" s="1"/>
     </row>
-    <row r="179" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A179" s="1"/>
       <c r="B179" s="33"/>
       <c r="C179" s="73">
@@ -14232,7 +14225,7 @@
       <c r="AA179" s="1"/>
       <c r="AB179" s="1"/>
     </row>
-    <row r="180" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A180" s="1"/>
       <c r="B180" s="33"/>
       <c r="C180" s="73">
@@ -14291,7 +14284,7 @@
       <c r="AA180" s="1"/>
       <c r="AB180" s="1"/>
     </row>
-    <row r="181" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A181" s="1"/>
       <c r="B181" s="33"/>
       <c r="C181" s="73">
@@ -14348,7 +14341,7 @@
       <c r="AA181" s="1"/>
       <c r="AB181" s="1"/>
     </row>
-    <row r="182" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A182" s="1"/>
       <c r="B182" s="33"/>
       <c r="C182" s="73">
@@ -14407,7 +14400,7 @@
       <c r="AA182" s="1"/>
       <c r="AB182" s="1"/>
     </row>
-    <row r="183" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A183" s="1"/>
       <c r="B183" s="33"/>
       <c r="C183" s="73">
@@ -14468,7 +14461,7 @@
       <c r="AA183" s="1"/>
       <c r="AB183" s="1"/>
     </row>
-    <row r="184" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A184" s="1"/>
       <c r="B184" s="33"/>
       <c r="C184" s="73">
@@ -14529,7 +14522,7 @@
       <c r="AA184" s="1"/>
       <c r="AB184" s="1"/>
     </row>
-    <row r="185" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A185" s="1"/>
       <c r="B185" s="33"/>
       <c r="C185" s="73">
@@ -14588,7 +14581,7 @@
       <c r="AA185" s="1"/>
       <c r="AB185" s="1"/>
     </row>
-    <row r="186" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A186" s="1"/>
       <c r="B186" s="33"/>
       <c r="C186" s="73">
@@ -14647,7 +14640,7 @@
       <c r="AA186" s="1"/>
       <c r="AB186" s="1"/>
     </row>
-    <row r="187" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A187" s="1"/>
       <c r="B187" s="33"/>
       <c r="C187" s="73">
@@ -14706,7 +14699,7 @@
       <c r="AA187" s="1"/>
       <c r="AB187" s="1"/>
     </row>
-    <row r="188" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A188" s="1"/>
       <c r="B188" s="33"/>
       <c r="C188" s="73">
@@ -14769,7 +14762,7 @@
       <c r="AA188" s="1"/>
       <c r="AB188" s="1"/>
     </row>
-    <row r="189" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A189" s="1"/>
       <c r="B189" s="33"/>
       <c r="C189" s="73">
@@ -14828,7 +14821,7 @@
       <c r="AA189" s="1"/>
       <c r="AB189" s="1"/>
     </row>
-    <row r="190" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A190" s="1"/>
       <c r="B190" s="33"/>
       <c r="C190" s="73">
@@ -14885,7 +14878,7 @@
       <c r="AA190" s="1"/>
       <c r="AB190" s="1"/>
     </row>
-    <row r="191" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A191" s="1"/>
       <c r="B191" s="33"/>
       <c r="C191" s="73">
@@ -14942,7 +14935,7 @@
       <c r="AA191" s="1"/>
       <c r="AB191" s="1"/>
     </row>
-    <row r="192" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A192" s="1"/>
       <c r="B192" s="33"/>
       <c r="C192" s="73">
@@ -14999,7 +14992,7 @@
       <c r="AA192" s="1"/>
       <c r="AB192" s="1"/>
     </row>
-    <row r="193" spans="1:30" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:30" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A193" s="1"/>
       <c r="B193" s="33"/>
       <c r="C193" s="73">
@@ -15058,7 +15051,7 @@
       <c r="AA193" s="1"/>
       <c r="AB193" s="1"/>
     </row>
-    <row r="194" spans="1:30" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:30" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A194" s="1"/>
       <c r="B194" s="33"/>
       <c r="C194" s="73">
@@ -15115,7 +15108,7 @@
       <c r="AA194" s="1"/>
       <c r="AB194" s="1"/>
     </row>
-    <row r="195" spans="1:30" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:30" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A195" s="1"/>
       <c r="B195" s="33"/>
       <c r="C195" s="73">
@@ -15172,7 +15165,7 @@
       <c r="AA195" s="1"/>
       <c r="AB195" s="1"/>
     </row>
-    <row r="196" spans="1:30" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:30" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A196" s="1"/>
       <c r="B196" s="33"/>
       <c r="C196" s="73">
@@ -15229,7 +15222,7 @@
       <c r="AA196" s="1"/>
       <c r="AB196" s="1"/>
     </row>
-    <row r="197" spans="1:30" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:30" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A197" s="1"/>
       <c r="B197" s="33"/>
       <c r="C197" s="73">
@@ -15286,7 +15279,7 @@
       <c r="AA197" s="1"/>
       <c r="AB197" s="1"/>
     </row>
-    <row r="198" spans="1:30" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:30" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A198" s="1"/>
       <c r="B198" s="33"/>
       <c r="C198" s="73">
@@ -15345,7 +15338,7 @@
       <c r="AA198" s="1"/>
       <c r="AB198" s="1"/>
     </row>
-    <row r="199" spans="1:30" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:30" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A199" s="1"/>
       <c r="B199" s="33"/>
       <c r="C199" s="73">
@@ -15402,7 +15395,7 @@
       <c r="AA199" s="1"/>
       <c r="AB199" s="1"/>
     </row>
-    <row r="200" spans="1:30" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:30" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A200" s="1"/>
       <c r="B200" s="33"/>
       <c r="C200" s="73">
@@ -15459,7 +15452,7 @@
       <c r="AA200" s="1"/>
       <c r="AB200" s="1"/>
     </row>
-    <row r="201" spans="1:30" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:30" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A201" s="1"/>
       <c r="B201" s="33"/>
       <c r="C201" s="73">
@@ -15516,7 +15509,7 @@
       <c r="AA201" s="1"/>
       <c r="AB201" s="1"/>
     </row>
-    <row r="202" spans="1:30" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:30" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A202" s="1"/>
       <c r="B202" s="33"/>
       <c r="C202" s="73">
@@ -15573,7 +15566,7 @@
       <c r="AA202" s="1"/>
       <c r="AB202" s="1"/>
     </row>
-    <row r="203" spans="1:30" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:30" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A203" s="1"/>
       <c r="B203" s="33"/>
       <c r="C203" s="73">
@@ -15632,7 +15625,7 @@
       <c r="AA203" s="1"/>
       <c r="AB203" s="1"/>
     </row>
-    <row r="204" spans="1:30" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:30" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A204" s="1"/>
       <c r="B204" s="33"/>
       <c r="C204" s="73">
@@ -15689,7 +15682,7 @@
       <c r="AA204" s="1"/>
       <c r="AB204" s="1"/>
     </row>
-    <row r="205" spans="1:30" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:30" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A205" s="1"/>
       <c r="B205" s="33"/>
       <c r="C205" s="73">
@@ -15746,7 +15739,7 @@
       <c r="AA205" s="1"/>
       <c r="AB205" s="1"/>
     </row>
-    <row r="206" spans="1:30" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:30" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A206" s="1"/>
       <c r="B206" s="33"/>
       <c r="C206" s="73">
@@ -15803,7 +15796,7 @@
       <c r="AA206" s="1"/>
       <c r="AB206" s="1"/>
     </row>
-    <row r="207" spans="1:30" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:30" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A207" s="1"/>
       <c r="B207" s="33"/>
       <c r="C207" s="73">
@@ -15860,7 +15853,7 @@
       <c r="AA207" s="1"/>
       <c r="AB207" s="1"/>
     </row>
-    <row r="208" spans="1:30" s="107" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:30" s="107" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A208" s="1"/>
       <c r="B208" s="33"/>
       <c r="C208" s="73">
@@ -15895,7 +15888,7 @@
       <c r="AC208" s="123"/>
       <c r="AD208" s="123"/>
     </row>
-    <row r="209" spans="1:28" s="126" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:28" s="126" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A209" s="1"/>
       <c r="B209" s="33"/>
       <c r="C209" s="73">
@@ -15955,7 +15948,7 @@
       <c r="AA209" s="1"/>
       <c r="AB209" s="1"/>
     </row>
-    <row r="210" spans="1:28" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:28" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A210" s="1"/>
       <c r="B210" s="33"/>
       <c r="C210" s="73">
@@ -16025,7 +16018,7 @@
       <c r="AA210" s="1"/>
       <c r="AB210" s="1"/>
     </row>
-    <row r="211" spans="1:28" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:28" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A211" s="1"/>
       <c r="B211" s="33"/>
       <c r="C211" s="73">
@@ -16095,7 +16088,7 @@
       <c r="AA211" s="1"/>
       <c r="AB211" s="1"/>
     </row>
-    <row r="212" spans="1:28" s="126" customFormat="1" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:28" s="126" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A212" s="1"/>
       <c r="B212" s="33"/>
       <c r="C212" s="73">
@@ -16130,7 +16123,7 @@
       <c r="AA212" s="1"/>
       <c r="AB212" s="1"/>
     </row>
-    <row r="213" spans="1:28" s="126" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:28" s="126" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A213" s="1"/>
       <c r="B213" s="33"/>
       <c r="C213" s="73">
@@ -16181,7 +16174,7 @@
       <c r="AA213" s="1"/>
       <c r="AB213" s="1"/>
     </row>
-    <row r="214" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A214" s="1"/>
       <c r="B214" s="33"/>
       <c r="C214" s="73">
@@ -16244,7 +16237,7 @@
       <c r="AA214" s="1"/>
       <c r="AB214" s="1"/>
     </row>
-    <row r="215" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A215" s="1"/>
       <c r="B215" s="33"/>
       <c r="C215" s="73">
@@ -16307,7 +16300,7 @@
       <c r="AA215" s="1"/>
       <c r="AB215" s="1"/>
     </row>
-    <row r="216" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A216" s="1"/>
       <c r="B216" s="33"/>
       <c r="C216" s="73">
@@ -16364,7 +16357,7 @@
       <c r="AA216" s="1"/>
       <c r="AB216" s="1"/>
     </row>
-    <row r="217" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A217" s="1"/>
       <c r="B217" s="33"/>
       <c r="C217" s="73">
@@ -16423,7 +16416,7 @@
       <c r="AA217" s="1"/>
       <c r="AB217" s="1"/>
     </row>
-    <row r="218" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A218" s="1"/>
       <c r="B218" s="33"/>
       <c r="C218" s="73">
@@ -16482,7 +16475,7 @@
       <c r="AA218" s="1"/>
       <c r="AB218" s="1"/>
     </row>
-    <row r="219" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A219" s="1"/>
       <c r="B219" s="33"/>
       <c r="C219" s="73">
@@ -16543,7 +16536,7 @@
       <c r="AA219" s="1"/>
       <c r="AB219" s="1"/>
     </row>
-    <row r="220" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A220" s="1"/>
       <c r="B220" s="33"/>
       <c r="C220" s="73">
@@ -16604,7 +16597,7 @@
       <c r="AA220" s="1"/>
       <c r="AB220" s="1"/>
     </row>
-    <row r="221" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A221" s="1"/>
       <c r="B221" s="33"/>
       <c r="C221" s="73">
@@ -16661,7 +16654,7 @@
       <c r="AA221" s="1"/>
       <c r="AB221" s="1"/>
     </row>
-    <row r="222" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A222" s="1"/>
       <c r="B222" s="33"/>
       <c r="C222" s="73">
@@ -16718,7 +16711,7 @@
       <c r="AA222" s="1"/>
       <c r="AB222" s="1"/>
     </row>
-    <row r="223" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A223" s="1"/>
       <c r="B223" s="33"/>
       <c r="C223" s="73">
@@ -16775,7 +16768,7 @@
       <c r="AA223" s="1"/>
       <c r="AB223" s="1"/>
     </row>
-    <row r="224" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A224" s="1"/>
       <c r="B224" s="33"/>
       <c r="C224" s="73">
@@ -16834,7 +16827,7 @@
       <c r="AA224" s="1"/>
       <c r="AB224" s="1"/>
     </row>
-    <row r="225" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A225" s="1"/>
       <c r="B225" s="33"/>
       <c r="C225" s="73">
@@ -16893,7 +16886,7 @@
       <c r="AA225" s="1"/>
       <c r="AB225" s="1"/>
     </row>
-    <row r="226" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A226" s="1"/>
       <c r="B226" s="33"/>
       <c r="C226" s="73">
@@ -16950,7 +16943,7 @@
       <c r="AA226" s="1"/>
       <c r="AB226" s="1"/>
     </row>
-    <row r="227" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A227" s="1"/>
       <c r="B227" s="33"/>
       <c r="C227" s="73">
@@ -17007,7 +17000,7 @@
       <c r="AA227" s="1"/>
       <c r="AB227" s="1"/>
     </row>
-    <row r="228" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A228" s="1"/>
       <c r="B228" s="33"/>
       <c r="C228" s="73">
@@ -17064,7 +17057,7 @@
       <c r="AA228" s="1"/>
       <c r="AB228" s="1"/>
     </row>
-    <row r="229" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A229" s="1"/>
       <c r="B229" s="33"/>
       <c r="C229" s="73">
@@ -17123,7 +17116,7 @@
       <c r="AA229" s="1"/>
       <c r="AB229" s="1"/>
     </row>
-    <row r="230" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A230" s="1"/>
       <c r="B230" s="33"/>
       <c r="C230" s="73">
@@ -17182,7 +17175,7 @@
       <c r="AA230" s="1"/>
       <c r="AB230" s="1"/>
     </row>
-    <row r="231" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A231" s="1"/>
       <c r="B231" s="33"/>
       <c r="C231" s="73">
@@ -17239,7 +17232,7 @@
       <c r="AA231" s="1"/>
       <c r="AB231" s="1"/>
     </row>
-    <row r="232" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A232" s="1"/>
       <c r="B232" s="33"/>
       <c r="C232" s="73">
@@ -17296,7 +17289,7 @@
       <c r="AA232" s="1"/>
       <c r="AB232" s="1"/>
     </row>
-    <row r="233" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A233" s="1"/>
       <c r="B233" s="33"/>
       <c r="C233" s="73">
@@ -17353,7 +17346,7 @@
       <c r="AA233" s="1"/>
       <c r="AB233" s="1"/>
     </row>
-    <row r="234" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A234" s="1"/>
       <c r="B234" s="33"/>
       <c r="C234" s="73">
@@ -17423,7 +17416,7 @@
       <c r="AA234" s="1"/>
       <c r="AB234" s="1"/>
     </row>
-    <row r="235" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A235" s="1"/>
       <c r="B235" s="33"/>
       <c r="C235" s="73">
@@ -17490,7 +17483,7 @@
       <c r="AA235" s="1"/>
       <c r="AB235" s="1"/>
     </row>
-    <row r="236" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A236" s="1"/>
       <c r="B236" s="33"/>
       <c r="C236" s="73">
@@ -17553,7 +17546,7 @@
       <c r="AA236" s="1"/>
       <c r="AB236" s="1"/>
     </row>
-    <row r="237" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A237" s="1"/>
       <c r="B237" s="33"/>
       <c r="C237" s="73">
@@ -17616,7 +17609,7 @@
       <c r="AA237" s="1"/>
       <c r="AB237" s="1"/>
     </row>
-    <row r="238" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A238" s="1"/>
       <c r="B238" s="33"/>
       <c r="C238" s="73">
@@ -17683,7 +17676,7 @@
       <c r="AA238" s="1"/>
       <c r="AB238" s="1"/>
     </row>
-    <row r="239" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A239" s="1"/>
       <c r="B239" s="33"/>
       <c r="C239" s="73">
@@ -17752,7 +17745,7 @@
       <c r="AA239" s="1"/>
       <c r="AB239" s="1"/>
     </row>
-    <row r="240" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A240" s="1"/>
       <c r="B240" s="33"/>
       <c r="C240" s="73">
@@ -17819,7 +17812,7 @@
       <c r="AA240" s="1"/>
       <c r="AB240" s="1"/>
     </row>
-    <row r="241" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A241" s="1"/>
       <c r="B241" s="33"/>
       <c r="C241" s="73">
@@ -17886,7 +17879,7 @@
       <c r="AA241" s="1"/>
       <c r="AB241" s="1"/>
     </row>
-    <row r="242" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A242" s="1"/>
       <c r="B242" s="33"/>
       <c r="C242" s="73">
@@ -17953,7 +17946,7 @@
       <c r="AA242" s="1"/>
       <c r="AB242" s="1"/>
     </row>
-    <row r="243" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A243" s="1"/>
       <c r="B243" s="33"/>
       <c r="C243" s="73">
@@ -18020,7 +18013,7 @@
       <c r="AA243" s="1"/>
       <c r="AB243" s="1"/>
     </row>
-    <row r="244" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A244" s="1"/>
       <c r="B244" s="33"/>
       <c r="C244" s="73">
@@ -18089,7 +18082,7 @@
       <c r="AA244" s="1"/>
       <c r="AB244" s="1"/>
     </row>
-    <row r="245" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A245" s="1"/>
       <c r="B245" s="33"/>
       <c r="C245" s="73">
@@ -18156,7 +18149,7 @@
       <c r="AA245" s="1"/>
       <c r="AB245" s="1"/>
     </row>
-    <row r="246" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A246" s="1"/>
       <c r="B246" s="33"/>
       <c r="C246" s="73">
@@ -18223,7 +18216,7 @@
       <c r="AA246" s="1"/>
       <c r="AB246" s="1"/>
     </row>
-    <row r="247" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A247" s="1"/>
       <c r="B247" s="33"/>
       <c r="C247" s="73">
@@ -18290,7 +18283,7 @@
       <c r="AA247" s="1"/>
       <c r="AB247" s="1"/>
     </row>
-    <row r="248" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A248" s="1"/>
       <c r="B248" s="33"/>
       <c r="C248" s="73">
@@ -18357,7 +18350,7 @@
       <c r="AA248" s="1"/>
       <c r="AB248" s="1"/>
     </row>
-    <row r="249" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A249" s="1"/>
       <c r="B249" s="33"/>
       <c r="C249" s="73">
@@ -18426,7 +18419,7 @@
       <c r="AA249" s="1"/>
       <c r="AB249" s="1"/>
     </row>
-    <row r="250" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A250" s="1"/>
       <c r="B250" s="33"/>
       <c r="C250" s="73">
@@ -18493,7 +18486,7 @@
       <c r="AA250" s="1"/>
       <c r="AB250" s="1"/>
     </row>
-    <row r="251" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A251" s="1"/>
       <c r="B251" s="33"/>
       <c r="C251" s="73">
@@ -18560,7 +18553,7 @@
       <c r="AA251" s="1"/>
       <c r="AB251" s="1"/>
     </row>
-    <row r="252" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A252" s="1"/>
       <c r="B252" s="33"/>
       <c r="C252" s="73">
@@ -18627,7 +18620,7 @@
       <c r="AA252" s="1"/>
       <c r="AB252" s="1"/>
     </row>
-    <row r="253" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A253" s="1"/>
       <c r="B253" s="33"/>
       <c r="C253" s="73">
@@ -18694,7 +18687,7 @@
       <c r="AA253" s="1"/>
       <c r="AB253" s="1"/>
     </row>
-    <row r="254" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A254" s="1"/>
       <c r="B254" s="33"/>
       <c r="C254" s="73">
@@ -18755,7 +18748,7 @@
       <c r="AA254" s="1"/>
       <c r="AB254" s="1"/>
     </row>
-    <row r="255" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A255" s="1"/>
       <c r="B255" s="33"/>
       <c r="C255" s="73">
@@ -18812,7 +18805,7 @@
       <c r="AA255" s="1"/>
       <c r="AB255" s="1"/>
     </row>
-    <row r="256" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A256" s="1"/>
       <c r="B256" s="33"/>
       <c r="C256" s="73">
@@ -18869,7 +18862,7 @@
       <c r="AA256" s="1"/>
       <c r="AB256" s="1"/>
     </row>
-    <row r="257" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A257" s="1"/>
       <c r="B257" s="33"/>
       <c r="C257" s="73">
@@ -18926,7 +18919,7 @@
       <c r="AA257" s="1"/>
       <c r="AB257" s="1"/>
     </row>
-    <row r="258" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A258" s="1"/>
       <c r="B258" s="33"/>
       <c r="C258" s="73">
@@ -18983,7 +18976,7 @@
       <c r="AA258" s="1"/>
       <c r="AB258" s="1"/>
     </row>
-    <row r="259" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A259" s="1"/>
       <c r="B259" s="33"/>
       <c r="C259" s="73">
@@ -19052,7 +19045,7 @@
       <c r="AA259" s="1"/>
       <c r="AB259" s="1"/>
     </row>
-    <row r="260" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A260" s="1"/>
       <c r="B260" s="33"/>
       <c r="C260" s="73">
@@ -19119,7 +19112,7 @@
       <c r="AA260" s="1"/>
       <c r="AB260" s="1"/>
     </row>
-    <row r="261" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A261" s="1"/>
       <c r="B261" s="33"/>
       <c r="C261" s="73">
@@ -19186,7 +19179,7 @@
       <c r="AA261" s="1"/>
       <c r="AB261" s="1"/>
     </row>
-    <row r="262" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A262" s="1"/>
       <c r="B262" s="33"/>
       <c r="C262" s="73">
@@ -19253,7 +19246,7 @@
       <c r="AA262" s="1"/>
       <c r="AB262" s="1"/>
     </row>
-    <row r="263" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A263" s="1"/>
       <c r="B263" s="33"/>
       <c r="C263" s="73">
@@ -19320,7 +19313,7 @@
       <c r="AA263" s="1"/>
       <c r="AB263" s="1"/>
     </row>
-    <row r="264" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A264" s="1"/>
       <c r="B264" s="33"/>
       <c r="C264" s="73">
@@ -19379,7 +19372,7 @@
       <c r="AA264" s="1"/>
       <c r="AB264" s="1"/>
     </row>
-    <row r="265" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A265" s="1"/>
       <c r="B265" s="33"/>
       <c r="C265" s="73">
@@ -19441,7 +19434,7 @@
       <c r="AA265" s="1"/>
       <c r="AB265" s="1"/>
     </row>
-    <row r="266" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A266" s="1"/>
       <c r="B266" s="33"/>
       <c r="C266" s="73">
@@ -19502,7 +19495,7 @@
       <c r="AA266" s="1"/>
       <c r="AB266" s="1"/>
     </row>
-    <row r="267" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A267" s="1"/>
       <c r="B267" s="33"/>
       <c r="C267" s="73">
@@ -19562,7 +19555,7 @@
       <c r="AA267" s="1"/>
       <c r="AB267" s="1"/>
     </row>
-    <row r="268" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A268" s="1"/>
       <c r="B268" s="33"/>
       <c r="C268" s="73">
@@ -19629,7 +19622,7 @@
       <c r="AA268" s="1"/>
       <c r="AB268" s="1"/>
     </row>
-    <row r="269" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A269" s="1"/>
       <c r="B269" s="33"/>
       <c r="C269" s="73">
@@ -19694,7 +19687,7 @@
       <c r="AA269" s="1"/>
       <c r="AB269" s="1"/>
     </row>
-    <row r="270" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A270" s="1"/>
       <c r="B270" s="33"/>
       <c r="C270" s="73">
@@ -19756,7 +19749,7 @@
       <c r="AA270" s="1"/>
       <c r="AB270" s="1"/>
     </row>
-    <row r="271" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A271" s="1"/>
       <c r="B271" s="33"/>
       <c r="C271" s="73">
@@ -19816,7 +19809,7 @@
       <c r="AA271" s="1"/>
       <c r="AB271" s="1"/>
     </row>
-    <row r="272" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A272" s="1"/>
       <c r="B272" s="33"/>
       <c r="C272" s="73">
@@ -19873,7 +19866,7 @@
       <c r="AA272" s="1"/>
       <c r="AB272" s="1"/>
     </row>
-    <row r="273" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A273" s="1"/>
       <c r="B273" s="33"/>
       <c r="C273" s="73">
@@ -19940,7 +19933,7 @@
       <c r="AA273" s="1"/>
       <c r="AB273" s="1"/>
     </row>
-    <row r="274" spans="1:28" s="126" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:28" s="126" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A274" s="1"/>
       <c r="B274" s="33"/>
       <c r="C274" s="73">
@@ -19973,7 +19966,7 @@
       <c r="AA274" s="1"/>
       <c r="AB274" s="1"/>
     </row>
-    <row r="275" spans="1:28" s="126" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:28" s="126" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A275" s="1"/>
       <c r="B275" s="33"/>
       <c r="C275" s="73">
@@ -20029,7 +20022,7 @@
       <c r="AA275" s="1"/>
       <c r="AB275" s="1"/>
     </row>
-    <row r="276" spans="1:28" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:28" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A276" s="1"/>
       <c r="B276" s="33"/>
       <c r="C276" s="73">
@@ -20082,7 +20075,7 @@
       <c r="AA276" s="1"/>
       <c r="AB276" s="1"/>
     </row>
-    <row r="277" spans="1:28" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:28" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A277" s="1"/>
       <c r="B277" s="33"/>
       <c r="C277" s="73">
@@ -20135,7 +20128,7 @@
       <c r="AA277" s="1"/>
       <c r="AB277" s="1"/>
     </row>
-    <row r="278" spans="1:28" s="126" customFormat="1" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:28" s="126" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A278" s="1"/>
       <c r="B278" s="33"/>
       <c r="C278" s="73">
@@ -20170,7 +20163,7 @@
       <c r="AA278" s="1"/>
       <c r="AB278" s="1"/>
     </row>
-    <row r="279" spans="1:28" s="126" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:28" s="126" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A279" s="1"/>
       <c r="B279" s="33"/>
       <c r="C279" s="73">
@@ -20220,7 +20213,7 @@
       <c r="AA279" s="1"/>
       <c r="AB279" s="1"/>
     </row>
-    <row r="280" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A280" s="1"/>
       <c r="B280" s="33"/>
       <c r="C280" s="73">
@@ -20278,7 +20271,7 @@
       <c r="AA280" s="1"/>
       <c r="AB280" s="1"/>
     </row>
-    <row r="281" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A281" s="1"/>
       <c r="B281" s="33"/>
       <c r="C281" s="73">
@@ -20336,7 +20329,7 @@
       <c r="AA281" s="1"/>
       <c r="AB281" s="1"/>
     </row>
-    <row r="282" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A282" s="1"/>
       <c r="B282" s="33"/>
       <c r="C282" s="73">
@@ -20389,7 +20382,7 @@
       <c r="AA282" s="1"/>
       <c r="AB282" s="1"/>
     </row>
-    <row r="283" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A283" s="1"/>
       <c r="B283" s="33"/>
       <c r="C283" s="73">
@@ -20441,7 +20434,7 @@
       <c r="AA283" s="1"/>
       <c r="AB283" s="1"/>
     </row>
-    <row r="284" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A284" s="1"/>
       <c r="B284" s="33"/>
       <c r="C284" s="73">
@@ -20496,7 +20489,7 @@
       <c r="AA284" s="1"/>
       <c r="AB284" s="1"/>
     </row>
-    <row r="285" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A285" s="1"/>
       <c r="B285" s="33"/>
       <c r="C285" s="73">
@@ -20550,7 +20543,7 @@
       <c r="AA285" s="1"/>
       <c r="AB285" s="1"/>
     </row>
-    <row r="286" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A286" s="1"/>
       <c r="B286" s="33"/>
       <c r="C286" s="73">
@@ -20604,7 +20597,7 @@
       <c r="AA286" s="1"/>
       <c r="AB286" s="1"/>
     </row>
-    <row r="287" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A287" s="1"/>
       <c r="B287" s="33"/>
       <c r="C287" s="73">
@@ -20654,7 +20647,7 @@
       <c r="AA287" s="1"/>
       <c r="AB287" s="1"/>
     </row>
-    <row r="288" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A288" s="1"/>
       <c r="B288" s="33"/>
       <c r="C288" s="73">
@@ -20704,7 +20697,7 @@
       <c r="AA288" s="1"/>
       <c r="AB288" s="1"/>
     </row>
-    <row r="289" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A289" s="1"/>
       <c r="B289" s="33"/>
       <c r="C289" s="73">
@@ -20757,7 +20750,7 @@
       <c r="AA289" s="1"/>
       <c r="AB289" s="1"/>
     </row>
-    <row r="290" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A290" s="1"/>
       <c r="B290" s="33"/>
       <c r="C290" s="73">
@@ -20811,7 +20804,7 @@
       <c r="AA290" s="1"/>
       <c r="AB290" s="1"/>
     </row>
-    <row r="291" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A291" s="1"/>
       <c r="B291" s="33"/>
       <c r="C291" s="73">
@@ -20865,7 +20858,7 @@
       <c r="AA291" s="1"/>
       <c r="AB291" s="1"/>
     </row>
-    <row r="292" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A292" s="1"/>
       <c r="B292" s="33"/>
       <c r="C292" s="73">
@@ -20915,7 +20908,7 @@
       <c r="AA292" s="1"/>
       <c r="AB292" s="1"/>
     </row>
-    <row r="293" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A293" s="1"/>
       <c r="B293" s="33"/>
       <c r="C293" s="73">
@@ -20965,7 +20958,7 @@
       <c r="AA293" s="1"/>
       <c r="AB293" s="1"/>
     </row>
-    <row r="294" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A294" s="1"/>
       <c r="B294" s="33"/>
       <c r="C294" s="73">
@@ -21018,7 +21011,7 @@
       <c r="AA294" s="1"/>
       <c r="AB294" s="1"/>
     </row>
-    <row r="295" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A295" s="1"/>
       <c r="B295" s="33"/>
       <c r="C295" s="73">
@@ -21070,7 +21063,7 @@
       <c r="AA295" s="1"/>
       <c r="AB295" s="1"/>
     </row>
-    <row r="296" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A296" s="1"/>
       <c r="B296" s="33"/>
       <c r="C296" s="73">
@@ -21122,7 +21115,7 @@
       <c r="AA296" s="1"/>
       <c r="AB296" s="1"/>
     </row>
-    <row r="297" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A297" s="1"/>
       <c r="B297" s="33"/>
       <c r="C297" s="73">
@@ -21171,7 +21164,7 @@
       <c r="AA297" s="1"/>
       <c r="AB297" s="1"/>
     </row>
-    <row r="298" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A298" s="1"/>
       <c r="B298" s="33"/>
       <c r="C298" s="73">
@@ -21218,7 +21211,7 @@
       <c r="AA298" s="1"/>
       <c r="AB298" s="1"/>
     </row>
-    <row r="299" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A299" s="1"/>
       <c r="B299" s="33"/>
       <c r="C299" s="73">
@@ -21271,7 +21264,7 @@
       <c r="AA299" s="1"/>
       <c r="AB299" s="1"/>
     </row>
-    <row r="300" spans="1:28" s="126" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:28" s="126" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A300" s="1"/>
       <c r="B300" s="33"/>
       <c r="C300" s="73">
@@ -21304,7 +21297,7 @@
       <c r="AA300" s="1"/>
       <c r="AB300" s="1"/>
     </row>
-    <row r="301" spans="1:28" s="95" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:28" s="95" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A301" s="1"/>
       <c r="B301" s="33"/>
       <c r="C301" s="73">
@@ -21337,7 +21330,7 @@
       <c r="AA301" s="1"/>
       <c r="AB301" s="1"/>
     </row>
-    <row r="302" spans="1:28" s="95" customFormat="1" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:28" s="95" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A302" s="1"/>
       <c r="B302" s="35"/>
       <c r="C302" s="76">
@@ -21372,7 +21365,7 @@
       <c r="AA302" s="1"/>
       <c r="AB302" s="1"/>
     </row>
-    <row r="303" spans="1:28" s="95" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:28" s="95" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A303" s="1"/>
       <c r="B303" s="19"/>
       <c r="C303" s="77">
@@ -21405,7 +21398,7 @@
       <c r="AA303" s="1"/>
       <c r="AB303" s="1"/>
     </row>
-    <row r="304" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A304" s="1"/>
       <c r="B304" s="1"/>
       <c r="C304" s="73">
@@ -21438,7 +21431,7 @@
       <c r="AA304" s="1"/>
       <c r="AB304" s="1"/>
     </row>
-    <row r="305" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A305" s="1"/>
       <c r="B305" s="1"/>
       <c r="C305" s="73">
@@ -21471,7 +21464,7 @@
       <c r="AA305" s="1"/>
       <c r="AB305" s="1"/>
     </row>
-    <row r="306" spans="1:28" s="97" customFormat="1" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="306" spans="1:28" s="97" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A306" s="1"/>
       <c r="B306" s="20"/>
       <c r="C306" s="74">
@@ -21504,7 +21497,7 @@
       <c r="AA306" s="1"/>
       <c r="AB306" s="1"/>
     </row>
-    <row r="307" spans="1:28" s="97" customFormat="1" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:28" s="97" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A307" s="1"/>
       <c r="B307" s="34" t="s">
         <v>21</v>
@@ -21539,7 +21532,7 @@
       <c r="AA307" s="1"/>
       <c r="AB307" s="1"/>
     </row>
-    <row r="308" spans="1:28" s="97" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:28" s="97" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A308" s="1"/>
       <c r="B308" s="33"/>
       <c r="C308" s="73">
@@ -21572,7 +21565,7 @@
       <c r="AA308" s="1"/>
       <c r="AB308" s="1"/>
     </row>
-    <row r="309" spans="1:28" s="97" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:28" s="97" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A309" s="1"/>
       <c r="B309" s="33"/>
       <c r="C309" s="73">
@@ -21609,7 +21602,7 @@
       <c r="AA309" s="1"/>
       <c r="AB309" s="1"/>
     </row>
-    <row r="310" spans="1:28" s="97" customFormat="1" ht="20.149999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:28" s="97" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A310" s="1"/>
       <c r="B310" s="33"/>
       <c r="C310" s="73">
@@ -21646,7 +21639,7 @@
       <c r="AA310" s="1"/>
       <c r="AB310" s="1"/>
     </row>
-    <row r="311" spans="1:28" s="97" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:28" s="97" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A311" s="1"/>
       <c r="B311" s="33"/>
       <c r="C311" s="73">
@@ -21679,7 +21672,7 @@
       <c r="AA311" s="1"/>
       <c r="AB311" s="1"/>
     </row>
-    <row r="312" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A312" s="1"/>
       <c r="B312" s="33"/>
       <c r="C312" s="73">
@@ -21712,7 +21705,7 @@
       <c r="AA312" s="1"/>
       <c r="AB312" s="1"/>
     </row>
-    <row r="313" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A313" s="1"/>
       <c r="B313" s="33"/>
       <c r="C313" s="73">
@@ -21751,7 +21744,7 @@
       <c r="AA313" s="1"/>
       <c r="AB313" s="1"/>
     </row>
-    <row r="314" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A314" s="1"/>
       <c r="B314" s="33"/>
       <c r="C314" s="73">
@@ -21790,7 +21783,7 @@
       <c r="AA314" s="1"/>
       <c r="AB314" s="1"/>
     </row>
-    <row r="315" spans="1:28" s="97" customFormat="1" ht="28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:28" s="97" customFormat="1" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A315" s="1"/>
       <c r="B315" s="33"/>
       <c r="C315" s="73">
@@ -21833,7 +21826,7 @@
       <c r="AA315" s="1"/>
       <c r="AB315" s="1"/>
     </row>
-    <row r="316" spans="1:28" s="97" customFormat="1" ht="11.5" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:28" s="97" customFormat="1" ht="11.45" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A316" s="1"/>
       <c r="B316" s="33" t="s">
         <v>20</v>
@@ -21874,7 +21867,7 @@
       <c r="AA316" s="1"/>
       <c r="AB316" s="1"/>
     </row>
-    <row r="317" spans="1:28" s="97" customFormat="1" ht="13" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:28" s="97" customFormat="1" ht="12.95" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A317" s="1"/>
       <c r="B317" s="33"/>
       <c r="C317" s="73">
@@ -21907,7 +21900,7 @@
       <c r="AA317" s="1"/>
       <c r="AB317" s="1"/>
     </row>
-    <row r="318" spans="1:28" s="97" customFormat="1" ht="8.5" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:28" s="97" customFormat="1" ht="8.4499999999999993" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A318" s="1"/>
       <c r="B318" s="33" t="s">
         <v>19</v>
@@ -21944,7 +21937,7 @@
       <c r="AA318" s="1"/>
       <c r="AB318" s="1"/>
     </row>
-    <row r="319" spans="1:28" s="97" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:28" s="97" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A319" s="1"/>
       <c r="B319" s="33"/>
       <c r="C319" s="73">
@@ -21979,7 +21972,7 @@
       <c r="AA319" s="1"/>
       <c r="AB319" s="1"/>
     </row>
-    <row r="320" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A320" s="1"/>
       <c r="B320" s="33"/>
       <c r="C320" s="73">
@@ -22000,7 +21993,7 @@
       <c r="K320" s="2"/>
       <c r="L320" s="125">
         <f>i_w_start_len1*i_n1_len^L323</f>
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="M320" s="2"/>
       <c r="N320" s="120" t="s">
@@ -22011,7 +22004,7 @@
       </c>
       <c r="P320" s="125">
         <f>i_w_start_len3*i_n3_len^P323</f>
-        <v>24</v>
+        <v>81</v>
       </c>
       <c r="Q320" s="2"/>
       <c r="R320" s="2"/>
@@ -22026,7 +22019,7 @@
       <c r="AA320" s="1"/>
       <c r="AB320" s="1"/>
     </row>
-    <row r="321" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A321" s="1"/>
       <c r="B321" s="33"/>
       <c r="C321" s="73"/>
@@ -22065,7 +22058,7 @@
       <c r="AA321" s="1"/>
       <c r="AB321" s="1"/>
     </row>
-    <row r="322" spans="1:28" s="97" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:28" s="97" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A322" s="1"/>
       <c r="B322" s="33"/>
       <c r="C322" s="73">
@@ -22085,13 +22078,13 @@
       </c>
       <c r="K322" s="119"/>
       <c r="L322" s="31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M322" s="119"/>
       <c r="N322" s="2"/>
       <c r="O322" s="2"/>
       <c r="P322" s="31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q322" s="119"/>
       <c r="R322" s="119"/>
@@ -22106,7 +22099,7 @@
       <c r="AA322" s="1"/>
       <c r="AB322" s="1"/>
     </row>
-    <row r="323" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A323" s="1"/>
       <c r="B323" s="33"/>
       <c r="C323" s="73"/>
@@ -22148,7 +22141,7 @@
       <c r="AA323" s="1"/>
       <c r="AB323" s="1"/>
     </row>
-    <row r="324" spans="1:28" s="97" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:28" s="97" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A324" s="1"/>
       <c r="B324" s="33"/>
       <c r="C324" s="73">
@@ -22191,7 +22184,7 @@
       <c r="AA324" s="1"/>
       <c r="AB324" s="1"/>
     </row>
-    <row r="325" spans="1:28" s="105" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:28" s="105" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A325" s="1"/>
       <c r="B325" s="33"/>
       <c r="C325" s="73">
@@ -22234,7 +22227,7 @@
       <c r="AA325" s="1"/>
       <c r="AB325" s="1"/>
     </row>
-    <row r="326" spans="1:28" s="124" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:28" s="124" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A326" s="1"/>
       <c r="B326" s="33"/>
       <c r="C326" s="73">
@@ -22275,7 +22268,7 @@
       <c r="AA326" s="1"/>
       <c r="AB326" s="1"/>
     </row>
-    <row r="327" spans="1:28" s="97" customFormat="1" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:28" s="97" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A327" s="1"/>
       <c r="B327" s="33"/>
       <c r="C327" s="73">
@@ -22310,7 +22303,7 @@
       <c r="AA327" s="1"/>
       <c r="AB327" s="1"/>
     </row>
-    <row r="328" spans="1:28" s="147" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:28" s="147" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A328" s="1"/>
       <c r="B328" s="33"/>
       <c r="C328" s="73">
@@ -22345,7 +22338,7 @@
       <c r="AA328" s="1"/>
       <c r="AB328" s="1"/>
     </row>
-    <row r="329" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A329" s="1"/>
       <c r="B329" s="33"/>
       <c r="C329" s="73">
@@ -22380,7 +22373,7 @@
       <c r="AA329" s="1"/>
       <c r="AB329" s="1"/>
     </row>
-    <row r="330" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A330" s="1"/>
       <c r="B330" s="33"/>
       <c r="C330" s="73">
@@ -22425,7 +22418,7 @@
       <c r="AA330" s="1"/>
       <c r="AB330" s="1"/>
     </row>
-    <row r="331" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A331" s="1"/>
       <c r="B331" s="33"/>
       <c r="C331" s="73">
@@ -22472,7 +22465,7 @@
       <c r="AA331" s="1"/>
       <c r="AB331" s="1"/>
     </row>
-    <row r="332" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A332" s="1"/>
       <c r="B332" s="33"/>
       <c r="C332" s="73">
@@ -22524,7 +22517,7 @@
       <c r="AA332" s="1"/>
       <c r="AB332" s="1"/>
     </row>
-    <row r="333" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A333" s="1"/>
       <c r="B333" s="33"/>
       <c r="C333" s="73"/>
@@ -22574,7 +22567,7 @@
       <c r="AA333" s="1"/>
       <c r="AB333" s="1"/>
     </row>
-    <row r="334" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A334" s="1"/>
       <c r="B334" s="33"/>
       <c r="C334" s="73">
@@ -22623,7 +22616,7 @@
       <c r="AA334" s="1"/>
       <c r="AB334" s="1"/>
     </row>
-    <row r="335" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A335" s="1"/>
       <c r="B335" s="33"/>
       <c r="C335" s="73"/>
@@ -22667,7 +22660,7 @@
       <c r="AA335" s="1"/>
       <c r="AB335" s="1"/>
     </row>
-    <row r="336" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A336" s="1"/>
       <c r="B336" s="33"/>
       <c r="C336" s="73">
@@ -22706,7 +22699,7 @@
       <c r="AA336" s="1"/>
       <c r="AB336" s="1"/>
     </row>
-    <row r="337" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A337" s="1"/>
       <c r="B337" s="33"/>
       <c r="C337" s="73">
@@ -22745,7 +22738,7 @@
       <c r="AA337" s="1"/>
       <c r="AB337" s="1"/>
     </row>
-    <row r="338" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A338" s="1"/>
       <c r="B338" s="33"/>
       <c r="C338" s="73">
@@ -22786,7 +22779,7 @@
       <c r="AA338" s="1"/>
       <c r="AB338" s="1"/>
     </row>
-    <row r="339" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A339" s="1"/>
       <c r="B339" s="33"/>
       <c r="C339" s="73"/>
@@ -22827,7 +22820,7 @@
       <c r="AA339" s="1"/>
       <c r="AB339" s="1"/>
     </row>
-    <row r="340" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A340" s="1"/>
       <c r="B340" s="33"/>
       <c r="C340" s="73"/>
@@ -22857,7 +22850,7 @@
       <c r="AA340" s="1"/>
       <c r="AB340" s="1"/>
     </row>
-    <row r="341" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A341" s="1"/>
       <c r="B341" s="33"/>
       <c r="C341" s="73">
@@ -22892,7 +22885,7 @@
       <c r="AA341" s="1"/>
       <c r="AB341" s="1"/>
     </row>
-    <row r="342" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A342" s="1"/>
       <c r="B342" s="33"/>
       <c r="C342" s="73">
@@ -22933,7 +22926,7 @@
       <c r="AA342" s="1"/>
       <c r="AB342" s="1"/>
     </row>
-    <row r="343" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A343" s="1"/>
       <c r="B343" s="33"/>
       <c r="C343" s="73">
@@ -22976,7 +22969,7 @@
       <c r="AA343" s="1"/>
       <c r="AB343" s="1"/>
     </row>
-    <row r="344" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A344" s="1"/>
       <c r="B344" s="33"/>
       <c r="C344" s="73">
@@ -23024,7 +23017,7 @@
       <c r="AA344" s="1"/>
       <c r="AB344" s="1"/>
     </row>
-    <row r="345" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A345" s="1"/>
       <c r="B345" s="33"/>
       <c r="C345" s="73"/>
@@ -23068,7 +23061,7 @@
       <c r="AA345" s="1"/>
       <c r="AB345" s="1"/>
     </row>
-    <row r="346" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A346" s="1"/>
       <c r="B346" s="33"/>
       <c r="C346" s="73">
@@ -23113,7 +23106,7 @@
       <c r="AA346" s="1"/>
       <c r="AB346" s="1"/>
     </row>
-    <row r="347" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A347" s="1"/>
       <c r="B347" s="33"/>
       <c r="C347" s="73">
@@ -23146,7 +23139,7 @@
       <c r="AA347" s="1"/>
       <c r="AB347" s="1"/>
     </row>
-    <row r="348" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A348" s="1"/>
       <c r="B348" s="33"/>
       <c r="C348" s="73">
@@ -23181,7 +23174,7 @@
       <c r="AA348" s="1"/>
       <c r="AB348" s="1"/>
     </row>
-    <row r="349" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A349" s="1"/>
       <c r="B349" s="33"/>
       <c r="C349" s="73">
@@ -23216,7 +23209,7 @@
       <c r="AA349" s="1"/>
       <c r="AB349" s="1"/>
     </row>
-    <row r="350" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A350" s="1"/>
       <c r="B350" s="33"/>
       <c r="C350" s="73">
@@ -23251,7 +23244,7 @@
       <c r="AA350" s="1"/>
       <c r="AB350" s="1"/>
     </row>
-    <row r="351" spans="1:28" s="147" customFormat="1" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:28" s="147" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A351" s="1"/>
       <c r="B351" s="33"/>
       <c r="C351" s="73">
@@ -23286,7 +23279,7 @@
       <c r="AA351" s="1"/>
       <c r="AB351" s="1"/>
     </row>
-    <row r="352" spans="1:28" s="135" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:28" s="135" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A352" s="1"/>
       <c r="B352" s="33"/>
       <c r="C352" s="73">
@@ -23319,7 +23312,7 @@
       <c r="AA352" s="1"/>
       <c r="AB352" s="1"/>
     </row>
-    <row r="353" spans="1:28" s="135" customFormat="1" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:28" s="135" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A353" s="1"/>
       <c r="B353" s="35"/>
       <c r="C353" s="76">
@@ -23354,7 +23347,7 @@
       <c r="AA353" s="1"/>
       <c r="AB353" s="1"/>
     </row>
-    <row r="354" spans="1:28" s="135" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:28" s="135" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A354" s="1"/>
       <c r="B354" s="19"/>
       <c r="C354" s="77">
@@ -23387,7 +23380,7 @@
       <c r="AA354" s="1"/>
       <c r="AB354" s="1"/>
     </row>
-    <row r="355" spans="1:28" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:28" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A355" s="1"/>
       <c r="B355" s="1"/>
       <c r="C355" s="73">
@@ -23420,7 +23413,7 @@
       <c r="AA355" s="1"/>
       <c r="AB355" s="1"/>
     </row>
-    <row r="356" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A356" s="1"/>
       <c r="B356" s="1"/>
       <c r="C356" s="66"/>
@@ -23450,7 +23443,7 @@
       <c r="AA356" s="1"/>
       <c r="AB356" s="1"/>
     </row>
-    <row r="357" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A357" s="1"/>
       <c r="B357" s="1"/>
       <c r="C357" s="66"/>
@@ -23480,7 +23473,7 @@
       <c r="AA357" s="1"/>
       <c r="AB357" s="1"/>
     </row>
-    <row r="358" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A358" s="1"/>
       <c r="B358" s="1"/>
       <c r="C358" s="66"/>
@@ -23510,7 +23503,7 @@
       <c r="AA358" s="1"/>
       <c r="AB358" s="1"/>
     </row>
-    <row r="359" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A359" s="1"/>
       <c r="B359" s="1"/>
       <c r="C359" s="66"/>
@@ -23540,7 +23533,7 @@
       <c r="AA359" s="1"/>
       <c r="AB359" s="1"/>
     </row>
-    <row r="360" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A360" s="1"/>
       <c r="B360" s="1"/>
       <c r="C360" s="66"/>
@@ -23570,7 +23563,7 @@
       <c r="AA360" s="1"/>
       <c r="AB360" s="1"/>
     </row>
-    <row r="361" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A361" s="1"/>
       <c r="B361" s="1"/>
       <c r="C361" s="66"/>
@@ -23600,7 +23593,7 @@
       <c r="AA361" s="1"/>
       <c r="AB361" s="1"/>
     </row>
-    <row r="362" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C362" s="72" t="s">
         <v>4</v>
       </c>
@@ -23630,22 +23623,22 @@
       <selection activeCell="U37" sqref="U37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" customWidth="1"/>
-    <col min="2" max="2" width="2.7265625" customWidth="1"/>
-    <col min="3" max="3" width="4.7265625" customWidth="1" outlineLevel="2"/>
-    <col min="4" max="4" width="1.7265625" customWidth="1"/>
-    <col min="5" max="6" width="9.1796875" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="1.7265625" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="15.7265625" customWidth="1"/>
-    <col min="12" max="12" width="9.1796875" customWidth="1"/>
-    <col min="26" max="26" width="1.7265625" customWidth="1"/>
-    <col min="27" max="28" width="4.7265625" customWidth="1"/>
-    <col min="30" max="30" width="46.1796875" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="4" max="4" width="1.7109375" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="1.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" customWidth="1"/>
+    <col min="26" max="26" width="1.7109375" customWidth="1"/>
+    <col min="27" max="28" width="4.7109375" customWidth="1"/>
+    <col min="30" max="30" width="46.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="66"/>
@@ -23677,7 +23670,7 @@
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
     </row>
-    <row r="2" spans="1:30" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="67">
@@ -23712,7 +23705,7 @@
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
-    <row r="3" spans="1:30" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:30" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="20"/>
       <c r="C3" s="68">
@@ -23747,7 +23740,7 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
     </row>
-    <row r="4" spans="1:30" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="34" t="s">
         <v>21</v>
@@ -23784,7 +23777,7 @@
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
     </row>
-    <row r="5" spans="1:30" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:30" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="33"/>
       <c r="C5" s="67">
@@ -23861,7 +23854,7 @@
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" spans="1:30" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="33"/>
       <c r="C6" s="67">
@@ -23901,7 +23894,7 @@
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
     </row>
-    <row r="7" spans="1:30" ht="20.149999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:30" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="33"/>
       <c r="C7" s="67">
@@ -23942,7 +23935,7 @@
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
     </row>
-    <row r="8" spans="1:30" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="33"/>
       <c r="C8" s="67">
@@ -23977,7 +23970,7 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
     </row>
-    <row r="9" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="33"/>
       <c r="C9" s="67">
@@ -24012,7 +24005,7 @@
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
     </row>
-    <row r="10" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="33"/>
       <c r="C10" s="67">
@@ -24047,7 +24040,7 @@
       <c r="AC10" s="1"/>
       <c r="AD10" s="1"/>
     </row>
-    <row r="11" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="33"/>
       <c r="C11" s="67">
@@ -24082,7 +24075,7 @@
       <c r="AC11" s="1"/>
       <c r="AD11" s="1"/>
     </row>
-    <row r="12" spans="1:30" ht="28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:30" ht="30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="33"/>
       <c r="C12" s="67">
@@ -24121,7 +24114,7 @@
       <c r="AC12" s="1"/>
       <c r="AD12" s="1"/>
     </row>
-    <row r="13" spans="1:30" ht="11.5" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:30" ht="11.45" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="33" t="s">
         <v>20</v>
@@ -24158,7 +24151,7 @@
       <c r="AC13" s="1"/>
       <c r="AD13" s="1"/>
     </row>
-    <row r="14" spans="1:30" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:30" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="33"/>
       <c r="C14" s="67">
@@ -24193,7 +24186,7 @@
       <c r="AC14" s="1"/>
       <c r="AD14" s="1"/>
     </row>
-    <row r="15" spans="1:30" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:30" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="33" t="s">
         <v>19</v>
@@ -24232,7 +24225,7 @@
       <c r="AC15" s="1"/>
       <c r="AD15" s="1"/>
     </row>
-    <row r="16" spans="1:30" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="33"/>
       <c r="C16" s="67">
@@ -24269,7 +24262,7 @@
       <c r="AC16" s="1"/>
       <c r="AD16" s="1"/>
     </row>
-    <row r="17" spans="1:30" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="33"/>
       <c r="C17" s="67">
@@ -24306,7 +24299,7 @@
       <c r="AC17" s="1"/>
       <c r="AD17" s="1"/>
     </row>
-    <row r="18" spans="1:30" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:30" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="33"/>
       <c r="C18" s="67">
@@ -24347,7 +24340,7 @@
       <c r="AC18" s="1"/>
       <c r="AD18" s="1"/>
     </row>
-    <row r="19" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="33"/>
       <c r="C19" s="67">
@@ -24382,7 +24375,7 @@
       <c r="AC19" s="1"/>
       <c r="AD19" s="1"/>
     </row>
-    <row r="20" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="33"/>
       <c r="C20" s="67">
@@ -24417,7 +24410,7 @@
       <c r="AC20" s="1"/>
       <c r="AD20" s="1"/>
     </row>
-    <row r="21" spans="1:30" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:30" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="33"/>
       <c r="C21" s="67">
@@ -24458,7 +24451,7 @@
       <c r="AC21" s="1"/>
       <c r="AD21" s="1"/>
     </row>
-    <row r="22" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="33"/>
       <c r="C22" s="67">
@@ -24493,7 +24486,7 @@
       <c r="AC22" s="1"/>
       <c r="AD22" s="1"/>
     </row>
-    <row r="23" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="33"/>
       <c r="C23" s="67">
@@ -24528,7 +24521,7 @@
       <c r="AC23" s="1"/>
       <c r="AD23" s="1"/>
     </row>
-    <row r="24" spans="1:30" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="33"/>
       <c r="C24" s="67">
@@ -24565,7 +24558,7 @@
       <c r="AC24" s="1"/>
       <c r="AD24" s="1"/>
     </row>
-    <row r="25" spans="1:30" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="33"/>
       <c r="C25" s="67">
@@ -24602,7 +24595,7 @@
       <c r="AC25" s="1"/>
       <c r="AD25" s="1"/>
     </row>
-    <row r="26" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="33"/>
       <c r="C26" s="67">
@@ -24651,7 +24644,7 @@
       <c r="AC26" s="1"/>
       <c r="AD26" s="1"/>
     </row>
-    <row r="27" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="33"/>
       <c r="C27" s="67">
@@ -24690,7 +24683,7 @@
       <c r="AC27" s="1"/>
       <c r="AD27" s="1"/>
     </row>
-    <row r="28" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="33"/>
       <c r="C28" s="67">
@@ -24729,7 +24722,7 @@
       <c r="AC28" s="1"/>
       <c r="AD28" s="1"/>
     </row>
-    <row r="29" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="33"/>
       <c r="C29" s="67">
@@ -24768,7 +24761,7 @@
       <c r="AC29" s="1"/>
       <c r="AD29" s="1"/>
     </row>
-    <row r="30" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="33"/>
       <c r="C30" s="67">
@@ -24807,7 +24800,7 @@
       <c r="AC30" s="1"/>
       <c r="AD30" s="1"/>
     </row>
-    <row r="31" spans="1:30" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="33"/>
       <c r="C31" s="67">
@@ -24844,7 +24837,7 @@
       <c r="AC31" s="1"/>
       <c r="AD31" s="1"/>
     </row>
-    <row r="32" spans="1:30" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="33"/>
       <c r="C32" s="67">
@@ -24881,7 +24874,7 @@
       <c r="AC32" s="1"/>
       <c r="AD32" s="1"/>
     </row>
-    <row r="33" spans="1:30" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:30" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="33"/>
       <c r="C33" s="67">
@@ -24942,7 +24935,7 @@
       <c r="AC33" s="1"/>
       <c r="AD33" s="1"/>
     </row>
-    <row r="34" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="33"/>
       <c r="C34" s="67">
@@ -25007,7 +25000,7 @@
       <c r="AC34" s="1"/>
       <c r="AD34" s="1"/>
     </row>
-    <row r="35" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="33"/>
       <c r="C35" s="67">
@@ -25042,7 +25035,7 @@
       <c r="AC35" s="1"/>
       <c r="AD35" s="1"/>
     </row>
-    <row r="36" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="33"/>
       <c r="C36" s="67">
@@ -25077,7 +25070,7 @@
       <c r="AC36" s="1"/>
       <c r="AD36" s="1"/>
     </row>
-    <row r="37" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="33"/>
       <c r="C37" s="67">
@@ -25112,7 +25105,7 @@
       <c r="AC37" s="1"/>
       <c r="AD37" s="1"/>
     </row>
-    <row r="38" spans="1:30" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="33"/>
       <c r="C38" s="67">
@@ -25149,7 +25142,7 @@
       <c r="AC38" s="1"/>
       <c r="AD38" s="1"/>
     </row>
-    <row r="39" spans="1:30" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="33"/>
       <c r="C39" s="67">
@@ -25184,7 +25177,7 @@
       <c r="AC39" s="1"/>
       <c r="AD39" s="1"/>
     </row>
-    <row r="40" spans="1:30" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="35"/>
       <c r="C40" s="70">
@@ -25221,7 +25214,7 @@
       <c r="AC40" s="1"/>
       <c r="AD40" s="1"/>
     </row>
-    <row r="41" spans="1:30" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:30" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="19"/>
       <c r="C41" s="71">
@@ -25256,7 +25249,7 @@
       <c r="AC41" s="1"/>
       <c r="AD41" s="1"/>
     </row>
-    <row r="42" spans="1:30" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="67">
@@ -25291,7 +25284,7 @@
       <c r="AC42" s="1"/>
       <c r="AD42" s="1"/>
     </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="66"/>
@@ -25323,7 +25316,7 @@
       <c r="AC43" s="1"/>
       <c r="AD43" s="1"/>
     </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="66"/>
@@ -25355,7 +25348,7 @@
       <c r="AC44" s="1"/>
       <c r="AD44" s="1"/>
     </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="66"/>
@@ -25387,7 +25380,7 @@
       <c r="AC45" s="1"/>
       <c r="AD45" s="1"/>
     </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="66"/>
@@ -25419,7 +25412,7 @@
       <c r="AC46" s="1"/>
       <c r="AD46" s="1"/>
     </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="66"/>
@@ -25451,7 +25444,7 @@
       <c r="AC47" s="1"/>
       <c r="AD47" s="1"/>
     </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="66"/>
@@ -25483,7 +25476,7 @@
       <c r="AC48" s="1"/>
       <c r="AD48" s="1"/>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C49" s="72" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Add comment in version control table
</commit_message>
<xml_diff>
--- a/Structural.xlsx
+++ b/Structural.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6C25F9-6D79-4BEC-9E85-EE60BA4DF9F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE59F82C-0FBC-471E-A32E-398AB8548986}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="0" yWindow="735" windowWidth="27870" windowHeight="15255" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -143,14 +143,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -641,7 +633,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Michael Young (21512438):</t>
         </r>
@@ -650,7 +642,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 dry at scanning.</t>
@@ -1200,7 +1192,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="276">
   <si>
     <t>Controls for this worksheet</t>
   </si>
@@ -2029,6 +2021,11 @@
   </si>
   <si>
     <t>is dry</t>
+  </si>
+  <si>
+    <t>30Mar21: Added inputs for % dry and number dams mated
+2: 17Jul20-Added structural inputs table
+1: 1Apr19-Created the version control table</t>
   </si>
 </sst>
 </file>
@@ -2038,7 +2035,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2235,19 +2232,6 @@
       <color rgb="FF0000FF"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="35">
@@ -3188,7 +3172,7 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="178">
+  <cellXfs count="179">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="25" xfId="3">
@@ -3636,6 +3620,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="15" fontId="1" fillId="11" borderId="1" xfId="12" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="Accent2" xfId="33" builtinId="33" customBuiltin="1"/>
@@ -4014,25 +4001,25 @@
       <selection activeCell="C43" sqref="C43:C46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" style="147" customWidth="1"/>
-    <col min="2" max="2" width="2.7265625" style="147" customWidth="1"/>
-    <col min="3" max="3" width="4.7265625" style="147" customWidth="1" outlineLevel="2"/>
-    <col min="4" max="4" width="1.7265625" style="147" customWidth="1"/>
-    <col min="5" max="6" width="9.7265625" style="147" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="1.7265625" style="147" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="37.26953125" style="147" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7265625" style="147" customWidth="1"/>
-    <col min="10" max="23" width="10.81640625" style="147" customWidth="1"/>
-    <col min="24" max="24" width="1.7265625" style="147" customWidth="1"/>
-    <col min="25" max="26" width="4.7265625" style="147" customWidth="1"/>
-    <col min="27" max="27" width="8.7265625" style="147"/>
-    <col min="28" max="28" width="46.1796875" style="147" customWidth="1"/>
-    <col min="29" max="16384" width="8.7265625" style="147"/>
+    <col min="1" max="1" width="4.7109375" style="147" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" style="147" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" style="147" customWidth="1" outlineLevel="2"/>
+    <col min="4" max="4" width="1.7109375" style="147" customWidth="1"/>
+    <col min="5" max="6" width="9.7109375" style="147" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="1.7109375" style="147" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="37.28515625" style="147" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="147" customWidth="1"/>
+    <col min="10" max="23" width="10.85546875" style="147" customWidth="1"/>
+    <col min="24" max="24" width="1.7109375" style="147" customWidth="1"/>
+    <col min="25" max="26" width="4.7109375" style="147" customWidth="1"/>
+    <col min="27" max="27" width="8.7109375" style="147"/>
+    <col min="28" max="28" width="46.140625" style="147" customWidth="1"/>
+    <col min="29" max="16384" width="8.7109375" style="147"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="66"/>
@@ -4062,7 +4049,7 @@
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
     </row>
-    <row r="2" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="67">
@@ -4095,7 +4082,7 @@
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
     </row>
-    <row r="3" spans="1:28" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:28" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="20"/>
       <c r="C3" s="68">
@@ -4128,7 +4115,7 @@
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
     </row>
-    <row r="4" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="34" t="s">
         <v>21</v>
@@ -4163,7 +4150,7 @@
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
     </row>
-    <row r="5" spans="1:28" hidden="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:28" hidden="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="33"/>
       <c r="C5" s="67">
@@ -4234,7 +4221,7 @@
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
     </row>
-    <row r="6" spans="1:28" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="33"/>
       <c r="C6" s="67">
@@ -4272,7 +4259,7 @@
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
     </row>
-    <row r="7" spans="1:28" ht="20.149999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="33"/>
       <c r="C7" s="67">
@@ -4311,7 +4298,7 @@
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
     </row>
-    <row r="8" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="33"/>
       <c r="C8" s="67">
@@ -4344,7 +4331,7 @@
       <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
     </row>
-    <row r="9" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="33"/>
       <c r="C9" s="67">
@@ -4377,7 +4364,7 @@
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
     </row>
-    <row r="10" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="33"/>
       <c r="C10" s="67">
@@ -4410,7 +4397,7 @@
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
     </row>
-    <row r="11" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="33"/>
       <c r="C11" s="67">
@@ -4443,7 +4430,7 @@
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
     </row>
-    <row r="12" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="33"/>
       <c r="C12" s="67">
@@ -4480,7 +4467,7 @@
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
     </row>
-    <row r="13" spans="1:28" ht="11.5" hidden="1" customHeight="1" outlineLevel="3" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:28" ht="11.45" hidden="1" customHeight="1" outlineLevel="3" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="33" t="s">
         <v>20</v>
@@ -4515,7 +4502,7 @@
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
     </row>
-    <row r="14" spans="1:28" hidden="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:28" hidden="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="33"/>
       <c r="C14" s="67">
@@ -4548,7 +4535,7 @@
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
     </row>
-    <row r="15" spans="1:28" hidden="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:28" hidden="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="33"/>
       <c r="C15" s="67">
@@ -4581,7 +4568,7 @@
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
     </row>
-    <row r="16" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="33" t="s">
         <v>19</v>
@@ -4618,7 +4605,7 @@
       <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>
     </row>
-    <row r="17" spans="1:28" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:28" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="33"/>
       <c r="C17" s="67">
@@ -4653,7 +4640,7 @@
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
     </row>
-    <row r="18" spans="1:28" ht="45" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:28" ht="45" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="33"/>
       <c r="C18" s="67">
@@ -4692,7 +4679,7 @@
       <c r="AA18" s="1"/>
       <c r="AB18" s="1"/>
     </row>
-    <row r="19" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="33"/>
       <c r="C19" s="67">
@@ -4725,7 +4712,7 @@
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
     </row>
-    <row r="20" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="33"/>
       <c r="C20" s="67">
@@ -4758,7 +4745,7 @@
       <c r="AA20" s="1"/>
       <c r="AB20" s="1"/>
     </row>
-    <row r="21" spans="1:28" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:28" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="33"/>
       <c r="C21" s="67">
@@ -4797,7 +4784,7 @@
       <c r="AA21" s="1"/>
       <c r="AB21" s="1"/>
     </row>
-    <row r="22" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="33"/>
       <c r="C22" s="67">
@@ -4830,7 +4817,7 @@
       <c r="AA22" s="1"/>
       <c r="AB22" s="1"/>
     </row>
-    <row r="23" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="33"/>
       <c r="C23" s="67">
@@ -4863,7 +4850,7 @@
       <c r="AA23" s="1"/>
       <c r="AB23" s="1"/>
     </row>
-    <row r="24" spans="1:28" ht="5.15" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="33"/>
       <c r="C24" s="67">
@@ -4898,7 +4885,7 @@
       <c r="AA24" s="1"/>
       <c r="AB24" s="1"/>
     </row>
-    <row r="25" spans="1:28" ht="5.15" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="33"/>
       <c r="C25" s="67">
@@ -4933,7 +4920,7 @@
       <c r="AA25" s="1"/>
       <c r="AB25" s="1"/>
     </row>
-    <row r="26" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="33"/>
       <c r="C26" s="67">
@@ -4980,7 +4967,7 @@
       <c r="AA26" s="1"/>
       <c r="AB26" s="1"/>
     </row>
-    <row r="27" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="33"/>
       <c r="C27" s="67">
@@ -5017,7 +5004,7 @@
       <c r="AA27" s="1"/>
       <c r="AB27" s="1"/>
     </row>
-    <row r="28" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="33"/>
       <c r="C28" s="67">
@@ -5054,7 +5041,7 @@
       <c r="AA28" s="1"/>
       <c r="AB28" s="1"/>
     </row>
-    <row r="29" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="33"/>
       <c r="C29" s="67">
@@ -5091,7 +5078,7 @@
       <c r="AA29" s="1"/>
       <c r="AB29" s="1"/>
     </row>
-    <row r="30" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="33"/>
       <c r="C30" s="67">
@@ -5128,7 +5115,7 @@
       <c r="AA30" s="1"/>
       <c r="AB30" s="1"/>
     </row>
-    <row r="31" spans="1:28" ht="5.15" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="33"/>
       <c r="C31" s="67">
@@ -5163,7 +5150,7 @@
       <c r="AA31" s="1"/>
       <c r="AB31" s="1"/>
     </row>
-    <row r="32" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="33"/>
       <c r="C32" s="67">
@@ -5196,7 +5183,7 @@
       <c r="AA32" s="1"/>
       <c r="AB32" s="1"/>
     </row>
-    <row r="33" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="35"/>
       <c r="C33" s="70">
@@ -5231,7 +5218,7 @@
       <c r="AA33" s="1"/>
       <c r="AB33" s="1"/>
     </row>
-    <row r="34" spans="1:28" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:28" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="19"/>
       <c r="C34" s="71">
@@ -5264,7 +5251,7 @@
       <c r="AA34" s="1"/>
       <c r="AB34" s="1"/>
     </row>
-    <row r="35" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="67">
@@ -5297,7 +5284,7 @@
       <c r="AA35" s="1"/>
       <c r="AB35" s="1"/>
     </row>
-    <row r="36" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="73">
@@ -5330,7 +5317,7 @@
       <c r="AA36" s="1"/>
       <c r="AB36" s="1"/>
     </row>
-    <row r="37" spans="1:28" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:28" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="20"/>
       <c r="C37" s="74">
@@ -5363,7 +5350,7 @@
       <c r="AA37" s="1"/>
       <c r="AB37" s="1"/>
     </row>
-    <row r="38" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="34" t="s">
         <v>21</v>
@@ -5398,7 +5385,7 @@
       <c r="AA38" s="1"/>
       <c r="AB38" s="1"/>
     </row>
-    <row r="39" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="33"/>
       <c r="C39" s="73">
@@ -5431,7 +5418,7 @@
       <c r="AA39" s="1"/>
       <c r="AB39" s="1"/>
     </row>
-    <row r="40" spans="1:28" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="33"/>
       <c r="C40" s="73">
@@ -5468,7 +5455,7 @@
       <c r="AA40" s="1"/>
       <c r="AB40" s="1"/>
     </row>
-    <row r="41" spans="1:28" ht="20.149999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:28" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="33"/>
       <c r="C41" s="73">
@@ -5507,7 +5494,7 @@
       <c r="AA41" s="1"/>
       <c r="AB41" s="1"/>
     </row>
-    <row r="42" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="33"/>
       <c r="C42" s="73">
@@ -5540,7 +5527,7 @@
       <c r="AA42" s="1"/>
       <c r="AB42" s="1"/>
     </row>
-    <row r="43" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="33"/>
       <c r="C43" s="73">
@@ -5573,7 +5560,7 @@
       <c r="AA43" s="1"/>
       <c r="AB43" s="1"/>
     </row>
-    <row r="44" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="33"/>
       <c r="C44" s="73">
@@ -5606,7 +5593,7 @@
       <c r="AA44" s="1"/>
       <c r="AB44" s="1"/>
     </row>
-    <row r="45" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="33"/>
       <c r="C45" s="73">
@@ -5639,7 +5626,7 @@
       <c r="AA45" s="1"/>
       <c r="AB45" s="1"/>
     </row>
-    <row r="46" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="33"/>
       <c r="C46" s="73">
@@ -5672,7 +5659,7 @@
       <c r="AA46" s="1"/>
       <c r="AB46" s="1"/>
     </row>
-    <row r="47" spans="1:28" ht="11.5" customHeight="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:28" ht="11.45" customHeight="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="33" t="s">
         <v>20</v>
@@ -5707,7 +5694,7 @@
       <c r="AA47" s="1"/>
       <c r="AB47" s="1"/>
     </row>
-    <row r="48" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="33"/>
       <c r="C48" s="73">
@@ -5740,7 +5727,7 @@
       <c r="AA48" s="1"/>
       <c r="AB48" s="1"/>
     </row>
-    <row r="49" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="33" t="s">
         <v>19</v>
@@ -5777,7 +5764,7 @@
       <c r="AA49" s="1"/>
       <c r="AB49" s="1"/>
     </row>
-    <row r="50" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="33"/>
       <c r="C50" s="73">
@@ -5812,7 +5799,7 @@
       <c r="AA50" s="1"/>
       <c r="AB50" s="1"/>
     </row>
-    <row r="51" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="33"/>
       <c r="C51" s="73">
@@ -5853,7 +5840,7 @@
       <c r="AA51" s="1"/>
       <c r="AB51" s="1"/>
     </row>
-    <row r="52" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="33"/>
       <c r="C52" s="73">
@@ -5886,7 +5873,7 @@
       <c r="AA52" s="1"/>
       <c r="AB52" s="1"/>
     </row>
-    <row r="53" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="33"/>
       <c r="C53" s="73">
@@ -5925,7 +5912,7 @@
       <c r="AA53" s="1"/>
       <c r="AB53" s="1"/>
     </row>
-    <row r="54" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="33"/>
       <c r="C54" s="73">
@@ -5958,7 +5945,7 @@
       <c r="AA54" s="1"/>
       <c r="AB54" s="1"/>
     </row>
-    <row r="55" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="33"/>
       <c r="C55" s="73">
@@ -5999,7 +5986,7 @@
       <c r="AA55" s="1"/>
       <c r="AB55" s="1"/>
     </row>
-    <row r="56" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="33"/>
       <c r="C56" s="73">
@@ -6040,7 +6027,7 @@
       <c r="AA56" s="1"/>
       <c r="AB56" s="1"/>
     </row>
-    <row r="57" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="33"/>
       <c r="C57" s="73">
@@ -6079,7 +6066,7 @@
       <c r="AA57" s="1"/>
       <c r="AB57" s="1"/>
     </row>
-    <row r="58" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="33"/>
       <c r="C58" s="73">
@@ -6122,7 +6109,7 @@
       <c r="AA58" s="1"/>
       <c r="AB58" s="1"/>
     </row>
-    <row r="59" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="33"/>
       <c r="C59" s="73">
@@ -6163,7 +6150,7 @@
       <c r="AA59" s="1"/>
       <c r="AB59" s="1"/>
     </row>
-    <row r="60" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="33"/>
       <c r="C60" s="73">
@@ -6196,7 +6183,7 @@
       <c r="AA60" s="1"/>
       <c r="AB60" s="1"/>
     </row>
-    <row r="61" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="33"/>
       <c r="C61" s="73">
@@ -6239,7 +6226,7 @@
       <c r="AA61" s="1"/>
       <c r="AB61" s="1"/>
     </row>
-    <row r="62" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="33"/>
       <c r="C62" s="73">
@@ -6272,7 +6259,7 @@
       <c r="AA62" s="1"/>
       <c r="AB62" s="1"/>
     </row>
-    <row r="63" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="33"/>
       <c r="C63" s="73">
@@ -6309,7 +6296,7 @@
       <c r="AA63" s="1"/>
       <c r="AB63" s="1"/>
     </row>
-    <row r="64" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="33"/>
       <c r="C64" s="73">
@@ -6342,7 +6329,7 @@
       <c r="AA64" s="1"/>
       <c r="AB64" s="1"/>
     </row>
-    <row r="65" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="33"/>
       <c r="C65" s="73">
@@ -6379,7 +6366,7 @@
       <c r="AA65" s="1"/>
       <c r="AB65" s="1"/>
     </row>
-    <row r="66" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="33"/>
       <c r="C66" s="73">
@@ -6412,7 +6399,7 @@
       <c r="AA66" s="1"/>
       <c r="AB66" s="1"/>
     </row>
-    <row r="67" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="33"/>
       <c r="C67" s="73">
@@ -6468,7 +6455,7 @@
       <c r="AS67" s="1"/>
       <c r="AT67" s="1"/>
     </row>
-    <row r="68" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="33"/>
       <c r="C68" s="73">
@@ -6532,7 +6519,7 @@
       <c r="AS68" s="1"/>
       <c r="AT68" s="1"/>
     </row>
-    <row r="69" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="33"/>
       <c r="C69" s="73">
@@ -6582,7 +6569,7 @@
       <c r="AS69" s="1"/>
       <c r="AT69" s="1"/>
     </row>
-    <row r="70" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="33"/>
       <c r="C70" s="73">
@@ -6632,7 +6619,7 @@
       <c r="AS70" s="1"/>
       <c r="AT70" s="1"/>
     </row>
-    <row r="71" spans="1:46" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:46" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="33"/>
       <c r="C71" s="73">
@@ -6667,7 +6654,7 @@
       <c r="AA71" s="1"/>
       <c r="AB71" s="1"/>
     </row>
-    <row r="72" spans="1:46" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:46" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="33"/>
       <c r="C72" s="73">
@@ -6700,7 +6687,7 @@
       <c r="AA72" s="1"/>
       <c r="AB72" s="1"/>
     </row>
-    <row r="73" spans="1:46" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:46" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="35"/>
       <c r="C73" s="76">
@@ -6735,7 +6722,7 @@
       <c r="AA73" s="1"/>
       <c r="AB73" s="1"/>
     </row>
-    <row r="74" spans="1:46" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:46" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="19"/>
       <c r="C74" s="77">
@@ -6768,7 +6755,7 @@
       <c r="AA74" s="1"/>
       <c r="AB74" s="1"/>
     </row>
-    <row r="75" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="73">
@@ -6801,7 +6788,7 @@
       <c r="AA75" s="1"/>
       <c r="AB75" s="1"/>
     </row>
-    <row r="76" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="73">
@@ -6834,7 +6821,7 @@
       <c r="AA76" s="1"/>
       <c r="AB76" s="1"/>
     </row>
-    <row r="77" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="66"/>
@@ -6864,7 +6851,7 @@
       <c r="AA77" s="1"/>
       <c r="AB77" s="1"/>
     </row>
-    <row r="78" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="66"/>
@@ -6894,7 +6881,7 @@
       <c r="AA78" s="1"/>
       <c r="AB78" s="1"/>
     </row>
-    <row r="79" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="66"/>
@@ -6924,7 +6911,7 @@
       <c r="AA79" s="1"/>
       <c r="AB79" s="1"/>
     </row>
-    <row r="80" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="66"/>
@@ -6954,7 +6941,7 @@
       <c r="AA80" s="1"/>
       <c r="AB80" s="1"/>
     </row>
-    <row r="81" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="66"/>
@@ -6984,7 +6971,7 @@
       <c r="AA81" s="1"/>
       <c r="AB81" s="1"/>
     </row>
-    <row r="82" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="66"/>
@@ -7014,7 +7001,7 @@
       <c r="AA82" s="1"/>
       <c r="AB82" s="1"/>
     </row>
-    <row r="83" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C83" s="72" t="s">
         <v>4</v>
       </c>
@@ -7038,27 +7025,27 @@
   </sheetPr>
   <dimension ref="A1:AE363"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B139" workbookViewId="0">
-      <selection activeCell="L157" sqref="L157:V157"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18:T18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" customWidth="1"/>
-    <col min="2" max="2" width="2.7265625" customWidth="1"/>
-    <col min="3" max="3" width="4.7265625" customWidth="1" outlineLevel="2"/>
-    <col min="4" max="4" width="1.7265625" customWidth="1"/>
-    <col min="5" max="6" width="9.7265625" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="1.7265625" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="37.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7265625" customWidth="1"/>
-    <col min="10" max="23" width="10.81640625" customWidth="1"/>
-    <col min="24" max="24" width="1.7265625" customWidth="1"/>
-    <col min="25" max="26" width="4.7265625" customWidth="1"/>
-    <col min="28" max="28" width="46.1796875" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="4" max="4" width="1.7109375" customWidth="1"/>
+    <col min="5" max="6" width="9.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="1.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" customWidth="1"/>
+    <col min="10" max="23" width="10.85546875" customWidth="1"/>
+    <col min="24" max="24" width="1.7109375" customWidth="1"/>
+    <col min="25" max="26" width="4.7109375" customWidth="1"/>
+    <col min="28" max="28" width="46.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="66"/>
@@ -7088,7 +7075,7 @@
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
     </row>
-    <row r="2" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="67">
@@ -7121,7 +7108,7 @@
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
     </row>
-    <row r="3" spans="1:28" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:28" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="20"/>
       <c r="C3" s="68">
@@ -7154,7 +7141,7 @@
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
     </row>
-    <row r="4" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="34" t="s">
         <v>21</v>
@@ -7189,7 +7176,7 @@
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
     </row>
-    <row r="5" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="33"/>
       <c r="C5" s="67">
@@ -7260,7 +7247,7 @@
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
     </row>
-    <row r="6" spans="1:28" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="33"/>
       <c r="C6" s="67">
@@ -7298,7 +7285,7 @@
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
     </row>
-    <row r="7" spans="1:28" ht="20.149999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="33"/>
       <c r="C7" s="67">
@@ -7337,7 +7324,7 @@
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
     </row>
-    <row r="8" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="33"/>
       <c r="C8" s="67">
@@ -7370,7 +7357,7 @@
       <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
     </row>
-    <row r="9" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="33"/>
       <c r="C9" s="67">
@@ -7403,7 +7390,7 @@
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
     </row>
-    <row r="10" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="33"/>
       <c r="C10" s="67">
@@ -7436,7 +7423,7 @@
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
     </row>
-    <row r="11" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="33"/>
       <c r="C11" s="67">
@@ -7469,7 +7456,7 @@
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
     </row>
-    <row r="12" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="33"/>
       <c r="C12" s="67">
@@ -7506,7 +7493,7 @@
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
     </row>
-    <row r="13" spans="1:28" ht="11.5" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:28" ht="11.45" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="33" t="s">
         <v>20</v>
@@ -7541,7 +7528,7 @@
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
     </row>
-    <row r="14" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="33"/>
       <c r="C14" s="67">
@@ -7574,7 +7561,7 @@
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
     </row>
-    <row r="15" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="33"/>
       <c r="C15" s="67">
@@ -7607,7 +7594,7 @@
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
     </row>
-    <row r="16" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="33" t="s">
         <v>19</v>
@@ -7644,7 +7631,7 @@
       <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>
     </row>
-    <row r="17" spans="1:28" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:28" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="33"/>
       <c r="C17" s="67">
@@ -7679,7 +7666,7 @@
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
     </row>
-    <row r="18" spans="1:28" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:28" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="33"/>
       <c r="C18" s="67">
@@ -7693,11 +7680,11 @@
       <c r="H18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I18" s="31">
-        <v>2</v>
+      <c r="I18" s="178">
+        <v>44285</v>
       </c>
       <c r="J18" s="162" t="s">
-        <v>70</v>
+        <v>275</v>
       </c>
       <c r="K18" s="163"/>
       <c r="L18" s="163"/>
@@ -7718,7 +7705,7 @@
       <c r="AA18" s="1"/>
       <c r="AB18" s="1"/>
     </row>
-    <row r="19" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="33"/>
       <c r="C19" s="67">
@@ -7751,7 +7738,7 @@
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
     </row>
-    <row r="20" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="33"/>
       <c r="C20" s="67">
@@ -7784,7 +7771,7 @@
       <c r="AA20" s="1"/>
       <c r="AB20" s="1"/>
     </row>
-    <row r="21" spans="1:28" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:28" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="33"/>
       <c r="C21" s="67">
@@ -7823,7 +7810,7 @@
       <c r="AA21" s="1"/>
       <c r="AB21" s="1"/>
     </row>
-    <row r="22" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="33"/>
       <c r="C22" s="67">
@@ -7856,7 +7843,7 @@
       <c r="AA22" s="1"/>
       <c r="AB22" s="1"/>
     </row>
-    <row r="23" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="33"/>
       <c r="C23" s="67">
@@ -7889,7 +7876,7 @@
       <c r="AA23" s="1"/>
       <c r="AB23" s="1"/>
     </row>
-    <row r="24" spans="1:28" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="33"/>
       <c r="C24" s="67">
@@ -7924,7 +7911,7 @@
       <c r="AA24" s="1"/>
       <c r="AB24" s="1"/>
     </row>
-    <row r="25" spans="1:28" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="33"/>
       <c r="C25" s="67">
@@ -7959,7 +7946,7 @@
       <c r="AA25" s="1"/>
       <c r="AB25" s="1"/>
     </row>
-    <row r="26" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="33"/>
       <c r="C26" s="67">
@@ -8006,7 +7993,7 @@
       <c r="AA26" s="1"/>
       <c r="AB26" s="1"/>
     </row>
-    <row r="27" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="33"/>
       <c r="C27" s="67">
@@ -8043,7 +8030,7 @@
       <c r="AA27" s="1"/>
       <c r="AB27" s="1"/>
     </row>
-    <row r="28" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="33"/>
       <c r="C28" s="67">
@@ -8080,7 +8067,7 @@
       <c r="AA28" s="1"/>
       <c r="AB28" s="1"/>
     </row>
-    <row r="29" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="33"/>
       <c r="C29" s="67">
@@ -8117,7 +8104,7 @@
       <c r="AA29" s="1"/>
       <c r="AB29" s="1"/>
     </row>
-    <row r="30" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="33"/>
       <c r="C30" s="67">
@@ -8154,7 +8141,7 @@
       <c r="AA30" s="1"/>
       <c r="AB30" s="1"/>
     </row>
-    <row r="31" spans="1:28" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="33"/>
       <c r="C31" s="67">
@@ -8189,7 +8176,7 @@
       <c r="AA31" s="1"/>
       <c r="AB31" s="1"/>
     </row>
-    <row r="32" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="33"/>
       <c r="C32" s="67">
@@ -8222,7 +8209,7 @@
       <c r="AA32" s="1"/>
       <c r="AB32" s="1"/>
     </row>
-    <row r="33" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="35"/>
       <c r="C33" s="70">
@@ -8257,7 +8244,7 @@
       <c r="AA33" s="1"/>
       <c r="AB33" s="1"/>
     </row>
-    <row r="34" spans="1:28" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:28" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="19"/>
       <c r="C34" s="71">
@@ -8290,7 +8277,7 @@
       <c r="AA34" s="1"/>
       <c r="AB34" s="1"/>
     </row>
-    <row r="35" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="67">
@@ -8323,7 +8310,7 @@
       <c r="AA35" s="1"/>
       <c r="AB35" s="1"/>
     </row>
-    <row r="36" spans="1:28" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:28" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="73">
@@ -8356,7 +8343,7 @@
       <c r="AA36" s="1"/>
       <c r="AB36" s="1"/>
     </row>
-    <row r="37" spans="1:28" s="135" customFormat="1" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:28" s="135" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="20"/>
       <c r="C37" s="74">
@@ -8389,7 +8376,7 @@
       <c r="AA37" s="1"/>
       <c r="AB37" s="1"/>
     </row>
-    <row r="38" spans="1:28" s="135" customFormat="1" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:28" s="135" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="34" t="s">
         <v>21</v>
@@ -8424,7 +8411,7 @@
       <c r="AA38" s="1"/>
       <c r="AB38" s="1"/>
     </row>
-    <row r="39" spans="1:28" s="135" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:28" s="135" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="33"/>
       <c r="C39" s="73">
@@ -8457,7 +8444,7 @@
       <c r="AA39" s="1"/>
       <c r="AB39" s="1"/>
     </row>
-    <row r="40" spans="1:28" s="135" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:28" s="135" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="33"/>
       <c r="C40" s="73">
@@ -8494,7 +8481,7 @@
       <c r="AA40" s="1"/>
       <c r="AB40" s="1"/>
     </row>
-    <row r="41" spans="1:28" s="135" customFormat="1" ht="20.149999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:28" s="135" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="33"/>
       <c r="C41" s="73">
@@ -8531,7 +8518,7 @@
       <c r="AA41" s="1"/>
       <c r="AB41" s="1"/>
     </row>
-    <row r="42" spans="1:28" s="135" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:28" s="135" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="33"/>
       <c r="C42" s="73">
@@ -8564,7 +8551,7 @@
       <c r="AA42" s="1"/>
       <c r="AB42" s="1"/>
     </row>
-    <row r="43" spans="1:28" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:28" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="33"/>
       <c r="C43" s="73">
@@ -8597,7 +8584,7 @@
       <c r="AA43" s="1"/>
       <c r="AB43" s="1"/>
     </row>
-    <row r="44" spans="1:28" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:28" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="33"/>
       <c r="C44" s="73">
@@ -8630,7 +8617,7 @@
       <c r="AA44" s="1"/>
       <c r="AB44" s="1"/>
     </row>
-    <row r="45" spans="1:28" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:28" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="33"/>
       <c r="C45" s="73">
@@ -8663,7 +8650,7 @@
       <c r="AA45" s="1"/>
       <c r="AB45" s="1"/>
     </row>
-    <row r="46" spans="1:28" s="135" customFormat="1" ht="28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:28" s="135" customFormat="1" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="33"/>
       <c r="C46" s="73">
@@ -8706,7 +8693,7 @@
       <c r="AA46" s="1"/>
       <c r="AB46" s="1"/>
     </row>
-    <row r="47" spans="1:28" s="135" customFormat="1" ht="11.5" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:28" s="135" customFormat="1" ht="11.45" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="33" t="s">
         <v>20</v>
@@ -8741,7 +8728,7 @@
       <c r="AA47" s="1"/>
       <c r="AB47" s="1"/>
     </row>
-    <row r="48" spans="1:28" s="135" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:28" s="135" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="33"/>
       <c r="C48" s="73">
@@ -8774,7 +8761,7 @@
       <c r="AA48" s="1"/>
       <c r="AB48" s="1"/>
     </row>
-    <row r="49" spans="1:28" s="135" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:28" s="135" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="33" t="s">
         <v>19</v>
@@ -8811,7 +8798,7 @@
       <c r="AA49" s="1"/>
       <c r="AB49" s="1"/>
     </row>
-    <row r="50" spans="1:28" s="135" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:28" s="135" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="33"/>
       <c r="C50" s="73">
@@ -8846,7 +8833,7 @@
       <c r="AA50" s="1"/>
       <c r="AB50" s="1"/>
     </row>
-    <row r="51" spans="1:28" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:28" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="33"/>
       <c r="C51" s="73">
@@ -8881,7 +8868,7 @@
       <c r="AA51" s="1"/>
       <c r="AB51" s="1"/>
     </row>
-    <row r="52" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="33"/>
       <c r="C52" s="73"/>
@@ -8915,7 +8902,7 @@
       <c r="AA52" s="1"/>
       <c r="AB52" s="1"/>
     </row>
-    <row r="53" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="33"/>
       <c r="C53" s="73"/>
@@ -8949,7 +8936,7 @@
       <c r="AA53" s="1"/>
       <c r="AB53" s="1"/>
     </row>
-    <row r="54" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="33"/>
       <c r="C54" s="73"/>
@@ -8983,7 +8970,7 @@
       <c r="AA54" s="1"/>
       <c r="AB54" s="1"/>
     </row>
-    <row r="55" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="33"/>
       <c r="C55" s="73"/>
@@ -9017,7 +9004,7 @@
       <c r="AA55" s="1"/>
       <c r="AB55" s="1"/>
     </row>
-    <row r="56" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="33"/>
       <c r="C56" s="73"/>
@@ -9051,7 +9038,7 @@
       <c r="AA56" s="1"/>
       <c r="AB56" s="1"/>
     </row>
-    <row r="57" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="33"/>
       <c r="C57" s="73"/>
@@ -9085,7 +9072,7 @@
       <c r="AA57" s="1"/>
       <c r="AB57" s="1"/>
     </row>
-    <row r="58" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="33"/>
       <c r="C58" s="73"/>
@@ -9119,7 +9106,7 @@
       <c r="AA58" s="1"/>
       <c r="AB58" s="1"/>
     </row>
-    <row r="59" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="33"/>
       <c r="C59" s="73"/>
@@ -9153,7 +9140,7 @@
       <c r="AA59" s="1"/>
       <c r="AB59" s="1"/>
     </row>
-    <row r="60" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="33"/>
       <c r="C60" s="73"/>
@@ -9187,7 +9174,7 @@
       <c r="AA60" s="1"/>
       <c r="AB60" s="1"/>
     </row>
-    <row r="61" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="33"/>
       <c r="C61" s="73"/>
@@ -9221,7 +9208,7 @@
       <c r="AA61" s="1"/>
       <c r="AB61" s="1"/>
     </row>
-    <row r="62" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="33"/>
       <c r="C62" s="73"/>
@@ -9255,7 +9242,7 @@
       <c r="AA62" s="1"/>
       <c r="AB62" s="1"/>
     </row>
-    <row r="63" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="33"/>
       <c r="C63" s="73"/>
@@ -9289,7 +9276,7 @@
       <c r="AA63" s="1"/>
       <c r="AB63" s="1"/>
     </row>
-    <row r="64" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="33"/>
       <c r="C64" s="73"/>
@@ -9323,7 +9310,7 @@
       <c r="AA64" s="1"/>
       <c r="AB64" s="1"/>
     </row>
-    <row r="65" spans="1:28" s="107" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:28" s="107" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="33"/>
       <c r="C65" s="73">
@@ -9362,7 +9349,7 @@
       <c r="AA65" s="1"/>
       <c r="AB65" s="1"/>
     </row>
-    <row r="66" spans="1:28" s="100" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:28" s="100" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="33"/>
       <c r="C66" s="73">
@@ -9399,7 +9386,7 @@
       <c r="AA66" s="1"/>
       <c r="AB66" s="1"/>
     </row>
-    <row r="67" spans="1:28" s="100" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:28" s="100" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="33"/>
       <c r="C67" s="73">
@@ -9436,7 +9423,7 @@
       <c r="AA67" s="1"/>
       <c r="AB67" s="1"/>
     </row>
-    <row r="68" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="33"/>
       <c r="C68" s="73">
@@ -9473,7 +9460,7 @@
       <c r="AA68" s="1"/>
       <c r="AB68" s="1"/>
     </row>
-    <row r="69" spans="1:28" s="138" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:28" s="138" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="33"/>
       <c r="C69" s="73">
@@ -9506,7 +9493,7 @@
       <c r="AA69" s="1"/>
       <c r="AB69" s="1"/>
     </row>
-    <row r="70" spans="1:28" s="103" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:28" s="103" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="33"/>
       <c r="C70" s="73">
@@ -9543,7 +9530,7 @@
       <c r="AA70" s="1"/>
       <c r="AB70" s="1"/>
     </row>
-    <row r="71" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="33"/>
       <c r="C71" s="73">
@@ -9584,7 +9571,7 @@
       <c r="AA71" s="1"/>
       <c r="AB71" s="1"/>
     </row>
-    <row r="72" spans="1:28" s="146" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:28" s="146" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="33"/>
       <c r="C72" s="73">
@@ -9625,7 +9612,7 @@
       <c r="AA72" s="1"/>
       <c r="AB72" s="1"/>
     </row>
-    <row r="73" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="33"/>
       <c r="C73" s="73"/>
@@ -9655,7 +9642,7 @@
       <c r="AA73" s="1"/>
       <c r="AB73" s="1"/>
     </row>
-    <row r="74" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="33"/>
       <c r="C74" s="73"/>
@@ -9691,7 +9678,7 @@
       <c r="AA74" s="1"/>
       <c r="AB74" s="1"/>
     </row>
-    <row r="75" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="33"/>
       <c r="C75" s="73"/>
@@ -9721,7 +9708,7 @@
       <c r="AA75" s="1"/>
       <c r="AB75" s="1"/>
     </row>
-    <row r="76" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="33"/>
       <c r="C76" s="73">
@@ -9756,7 +9743,7 @@
       <c r="AA76" s="1"/>
       <c r="AB76" s="1"/>
     </row>
-    <row r="77" spans="1:28" s="97" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:28" s="97" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="33"/>
       <c r="C77" s="73">
@@ -9797,7 +9784,7 @@
       <c r="AA77" s="1"/>
       <c r="AB77" s="1"/>
     </row>
-    <row r="78" spans="1:28" s="97" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:28" s="97" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="33"/>
       <c r="C78" s="73">
@@ -9838,7 +9825,7 @@
       <c r="AA78" s="1"/>
       <c r="AB78" s="1"/>
     </row>
-    <row r="79" spans="1:28" s="97" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:28" s="97" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="33"/>
       <c r="C79" s="73">
@@ -9871,7 +9858,7 @@
       <c r="AA79" s="1"/>
       <c r="AB79" s="1"/>
     </row>
-    <row r="80" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="33"/>
       <c r="C80" s="73">
@@ -9908,7 +9895,7 @@
       <c r="AA80" s="1"/>
       <c r="AB80" s="1"/>
     </row>
-    <row r="81" spans="1:28" s="144" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:28" s="144" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="33"/>
       <c r="C81" s="73">
@@ -9941,7 +9928,7 @@
       <c r="AA81" s="1"/>
       <c r="AB81" s="1"/>
     </row>
-    <row r="82" spans="1:28" s="97" customFormat="1" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:28" s="97" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="33"/>
       <c r="C82" s="73">
@@ -9976,7 +9963,7 @@
       <c r="AA82" s="1"/>
       <c r="AB82" s="1"/>
     </row>
-    <row r="83" spans="1:28" s="97" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:28" s="97" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="33"/>
       <c r="C83" s="73">
@@ -10009,7 +9996,7 @@
       <c r="AA83" s="1"/>
       <c r="AB83" s="1"/>
     </row>
-    <row r="84" spans="1:28" s="97" customFormat="1" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:28" s="97" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="35"/>
       <c r="C84" s="76">
@@ -10044,7 +10031,7 @@
       <c r="AA84" s="1"/>
       <c r="AB84" s="1"/>
     </row>
-    <row r="85" spans="1:28" s="97" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:28" s="97" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="19"/>
       <c r="C85" s="77">
@@ -10077,7 +10064,7 @@
       <c r="AA85" s="1"/>
       <c r="AB85" s="1"/>
     </row>
-    <row r="86" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="73">
@@ -10110,7 +10097,7 @@
       <c r="AA86" s="1"/>
       <c r="AB86" s="1"/>
     </row>
-    <row r="87" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="73">
@@ -10143,7 +10130,7 @@
       <c r="AA87" s="1"/>
       <c r="AB87" s="1"/>
     </row>
-    <row r="88" spans="1:28" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:28" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="1"/>
       <c r="B88" s="20"/>
       <c r="C88" s="74">
@@ -10176,7 +10163,7 @@
       <c r="AA88" s="1"/>
       <c r="AB88" s="1"/>
     </row>
-    <row r="89" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="34" t="s">
         <v>21</v>
@@ -10211,7 +10198,7 @@
       <c r="AA89" s="1"/>
       <c r="AB89" s="1"/>
     </row>
-    <row r="90" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="33"/>
       <c r="C90" s="73">
@@ -10244,7 +10231,7 @@
       <c r="AA90" s="1"/>
       <c r="AB90" s="1"/>
     </row>
-    <row r="91" spans="1:28" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="33"/>
       <c r="C91" s="73">
@@ -10281,7 +10268,7 @@
       <c r="AA91" s="1"/>
       <c r="AB91" s="1"/>
     </row>
-    <row r="92" spans="1:28" ht="20.149999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:28" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="33"/>
       <c r="C92" s="73">
@@ -10318,7 +10305,7 @@
       <c r="AA92" s="1"/>
       <c r="AB92" s="1"/>
     </row>
-    <row r="93" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="33"/>
       <c r="C93" s="73">
@@ -10351,7 +10338,7 @@
       <c r="AA93" s="1"/>
       <c r="AB93" s="1"/>
     </row>
-    <row r="94" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="33"/>
       <c r="C94" s="73">
@@ -10384,7 +10371,7 @@
       <c r="AA94" s="1"/>
       <c r="AB94" s="1"/>
     </row>
-    <row r="95" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="33"/>
       <c r="C95" s="73">
@@ -10417,7 +10404,7 @@
       <c r="AA95" s="1"/>
       <c r="AB95" s="1"/>
     </row>
-    <row r="96" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="33"/>
       <c r="C96" s="73">
@@ -10456,7 +10443,7 @@
       <c r="AA96" s="1"/>
       <c r="AB96" s="1"/>
     </row>
-    <row r="97" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="33"/>
       <c r="C97" s="73">
@@ -10505,7 +10492,7 @@
       <c r="AA97" s="1"/>
       <c r="AB97" s="1"/>
     </row>
-    <row r="98" spans="1:28" ht="11.5" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:28" ht="11.45" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="33" t="s">
         <v>20</v>
@@ -10540,7 +10527,7 @@
       <c r="AA98" s="1"/>
       <c r="AB98" s="1"/>
     </row>
-    <row r="99" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="33"/>
       <c r="C99" s="73">
@@ -10573,7 +10560,7 @@
       <c r="AA99" s="1"/>
       <c r="AB99" s="1"/>
     </row>
-    <row r="100" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="33" t="s">
         <v>19</v>
@@ -10610,7 +10597,7 @@
       <c r="AA100" s="1"/>
       <c r="AB100" s="1"/>
     </row>
-    <row r="101" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="33"/>
       <c r="C101" s="73">
@@ -10645,7 +10632,7 @@
       <c r="AA101" s="1"/>
       <c r="AB101" s="1"/>
     </row>
-    <row r="102" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="33"/>
       <c r="C102" s="73">
@@ -10698,7 +10685,7 @@
       <c r="AA102" s="1"/>
       <c r="AB102" s="1"/>
     </row>
-    <row r="103" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="33"/>
       <c r="C103" s="73">
@@ -10749,7 +10736,7 @@
       <c r="AA103" s="1"/>
       <c r="AB103" s="1"/>
     </row>
-    <row r="104" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="33"/>
       <c r="C104" s="73">
@@ -10800,7 +10787,7 @@
       <c r="AA104" s="1"/>
       <c r="AB104" s="1"/>
     </row>
-    <row r="105" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="33"/>
       <c r="C105" s="73">
@@ -10833,7 +10820,7 @@
       <c r="AA105" s="1"/>
       <c r="AB105" s="1"/>
     </row>
-    <row r="106" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="33"/>
       <c r="C106" s="73">
@@ -10884,7 +10871,7 @@
       <c r="AA106" s="1"/>
       <c r="AB106" s="1"/>
     </row>
-    <row r="107" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="33"/>
       <c r="C107" s="73">
@@ -10933,7 +10920,7 @@
       <c r="AA107" s="1"/>
       <c r="AB107" s="1"/>
     </row>
-    <row r="108" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="33"/>
       <c r="C108" s="73">
@@ -10982,7 +10969,7 @@
       <c r="AA108" s="1"/>
       <c r="AB108" s="1"/>
     </row>
-    <row r="109" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="33"/>
       <c r="C109" s="73">
@@ -11031,7 +11018,7 @@
       <c r="AA109" s="1"/>
       <c r="AB109" s="1"/>
     </row>
-    <row r="110" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="33"/>
       <c r="C110" s="73">
@@ -11064,7 +11051,7 @@
       <c r="AA110" s="1"/>
       <c r="AB110" s="1"/>
     </row>
-    <row r="111" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111" s="33"/>
       <c r="C111" s="73">
@@ -11115,7 +11102,7 @@
       <c r="AA111" s="1"/>
       <c r="AB111" s="1"/>
     </row>
-    <row r="112" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="33"/>
       <c r="C112" s="73">
@@ -11164,7 +11151,7 @@
       <c r="AA112" s="1"/>
       <c r="AB112" s="1"/>
     </row>
-    <row r="113" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="33"/>
       <c r="C113" s="73">
@@ -11213,7 +11200,7 @@
       <c r="AA113" s="1"/>
       <c r="AB113" s="1"/>
     </row>
-    <row r="114" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="33"/>
       <c r="C114" s="73">
@@ -11262,7 +11249,7 @@
       <c r="AA114" s="1"/>
       <c r="AB114" s="1"/>
     </row>
-    <row r="115" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="33"/>
       <c r="C115" s="73">
@@ -11295,7 +11282,7 @@
       <c r="AA115" s="1"/>
       <c r="AB115" s="1"/>
     </row>
-    <row r="116" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="33"/>
       <c r="C116" s="73">
@@ -11346,7 +11333,7 @@
       <c r="AA116" s="1"/>
       <c r="AB116" s="1"/>
     </row>
-    <row r="117" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="33"/>
       <c r="C117" s="73">
@@ -11395,7 +11382,7 @@
       <c r="AA117" s="1"/>
       <c r="AB117" s="1"/>
     </row>
-    <row r="118" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="33"/>
       <c r="C118" s="73">
@@ -11444,7 +11431,7 @@
       <c r="AA118" s="1"/>
       <c r="AB118" s="1"/>
     </row>
-    <row r="119" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="33"/>
       <c r="C119" s="73">
@@ -11493,7 +11480,7 @@
       <c r="AA119" s="1"/>
       <c r="AB119" s="1"/>
     </row>
-    <row r="120" spans="1:28" s="143" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:28" s="143" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="33"/>
       <c r="C120" s="73">
@@ -11526,7 +11513,7 @@
       <c r="AA120" s="1"/>
       <c r="AB120" s="1"/>
     </row>
-    <row r="121" spans="1:28" s="143" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:28" s="143" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="33"/>
       <c r="C121" s="73">
@@ -11561,7 +11548,7 @@
       <c r="AA121" s="1"/>
       <c r="AB121" s="1"/>
     </row>
-    <row r="122" spans="1:28" s="143" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:28" s="143" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="33"/>
       <c r="C122" s="73">
@@ -11602,7 +11589,7 @@
       <c r="AA122" s="1"/>
       <c r="AB122" s="1"/>
     </row>
-    <row r="123" spans="1:28" s="143" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:28" s="143" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
       <c r="B123" s="33"/>
       <c r="C123" s="73">
@@ -11650,7 +11637,7 @@
       <c r="AA123" s="1"/>
       <c r="AB123" s="1"/>
     </row>
-    <row r="124" spans="1:28" s="143" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:28" s="143" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
       <c r="B124" s="33"/>
       <c r="C124" s="73">
@@ -11696,7 +11683,7 @@
       <c r="AA124" s="1"/>
       <c r="AB124" s="1"/>
     </row>
-    <row r="125" spans="1:28" s="143" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:28" s="143" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="B125" s="33"/>
       <c r="C125" s="73">
@@ -11739,7 +11726,7 @@
       <c r="AA125" s="1"/>
       <c r="AB125" s="1"/>
     </row>
-    <row r="126" spans="1:28" s="143" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:28" s="143" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
       <c r="B126" s="33"/>
       <c r="C126" s="73">
@@ -11772,7 +11759,7 @@
       <c r="AA126" s="1"/>
       <c r="AB126" s="1"/>
     </row>
-    <row r="127" spans="1:28" s="143" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:28" s="143" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="B127" s="33"/>
       <c r="C127" s="73">
@@ -11819,7 +11806,7 @@
       <c r="AA127" s="1"/>
       <c r="AB127" s="1"/>
     </row>
-    <row r="128" spans="1:28" s="143" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:28" s="143" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
       <c r="B128" s="33"/>
       <c r="C128" s="73">
@@ -11864,7 +11851,7 @@
       <c r="AA128" s="1"/>
       <c r="AB128" s="1"/>
     </row>
-    <row r="129" spans="1:28" s="143" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:28" s="143" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
       <c r="B129" s="33"/>
       <c r="C129" s="73">
@@ -11907,7 +11894,7 @@
       <c r="AA129" s="1"/>
       <c r="AB129" s="1"/>
     </row>
-    <row r="130" spans="1:28" s="143" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:28" s="143" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="B130" s="33"/>
       <c r="C130" s="73">
@@ -11940,7 +11927,7 @@
       <c r="AA130" s="1"/>
       <c r="AB130" s="1"/>
     </row>
-    <row r="131" spans="1:28" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131" s="33"/>
       <c r="C131" s="73">
@@ -11975,7 +11962,7 @@
       <c r="AA131" s="1"/>
       <c r="AB131" s="1"/>
     </row>
-    <row r="132" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="33"/>
       <c r="C132" s="73">
@@ -12008,7 +11995,7 @@
       <c r="AA132" s="1"/>
       <c r="AB132" s="1"/>
     </row>
-    <row r="133" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" s="35"/>
       <c r="C133" s="76">
@@ -12043,7 +12030,7 @@
       <c r="AA133" s="1"/>
       <c r="AB133" s="1"/>
     </row>
-    <row r="134" spans="1:28" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:28" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134" s="19"/>
       <c r="C134" s="77">
@@ -12076,7 +12063,7 @@
       <c r="AA134" s="1"/>
       <c r="AB134" s="1"/>
     </row>
-    <row r="135" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="73">
@@ -12109,7 +12096,7 @@
       <c r="AA135" s="1"/>
       <c r="AB135" s="1"/>
     </row>
-    <row r="136" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="73">
@@ -12142,7 +12129,7 @@
       <c r="AA136" s="1"/>
       <c r="AB136" s="1"/>
     </row>
-    <row r="137" spans="1:28" s="95" customFormat="1" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:28" s="95" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="1"/>
       <c r="B137" s="20"/>
       <c r="C137" s="74">
@@ -12175,7 +12162,7 @@
       <c r="AA137" s="1"/>
       <c r="AB137" s="1"/>
     </row>
-    <row r="138" spans="1:28" s="95" customFormat="1" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:28" s="95" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
       <c r="B138" s="34" t="s">
         <v>21</v>
@@ -12210,7 +12197,7 @@
       <c r="AA138" s="1"/>
       <c r="AB138" s="1"/>
     </row>
-    <row r="139" spans="1:28" s="95" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:28" s="95" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
       <c r="B139" s="33"/>
       <c r="C139" s="73">
@@ -12243,7 +12230,7 @@
       <c r="AA139" s="1"/>
       <c r="AB139" s="1"/>
     </row>
-    <row r="140" spans="1:28" s="95" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:28" s="95" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
       <c r="B140" s="33"/>
       <c r="C140" s="73">
@@ -12280,7 +12267,7 @@
       <c r="AA140" s="1"/>
       <c r="AB140" s="1"/>
     </row>
-    <row r="141" spans="1:28" s="95" customFormat="1" ht="20.149999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:28" s="95" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
       <c r="B141" s="33"/>
       <c r="C141" s="73">
@@ -12317,7 +12304,7 @@
       <c r="AA141" s="1"/>
       <c r="AB141" s="1"/>
     </row>
-    <row r="142" spans="1:28" s="95" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:28" s="95" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
       <c r="B142" s="33"/>
       <c r="C142" s="73">
@@ -12350,7 +12337,7 @@
       <c r="AA142" s="1"/>
       <c r="AB142" s="1"/>
     </row>
-    <row r="143" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
       <c r="B143" s="33"/>
       <c r="C143" s="73">
@@ -12383,7 +12370,7 @@
       <c r="AA143" s="1"/>
       <c r="AB143" s="1"/>
     </row>
-    <row r="144" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
       <c r="B144" s="33"/>
       <c r="C144" s="73">
@@ -12418,7 +12405,7 @@
       <c r="AA144" s="1"/>
       <c r="AB144" s="1"/>
     </row>
-    <row r="145" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
       <c r="B145" s="33"/>
       <c r="C145" s="73">
@@ -12453,7 +12440,7 @@
       <c r="AA145" s="1"/>
       <c r="AB145" s="1"/>
     </row>
-    <row r="146" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
       <c r="B146" s="33"/>
       <c r="C146" s="73">
@@ -12508,7 +12495,7 @@
       <c r="AA146" s="1"/>
       <c r="AB146" s="1"/>
     </row>
-    <row r="147" spans="1:28" s="95" customFormat="1" ht="11.5" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:28" s="95" customFormat="1" ht="11.45" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
       <c r="B147" s="33" t="s">
         <v>20</v>
@@ -12543,7 +12530,7 @@
       <c r="AA147" s="1"/>
       <c r="AB147" s="1"/>
     </row>
-    <row r="148" spans="1:28" s="95" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:28" s="95" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
       <c r="B148" s="33"/>
       <c r="C148" s="73">
@@ -12598,7 +12585,7 @@
       <c r="AA148" s="1"/>
       <c r="AB148" s="1"/>
     </row>
-    <row r="149" spans="1:28" s="95" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:28" s="95" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
       <c r="B149" s="33" t="s">
         <v>19</v>
@@ -12635,7 +12622,7 @@
       <c r="AA149" s="1"/>
       <c r="AB149" s="1"/>
     </row>
-    <row r="150" spans="1:28" s="95" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:28" s="95" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
       <c r="B150" s="33"/>
       <c r="C150" s="73">
@@ -12670,7 +12657,7 @@
       <c r="AA150" s="1"/>
       <c r="AB150" s="1"/>
     </row>
-    <row r="151" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
       <c r="B151" s="33"/>
       <c r="C151" s="73">
@@ -12705,7 +12692,7 @@
       <c r="AA151" s="1"/>
       <c r="AB151" s="1"/>
     </row>
-    <row r="152" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
       <c r="B152" s="33"/>
       <c r="C152" s="73">
@@ -12744,7 +12731,7 @@
       <c r="AA152" s="1"/>
       <c r="AB152" s="1"/>
     </row>
-    <row r="153" spans="1:28" s="95" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:28" s="95" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A153" s="1"/>
       <c r="B153" s="33"/>
       <c r="C153" s="73">
@@ -12803,7 +12790,7 @@
       <c r="AA153" s="1"/>
       <c r="AB153" s="1"/>
     </row>
-    <row r="154" spans="1:28" s="95" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:28" s="95" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A154" s="1"/>
       <c r="B154" s="33"/>
       <c r="C154" s="73">
@@ -12860,7 +12847,7 @@
       <c r="AA154" s="1"/>
       <c r="AB154" s="1"/>
     </row>
-    <row r="155" spans="1:28" s="95" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:28" s="95" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
       <c r="B155" s="33"/>
       <c r="C155" s="73">
@@ -12897,7 +12884,7 @@
       <c r="AA155" s="1"/>
       <c r="AB155" s="1"/>
     </row>
-    <row r="156" spans="1:28" s="95" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:28" s="95" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A156" s="1"/>
       <c r="B156" s="33"/>
       <c r="C156" s="73">
@@ -12954,7 +12941,7 @@
       <c r="AA156" s="1"/>
       <c r="AB156" s="1"/>
     </row>
-    <row r="157" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
       <c r="B157" s="33"/>
       <c r="C157" s="73">
@@ -13011,7 +12998,7 @@
       <c r="AA157" s="1"/>
       <c r="AB157" s="1"/>
     </row>
-    <row r="158" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
       <c r="B158" s="33"/>
       <c r="C158" s="73">
@@ -13068,7 +13055,7 @@
       <c r="AA158" s="1"/>
       <c r="AB158" s="1"/>
     </row>
-    <row r="159" spans="1:28" s="118" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:28" s="118" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A159" s="1"/>
       <c r="B159" s="33"/>
       <c r="C159" s="73">
@@ -13125,7 +13112,7 @@
       <c r="AA159" s="1"/>
       <c r="AB159" s="1"/>
     </row>
-    <row r="160" spans="1:28" s="118" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:28" s="118" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
       <c r="B160" s="33"/>
       <c r="C160" s="73">
@@ -13182,7 +13169,7 @@
       <c r="AA160" s="1"/>
       <c r="AB160" s="1"/>
     </row>
-    <row r="161" spans="1:31" s="95" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:31" s="95" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A161" s="1"/>
       <c r="B161" s="33"/>
       <c r="C161" s="73">
@@ -13239,7 +13226,7 @@
       <c r="AA161" s="1"/>
       <c r="AB161" s="1"/>
     </row>
-    <row r="162" spans="1:31" s="95" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:31" s="95" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A162" s="1"/>
       <c r="B162" s="33"/>
       <c r="C162" s="73">
@@ -13296,7 +13283,7 @@
       <c r="AA162" s="1"/>
       <c r="AB162" s="1"/>
     </row>
-    <row r="163" spans="1:31" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:31" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A163" s="1"/>
       <c r="B163" s="33"/>
       <c r="C163" s="73">
@@ -13356,7 +13343,7 @@
       <c r="AD163" s="123"/>
       <c r="AE163" s="123"/>
     </row>
-    <row r="164" spans="1:31" s="139" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:31" s="139" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A164" s="1"/>
       <c r="B164" s="33"/>
       <c r="C164" s="73">
@@ -13413,7 +13400,7 @@
       <c r="AA164" s="1"/>
       <c r="AB164" s="1"/>
     </row>
-    <row r="165" spans="1:31" s="107" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:31" s="107" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A165" s="1"/>
       <c r="B165" s="33"/>
       <c r="C165" s="73">
@@ -13449,7 +13436,7 @@
       <c r="AD165" s="123"/>
       <c r="AE165" s="123"/>
     </row>
-    <row r="166" spans="1:31" s="107" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:31" s="107" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1"/>
       <c r="B166" s="33"/>
       <c r="C166" s="73">
@@ -13512,7 +13499,7 @@
       <c r="AD166" s="123"/>
       <c r="AE166" s="123"/>
     </row>
-    <row r="167" spans="1:31" s="107" customFormat="1" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:31" s="107" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A167" s="1"/>
       <c r="B167" s="33"/>
       <c r="C167" s="73">
@@ -13550,7 +13537,7 @@
       <c r="AD167" s="123"/>
       <c r="AE167" s="123"/>
     </row>
-    <row r="168" spans="1:31" s="106" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:31" s="106" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A168" s="1"/>
       <c r="B168" s="33"/>
       <c r="C168" s="73">
@@ -13604,7 +13591,7 @@
       <c r="AD168" s="123"/>
       <c r="AE168" s="123"/>
     </row>
-    <row r="169" spans="1:31" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:31" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A169" s="1"/>
       <c r="B169" s="33"/>
       <c r="C169" s="73">
@@ -13667,7 +13654,7 @@
       <c r="AA169" s="1"/>
       <c r="AB169" s="1"/>
     </row>
-    <row r="170" spans="1:31" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:31" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A170" s="1"/>
       <c r="B170" s="33"/>
       <c r="C170" s="73">
@@ -13728,7 +13715,7 @@
       <c r="AA170" s="1"/>
       <c r="AB170" s="1"/>
     </row>
-    <row r="171" spans="1:31" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:31" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A171" s="1"/>
       <c r="B171" s="33"/>
       <c r="C171" s="73">
@@ -13787,7 +13774,7 @@
       <c r="AA171" s="1"/>
       <c r="AB171" s="1"/>
     </row>
-    <row r="172" spans="1:31" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:31" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A172" s="1"/>
       <c r="B172" s="33"/>
       <c r="C172" s="73">
@@ -13846,7 +13833,7 @@
       <c r="AA172" s="1"/>
       <c r="AB172" s="1"/>
     </row>
-    <row r="173" spans="1:31" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:31" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A173" s="1"/>
       <c r="B173" s="33"/>
       <c r="C173" s="73">
@@ -13905,7 +13892,7 @@
       <c r="AA173" s="1"/>
       <c r="AB173" s="1"/>
     </row>
-    <row r="174" spans="1:31" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:31" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A174" s="1"/>
       <c r="B174" s="33"/>
       <c r="C174" s="73">
@@ -13966,7 +13953,7 @@
       <c r="AA174" s="1"/>
       <c r="AB174" s="1"/>
     </row>
-    <row r="175" spans="1:31" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:31" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A175" s="1"/>
       <c r="B175" s="33"/>
       <c r="C175" s="73">
@@ -14027,7 +14014,7 @@
       <c r="AA175" s="1"/>
       <c r="AB175" s="1"/>
     </row>
-    <row r="176" spans="1:31" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:31" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A176" s="1"/>
       <c r="B176" s="33"/>
       <c r="C176" s="73">
@@ -14086,7 +14073,7 @@
       <c r="AA176" s="1"/>
       <c r="AB176" s="1"/>
     </row>
-    <row r="177" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A177" s="1"/>
       <c r="B177" s="33"/>
       <c r="C177" s="73">
@@ -14145,7 +14132,7 @@
       <c r="AA177" s="1"/>
       <c r="AB177" s="1"/>
     </row>
-    <row r="178" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A178" s="1"/>
       <c r="B178" s="33"/>
       <c r="C178" s="73">
@@ -14204,7 +14191,7 @@
       <c r="AA178" s="1"/>
       <c r="AB178" s="1"/>
     </row>
-    <row r="179" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A179" s="1"/>
       <c r="B179" s="33"/>
       <c r="C179" s="73">
@@ -14265,7 +14252,7 @@
       <c r="AA179" s="1"/>
       <c r="AB179" s="1"/>
     </row>
-    <row r="180" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A180" s="1"/>
       <c r="B180" s="33"/>
       <c r="C180" s="73">
@@ -14326,7 +14313,7 @@
       <c r="AA180" s="1"/>
       <c r="AB180" s="1"/>
     </row>
-    <row r="181" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A181" s="1"/>
       <c r="B181" s="33"/>
       <c r="C181" s="73">
@@ -14385,7 +14372,7 @@
       <c r="AA181" s="1"/>
       <c r="AB181" s="1"/>
     </row>
-    <row r="182" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A182" s="1"/>
       <c r="B182" s="33"/>
       <c r="C182" s="73">
@@ -14442,7 +14429,7 @@
       <c r="AA182" s="1"/>
       <c r="AB182" s="1"/>
     </row>
-    <row r="183" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A183" s="1"/>
       <c r="B183" s="33"/>
       <c r="C183" s="73">
@@ -14501,7 +14488,7 @@
       <c r="AA183" s="1"/>
       <c r="AB183" s="1"/>
     </row>
-    <row r="184" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A184" s="1"/>
       <c r="B184" s="33"/>
       <c r="C184" s="73">
@@ -14562,7 +14549,7 @@
       <c r="AA184" s="1"/>
       <c r="AB184" s="1"/>
     </row>
-    <row r="185" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A185" s="1"/>
       <c r="B185" s="33"/>
       <c r="C185" s="73">
@@ -14623,7 +14610,7 @@
       <c r="AA185" s="1"/>
       <c r="AB185" s="1"/>
     </row>
-    <row r="186" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A186" s="1"/>
       <c r="B186" s="33"/>
       <c r="C186" s="73">
@@ -14682,7 +14669,7 @@
       <c r="AA186" s="1"/>
       <c r="AB186" s="1"/>
     </row>
-    <row r="187" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A187" s="1"/>
       <c r="B187" s="33"/>
       <c r="C187" s="73">
@@ -14741,7 +14728,7 @@
       <c r="AA187" s="1"/>
       <c r="AB187" s="1"/>
     </row>
-    <row r="188" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A188" s="1"/>
       <c r="B188" s="33"/>
       <c r="C188" s="73">
@@ -14800,7 +14787,7 @@
       <c r="AA188" s="1"/>
       <c r="AB188" s="1"/>
     </row>
-    <row r="189" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A189" s="1"/>
       <c r="B189" s="33"/>
       <c r="C189" s="73">
@@ -14863,7 +14850,7 @@
       <c r="AA189" s="1"/>
       <c r="AB189" s="1"/>
     </row>
-    <row r="190" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A190" s="1"/>
       <c r="B190" s="33"/>
       <c r="C190" s="73">
@@ -14922,7 +14909,7 @@
       <c r="AA190" s="1"/>
       <c r="AB190" s="1"/>
     </row>
-    <row r="191" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A191" s="1"/>
       <c r="B191" s="33"/>
       <c r="C191" s="73">
@@ -14979,7 +14966,7 @@
       <c r="AA191" s="1"/>
       <c r="AB191" s="1"/>
     </row>
-    <row r="192" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A192" s="1"/>
       <c r="B192" s="33"/>
       <c r="C192" s="73">
@@ -15036,7 +15023,7 @@
       <c r="AA192" s="1"/>
       <c r="AB192" s="1"/>
     </row>
-    <row r="193" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A193" s="1"/>
       <c r="B193" s="33"/>
       <c r="C193" s="73">
@@ -15093,7 +15080,7 @@
       <c r="AA193" s="1"/>
       <c r="AB193" s="1"/>
     </row>
-    <row r="194" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A194" s="1"/>
       <c r="B194" s="33"/>
       <c r="C194" s="73">
@@ -15152,7 +15139,7 @@
       <c r="AA194" s="1"/>
       <c r="AB194" s="1"/>
     </row>
-    <row r="195" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A195" s="1"/>
       <c r="B195" s="33"/>
       <c r="C195" s="73">
@@ -15209,7 +15196,7 @@
       <c r="AA195" s="1"/>
       <c r="AB195" s="1"/>
     </row>
-    <row r="196" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A196" s="1"/>
       <c r="B196" s="33"/>
       <c r="C196" s="73">
@@ -15266,7 +15253,7 @@
       <c r="AA196" s="1"/>
       <c r="AB196" s="1"/>
     </row>
-    <row r="197" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A197" s="1"/>
       <c r="B197" s="33"/>
       <c r="C197" s="73">
@@ -15323,7 +15310,7 @@
       <c r="AA197" s="1"/>
       <c r="AB197" s="1"/>
     </row>
-    <row r="198" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A198" s="1"/>
       <c r="B198" s="33"/>
       <c r="C198" s="73">
@@ -15380,7 +15367,7 @@
       <c r="AA198" s="1"/>
       <c r="AB198" s="1"/>
     </row>
-    <row r="199" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A199" s="1"/>
       <c r="B199" s="33"/>
       <c r="C199" s="73">
@@ -15439,7 +15426,7 @@
       <c r="AA199" s="1"/>
       <c r="AB199" s="1"/>
     </row>
-    <row r="200" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A200" s="1"/>
       <c r="B200" s="33"/>
       <c r="C200" s="73">
@@ -15496,7 +15483,7 @@
       <c r="AA200" s="1"/>
       <c r="AB200" s="1"/>
     </row>
-    <row r="201" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A201" s="1"/>
       <c r="B201" s="33"/>
       <c r="C201" s="73">
@@ -15553,7 +15540,7 @@
       <c r="AA201" s="1"/>
       <c r="AB201" s="1"/>
     </row>
-    <row r="202" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A202" s="1"/>
       <c r="B202" s="33"/>
       <c r="C202" s="73">
@@ -15610,7 +15597,7 @@
       <c r="AA202" s="1"/>
       <c r="AB202" s="1"/>
     </row>
-    <row r="203" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A203" s="1"/>
       <c r="B203" s="33"/>
       <c r="C203" s="73">
@@ -15667,7 +15654,7 @@
       <c r="AA203" s="1"/>
       <c r="AB203" s="1"/>
     </row>
-    <row r="204" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A204" s="1"/>
       <c r="B204" s="33"/>
       <c r="C204" s="73">
@@ -15726,7 +15713,7 @@
       <c r="AA204" s="1"/>
       <c r="AB204" s="1"/>
     </row>
-    <row r="205" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A205" s="1"/>
       <c r="B205" s="33"/>
       <c r="C205" s="73">
@@ -15783,7 +15770,7 @@
       <c r="AA205" s="1"/>
       <c r="AB205" s="1"/>
     </row>
-    <row r="206" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A206" s="1"/>
       <c r="B206" s="33"/>
       <c r="C206" s="73">
@@ -15840,7 +15827,7 @@
       <c r="AA206" s="1"/>
       <c r="AB206" s="1"/>
     </row>
-    <row r="207" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A207" s="1"/>
       <c r="B207" s="33"/>
       <c r="C207" s="73">
@@ -15897,7 +15884,7 @@
       <c r="AA207" s="1"/>
       <c r="AB207" s="1"/>
     </row>
-    <row r="208" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:28" s="106" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A208" s="1"/>
       <c r="B208" s="33"/>
       <c r="C208" s="73">
@@ -15954,7 +15941,7 @@
       <c r="AA208" s="1"/>
       <c r="AB208" s="1"/>
     </row>
-    <row r="209" spans="1:30" s="107" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:30" s="107" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A209" s="1"/>
       <c r="B209" s="33"/>
       <c r="C209" s="73">
@@ -15989,7 +15976,7 @@
       <c r="AC209" s="123"/>
       <c r="AD209" s="123"/>
     </row>
-    <row r="210" spans="1:30" s="126" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:30" s="126" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A210" s="1"/>
       <c r="B210" s="33"/>
       <c r="C210" s="73">
@@ -16049,7 +16036,7 @@
       <c r="AA210" s="1"/>
       <c r="AB210" s="1"/>
     </row>
-    <row r="211" spans="1:30" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:30" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A211" s="1"/>
       <c r="B211" s="33"/>
       <c r="C211" s="73">
@@ -16119,7 +16106,7 @@
       <c r="AA211" s="1"/>
       <c r="AB211" s="1"/>
     </row>
-    <row r="212" spans="1:30" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:30" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A212" s="1"/>
       <c r="B212" s="33"/>
       <c r="C212" s="73">
@@ -16189,7 +16176,7 @@
       <c r="AA212" s="1"/>
       <c r="AB212" s="1"/>
     </row>
-    <row r="213" spans="1:30" s="126" customFormat="1" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:30" s="126" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A213" s="1"/>
       <c r="B213" s="33"/>
       <c r="C213" s="73">
@@ -16224,7 +16211,7 @@
       <c r="AA213" s="1"/>
       <c r="AB213" s="1"/>
     </row>
-    <row r="214" spans="1:30" s="126" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:30" s="126" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A214" s="1"/>
       <c r="B214" s="33"/>
       <c r="C214" s="73">
@@ -16275,7 +16262,7 @@
       <c r="AA214" s="1"/>
       <c r="AB214" s="1"/>
     </row>
-    <row r="215" spans="1:30" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:30" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A215" s="1"/>
       <c r="B215" s="33"/>
       <c r="C215" s="73">
@@ -16338,7 +16325,7 @@
       <c r="AA215" s="1"/>
       <c r="AB215" s="1"/>
     </row>
-    <row r="216" spans="1:30" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:30" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A216" s="1"/>
       <c r="B216" s="33"/>
       <c r="C216" s="73">
@@ -16401,7 +16388,7 @@
       <c r="AA216" s="1"/>
       <c r="AB216" s="1"/>
     </row>
-    <row r="217" spans="1:30" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:30" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A217" s="1"/>
       <c r="B217" s="33"/>
       <c r="C217" s="73">
@@ -16458,7 +16445,7 @@
       <c r="AA217" s="1"/>
       <c r="AB217" s="1"/>
     </row>
-    <row r="218" spans="1:30" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:30" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A218" s="1"/>
       <c r="B218" s="33"/>
       <c r="C218" s="73">
@@ -16517,7 +16504,7 @@
       <c r="AA218" s="1"/>
       <c r="AB218" s="1"/>
     </row>
-    <row r="219" spans="1:30" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:30" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A219" s="1"/>
       <c r="B219" s="33"/>
       <c r="C219" s="73">
@@ -16576,7 +16563,7 @@
       <c r="AA219" s="1"/>
       <c r="AB219" s="1"/>
     </row>
-    <row r="220" spans="1:30" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:30" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A220" s="1"/>
       <c r="B220" s="33"/>
       <c r="C220" s="73">
@@ -16637,7 +16624,7 @@
       <c r="AA220" s="1"/>
       <c r="AB220" s="1"/>
     </row>
-    <row r="221" spans="1:30" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:30" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A221" s="1"/>
       <c r="B221" s="33"/>
       <c r="C221" s="73">
@@ -16698,7 +16685,7 @@
       <c r="AA221" s="1"/>
       <c r="AB221" s="1"/>
     </row>
-    <row r="222" spans="1:30" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:30" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A222" s="1"/>
       <c r="B222" s="33"/>
       <c r="C222" s="73">
@@ -16755,7 +16742,7 @@
       <c r="AA222" s="1"/>
       <c r="AB222" s="1"/>
     </row>
-    <row r="223" spans="1:30" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:30" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A223" s="1"/>
       <c r="B223" s="33"/>
       <c r="C223" s="73">
@@ -16812,7 +16799,7 @@
       <c r="AA223" s="1"/>
       <c r="AB223" s="1"/>
     </row>
-    <row r="224" spans="1:30" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:30" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A224" s="1"/>
       <c r="B224" s="33"/>
       <c r="C224" s="73">
@@ -16869,7 +16856,7 @@
       <c r="AA224" s="1"/>
       <c r="AB224" s="1"/>
     </row>
-    <row r="225" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A225" s="1"/>
       <c r="B225" s="33"/>
       <c r="C225" s="73">
@@ -16928,7 +16915,7 @@
       <c r="AA225" s="1"/>
       <c r="AB225" s="1"/>
     </row>
-    <row r="226" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A226" s="1"/>
       <c r="B226" s="33"/>
       <c r="C226" s="73">
@@ -16987,7 +16974,7 @@
       <c r="AA226" s="1"/>
       <c r="AB226" s="1"/>
     </row>
-    <row r="227" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A227" s="1"/>
       <c r="B227" s="33"/>
       <c r="C227" s="73">
@@ -17044,7 +17031,7 @@
       <c r="AA227" s="1"/>
       <c r="AB227" s="1"/>
     </row>
-    <row r="228" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A228" s="1"/>
       <c r="B228" s="33"/>
       <c r="C228" s="73">
@@ -17101,7 +17088,7 @@
       <c r="AA228" s="1"/>
       <c r="AB228" s="1"/>
     </row>
-    <row r="229" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A229" s="1"/>
       <c r="B229" s="33"/>
       <c r="C229" s="73">
@@ -17158,7 +17145,7 @@
       <c r="AA229" s="1"/>
       <c r="AB229" s="1"/>
     </row>
-    <row r="230" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A230" s="1"/>
       <c r="B230" s="33"/>
       <c r="C230" s="73">
@@ -17217,7 +17204,7 @@
       <c r="AA230" s="1"/>
       <c r="AB230" s="1"/>
     </row>
-    <row r="231" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A231" s="1"/>
       <c r="B231" s="33"/>
       <c r="C231" s="73">
@@ -17276,7 +17263,7 @@
       <c r="AA231" s="1"/>
       <c r="AB231" s="1"/>
     </row>
-    <row r="232" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A232" s="1"/>
       <c r="B232" s="33"/>
       <c r="C232" s="73">
@@ -17333,7 +17320,7 @@
       <c r="AA232" s="1"/>
       <c r="AB232" s="1"/>
     </row>
-    <row r="233" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A233" s="1"/>
       <c r="B233" s="33"/>
       <c r="C233" s="73">
@@ -17390,7 +17377,7 @@
       <c r="AA233" s="1"/>
       <c r="AB233" s="1"/>
     </row>
-    <row r="234" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A234" s="1"/>
       <c r="B234" s="33"/>
       <c r="C234" s="73">
@@ -17447,7 +17434,7 @@
       <c r="AA234" s="1"/>
       <c r="AB234" s="1"/>
     </row>
-    <row r="235" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A235" s="1"/>
       <c r="B235" s="33"/>
       <c r="C235" s="73">
@@ -17517,7 +17504,7 @@
       <c r="AA235" s="1"/>
       <c r="AB235" s="1"/>
     </row>
-    <row r="236" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A236" s="1"/>
       <c r="B236" s="33"/>
       <c r="C236" s="73">
@@ -17584,7 +17571,7 @@
       <c r="AA236" s="1"/>
       <c r="AB236" s="1"/>
     </row>
-    <row r="237" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A237" s="1"/>
       <c r="B237" s="33"/>
       <c r="C237" s="73">
@@ -17647,7 +17634,7 @@
       <c r="AA237" s="1"/>
       <c r="AB237" s="1"/>
     </row>
-    <row r="238" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A238" s="1"/>
       <c r="B238" s="33"/>
       <c r="C238" s="73">
@@ -17710,7 +17697,7 @@
       <c r="AA238" s="1"/>
       <c r="AB238" s="1"/>
     </row>
-    <row r="239" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A239" s="1"/>
       <c r="B239" s="33"/>
       <c r="C239" s="73">
@@ -17777,7 +17764,7 @@
       <c r="AA239" s="1"/>
       <c r="AB239" s="1"/>
     </row>
-    <row r="240" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A240" s="1"/>
       <c r="B240" s="33"/>
       <c r="C240" s="73">
@@ -17846,7 +17833,7 @@
       <c r="AA240" s="1"/>
       <c r="AB240" s="1"/>
     </row>
-    <row r="241" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A241" s="1"/>
       <c r="B241" s="33"/>
       <c r="C241" s="73">
@@ -17913,7 +17900,7 @@
       <c r="AA241" s="1"/>
       <c r="AB241" s="1"/>
     </row>
-    <row r="242" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A242" s="1"/>
       <c r="B242" s="33"/>
       <c r="C242" s="73">
@@ -17980,7 +17967,7 @@
       <c r="AA242" s="1"/>
       <c r="AB242" s="1"/>
     </row>
-    <row r="243" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A243" s="1"/>
       <c r="B243" s="33"/>
       <c r="C243" s="73">
@@ -18047,7 +18034,7 @@
       <c r="AA243" s="1"/>
       <c r="AB243" s="1"/>
     </row>
-    <row r="244" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A244" s="1"/>
       <c r="B244" s="33"/>
       <c r="C244" s="73">
@@ -18114,7 +18101,7 @@
       <c r="AA244" s="1"/>
       <c r="AB244" s="1"/>
     </row>
-    <row r="245" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A245" s="1"/>
       <c r="B245" s="33"/>
       <c r="C245" s="73">
@@ -18183,7 +18170,7 @@
       <c r="AA245" s="1"/>
       <c r="AB245" s="1"/>
     </row>
-    <row r="246" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A246" s="1"/>
       <c r="B246" s="33"/>
       <c r="C246" s="73">
@@ -18250,7 +18237,7 @@
       <c r="AA246" s="1"/>
       <c r="AB246" s="1"/>
     </row>
-    <row r="247" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A247" s="1"/>
       <c r="B247" s="33"/>
       <c r="C247" s="73">
@@ -18317,7 +18304,7 @@
       <c r="AA247" s="1"/>
       <c r="AB247" s="1"/>
     </row>
-    <row r="248" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A248" s="1"/>
       <c r="B248" s="33"/>
       <c r="C248" s="73">
@@ -18384,7 +18371,7 @@
       <c r="AA248" s="1"/>
       <c r="AB248" s="1"/>
     </row>
-    <row r="249" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A249" s="1"/>
       <c r="B249" s="33"/>
       <c r="C249" s="73">
@@ -18451,7 +18438,7 @@
       <c r="AA249" s="1"/>
       <c r="AB249" s="1"/>
     </row>
-    <row r="250" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A250" s="1"/>
       <c r="B250" s="33"/>
       <c r="C250" s="73">
@@ -18520,7 +18507,7 @@
       <c r="AA250" s="1"/>
       <c r="AB250" s="1"/>
     </row>
-    <row r="251" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A251" s="1"/>
       <c r="B251" s="33"/>
       <c r="C251" s="73">
@@ -18587,7 +18574,7 @@
       <c r="AA251" s="1"/>
       <c r="AB251" s="1"/>
     </row>
-    <row r="252" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A252" s="1"/>
       <c r="B252" s="33"/>
       <c r="C252" s="73">
@@ -18654,7 +18641,7 @@
       <c r="AA252" s="1"/>
       <c r="AB252" s="1"/>
     </row>
-    <row r="253" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A253" s="1"/>
       <c r="B253" s="33"/>
       <c r="C253" s="73">
@@ -18721,7 +18708,7 @@
       <c r="AA253" s="1"/>
       <c r="AB253" s="1"/>
     </row>
-    <row r="254" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A254" s="1"/>
       <c r="B254" s="33"/>
       <c r="C254" s="73">
@@ -18788,7 +18775,7 @@
       <c r="AA254" s="1"/>
       <c r="AB254" s="1"/>
     </row>
-    <row r="255" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A255" s="1"/>
       <c r="B255" s="33"/>
       <c r="C255" s="73">
@@ -18849,7 +18836,7 @@
       <c r="AA255" s="1"/>
       <c r="AB255" s="1"/>
     </row>
-    <row r="256" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A256" s="1"/>
       <c r="B256" s="33"/>
       <c r="C256" s="73">
@@ -18906,7 +18893,7 @@
       <c r="AA256" s="1"/>
       <c r="AB256" s="1"/>
     </row>
-    <row r="257" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A257" s="1"/>
       <c r="B257" s="33"/>
       <c r="C257" s="73">
@@ -18963,7 +18950,7 @@
       <c r="AA257" s="1"/>
       <c r="AB257" s="1"/>
     </row>
-    <row r="258" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A258" s="1"/>
       <c r="B258" s="33"/>
       <c r="C258" s="73">
@@ -19020,7 +19007,7 @@
       <c r="AA258" s="1"/>
       <c r="AB258" s="1"/>
     </row>
-    <row r="259" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A259" s="1"/>
       <c r="B259" s="33"/>
       <c r="C259" s="73">
@@ -19077,7 +19064,7 @@
       <c r="AA259" s="1"/>
       <c r="AB259" s="1"/>
     </row>
-    <row r="260" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A260" s="1"/>
       <c r="B260" s="33"/>
       <c r="C260" s="73">
@@ -19146,7 +19133,7 @@
       <c r="AA260" s="1"/>
       <c r="AB260" s="1"/>
     </row>
-    <row r="261" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A261" s="1"/>
       <c r="B261" s="33"/>
       <c r="C261" s="73">
@@ -19213,7 +19200,7 @@
       <c r="AA261" s="1"/>
       <c r="AB261" s="1"/>
     </row>
-    <row r="262" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A262" s="1"/>
       <c r="B262" s="33"/>
       <c r="C262" s="73">
@@ -19280,7 +19267,7 @@
       <c r="AA262" s="1"/>
       <c r="AB262" s="1"/>
     </row>
-    <row r="263" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A263" s="1"/>
       <c r="B263" s="33"/>
       <c r="C263" s="73">
@@ -19347,7 +19334,7 @@
       <c r="AA263" s="1"/>
       <c r="AB263" s="1"/>
     </row>
-    <row r="264" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A264" s="1"/>
       <c r="B264" s="33"/>
       <c r="C264" s="73">
@@ -19414,7 +19401,7 @@
       <c r="AA264" s="1"/>
       <c r="AB264" s="1"/>
     </row>
-    <row r="265" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A265" s="1"/>
       <c r="B265" s="33"/>
       <c r="C265" s="73">
@@ -19473,7 +19460,7 @@
       <c r="AA265" s="1"/>
       <c r="AB265" s="1"/>
     </row>
-    <row r="266" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A266" s="1"/>
       <c r="B266" s="33"/>
       <c r="C266" s="73">
@@ -19535,7 +19522,7 @@
       <c r="AA266" s="1"/>
       <c r="AB266" s="1"/>
     </row>
-    <row r="267" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A267" s="1"/>
       <c r="B267" s="33"/>
       <c r="C267" s="73">
@@ -19596,7 +19583,7 @@
       <c r="AA267" s="1"/>
       <c r="AB267" s="1"/>
     </row>
-    <row r="268" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A268" s="1"/>
       <c r="B268" s="33"/>
       <c r="C268" s="73">
@@ -19656,7 +19643,7 @@
       <c r="AA268" s="1"/>
       <c r="AB268" s="1"/>
     </row>
-    <row r="269" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A269" s="1"/>
       <c r="B269" s="33"/>
       <c r="C269" s="73">
@@ -19723,7 +19710,7 @@
       <c r="AA269" s="1"/>
       <c r="AB269" s="1"/>
     </row>
-    <row r="270" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A270" s="1"/>
       <c r="B270" s="33"/>
       <c r="C270" s="73">
@@ -19788,7 +19775,7 @@
       <c r="AA270" s="1"/>
       <c r="AB270" s="1"/>
     </row>
-    <row r="271" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A271" s="1"/>
       <c r="B271" s="33"/>
       <c r="C271" s="73">
@@ -19850,7 +19837,7 @@
       <c r="AA271" s="1"/>
       <c r="AB271" s="1"/>
     </row>
-    <row r="272" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A272" s="1"/>
       <c r="B272" s="33"/>
       <c r="C272" s="73">
@@ -19910,7 +19897,7 @@
       <c r="AA272" s="1"/>
       <c r="AB272" s="1"/>
     </row>
-    <row r="273" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A273" s="1"/>
       <c r="B273" s="33"/>
       <c r="C273" s="73">
@@ -19967,7 +19954,7 @@
       <c r="AA273" s="1"/>
       <c r="AB273" s="1"/>
     </row>
-    <row r="274" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A274" s="1"/>
       <c r="B274" s="33"/>
       <c r="C274" s="73">
@@ -20034,7 +20021,7 @@
       <c r="AA274" s="1"/>
       <c r="AB274" s="1"/>
     </row>
-    <row r="275" spans="1:28" s="126" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:28" s="126" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A275" s="1"/>
       <c r="B275" s="33"/>
       <c r="C275" s="73">
@@ -20067,7 +20054,7 @@
       <c r="AA275" s="1"/>
       <c r="AB275" s="1"/>
     </row>
-    <row r="276" spans="1:28" s="126" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:28" s="126" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A276" s="1"/>
       <c r="B276" s="33"/>
       <c r="C276" s="73">
@@ -20123,7 +20110,7 @@
       <c r="AA276" s="1"/>
       <c r="AB276" s="1"/>
     </row>
-    <row r="277" spans="1:28" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:28" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A277" s="1"/>
       <c r="B277" s="33"/>
       <c r="C277" s="73">
@@ -20176,7 +20163,7 @@
       <c r="AA277" s="1"/>
       <c r="AB277" s="1"/>
     </row>
-    <row r="278" spans="1:28" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:28" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A278" s="1"/>
       <c r="B278" s="33"/>
       <c r="C278" s="73">
@@ -20229,7 +20216,7 @@
       <c r="AA278" s="1"/>
       <c r="AB278" s="1"/>
     </row>
-    <row r="279" spans="1:28" s="126" customFormat="1" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:28" s="126" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A279" s="1"/>
       <c r="B279" s="33"/>
       <c r="C279" s="73">
@@ -20264,7 +20251,7 @@
       <c r="AA279" s="1"/>
       <c r="AB279" s="1"/>
     </row>
-    <row r="280" spans="1:28" s="126" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:28" s="126" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A280" s="1"/>
       <c r="B280" s="33"/>
       <c r="C280" s="73">
@@ -20314,7 +20301,7 @@
       <c r="AA280" s="1"/>
       <c r="AB280" s="1"/>
     </row>
-    <row r="281" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A281" s="1"/>
       <c r="B281" s="33"/>
       <c r="C281" s="73">
@@ -20372,7 +20359,7 @@
       <c r="AA281" s="1"/>
       <c r="AB281" s="1"/>
     </row>
-    <row r="282" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A282" s="1"/>
       <c r="B282" s="33"/>
       <c r="C282" s="73">
@@ -20430,7 +20417,7 @@
       <c r="AA282" s="1"/>
       <c r="AB282" s="1"/>
     </row>
-    <row r="283" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A283" s="1"/>
       <c r="B283" s="33"/>
       <c r="C283" s="73">
@@ -20483,7 +20470,7 @@
       <c r="AA283" s="1"/>
       <c r="AB283" s="1"/>
     </row>
-    <row r="284" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A284" s="1"/>
       <c r="B284" s="33"/>
       <c r="C284" s="73">
@@ -20535,7 +20522,7 @@
       <c r="AA284" s="1"/>
       <c r="AB284" s="1"/>
     </row>
-    <row r="285" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A285" s="1"/>
       <c r="B285" s="33"/>
       <c r="C285" s="73">
@@ -20590,7 +20577,7 @@
       <c r="AA285" s="1"/>
       <c r="AB285" s="1"/>
     </row>
-    <row r="286" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A286" s="1"/>
       <c r="B286" s="33"/>
       <c r="C286" s="73">
@@ -20644,7 +20631,7 @@
       <c r="AA286" s="1"/>
       <c r="AB286" s="1"/>
     </row>
-    <row r="287" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A287" s="1"/>
       <c r="B287" s="33"/>
       <c r="C287" s="73">
@@ -20698,7 +20685,7 @@
       <c r="AA287" s="1"/>
       <c r="AB287" s="1"/>
     </row>
-    <row r="288" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A288" s="1"/>
       <c r="B288" s="33"/>
       <c r="C288" s="73">
@@ -20748,7 +20735,7 @@
       <c r="AA288" s="1"/>
       <c r="AB288" s="1"/>
     </row>
-    <row r="289" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A289" s="1"/>
       <c r="B289" s="33"/>
       <c r="C289" s="73">
@@ -20798,7 +20785,7 @@
       <c r="AA289" s="1"/>
       <c r="AB289" s="1"/>
     </row>
-    <row r="290" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A290" s="1"/>
       <c r="B290" s="33"/>
       <c r="C290" s="73">
@@ -20851,7 +20838,7 @@
       <c r="AA290" s="1"/>
       <c r="AB290" s="1"/>
     </row>
-    <row r="291" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A291" s="1"/>
       <c r="B291" s="33"/>
       <c r="C291" s="73">
@@ -20905,7 +20892,7 @@
       <c r="AA291" s="1"/>
       <c r="AB291" s="1"/>
     </row>
-    <row r="292" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A292" s="1"/>
       <c r="B292" s="33"/>
       <c r="C292" s="73">
@@ -20959,7 +20946,7 @@
       <c r="AA292" s="1"/>
       <c r="AB292" s="1"/>
     </row>
-    <row r="293" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A293" s="1"/>
       <c r="B293" s="33"/>
       <c r="C293" s="73">
@@ -21009,7 +20996,7 @@
       <c r="AA293" s="1"/>
       <c r="AB293" s="1"/>
     </row>
-    <row r="294" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A294" s="1"/>
       <c r="B294" s="33"/>
       <c r="C294" s="73">
@@ -21059,7 +21046,7 @@
       <c r="AA294" s="1"/>
       <c r="AB294" s="1"/>
     </row>
-    <row r="295" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A295" s="1"/>
       <c r="B295" s="33"/>
       <c r="C295" s="73">
@@ -21112,7 +21099,7 @@
       <c r="AA295" s="1"/>
       <c r="AB295" s="1"/>
     </row>
-    <row r="296" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A296" s="1"/>
       <c r="B296" s="33"/>
       <c r="C296" s="73">
@@ -21164,7 +21151,7 @@
       <c r="AA296" s="1"/>
       <c r="AB296" s="1"/>
     </row>
-    <row r="297" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A297" s="1"/>
       <c r="B297" s="33"/>
       <c r="C297" s="73">
@@ -21216,7 +21203,7 @@
       <c r="AA297" s="1"/>
       <c r="AB297" s="1"/>
     </row>
-    <row r="298" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A298" s="1"/>
       <c r="B298" s="33"/>
       <c r="C298" s="73">
@@ -21265,7 +21252,7 @@
       <c r="AA298" s="1"/>
       <c r="AB298" s="1"/>
     </row>
-    <row r="299" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A299" s="1"/>
       <c r="B299" s="33"/>
       <c r="C299" s="73">
@@ -21312,7 +21299,7 @@
       <c r="AA299" s="1"/>
       <c r="AB299" s="1"/>
     </row>
-    <row r="300" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:28" s="126" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A300" s="1"/>
       <c r="B300" s="33"/>
       <c r="C300" s="73">
@@ -21365,7 +21352,7 @@
       <c r="AA300" s="1"/>
       <c r="AB300" s="1"/>
     </row>
-    <row r="301" spans="1:28" s="126" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:28" s="126" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A301" s="1"/>
       <c r="B301" s="33"/>
       <c r="C301" s="73">
@@ -21398,7 +21385,7 @@
       <c r="AA301" s="1"/>
       <c r="AB301" s="1"/>
     </row>
-    <row r="302" spans="1:28" s="95" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:28" s="95" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A302" s="1"/>
       <c r="B302" s="33"/>
       <c r="C302" s="73">
@@ -21431,7 +21418,7 @@
       <c r="AA302" s="1"/>
       <c r="AB302" s="1"/>
     </row>
-    <row r="303" spans="1:28" s="95" customFormat="1" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:28" s="95" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A303" s="1"/>
       <c r="B303" s="35"/>
       <c r="C303" s="76">
@@ -21466,7 +21453,7 @@
       <c r="AA303" s="1"/>
       <c r="AB303" s="1"/>
     </row>
-    <row r="304" spans="1:28" s="95" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:28" s="95" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A304" s="1"/>
       <c r="B304" s="19"/>
       <c r="C304" s="77">
@@ -21499,7 +21486,7 @@
       <c r="AA304" s="1"/>
       <c r="AB304" s="1"/>
     </row>
-    <row r="305" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A305" s="1"/>
       <c r="B305" s="1"/>
       <c r="C305" s="73">
@@ -21532,7 +21519,7 @@
       <c r="AA305" s="1"/>
       <c r="AB305" s="1"/>
     </row>
-    <row r="306" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A306" s="1"/>
       <c r="B306" s="1"/>
       <c r="C306" s="73">
@@ -21565,7 +21552,7 @@
       <c r="AA306" s="1"/>
       <c r="AB306" s="1"/>
     </row>
-    <row r="307" spans="1:28" s="97" customFormat="1" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="307" spans="1:28" s="97" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A307" s="1"/>
       <c r="B307" s="20"/>
       <c r="C307" s="74">
@@ -21598,7 +21585,7 @@
       <c r="AA307" s="1"/>
       <c r="AB307" s="1"/>
     </row>
-    <row r="308" spans="1:28" s="97" customFormat="1" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:28" s="97" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A308" s="1"/>
       <c r="B308" s="34" t="s">
         <v>21</v>
@@ -21633,7 +21620,7 @@
       <c r="AA308" s="1"/>
       <c r="AB308" s="1"/>
     </row>
-    <row r="309" spans="1:28" s="97" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:28" s="97" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A309" s="1"/>
       <c r="B309" s="33"/>
       <c r="C309" s="73">
@@ -21666,7 +21653,7 @@
       <c r="AA309" s="1"/>
       <c r="AB309" s="1"/>
     </row>
-    <row r="310" spans="1:28" s="97" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:28" s="97" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A310" s="1"/>
       <c r="B310" s="33"/>
       <c r="C310" s="73">
@@ -21703,7 +21690,7 @@
       <c r="AA310" s="1"/>
       <c r="AB310" s="1"/>
     </row>
-    <row r="311" spans="1:28" s="97" customFormat="1" ht="20.149999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:28" s="97" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A311" s="1"/>
       <c r="B311" s="33"/>
       <c r="C311" s="73">
@@ -21740,7 +21727,7 @@
       <c r="AA311" s="1"/>
       <c r="AB311" s="1"/>
     </row>
-    <row r="312" spans="1:28" s="97" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:28" s="97" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A312" s="1"/>
       <c r="B312" s="33"/>
       <c r="C312" s="73">
@@ -21773,7 +21760,7 @@
       <c r="AA312" s="1"/>
       <c r="AB312" s="1"/>
     </row>
-    <row r="313" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A313" s="1"/>
       <c r="B313" s="33"/>
       <c r="C313" s="73">
@@ -21806,7 +21793,7 @@
       <c r="AA313" s="1"/>
       <c r="AB313" s="1"/>
     </row>
-    <row r="314" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A314" s="1"/>
       <c r="B314" s="33"/>
       <c r="C314" s="73">
@@ -21845,7 +21832,7 @@
       <c r="AA314" s="1"/>
       <c r="AB314" s="1"/>
     </row>
-    <row r="315" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A315" s="1"/>
       <c r="B315" s="33"/>
       <c r="C315" s="73">
@@ -21884,7 +21871,7 @@
       <c r="AA315" s="1"/>
       <c r="AB315" s="1"/>
     </row>
-    <row r="316" spans="1:28" s="97" customFormat="1" ht="28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:28" s="97" customFormat="1" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A316" s="1"/>
       <c r="B316" s="33"/>
       <c r="C316" s="73">
@@ -21927,7 +21914,7 @@
       <c r="AA316" s="1"/>
       <c r="AB316" s="1"/>
     </row>
-    <row r="317" spans="1:28" s="97" customFormat="1" ht="11.5" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:28" s="97" customFormat="1" ht="11.45" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A317" s="1"/>
       <c r="B317" s="33" t="s">
         <v>20</v>
@@ -21968,7 +21955,7 @@
       <c r="AA317" s="1"/>
       <c r="AB317" s="1"/>
     </row>
-    <row r="318" spans="1:28" s="97" customFormat="1" ht="13" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:28" s="97" customFormat="1" ht="12.95" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A318" s="1"/>
       <c r="B318" s="33"/>
       <c r="C318" s="73">
@@ -22001,7 +21988,7 @@
       <c r="AA318" s="1"/>
       <c r="AB318" s="1"/>
     </row>
-    <row r="319" spans="1:28" s="97" customFormat="1" ht="8.5" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:28" s="97" customFormat="1" ht="8.4499999999999993" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A319" s="1"/>
       <c r="B319" s="33" t="s">
         <v>19</v>
@@ -22038,7 +22025,7 @@
       <c r="AA319" s="1"/>
       <c r="AB319" s="1"/>
     </row>
-    <row r="320" spans="1:28" s="97" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:28" s="97" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A320" s="1"/>
       <c r="B320" s="33"/>
       <c r="C320" s="73">
@@ -22073,7 +22060,7 @@
       <c r="AA320" s="1"/>
       <c r="AB320" s="1"/>
     </row>
-    <row r="321" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A321" s="1"/>
       <c r="B321" s="33"/>
       <c r="C321" s="73">
@@ -22120,7 +22107,7 @@
       <c r="AA321" s="1"/>
       <c r="AB321" s="1"/>
     </row>
-    <row r="322" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A322" s="1"/>
       <c r="B322" s="33"/>
       <c r="C322" s="73"/>
@@ -22159,7 +22146,7 @@
       <c r="AA322" s="1"/>
       <c r="AB322" s="1"/>
     </row>
-    <row r="323" spans="1:28" s="97" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:28" s="97" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A323" s="1"/>
       <c r="B323" s="33"/>
       <c r="C323" s="73">
@@ -22200,7 +22187,7 @@
       <c r="AA323" s="1"/>
       <c r="AB323" s="1"/>
     </row>
-    <row r="324" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A324" s="1"/>
       <c r="B324" s="33"/>
       <c r="C324" s="73"/>
@@ -22242,7 +22229,7 @@
       <c r="AA324" s="1"/>
       <c r="AB324" s="1"/>
     </row>
-    <row r="325" spans="1:28" s="97" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:28" s="97" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A325" s="1"/>
       <c r="B325" s="33"/>
       <c r="C325" s="73">
@@ -22285,7 +22272,7 @@
       <c r="AA325" s="1"/>
       <c r="AB325" s="1"/>
     </row>
-    <row r="326" spans="1:28" s="105" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:28" s="105" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A326" s="1"/>
       <c r="B326" s="33"/>
       <c r="C326" s="73">
@@ -22328,7 +22315,7 @@
       <c r="AA326" s="1"/>
       <c r="AB326" s="1"/>
     </row>
-    <row r="327" spans="1:28" s="124" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:28" s="124" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A327" s="1"/>
       <c r="B327" s="33"/>
       <c r="C327" s="73">
@@ -22369,7 +22356,7 @@
       <c r="AA327" s="1"/>
       <c r="AB327" s="1"/>
     </row>
-    <row r="328" spans="1:28" s="97" customFormat="1" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:28" s="97" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A328" s="1"/>
       <c r="B328" s="33"/>
       <c r="C328" s="73">
@@ -22404,7 +22391,7 @@
       <c r="AA328" s="1"/>
       <c r="AB328" s="1"/>
     </row>
-    <row r="329" spans="1:28" s="147" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:28" s="147" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A329" s="1"/>
       <c r="B329" s="33"/>
       <c r="C329" s="73">
@@ -22439,7 +22426,7 @@
       <c r="AA329" s="1"/>
       <c r="AB329" s="1"/>
     </row>
-    <row r="330" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A330" s="1"/>
       <c r="B330" s="33"/>
       <c r="C330" s="73">
@@ -22474,7 +22461,7 @@
       <c r="AA330" s="1"/>
       <c r="AB330" s="1"/>
     </row>
-    <row r="331" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A331" s="1"/>
       <c r="B331" s="33"/>
       <c r="C331" s="73">
@@ -22519,7 +22506,7 @@
       <c r="AA331" s="1"/>
       <c r="AB331" s="1"/>
     </row>
-    <row r="332" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A332" s="1"/>
       <c r="B332" s="33"/>
       <c r="C332" s="73">
@@ -22566,7 +22553,7 @@
       <c r="AA332" s="1"/>
       <c r="AB332" s="1"/>
     </row>
-    <row r="333" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A333" s="1"/>
       <c r="B333" s="33"/>
       <c r="C333" s="73">
@@ -22618,7 +22605,7 @@
       <c r="AA333" s="1"/>
       <c r="AB333" s="1"/>
     </row>
-    <row r="334" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A334" s="1"/>
       <c r="B334" s="33"/>
       <c r="C334" s="73"/>
@@ -22668,7 +22655,7 @@
       <c r="AA334" s="1"/>
       <c r="AB334" s="1"/>
     </row>
-    <row r="335" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A335" s="1"/>
       <c r="B335" s="33"/>
       <c r="C335" s="73">
@@ -22717,7 +22704,7 @@
       <c r="AA335" s="1"/>
       <c r="AB335" s="1"/>
     </row>
-    <row r="336" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A336" s="1"/>
       <c r="B336" s="33"/>
       <c r="C336" s="73"/>
@@ -22761,7 +22748,7 @@
       <c r="AA336" s="1"/>
       <c r="AB336" s="1"/>
     </row>
-    <row r="337" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A337" s="1"/>
       <c r="B337" s="33"/>
       <c r="C337" s="73">
@@ -22800,7 +22787,7 @@
       <c r="AA337" s="1"/>
       <c r="AB337" s="1"/>
     </row>
-    <row r="338" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A338" s="1"/>
       <c r="B338" s="33"/>
       <c r="C338" s="73">
@@ -22839,7 +22826,7 @@
       <c r="AA338" s="1"/>
       <c r="AB338" s="1"/>
     </row>
-    <row r="339" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A339" s="1"/>
       <c r="B339" s="33"/>
       <c r="C339" s="73">
@@ -22880,7 +22867,7 @@
       <c r="AA339" s="1"/>
       <c r="AB339" s="1"/>
     </row>
-    <row r="340" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A340" s="1"/>
       <c r="B340" s="33"/>
       <c r="C340" s="73"/>
@@ -22921,7 +22908,7 @@
       <c r="AA340" s="1"/>
       <c r="AB340" s="1"/>
     </row>
-    <row r="341" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A341" s="1"/>
       <c r="B341" s="33"/>
       <c r="C341" s="73"/>
@@ -22951,7 +22938,7 @@
       <c r="AA341" s="1"/>
       <c r="AB341" s="1"/>
     </row>
-    <row r="342" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A342" s="1"/>
       <c r="B342" s="33"/>
       <c r="C342" s="73">
@@ -22986,7 +22973,7 @@
       <c r="AA342" s="1"/>
       <c r="AB342" s="1"/>
     </row>
-    <row r="343" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A343" s="1"/>
       <c r="B343" s="33"/>
       <c r="C343" s="73">
@@ -23027,7 +23014,7 @@
       <c r="AA343" s="1"/>
       <c r="AB343" s="1"/>
     </row>
-    <row r="344" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A344" s="1"/>
       <c r="B344" s="33"/>
       <c r="C344" s="73">
@@ -23070,7 +23057,7 @@
       <c r="AA344" s="1"/>
       <c r="AB344" s="1"/>
     </row>
-    <row r="345" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A345" s="1"/>
       <c r="B345" s="33"/>
       <c r="C345" s="73">
@@ -23118,7 +23105,7 @@
       <c r="AA345" s="1"/>
       <c r="AB345" s="1"/>
     </row>
-    <row r="346" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A346" s="1"/>
       <c r="B346" s="33"/>
       <c r="C346" s="73"/>
@@ -23162,7 +23149,7 @@
       <c r="AA346" s="1"/>
       <c r="AB346" s="1"/>
     </row>
-    <row r="347" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A347" s="1"/>
       <c r="B347" s="33"/>
       <c r="C347" s="73">
@@ -23207,7 +23194,7 @@
       <c r="AA347" s="1"/>
       <c r="AB347" s="1"/>
     </row>
-    <row r="348" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A348" s="1"/>
       <c r="B348" s="33"/>
       <c r="C348" s="73">
@@ -23240,7 +23227,7 @@
       <c r="AA348" s="1"/>
       <c r="AB348" s="1"/>
     </row>
-    <row r="349" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A349" s="1"/>
       <c r="B349" s="33"/>
       <c r="C349" s="73">
@@ -23275,7 +23262,7 @@
       <c r="AA349" s="1"/>
       <c r="AB349" s="1"/>
     </row>
-    <row r="350" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A350" s="1"/>
       <c r="B350" s="33"/>
       <c r="C350" s="73">
@@ -23310,7 +23297,7 @@
       <c r="AA350" s="1"/>
       <c r="AB350" s="1"/>
     </row>
-    <row r="351" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A351" s="1"/>
       <c r="B351" s="33"/>
       <c r="C351" s="73">
@@ -23345,7 +23332,7 @@
       <c r="AA351" s="1"/>
       <c r="AB351" s="1"/>
     </row>
-    <row r="352" spans="1:28" s="147" customFormat="1" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:28" s="147" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A352" s="1"/>
       <c r="B352" s="33"/>
       <c r="C352" s="73">
@@ -23380,7 +23367,7 @@
       <c r="AA352" s="1"/>
       <c r="AB352" s="1"/>
     </row>
-    <row r="353" spans="1:28" s="135" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:28" s="135" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A353" s="1"/>
       <c r="B353" s="33"/>
       <c r="C353" s="73">
@@ -23413,7 +23400,7 @@
       <c r="AA353" s="1"/>
       <c r="AB353" s="1"/>
     </row>
-    <row r="354" spans="1:28" s="135" customFormat="1" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:28" s="135" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A354" s="1"/>
       <c r="B354" s="35"/>
       <c r="C354" s="76">
@@ -23448,7 +23435,7 @@
       <c r="AA354" s="1"/>
       <c r="AB354" s="1"/>
     </row>
-    <row r="355" spans="1:28" s="135" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:28" s="135" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A355" s="1"/>
       <c r="B355" s="19"/>
       <c r="C355" s="77">
@@ -23481,7 +23468,7 @@
       <c r="AA355" s="1"/>
       <c r="AB355" s="1"/>
     </row>
-    <row r="356" spans="1:28" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:28" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A356" s="1"/>
       <c r="B356" s="1"/>
       <c r="C356" s="73">
@@ -23514,7 +23501,7 @@
       <c r="AA356" s="1"/>
       <c r="AB356" s="1"/>
     </row>
-    <row r="357" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A357" s="1"/>
       <c r="B357" s="1"/>
       <c r="C357" s="66"/>
@@ -23544,7 +23531,7 @@
       <c r="AA357" s="1"/>
       <c r="AB357" s="1"/>
     </row>
-    <row r="358" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A358" s="1"/>
       <c r="B358" s="1"/>
       <c r="C358" s="66"/>
@@ -23574,7 +23561,7 @@
       <c r="AA358" s="1"/>
       <c r="AB358" s="1"/>
     </row>
-    <row r="359" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A359" s="1"/>
       <c r="B359" s="1"/>
       <c r="C359" s="66"/>
@@ -23604,7 +23591,7 @@
       <c r="AA359" s="1"/>
       <c r="AB359" s="1"/>
     </row>
-    <row r="360" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A360" s="1"/>
       <c r="B360" s="1"/>
       <c r="C360" s="66"/>
@@ -23634,7 +23621,7 @@
       <c r="AA360" s="1"/>
       <c r="AB360" s="1"/>
     </row>
-    <row r="361" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A361" s="1"/>
       <c r="B361" s="1"/>
       <c r="C361" s="66"/>
@@ -23664,7 +23651,7 @@
       <c r="AA361" s="1"/>
       <c r="AB361" s="1"/>
     </row>
-    <row r="362" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A362" s="1"/>
       <c r="B362" s="1"/>
       <c r="C362" s="66"/>
@@ -23694,7 +23681,7 @@
       <c r="AA362" s="1"/>
       <c r="AB362" s="1"/>
     </row>
-    <row r="363" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C363" s="72" t="s">
         <v>4</v>
       </c>
@@ -23724,22 +23711,22 @@
       <selection activeCell="U37" sqref="U37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" customWidth="1"/>
-    <col min="2" max="2" width="2.7265625" customWidth="1"/>
-    <col min="3" max="3" width="4.7265625" customWidth="1" outlineLevel="2"/>
-    <col min="4" max="4" width="1.7265625" customWidth="1"/>
-    <col min="5" max="6" width="9.1796875" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="1.7265625" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="15.7265625" customWidth="1"/>
-    <col min="12" max="12" width="9.1796875" customWidth="1"/>
-    <col min="26" max="26" width="1.7265625" customWidth="1"/>
-    <col min="27" max="28" width="4.7265625" customWidth="1"/>
-    <col min="30" max="30" width="46.1796875" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="4" max="4" width="1.7109375" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="1.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" customWidth="1"/>
+    <col min="26" max="26" width="1.7109375" customWidth="1"/>
+    <col min="27" max="28" width="4.7109375" customWidth="1"/>
+    <col min="30" max="30" width="46.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="66"/>
@@ -23771,7 +23758,7 @@
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
     </row>
-    <row r="2" spans="1:30" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="67">
@@ -23806,7 +23793,7 @@
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
-    <row r="3" spans="1:30" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:30" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="20"/>
       <c r="C3" s="68">
@@ -23841,7 +23828,7 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
     </row>
-    <row r="4" spans="1:30" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="34" t="s">
         <v>21</v>
@@ -23878,7 +23865,7 @@
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
     </row>
-    <row r="5" spans="1:30" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:30" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="33"/>
       <c r="C5" s="67">
@@ -23955,7 +23942,7 @@
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" spans="1:30" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="33"/>
       <c r="C6" s="67">
@@ -23995,7 +23982,7 @@
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
     </row>
-    <row r="7" spans="1:30" ht="20.149999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:30" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="33"/>
       <c r="C7" s="67">
@@ -24036,7 +24023,7 @@
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
     </row>
-    <row r="8" spans="1:30" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="33"/>
       <c r="C8" s="67">
@@ -24071,7 +24058,7 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
     </row>
-    <row r="9" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="33"/>
       <c r="C9" s="67">
@@ -24106,7 +24093,7 @@
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
     </row>
-    <row r="10" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="33"/>
       <c r="C10" s="67">
@@ -24141,7 +24128,7 @@
       <c r="AC10" s="1"/>
       <c r="AD10" s="1"/>
     </row>
-    <row r="11" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="33"/>
       <c r="C11" s="67">
@@ -24176,7 +24163,7 @@
       <c r="AC11" s="1"/>
       <c r="AD11" s="1"/>
     </row>
-    <row r="12" spans="1:30" ht="28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:30" ht="30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="33"/>
       <c r="C12" s="67">
@@ -24215,7 +24202,7 @@
       <c r="AC12" s="1"/>
       <c r="AD12" s="1"/>
     </row>
-    <row r="13" spans="1:30" ht="11.5" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:30" ht="11.45" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="33" t="s">
         <v>20</v>
@@ -24252,7 +24239,7 @@
       <c r="AC13" s="1"/>
       <c r="AD13" s="1"/>
     </row>
-    <row r="14" spans="1:30" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:30" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="33"/>
       <c r="C14" s="67">
@@ -24287,7 +24274,7 @@
       <c r="AC14" s="1"/>
       <c r="AD14" s="1"/>
     </row>
-    <row r="15" spans="1:30" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:30" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="33" t="s">
         <v>19</v>
@@ -24326,7 +24313,7 @@
       <c r="AC15" s="1"/>
       <c r="AD15" s="1"/>
     </row>
-    <row r="16" spans="1:30" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="33"/>
       <c r="C16" s="67">
@@ -24363,7 +24350,7 @@
       <c r="AC16" s="1"/>
       <c r="AD16" s="1"/>
     </row>
-    <row r="17" spans="1:30" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="33"/>
       <c r="C17" s="67">
@@ -24400,7 +24387,7 @@
       <c r="AC17" s="1"/>
       <c r="AD17" s="1"/>
     </row>
-    <row r="18" spans="1:30" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:30" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="33"/>
       <c r="C18" s="67">
@@ -24441,7 +24428,7 @@
       <c r="AC18" s="1"/>
       <c r="AD18" s="1"/>
     </row>
-    <row r="19" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="33"/>
       <c r="C19" s="67">
@@ -24476,7 +24463,7 @@
       <c r="AC19" s="1"/>
       <c r="AD19" s="1"/>
     </row>
-    <row r="20" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="33"/>
       <c r="C20" s="67">
@@ -24511,7 +24498,7 @@
       <c r="AC20" s="1"/>
       <c r="AD20" s="1"/>
     </row>
-    <row r="21" spans="1:30" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:30" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="33"/>
       <c r="C21" s="67">
@@ -24552,7 +24539,7 @@
       <c r="AC21" s="1"/>
       <c r="AD21" s="1"/>
     </row>
-    <row r="22" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="33"/>
       <c r="C22" s="67">
@@ -24587,7 +24574,7 @@
       <c r="AC22" s="1"/>
       <c r="AD22" s="1"/>
     </row>
-    <row r="23" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="33"/>
       <c r="C23" s="67">
@@ -24622,7 +24609,7 @@
       <c r="AC23" s="1"/>
       <c r="AD23" s="1"/>
     </row>
-    <row r="24" spans="1:30" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="33"/>
       <c r="C24" s="67">
@@ -24659,7 +24646,7 @@
       <c r="AC24" s="1"/>
       <c r="AD24" s="1"/>
     </row>
-    <row r="25" spans="1:30" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="33"/>
       <c r="C25" s="67">
@@ -24696,7 +24683,7 @@
       <c r="AC25" s="1"/>
       <c r="AD25" s="1"/>
     </row>
-    <row r="26" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="33"/>
       <c r="C26" s="67">
@@ -24745,7 +24732,7 @@
       <c r="AC26" s="1"/>
       <c r="AD26" s="1"/>
     </row>
-    <row r="27" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="33"/>
       <c r="C27" s="67">
@@ -24784,7 +24771,7 @@
       <c r="AC27" s="1"/>
       <c r="AD27" s="1"/>
     </row>
-    <row r="28" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="33"/>
       <c r="C28" s="67">
@@ -24823,7 +24810,7 @@
       <c r="AC28" s="1"/>
       <c r="AD28" s="1"/>
     </row>
-    <row r="29" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="33"/>
       <c r="C29" s="67">
@@ -24862,7 +24849,7 @@
       <c r="AC29" s="1"/>
       <c r="AD29" s="1"/>
     </row>
-    <row r="30" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="33"/>
       <c r="C30" s="67">
@@ -24901,7 +24888,7 @@
       <c r="AC30" s="1"/>
       <c r="AD30" s="1"/>
     </row>
-    <row r="31" spans="1:30" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="33"/>
       <c r="C31" s="67">
@@ -24938,7 +24925,7 @@
       <c r="AC31" s="1"/>
       <c r="AD31" s="1"/>
     </row>
-    <row r="32" spans="1:30" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="33"/>
       <c r="C32" s="67">
@@ -24975,7 +24962,7 @@
       <c r="AC32" s="1"/>
       <c r="AD32" s="1"/>
     </row>
-    <row r="33" spans="1:30" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:30" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="33"/>
       <c r="C33" s="67">
@@ -25036,7 +25023,7 @@
       <c r="AC33" s="1"/>
       <c r="AD33" s="1"/>
     </row>
-    <row r="34" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="33"/>
       <c r="C34" s="67">
@@ -25101,7 +25088,7 @@
       <c r="AC34" s="1"/>
       <c r="AD34" s="1"/>
     </row>
-    <row r="35" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="33"/>
       <c r="C35" s="67">
@@ -25136,7 +25123,7 @@
       <c r="AC35" s="1"/>
       <c r="AD35" s="1"/>
     </row>
-    <row r="36" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="33"/>
       <c r="C36" s="67">
@@ -25171,7 +25158,7 @@
       <c r="AC36" s="1"/>
       <c r="AD36" s="1"/>
     </row>
-    <row r="37" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="33"/>
       <c r="C37" s="67">
@@ -25206,7 +25193,7 @@
       <c r="AC37" s="1"/>
       <c r="AD37" s="1"/>
     </row>
-    <row r="38" spans="1:30" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="33"/>
       <c r="C38" s="67">
@@ -25243,7 +25230,7 @@
       <c r="AC38" s="1"/>
       <c r="AD38" s="1"/>
     </row>
-    <row r="39" spans="1:30" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="33"/>
       <c r="C39" s="67">
@@ -25278,7 +25265,7 @@
       <c r="AC39" s="1"/>
       <c r="AD39" s="1"/>
     </row>
-    <row r="40" spans="1:30" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="35"/>
       <c r="C40" s="70">
@@ -25315,7 +25302,7 @@
       <c r="AC40" s="1"/>
       <c r="AD40" s="1"/>
     </row>
-    <row r="41" spans="1:30" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:30" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="19"/>
       <c r="C41" s="71">
@@ -25350,7 +25337,7 @@
       <c r="AC41" s="1"/>
       <c r="AD41" s="1"/>
     </row>
-    <row r="42" spans="1:30" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="67">
@@ -25385,7 +25372,7 @@
       <c r="AC42" s="1"/>
       <c r="AD42" s="1"/>
     </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="66"/>
@@ -25417,7 +25404,7 @@
       <c r="AC43" s="1"/>
       <c r="AD43" s="1"/>
     </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="66"/>
@@ -25449,7 +25436,7 @@
       <c r="AC44" s="1"/>
       <c r="AD44" s="1"/>
     </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="66"/>
@@ -25481,7 +25468,7 @@
       <c r="AC45" s="1"/>
       <c r="AD45" s="1"/>
     </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="66"/>
@@ -25513,7 +25500,7 @@
       <c r="AC46" s="1"/>
       <c r="AD46" s="1"/>
     </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="66"/>
@@ -25545,7 +25532,7 @@
       <c r="AC47" s="1"/>
       <c r="AD47" s="1"/>
     </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="66"/>
@@ -25577,7 +25564,7 @@
       <c r="AC48" s="1"/>
       <c r="AD48" s="1"/>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C49" s="72" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Add '-0' to index of k2 cluster
</commit_message>
<xml_diff>
--- a/Structural.xlsx
+++ b/Structural.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE59F82C-0FBC-471E-A32E-398AB8548986}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F19FD2ED-EF4E-49FA-AFB9-2676191FF8E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="735" windowWidth="27870" windowHeight="15255" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -1192,7 +1192,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="287">
   <si>
     <t>Controls for this worksheet</t>
   </si>
@@ -2013,11 +2013,6 @@
   </si>
   <si>
     <t xml:space="preserve">         Therefore think about the final sale date relative to 1 Jan, rather than the age of the animal</t>
-  </si>
-  <si>
-    <t>29Mar21: Changed to FVP3, 1N for dams, 3N for Offs
-22Mar21: Alter the initial weight &amp; wool spread for the weaners
-1: 1Apr19-Blank worksheet</t>
   </si>
   <si>
     <t>is dry</t>
@@ -2026,6 +2021,45 @@
     <t>30Mar21: Added inputs for % dry and number dams mated
 2: 17Jul20-Added structural inputs table
 1: 1Apr19-Created the version control table</t>
+  </si>
+  <si>
+    <t>31Mar21: Change the index for the k2 cluster (for the seasonality model)
+29Mar21: Changed to FVP3, 1N for dams, 3N for Offs
+22Mar21: Alter the initial weight &amp; wool spread for the weaners
+1: 1Apr19-Blank worksheet</t>
+  </si>
+  <si>
+    <t>NM-0</t>
+  </si>
+  <si>
+    <t>00-0</t>
+  </si>
+  <si>
+    <t>11-0</t>
+  </si>
+  <si>
+    <t>22-0</t>
+  </si>
+  <si>
+    <t>33-0</t>
+  </si>
+  <si>
+    <t>21-0</t>
+  </si>
+  <si>
+    <t>32-0</t>
+  </si>
+  <si>
+    <t>31-0</t>
+  </si>
+  <si>
+    <t>10-0</t>
+  </si>
+  <si>
+    <t>20-0</t>
+  </si>
+  <si>
+    <t>30-0</t>
   </si>
 </sst>
 </file>
@@ -3569,6 +3603,9 @@
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="15" fontId="1" fillId="11" borderId="1" xfId="12" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="38" xfId="12" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3619,9 +3656,6 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="23" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="15" fontId="1" fillId="11" borderId="1" xfId="12" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -4657,19 +4691,19 @@
       <c r="I18" s="31">
         <v>2</v>
       </c>
-      <c r="J18" s="162" t="s">
+      <c r="J18" s="163" t="s">
         <v>70</v>
       </c>
-      <c r="K18" s="163"/>
-      <c r="L18" s="163"/>
-      <c r="M18" s="163"/>
-      <c r="N18" s="163"/>
-      <c r="O18" s="163"/>
-      <c r="P18" s="163"/>
-      <c r="Q18" s="163"/>
-      <c r="R18" s="163"/>
-      <c r="S18" s="163"/>
-      <c r="T18" s="164"/>
+      <c r="K18" s="164"/>
+      <c r="L18" s="164"/>
+      <c r="M18" s="164"/>
+      <c r="N18" s="164"/>
+      <c r="O18" s="164"/>
+      <c r="P18" s="164"/>
+      <c r="Q18" s="164"/>
+      <c r="R18" s="164"/>
+      <c r="S18" s="164"/>
+      <c r="T18" s="165"/>
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
       <c r="W18" s="2"/>
@@ -4762,19 +4796,19 @@
       <c r="I21" s="23">
         <v>1</v>
       </c>
-      <c r="J21" s="165" t="s">
+      <c r="J21" s="166" t="s">
         <v>35</v>
       </c>
-      <c r="K21" s="166"/>
-      <c r="L21" s="166"/>
-      <c r="M21" s="166"/>
-      <c r="N21" s="166"/>
-      <c r="O21" s="166"/>
-      <c r="P21" s="166"/>
-      <c r="Q21" s="166"/>
-      <c r="R21" s="166"/>
-      <c r="S21" s="166"/>
-      <c r="T21" s="166"/>
+      <c r="K21" s="167"/>
+      <c r="L21" s="167"/>
+      <c r="M21" s="167"/>
+      <c r="N21" s="167"/>
+      <c r="O21" s="167"/>
+      <c r="P21" s="167"/>
+      <c r="Q21" s="167"/>
+      <c r="R21" s="167"/>
+      <c r="S21" s="167"/>
+      <c r="T21" s="167"/>
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
       <c r="W21" s="2"/>
@@ -7026,7 +7060,7 @@
   <dimension ref="A1:AE363"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18:T18"/>
+      <selection activeCell="J21" sqref="J21:T21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -7045,7 +7079,7 @@
     <col min="28" max="28" width="46.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="66"/>
@@ -7075,7 +7109,7 @@
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
     </row>
-    <row r="2" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="67">
@@ -7108,7 +7142,7 @@
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
     </row>
-    <row r="3" spans="1:28" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" ht="5.0999999999999996" customHeight="1" collapsed="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="20"/>
       <c r="C3" s="68">
@@ -7141,7 +7175,7 @@
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
     </row>
-    <row r="4" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="34" t="s">
         <v>21</v>
@@ -7176,7 +7210,7 @@
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
     </row>
-    <row r="5" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" hidden="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="33"/>
       <c r="C5" s="67">
@@ -7285,7 +7319,7 @@
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
     </row>
-    <row r="7" spans="1:28" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" ht="20.100000000000001" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="33"/>
       <c r="C7" s="67">
@@ -7324,7 +7358,7 @@
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
     </row>
-    <row r="8" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="33"/>
       <c r="C8" s="67">
@@ -7357,7 +7391,7 @@
       <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
     </row>
-    <row r="9" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="33"/>
       <c r="C9" s="67">
@@ -7390,7 +7424,7 @@
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
     </row>
-    <row r="10" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="33"/>
       <c r="C10" s="67">
@@ -7423,7 +7457,7 @@
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
     </row>
-    <row r="11" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="33"/>
       <c r="C11" s="67">
@@ -7456,7 +7490,7 @@
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
     </row>
-    <row r="12" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="33"/>
       <c r="C12" s="67">
@@ -7493,7 +7527,7 @@
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
     </row>
-    <row r="13" spans="1:28" ht="11.45" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" ht="11.45" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="33" t="s">
         <v>20</v>
@@ -7528,7 +7562,7 @@
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
     </row>
-    <row r="14" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" hidden="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="33"/>
       <c r="C14" s="67">
@@ -7561,7 +7595,7 @@
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
     </row>
-    <row r="15" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" hidden="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="33"/>
       <c r="C15" s="67">
@@ -7666,7 +7700,7 @@
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
     </row>
-    <row r="18" spans="1:28" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" ht="45" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="33"/>
       <c r="C18" s="67">
@@ -7680,22 +7714,22 @@
       <c r="H18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I18" s="178">
+      <c r="I18" s="162">
         <v>44285</v>
       </c>
-      <c r="J18" s="162" t="s">
-        <v>275</v>
-      </c>
-      <c r="K18" s="163"/>
-      <c r="L18" s="163"/>
-      <c r="M18" s="163"/>
-      <c r="N18" s="163"/>
-      <c r="O18" s="163"/>
-      <c r="P18" s="163"/>
-      <c r="Q18" s="163"/>
-      <c r="R18" s="163"/>
-      <c r="S18" s="163"/>
-      <c r="T18" s="164"/>
+      <c r="J18" s="163" t="s">
+        <v>274</v>
+      </c>
+      <c r="K18" s="164"/>
+      <c r="L18" s="164"/>
+      <c r="M18" s="164"/>
+      <c r="N18" s="164"/>
+      <c r="O18" s="164"/>
+      <c r="P18" s="164"/>
+      <c r="Q18" s="164"/>
+      <c r="R18" s="164"/>
+      <c r="S18" s="164"/>
+      <c r="T18" s="165"/>
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
       <c r="W18" s="2"/>
@@ -7705,7 +7739,7 @@
       <c r="AA18" s="1"/>
       <c r="AB18" s="1"/>
     </row>
-    <row r="19" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="33"/>
       <c r="C19" s="67">
@@ -7738,7 +7772,7 @@
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
     </row>
-    <row r="20" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="33"/>
       <c r="C20" s="67">
@@ -7771,7 +7805,7 @@
       <c r="AA20" s="1"/>
       <c r="AB20" s="1"/>
     </row>
-    <row r="21" spans="1:28" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" ht="45" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="33"/>
       <c r="C21" s="67">
@@ -7786,21 +7820,21 @@
         <v>17</v>
       </c>
       <c r="I21" s="161">
-        <v>44284</v>
-      </c>
-      <c r="J21" s="165" t="s">
-        <v>273</v>
-      </c>
-      <c r="K21" s="166"/>
-      <c r="L21" s="166"/>
-      <c r="M21" s="166"/>
-      <c r="N21" s="166"/>
-      <c r="O21" s="166"/>
-      <c r="P21" s="166"/>
-      <c r="Q21" s="166"/>
-      <c r="R21" s="166"/>
-      <c r="S21" s="166"/>
-      <c r="T21" s="166"/>
+        <v>44286</v>
+      </c>
+      <c r="J21" s="166" t="s">
+        <v>275</v>
+      </c>
+      <c r="K21" s="167"/>
+      <c r="L21" s="167"/>
+      <c r="M21" s="167"/>
+      <c r="N21" s="167"/>
+      <c r="O21" s="167"/>
+      <c r="P21" s="167"/>
+      <c r="Q21" s="167"/>
+      <c r="R21" s="167"/>
+      <c r="S21" s="167"/>
+      <c r="T21" s="167"/>
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
       <c r="W21" s="2"/>
@@ -7810,7 +7844,7 @@
       <c r="AA21" s="1"/>
       <c r="AB21" s="1"/>
     </row>
-    <row r="22" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="33"/>
       <c r="C22" s="67">
@@ -7843,7 +7877,7 @@
       <c r="AA22" s="1"/>
       <c r="AB22" s="1"/>
     </row>
-    <row r="23" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="33"/>
       <c r="C23" s="67">
@@ -7876,7 +7910,7 @@
       <c r="AA23" s="1"/>
       <c r="AB23" s="1"/>
     </row>
-    <row r="24" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="33"/>
       <c r="C24" s="67">
@@ -7911,7 +7945,7 @@
       <c r="AA24" s="1"/>
       <c r="AB24" s="1"/>
     </row>
-    <row r="25" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="33"/>
       <c r="C25" s="67">
@@ -7946,7 +7980,7 @@
       <c r="AA25" s="1"/>
       <c r="AB25" s="1"/>
     </row>
-    <row r="26" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="33"/>
       <c r="C26" s="67">
@@ -7993,7 +8027,7 @@
       <c r="AA26" s="1"/>
       <c r="AB26" s="1"/>
     </row>
-    <row r="27" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="33"/>
       <c r="C27" s="67">
@@ -8030,7 +8064,7 @@
       <c r="AA27" s="1"/>
       <c r="AB27" s="1"/>
     </row>
-    <row r="28" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="33"/>
       <c r="C28" s="67">
@@ -8067,7 +8101,7 @@
       <c r="AA28" s="1"/>
       <c r="AB28" s="1"/>
     </row>
-    <row r="29" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="33"/>
       <c r="C29" s="67">
@@ -8104,7 +8138,7 @@
       <c r="AA29" s="1"/>
       <c r="AB29" s="1"/>
     </row>
-    <row r="30" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="33"/>
       <c r="C30" s="67">
@@ -8141,7 +8175,7 @@
       <c r="AA30" s="1"/>
       <c r="AB30" s="1"/>
     </row>
-    <row r="31" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="33"/>
       <c r="C31" s="67">
@@ -8176,7 +8210,7 @@
       <c r="AA31" s="1"/>
       <c r="AB31" s="1"/>
     </row>
-    <row r="32" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="33"/>
       <c r="C32" s="67">
@@ -8244,7 +8278,7 @@
       <c r="AA33" s="1"/>
       <c r="AB33" s="1"/>
     </row>
-    <row r="34" spans="1:28" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28" ht="5.0999999999999996" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="19"/>
       <c r="C34" s="71">
@@ -8277,7 +8311,7 @@
       <c r="AA34" s="1"/>
       <c r="AB34" s="1"/>
     </row>
-    <row r="35" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:28" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="67">
@@ -8310,7 +8344,7 @@
       <c r="AA35" s="1"/>
       <c r="AB35" s="1"/>
     </row>
-    <row r="36" spans="1:28" s="135" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28" s="135" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="73">
@@ -12953,7 +12987,7 @@
       <c r="F157" s="5"/>
       <c r="G157" s="4"/>
       <c r="H157" s="64" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I157" s="2"/>
       <c r="J157" s="2"/>
@@ -15997,37 +16031,37 @@
       <c r="J210" s="49"/>
       <c r="K210" s="49"/>
       <c r="L210" s="94" t="s">
-        <v>48</v>
+        <v>276</v>
       </c>
       <c r="M210" s="94" t="s">
-        <v>82</v>
-      </c>
-      <c r="N210" s="94">
-        <v>11</v>
-      </c>
-      <c r="O210" s="94">
-        <v>22</v>
-      </c>
-      <c r="P210" s="94">
-        <v>33</v>
-      </c>
-      <c r="Q210" s="94">
-        <v>21</v>
-      </c>
-      <c r="R210" s="94">
-        <v>32</v>
-      </c>
-      <c r="S210" s="94">
-        <v>31</v>
-      </c>
-      <c r="T210" s="94">
-        <v>10</v>
-      </c>
-      <c r="U210" s="94">
-        <v>20</v>
-      </c>
-      <c r="V210" s="94">
-        <v>30</v>
+        <v>277</v>
+      </c>
+      <c r="N210" s="94" t="s">
+        <v>278</v>
+      </c>
+      <c r="O210" s="94" t="s">
+        <v>279</v>
+      </c>
+      <c r="P210" s="94" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q210" s="94" t="s">
+        <v>281</v>
+      </c>
+      <c r="R210" s="94" t="s">
+        <v>282</v>
+      </c>
+      <c r="S210" s="94" t="s">
+        <v>283</v>
+      </c>
+      <c r="T210" s="94" t="s">
+        <v>284</v>
+      </c>
+      <c r="U210" s="94" t="s">
+        <v>285</v>
+      </c>
+      <c r="V210" s="94" t="s">
+        <v>286</v>
       </c>
       <c r="W210" s="94"/>
       <c r="X210" s="4"/>
@@ -16056,11 +16090,11 @@
         <v>1</v>
       </c>
       <c r="L211" s="140" t="str">
-        <f t="shared" ref="L211:V212" si="5">L$210&amp;"-"&amp;$K211</f>
+        <f>LEFT(L$210,LEN(L$210)-1)&amp;$K211</f>
         <v>NM-1</v>
       </c>
       <c r="M211" s="140" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="M211:V212" si="5">LEFT(M$210,LEN(M$210)-1)&amp;$K211</f>
         <v>00-1</v>
       </c>
       <c r="N211" s="94" t="str">
@@ -16126,7 +16160,7 @@
         <v>2</v>
       </c>
       <c r="L212" s="140" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="L212:V212" si="6">LEFT(L$210,LEN(L$210)-1)&amp;$K212</f>
         <v>NM-2</v>
       </c>
       <c r="M212" s="140" t="str">
@@ -16266,7 +16300,7 @@
       <c r="A215" s="1"/>
       <c r="B215" s="33"/>
       <c r="C215" s="73">
-        <f t="shared" ref="C215:C274" si="6">INT($C$140)+3</f>
+        <f t="shared" ref="C215:C274" si="7">INT($C$140)+3</f>
         <v>4</v>
       </c>
       <c r="D215" s="4"/>
@@ -16329,7 +16363,7 @@
       <c r="A216" s="1"/>
       <c r="B216" s="33"/>
       <c r="C216" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D216" s="4"/>
@@ -16392,7 +16426,7 @@
       <c r="A217" s="1"/>
       <c r="B217" s="33"/>
       <c r="C217" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D217" s="4"/>
@@ -16449,7 +16483,7 @@
       <c r="A218" s="1"/>
       <c r="B218" s="33"/>
       <c r="C218" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D218" s="4"/>
@@ -16508,7 +16542,7 @@
       <c r="A219" s="1"/>
       <c r="B219" s="33"/>
       <c r="C219" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D219" s="4"/>
@@ -16567,7 +16601,7 @@
       <c r="A220" s="1"/>
       <c r="B220" s="33"/>
       <c r="C220" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D220" s="4"/>
@@ -16628,7 +16662,7 @@
       <c r="A221" s="1"/>
       <c r="B221" s="33"/>
       <c r="C221" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D221" s="4"/>
@@ -16689,7 +16723,7 @@
       <c r="A222" s="1"/>
       <c r="B222" s="33"/>
       <c r="C222" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D222" s="4"/>
@@ -16746,7 +16780,7 @@
       <c r="A223" s="1"/>
       <c r="B223" s="33"/>
       <c r="C223" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D223" s="4"/>
@@ -16803,7 +16837,7 @@
       <c r="A224" s="1"/>
       <c r="B224" s="33"/>
       <c r="C224" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D224" s="4"/>
@@ -16860,7 +16894,7 @@
       <c r="A225" s="1"/>
       <c r="B225" s="33"/>
       <c r="C225" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D225" s="4"/>
@@ -16919,7 +16953,7 @@
       <c r="A226" s="1"/>
       <c r="B226" s="33"/>
       <c r="C226" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D226" s="4"/>
@@ -16978,7 +17012,7 @@
       <c r="A227" s="1"/>
       <c r="B227" s="33"/>
       <c r="C227" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D227" s="4"/>
@@ -17035,7 +17069,7 @@
       <c r="A228" s="1"/>
       <c r="B228" s="33"/>
       <c r="C228" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D228" s="4"/>
@@ -17092,7 +17126,7 @@
       <c r="A229" s="1"/>
       <c r="B229" s="33"/>
       <c r="C229" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D229" s="4"/>
@@ -17149,7 +17183,7 @@
       <c r="A230" s="1"/>
       <c r="B230" s="33"/>
       <c r="C230" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D230" s="4"/>
@@ -17208,7 +17242,7 @@
       <c r="A231" s="1"/>
       <c r="B231" s="33"/>
       <c r="C231" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D231" s="4"/>
@@ -17267,7 +17301,7 @@
       <c r="A232" s="1"/>
       <c r="B232" s="33"/>
       <c r="C232" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D232" s="4"/>
@@ -17324,7 +17358,7 @@
       <c r="A233" s="1"/>
       <c r="B233" s="33"/>
       <c r="C233" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D233" s="4"/>
@@ -17381,7 +17415,7 @@
       <c r="A234" s="1"/>
       <c r="B234" s="33"/>
       <c r="C234" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D234" s="4"/>
@@ -17438,7 +17472,7 @@
       <c r="A235" s="1"/>
       <c r="B235" s="33"/>
       <c r="C235" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D235" s="4"/>
@@ -17462,39 +17496,39 @@
         <v>1</v>
       </c>
       <c r="N235" s="128">
-        <f t="shared" ref="N235:V235" si="7">M235</f>
+        <f t="shared" ref="N235:V235" si="8">M235</f>
         <v>1</v>
       </c>
       <c r="O235" s="128">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P235" s="128">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="Q235" s="128">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="R235" s="128">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="S235" s="128">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="T235" s="128">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="U235" s="128">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="V235" s="128">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="W235" s="2"/>
@@ -17508,7 +17542,7 @@
       <c r="A236" s="1"/>
       <c r="B236" s="33"/>
       <c r="C236" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D236" s="4"/>
@@ -17533,35 +17567,35 @@
         <v>2</v>
       </c>
       <c r="O236" s="128">
-        <f t="shared" ref="O236:V236" si="8">N236</f>
+        <f t="shared" ref="O236:V236" si="9">N236</f>
         <v>2</v>
       </c>
       <c r="P236" s="128">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="Q236" s="128">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="R236" s="128">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="S236" s="128">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="T236" s="128">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="U236" s="128">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="V236" s="128">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="W236" s="2"/>
@@ -17575,7 +17609,7 @@
       <c r="A237" s="1"/>
       <c r="B237" s="33"/>
       <c r="C237" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D237" s="4"/>
@@ -17616,15 +17650,15 @@
         <v>3</v>
       </c>
       <c r="T237" s="131">
-        <f t="shared" ref="T237:V238" si="9">N237</f>
+        <f t="shared" ref="T237:V238" si="10">N237</f>
         <v>2</v>
       </c>
       <c r="U237" s="131">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="V237" s="131">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="W237" s="2"/>
@@ -17638,7 +17672,7 @@
       <c r="A238" s="1"/>
       <c r="B238" s="33"/>
       <c r="C238" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D238" s="4"/>
@@ -17679,15 +17713,15 @@
         <v>4</v>
       </c>
       <c r="T238" s="131">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="U238" s="131">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="V238" s="131">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="W238" s="2"/>
@@ -17701,7 +17735,7 @@
       <c r="A239" s="1"/>
       <c r="B239" s="33"/>
       <c r="C239" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D239" s="4"/>
@@ -17722,39 +17756,39 @@
         <v>1</v>
       </c>
       <c r="N239" s="136">
-        <f t="shared" ref="N239:V239" si="10">N238</f>
+        <f t="shared" ref="N239:V239" si="11">N238</f>
         <v>2</v>
       </c>
       <c r="O239" s="136">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="P239" s="136">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="Q239" s="136">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="R239" s="136">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="S239" s="136">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="T239" s="136">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="U239" s="136">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="V239" s="136">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="W239" s="2"/>
@@ -17768,7 +17802,7 @@
       <c r="A240" s="1"/>
       <c r="B240" s="33"/>
       <c r="C240" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D240" s="4"/>
@@ -17791,39 +17825,39 @@
         <v>1</v>
       </c>
       <c r="N240" s="132">
-        <f t="shared" ref="N240:V240" si="11">N235</f>
+        <f t="shared" ref="N240:V240" si="12">N235</f>
         <v>1</v>
       </c>
       <c r="O240" s="132">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="P240" s="132">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="Q240" s="132">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="R240" s="132">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="S240" s="132">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="T240" s="132">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="U240" s="132">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="V240" s="132">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="W240" s="2"/>
@@ -17837,7 +17871,7 @@
       <c r="A241" s="1"/>
       <c r="B241" s="33"/>
       <c r="C241" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D241" s="4"/>
@@ -17854,43 +17888,43 @@
         <v>0</v>
       </c>
       <c r="M241" s="132">
-        <f t="shared" ref="M241:V241" si="12">M236</f>
+        <f t="shared" ref="M241:V241" si="13">M236</f>
         <v>1</v>
       </c>
       <c r="N241" s="132">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2</v>
       </c>
       <c r="O241" s="132">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2</v>
       </c>
       <c r="P241" s="132">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2</v>
       </c>
       <c r="Q241" s="132">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2</v>
       </c>
       <c r="R241" s="132">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2</v>
       </c>
       <c r="S241" s="132">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2</v>
       </c>
       <c r="T241" s="132">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2</v>
       </c>
       <c r="U241" s="132">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2</v>
       </c>
       <c r="V241" s="132">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2</v>
       </c>
       <c r="W241" s="2"/>
@@ -17904,7 +17938,7 @@
       <c r="A242" s="1"/>
       <c r="B242" s="33"/>
       <c r="C242" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D242" s="4"/>
@@ -17921,43 +17955,43 @@
         <v>0</v>
       </c>
       <c r="M242" s="132">
-        <f t="shared" ref="M242:V242" si="13">M237</f>
+        <f t="shared" ref="M242:V242" si="14">M237</f>
         <v>1</v>
       </c>
       <c r="N242" s="132">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="O242" s="132">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3</v>
       </c>
       <c r="P242" s="132">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3</v>
       </c>
       <c r="Q242" s="132">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3</v>
       </c>
       <c r="R242" s="132">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3</v>
       </c>
       <c r="S242" s="132">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3</v>
       </c>
       <c r="T242" s="132">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="U242" s="132">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3</v>
       </c>
       <c r="V242" s="132">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3</v>
       </c>
       <c r="W242" s="2"/>
@@ -17971,7 +18005,7 @@
       <c r="A243" s="1"/>
       <c r="B243" s="33"/>
       <c r="C243" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D243" s="4"/>
@@ -17988,43 +18022,43 @@
         <v>0</v>
       </c>
       <c r="M243" s="132">
-        <f t="shared" ref="M243:V243" si="14">M238</f>
+        <f t="shared" ref="M243:V243" si="15">M238</f>
         <v>1</v>
       </c>
       <c r="N243" s="132">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2</v>
       </c>
       <c r="O243" s="132">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>3</v>
       </c>
       <c r="P243" s="132">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>4</v>
       </c>
       <c r="Q243" s="132">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>3</v>
       </c>
       <c r="R243" s="132">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>4</v>
       </c>
       <c r="S243" s="132">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>4</v>
       </c>
       <c r="T243" s="132">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2</v>
       </c>
       <c r="U243" s="132">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>3</v>
       </c>
       <c r="V243" s="132">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>4</v>
       </c>
       <c r="W243" s="2"/>
@@ -18038,7 +18072,7 @@
       <c r="A244" s="1"/>
       <c r="B244" s="33"/>
       <c r="C244" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D244" s="4"/>
@@ -18055,43 +18089,43 @@
         <v>0</v>
       </c>
       <c r="M244" s="136">
-        <f t="shared" ref="M244:V244" si="15">M243</f>
+        <f t="shared" ref="M244:V244" si="16">M243</f>
         <v>1</v>
       </c>
       <c r="N244" s="136">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="O244" s="136">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>3</v>
       </c>
       <c r="P244" s="136">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>4</v>
       </c>
       <c r="Q244" s="136">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>3</v>
       </c>
       <c r="R244" s="136">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>4</v>
       </c>
       <c r="S244" s="136">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>4</v>
       </c>
       <c r="T244" s="136">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="U244" s="136">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>3</v>
       </c>
       <c r="V244" s="136">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>4</v>
       </c>
       <c r="W244" s="2"/>
@@ -18105,7 +18139,7 @@
       <c r="A245" s="1"/>
       <c r="B245" s="33"/>
       <c r="C245" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D245" s="4"/>
@@ -18124,43 +18158,43 @@
         <v>0</v>
       </c>
       <c r="M245" s="132">
-        <f t="shared" ref="M245:V245" si="16">M240</f>
+        <f t="shared" ref="M245:V245" si="17">M240</f>
         <v>1</v>
       </c>
       <c r="N245" s="132">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
       <c r="O245" s="132">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
       <c r="P245" s="132">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
       <c r="Q245" s="132">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
       <c r="R245" s="132">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
       <c r="S245" s="132">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
       <c r="T245" s="132">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
       <c r="U245" s="132">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
       <c r="V245" s="132">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
       <c r="W245" s="2"/>
@@ -18174,7 +18208,7 @@
       <c r="A246" s="1"/>
       <c r="B246" s="33"/>
       <c r="C246" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D246" s="4"/>
@@ -18191,43 +18225,43 @@
         <v>0</v>
       </c>
       <c r="M246" s="132">
-        <f t="shared" ref="M246:V246" si="17">M241</f>
+        <f t="shared" ref="M246:V246" si="18">M241</f>
         <v>1</v>
       </c>
       <c r="N246" s="132">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2</v>
       </c>
       <c r="O246" s="132">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2</v>
       </c>
       <c r="P246" s="132">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2</v>
       </c>
       <c r="Q246" s="132">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2</v>
       </c>
       <c r="R246" s="132">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2</v>
       </c>
       <c r="S246" s="132">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2</v>
       </c>
       <c r="T246" s="132">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2</v>
       </c>
       <c r="U246" s="132">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2</v>
       </c>
       <c r="V246" s="132">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2</v>
       </c>
       <c r="W246" s="2"/>
@@ -18241,7 +18275,7 @@
       <c r="A247" s="1"/>
       <c r="B247" s="33"/>
       <c r="C247" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D247" s="4"/>
@@ -18258,43 +18292,43 @@
         <v>0</v>
       </c>
       <c r="M247" s="132">
-        <f t="shared" ref="M247:V247" si="18">M242</f>
+        <f t="shared" ref="M247:V247" si="19">M242</f>
         <v>1</v>
       </c>
       <c r="N247" s="132">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>2</v>
       </c>
       <c r="O247" s="132">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>3</v>
       </c>
       <c r="P247" s="132">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>3</v>
       </c>
       <c r="Q247" s="132">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>3</v>
       </c>
       <c r="R247" s="132">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>3</v>
       </c>
       <c r="S247" s="132">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>3</v>
       </c>
       <c r="T247" s="132">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>2</v>
       </c>
       <c r="U247" s="132">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>3</v>
       </c>
       <c r="V247" s="132">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>3</v>
       </c>
       <c r="W247" s="2"/>
@@ -18308,7 +18342,7 @@
       <c r="A248" s="1"/>
       <c r="B248" s="33"/>
       <c r="C248" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D248" s="4"/>
@@ -18325,43 +18359,43 @@
         <v>0</v>
       </c>
       <c r="M248" s="132">
-        <f t="shared" ref="M248:V248" si="19">M243</f>
+        <f t="shared" ref="M248:V248" si="20">M243</f>
         <v>1</v>
       </c>
       <c r="N248" s="132">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>2</v>
       </c>
       <c r="O248" s="132">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>3</v>
       </c>
       <c r="P248" s="132">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>4</v>
       </c>
       <c r="Q248" s="132">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>3</v>
       </c>
       <c r="R248" s="132">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>4</v>
       </c>
       <c r="S248" s="132">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>4</v>
       </c>
       <c r="T248" s="132">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>2</v>
       </c>
       <c r="U248" s="132">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>3</v>
       </c>
       <c r="V248" s="132">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>4</v>
       </c>
       <c r="W248" s="2"/>
@@ -18375,7 +18409,7 @@
       <c r="A249" s="1"/>
       <c r="B249" s="33"/>
       <c r="C249" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D249" s="4"/>
@@ -18392,43 +18426,43 @@
         <v>0</v>
       </c>
       <c r="M249" s="136">
-        <f t="shared" ref="M249:V249" si="20">M248</f>
+        <f t="shared" ref="M249:V249" si="21">M248</f>
         <v>1</v>
       </c>
       <c r="N249" s="136">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
       <c r="O249" s="136">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>3</v>
       </c>
       <c r="P249" s="136">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>4</v>
       </c>
       <c r="Q249" s="136">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>3</v>
       </c>
       <c r="R249" s="136">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>4</v>
       </c>
       <c r="S249" s="136">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>4</v>
       </c>
       <c r="T249" s="136">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
       <c r="U249" s="136">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>3</v>
       </c>
       <c r="V249" s="136">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>4</v>
       </c>
       <c r="W249" s="2"/>
@@ -18442,7 +18476,7 @@
       <c r="A250" s="1"/>
       <c r="B250" s="33"/>
       <c r="C250" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D250" s="4"/>
@@ -18461,43 +18495,43 @@
         <v>0</v>
       </c>
       <c r="M250" s="132">
-        <f t="shared" ref="M250:V250" si="21">M245</f>
+        <f t="shared" ref="M250:V250" si="22">M245</f>
         <v>1</v>
       </c>
       <c r="N250" s="132">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="O250" s="132">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="P250" s="132">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="Q250" s="132">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="R250" s="132">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="S250" s="132">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="T250" s="132">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="U250" s="132">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="V250" s="132">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="W250" s="2"/>
@@ -18511,7 +18545,7 @@
       <c r="A251" s="1"/>
       <c r="B251" s="33"/>
       <c r="C251" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D251" s="4"/>
@@ -18528,43 +18562,43 @@
         <v>0</v>
       </c>
       <c r="M251" s="132">
-        <f t="shared" ref="M251:V251" si="22">M246</f>
+        <f t="shared" ref="M251:V251" si="23">M246</f>
         <v>1</v>
       </c>
       <c r="N251" s="132">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>2</v>
       </c>
       <c r="O251" s="132">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>2</v>
       </c>
       <c r="P251" s="132">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>2</v>
       </c>
       <c r="Q251" s="132">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>2</v>
       </c>
       <c r="R251" s="132">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>2</v>
       </c>
       <c r="S251" s="132">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>2</v>
       </c>
       <c r="T251" s="132">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>2</v>
       </c>
       <c r="U251" s="132">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>2</v>
       </c>
       <c r="V251" s="132">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>2</v>
       </c>
       <c r="W251" s="2"/>
@@ -18578,7 +18612,7 @@
       <c r="A252" s="1"/>
       <c r="B252" s="33"/>
       <c r="C252" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D252" s="4"/>
@@ -18595,43 +18629,43 @@
         <v>0</v>
       </c>
       <c r="M252" s="132">
-        <f t="shared" ref="M252:V252" si="23">M247</f>
+        <f t="shared" ref="M252:V252" si="24">M247</f>
         <v>1</v>
       </c>
       <c r="N252" s="132">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>2</v>
       </c>
       <c r="O252" s="132">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>3</v>
       </c>
       <c r="P252" s="132">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>3</v>
       </c>
       <c r="Q252" s="132">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>3</v>
       </c>
       <c r="R252" s="132">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>3</v>
       </c>
       <c r="S252" s="132">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>3</v>
       </c>
       <c r="T252" s="132">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>2</v>
       </c>
       <c r="U252" s="132">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>3</v>
       </c>
       <c r="V252" s="132">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>3</v>
       </c>
       <c r="W252" s="2"/>
@@ -18645,7 +18679,7 @@
       <c r="A253" s="1"/>
       <c r="B253" s="33"/>
       <c r="C253" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D253" s="4"/>
@@ -18662,43 +18696,43 @@
         <v>0</v>
       </c>
       <c r="M253" s="132">
-        <f t="shared" ref="M253:V253" si="24">M248</f>
+        <f t="shared" ref="M253:V253" si="25">M248</f>
         <v>1</v>
       </c>
       <c r="N253" s="132">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>2</v>
       </c>
       <c r="O253" s="132">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>3</v>
       </c>
       <c r="P253" s="132">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>4</v>
       </c>
       <c r="Q253" s="132">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>3</v>
       </c>
       <c r="R253" s="132">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>4</v>
       </c>
       <c r="S253" s="132">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>4</v>
       </c>
       <c r="T253" s="132">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>2</v>
       </c>
       <c r="U253" s="132">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>3</v>
       </c>
       <c r="V253" s="132">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>4</v>
       </c>
       <c r="W253" s="2"/>
@@ -18712,7 +18746,7 @@
       <c r="A254" s="1"/>
       <c r="B254" s="33"/>
       <c r="C254" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D254" s="4"/>
@@ -18729,43 +18763,43 @@
         <v>0</v>
       </c>
       <c r="M254" s="136">
-        <f t="shared" ref="M254:V254" si="25">M253</f>
+        <f t="shared" ref="M254:V254" si="26">M253</f>
         <v>1</v>
       </c>
       <c r="N254" s="136">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>2</v>
       </c>
       <c r="O254" s="136">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>3</v>
       </c>
       <c r="P254" s="136">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>4</v>
       </c>
       <c r="Q254" s="136">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>3</v>
       </c>
       <c r="R254" s="136">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>4</v>
       </c>
       <c r="S254" s="136">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>4</v>
       </c>
       <c r="T254" s="136">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>2</v>
       </c>
       <c r="U254" s="136">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>3</v>
       </c>
       <c r="V254" s="136">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>4</v>
       </c>
       <c r="W254" s="2"/>
@@ -18779,7 +18813,7 @@
       <c r="A255" s="1"/>
       <c r="B255" s="33"/>
       <c r="C255" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D255" s="4"/>
@@ -18840,7 +18874,7 @@
       <c r="A256" s="1"/>
       <c r="B256" s="33"/>
       <c r="C256" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D256" s="4"/>
@@ -18897,7 +18931,7 @@
       <c r="A257" s="1"/>
       <c r="B257" s="33"/>
       <c r="C257" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D257" s="4"/>
@@ -18954,7 +18988,7 @@
       <c r="A258" s="1"/>
       <c r="B258" s="33"/>
       <c r="C258" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D258" s="4"/>
@@ -19011,7 +19045,7 @@
       <c r="A259" s="1"/>
       <c r="B259" s="33"/>
       <c r="C259" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D259" s="4"/>
@@ -19068,7 +19102,7 @@
       <c r="A260" s="1"/>
       <c r="B260" s="33"/>
       <c r="C260" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D260" s="4"/>
@@ -19091,39 +19125,39 @@
         <v>1</v>
       </c>
       <c r="N260" s="132">
-        <f t="shared" ref="N260:V260" si="26">N235</f>
+        <f t="shared" ref="N260:V260" si="27">N235</f>
         <v>1</v>
       </c>
       <c r="O260" s="132">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="P260" s="132">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="Q260" s="132">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="R260" s="132">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="S260" s="132">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="T260" s="132">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="U260" s="132">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="V260" s="132">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="W260" s="2"/>
@@ -19137,7 +19171,7 @@
       <c r="A261" s="1"/>
       <c r="B261" s="33"/>
       <c r="C261" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D261" s="4"/>
@@ -19154,43 +19188,43 @@
         <v>0</v>
       </c>
       <c r="M261" s="132">
-        <f t="shared" ref="M261:V261" si="27">M236</f>
+        <f t="shared" ref="M261:V261" si="28">M236</f>
         <v>1</v>
       </c>
       <c r="N261" s="132">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>2</v>
       </c>
       <c r="O261" s="132">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>2</v>
       </c>
       <c r="P261" s="132">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>2</v>
       </c>
       <c r="Q261" s="132">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>2</v>
       </c>
       <c r="R261" s="132">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>2</v>
       </c>
       <c r="S261" s="132">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>2</v>
       </c>
       <c r="T261" s="132">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>2</v>
       </c>
       <c r="U261" s="132">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>2</v>
       </c>
       <c r="V261" s="132">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>2</v>
       </c>
       <c r="W261" s="2"/>
@@ -19204,7 +19238,7 @@
       <c r="A262" s="1"/>
       <c r="B262" s="33"/>
       <c r="C262" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D262" s="4"/>
@@ -19221,43 +19255,43 @@
         <v>0</v>
       </c>
       <c r="M262" s="132">
-        <f t="shared" ref="M262:V262" si="28">M237</f>
+        <f t="shared" ref="M262:V262" si="29">M237</f>
         <v>1</v>
       </c>
       <c r="N262" s="132">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>2</v>
       </c>
       <c r="O262" s="132">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>3</v>
       </c>
       <c r="P262" s="132">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>3</v>
       </c>
       <c r="Q262" s="132">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>3</v>
       </c>
       <c r="R262" s="132">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>3</v>
       </c>
       <c r="S262" s="132">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>3</v>
       </c>
       <c r="T262" s="132">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>2</v>
       </c>
       <c r="U262" s="132">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>3</v>
       </c>
       <c r="V262" s="132">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>3</v>
       </c>
       <c r="W262" s="2"/>
@@ -19271,7 +19305,7 @@
       <c r="A263" s="1"/>
       <c r="B263" s="33"/>
       <c r="C263" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D263" s="4"/>
@@ -19288,43 +19322,43 @@
         <v>0</v>
       </c>
       <c r="M263" s="132">
-        <f t="shared" ref="M263:V263" si="29">M238</f>
+        <f t="shared" ref="M263:V263" si="30">M238</f>
         <v>1</v>
       </c>
       <c r="N263" s="132">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>2</v>
       </c>
       <c r="O263" s="132">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>3</v>
       </c>
       <c r="P263" s="132">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>4</v>
       </c>
       <c r="Q263" s="132">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>3</v>
       </c>
       <c r="R263" s="132">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>4</v>
       </c>
       <c r="S263" s="132">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>4</v>
       </c>
       <c r="T263" s="132">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>2</v>
       </c>
       <c r="U263" s="132">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>3</v>
       </c>
       <c r="V263" s="132">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>4</v>
       </c>
       <c r="W263" s="2"/>
@@ -19338,7 +19372,7 @@
       <c r="A264" s="1"/>
       <c r="B264" s="33"/>
       <c r="C264" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D264" s="4"/>
@@ -19355,43 +19389,43 @@
         <v>0</v>
       </c>
       <c r="M264" s="136">
-        <f t="shared" ref="M264:V264" si="30">M263</f>
+        <f t="shared" ref="M264:V264" si="31">M263</f>
         <v>1</v>
       </c>
       <c r="N264" s="136">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>2</v>
       </c>
       <c r="O264" s="136">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>3</v>
       </c>
       <c r="P264" s="136">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>4</v>
       </c>
       <c r="Q264" s="136">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>3</v>
       </c>
       <c r="R264" s="136">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>4</v>
       </c>
       <c r="S264" s="136">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>4</v>
       </c>
       <c r="T264" s="136">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>2</v>
       </c>
       <c r="U264" s="136">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>3</v>
       </c>
       <c r="V264" s="136">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>4</v>
       </c>
       <c r="W264" s="2"/>
@@ -19405,7 +19439,7 @@
       <c r="A265" s="1"/>
       <c r="B265" s="33"/>
       <c r="C265" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D265" s="4"/>
@@ -19464,7 +19498,7 @@
       <c r="A266" s="1"/>
       <c r="B266" s="33"/>
       <c r="C266" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D266" s="4"/>
@@ -19526,7 +19560,7 @@
       <c r="A267" s="1"/>
       <c r="B267" s="33"/>
       <c r="C267" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D267" s="4"/>
@@ -19587,7 +19621,7 @@
       <c r="A268" s="1"/>
       <c r="B268" s="33"/>
       <c r="C268" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D268" s="4"/>
@@ -19647,7 +19681,7 @@
       <c r="A269" s="1"/>
       <c r="B269" s="33"/>
       <c r="C269" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D269" s="4"/>
@@ -19664,43 +19698,43 @@
         <v>0</v>
       </c>
       <c r="M269" s="136">
-        <f t="shared" ref="M269:V269" si="31">M268</f>
+        <f t="shared" ref="M269:V269" si="32">M268</f>
         <v>1</v>
       </c>
       <c r="N269" s="136">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>2</v>
       </c>
       <c r="O269" s="136">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>3</v>
       </c>
       <c r="P269" s="136">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>4</v>
       </c>
       <c r="Q269" s="136">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>3</v>
       </c>
       <c r="R269" s="136">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>4</v>
       </c>
       <c r="S269" s="136">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>4</v>
       </c>
       <c r="T269" s="136">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>8</v>
       </c>
       <c r="U269" s="136">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>9</v>
       </c>
       <c r="V269" s="136">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>10</v>
       </c>
       <c r="W269" s="2"/>
@@ -19714,7 +19748,7 @@
       <c r="A270" s="1"/>
       <c r="B270" s="33"/>
       <c r="C270" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D270" s="4"/>
@@ -19779,7 +19813,7 @@
       <c r="A271" s="1"/>
       <c r="B271" s="33"/>
       <c r="C271" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D271" s="4"/>
@@ -19841,7 +19875,7 @@
       <c r="A272" s="1"/>
       <c r="B272" s="33"/>
       <c r="C272" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D272" s="4"/>
@@ -19901,7 +19935,7 @@
       <c r="A273" s="1"/>
       <c r="B273" s="33"/>
       <c r="C273" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D273" s="4"/>
@@ -19958,7 +19992,7 @@
       <c r="A274" s="1"/>
       <c r="B274" s="33"/>
       <c r="C274" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D274" s="4"/>
@@ -19975,43 +20009,43 @@
         <v>0</v>
       </c>
       <c r="M274" s="136">
-        <f t="shared" ref="M274:V274" si="32">M273</f>
+        <f t="shared" ref="M274:V274" si="33">M273</f>
         <v>1</v>
       </c>
       <c r="N274" s="136">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2</v>
       </c>
       <c r="O274" s="136">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>3</v>
       </c>
       <c r="P274" s="136">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>4</v>
       </c>
       <c r="Q274" s="136">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
       <c r="R274" s="136">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>6</v>
       </c>
       <c r="S274" s="136">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>7</v>
       </c>
       <c r="T274" s="136">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>8</v>
       </c>
       <c r="U274" s="136">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>9</v>
       </c>
       <c r="V274" s="136">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>10</v>
       </c>
       <c r="W274" s="2"/>
@@ -20074,29 +20108,29 @@
       </c>
       <c r="J276" s="49"/>
       <c r="K276" s="49"/>
-      <c r="L276" s="94">
-        <f t="shared" ref="L276:Q276" si="33">N210</f>
-        <v>11</v>
-      </c>
-      <c r="M276" s="94">
-        <f t="shared" si="33"/>
-        <v>22</v>
-      </c>
-      <c r="N276" s="94">
-        <f t="shared" si="33"/>
-        <v>33</v>
-      </c>
-      <c r="O276" s="94">
-        <f t="shared" si="33"/>
-        <v>21</v>
-      </c>
-      <c r="P276" s="94">
-        <f t="shared" si="33"/>
-        <v>32</v>
-      </c>
-      <c r="Q276" s="94">
-        <f t="shared" si="33"/>
-        <v>31</v>
+      <c r="L276" s="94" t="str">
+        <f t="shared" ref="L276:Q276" si="34">N210</f>
+        <v>11-0</v>
+      </c>
+      <c r="M276" s="94" t="str">
+        <f t="shared" si="34"/>
+        <v>22-0</v>
+      </c>
+      <c r="N276" s="94" t="str">
+        <f t="shared" si="34"/>
+        <v>33-0</v>
+      </c>
+      <c r="O276" s="94" t="str">
+        <f t="shared" si="34"/>
+        <v>21-0</v>
+      </c>
+      <c r="P276" s="94" t="str">
+        <f t="shared" si="34"/>
+        <v>32-0</v>
+      </c>
+      <c r="Q276" s="94" t="str">
+        <f t="shared" si="34"/>
+        <v>31-0</v>
       </c>
       <c r="R276" s="94"/>
       <c r="S276" s="94"/>
@@ -20128,27 +20162,27 @@
         <v>1</v>
       </c>
       <c r="L277" s="94" t="str">
-        <f t="shared" ref="L277:Q277" si="34">N211</f>
+        <f t="shared" ref="L277:Q277" si="35">N211</f>
         <v>11-1</v>
       </c>
       <c r="M277" s="94" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>22-1</v>
       </c>
       <c r="N277" s="94" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>33-1</v>
       </c>
       <c r="O277" s="94" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>21-1</v>
       </c>
       <c r="P277" s="94" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>32-1</v>
       </c>
       <c r="Q277" s="94" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>31-1</v>
       </c>
       <c r="R277" s="94"/>
@@ -20181,27 +20215,27 @@
         <v>2</v>
       </c>
       <c r="L278" s="94" t="str">
-        <f t="shared" ref="L278:Q278" si="35">N212</f>
+        <f t="shared" ref="L278:Q278" si="36">N212</f>
         <v>11-2</v>
       </c>
       <c r="M278" s="94" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>22-2</v>
       </c>
       <c r="N278" s="94" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>33-2</v>
       </c>
       <c r="O278" s="94" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>21-2</v>
       </c>
       <c r="P278" s="94" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>32-2</v>
       </c>
       <c r="Q278" s="94" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>31-2</v>
       </c>
       <c r="R278" s="94"/>
@@ -20305,7 +20339,7 @@
       <c r="A281" s="1"/>
       <c r="B281" s="33"/>
       <c r="C281" s="73">
-        <f t="shared" ref="C281:C300" si="36">INT($C$140)+3</f>
+        <f t="shared" ref="C281:C300" si="37">INT($C$140)+3</f>
         <v>4</v>
       </c>
       <c r="D281" s="4"/>
@@ -20340,11 +20374,11 @@
         <v>0</v>
       </c>
       <c r="P281" s="130">
-        <f t="shared" ref="P281:Q284" si="37">$N281</f>
+        <f t="shared" ref="P281:Q284" si="38">$N281</f>
         <v>0</v>
       </c>
       <c r="Q281" s="130">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="R281" s="55"/>
@@ -20363,7 +20397,7 @@
       <c r="A282" s="1"/>
       <c r="B282" s="33"/>
       <c r="C282" s="73">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>4</v>
       </c>
       <c r="D282" s="4"/>
@@ -20398,11 +20432,11 @@
         <v>0</v>
       </c>
       <c r="P282" s="130">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="Q282" s="130">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="R282" s="55"/>
@@ -20421,7 +20455,7 @@
       <c r="A283" s="1"/>
       <c r="B283" s="33"/>
       <c r="C283" s="73">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>4</v>
       </c>
       <c r="D283" s="4"/>
@@ -20451,11 +20485,11 @@
         <v>0</v>
       </c>
       <c r="P283" s="130">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="Q283" s="130">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="R283" s="55"/>
@@ -20474,7 +20508,7 @@
       <c r="A284" s="1"/>
       <c r="B284" s="33"/>
       <c r="C284" s="73">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>4</v>
       </c>
       <c r="D284" s="4"/>
@@ -20503,11 +20537,11 @@
         <v>0</v>
       </c>
       <c r="P284" s="130">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="Q284" s="130">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="R284" s="55"/>
@@ -20526,7 +20560,7 @@
       <c r="A285" s="1"/>
       <c r="B285" s="33"/>
       <c r="C285" s="73">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>4</v>
       </c>
       <c r="D285" s="4"/>
@@ -20542,27 +20576,27 @@
         <v>4</v>
       </c>
       <c r="L285" s="136">
-        <f t="shared" ref="L285:Q285" si="38">L284</f>
+        <f t="shared" ref="L285:Q285" si="39">L284</f>
         <v>0</v>
       </c>
       <c r="M285" s="136">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="N285" s="136">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="O285" s="136">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="P285" s="136">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Q285" s="136">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="R285" s="55"/>
@@ -20581,7 +20615,7 @@
       <c r="A286" s="1"/>
       <c r="B286" s="33"/>
       <c r="C286" s="73">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>4</v>
       </c>
       <c r="D286" s="4"/>
@@ -20612,11 +20646,11 @@
         <v>0</v>
       </c>
       <c r="P286" s="130">
-        <f t="shared" ref="P286:Q294" si="39">$N286</f>
+        <f t="shared" ref="P286:Q294" si="40">$N286</f>
         <v>0</v>
       </c>
       <c r="Q286" s="130">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="R286" s="2"/>
@@ -20635,7 +20669,7 @@
       <c r="A287" s="1"/>
       <c r="B287" s="33"/>
       <c r="C287" s="73">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>4</v>
       </c>
       <c r="D287" s="4"/>
@@ -20666,11 +20700,11 @@
         <v>0</v>
       </c>
       <c r="P287" s="130">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="Q287" s="130">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="R287" s="2"/>
@@ -20689,7 +20723,7 @@
       <c r="A288" s="1"/>
       <c r="B288" s="33"/>
       <c r="C288" s="73">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>4</v>
       </c>
       <c r="D288" s="4"/>
@@ -20716,11 +20750,11 @@
         <v>1</v>
       </c>
       <c r="P288" s="130">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>1</v>
       </c>
       <c r="Q288" s="130">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>1</v>
       </c>
       <c r="R288" s="2"/>
@@ -20739,7 +20773,7 @@
       <c r="A289" s="1"/>
       <c r="B289" s="33"/>
       <c r="C289" s="73">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>4</v>
       </c>
       <c r="D289" s="4"/>
@@ -20766,11 +20800,11 @@
         <v>1</v>
       </c>
       <c r="P289" s="130">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>2</v>
       </c>
       <c r="Q289" s="130">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>2</v>
       </c>
       <c r="R289" s="2"/>
@@ -20789,7 +20823,7 @@
       <c r="A290" s="1"/>
       <c r="B290" s="33"/>
       <c r="C290" s="73">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>4</v>
       </c>
       <c r="D290" s="4"/>
@@ -20803,27 +20837,27 @@
         <v>4</v>
       </c>
       <c r="L290" s="136">
-        <f t="shared" ref="L290:Q290" si="40">L289</f>
+        <f t="shared" ref="L290:Q290" si="41">L289</f>
         <v>0</v>
       </c>
       <c r="M290" s="136">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>1</v>
       </c>
       <c r="N290" s="136">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>2</v>
       </c>
       <c r="O290" s="136">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>1</v>
       </c>
       <c r="P290" s="136">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>2</v>
       </c>
       <c r="Q290" s="136">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>2</v>
       </c>
       <c r="R290" s="2"/>
@@ -20842,7 +20876,7 @@
       <c r="A291" s="1"/>
       <c r="B291" s="33"/>
       <c r="C291" s="73">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>4</v>
       </c>
       <c r="D291" s="4"/>
@@ -20873,11 +20907,11 @@
         <v>0</v>
       </c>
       <c r="P291" s="130">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="Q291" s="130">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="R291" s="55"/>
@@ -20896,7 +20930,7 @@
       <c r="A292" s="1"/>
       <c r="B292" s="33"/>
       <c r="C292" s="73">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>4</v>
       </c>
       <c r="D292" s="4"/>
@@ -20927,11 +20961,11 @@
         <v>0</v>
       </c>
       <c r="P292" s="130">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="Q292" s="130">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="R292" s="55"/>
@@ -20950,7 +20984,7 @@
       <c r="A293" s="1"/>
       <c r="B293" s="33"/>
       <c r="C293" s="73">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>4</v>
       </c>
       <c r="D293" s="4"/>
@@ -20977,11 +21011,11 @@
         <v>1</v>
       </c>
       <c r="P293" s="130">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>1</v>
       </c>
       <c r="Q293" s="130">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>1</v>
       </c>
       <c r="R293" s="55"/>
@@ -21000,7 +21034,7 @@
       <c r="A294" s="1"/>
       <c r="B294" s="33"/>
       <c r="C294" s="73">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>4</v>
       </c>
       <c r="D294" s="4"/>
@@ -21027,11 +21061,11 @@
         <v>1</v>
       </c>
       <c r="P294" s="130">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>2</v>
       </c>
       <c r="Q294" s="130">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>2</v>
       </c>
       <c r="R294" s="55"/>
@@ -21050,7 +21084,7 @@
       <c r="A295" s="1"/>
       <c r="B295" s="33"/>
       <c r="C295" s="73">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>4</v>
       </c>
       <c r="D295" s="4"/>
@@ -21064,27 +21098,27 @@
         <v>4</v>
       </c>
       <c r="L295" s="136">
-        <f t="shared" ref="L295:Q295" si="41">L294</f>
+        <f t="shared" ref="L295:Q295" si="42">L294</f>
         <v>0</v>
       </c>
       <c r="M295" s="136">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>1</v>
       </c>
       <c r="N295" s="136">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>2</v>
       </c>
       <c r="O295" s="136">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>1</v>
       </c>
       <c r="P295" s="136">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>2</v>
       </c>
       <c r="Q295" s="136">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>2</v>
       </c>
       <c r="R295" s="55"/>
@@ -21103,7 +21137,7 @@
       <c r="A296" s="1"/>
       <c r="B296" s="33"/>
       <c r="C296" s="73">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>4</v>
       </c>
       <c r="D296" s="4"/>
@@ -21155,7 +21189,7 @@
       <c r="A297" s="1"/>
       <c r="B297" s="33"/>
       <c r="C297" s="73">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>4</v>
       </c>
       <c r="D297" s="4"/>
@@ -21207,7 +21241,7 @@
       <c r="A298" s="1"/>
       <c r="B298" s="33"/>
       <c r="C298" s="73">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>4</v>
       </c>
       <c r="D298" s="4"/>
@@ -21256,7 +21290,7 @@
       <c r="A299" s="1"/>
       <c r="B299" s="33"/>
       <c r="C299" s="73">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>4</v>
       </c>
       <c r="D299" s="4"/>
@@ -21303,7 +21337,7 @@
       <c r="A300" s="1"/>
       <c r="B300" s="33"/>
       <c r="C300" s="73">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>4</v>
       </c>
       <c r="D300" s="4"/>
@@ -21317,27 +21351,27 @@
         <v>4</v>
       </c>
       <c r="L300" s="136">
-        <f t="shared" ref="L300:Q300" si="42">L299</f>
+        <f t="shared" ref="L300:Q300" si="43">L299</f>
         <v>0</v>
       </c>
       <c r="M300" s="136">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>1</v>
       </c>
       <c r="N300" s="136">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>2</v>
       </c>
       <c r="O300" s="136">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>3</v>
       </c>
       <c r="P300" s="136">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>4</v>
       </c>
       <c r="Q300" s="136">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>5</v>
       </c>
       <c r="R300" s="2"/>
@@ -22150,7 +22184,7 @@
       <c r="A323" s="1"/>
       <c r="B323" s="33"/>
       <c r="C323" s="73">
-        <f t="shared" ref="C323:C326" si="43">INT($C$310)+3</f>
+        <f t="shared" ref="C323:C326" si="44">INT($C$310)+3</f>
         <v>4</v>
       </c>
       <c r="D323" s="4"/>
@@ -22215,14 +22249,14 @@
         <v>3</v>
       </c>
       <c r="Q324" s="119"/>
-      <c r="R324" s="167" t="s">
+      <c r="R324" s="168" t="s">
         <v>156</v>
       </c>
-      <c r="S324" s="168"/>
-      <c r="T324" s="168"/>
-      <c r="U324" s="168"/>
-      <c r="V324" s="168"/>
-      <c r="W324" s="169"/>
+      <c r="S324" s="169"/>
+      <c r="T324" s="169"/>
+      <c r="U324" s="169"/>
+      <c r="V324" s="169"/>
+      <c r="W324" s="170"/>
       <c r="X324" s="4"/>
       <c r="Y324" s="16"/>
       <c r="Z324" s="1"/>
@@ -22233,7 +22267,7 @@
       <c r="A325" s="1"/>
       <c r="B325" s="33"/>
       <c r="C325" s="73">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>4</v>
       </c>
       <c r="D325" s="4"/>
@@ -22260,12 +22294,12 @@
         <v>1</v>
       </c>
       <c r="Q325" s="2"/>
-      <c r="R325" s="170"/>
-      <c r="S325" s="171"/>
-      <c r="T325" s="171"/>
-      <c r="U325" s="171"/>
-      <c r="V325" s="171"/>
-      <c r="W325" s="172"/>
+      <c r="R325" s="171"/>
+      <c r="S325" s="172"/>
+      <c r="T325" s="172"/>
+      <c r="U325" s="172"/>
+      <c r="V325" s="172"/>
+      <c r="W325" s="173"/>
       <c r="X325" s="4"/>
       <c r="Y325" s="16"/>
       <c r="Z325" s="1"/>
@@ -22276,7 +22310,7 @@
       <c r="A326" s="1"/>
       <c r="B326" s="33"/>
       <c r="C326" s="73">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>4</v>
       </c>
       <c r="D326" s="4"/>
@@ -22303,12 +22337,12 @@
         <v>1</v>
       </c>
       <c r="Q326" s="2"/>
-      <c r="R326" s="170"/>
-      <c r="S326" s="171"/>
-      <c r="T326" s="171"/>
-      <c r="U326" s="171"/>
-      <c r="V326" s="171"/>
-      <c r="W326" s="172"/>
+      <c r="R326" s="171"/>
+      <c r="S326" s="172"/>
+      <c r="T326" s="172"/>
+      <c r="U326" s="172"/>
+      <c r="V326" s="172"/>
+      <c r="W326" s="173"/>
       <c r="X326" s="4"/>
       <c r="Y326" s="16"/>
       <c r="Z326" s="1"/>
@@ -22465,7 +22499,7 @@
       <c r="A331" s="1"/>
       <c r="B331" s="33"/>
       <c r="C331" s="73">
-        <f t="shared" ref="C331:C351" si="44">INT($C$310)+3</f>
+        <f t="shared" ref="C331:C351" si="45">INT($C$310)+3</f>
         <v>4</v>
       </c>
       <c r="D331" s="4"/>
@@ -22510,7 +22544,7 @@
       <c r="A332" s="1"/>
       <c r="B332" s="33"/>
       <c r="C332" s="73">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>4</v>
       </c>
       <c r="D332" s="4"/>
@@ -22557,7 +22591,7 @@
       <c r="A333" s="1"/>
       <c r="B333" s="33"/>
       <c r="C333" s="73">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>4</v>
       </c>
       <c r="D333" s="4"/>
@@ -22791,7 +22825,7 @@
       <c r="A338" s="1"/>
       <c r="B338" s="33"/>
       <c r="C338" s="73">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>4</v>
       </c>
       <c r="D338" s="4"/>
@@ -22830,7 +22864,7 @@
       <c r="A339" s="1"/>
       <c r="B339" s="33"/>
       <c r="C339" s="73">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>4</v>
       </c>
       <c r="D339" s="4"/>
@@ -22884,7 +22918,7 @@
         <v>0</v>
       </c>
       <c r="K340" s="31">
-        <f t="shared" ref="K340" si="45">L334</f>
+        <f t="shared" ref="K340" si="46">L334</f>
         <v>1</v>
       </c>
       <c r="L340" s="31">
@@ -22977,7 +23011,7 @@
       <c r="A343" s="1"/>
       <c r="B343" s="33"/>
       <c r="C343" s="73">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>4</v>
       </c>
       <c r="D343" s="4"/>
@@ -23018,7 +23052,7 @@
       <c r="A344" s="1"/>
       <c r="B344" s="33"/>
       <c r="C344" s="73">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>4</v>
       </c>
       <c r="D344" s="4"/>
@@ -23061,7 +23095,7 @@
       <c r="A345" s="1"/>
       <c r="B345" s="33"/>
       <c r="C345" s="73">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>4</v>
       </c>
       <c r="D345" s="4"/>
@@ -23231,7 +23265,7 @@
       <c r="A349" s="1"/>
       <c r="B349" s="33"/>
       <c r="C349" s="73">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>4</v>
       </c>
       <c r="D349" s="4"/>
@@ -23266,7 +23300,7 @@
       <c r="A350" s="1"/>
       <c r="B350" s="33"/>
       <c r="C350" s="73">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>4</v>
       </c>
       <c r="D350" s="4"/>
@@ -23284,13 +23318,13 @@
       <c r="N350" s="2"/>
       <c r="O350" s="2"/>
       <c r="P350" s="2"/>
-      <c r="Q350" s="173"/>
-      <c r="R350" s="174"/>
-      <c r="S350" s="174"/>
-      <c r="T350" s="174"/>
-      <c r="U350" s="174"/>
-      <c r="V350" s="174"/>
-      <c r="W350" s="175"/>
+      <c r="Q350" s="174"/>
+      <c r="R350" s="175"/>
+      <c r="S350" s="175"/>
+      <c r="T350" s="175"/>
+      <c r="U350" s="175"/>
+      <c r="V350" s="175"/>
+      <c r="W350" s="176"/>
       <c r="X350" s="4"/>
       <c r="Y350" s="16"/>
       <c r="Z350" s="1"/>
@@ -23301,7 +23335,7 @@
       <c r="A351" s="1"/>
       <c r="B351" s="33"/>
       <c r="C351" s="73">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>4</v>
       </c>
       <c r="D351" s="4"/>
@@ -24404,23 +24438,23 @@
       <c r="I18" s="31">
         <v>1</v>
       </c>
-      <c r="J18" s="176" t="s">
+      <c r="J18" s="177" t="s">
         <v>22</v>
       </c>
-      <c r="K18" s="176"/>
-      <c r="L18" s="176"/>
-      <c r="M18" s="176"/>
-      <c r="N18" s="176"/>
-      <c r="O18" s="176"/>
-      <c r="P18" s="176"/>
-      <c r="Q18" s="176"/>
-      <c r="R18" s="176"/>
-      <c r="S18" s="176"/>
-      <c r="T18" s="176"/>
-      <c r="U18" s="176"/>
-      <c r="V18" s="176"/>
-      <c r="W18" s="176"/>
-      <c r="X18" s="176"/>
+      <c r="K18" s="177"/>
+      <c r="L18" s="177"/>
+      <c r="M18" s="177"/>
+      <c r="N18" s="177"/>
+      <c r="O18" s="177"/>
+      <c r="P18" s="177"/>
+      <c r="Q18" s="177"/>
+      <c r="R18" s="177"/>
+      <c r="S18" s="177"/>
+      <c r="T18" s="177"/>
+      <c r="U18" s="177"/>
+      <c r="V18" s="177"/>
+      <c r="W18" s="177"/>
+      <c r="X18" s="177"/>
       <c r="Y18" s="2"/>
       <c r="Z18" s="4"/>
       <c r="AA18" s="16"/>
@@ -24515,23 +24549,23 @@
       <c r="I21" s="23">
         <v>1</v>
       </c>
-      <c r="J21" s="165" t="s">
+      <c r="J21" s="166" t="s">
         <v>34</v>
       </c>
-      <c r="K21" s="166"/>
-      <c r="L21" s="166"/>
-      <c r="M21" s="166"/>
-      <c r="N21" s="166"/>
-      <c r="O21" s="166"/>
-      <c r="P21" s="166"/>
-      <c r="Q21" s="166"/>
-      <c r="R21" s="166"/>
-      <c r="S21" s="166"/>
-      <c r="T21" s="166"/>
-      <c r="U21" s="166"/>
-      <c r="V21" s="166"/>
-      <c r="W21" s="166"/>
-      <c r="X21" s="177"/>
+      <c r="K21" s="167"/>
+      <c r="L21" s="167"/>
+      <c r="M21" s="167"/>
+      <c r="N21" s="167"/>
+      <c r="O21" s="167"/>
+      <c r="P21" s="167"/>
+      <c r="Q21" s="167"/>
+      <c r="R21" s="167"/>
+      <c r="S21" s="167"/>
+      <c r="T21" s="167"/>
+      <c r="U21" s="167"/>
+      <c r="V21" s="167"/>
+      <c r="W21" s="167"/>
+      <c r="X21" s="178"/>
       <c r="Y21" s="2"/>
       <c r="Z21" s="4"/>
       <c r="AA21" s="16"/>

</xml_diff>

<commit_message>
Formatting change. Set for FVP3 & 3N
</commit_message>
<xml_diff>
--- a/Structural.xlsx
+++ b/Structural.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F19FD2ED-EF4E-49FA-AFB9-2676191FF8E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D250FFA-640F-4922-8814-CE059F62FB04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
@@ -2018,48 +2018,51 @@
     <t>is dry</t>
   </si>
   <si>
-    <t>30Mar21: Added inputs for % dry and number dams mated
-2: 17Jul20-Added structural inputs table
-1: 1Apr19-Created the version control table</t>
-  </si>
-  <si>
-    <t>31Mar21: Change the index for the k2 cluster (for the seasonality model)
+    <t>NM-0</t>
+  </si>
+  <si>
+    <t>00-0</t>
+  </si>
+  <si>
+    <t>11-0</t>
+  </si>
+  <si>
+    <t>22-0</t>
+  </si>
+  <si>
+    <t>33-0</t>
+  </si>
+  <si>
+    <t>21-0</t>
+  </si>
+  <si>
+    <t>32-0</t>
+  </si>
+  <si>
+    <t>31-0</t>
+  </si>
+  <si>
+    <t>10-0</t>
+  </si>
+  <si>
+    <t>20-0</t>
+  </si>
+  <si>
+    <t>30-0</t>
+  </si>
+  <si>
+    <t>4Apr21: Change to 3FVP with 3N
+2Apr21: Change to 3N for dams &amp; 5FVP
+31Mar21: Change the index for the k2 cluster (for the seasonality model)
 29Mar21: Changed to FVP3, 1N for dams, 3N for Offs
 22Mar21: Alter the initial weight &amp; wool spread for the weaners
 1: 1Apr19-Blank worksheet</t>
   </si>
   <si>
-    <t>NM-0</t>
-  </si>
-  <si>
-    <t>00-0</t>
-  </si>
-  <si>
-    <t>11-0</t>
-  </si>
-  <si>
-    <t>22-0</t>
-  </si>
-  <si>
-    <t>33-0</t>
-  </si>
-  <si>
-    <t>21-0</t>
-  </si>
-  <si>
-    <t>32-0</t>
-  </si>
-  <si>
-    <t>31-0</t>
-  </si>
-  <si>
-    <t>10-0</t>
-  </si>
-  <si>
-    <t>20-0</t>
-  </si>
-  <si>
-    <t>30-0</t>
+    <t>9Apr21: Fix formatting (box) around k2 cluster definition.
+30Mar21: Added inputs for % dry and number dams mated
+2: 17Jul20-Added structural inputs table
+1: 1Apr19-Created the version control table</t>
   </si>
 </sst>
 </file>
@@ -2471,7 +2474,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="52">
+  <borders count="55">
     <border>
       <left/>
       <right/>
@@ -3042,45 +3045,62 @@
       <diagonal/>
     </border>
     <border>
-      <left style="hair">
-        <color theme="0" tint="-0.24994659260841701"/>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
-      <right style="hair">
-        <color theme="0" tint="-0.24994659260841701"/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="hair">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -3206,7 +3226,7 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="179">
+  <cellXfs count="186">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="25" xfId="3">
@@ -3546,9 +3566,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="29" fillId="10" borderId="0" xfId="18" applyFont="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -3567,15 +3584,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="46" xfId="11" applyBorder="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="50" xfId="11" quotePrefix="1" applyBorder="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="49" xfId="11" applyBorder="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="51" xfId="11" applyBorder="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="8" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3656,6 +3664,39 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="23" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="49" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="18" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="50" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="51" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="52" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="53" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="16" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="16" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="54" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -4037,20 +4078,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" style="147" customWidth="1"/>
-    <col min="2" max="2" width="2.7109375" style="147" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" style="147" customWidth="1" outlineLevel="2"/>
-    <col min="4" max="4" width="1.7109375" style="147" customWidth="1"/>
-    <col min="5" max="6" width="9.7109375" style="147" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="1.7109375" style="147" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="37.28515625" style="147" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="147" customWidth="1"/>
-    <col min="10" max="23" width="10.85546875" style="147" customWidth="1"/>
-    <col min="24" max="24" width="1.7109375" style="147" customWidth="1"/>
-    <col min="25" max="26" width="4.7109375" style="147" customWidth="1"/>
-    <col min="27" max="27" width="8.7109375" style="147"/>
-    <col min="28" max="28" width="46.140625" style="147" customWidth="1"/>
-    <col min="29" max="16384" width="8.7109375" style="147"/>
+    <col min="1" max="1" width="4.7109375" style="146" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" style="146" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" style="146" customWidth="1" outlineLevel="2"/>
+    <col min="4" max="4" width="1.7109375" style="146" customWidth="1"/>
+    <col min="5" max="6" width="9.7109375" style="146" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="1.7109375" style="146" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="37.28515625" style="146" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="146" customWidth="1"/>
+    <col min="10" max="23" width="10.85546875" style="146" customWidth="1"/>
+    <col min="24" max="24" width="1.7109375" style="146" customWidth="1"/>
+    <col min="25" max="26" width="4.7109375" style="146" customWidth="1"/>
+    <col min="27" max="27" width="8.7109375" style="146"/>
+    <col min="28" max="28" width="46.140625" style="146" customWidth="1"/>
+    <col min="29" max="16384" width="8.7109375" style="146"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -4691,19 +4732,19 @@
       <c r="I18" s="31">
         <v>2</v>
       </c>
-      <c r="J18" s="163" t="s">
+      <c r="J18" s="159" t="s">
         <v>70</v>
       </c>
-      <c r="K18" s="164"/>
-      <c r="L18" s="164"/>
-      <c r="M18" s="164"/>
-      <c r="N18" s="164"/>
-      <c r="O18" s="164"/>
-      <c r="P18" s="164"/>
-      <c r="Q18" s="164"/>
-      <c r="R18" s="164"/>
-      <c r="S18" s="164"/>
-      <c r="T18" s="165"/>
+      <c r="K18" s="160"/>
+      <c r="L18" s="160"/>
+      <c r="M18" s="160"/>
+      <c r="N18" s="160"/>
+      <c r="O18" s="160"/>
+      <c r="P18" s="160"/>
+      <c r="Q18" s="160"/>
+      <c r="R18" s="160"/>
+      <c r="S18" s="160"/>
+      <c r="T18" s="161"/>
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
       <c r="W18" s="2"/>
@@ -4796,19 +4837,19 @@
       <c r="I21" s="23">
         <v>1</v>
       </c>
-      <c r="J21" s="166" t="s">
+      <c r="J21" s="162" t="s">
         <v>35</v>
       </c>
-      <c r="K21" s="167"/>
-      <c r="L21" s="167"/>
-      <c r="M21" s="167"/>
-      <c r="N21" s="167"/>
-      <c r="O21" s="167"/>
-      <c r="P21" s="167"/>
-      <c r="Q21" s="167"/>
-      <c r="R21" s="167"/>
-      <c r="S21" s="167"/>
-      <c r="T21" s="167"/>
+      <c r="K21" s="163"/>
+      <c r="L21" s="163"/>
+      <c r="M21" s="163"/>
+      <c r="N21" s="163"/>
+      <c r="O21" s="163"/>
+      <c r="P21" s="163"/>
+      <c r="Q21" s="163"/>
+      <c r="R21" s="163"/>
+      <c r="S21" s="163"/>
+      <c r="T21" s="163"/>
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
       <c r="W21" s="2"/>
@@ -5776,7 +5817,7 @@
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
       <c r="G49" s="4"/>
-      <c r="H49" s="148"/>
+      <c r="H49" s="147"/>
       <c r="I49" s="5"/>
       <c r="J49" s="5"/>
       <c r="K49" s="5"/>
@@ -5856,7 +5897,7 @@
       <c r="K51" s="102" t="s">
         <v>199</v>
       </c>
-      <c r="L51" s="149"/>
+      <c r="L51" s="148"/>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
@@ -5886,10 +5927,10 @@
       <c r="F52" s="5"/>
       <c r="G52" s="4"/>
       <c r="H52" s="2"/>
-      <c r="I52" s="149"/>
-      <c r="J52" s="149"/>
-      <c r="K52" s="149"/>
-      <c r="L52" s="149"/>
+      <c r="I52" s="148"/>
+      <c r="J52" s="148"/>
+      <c r="K52" s="148"/>
+      <c r="L52" s="148"/>
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
       <c r="O52" s="2"/>
@@ -5927,8 +5968,8 @@
       <c r="J53" s="102" t="s">
         <v>202</v>
       </c>
-      <c r="K53" s="149"/>
-      <c r="L53" s="149"/>
+      <c r="K53" s="148"/>
+      <c r="L53" s="148"/>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
       <c r="O53" s="2"/>
@@ -5958,10 +5999,10 @@
       <c r="F54" s="5"/>
       <c r="G54" s="4"/>
       <c r="H54" s="2"/>
-      <c r="I54" s="149"/>
-      <c r="J54" s="149"/>
-      <c r="K54" s="149"/>
-      <c r="L54" s="149"/>
+      <c r="I54" s="148"/>
+      <c r="J54" s="148"/>
+      <c r="K54" s="148"/>
+      <c r="L54" s="148"/>
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
       <c r="O54" s="2"/>
@@ -6002,7 +6043,7 @@
       <c r="K55" s="102" t="s">
         <v>210</v>
       </c>
-      <c r="L55" s="149"/>
+      <c r="L55" s="148"/>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
       <c r="O55" s="2"/>
@@ -6043,7 +6084,7 @@
       <c r="K56" s="102" t="b">
         <v>0</v>
       </c>
-      <c r="L56" s="149"/>
+      <c r="L56" s="148"/>
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
       <c r="O56" s="2"/>
@@ -6081,8 +6122,8 @@
       <c r="J57" s="102" t="s">
         <v>212</v>
       </c>
-      <c r="K57" s="149"/>
-      <c r="L57" s="149"/>
+      <c r="K57" s="148"/>
+      <c r="L57" s="148"/>
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
       <c r="O57" s="2"/>
@@ -6166,7 +6207,7 @@
       <c r="K59" s="102" t="s">
         <v>219</v>
       </c>
-      <c r="L59" s="149"/>
+      <c r="L59" s="148"/>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
       <c r="O59" s="2"/>
@@ -6196,10 +6237,10 @@
       <c r="F60" s="5"/>
       <c r="G60" s="4"/>
       <c r="H60" s="2"/>
-      <c r="I60" s="149"/>
-      <c r="J60" s="149"/>
-      <c r="K60" s="149"/>
-      <c r="L60" s="149"/>
+      <c r="I60" s="148"/>
+      <c r="J60" s="148"/>
+      <c r="K60" s="148"/>
+      <c r="L60" s="148"/>
       <c r="M60" s="2"/>
       <c r="N60" s="2"/>
       <c r="O60" s="2"/>
@@ -6447,7 +6488,7 @@
       <c r="H67" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="I67" s="145">
+      <c r="I67" s="144">
         <v>43466</v>
       </c>
       <c r="J67" s="2"/>
@@ -6503,22 +6544,22 @@
       <c r="H68" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="I68" s="145" t="s">
+      <c r="I68" s="144" t="s">
         <v>190</v>
       </c>
-      <c r="J68" s="145" t="s">
+      <c r="J68" s="144" t="s">
         <v>191</v>
       </c>
-      <c r="K68" s="145" t="s">
+      <c r="K68" s="144" t="s">
         <v>192</v>
       </c>
-      <c r="L68" s="145" t="s">
+      <c r="L68" s="144" t="s">
         <v>193</v>
       </c>
-      <c r="M68" s="145" t="s">
+      <c r="M68" s="144" t="s">
         <v>194</v>
       </c>
-      <c r="N68" s="145" t="s">
+      <c r="N68" s="144" t="s">
         <v>195</v>
       </c>
       <c r="O68" s="2"/>
@@ -7059,8 +7100,8 @@
   </sheetPr>
   <dimension ref="A1:AE363"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21:T21"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18:T18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -7714,22 +7755,22 @@
       <c r="H18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I18" s="162">
-        <v>44285</v>
-      </c>
-      <c r="J18" s="163" t="s">
-        <v>274</v>
-      </c>
-      <c r="K18" s="164"/>
-      <c r="L18" s="164"/>
-      <c r="M18" s="164"/>
-      <c r="N18" s="164"/>
-      <c r="O18" s="164"/>
-      <c r="P18" s="164"/>
-      <c r="Q18" s="164"/>
-      <c r="R18" s="164"/>
-      <c r="S18" s="164"/>
-      <c r="T18" s="165"/>
+      <c r="I18" s="158">
+        <v>44295</v>
+      </c>
+      <c r="J18" s="159" t="s">
+        <v>286</v>
+      </c>
+      <c r="K18" s="160"/>
+      <c r="L18" s="160"/>
+      <c r="M18" s="160"/>
+      <c r="N18" s="160"/>
+      <c r="O18" s="160"/>
+      <c r="P18" s="160"/>
+      <c r="Q18" s="160"/>
+      <c r="R18" s="160"/>
+      <c r="S18" s="160"/>
+      <c r="T18" s="161"/>
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
       <c r="W18" s="2"/>
@@ -7819,22 +7860,22 @@
       <c r="H21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I21" s="161">
-        <v>44286</v>
-      </c>
-      <c r="J21" s="166" t="s">
-        <v>275</v>
-      </c>
-      <c r="K21" s="167"/>
-      <c r="L21" s="167"/>
-      <c r="M21" s="167"/>
-      <c r="N21" s="167"/>
-      <c r="O21" s="167"/>
-      <c r="P21" s="167"/>
-      <c r="Q21" s="167"/>
-      <c r="R21" s="167"/>
-      <c r="S21" s="167"/>
-      <c r="T21" s="167"/>
+      <c r="I21" s="157">
+        <v>44290</v>
+      </c>
+      <c r="J21" s="162" t="s">
+        <v>285</v>
+      </c>
+      <c r="K21" s="163"/>
+      <c r="L21" s="163"/>
+      <c r="M21" s="163"/>
+      <c r="N21" s="163"/>
+      <c r="O21" s="163"/>
+      <c r="P21" s="163"/>
+      <c r="Q21" s="163"/>
+      <c r="R21" s="163"/>
+      <c r="S21" s="163"/>
+      <c r="T21" s="163"/>
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
       <c r="W21" s="2"/>
@@ -8902,7 +8943,7 @@
       <c r="AA51" s="1"/>
       <c r="AB51" s="1"/>
     </row>
-    <row r="52" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:28" s="146" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="33"/>
       <c r="C52" s="73"/>
@@ -8936,7 +8977,7 @@
       <c r="AA52" s="1"/>
       <c r="AB52" s="1"/>
     </row>
-    <row r="53" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:28" s="146" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="33"/>
       <c r="C53" s="73"/>
@@ -8970,7 +9011,7 @@
       <c r="AA53" s="1"/>
       <c r="AB53" s="1"/>
     </row>
-    <row r="54" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:28" s="146" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="33"/>
       <c r="C54" s="73"/>
@@ -9004,7 +9045,7 @@
       <c r="AA54" s="1"/>
       <c r="AB54" s="1"/>
     </row>
-    <row r="55" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:28" s="146" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="33"/>
       <c r="C55" s="73"/>
@@ -9038,7 +9079,7 @@
       <c r="AA55" s="1"/>
       <c r="AB55" s="1"/>
     </row>
-    <row r="56" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:28" s="146" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="33"/>
       <c r="C56" s="73"/>
@@ -9072,7 +9113,7 @@
       <c r="AA56" s="1"/>
       <c r="AB56" s="1"/>
     </row>
-    <row r="57" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:28" s="146" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="33"/>
       <c r="C57" s="73"/>
@@ -9106,7 +9147,7 @@
       <c r="AA57" s="1"/>
       <c r="AB57" s="1"/>
     </row>
-    <row r="58" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:28" s="146" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="33"/>
       <c r="C58" s="73"/>
@@ -9140,7 +9181,7 @@
       <c r="AA58" s="1"/>
       <c r="AB58" s="1"/>
     </row>
-    <row r="59" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:28" s="146" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="33"/>
       <c r="C59" s="73"/>
@@ -9174,7 +9215,7 @@
       <c r="AA59" s="1"/>
       <c r="AB59" s="1"/>
     </row>
-    <row r="60" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:28" s="146" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="33"/>
       <c r="C60" s="73"/>
@@ -9208,7 +9249,7 @@
       <c r="AA60" s="1"/>
       <c r="AB60" s="1"/>
     </row>
-    <row r="61" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:28" s="146" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="33"/>
       <c r="C61" s="73"/>
@@ -9242,7 +9283,7 @@
       <c r="AA61" s="1"/>
       <c r="AB61" s="1"/>
     </row>
-    <row r="62" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:28" s="146" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="33"/>
       <c r="C62" s="73"/>
@@ -9276,7 +9317,7 @@
       <c r="AA62" s="1"/>
       <c r="AB62" s="1"/>
     </row>
-    <row r="63" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:28" s="146" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="33"/>
       <c r="C63" s="73"/>
@@ -9310,7 +9351,7 @@
       <c r="AA63" s="1"/>
       <c r="AB63" s="1"/>
     </row>
-    <row r="64" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:28" s="146" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="33"/>
       <c r="C64" s="73"/>
@@ -9605,7 +9646,7 @@
       <c r="AA71" s="1"/>
       <c r="AB71" s="1"/>
     </row>
-    <row r="72" spans="1:28" s="146" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:28" s="145" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="33"/>
       <c r="C72" s="73">
@@ -9646,7 +9687,7 @@
       <c r="AA72" s="1"/>
       <c r="AB72" s="1"/>
     </row>
-    <row r="73" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:28" s="146" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="33"/>
       <c r="C73" s="73"/>
@@ -9676,7 +9717,7 @@
       <c r="AA73" s="1"/>
       <c r="AB73" s="1"/>
     </row>
-    <row r="74" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:28" s="146" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="33"/>
       <c r="C74" s="73"/>
@@ -9712,7 +9753,7 @@
       <c r="AA74" s="1"/>
       <c r="AB74" s="1"/>
     </row>
-    <row r="75" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:28" s="146" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="33"/>
       <c r="C75" s="73"/>
@@ -9929,7 +9970,7 @@
       <c r="AA80" s="1"/>
       <c r="AB80" s="1"/>
     </row>
-    <row r="81" spans="1:28" s="144" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:28" s="143" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="33"/>
       <c r="C81" s="73">
@@ -11514,7 +11555,7 @@
       <c r="AA119" s="1"/>
       <c r="AB119" s="1"/>
     </row>
-    <row r="120" spans="1:28" s="143" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="33"/>
       <c r="C120" s="73">
@@ -11547,7 +11588,7 @@
       <c r="AA120" s="1"/>
       <c r="AB120" s="1"/>
     </row>
-    <row r="121" spans="1:28" s="143" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="33"/>
       <c r="C121" s="73">
@@ -11582,7 +11623,7 @@
       <c r="AA121" s="1"/>
       <c r="AB121" s="1"/>
     </row>
-    <row r="122" spans="1:28" s="143" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="33"/>
       <c r="C122" s="73">
@@ -11623,7 +11664,7 @@
       <c r="AA122" s="1"/>
       <c r="AB122" s="1"/>
     </row>
-    <row r="123" spans="1:28" s="143" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
       <c r="B123" s="33"/>
       <c r="C123" s="73">
@@ -11671,7 +11712,7 @@
       <c r="AA123" s="1"/>
       <c r="AB123" s="1"/>
     </row>
-    <row r="124" spans="1:28" s="143" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
       <c r="B124" s="33"/>
       <c r="C124" s="73">
@@ -11717,7 +11758,7 @@
       <c r="AA124" s="1"/>
       <c r="AB124" s="1"/>
     </row>
-    <row r="125" spans="1:28" s="143" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="B125" s="33"/>
       <c r="C125" s="73">
@@ -11760,7 +11801,7 @@
       <c r="AA125" s="1"/>
       <c r="AB125" s="1"/>
     </row>
-    <row r="126" spans="1:28" s="143" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
       <c r="B126" s="33"/>
       <c r="C126" s="73">
@@ -11793,7 +11834,7 @@
       <c r="AA126" s="1"/>
       <c r="AB126" s="1"/>
     </row>
-    <row r="127" spans="1:28" s="143" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="B127" s="33"/>
       <c r="C127" s="73">
@@ -11840,7 +11881,7 @@
       <c r="AA127" s="1"/>
       <c r="AB127" s="1"/>
     </row>
-    <row r="128" spans="1:28" s="143" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
       <c r="B128" s="33"/>
       <c r="C128" s="73">
@@ -11885,7 +11926,7 @@
       <c r="AA128" s="1"/>
       <c r="AB128" s="1"/>
     </row>
-    <row r="129" spans="1:28" s="143" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
       <c r="B129" s="33"/>
       <c r="C129" s="73">
@@ -11928,7 +11969,7 @@
       <c r="AA129" s="1"/>
       <c r="AB129" s="1"/>
     </row>
-    <row r="130" spans="1:28" s="143" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="B130" s="33"/>
       <c r="C130" s="73">
@@ -12488,38 +12529,38 @@
       <c r="H146" s="29"/>
       <c r="I146" s="29"/>
       <c r="J146" s="29"/>
-      <c r="K146" s="150"/>
-      <c r="L146" s="151" t="s">
+      <c r="K146" s="149"/>
+      <c r="L146" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="M146" s="152" t="s">
+      <c r="M146" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="N146" s="152">
+      <c r="N146" s="29">
         <v>11</v>
       </c>
-      <c r="O146" s="152">
+      <c r="O146" s="29">
         <v>22</v>
       </c>
-      <c r="P146" s="152">
+      <c r="P146" s="29">
         <v>33</v>
       </c>
-      <c r="Q146" s="152">
+      <c r="Q146" s="29">
         <v>21</v>
       </c>
-      <c r="R146" s="152">
+      <c r="R146" s="29">
         <v>32</v>
       </c>
-      <c r="S146" s="152">
+      <c r="S146" s="29">
         <v>31</v>
       </c>
-      <c r="T146" s="152">
+      <c r="T146" s="29">
         <v>10</v>
       </c>
-      <c r="U146" s="152">
+      <c r="U146" s="29">
         <v>20</v>
       </c>
-      <c r="V146" s="153">
+      <c r="V146" s="29">
         <v>30</v>
       </c>
       <c r="W146" s="78"/>
@@ -12975,7 +13016,7 @@
       <c r="AA156" s="1"/>
       <c r="AB156" s="1"/>
     </row>
-    <row r="157" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:28" s="146" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
       <c r="B157" s="33"/>
       <c r="C157" s="73">
@@ -13032,7 +13073,7 @@
       <c r="AA157" s="1"/>
       <c r="AB157" s="1"/>
     </row>
-    <row r="158" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:28" s="141" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
       <c r="B158" s="33"/>
       <c r="C158" s="73">
@@ -16030,38 +16071,38 @@
       </c>
       <c r="J210" s="49"/>
       <c r="K210" s="49"/>
-      <c r="L210" s="94" t="s">
+      <c r="L210" s="175" t="s">
+        <v>274</v>
+      </c>
+      <c r="M210" s="176" t="s">
+        <v>275</v>
+      </c>
+      <c r="N210" s="176" t="s">
         <v>276</v>
       </c>
-      <c r="M210" s="94" t="s">
+      <c r="O210" s="176" t="s">
         <v>277</v>
       </c>
-      <c r="N210" s="94" t="s">
+      <c r="P210" s="176" t="s">
         <v>278</v>
       </c>
-      <c r="O210" s="94" t="s">
+      <c r="Q210" s="176" t="s">
         <v>279</v>
       </c>
-      <c r="P210" s="94" t="s">
+      <c r="R210" s="176" t="s">
         <v>280</v>
       </c>
-      <c r="Q210" s="94" t="s">
+      <c r="S210" s="176" t="s">
         <v>281</v>
       </c>
-      <c r="R210" s="94" t="s">
+      <c r="T210" s="176" t="s">
         <v>282</v>
       </c>
-      <c r="S210" s="94" t="s">
+      <c r="U210" s="176" t="s">
         <v>283</v>
       </c>
-      <c r="T210" s="94" t="s">
+      <c r="V210" s="177" t="s">
         <v>284</v>
-      </c>
-      <c r="U210" s="94" t="s">
-        <v>285</v>
-      </c>
-      <c r="V210" s="94" t="s">
-        <v>286</v>
       </c>
       <c r="W210" s="94"/>
       <c r="X210" s="4"/>
@@ -16081,7 +16122,7 @@
       <c r="E211" s="5"/>
       <c r="F211" s="5"/>
       <c r="G211" s="4"/>
-      <c r="H211" s="141" t="s">
+      <c r="H211" s="140" t="s">
         <v>163</v>
       </c>
       <c r="I211" s="60"/>
@@ -16089,47 +16130,47 @@
       <c r="K211" s="49">
         <v>1</v>
       </c>
-      <c r="L211" s="140" t="str">
+      <c r="L211" s="178" t="str">
         <f>LEFT(L$210,LEN(L$210)-1)&amp;$K211</f>
         <v>NM-1</v>
       </c>
-      <c r="M211" s="140" t="str">
+      <c r="M211" s="179" t="str">
         <f t="shared" ref="M211:V212" si="5">LEFT(M$210,LEN(M$210)-1)&amp;$K211</f>
         <v>00-1</v>
       </c>
-      <c r="N211" s="94" t="str">
+      <c r="N211" s="180" t="str">
         <f t="shared" si="5"/>
         <v>11-1</v>
       </c>
-      <c r="O211" s="94" t="str">
+      <c r="O211" s="180" t="str">
         <f t="shared" si="5"/>
         <v>22-1</v>
       </c>
-      <c r="P211" s="94" t="str">
+      <c r="P211" s="180" t="str">
         <f t="shared" si="5"/>
         <v>33-1</v>
       </c>
-      <c r="Q211" s="94" t="str">
+      <c r="Q211" s="180" t="str">
         <f t="shared" si="5"/>
         <v>21-1</v>
       </c>
-      <c r="R211" s="94" t="str">
+      <c r="R211" s="180" t="str">
         <f t="shared" si="5"/>
         <v>32-1</v>
       </c>
-      <c r="S211" s="94" t="str">
+      <c r="S211" s="180" t="str">
         <f t="shared" si="5"/>
         <v>31-1</v>
       </c>
-      <c r="T211" s="94" t="str">
+      <c r="T211" s="180" t="str">
         <f t="shared" si="5"/>
         <v>10-1</v>
       </c>
-      <c r="U211" s="94" t="str">
+      <c r="U211" s="180" t="str">
         <f t="shared" si="5"/>
         <v>20-1</v>
       </c>
-      <c r="V211" s="94" t="str">
+      <c r="V211" s="181" t="str">
         <f t="shared" si="5"/>
         <v>30-1</v>
       </c>
@@ -16151,7 +16192,7 @@
       <c r="E212" s="5"/>
       <c r="F212" s="5"/>
       <c r="G212" s="4"/>
-      <c r="H212" s="141" t="s">
+      <c r="H212" s="140" t="s">
         <v>164</v>
       </c>
       <c r="I212" s="60"/>
@@ -16159,47 +16200,47 @@
       <c r="K212" s="49">
         <v>2</v>
       </c>
-      <c r="L212" s="140" t="str">
-        <f t="shared" ref="L212:V212" si="6">LEFT(L$210,LEN(L$210)-1)&amp;$K212</f>
+      <c r="L212" s="182" t="str">
+        <f t="shared" ref="L212" si="6">LEFT(L$210,LEN(L$210)-1)&amp;$K212</f>
         <v>NM-2</v>
       </c>
-      <c r="M212" s="140" t="str">
+      <c r="M212" s="183" t="str">
         <f t="shared" si="5"/>
         <v>00-2</v>
       </c>
-      <c r="N212" s="94" t="str">
+      <c r="N212" s="184" t="str">
         <f t="shared" si="5"/>
         <v>11-2</v>
       </c>
-      <c r="O212" s="94" t="str">
+      <c r="O212" s="184" t="str">
         <f t="shared" si="5"/>
         <v>22-2</v>
       </c>
-      <c r="P212" s="94" t="str">
+      <c r="P212" s="184" t="str">
         <f t="shared" si="5"/>
         <v>33-2</v>
       </c>
-      <c r="Q212" s="94" t="str">
+      <c r="Q212" s="184" t="str">
         <f t="shared" si="5"/>
         <v>21-2</v>
       </c>
-      <c r="R212" s="94" t="str">
+      <c r="R212" s="184" t="str">
         <f t="shared" si="5"/>
         <v>32-2</v>
       </c>
-      <c r="S212" s="94" t="str">
+      <c r="S212" s="184" t="str">
         <f t="shared" si="5"/>
         <v>31-2</v>
       </c>
-      <c r="T212" s="94" t="str">
+      <c r="T212" s="184" t="str">
         <f t="shared" si="5"/>
         <v>10-2</v>
       </c>
-      <c r="U212" s="94" t="str">
+      <c r="U212" s="184" t="str">
         <f t="shared" si="5"/>
         <v>20-2</v>
       </c>
-      <c r="V212" s="94" t="str">
+      <c r="V212" s="185" t="str">
         <f t="shared" si="5"/>
         <v>30-2</v>
       </c>
@@ -21840,20 +21881,20 @@
       <c r="G314" s="3"/>
       <c r="H314" s="29"/>
       <c r="I314" s="29"/>
-      <c r="J314" s="160" t="s">
+      <c r="J314" s="156" t="s">
         <v>45</v>
       </c>
-      <c r="K314" s="160"/>
-      <c r="L314" s="160" t="s">
+      <c r="K314" s="156"/>
+      <c r="L314" s="156" t="s">
         <v>45</v>
       </c>
-      <c r="M314" s="160"/>
+      <c r="M314" s="156"/>
       <c r="N314" s="29"/>
       <c r="O314" s="29"/>
-      <c r="P314" s="160" t="s">
+      <c r="P314" s="156" t="s">
         <v>45</v>
       </c>
-      <c r="Q314" s="160"/>
+      <c r="Q314" s="156"/>
       <c r="R314" s="29"/>
       <c r="S314" s="29"/>
       <c r="T314" s="29"/>
@@ -21879,20 +21920,20 @@
       <c r="G315" s="3"/>
       <c r="H315" s="29"/>
       <c r="I315" s="29"/>
-      <c r="J315" s="160" t="s">
+      <c r="J315" s="156" t="s">
         <v>45</v>
       </c>
-      <c r="K315" s="160"/>
-      <c r="L315" s="160" t="s">
+      <c r="K315" s="156"/>
+      <c r="L315" s="156" t="s">
         <v>45</v>
       </c>
-      <c r="M315" s="160"/>
+      <c r="M315" s="156"/>
       <c r="N315" s="29"/>
       <c r="O315" s="29"/>
-      <c r="P315" s="160" t="s">
+      <c r="P315" s="156" t="s">
         <v>45</v>
       </c>
-      <c r="Q315" s="160"/>
+      <c r="Q315" s="156"/>
       <c r="R315" s="29"/>
       <c r="S315" s="29"/>
       <c r="T315" s="29"/>
@@ -21918,24 +21959,24 @@
       <c r="G316" s="3"/>
       <c r="H316" s="29"/>
       <c r="I316" s="29"/>
-      <c r="J316" s="160" t="s">
+      <c r="J316" s="156" t="s">
         <v>75</v>
       </c>
-      <c r="K316" s="160"/>
-      <c r="L316" s="160" t="s">
+      <c r="K316" s="156"/>
+      <c r="L316" s="156" t="s">
         <v>76</v>
       </c>
-      <c r="M316" s="160"/>
+      <c r="M316" s="156"/>
       <c r="N316" s="29" t="s">
         <v>112</v>
       </c>
       <c r="O316" s="29" t="s">
         <v>171</v>
       </c>
-      <c r="P316" s="160" t="s">
+      <c r="P316" s="156" t="s">
         <v>78</v>
       </c>
-      <c r="Q316" s="160"/>
+      <c r="Q316" s="156"/>
       <c r="R316" s="29"/>
       <c r="S316" s="29"/>
       <c r="T316" s="29"/>
@@ -21963,20 +22004,20 @@
       <c r="G317" s="3"/>
       <c r="H317" s="29"/>
       <c r="I317" s="29"/>
-      <c r="J317" s="160" t="s">
+      <c r="J317" s="156" t="s">
         <v>45</v>
       </c>
-      <c r="K317" s="160"/>
-      <c r="L317" s="160" t="s">
+      <c r="K317" s="156"/>
+      <c r="L317" s="156" t="s">
         <v>45</v>
       </c>
-      <c r="M317" s="160"/>
+      <c r="M317" s="156"/>
       <c r="N317" s="29"/>
       <c r="O317" s="29"/>
-      <c r="P317" s="160" t="s">
+      <c r="P317" s="156" t="s">
         <v>45</v>
       </c>
-      <c r="Q317" s="160"/>
+      <c r="Q317" s="156"/>
       <c r="R317" s="29"/>
       <c r="S317" s="29"/>
       <c r="T317" s="29"/>
@@ -22115,7 +22156,7 @@
       <c r="K321" s="2"/>
       <c r="L321" s="125">
         <f>i_w_start_len1*i_n1_len^L324</f>
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="M321" s="2"/>
       <c r="N321" s="120" t="s">
@@ -22141,7 +22182,7 @@
       <c r="AA321" s="1"/>
       <c r="AB321" s="1"/>
     </row>
-    <row r="322" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:28" s="146" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A322" s="1"/>
       <c r="B322" s="33"/>
       <c r="C322" s="73"/>
@@ -22200,7 +22241,7 @@
       </c>
       <c r="K323" s="119"/>
       <c r="L323" s="31">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M323" s="119"/>
       <c r="N323" s="2"/>
@@ -22221,7 +22262,7 @@
       <c r="AA323" s="1"/>
       <c r="AB323" s="1"/>
     </row>
-    <row r="324" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:28" s="146" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A324" s="1"/>
       <c r="B324" s="33"/>
       <c r="C324" s="73"/>
@@ -22249,14 +22290,14 @@
         <v>3</v>
       </c>
       <c r="Q324" s="119"/>
-      <c r="R324" s="168" t="s">
+      <c r="R324" s="164" t="s">
         <v>156</v>
       </c>
-      <c r="S324" s="169"/>
-      <c r="T324" s="169"/>
-      <c r="U324" s="169"/>
-      <c r="V324" s="169"/>
-      <c r="W324" s="170"/>
+      <c r="S324" s="165"/>
+      <c r="T324" s="165"/>
+      <c r="U324" s="165"/>
+      <c r="V324" s="165"/>
+      <c r="W324" s="166"/>
       <c r="X324" s="4"/>
       <c r="Y324" s="16"/>
       <c r="Z324" s="1"/>
@@ -22294,12 +22335,12 @@
         <v>1</v>
       </c>
       <c r="Q325" s="2"/>
-      <c r="R325" s="171"/>
-      <c r="S325" s="172"/>
-      <c r="T325" s="172"/>
-      <c r="U325" s="172"/>
-      <c r="V325" s="172"/>
-      <c r="W325" s="173"/>
+      <c r="R325" s="167"/>
+      <c r="S325" s="168"/>
+      <c r="T325" s="168"/>
+      <c r="U325" s="168"/>
+      <c r="V325" s="168"/>
+      <c r="W325" s="169"/>
       <c r="X325" s="4"/>
       <c r="Y325" s="16"/>
       <c r="Z325" s="1"/>
@@ -22337,12 +22378,12 @@
         <v>1</v>
       </c>
       <c r="Q326" s="2"/>
-      <c r="R326" s="171"/>
-      <c r="S326" s="172"/>
-      <c r="T326" s="172"/>
-      <c r="U326" s="172"/>
-      <c r="V326" s="172"/>
-      <c r="W326" s="173"/>
+      <c r="R326" s="167"/>
+      <c r="S326" s="168"/>
+      <c r="T326" s="168"/>
+      <c r="U326" s="168"/>
+      <c r="V326" s="168"/>
+      <c r="W326" s="169"/>
       <c r="X326" s="4"/>
       <c r="Y326" s="16"/>
       <c r="Z326" s="1"/>
@@ -22378,12 +22419,12 @@
         <v>1</v>
       </c>
       <c r="Q327" s="2"/>
-      <c r="R327" s="154"/>
-      <c r="S327" s="155"/>
-      <c r="T327" s="155"/>
-      <c r="U327" s="155"/>
-      <c r="V327" s="155"/>
-      <c r="W327" s="156"/>
+      <c r="R327" s="150"/>
+      <c r="S327" s="151"/>
+      <c r="T327" s="151"/>
+      <c r="U327" s="151"/>
+      <c r="V327" s="151"/>
+      <c r="W327" s="152"/>
       <c r="X327" s="4"/>
       <c r="Y327" s="16"/>
       <c r="Z327" s="1"/>
@@ -22425,7 +22466,7 @@
       <c r="AA328" s="1"/>
       <c r="AB328" s="1"/>
     </row>
-    <row r="329" spans="1:28" s="147" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:28" s="146" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A329" s="1"/>
       <c r="B329" s="33"/>
       <c r="C329" s="73">
@@ -22460,7 +22501,7 @@
       <c r="AA329" s="1"/>
       <c r="AB329" s="1"/>
     </row>
-    <row r="330" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:28" s="146" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A330" s="1"/>
       <c r="B330" s="33"/>
       <c r="C330" s="73">
@@ -22495,7 +22536,7 @@
       <c r="AA330" s="1"/>
       <c r="AB330" s="1"/>
     </row>
-    <row r="331" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:28" s="146" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A331" s="1"/>
       <c r="B331" s="33"/>
       <c r="C331" s="73">
@@ -22540,7 +22581,7 @@
       <c r="AA331" s="1"/>
       <c r="AB331" s="1"/>
     </row>
-    <row r="332" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:28" s="146" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A332" s="1"/>
       <c r="B332" s="33"/>
       <c r="C332" s="73">
@@ -22587,7 +22628,7 @@
       <c r="AA332" s="1"/>
       <c r="AB332" s="1"/>
     </row>
-    <row r="333" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:28" s="146" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A333" s="1"/>
       <c r="B333" s="33"/>
       <c r="C333" s="73">
@@ -22639,7 +22680,7 @@
       <c r="AA333" s="1"/>
       <c r="AB333" s="1"/>
     </row>
-    <row r="334" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:28" s="146" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A334" s="1"/>
       <c r="B334" s="33"/>
       <c r="C334" s="73"/>
@@ -22689,7 +22730,7 @@
       <c r="AA334" s="1"/>
       <c r="AB334" s="1"/>
     </row>
-    <row r="335" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:28" s="146" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A335" s="1"/>
       <c r="B335" s="33"/>
       <c r="C335" s="73">
@@ -22738,7 +22779,7 @@
       <c r="AA335" s="1"/>
       <c r="AB335" s="1"/>
     </row>
-    <row r="336" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:28" s="146" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A336" s="1"/>
       <c r="B336" s="33"/>
       <c r="C336" s="73"/>
@@ -22782,7 +22823,7 @@
       <c r="AA336" s="1"/>
       <c r="AB336" s="1"/>
     </row>
-    <row r="337" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:28" s="146" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A337" s="1"/>
       <c r="B337" s="33"/>
       <c r="C337" s="73">
@@ -22804,7 +22845,7 @@
       <c r="L337" s="2"/>
       <c r="M337" s="2"/>
       <c r="N337" s="2"/>
-      <c r="O337" s="157">
+      <c r="O337" s="153">
         <v>43755</v>
       </c>
       <c r="P337" s="2"/>
@@ -22821,7 +22862,7 @@
       <c r="AA337" s="1"/>
       <c r="AB337" s="1"/>
     </row>
-    <row r="338" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:28" s="146" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A338" s="1"/>
       <c r="B338" s="33"/>
       <c r="C338" s="73">
@@ -22843,7 +22884,7 @@
       <c r="L338" s="2"/>
       <c r="M338" s="2"/>
       <c r="N338" s="2"/>
-      <c r="O338" s="157">
+      <c r="O338" s="153">
         <v>43826</v>
       </c>
       <c r="P338" s="2"/>
@@ -22860,7 +22901,7 @@
       <c r="AA338" s="1"/>
       <c r="AB338" s="1"/>
     </row>
-    <row r="339" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:28" s="146" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A339" s="1"/>
       <c r="B339" s="33"/>
       <c r="C339" s="73">
@@ -22874,14 +22915,14 @@
       <c r="F339" s="5"/>
       <c r="G339" s="4"/>
       <c r="H339" s="2"/>
-      <c r="I339" s="158"/>
-      <c r="J339" s="159" t="s">
+      <c r="I339" s="154"/>
+      <c r="J339" s="155" t="s">
         <v>264</v>
       </c>
-      <c r="K339" s="159" t="s">
+      <c r="K339" s="155" t="s">
         <v>265</v>
       </c>
-      <c r="L339" s="159" t="s">
+      <c r="L339" s="155" t="s">
         <v>266</v>
       </c>
       <c r="M339" s="2"/>
@@ -22901,7 +22942,7 @@
       <c r="AA339" s="1"/>
       <c r="AB339" s="1"/>
     </row>
-    <row r="340" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:28" s="146" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A340" s="1"/>
       <c r="B340" s="33"/>
       <c r="C340" s="73"/>
@@ -22912,7 +22953,7 @@
       <c r="H340" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="I340" s="158"/>
+      <c r="I340" s="154"/>
       <c r="J340" s="31">
         <f>K334</f>
         <v>0</v>
@@ -22942,7 +22983,7 @@
       <c r="AA340" s="1"/>
       <c r="AB340" s="1"/>
     </row>
-    <row r="341" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:28" s="146" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A341" s="1"/>
       <c r="B341" s="33"/>
       <c r="C341" s="73"/>
@@ -22951,10 +22992,10 @@
       <c r="F341" s="5"/>
       <c r="G341" s="4"/>
       <c r="H341" s="2"/>
-      <c r="I341" s="158"/>
-      <c r="J341" s="159"/>
-      <c r="K341" s="159"/>
-      <c r="L341" s="159"/>
+      <c r="I341" s="154"/>
+      <c r="J341" s="155"/>
+      <c r="K341" s="155"/>
+      <c r="L341" s="155"/>
       <c r="M341" s="2"/>
       <c r="N341" s="2"/>
       <c r="O341" s="2"/>
@@ -22972,7 +23013,7 @@
       <c r="AA341" s="1"/>
       <c r="AB341" s="1"/>
     </row>
-    <row r="342" spans="1:28" s="147" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:28" s="146" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A342" s="1"/>
       <c r="B342" s="33"/>
       <c r="C342" s="73">
@@ -23007,7 +23048,7 @@
       <c r="AA342" s="1"/>
       <c r="AB342" s="1"/>
     </row>
-    <row r="343" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:28" s="146" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A343" s="1"/>
       <c r="B343" s="33"/>
       <c r="C343" s="73">
@@ -23048,7 +23089,7 @@
       <c r="AA343" s="1"/>
       <c r="AB343" s="1"/>
     </row>
-    <row r="344" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:28" s="146" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A344" s="1"/>
       <c r="B344" s="33"/>
       <c r="C344" s="73">
@@ -23091,7 +23132,7 @@
       <c r="AA344" s="1"/>
       <c r="AB344" s="1"/>
     </row>
-    <row r="345" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:28" s="146" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A345" s="1"/>
       <c r="B345" s="33"/>
       <c r="C345" s="73">
@@ -23139,7 +23180,7 @@
       <c r="AA345" s="1"/>
       <c r="AB345" s="1"/>
     </row>
-    <row r="346" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:28" s="146" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A346" s="1"/>
       <c r="B346" s="33"/>
       <c r="C346" s="73"/>
@@ -23183,7 +23224,7 @@
       <c r="AA346" s="1"/>
       <c r="AB346" s="1"/>
     </row>
-    <row r="347" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:28" s="146" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A347" s="1"/>
       <c r="B347" s="33"/>
       <c r="C347" s="73">
@@ -23228,7 +23269,7 @@
       <c r="AA347" s="1"/>
       <c r="AB347" s="1"/>
     </row>
-    <row r="348" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:28" s="146" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A348" s="1"/>
       <c r="B348" s="33"/>
       <c r="C348" s="73">
@@ -23261,7 +23302,7 @@
       <c r="AA348" s="1"/>
       <c r="AB348" s="1"/>
     </row>
-    <row r="349" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:28" s="146" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A349" s="1"/>
       <c r="B349" s="33"/>
       <c r="C349" s="73">
@@ -23296,7 +23337,7 @@
       <c r="AA349" s="1"/>
       <c r="AB349" s="1"/>
     </row>
-    <row r="350" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:28" s="146" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A350" s="1"/>
       <c r="B350" s="33"/>
       <c r="C350" s="73">
@@ -23318,20 +23359,20 @@
       <c r="N350" s="2"/>
       <c r="O350" s="2"/>
       <c r="P350" s="2"/>
-      <c r="Q350" s="174"/>
-      <c r="R350" s="175"/>
-      <c r="S350" s="175"/>
-      <c r="T350" s="175"/>
-      <c r="U350" s="175"/>
-      <c r="V350" s="175"/>
-      <c r="W350" s="176"/>
+      <c r="Q350" s="170"/>
+      <c r="R350" s="171"/>
+      <c r="S350" s="171"/>
+      <c r="T350" s="171"/>
+      <c r="U350" s="171"/>
+      <c r="V350" s="171"/>
+      <c r="W350" s="172"/>
       <c r="X350" s="4"/>
       <c r="Y350" s="16"/>
       <c r="Z350" s="1"/>
       <c r="AA350" s="1"/>
       <c r="AB350" s="1"/>
     </row>
-    <row r="351" spans="1:28" s="147" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:28" s="146" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A351" s="1"/>
       <c r="B351" s="33"/>
       <c r="C351" s="73">
@@ -23366,7 +23407,7 @@
       <c r="AA351" s="1"/>
       <c r="AB351" s="1"/>
     </row>
-    <row r="352" spans="1:28" s="147" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:28" s="146" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A352" s="1"/>
       <c r="B352" s="33"/>
       <c r="C352" s="73">
@@ -24438,23 +24479,23 @@
       <c r="I18" s="31">
         <v>1</v>
       </c>
-      <c r="J18" s="177" t="s">
+      <c r="J18" s="173" t="s">
         <v>22</v>
       </c>
-      <c r="K18" s="177"/>
-      <c r="L18" s="177"/>
-      <c r="M18" s="177"/>
-      <c r="N18" s="177"/>
-      <c r="O18" s="177"/>
-      <c r="P18" s="177"/>
-      <c r="Q18" s="177"/>
-      <c r="R18" s="177"/>
-      <c r="S18" s="177"/>
-      <c r="T18" s="177"/>
-      <c r="U18" s="177"/>
-      <c r="V18" s="177"/>
-      <c r="W18" s="177"/>
-      <c r="X18" s="177"/>
+      <c r="K18" s="173"/>
+      <c r="L18" s="173"/>
+      <c r="M18" s="173"/>
+      <c r="N18" s="173"/>
+      <c r="O18" s="173"/>
+      <c r="P18" s="173"/>
+      <c r="Q18" s="173"/>
+      <c r="R18" s="173"/>
+      <c r="S18" s="173"/>
+      <c r="T18" s="173"/>
+      <c r="U18" s="173"/>
+      <c r="V18" s="173"/>
+      <c r="W18" s="173"/>
+      <c r="X18" s="173"/>
       <c r="Y18" s="2"/>
       <c r="Z18" s="4"/>
       <c r="AA18" s="16"/>
@@ -24549,23 +24590,23 @@
       <c r="I21" s="23">
         <v>1</v>
       </c>
-      <c r="J21" s="166" t="s">
+      <c r="J21" s="162" t="s">
         <v>34</v>
       </c>
-      <c r="K21" s="167"/>
-      <c r="L21" s="167"/>
-      <c r="M21" s="167"/>
-      <c r="N21" s="167"/>
-      <c r="O21" s="167"/>
-      <c r="P21" s="167"/>
-      <c r="Q21" s="167"/>
-      <c r="R21" s="167"/>
-      <c r="S21" s="167"/>
-      <c r="T21" s="167"/>
-      <c r="U21" s="167"/>
-      <c r="V21" s="167"/>
-      <c r="W21" s="167"/>
-      <c r="X21" s="178"/>
+      <c r="K21" s="163"/>
+      <c r="L21" s="163"/>
+      <c r="M21" s="163"/>
+      <c r="N21" s="163"/>
+      <c r="O21" s="163"/>
+      <c r="P21" s="163"/>
+      <c r="Q21" s="163"/>
+      <c r="R21" s="163"/>
+      <c r="S21" s="163"/>
+      <c r="T21" s="163"/>
+      <c r="U21" s="163"/>
+      <c r="V21" s="163"/>
+      <c r="W21" s="163"/>
+      <c r="X21" s="174"/>
       <c r="Y21" s="2"/>
       <c r="Z21" s="4"/>
       <c r="AA21" s="16"/>

</xml_diff>

<commit_message>
add ev confinement bool
</commit_message>
<xml_diff>
--- a/Structural.xlsx
+++ b/Structural.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A86B547-037F-40F2-84A8-52E8714D9AB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65BA74A-A3D5-4B54-958F-782253E3FC0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -23,8 +23,9 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Stock!$E$13:$W$31</definedName>
     <definedName name="a_nfoet_b1">Stock!$L$161:$V$161</definedName>
     <definedName name="a_nyatf_b1">Stock!$L$162:$V$162</definedName>
-    <definedName name="cashflow_periods" localSheetId="0">General!$I$68:$N$68</definedName>
+    <definedName name="cashflow_periods" localSheetId="0">General!$I$69:$N$69</definedName>
     <definedName name="dry_groups" localSheetId="0">General!$I$57:$J$57</definedName>
+    <definedName name="ev_is_confinement" localSheetId="0">General!$I$62:$M$62</definedName>
     <definedName name="foo_levels" localSheetId="0">General!$I$59:$K$59</definedName>
     <definedName name="grain_pools" localSheetId="0">General!$I$53:$J$53</definedName>
     <definedName name="grazing_int" localSheetId="0">General!$I$58:$L$58</definedName>
@@ -38,7 +39,7 @@
     <definedName name="i_condensefvp_type1">Stock!$Q$331</definedName>
     <definedName name="i_condensefvp_type3">Stock!$Q$343</definedName>
     <definedName name="i_d_pos">Stock!$I$56</definedName>
-    <definedName name="i_date_assetvalue" localSheetId="0">General!$I$67</definedName>
+    <definedName name="i_date_assetvalue" localSheetId="0">General!$I$68</definedName>
     <definedName name="i_dvp_mask_f1">Stock!$J$333:$O$333</definedName>
     <definedName name="i_dvp_mask_f3">Stock!$J$345:$M$345</definedName>
     <definedName name="i_e0_pos">Stock!$I$57</definedName>
@@ -110,10 +111,10 @@
     <definedName name="ia_prepost_b1">Stock!$L$160:$V$160</definedName>
     <definedName name="ia_sire_dsegroup">Stock!$L$152</definedName>
     <definedName name="ia_yatf_dsegroup_b1">Stock!$L$154:$V$154</definedName>
-    <definedName name="labour_period_len" localSheetId="0">General!$I$65</definedName>
+    <definedName name="labour_period_len" localSheetId="0">General!$I$66</definedName>
     <definedName name="pastures" localSheetId="0">General!$I$55:$K$55</definedName>
     <definedName name="pastures_exist" localSheetId="0">General!$I$56:$K$56</definedName>
-    <definedName name="phase_len" localSheetId="0">General!$I$63</definedName>
+    <definedName name="phase_len" localSheetId="0">General!$I$64</definedName>
     <definedName name="rdvp_type_r">Stock!$J$338:$L$338</definedName>
     <definedName name="sheep_pools" localSheetId="0">General!$I$61:$M$61</definedName>
     <definedName name="TL.d" localSheetId="0">[0]!L.d</definedName>
@@ -352,7 +353,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H65" authorId="0" shapeId="0" xr:uid="{A77A1A40-0F21-448B-8603-3590BB2B7FCC}">
+    <comment ref="H66" authorId="0" shapeId="0" xr:uid="{A77A1A40-0F21-448B-8603-3590BB2B7FCC}">
       <text>
         <r>
           <rPr>
@@ -376,7 +377,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H67" authorId="0" shapeId="0" xr:uid="{7111B94E-0C66-45F9-9AE6-D73FF089672B}">
+    <comment ref="H68" authorId="0" shapeId="0" xr:uid="{7111B94E-0C66-45F9-9AE6-D73FF089672B}">
       <text>
         <r>
           <rPr>
@@ -401,7 +402,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H68" authorId="0" shapeId="0" xr:uid="{D986A23C-0EF8-4BD4-9A81-D1BFD4E62E8B}">
+    <comment ref="H69" authorId="0" shapeId="0" xr:uid="{D986A23C-0EF8-4BD4-9A81-D1BFD4E62E8B}">
       <text>
         <r>
           <rPr>
@@ -1374,7 +1375,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="285">
   <si>
     <t>Controls for this worksheet</t>
   </si>
@@ -2240,6 +2241,9 @@
   </si>
   <si>
     <t>ev4</t>
+  </si>
+  <si>
+    <t>ev_is_confinement</t>
   </si>
 </sst>
 </file>
@@ -4345,10 +4349,10 @@
   <sheetPr codeName="Sheet2">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AT83"/>
+  <dimension ref="A1:AT84"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="L63" sqref="L63"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="I62" sqref="I62:M62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.35"/>
@@ -5739,7 +5743,7 @@
       <c r="A39" s="1"/>
       <c r="B39" s="33"/>
       <c r="C39" s="73">
-        <f>INT(MAX($C$50:$C$71))+1</f>
+        <f>INT(MAX($C$50:$C$72))+1</f>
         <v>4</v>
       </c>
       <c r="D39" s="3"/>
@@ -6153,7 +6157,7 @@
       <c r="A51" s="1"/>
       <c r="B51" s="33"/>
       <c r="C51" s="73">
-        <f t="shared" ref="C51:C70" si="1">INT($C$40)+2</f>
+        <f t="shared" ref="C51:C71" si="1">INT($C$40)+2</f>
         <v>3</v>
       </c>
       <c r="D51" s="4"/>
@@ -6581,20 +6585,29 @@
     <row r="62" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A62" s="1"/>
       <c r="B62" s="33"/>
-      <c r="C62" s="73">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
+      <c r="C62" s="73"/>
       <c r="D62" s="4"/>
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
       <c r="G62" s="4"/>
-      <c r="H62" s="2"/>
-      <c r="I62" s="2"/>
-      <c r="J62" s="2"/>
-      <c r="K62" s="2"/>
-      <c r="L62" s="2"/>
-      <c r="M62" s="2"/>
+      <c r="H62" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="I62" s="101" t="b">
+        <v>0</v>
+      </c>
+      <c r="J62" s="101" t="b">
+        <v>0</v>
+      </c>
+      <c r="K62" s="101" t="b">
+        <v>0</v>
+      </c>
+      <c r="L62" s="101" t="b">
+        <v>0</v>
+      </c>
+      <c r="M62" s="101" t="b">
+        <v>1</v>
+      </c>
       <c r="N62" s="2"/>
       <c r="O62" s="2"/>
       <c r="P62" s="2"/>
@@ -6622,12 +6635,8 @@
       <c r="E63" s="5"/>
       <c r="F63" s="5"/>
       <c r="G63" s="4"/>
-      <c r="H63" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="I63" s="101">
-        <v>6</v>
-      </c>
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
@@ -6659,8 +6668,12 @@
       <c r="E64" s="5"/>
       <c r="F64" s="5"/>
       <c r="G64" s="4"/>
-      <c r="H64" s="2"/>
-      <c r="I64" s="2"/>
+      <c r="H64" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="I64" s="101">
+        <v>6</v>
+      </c>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
@@ -6692,12 +6705,8 @@
       <c r="E65" s="5"/>
       <c r="F65" s="5"/>
       <c r="G65" s="4"/>
-      <c r="H65" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="I65" s="101">
-        <v>1</v>
-      </c>
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
       <c r="J65" s="2"/>
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
@@ -6729,8 +6738,12 @@
       <c r="E66" s="5"/>
       <c r="F66" s="5"/>
       <c r="G66" s="4"/>
-      <c r="H66" s="2"/>
-      <c r="I66" s="2"/>
+      <c r="H66" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="I66" s="101">
+        <v>1</v>
+      </c>
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
@@ -6762,16 +6775,10 @@
       <c r="E67" s="5"/>
       <c r="F67" s="5"/>
       <c r="G67" s="4"/>
-      <c r="H67" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="I67" s="140">
-        <v>43466</v>
-      </c>
+      <c r="H67" s="2"/>
+      <c r="I67" s="2"/>
       <c r="J67" s="2"/>
-      <c r="K67" s="2" t="s">
-        <v>169</v>
-      </c>
+      <c r="K67" s="2"/>
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
@@ -6789,23 +6796,6 @@
       <c r="Z67" s="1"/>
       <c r="AA67" s="1"/>
       <c r="AB67" s="1"/>
-      <c r="AD67" s="2"/>
-      <c r="AE67" s="2"/>
-      <c r="AF67" s="2"/>
-      <c r="AG67" s="2"/>
-      <c r="AH67" s="2"/>
-      <c r="AI67" s="2"/>
-      <c r="AJ67" s="2"/>
-      <c r="AK67" s="2"/>
-      <c r="AL67" s="2"/>
-      <c r="AM67" s="2"/>
-      <c r="AN67" s="2"/>
-      <c r="AO67" s="2"/>
-      <c r="AP67" s="4"/>
-      <c r="AQ67" s="16"/>
-      <c r="AR67" s="1"/>
-      <c r="AS67" s="1"/>
-      <c r="AT67" s="1"/>
     </row>
     <row r="68" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A68" s="1"/>
@@ -6819,26 +6809,18 @@
       <c r="F68" s="5"/>
       <c r="G68" s="4"/>
       <c r="H68" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="I68" s="140" t="s">
-        <v>185</v>
-      </c>
-      <c r="J68" s="140" t="s">
-        <v>186</v>
-      </c>
-      <c r="K68" s="140" t="s">
-        <v>187</v>
-      </c>
-      <c r="L68" s="140" t="s">
-        <v>188</v>
-      </c>
-      <c r="M68" s="140" t="s">
-        <v>189</v>
-      </c>
-      <c r="N68" s="140" t="s">
-        <v>190</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="I68" s="140">
+        <v>43466</v>
+      </c>
+      <c r="J68" s="2"/>
+      <c r="K68" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="L68" s="2"/>
+      <c r="M68" s="2"/>
+      <c r="N68" s="2"/>
       <c r="O68" s="2"/>
       <c r="P68" s="2"/>
       <c r="Q68" s="2"/>
@@ -6866,7 +6848,7 @@
       <c r="AN68" s="2"/>
       <c r="AO68" s="2"/>
       <c r="AP68" s="4"/>
-      <c r="AQ68" s="82"/>
+      <c r="AQ68" s="16"/>
       <c r="AR68" s="1"/>
       <c r="AS68" s="1"/>
       <c r="AT68" s="1"/>
@@ -6882,13 +6864,27 @@
       <c r="E69" s="5"/>
       <c r="F69" s="5"/>
       <c r="G69" s="4"/>
-      <c r="H69" s="2"/>
-      <c r="I69" s="2"/>
-      <c r="J69" s="2"/>
-      <c r="K69" s="2"/>
-      <c r="L69" s="2"/>
-      <c r="M69" s="2"/>
-      <c r="N69" s="2"/>
+      <c r="H69" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="I69" s="140" t="s">
+        <v>185</v>
+      </c>
+      <c r="J69" s="140" t="s">
+        <v>186</v>
+      </c>
+      <c r="K69" s="140" t="s">
+        <v>187</v>
+      </c>
+      <c r="L69" s="140" t="s">
+        <v>188</v>
+      </c>
+      <c r="M69" s="140" t="s">
+        <v>189</v>
+      </c>
+      <c r="N69" s="140" t="s">
+        <v>190</v>
+      </c>
       <c r="O69" s="2"/>
       <c r="P69" s="2"/>
       <c r="Q69" s="2"/>
@@ -6971,40 +6967,55 @@
       <c r="AS70" s="1"/>
       <c r="AT70" s="1"/>
     </row>
-    <row r="71" spans="1:46" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A71" s="1"/>
       <c r="B71" s="33"/>
       <c r="C71" s="73">
-        <f>INT($C$40)+2.005</f>
-        <v>3.0049999999999999</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="D71" s="4"/>
-      <c r="E71" s="4"/>
-      <c r="F71" s="4"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="5"/>
       <c r="G71" s="4"/>
-      <c r="H71" s="4"/>
-      <c r="I71" s="4"/>
-      <c r="J71" s="4"/>
-      <c r="K71" s="4"/>
-      <c r="L71" s="4"/>
-      <c r="M71" s="4"/>
-      <c r="N71" s="4"/>
-      <c r="O71" s="4"/>
-      <c r="P71" s="4"/>
-      <c r="Q71" s="4"/>
-      <c r="R71" s="4"/>
-      <c r="S71" s="4"/>
-      <c r="T71" s="4"/>
-      <c r="U71" s="4"/>
-      <c r="V71" s="4"/>
-      <c r="W71" s="4"/>
-      <c r="X71" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="H71" s="2"/>
+      <c r="I71" s="2"/>
+      <c r="J71" s="2"/>
+      <c r="K71" s="2"/>
+      <c r="L71" s="2"/>
+      <c r="M71" s="2"/>
+      <c r="N71" s="2"/>
+      <c r="O71" s="2"/>
+      <c r="P71" s="2"/>
+      <c r="Q71" s="2"/>
+      <c r="R71" s="2"/>
+      <c r="S71" s="2"/>
+      <c r="T71" s="2"/>
+      <c r="U71" s="2"/>
+      <c r="V71" s="2"/>
+      <c r="W71" s="2"/>
+      <c r="X71" s="4"/>
       <c r="Y71" s="16"/>
       <c r="Z71" s="1"/>
       <c r="AA71" s="1"/>
       <c r="AB71" s="1"/>
+      <c r="AD71" s="2"/>
+      <c r="AE71" s="2"/>
+      <c r="AF71" s="2"/>
+      <c r="AG71" s="2"/>
+      <c r="AH71" s="2"/>
+      <c r="AI71" s="2"/>
+      <c r="AJ71" s="2"/>
+      <c r="AK71" s="2"/>
+      <c r="AL71" s="2"/>
+      <c r="AM71" s="2"/>
+      <c r="AN71" s="2"/>
+      <c r="AO71" s="2"/>
+      <c r="AP71" s="4"/>
+      <c r="AQ71" s="82"/>
+      <c r="AR71" s="1"/>
+      <c r="AS71" s="1"/>
+      <c r="AT71" s="1"/>
     </row>
     <row r="72" spans="1:46" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A72" s="1"/>
@@ -7033,109 +7044,111 @@
       <c r="U72" s="4"/>
       <c r="V72" s="4"/>
       <c r="W72" s="4"/>
-      <c r="X72" s="4"/>
+      <c r="X72" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="Y72" s="16"/>
       <c r="Z72" s="1"/>
       <c r="AA72" s="1"/>
       <c r="AB72" s="1"/>
     </row>
-    <row r="73" spans="1:46" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:46" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A73" s="1"/>
-      <c r="B73" s="35"/>
-      <c r="C73" s="76">
-        <f>INT($C$40)+1.005</f>
-        <v>2.0049999999999999</v>
-      </c>
-      <c r="D73" s="17"/>
-      <c r="E73" s="17"/>
-      <c r="F73" s="17"/>
-      <c r="G73" s="17"/>
-      <c r="H73" s="17"/>
-      <c r="I73" s="17"/>
-      <c r="J73" s="17"/>
-      <c r="K73" s="17"/>
-      <c r="L73" s="17"/>
-      <c r="M73" s="17"/>
-      <c r="N73" s="17"/>
-      <c r="O73" s="17"/>
-      <c r="P73" s="17"/>
-      <c r="Q73" s="17"/>
-      <c r="R73" s="17"/>
-      <c r="S73" s="17"/>
-      <c r="T73" s="17"/>
-      <c r="U73" s="17"/>
-      <c r="V73" s="17"/>
-      <c r="W73" s="17"/>
-      <c r="X73" s="17"/>
-      <c r="Y73" s="18" t="s">
-        <v>1</v>
-      </c>
+      <c r="B73" s="33"/>
+      <c r="C73" s="73">
+        <f>INT($C$40)+2.005</f>
+        <v>3.0049999999999999</v>
+      </c>
+      <c r="D73" s="4"/>
+      <c r="E73" s="4"/>
+      <c r="F73" s="4"/>
+      <c r="G73" s="4"/>
+      <c r="H73" s="4"/>
+      <c r="I73" s="4"/>
+      <c r="J73" s="4"/>
+      <c r="K73" s="4"/>
+      <c r="L73" s="4"/>
+      <c r="M73" s="4"/>
+      <c r="N73" s="4"/>
+      <c r="O73" s="4"/>
+      <c r="P73" s="4"/>
+      <c r="Q73" s="4"/>
+      <c r="R73" s="4"/>
+      <c r="S73" s="4"/>
+      <c r="T73" s="4"/>
+      <c r="U73" s="4"/>
+      <c r="V73" s="4"/>
+      <c r="W73" s="4"/>
+      <c r="X73" s="4"/>
+      <c r="Y73" s="16"/>
       <c r="Z73" s="1"/>
       <c r="AA73" s="1"/>
       <c r="AB73" s="1"/>
     </row>
-    <row r="74" spans="1:46" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:46" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A74" s="1"/>
-      <c r="B74" s="19"/>
-      <c r="C74" s="77">
-        <f>INT($C$40)+0.005</f>
-        <v>1.0049999999999999</v>
-      </c>
-      <c r="D74" s="19"/>
-      <c r="E74" s="19"/>
-      <c r="F74" s="19"/>
-      <c r="G74" s="19"/>
-      <c r="H74" s="19"/>
-      <c r="I74" s="19"/>
-      <c r="J74" s="19"/>
-      <c r="K74" s="19"/>
-      <c r="L74" s="19"/>
-      <c r="M74" s="19"/>
-      <c r="N74" s="19"/>
-      <c r="O74" s="19"/>
-      <c r="P74" s="19"/>
-      <c r="Q74" s="19"/>
-      <c r="R74" s="19"/>
-      <c r="S74" s="19"/>
-      <c r="T74" s="19"/>
-      <c r="U74" s="19"/>
-      <c r="V74" s="19"/>
-      <c r="W74" s="19"/>
-      <c r="X74" s="19"/>
-      <c r="Y74" s="19"/>
+      <c r="B74" s="35"/>
+      <c r="C74" s="76">
+        <f>INT($C$40)+1.005</f>
+        <v>2.0049999999999999</v>
+      </c>
+      <c r="D74" s="17"/>
+      <c r="E74" s="17"/>
+      <c r="F74" s="17"/>
+      <c r="G74" s="17"/>
+      <c r="H74" s="17"/>
+      <c r="I74" s="17"/>
+      <c r="J74" s="17"/>
+      <c r="K74" s="17"/>
+      <c r="L74" s="17"/>
+      <c r="M74" s="17"/>
+      <c r="N74" s="17"/>
+      <c r="O74" s="17"/>
+      <c r="P74" s="17"/>
+      <c r="Q74" s="17"/>
+      <c r="R74" s="17"/>
+      <c r="S74" s="17"/>
+      <c r="T74" s="17"/>
+      <c r="U74" s="17"/>
+      <c r="V74" s="17"/>
+      <c r="W74" s="17"/>
+      <c r="X74" s="17"/>
+      <c r="Y74" s="18" t="s">
+        <v>1</v>
+      </c>
       <c r="Z74" s="1"/>
       <c r="AA74" s="1"/>
       <c r="AB74" s="1"/>
     </row>
-    <row r="75" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:46" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="1"/>
-      <c r="B75" s="1"/>
-      <c r="C75" s="73">
-        <f>INT($C$40)+2</f>
-        <v>3</v>
-      </c>
-      <c r="D75" s="1"/>
-      <c r="E75" s="1"/>
-      <c r="F75" s="1"/>
-      <c r="G75" s="1"/>
-      <c r="H75" s="1"/>
-      <c r="I75" s="1"/>
-      <c r="J75" s="1"/>
-      <c r="K75" s="1"/>
-      <c r="L75" s="1"/>
-      <c r="M75" s="1"/>
-      <c r="N75" s="1"/>
-      <c r="O75" s="1"/>
-      <c r="P75" s="1"/>
-      <c r="Q75" s="1"/>
-      <c r="R75" s="1"/>
-      <c r="S75" s="1"/>
-      <c r="T75" s="1"/>
-      <c r="U75" s="1"/>
-      <c r="V75" s="1"/>
-      <c r="W75" s="1"/>
-      <c r="X75" s="1"/>
-      <c r="Y75" s="1"/>
+      <c r="B75" s="19"/>
+      <c r="C75" s="77">
+        <f>INT($C$40)+0.005</f>
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="D75" s="19"/>
+      <c r="E75" s="19"/>
+      <c r="F75" s="19"/>
+      <c r="G75" s="19"/>
+      <c r="H75" s="19"/>
+      <c r="I75" s="19"/>
+      <c r="J75" s="19"/>
+      <c r="K75" s="19"/>
+      <c r="L75" s="19"/>
+      <c r="M75" s="19"/>
+      <c r="N75" s="19"/>
+      <c r="O75" s="19"/>
+      <c r="P75" s="19"/>
+      <c r="Q75" s="19"/>
+      <c r="R75" s="19"/>
+      <c r="S75" s="19"/>
+      <c r="T75" s="19"/>
+      <c r="U75" s="19"/>
+      <c r="V75" s="19"/>
+      <c r="W75" s="19"/>
+      <c r="X75" s="19"/>
+      <c r="Y75" s="19"/>
       <c r="Z75" s="1"/>
       <c r="AA75" s="1"/>
       <c r="AB75" s="1"/>
@@ -7173,10 +7186,13 @@
       <c r="AA76" s="1"/>
       <c r="AB76" s="1"/>
     </row>
-    <row r="77" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
-      <c r="C77" s="66"/>
+      <c r="C77" s="73">
+        <f>INT($C$40)+2</f>
+        <v>3</v>
+      </c>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
@@ -7354,7 +7370,37 @@
       <c r="AB82" s="1"/>
     </row>
     <row r="83" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="C83" s="72" t="s">
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
+      <c r="C83" s="66"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1"/>
+      <c r="F83" s="1"/>
+      <c r="G83" s="1"/>
+      <c r="H83" s="1"/>
+      <c r="I83" s="1"/>
+      <c r="J83" s="1"/>
+      <c r="K83" s="1"/>
+      <c r="L83" s="1"/>
+      <c r="M83" s="1"/>
+      <c r="N83" s="1"/>
+      <c r="O83" s="1"/>
+      <c r="P83" s="1"/>
+      <c r="Q83" s="1"/>
+      <c r="R83" s="1"/>
+      <c r="S83" s="1"/>
+      <c r="T83" s="1"/>
+      <c r="U83" s="1"/>
+      <c r="V83" s="1"/>
+      <c r="W83" s="1"/>
+      <c r="X83" s="1"/>
+      <c r="Y83" s="1"/>
+      <c r="Z83" s="1"/>
+      <c r="AA83" s="1"/>
+      <c r="AB83" s="1"/>
+    </row>
+    <row r="84" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="C84" s="72" t="s">
         <v>4</v>
       </c>
     </row>
@@ -7377,7 +7423,7 @@
   </sheetPr>
   <dimension ref="A1:AE361"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B312" workbookViewId="0">
+    <sheetView topLeftCell="B312" workbookViewId="0">
       <selection activeCell="R323" sqref="R323:W325"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Change to confinement feeding patterns
</commit_message>
<xml_diff>
--- a/Structural.xlsx
+++ b/Structural.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48FDBA6A-17FA-43AE-AC8E-16E3FF222D2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8453274D-35C0-4FAE-9DCE-DAB105641A4F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="0" yWindow="690" windowWidth="27870" windowHeight="15255" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -141,14 +141,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -2253,7 +2245,14 @@
     <t>post birth</t>
   </si>
   <si>
-    <t>12Apr21: Change back to 3N for analysis
+    <t>ev4</t>
+  </si>
+  <si>
+    <t>ev_is_not_confinement</t>
+  </si>
+  <si>
+    <t>14Apr21: MRY changes for EV pools and confinement (removed about confinement patterns being included)
+12Apr21: Change back to 3N for analysis
                   1N for LW profile comparisons
 10Apr21: Altered k2 cluster for scan 0 to allocate all ewes to the 11 slice
                    Changed inputs for GBAL because it can't be represented in the matrix
@@ -2263,12 +2262,6 @@
 29Mar21: Changed to FVP3, 1N for dams, 3N for Offs
 22Mar21: Alter the initial weight &amp; wool spread for the weaners
 1: 1Apr19-Blank worksheet</t>
-  </si>
-  <si>
-    <t>ev4</t>
-  </si>
-  <si>
-    <t>ev_is_not_confinement</t>
   </si>
 </sst>
 </file>
@@ -4380,25 +4373,25 @@
       <selection activeCell="I62" sqref="I62:M62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" style="142" customWidth="1"/>
-    <col min="2" max="2" width="2.7265625" style="142" customWidth="1"/>
-    <col min="3" max="3" width="4.7265625" style="142" customWidth="1" outlineLevel="2"/>
-    <col min="4" max="4" width="1.7265625" style="142" customWidth="1"/>
-    <col min="5" max="6" width="9.7265625" style="142" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="1.7265625" style="142" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="37.26953125" style="142" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7265625" style="142" customWidth="1"/>
-    <col min="10" max="23" width="10.81640625" style="142" customWidth="1"/>
-    <col min="24" max="24" width="1.7265625" style="142" customWidth="1"/>
-    <col min="25" max="26" width="4.7265625" style="142" customWidth="1"/>
-    <col min="27" max="27" width="8.7265625" style="142"/>
-    <col min="28" max="28" width="46.1796875" style="142" customWidth="1"/>
-    <col min="29" max="16384" width="8.7265625" style="142"/>
+    <col min="1" max="1" width="4.7109375" style="142" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" style="142" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" style="142" customWidth="1" outlineLevel="2"/>
+    <col min="4" max="4" width="1.7109375" style="142" customWidth="1"/>
+    <col min="5" max="6" width="9.7109375" style="142" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="1.7109375" style="142" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="37.28515625" style="142" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="142" customWidth="1"/>
+    <col min="10" max="23" width="10.85546875" style="142" customWidth="1"/>
+    <col min="24" max="24" width="1.7109375" style="142" customWidth="1"/>
+    <col min="25" max="26" width="4.7109375" style="142" customWidth="1"/>
+    <col min="27" max="27" width="8.7109375" style="142"/>
+    <col min="28" max="28" width="46.140625" style="142" customWidth="1"/>
+    <col min="29" max="16384" width="8.7109375" style="142"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="66"/>
@@ -4428,7 +4421,7 @@
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
     </row>
-    <row r="2" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="67">
@@ -4461,7 +4454,7 @@
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
     </row>
-    <row r="3" spans="1:28" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:28" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="20"/>
       <c r="C3" s="68">
@@ -4494,7 +4487,7 @@
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
     </row>
-    <row r="4" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="34" t="s">
         <v>21</v>
@@ -4529,7 +4522,7 @@
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
     </row>
-    <row r="5" spans="1:28" hidden="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:28" hidden="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="33"/>
       <c r="C5" s="67">
@@ -4600,7 +4593,7 @@
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
     </row>
-    <row r="6" spans="1:28" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="33"/>
       <c r="C6" s="67">
@@ -4638,7 +4631,7 @@
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
     </row>
-    <row r="7" spans="1:28" ht="20.149999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="33"/>
       <c r="C7" s="67">
@@ -4677,7 +4670,7 @@
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
     </row>
-    <row r="8" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="33"/>
       <c r="C8" s="67">
@@ -4710,7 +4703,7 @@
       <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
     </row>
-    <row r="9" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="33"/>
       <c r="C9" s="67">
@@ -4743,7 +4736,7 @@
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
     </row>
-    <row r="10" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="33"/>
       <c r="C10" s="67">
@@ -4776,7 +4769,7 @@
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
     </row>
-    <row r="11" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="33"/>
       <c r="C11" s="67">
@@ -4809,7 +4802,7 @@
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
     </row>
-    <row r="12" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="33"/>
       <c r="C12" s="67">
@@ -4846,7 +4839,7 @@
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
     </row>
-    <row r="13" spans="1:28" ht="11.5" hidden="1" customHeight="1" outlineLevel="3" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:28" ht="11.45" hidden="1" customHeight="1" outlineLevel="3" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="33" t="s">
         <v>20</v>
@@ -4881,7 +4874,7 @@
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
     </row>
-    <row r="14" spans="1:28" hidden="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:28" hidden="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="33"/>
       <c r="C14" s="67">
@@ -4914,7 +4907,7 @@
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
     </row>
-    <row r="15" spans="1:28" hidden="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:28" hidden="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="33"/>
       <c r="C15" s="67">
@@ -4947,7 +4940,7 @@
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
     </row>
-    <row r="16" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="33" t="s">
         <v>19</v>
@@ -4984,7 +4977,7 @@
       <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>
     </row>
-    <row r="17" spans="1:28" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:28" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="33"/>
       <c r="C17" s="67">
@@ -5019,7 +5012,7 @@
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
     </row>
-    <row r="18" spans="1:28" ht="45" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:28" ht="45" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="33"/>
       <c r="C18" s="67">
@@ -5058,7 +5051,7 @@
       <c r="AA18" s="1"/>
       <c r="AB18" s="1"/>
     </row>
-    <row r="19" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="33"/>
       <c r="C19" s="67">
@@ -5091,7 +5084,7 @@
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
     </row>
-    <row r="20" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="33"/>
       <c r="C20" s="67">
@@ -5124,7 +5117,7 @@
       <c r="AA20" s="1"/>
       <c r="AB20" s="1"/>
     </row>
-    <row r="21" spans="1:28" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:28" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="33"/>
       <c r="C21" s="67">
@@ -5163,7 +5156,7 @@
       <c r="AA21" s="1"/>
       <c r="AB21" s="1"/>
     </row>
-    <row r="22" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="33"/>
       <c r="C22" s="67">
@@ -5196,7 +5189,7 @@
       <c r="AA22" s="1"/>
       <c r="AB22" s="1"/>
     </row>
-    <row r="23" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="33"/>
       <c r="C23" s="67">
@@ -5229,7 +5222,7 @@
       <c r="AA23" s="1"/>
       <c r="AB23" s="1"/>
     </row>
-    <row r="24" spans="1:28" ht="5.15" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="33"/>
       <c r="C24" s="67">
@@ -5264,7 +5257,7 @@
       <c r="AA24" s="1"/>
       <c r="AB24" s="1"/>
     </row>
-    <row r="25" spans="1:28" ht="5.15" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="33"/>
       <c r="C25" s="67">
@@ -5299,7 +5292,7 @@
       <c r="AA25" s="1"/>
       <c r="AB25" s="1"/>
     </row>
-    <row r="26" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="33"/>
       <c r="C26" s="67">
@@ -5346,7 +5339,7 @@
       <c r="AA26" s="1"/>
       <c r="AB26" s="1"/>
     </row>
-    <row r="27" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="33"/>
       <c r="C27" s="67">
@@ -5383,7 +5376,7 @@
       <c r="AA27" s="1"/>
       <c r="AB27" s="1"/>
     </row>
-    <row r="28" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="33"/>
       <c r="C28" s="67">
@@ -5420,7 +5413,7 @@
       <c r="AA28" s="1"/>
       <c r="AB28" s="1"/>
     </row>
-    <row r="29" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="33"/>
       <c r="C29" s="67">
@@ -5457,7 +5450,7 @@
       <c r="AA29" s="1"/>
       <c r="AB29" s="1"/>
     </row>
-    <row r="30" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="33"/>
       <c r="C30" s="67">
@@ -5494,7 +5487,7 @@
       <c r="AA30" s="1"/>
       <c r="AB30" s="1"/>
     </row>
-    <row r="31" spans="1:28" ht="5.15" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="33"/>
       <c r="C31" s="67">
@@ -5529,7 +5522,7 @@
       <c r="AA31" s="1"/>
       <c r="AB31" s="1"/>
     </row>
-    <row r="32" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="33"/>
       <c r="C32" s="67">
@@ -5562,7 +5555,7 @@
       <c r="AA32" s="1"/>
       <c r="AB32" s="1"/>
     </row>
-    <row r="33" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="35"/>
       <c r="C33" s="70">
@@ -5597,7 +5590,7 @@
       <c r="AA33" s="1"/>
       <c r="AB33" s="1"/>
     </row>
-    <row r="34" spans="1:28" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:28" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="19"/>
       <c r="C34" s="71">
@@ -5630,7 +5623,7 @@
       <c r="AA34" s="1"/>
       <c r="AB34" s="1"/>
     </row>
-    <row r="35" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="67">
@@ -5663,7 +5656,7 @@
       <c r="AA35" s="1"/>
       <c r="AB35" s="1"/>
     </row>
-    <row r="36" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="73">
@@ -5696,7 +5689,7 @@
       <c r="AA36" s="1"/>
       <c r="AB36" s="1"/>
     </row>
-    <row r="37" spans="1:28" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:28" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="20"/>
       <c r="C37" s="74">
@@ -5729,7 +5722,7 @@
       <c r="AA37" s="1"/>
       <c r="AB37" s="1"/>
     </row>
-    <row r="38" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="34" t="s">
         <v>21</v>
@@ -5764,7 +5757,7 @@
       <c r="AA38" s="1"/>
       <c r="AB38" s="1"/>
     </row>
-    <row r="39" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="33"/>
       <c r="C39" s="73">
@@ -5797,7 +5790,7 @@
       <c r="AA39" s="1"/>
       <c r="AB39" s="1"/>
     </row>
-    <row r="40" spans="1:28" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="33"/>
       <c r="C40" s="73">
@@ -5834,7 +5827,7 @@
       <c r="AA40" s="1"/>
       <c r="AB40" s="1"/>
     </row>
-    <row r="41" spans="1:28" ht="20.149999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:28" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="33"/>
       <c r="C41" s="73">
@@ -5873,7 +5866,7 @@
       <c r="AA41" s="1"/>
       <c r="AB41" s="1"/>
     </row>
-    <row r="42" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="33"/>
       <c r="C42" s="73">
@@ -5906,7 +5899,7 @@
       <c r="AA42" s="1"/>
       <c r="AB42" s="1"/>
     </row>
-    <row r="43" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="33"/>
       <c r="C43" s="73">
@@ -5939,7 +5932,7 @@
       <c r="AA43" s="1"/>
       <c r="AB43" s="1"/>
     </row>
-    <row r="44" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="33"/>
       <c r="C44" s="73">
@@ -5972,7 +5965,7 @@
       <c r="AA44" s="1"/>
       <c r="AB44" s="1"/>
     </row>
-    <row r="45" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="33"/>
       <c r="C45" s="73">
@@ -6005,7 +5998,7 @@
       <c r="AA45" s="1"/>
       <c r="AB45" s="1"/>
     </row>
-    <row r="46" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="33"/>
       <c r="C46" s="73">
@@ -6038,7 +6031,7 @@
       <c r="AA46" s="1"/>
       <c r="AB46" s="1"/>
     </row>
-    <row r="47" spans="1:28" ht="11.5" customHeight="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:28" ht="11.45" customHeight="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="33" t="s">
         <v>20</v>
@@ -6073,7 +6066,7 @@
       <c r="AA47" s="1"/>
       <c r="AB47" s="1"/>
     </row>
-    <row r="48" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="33"/>
       <c r="C48" s="73">
@@ -6106,7 +6099,7 @@
       <c r="AA48" s="1"/>
       <c r="AB48" s="1"/>
     </row>
-    <row r="49" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="33" t="s">
         <v>19</v>
@@ -6143,7 +6136,7 @@
       <c r="AA49" s="1"/>
       <c r="AB49" s="1"/>
     </row>
-    <row r="50" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="33"/>
       <c r="C50" s="73">
@@ -6178,7 +6171,7 @@
       <c r="AA50" s="1"/>
       <c r="AB50" s="1"/>
     </row>
-    <row r="51" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="33"/>
       <c r="C51" s="73">
@@ -6219,7 +6212,7 @@
       <c r="AA51" s="1"/>
       <c r="AB51" s="1"/>
     </row>
-    <row r="52" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="33"/>
       <c r="C52" s="73">
@@ -6252,7 +6245,7 @@
       <c r="AA52" s="1"/>
       <c r="AB52" s="1"/>
     </row>
-    <row r="53" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="33"/>
       <c r="C53" s="73">
@@ -6291,7 +6284,7 @@
       <c r="AA53" s="1"/>
       <c r="AB53" s="1"/>
     </row>
-    <row r="54" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="33"/>
       <c r="C54" s="73">
@@ -6324,7 +6317,7 @@
       <c r="AA54" s="1"/>
       <c r="AB54" s="1"/>
     </row>
-    <row r="55" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="33"/>
       <c r="C55" s="73">
@@ -6365,7 +6358,7 @@
       <c r="AA55" s="1"/>
       <c r="AB55" s="1"/>
     </row>
-    <row r="56" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="33"/>
       <c r="C56" s="73">
@@ -6406,7 +6399,7 @@
       <c r="AA56" s="1"/>
       <c r="AB56" s="1"/>
     </row>
-    <row r="57" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="33"/>
       <c r="C57" s="73">
@@ -6445,7 +6438,7 @@
       <c r="AA57" s="1"/>
       <c r="AB57" s="1"/>
     </row>
-    <row r="58" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="33"/>
       <c r="C58" s="73">
@@ -6488,7 +6481,7 @@
       <c r="AA58" s="1"/>
       <c r="AB58" s="1"/>
     </row>
-    <row r="59" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="33"/>
       <c r="C59" s="73">
@@ -6529,7 +6522,7 @@
       <c r="AA59" s="1"/>
       <c r="AB59" s="1"/>
     </row>
-    <row r="60" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="33"/>
       <c r="C60" s="73">
@@ -6562,7 +6555,7 @@
       <c r="AA60" s="1"/>
       <c r="AB60" s="1"/>
     </row>
-    <row r="61" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="33"/>
       <c r="C61" s="73">
@@ -6589,7 +6582,7 @@
         <v>265</v>
       </c>
       <c r="M61" s="101" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="N61" s="2"/>
       <c r="O61" s="2"/>
@@ -6607,7 +6600,7 @@
       <c r="AA61" s="1"/>
       <c r="AB61" s="1"/>
     </row>
-    <row r="62" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="33"/>
       <c r="C62" s="73"/>
@@ -6616,7 +6609,7 @@
       <c r="F62" s="5"/>
       <c r="G62" s="4"/>
       <c r="H62" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I62" s="101" t="b">
         <v>1</v>
@@ -6649,7 +6642,7 @@
       <c r="AA62" s="1"/>
       <c r="AB62" s="1"/>
     </row>
-    <row r="63" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="33"/>
       <c r="C63" s="73">
@@ -6682,7 +6675,7 @@
       <c r="AA63" s="1"/>
       <c r="AB63" s="1"/>
     </row>
-    <row r="64" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="33"/>
       <c r="C64" s="73">
@@ -6719,7 +6712,7 @@
       <c r="AA64" s="1"/>
       <c r="AB64" s="1"/>
     </row>
-    <row r="65" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="33"/>
       <c r="C65" s="73">
@@ -6752,7 +6745,7 @@
       <c r="AA65" s="1"/>
       <c r="AB65" s="1"/>
     </row>
-    <row r="66" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="33"/>
       <c r="C66" s="73">
@@ -6789,7 +6782,7 @@
       <c r="AA66" s="1"/>
       <c r="AB66" s="1"/>
     </row>
-    <row r="67" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="33"/>
       <c r="C67" s="73">
@@ -6822,7 +6815,7 @@
       <c r="AA67" s="1"/>
       <c r="AB67" s="1"/>
     </row>
-    <row r="68" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="33"/>
       <c r="C68" s="73">
@@ -6878,7 +6871,7 @@
       <c r="AS68" s="1"/>
       <c r="AT68" s="1"/>
     </row>
-    <row r="69" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="33"/>
       <c r="C69" s="73">
@@ -6942,7 +6935,7 @@
       <c r="AS69" s="1"/>
       <c r="AT69" s="1"/>
     </row>
-    <row r="70" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="33"/>
       <c r="C70" s="73">
@@ -6992,7 +6985,7 @@
       <c r="AS70" s="1"/>
       <c r="AT70" s="1"/>
     </row>
-    <row r="71" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="33"/>
       <c r="C71" s="73">
@@ -7042,7 +7035,7 @@
       <c r="AS71" s="1"/>
       <c r="AT71" s="1"/>
     </row>
-    <row r="72" spans="1:46" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:46" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="33"/>
       <c r="C72" s="73">
@@ -7077,7 +7070,7 @@
       <c r="AA72" s="1"/>
       <c r="AB72" s="1"/>
     </row>
-    <row r="73" spans="1:46" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:46" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="33"/>
       <c r="C73" s="73">
@@ -7110,7 +7103,7 @@
       <c r="AA73" s="1"/>
       <c r="AB73" s="1"/>
     </row>
-    <row r="74" spans="1:46" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:46" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="35"/>
       <c r="C74" s="76">
@@ -7145,7 +7138,7 @@
       <c r="AA74" s="1"/>
       <c r="AB74" s="1"/>
     </row>
-    <row r="75" spans="1:46" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:46" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="19"/>
       <c r="C75" s="77">
@@ -7178,7 +7171,7 @@
       <c r="AA75" s="1"/>
       <c r="AB75" s="1"/>
     </row>
-    <row r="76" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="73">
@@ -7211,7 +7204,7 @@
       <c r="AA76" s="1"/>
       <c r="AB76" s="1"/>
     </row>
-    <row r="77" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:46" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="73">
@@ -7244,7 +7237,7 @@
       <c r="AA77" s="1"/>
       <c r="AB77" s="1"/>
     </row>
-    <row r="78" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="66"/>
@@ -7274,7 +7267,7 @@
       <c r="AA78" s="1"/>
       <c r="AB78" s="1"/>
     </row>
-    <row r="79" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="66"/>
@@ -7304,7 +7297,7 @@
       <c r="AA79" s="1"/>
       <c r="AB79" s="1"/>
     </row>
-    <row r="80" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="66"/>
@@ -7334,7 +7327,7 @@
       <c r="AA80" s="1"/>
       <c r="AB80" s="1"/>
     </row>
-    <row r="81" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="66"/>
@@ -7364,7 +7357,7 @@
       <c r="AA81" s="1"/>
       <c r="AB81" s="1"/>
     </row>
-    <row r="82" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="66"/>
@@ -7394,7 +7387,7 @@
       <c r="AA82" s="1"/>
       <c r="AB82" s="1"/>
     </row>
-    <row r="83" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="66"/>
@@ -7424,7 +7417,7 @@
       <c r="AA83" s="1"/>
       <c r="AB83" s="1"/>
     </row>
-    <row r="84" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C84" s="72" t="s">
         <v>4</v>
       </c>
@@ -7448,27 +7441,27 @@
   </sheetPr>
   <dimension ref="A1:AE361"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B312" workbookViewId="0">
-      <selection activeCell="P324" sqref="P324"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21:T21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" customWidth="1"/>
-    <col min="2" max="2" width="2.7265625" customWidth="1"/>
-    <col min="3" max="3" width="4.7265625" customWidth="1" outlineLevel="2"/>
-    <col min="4" max="4" width="1.7265625" customWidth="1"/>
-    <col min="5" max="6" width="9.7265625" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="1.7265625" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="37.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.54296875" customWidth="1"/>
-    <col min="10" max="23" width="10.81640625" customWidth="1"/>
-    <col min="24" max="24" width="1.7265625" customWidth="1"/>
-    <col min="25" max="26" width="4.7265625" customWidth="1"/>
-    <col min="28" max="28" width="46.1796875" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="4" max="4" width="1.7109375" customWidth="1"/>
+    <col min="5" max="6" width="9.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="1.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" customWidth="1"/>
+    <col min="10" max="23" width="10.85546875" customWidth="1"/>
+    <col min="24" max="24" width="1.7109375" customWidth="1"/>
+    <col min="25" max="26" width="4.7109375" customWidth="1"/>
+    <col min="28" max="28" width="46.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="66"/>
@@ -7498,7 +7491,7 @@
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
     </row>
-    <row r="2" spans="1:28" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="67">
@@ -7531,7 +7524,7 @@
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
     </row>
-    <row r="3" spans="1:28" ht="5.15" customHeight="1" collapsed="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:28" ht="5.0999999999999996" customHeight="1" collapsed="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="20"/>
       <c r="C3" s="68">
@@ -7564,7 +7557,7 @@
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
     </row>
-    <row r="4" spans="1:28" ht="5.15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="34" t="s">
         <v>21</v>
@@ -7599,7 +7592,7 @@
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
     </row>
-    <row r="5" spans="1:28" hidden="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:28" hidden="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="33"/>
       <c r="C5" s="67">
@@ -7670,7 +7663,7 @@
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
     </row>
-    <row r="6" spans="1:28" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="33"/>
       <c r="C6" s="67">
@@ -7708,7 +7701,7 @@
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
     </row>
-    <row r="7" spans="1:28" ht="20.149999999999999" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" ht="20.100000000000001" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="33"/>
       <c r="C7" s="67">
@@ -7747,7 +7740,7 @@
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
     </row>
-    <row r="8" spans="1:28" ht="5.15" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="33"/>
       <c r="C8" s="67">
@@ -7780,7 +7773,7 @@
       <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
     </row>
-    <row r="9" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="33"/>
       <c r="C9" s="67">
@@ -7813,7 +7806,7 @@
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
     </row>
-    <row r="10" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="33"/>
       <c r="C10" s="67">
@@ -7846,7 +7839,7 @@
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
     </row>
-    <row r="11" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="33"/>
       <c r="C11" s="67">
@@ -7879,7 +7872,7 @@
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
     </row>
-    <row r="12" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="33"/>
       <c r="C12" s="67">
@@ -7916,7 +7909,7 @@
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
     </row>
-    <row r="13" spans="1:28" ht="11.5" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:28" ht="11.45" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="33" t="s">
         <v>20</v>
@@ -7951,7 +7944,7 @@
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
     </row>
-    <row r="14" spans="1:28" hidden="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:28" hidden="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="33"/>
       <c r="C14" s="67">
@@ -7984,7 +7977,7 @@
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
     </row>
-    <row r="15" spans="1:28" hidden="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:28" hidden="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="33"/>
       <c r="C15" s="67">
@@ -8017,7 +8010,7 @@
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
     </row>
-    <row r="16" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="33" t="s">
         <v>19</v>
@@ -8054,7 +8047,7 @@
       <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>
     </row>
-    <row r="17" spans="1:28" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:28" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="33"/>
       <c r="C17" s="67">
@@ -8089,7 +8082,7 @@
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
     </row>
-    <row r="18" spans="1:28" ht="45" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:28" ht="45" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="33"/>
       <c r="C18" s="67">
@@ -8128,7 +8121,7 @@
       <c r="AA18" s="1"/>
       <c r="AB18" s="1"/>
     </row>
-    <row r="19" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="33"/>
       <c r="C19" s="67">
@@ -8161,7 +8154,7 @@
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
     </row>
-    <row r="20" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="33"/>
       <c r="C20" s="67">
@@ -8194,7 +8187,7 @@
       <c r="AA20" s="1"/>
       <c r="AB20" s="1"/>
     </row>
-    <row r="21" spans="1:28" ht="45" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:28" ht="45" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="33"/>
       <c r="C21" s="67">
@@ -8209,10 +8202,10 @@
         <v>17</v>
       </c>
       <c r="I21" s="150">
-        <v>44298</v>
+        <v>44300</v>
       </c>
       <c r="J21" s="176" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="K21" s="177"/>
       <c r="L21" s="177"/>
@@ -8233,7 +8226,7 @@
       <c r="AA21" s="1"/>
       <c r="AB21" s="1"/>
     </row>
-    <row r="22" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="33"/>
       <c r="C22" s="67">
@@ -8266,7 +8259,7 @@
       <c r="AA22" s="1"/>
       <c r="AB22" s="1"/>
     </row>
-    <row r="23" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="33"/>
       <c r="C23" s="67">
@@ -8299,7 +8292,7 @@
       <c r="AA23" s="1"/>
       <c r="AB23" s="1"/>
     </row>
-    <row r="24" spans="1:28" ht="5.15" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="33"/>
       <c r="C24" s="67">
@@ -8334,7 +8327,7 @@
       <c r="AA24" s="1"/>
       <c r="AB24" s="1"/>
     </row>
-    <row r="25" spans="1:28" ht="5.15" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="33"/>
       <c r="C25" s="67">
@@ -8369,7 +8362,7 @@
       <c r="AA25" s="1"/>
       <c r="AB25" s="1"/>
     </row>
-    <row r="26" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="33"/>
       <c r="C26" s="67">
@@ -8416,7 +8409,7 @@
       <c r="AA26" s="1"/>
       <c r="AB26" s="1"/>
     </row>
-    <row r="27" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="33"/>
       <c r="C27" s="67">
@@ -8453,7 +8446,7 @@
       <c r="AA27" s="1"/>
       <c r="AB27" s="1"/>
     </row>
-    <row r="28" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="33"/>
       <c r="C28" s="67">
@@ -8490,7 +8483,7 @@
       <c r="AA28" s="1"/>
       <c r="AB28" s="1"/>
     </row>
-    <row r="29" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="33"/>
       <c r="C29" s="67">
@@ -8527,7 +8520,7 @@
       <c r="AA29" s="1"/>
       <c r="AB29" s="1"/>
     </row>
-    <row r="30" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="33"/>
       <c r="C30" s="67">
@@ -8564,7 +8557,7 @@
       <c r="AA30" s="1"/>
       <c r="AB30" s="1"/>
     </row>
-    <row r="31" spans="1:28" ht="5.15" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="33"/>
       <c r="C31" s="67">
@@ -8599,7 +8592,7 @@
       <c r="AA31" s="1"/>
       <c r="AB31" s="1"/>
     </row>
-    <row r="32" spans="1:28" ht="5.15" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="33"/>
       <c r="C32" s="67">
@@ -8632,7 +8625,7 @@
       <c r="AA32" s="1"/>
       <c r="AB32" s="1"/>
     </row>
-    <row r="33" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="35"/>
       <c r="C33" s="70">
@@ -8667,7 +8660,7 @@
       <c r="AA33" s="1"/>
       <c r="AB33" s="1"/>
     </row>
-    <row r="34" spans="1:28" ht="5.15" customHeight="1" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:28" ht="5.0999999999999996" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="19"/>
       <c r="C34" s="71">
@@ -8700,7 +8693,7 @@
       <c r="AA34" s="1"/>
       <c r="AB34" s="1"/>
     </row>
-    <row r="35" spans="1:28" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:28" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="67">
@@ -8733,7 +8726,7 @@
       <c r="AA35" s="1"/>
       <c r="AB35" s="1"/>
     </row>
-    <row r="36" spans="1:28" s="131" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:28" s="131" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="73">
@@ -8766,7 +8759,7 @@
       <c r="AA36" s="1"/>
       <c r="AB36" s="1"/>
     </row>
-    <row r="37" spans="1:28" s="131" customFormat="1" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:28" s="131" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="20"/>
       <c r="C37" s="74">
@@ -8799,7 +8792,7 @@
       <c r="AA37" s="1"/>
       <c r="AB37" s="1"/>
     </row>
-    <row r="38" spans="1:28" s="131" customFormat="1" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:28" s="131" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="34" t="s">
         <v>21</v>
@@ -8834,7 +8827,7 @@
       <c r="AA38" s="1"/>
       <c r="AB38" s="1"/>
     </row>
-    <row r="39" spans="1:28" s="131" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:28" s="131" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="33"/>
       <c r="C39" s="73">
@@ -8867,7 +8860,7 @@
       <c r="AA39" s="1"/>
       <c r="AB39" s="1"/>
     </row>
-    <row r="40" spans="1:28" s="131" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:28" s="131" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="33"/>
       <c r="C40" s="73">
@@ -8904,7 +8897,7 @@
       <c r="AA40" s="1"/>
       <c r="AB40" s="1"/>
     </row>
-    <row r="41" spans="1:28" s="131" customFormat="1" ht="20.149999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:28" s="131" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="33"/>
       <c r="C41" s="73">
@@ -8941,7 +8934,7 @@
       <c r="AA41" s="1"/>
       <c r="AB41" s="1"/>
     </row>
-    <row r="42" spans="1:28" s="131" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:28" s="131" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="33"/>
       <c r="C42" s="73">
@@ -8974,7 +8967,7 @@
       <c r="AA42" s="1"/>
       <c r="AB42" s="1"/>
     </row>
-    <row r="43" spans="1:28" s="131" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:28" s="131" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="33"/>
       <c r="C43" s="73">
@@ -9007,7 +9000,7 @@
       <c r="AA43" s="1"/>
       <c r="AB43" s="1"/>
     </row>
-    <row r="44" spans="1:28" s="131" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:28" s="131" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="33"/>
       <c r="C44" s="73">
@@ -9040,7 +9033,7 @@
       <c r="AA44" s="1"/>
       <c r="AB44" s="1"/>
     </row>
-    <row r="45" spans="1:28" s="131" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:28" s="131" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="33"/>
       <c r="C45" s="73">
@@ -9073,7 +9066,7 @@
       <c r="AA45" s="1"/>
       <c r="AB45" s="1"/>
     </row>
-    <row r="46" spans="1:28" s="131" customFormat="1" ht="28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:28" s="131" customFormat="1" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="33"/>
       <c r="C46" s="73">
@@ -9116,7 +9109,7 @@
       <c r="AA46" s="1"/>
       <c r="AB46" s="1"/>
     </row>
-    <row r="47" spans="1:28" s="131" customFormat="1" ht="11.5" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:28" s="131" customFormat="1" ht="11.45" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="33" t="s">
         <v>20</v>
@@ -9151,7 +9144,7 @@
       <c r="AA47" s="1"/>
       <c r="AB47" s="1"/>
     </row>
-    <row r="48" spans="1:28" s="131" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:28" s="131" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="33"/>
       <c r="C48" s="73">
@@ -9184,7 +9177,7 @@
       <c r="AA48" s="1"/>
       <c r="AB48" s="1"/>
     </row>
-    <row r="49" spans="1:28" s="131" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:28" s="131" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="33" t="s">
         <v>19</v>
@@ -9221,7 +9214,7 @@
       <c r="AA49" s="1"/>
       <c r="AB49" s="1"/>
     </row>
-    <row r="50" spans="1:28" s="131" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:28" s="131" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="33"/>
       <c r="C50" s="73">
@@ -9256,7 +9249,7 @@
       <c r="AA50" s="1"/>
       <c r="AB50" s="1"/>
     </row>
-    <row r="51" spans="1:28" s="131" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:28" s="131" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="33"/>
       <c r="C51" s="73">
@@ -9291,7 +9284,7 @@
       <c r="AA51" s="1"/>
       <c r="AB51" s="1"/>
     </row>
-    <row r="52" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="33"/>
       <c r="C52" s="73"/>
@@ -9325,7 +9318,7 @@
       <c r="AA52" s="1"/>
       <c r="AB52" s="1"/>
     </row>
-    <row r="53" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="33"/>
       <c r="C53" s="73"/>
@@ -9359,7 +9352,7 @@
       <c r="AA53" s="1"/>
       <c r="AB53" s="1"/>
     </row>
-    <row r="54" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="33"/>
       <c r="C54" s="73"/>
@@ -9393,7 +9386,7 @@
       <c r="AA54" s="1"/>
       <c r="AB54" s="1"/>
     </row>
-    <row r="55" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="33"/>
       <c r="C55" s="73"/>
@@ -9427,7 +9420,7 @@
       <c r="AA55" s="1"/>
       <c r="AB55" s="1"/>
     </row>
-    <row r="56" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="33"/>
       <c r="C56" s="73"/>
@@ -9461,7 +9454,7 @@
       <c r="AA56" s="1"/>
       <c r="AB56" s="1"/>
     </row>
-    <row r="57" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="33"/>
       <c r="C57" s="73"/>
@@ -9495,7 +9488,7 @@
       <c r="AA57" s="1"/>
       <c r="AB57" s="1"/>
     </row>
-    <row r="58" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="33"/>
       <c r="C58" s="73"/>
@@ -9529,7 +9522,7 @@
       <c r="AA58" s="1"/>
       <c r="AB58" s="1"/>
     </row>
-    <row r="59" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="33"/>
       <c r="C59" s="73"/>
@@ -9563,7 +9556,7 @@
       <c r="AA59" s="1"/>
       <c r="AB59" s="1"/>
     </row>
-    <row r="60" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="33"/>
       <c r="C60" s="73"/>
@@ -9597,7 +9590,7 @@
       <c r="AA60" s="1"/>
       <c r="AB60" s="1"/>
     </row>
-    <row r="61" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="33"/>
       <c r="C61" s="73"/>
@@ -9631,7 +9624,7 @@
       <c r="AA61" s="1"/>
       <c r="AB61" s="1"/>
     </row>
-    <row r="62" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="33"/>
       <c r="C62" s="73"/>
@@ -9665,7 +9658,7 @@
       <c r="AA62" s="1"/>
       <c r="AB62" s="1"/>
     </row>
-    <row r="63" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="33"/>
       <c r="C63" s="73"/>
@@ -9699,7 +9692,7 @@
       <c r="AA63" s="1"/>
       <c r="AB63" s="1"/>
     </row>
-    <row r="64" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="33"/>
       <c r="C64" s="73"/>
@@ -9733,7 +9726,7 @@
       <c r="AA64" s="1"/>
       <c r="AB64" s="1"/>
     </row>
-    <row r="65" spans="1:28" s="105" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:28" s="105" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="33"/>
       <c r="C65" s="73">
@@ -9772,7 +9765,7 @@
       <c r="AA65" s="1"/>
       <c r="AB65" s="1"/>
     </row>
-    <row r="66" spans="1:28" s="99" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:28" s="99" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="33"/>
       <c r="C66" s="73">
@@ -9809,7 +9802,7 @@
       <c r="AA66" s="1"/>
       <c r="AB66" s="1"/>
     </row>
-    <row r="67" spans="1:28" s="99" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:28" s="99" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="33"/>
       <c r="C67" s="73">
@@ -9846,7 +9839,7 @@
       <c r="AA67" s="1"/>
       <c r="AB67" s="1"/>
     </row>
-    <row r="68" spans="1:28" s="118" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:28" s="118" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="33"/>
       <c r="C68" s="73">
@@ -9883,7 +9876,7 @@
       <c r="AA68" s="1"/>
       <c r="AB68" s="1"/>
     </row>
-    <row r="69" spans="1:28" s="134" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:28" s="134" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="33"/>
       <c r="C69" s="73">
@@ -9916,7 +9909,7 @@
       <c r="AA69" s="1"/>
       <c r="AB69" s="1"/>
     </row>
-    <row r="70" spans="1:28" s="102" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:28" s="102" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="33"/>
       <c r="C70" s="73">
@@ -9953,7 +9946,7 @@
       <c r="AA70" s="1"/>
       <c r="AB70" s="1"/>
     </row>
-    <row r="71" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="33"/>
       <c r="C71" s="73">
@@ -9994,7 +9987,7 @@
       <c r="AA71" s="1"/>
       <c r="AB71" s="1"/>
     </row>
-    <row r="72" spans="1:28" s="141" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:28" s="141" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="33"/>
       <c r="C72" s="73">
@@ -10035,7 +10028,7 @@
       <c r="AA72" s="1"/>
       <c r="AB72" s="1"/>
     </row>
-    <row r="73" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="33"/>
       <c r="C73" s="73"/>
@@ -10065,7 +10058,7 @@
       <c r="AA73" s="1"/>
       <c r="AB73" s="1"/>
     </row>
-    <row r="74" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="33"/>
       <c r="C74" s="73"/>
@@ -10101,7 +10094,7 @@
       <c r="AA74" s="1"/>
       <c r="AB74" s="1"/>
     </row>
-    <row r="75" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="33"/>
       <c r="C75" s="73"/>
@@ -10131,7 +10124,7 @@
       <c r="AA75" s="1"/>
       <c r="AB75" s="1"/>
     </row>
-    <row r="76" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="33"/>
       <c r="C76" s="73">
@@ -10166,7 +10159,7 @@
       <c r="AA76" s="1"/>
       <c r="AB76" s="1"/>
     </row>
-    <row r="77" spans="1:28" s="97" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:28" s="97" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="33"/>
       <c r="C77" s="73">
@@ -10207,7 +10200,7 @@
       <c r="AA77" s="1"/>
       <c r="AB77" s="1"/>
     </row>
-    <row r="78" spans="1:28" s="97" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:28" s="97" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="33"/>
       <c r="C78" s="73">
@@ -10248,7 +10241,7 @@
       <c r="AA78" s="1"/>
       <c r="AB78" s="1"/>
     </row>
-    <row r="79" spans="1:28" s="97" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:28" s="97" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="33"/>
       <c r="C79" s="73">
@@ -10281,7 +10274,7 @@
       <c r="AA79" s="1"/>
       <c r="AB79" s="1"/>
     </row>
-    <row r="80" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="33"/>
       <c r="C80" s="73">
@@ -10318,7 +10311,7 @@
       <c r="AA80" s="1"/>
       <c r="AB80" s="1"/>
     </row>
-    <row r="81" spans="1:28" s="139" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:28" s="139" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="33"/>
       <c r="C81" s="73">
@@ -10351,7 +10344,7 @@
       <c r="AA81" s="1"/>
       <c r="AB81" s="1"/>
     </row>
-    <row r="82" spans="1:28" s="97" customFormat="1" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:28" s="97" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="33"/>
       <c r="C82" s="73">
@@ -10386,7 +10379,7 @@
       <c r="AA82" s="1"/>
       <c r="AB82" s="1"/>
     </row>
-    <row r="83" spans="1:28" s="97" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:28" s="97" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="33"/>
       <c r="C83" s="73">
@@ -10419,7 +10412,7 @@
       <c r="AA83" s="1"/>
       <c r="AB83" s="1"/>
     </row>
-    <row r="84" spans="1:28" s="97" customFormat="1" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:28" s="97" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="35"/>
       <c r="C84" s="76">
@@ -10454,7 +10447,7 @@
       <c r="AA84" s="1"/>
       <c r="AB84" s="1"/>
     </row>
-    <row r="85" spans="1:28" s="97" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:28" s="97" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="19"/>
       <c r="C85" s="77">
@@ -10487,7 +10480,7 @@
       <c r="AA85" s="1"/>
       <c r="AB85" s="1"/>
     </row>
-    <row r="86" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="73">
@@ -10520,7 +10513,7 @@
       <c r="AA86" s="1"/>
       <c r="AB86" s="1"/>
     </row>
-    <row r="87" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="73">
@@ -10553,7 +10546,7 @@
       <c r="AA87" s="1"/>
       <c r="AB87" s="1"/>
     </row>
-    <row r="88" spans="1:28" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:28" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="1"/>
       <c r="B88" s="20"/>
       <c r="C88" s="74">
@@ -10586,7 +10579,7 @@
       <c r="AA88" s="1"/>
       <c r="AB88" s="1"/>
     </row>
-    <row r="89" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="34" t="s">
         <v>21</v>
@@ -10621,7 +10614,7 @@
       <c r="AA89" s="1"/>
       <c r="AB89" s="1"/>
     </row>
-    <row r="90" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="33"/>
       <c r="C90" s="73">
@@ -10654,7 +10647,7 @@
       <c r="AA90" s="1"/>
       <c r="AB90" s="1"/>
     </row>
-    <row r="91" spans="1:28" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="33"/>
       <c r="C91" s="73">
@@ -10691,7 +10684,7 @@
       <c r="AA91" s="1"/>
       <c r="AB91" s="1"/>
     </row>
-    <row r="92" spans="1:28" ht="20.149999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:28" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="33"/>
       <c r="C92" s="73">
@@ -10728,7 +10721,7 @@
       <c r="AA92" s="1"/>
       <c r="AB92" s="1"/>
     </row>
-    <row r="93" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="33"/>
       <c r="C93" s="73">
@@ -10761,7 +10754,7 @@
       <c r="AA93" s="1"/>
       <c r="AB93" s="1"/>
     </row>
-    <row r="94" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="33"/>
       <c r="C94" s="73">
@@ -10794,7 +10787,7 @@
       <c r="AA94" s="1"/>
       <c r="AB94" s="1"/>
     </row>
-    <row r="95" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="33"/>
       <c r="C95" s="73">
@@ -10827,7 +10820,7 @@
       <c r="AA95" s="1"/>
       <c r="AB95" s="1"/>
     </row>
-    <row r="96" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="33"/>
       <c r="C96" s="73">
@@ -10866,7 +10859,7 @@
       <c r="AA96" s="1"/>
       <c r="AB96" s="1"/>
     </row>
-    <row r="97" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="33"/>
       <c r="C97" s="73">
@@ -10915,7 +10908,7 @@
       <c r="AA97" s="1"/>
       <c r="AB97" s="1"/>
     </row>
-    <row r="98" spans="1:28" ht="11.5" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:28" ht="11.45" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="33" t="s">
         <v>20</v>
@@ -10950,7 +10943,7 @@
       <c r="AA98" s="1"/>
       <c r="AB98" s="1"/>
     </row>
-    <row r="99" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="33"/>
       <c r="C99" s="73">
@@ -10983,7 +10976,7 @@
       <c r="AA99" s="1"/>
       <c r="AB99" s="1"/>
     </row>
-    <row r="100" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="33" t="s">
         <v>19</v>
@@ -11020,7 +11013,7 @@
       <c r="AA100" s="1"/>
       <c r="AB100" s="1"/>
     </row>
-    <row r="101" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="33"/>
       <c r="C101" s="73">
@@ -11055,7 +11048,7 @@
       <c r="AA101" s="1"/>
       <c r="AB101" s="1"/>
     </row>
-    <row r="102" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="33"/>
       <c r="C102" s="73">
@@ -11108,7 +11101,7 @@
       <c r="AA102" s="1"/>
       <c r="AB102" s="1"/>
     </row>
-    <row r="103" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="33"/>
       <c r="C103" s="73">
@@ -11159,7 +11152,7 @@
       <c r="AA103" s="1"/>
       <c r="AB103" s="1"/>
     </row>
-    <row r="104" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="33"/>
       <c r="C104" s="73">
@@ -11210,7 +11203,7 @@
       <c r="AA104" s="1"/>
       <c r="AB104" s="1"/>
     </row>
-    <row r="105" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="33"/>
       <c r="C105" s="73">
@@ -11243,7 +11236,7 @@
       <c r="AA105" s="1"/>
       <c r="AB105" s="1"/>
     </row>
-    <row r="106" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="33"/>
       <c r="C106" s="73">
@@ -11294,7 +11287,7 @@
       <c r="AA106" s="1"/>
       <c r="AB106" s="1"/>
     </row>
-    <row r="107" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="33"/>
       <c r="C107" s="73">
@@ -11343,7 +11336,7 @@
       <c r="AA107" s="1"/>
       <c r="AB107" s="1"/>
     </row>
-    <row r="108" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="33"/>
       <c r="C108" s="73">
@@ -11392,7 +11385,7 @@
       <c r="AA108" s="1"/>
       <c r="AB108" s="1"/>
     </row>
-    <row r="109" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="33"/>
       <c r="C109" s="73">
@@ -11441,7 +11434,7 @@
       <c r="AA109" s="1"/>
       <c r="AB109" s="1"/>
     </row>
-    <row r="110" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="33"/>
       <c r="C110" s="73">
@@ -11474,7 +11467,7 @@
       <c r="AA110" s="1"/>
       <c r="AB110" s="1"/>
     </row>
-    <row r="111" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111" s="33"/>
       <c r="C111" s="73">
@@ -11525,7 +11518,7 @@
       <c r="AA111" s="1"/>
       <c r="AB111" s="1"/>
     </row>
-    <row r="112" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="33"/>
       <c r="C112" s="73">
@@ -11574,7 +11567,7 @@
       <c r="AA112" s="1"/>
       <c r="AB112" s="1"/>
     </row>
-    <row r="113" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="33"/>
       <c r="C113" s="73">
@@ -11623,7 +11616,7 @@
       <c r="AA113" s="1"/>
       <c r="AB113" s="1"/>
     </row>
-    <row r="114" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="33"/>
       <c r="C114" s="73">
@@ -11672,7 +11665,7 @@
       <c r="AA114" s="1"/>
       <c r="AB114" s="1"/>
     </row>
-    <row r="115" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="33"/>
       <c r="C115" s="73">
@@ -11705,7 +11698,7 @@
       <c r="AA115" s="1"/>
       <c r="AB115" s="1"/>
     </row>
-    <row r="116" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="33"/>
       <c r="C116" s="73">
@@ -11756,7 +11749,7 @@
       <c r="AA116" s="1"/>
       <c r="AB116" s="1"/>
     </row>
-    <row r="117" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="33"/>
       <c r="C117" s="73">
@@ -11805,7 +11798,7 @@
       <c r="AA117" s="1"/>
       <c r="AB117" s="1"/>
     </row>
-    <row r="118" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="33"/>
       <c r="C118" s="73">
@@ -11854,7 +11847,7 @@
       <c r="AA118" s="1"/>
       <c r="AB118" s="1"/>
     </row>
-    <row r="119" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="33"/>
       <c r="C119" s="73">
@@ -11903,7 +11896,7 @@
       <c r="AA119" s="1"/>
       <c r="AB119" s="1"/>
     </row>
-    <row r="120" spans="1:28" s="138" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:28" s="138" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="33"/>
       <c r="C120" s="73">
@@ -11936,7 +11929,7 @@
       <c r="AA120" s="1"/>
       <c r="AB120" s="1"/>
     </row>
-    <row r="121" spans="1:28" s="138" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:28" s="138" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="33"/>
       <c r="C121" s="73">
@@ -11971,7 +11964,7 @@
       <c r="AA121" s="1"/>
       <c r="AB121" s="1"/>
     </row>
-    <row r="122" spans="1:28" s="138" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:28" s="138" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="33"/>
       <c r="C122" s="73">
@@ -12012,7 +12005,7 @@
       <c r="AA122" s="1"/>
       <c r="AB122" s="1"/>
     </row>
-    <row r="123" spans="1:28" s="138" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:28" s="138" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
       <c r="B123" s="33"/>
       <c r="C123" s="73">
@@ -12060,7 +12053,7 @@
       <c r="AA123" s="1"/>
       <c r="AB123" s="1"/>
     </row>
-    <row r="124" spans="1:28" s="138" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:28" s="138" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
       <c r="B124" s="33"/>
       <c r="C124" s="73">
@@ -12106,7 +12099,7 @@
       <c r="AA124" s="1"/>
       <c r="AB124" s="1"/>
     </row>
-    <row r="125" spans="1:28" s="138" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:28" s="138" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="B125" s="33"/>
       <c r="C125" s="73">
@@ -12149,7 +12142,7 @@
       <c r="AA125" s="1"/>
       <c r="AB125" s="1"/>
     </row>
-    <row r="126" spans="1:28" s="138" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:28" s="138" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
       <c r="B126" s="33"/>
       <c r="C126" s="73">
@@ -12182,7 +12175,7 @@
       <c r="AA126" s="1"/>
       <c r="AB126" s="1"/>
     </row>
-    <row r="127" spans="1:28" s="138" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:28" s="138" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="B127" s="33"/>
       <c r="C127" s="73">
@@ -12229,7 +12222,7 @@
       <c r="AA127" s="1"/>
       <c r="AB127" s="1"/>
     </row>
-    <row r="128" spans="1:28" s="138" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:28" s="138" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
       <c r="B128" s="33"/>
       <c r="C128" s="73">
@@ -12274,7 +12267,7 @@
       <c r="AA128" s="1"/>
       <c r="AB128" s="1"/>
     </row>
-    <row r="129" spans="1:28" s="138" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:28" s="138" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
       <c r="B129" s="33"/>
       <c r="C129" s="73">
@@ -12317,7 +12310,7 @@
       <c r="AA129" s="1"/>
       <c r="AB129" s="1"/>
     </row>
-    <row r="130" spans="1:28" s="138" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:28" s="138" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="B130" s="33"/>
       <c r="C130" s="73">
@@ -12350,7 +12343,7 @@
       <c r="AA130" s="1"/>
       <c r="AB130" s="1"/>
     </row>
-    <row r="131" spans="1:28" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131" s="33"/>
       <c r="C131" s="73">
@@ -12385,7 +12378,7 @@
       <c r="AA131" s="1"/>
       <c r="AB131" s="1"/>
     </row>
-    <row r="132" spans="1:28" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="33"/>
       <c r="C132" s="73">
@@ -12418,7 +12411,7 @@
       <c r="AA132" s="1"/>
       <c r="AB132" s="1"/>
     </row>
-    <row r="133" spans="1:28" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" s="35"/>
       <c r="C133" s="76">
@@ -12453,7 +12446,7 @@
       <c r="AA133" s="1"/>
       <c r="AB133" s="1"/>
     </row>
-    <row r="134" spans="1:28" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:28" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134" s="19"/>
       <c r="C134" s="77">
@@ -12486,7 +12479,7 @@
       <c r="AA134" s="1"/>
       <c r="AB134" s="1"/>
     </row>
-    <row r="135" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="73">
@@ -12519,7 +12512,7 @@
       <c r="AA135" s="1"/>
       <c r="AB135" s="1"/>
     </row>
-    <row r="136" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="73">
@@ -12552,7 +12545,7 @@
       <c r="AA136" s="1"/>
       <c r="AB136" s="1"/>
     </row>
-    <row r="137" spans="1:28" s="95" customFormat="1" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:28" s="95" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="1"/>
       <c r="B137" s="20"/>
       <c r="C137" s="74">
@@ -12585,7 +12578,7 @@
       <c r="AA137" s="1"/>
       <c r="AB137" s="1"/>
     </row>
-    <row r="138" spans="1:28" s="95" customFormat="1" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:28" s="95" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
       <c r="B138" s="34" t="s">
         <v>21</v>
@@ -12620,7 +12613,7 @@
       <c r="AA138" s="1"/>
       <c r="AB138" s="1"/>
     </row>
-    <row r="139" spans="1:28" s="95" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:28" s="95" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
       <c r="B139" s="33"/>
       <c r="C139" s="73">
@@ -12653,7 +12646,7 @@
       <c r="AA139" s="1"/>
       <c r="AB139" s="1"/>
     </row>
-    <row r="140" spans="1:28" s="95" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:28" s="95" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
       <c r="B140" s="33"/>
       <c r="C140" s="73">
@@ -12690,7 +12683,7 @@
       <c r="AA140" s="1"/>
       <c r="AB140" s="1"/>
     </row>
-    <row r="141" spans="1:28" s="95" customFormat="1" ht="20.149999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:28" s="95" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
       <c r="B141" s="33"/>
       <c r="C141" s="73">
@@ -12727,7 +12720,7 @@
       <c r="AA141" s="1"/>
       <c r="AB141" s="1"/>
     </row>
-    <row r="142" spans="1:28" s="95" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:28" s="95" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
       <c r="B142" s="33"/>
       <c r="C142" s="73">
@@ -12760,7 +12753,7 @@
       <c r="AA142" s="1"/>
       <c r="AB142" s="1"/>
     </row>
-    <row r="143" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
       <c r="B143" s="33"/>
       <c r="C143" s="73">
@@ -12793,7 +12786,7 @@
       <c r="AA143" s="1"/>
       <c r="AB143" s="1"/>
     </row>
-    <row r="144" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
       <c r="B144" s="33"/>
       <c r="C144" s="73">
@@ -12828,7 +12821,7 @@
       <c r="AA144" s="1"/>
       <c r="AB144" s="1"/>
     </row>
-    <row r="145" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
       <c r="B145" s="33"/>
       <c r="C145" s="73">
@@ -12863,7 +12856,7 @@
       <c r="AA145" s="1"/>
       <c r="AB145" s="1"/>
     </row>
-    <row r="146" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
       <c r="B146" s="33"/>
       <c r="C146" s="73">
@@ -12918,7 +12911,7 @@
       <c r="AA146" s="1"/>
       <c r="AB146" s="1"/>
     </row>
-    <row r="147" spans="1:28" s="95" customFormat="1" ht="11.5" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:28" s="95" customFormat="1" ht="11.45" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
       <c r="B147" s="33" t="s">
         <v>20</v>
@@ -12953,7 +12946,7 @@
       <c r="AA147" s="1"/>
       <c r="AB147" s="1"/>
     </row>
-    <row r="148" spans="1:28" s="95" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:28" s="95" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
       <c r="B148" s="33"/>
       <c r="C148" s="73">
@@ -13008,7 +13001,7 @@
       <c r="AA148" s="1"/>
       <c r="AB148" s="1"/>
     </row>
-    <row r="149" spans="1:28" s="95" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:28" s="95" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
       <c r="B149" s="33" t="s">
         <v>19</v>
@@ -13045,7 +13038,7 @@
       <c r="AA149" s="1"/>
       <c r="AB149" s="1"/>
     </row>
-    <row r="150" spans="1:28" s="95" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:28" s="95" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
       <c r="B150" s="33"/>
       <c r="C150" s="73">
@@ -13080,7 +13073,7 @@
       <c r="AA150" s="1"/>
       <c r="AB150" s="1"/>
     </row>
-    <row r="151" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
       <c r="B151" s="33"/>
       <c r="C151" s="73">
@@ -13115,7 +13108,7 @@
       <c r="AA151" s="1"/>
       <c r="AB151" s="1"/>
     </row>
-    <row r="152" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
       <c r="B152" s="33"/>
       <c r="C152" s="73">
@@ -13154,7 +13147,7 @@
       <c r="AA152" s="1"/>
       <c r="AB152" s="1"/>
     </row>
-    <row r="153" spans="1:28" s="95" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:28" s="95" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A153" s="1"/>
       <c r="B153" s="33"/>
       <c r="C153" s="73">
@@ -13213,7 +13206,7 @@
       <c r="AA153" s="1"/>
       <c r="AB153" s="1"/>
     </row>
-    <row r="154" spans="1:28" s="95" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:28" s="95" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A154" s="1"/>
       <c r="B154" s="33"/>
       <c r="C154" s="73">
@@ -13270,7 +13263,7 @@
       <c r="AA154" s="1"/>
       <c r="AB154" s="1"/>
     </row>
-    <row r="155" spans="1:28" s="95" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:28" s="95" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
       <c r="B155" s="33"/>
       <c r="C155" s="73">
@@ -13307,7 +13300,7 @@
       <c r="AA155" s="1"/>
       <c r="AB155" s="1"/>
     </row>
-    <row r="156" spans="1:28" s="95" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:28" s="95" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A156" s="1"/>
       <c r="B156" s="33"/>
       <c r="C156" s="73">
@@ -13364,7 +13357,7 @@
       <c r="AA156" s="1"/>
       <c r="AB156" s="1"/>
     </row>
-    <row r="157" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
       <c r="B157" s="33"/>
       <c r="C157" s="73">
@@ -13421,7 +13414,7 @@
       <c r="AA157" s="1"/>
       <c r="AB157" s="1"/>
     </row>
-    <row r="158" spans="1:28" s="137" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:28" s="137" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
       <c r="B158" s="33"/>
       <c r="C158" s="73">
@@ -13478,7 +13471,7 @@
       <c r="AA158" s="1"/>
       <c r="AB158" s="1"/>
     </row>
-    <row r="159" spans="1:28" s="114" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:28" s="114" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A159" s="1"/>
       <c r="B159" s="33"/>
       <c r="C159" s="73">
@@ -13535,7 +13528,7 @@
       <c r="AA159" s="1"/>
       <c r="AB159" s="1"/>
     </row>
-    <row r="160" spans="1:28" s="114" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:28" s="114" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
       <c r="B160" s="33"/>
       <c r="C160" s="73">
@@ -13592,7 +13585,7 @@
       <c r="AA160" s="1"/>
       <c r="AB160" s="1"/>
     </row>
-    <row r="161" spans="1:31" s="95" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:31" s="95" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A161" s="1"/>
       <c r="B161" s="33"/>
       <c r="C161" s="73">
@@ -13649,7 +13642,7 @@
       <c r="AA161" s="1"/>
       <c r="AB161" s="1"/>
     </row>
-    <row r="162" spans="1:31" s="95" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:31" s="95" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A162" s="1"/>
       <c r="B162" s="33"/>
       <c r="C162" s="73">
@@ -13706,7 +13699,7 @@
       <c r="AA162" s="1"/>
       <c r="AB162" s="1"/>
     </row>
-    <row r="163" spans="1:31" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:31" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A163" s="1"/>
       <c r="B163" s="33"/>
       <c r="C163" s="73">
@@ -13766,7 +13759,7 @@
       <c r="AD163" s="119"/>
       <c r="AE163" s="119"/>
     </row>
-    <row r="164" spans="1:31" s="135" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:31" s="135" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A164" s="1"/>
       <c r="B164" s="33"/>
       <c r="C164" s="73">
@@ -13823,7 +13816,7 @@
       <c r="AA164" s="1"/>
       <c r="AB164" s="1"/>
     </row>
-    <row r="165" spans="1:31" s="105" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:31" s="105" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A165" s="1"/>
       <c r="B165" s="33"/>
       <c r="C165" s="73">
@@ -13859,7 +13852,7 @@
       <c r="AD165" s="119"/>
       <c r="AE165" s="119"/>
     </row>
-    <row r="166" spans="1:31" s="105" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:31" s="105" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1"/>
       <c r="B166" s="33"/>
       <c r="C166" s="73">
@@ -13922,7 +13915,7 @@
       <c r="AD166" s="119"/>
       <c r="AE166" s="119"/>
     </row>
-    <row r="167" spans="1:31" s="105" customFormat="1" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:31" s="105" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A167" s="1"/>
       <c r="B167" s="33"/>
       <c r="C167" s="73">
@@ -13960,7 +13953,7 @@
       <c r="AD167" s="119"/>
       <c r="AE167" s="119"/>
     </row>
-    <row r="168" spans="1:31" s="104" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:31" s="104" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A168" s="1"/>
       <c r="B168" s="33"/>
       <c r="C168" s="73">
@@ -14014,7 +14007,7 @@
       <c r="AD168" s="119"/>
       <c r="AE168" s="119"/>
     </row>
-    <row r="169" spans="1:31" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:31" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A169" s="1"/>
       <c r="B169" s="33"/>
       <c r="C169" s="73">
@@ -14077,7 +14070,7 @@
       <c r="AA169" s="1"/>
       <c r="AB169" s="1"/>
     </row>
-    <row r="170" spans="1:31" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:31" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A170" s="1"/>
       <c r="B170" s="33"/>
       <c r="C170" s="73">
@@ -14138,7 +14131,7 @@
       <c r="AA170" s="1"/>
       <c r="AB170" s="1"/>
     </row>
-    <row r="171" spans="1:31" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:31" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A171" s="1"/>
       <c r="B171" s="33"/>
       <c r="C171" s="73">
@@ -14197,7 +14190,7 @@
       <c r="AA171" s="1"/>
       <c r="AB171" s="1"/>
     </row>
-    <row r="172" spans="1:31" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:31" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A172" s="1"/>
       <c r="B172" s="33"/>
       <c r="C172" s="73">
@@ -14256,7 +14249,7 @@
       <c r="AA172" s="1"/>
       <c r="AB172" s="1"/>
     </row>
-    <row r="173" spans="1:31" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:31" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A173" s="1"/>
       <c r="B173" s="33"/>
       <c r="C173" s="73">
@@ -14315,7 +14308,7 @@
       <c r="AA173" s="1"/>
       <c r="AB173" s="1"/>
     </row>
-    <row r="174" spans="1:31" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:31" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A174" s="1"/>
       <c r="B174" s="33"/>
       <c r="C174" s="73">
@@ -14376,7 +14369,7 @@
       <c r="AA174" s="1"/>
       <c r="AB174" s="1"/>
     </row>
-    <row r="175" spans="1:31" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:31" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A175" s="1"/>
       <c r="B175" s="33"/>
       <c r="C175" s="73">
@@ -14437,7 +14430,7 @@
       <c r="AA175" s="1"/>
       <c r="AB175" s="1"/>
     </row>
-    <row r="176" spans="1:31" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:31" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A176" s="1"/>
       <c r="B176" s="33"/>
       <c r="C176" s="73">
@@ -14496,7 +14489,7 @@
       <c r="AA176" s="1"/>
       <c r="AB176" s="1"/>
     </row>
-    <row r="177" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A177" s="1"/>
       <c r="B177" s="33"/>
       <c r="C177" s="73">
@@ -14555,7 +14548,7 @@
       <c r="AA177" s="1"/>
       <c r="AB177" s="1"/>
     </row>
-    <row r="178" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A178" s="1"/>
       <c r="B178" s="33"/>
       <c r="C178" s="73">
@@ -14614,7 +14607,7 @@
       <c r="AA178" s="1"/>
       <c r="AB178" s="1"/>
     </row>
-    <row r="179" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A179" s="1"/>
       <c r="B179" s="33"/>
       <c r="C179" s="73">
@@ -14675,7 +14668,7 @@
       <c r="AA179" s="1"/>
       <c r="AB179" s="1"/>
     </row>
-    <row r="180" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A180" s="1"/>
       <c r="B180" s="33"/>
       <c r="C180" s="73">
@@ -14736,7 +14729,7 @@
       <c r="AA180" s="1"/>
       <c r="AB180" s="1"/>
     </row>
-    <row r="181" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A181" s="1"/>
       <c r="B181" s="33"/>
       <c r="C181" s="73">
@@ -14795,7 +14788,7 @@
       <c r="AA181" s="1"/>
       <c r="AB181" s="1"/>
     </row>
-    <row r="182" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A182" s="1"/>
       <c r="B182" s="33"/>
       <c r="C182" s="73">
@@ -14852,7 +14845,7 @@
       <c r="AA182" s="1"/>
       <c r="AB182" s="1"/>
     </row>
-    <row r="183" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A183" s="1"/>
       <c r="B183" s="33"/>
       <c r="C183" s="73">
@@ -14911,7 +14904,7 @@
       <c r="AA183" s="1"/>
       <c r="AB183" s="1"/>
     </row>
-    <row r="184" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A184" s="1"/>
       <c r="B184" s="33"/>
       <c r="C184" s="73">
@@ -14972,7 +14965,7 @@
       <c r="AA184" s="1"/>
       <c r="AB184" s="1"/>
     </row>
-    <row r="185" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A185" s="1"/>
       <c r="B185" s="33"/>
       <c r="C185" s="73">
@@ -15033,7 +15026,7 @@
       <c r="AA185" s="1"/>
       <c r="AB185" s="1"/>
     </row>
-    <row r="186" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A186" s="1"/>
       <c r="B186" s="33"/>
       <c r="C186" s="73">
@@ -15092,7 +15085,7 @@
       <c r="AA186" s="1"/>
       <c r="AB186" s="1"/>
     </row>
-    <row r="187" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A187" s="1"/>
       <c r="B187" s="33"/>
       <c r="C187" s="73">
@@ -15151,7 +15144,7 @@
       <c r="AA187" s="1"/>
       <c r="AB187" s="1"/>
     </row>
-    <row r="188" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A188" s="1"/>
       <c r="B188" s="33"/>
       <c r="C188" s="73">
@@ -15210,7 +15203,7 @@
       <c r="AA188" s="1"/>
       <c r="AB188" s="1"/>
     </row>
-    <row r="189" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A189" s="1"/>
       <c r="B189" s="33"/>
       <c r="C189" s="73">
@@ -15273,7 +15266,7 @@
       <c r="AA189" s="1"/>
       <c r="AB189" s="1"/>
     </row>
-    <row r="190" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A190" s="1"/>
       <c r="B190" s="33"/>
       <c r="C190" s="73">
@@ -15332,7 +15325,7 @@
       <c r="AA190" s="1"/>
       <c r="AB190" s="1"/>
     </row>
-    <row r="191" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A191" s="1"/>
       <c r="B191" s="33"/>
       <c r="C191" s="73">
@@ -15389,7 +15382,7 @@
       <c r="AA191" s="1"/>
       <c r="AB191" s="1"/>
     </row>
-    <row r="192" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A192" s="1"/>
       <c r="B192" s="33"/>
       <c r="C192" s="73">
@@ -15446,7 +15439,7 @@
       <c r="AA192" s="1"/>
       <c r="AB192" s="1"/>
     </row>
-    <row r="193" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A193" s="1"/>
       <c r="B193" s="33"/>
       <c r="C193" s="73">
@@ -15503,7 +15496,7 @@
       <c r="AA193" s="1"/>
       <c r="AB193" s="1"/>
     </row>
-    <row r="194" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A194" s="1"/>
       <c r="B194" s="33"/>
       <c r="C194" s="73">
@@ -15562,7 +15555,7 @@
       <c r="AA194" s="1"/>
       <c r="AB194" s="1"/>
     </row>
-    <row r="195" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A195" s="1"/>
       <c r="B195" s="33"/>
       <c r="C195" s="73">
@@ -15619,7 +15612,7 @@
       <c r="AA195" s="1"/>
       <c r="AB195" s="1"/>
     </row>
-    <row r="196" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A196" s="1"/>
       <c r="B196" s="33"/>
       <c r="C196" s="73">
@@ -15676,7 +15669,7 @@
       <c r="AA196" s="1"/>
       <c r="AB196" s="1"/>
     </row>
-    <row r="197" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A197" s="1"/>
       <c r="B197" s="33"/>
       <c r="C197" s="73">
@@ -15733,7 +15726,7 @@
       <c r="AA197" s="1"/>
       <c r="AB197" s="1"/>
     </row>
-    <row r="198" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A198" s="1"/>
       <c r="B198" s="33"/>
       <c r="C198" s="73">
@@ -15790,7 +15783,7 @@
       <c r="AA198" s="1"/>
       <c r="AB198" s="1"/>
     </row>
-    <row r="199" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A199" s="1"/>
       <c r="B199" s="33"/>
       <c r="C199" s="73">
@@ -15849,7 +15842,7 @@
       <c r="AA199" s="1"/>
       <c r="AB199" s="1"/>
     </row>
-    <row r="200" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A200" s="1"/>
       <c r="B200" s="33"/>
       <c r="C200" s="73">
@@ -15906,7 +15899,7 @@
       <c r="AA200" s="1"/>
       <c r="AB200" s="1"/>
     </row>
-    <row r="201" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A201" s="1"/>
       <c r="B201" s="33"/>
       <c r="C201" s="73">
@@ -15963,7 +15956,7 @@
       <c r="AA201" s="1"/>
       <c r="AB201" s="1"/>
     </row>
-    <row r="202" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A202" s="1"/>
       <c r="B202" s="33"/>
       <c r="C202" s="73">
@@ -16020,7 +16013,7 @@
       <c r="AA202" s="1"/>
       <c r="AB202" s="1"/>
     </row>
-    <row r="203" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A203" s="1"/>
       <c r="B203" s="33"/>
       <c r="C203" s="73">
@@ -16077,7 +16070,7 @@
       <c r="AA203" s="1"/>
       <c r="AB203" s="1"/>
     </row>
-    <row r="204" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A204" s="1"/>
       <c r="B204" s="33"/>
       <c r="C204" s="73">
@@ -16136,7 +16129,7 @@
       <c r="AA204" s="1"/>
       <c r="AB204" s="1"/>
     </row>
-    <row r="205" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A205" s="1"/>
       <c r="B205" s="33"/>
       <c r="C205" s="73">
@@ -16193,7 +16186,7 @@
       <c r="AA205" s="1"/>
       <c r="AB205" s="1"/>
     </row>
-    <row r="206" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A206" s="1"/>
       <c r="B206" s="33"/>
       <c r="C206" s="73">
@@ -16250,7 +16243,7 @@
       <c r="AA206" s="1"/>
       <c r="AB206" s="1"/>
     </row>
-    <row r="207" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A207" s="1"/>
       <c r="B207" s="33"/>
       <c r="C207" s="73">
@@ -16307,7 +16300,7 @@
       <c r="AA207" s="1"/>
       <c r="AB207" s="1"/>
     </row>
-    <row r="208" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:28" s="104" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A208" s="1"/>
       <c r="B208" s="33"/>
       <c r="C208" s="73">
@@ -16364,7 +16357,7 @@
       <c r="AA208" s="1"/>
       <c r="AB208" s="1"/>
     </row>
-    <row r="209" spans="1:30" s="105" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:30" s="105" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A209" s="1"/>
       <c r="B209" s="33"/>
       <c r="C209" s="73">
@@ -16399,7 +16392,7 @@
       <c r="AC209" s="119"/>
       <c r="AD209" s="119"/>
     </row>
-    <row r="210" spans="1:30" s="122" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:30" s="122" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A210" s="1"/>
       <c r="B210" s="33"/>
       <c r="C210" s="73">
@@ -16459,7 +16452,7 @@
       <c r="AA210" s="1"/>
       <c r="AB210" s="1"/>
     </row>
-    <row r="211" spans="1:30" s="131" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:30" s="131" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A211" s="1"/>
       <c r="B211" s="33"/>
       <c r="C211" s="73">
@@ -16527,7 +16520,7 @@
       <c r="AA211" s="1"/>
       <c r="AB211" s="1"/>
     </row>
-    <row r="212" spans="1:30" s="131" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:30" s="131" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A212" s="1"/>
       <c r="B212" s="33"/>
       <c r="C212" s="73">
@@ -16595,7 +16588,7 @@
       <c r="AA212" s="1"/>
       <c r="AB212" s="1"/>
     </row>
-    <row r="213" spans="1:30" s="122" customFormat="1" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:30" s="122" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A213" s="1"/>
       <c r="B213" s="33"/>
       <c r="C213" s="73">
@@ -16630,7 +16623,7 @@
       <c r="AA213" s="1"/>
       <c r="AB213" s="1"/>
     </row>
-    <row r="214" spans="1:30" s="122" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:30" s="122" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A214" s="1"/>
       <c r="B214" s="33"/>
       <c r="C214" s="73">
@@ -16681,7 +16674,7 @@
       <c r="AA214" s="1"/>
       <c r="AB214" s="1"/>
     </row>
-    <row r="215" spans="1:30" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:30" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A215" s="1"/>
       <c r="B215" s="33"/>
       <c r="C215" s="73">
@@ -16753,7 +16746,7 @@
       <c r="AA215" s="1"/>
       <c r="AB215" s="1"/>
     </row>
-    <row r="216" spans="1:30" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:30" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A216" s="1"/>
       <c r="B216" s="33"/>
       <c r="C216" s="73">
@@ -16826,7 +16819,7 @@
       <c r="AA216" s="1"/>
       <c r="AB216" s="1"/>
     </row>
-    <row r="217" spans="1:30" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:30" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A217" s="1"/>
       <c r="B217" s="33"/>
       <c r="C217" s="73">
@@ -16893,7 +16886,7 @@
       <c r="AA217" s="1"/>
       <c r="AB217" s="1"/>
     </row>
-    <row r="218" spans="1:30" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:30" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A218" s="1"/>
       <c r="B218" s="33"/>
       <c r="C218" s="73">
@@ -16962,7 +16955,7 @@
       <c r="AA218" s="1"/>
       <c r="AB218" s="1"/>
     </row>
-    <row r="219" spans="1:30" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:30" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A219" s="1"/>
       <c r="B219" s="33"/>
       <c r="C219" s="73">
@@ -17031,7 +17024,7 @@
       <c r="AA219" s="1"/>
       <c r="AB219" s="1"/>
     </row>
-    <row r="220" spans="1:30" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:30" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A220" s="1"/>
       <c r="B220" s="33"/>
       <c r="C220" s="73">
@@ -17102,7 +17095,7 @@
       <c r="AA220" s="1"/>
       <c r="AB220" s="1"/>
     </row>
-    <row r="221" spans="1:30" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:30" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A221" s="1"/>
       <c r="B221" s="33"/>
       <c r="C221" s="73">
@@ -17173,7 +17166,7 @@
       <c r="AA221" s="1"/>
       <c r="AB221" s="1"/>
     </row>
-    <row r="222" spans="1:30" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:30" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A222" s="1"/>
       <c r="B222" s="33"/>
       <c r="C222" s="73">
@@ -17240,7 +17233,7 @@
       <c r="AA222" s="1"/>
       <c r="AB222" s="1"/>
     </row>
-    <row r="223" spans="1:30" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:30" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A223" s="1"/>
       <c r="B223" s="33"/>
       <c r="C223" s="73">
@@ -17307,7 +17300,7 @@
       <c r="AA223" s="1"/>
       <c r="AB223" s="1"/>
     </row>
-    <row r="224" spans="1:30" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:30" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A224" s="1"/>
       <c r="B224" s="33"/>
       <c r="C224" s="73">
@@ -17374,7 +17367,7 @@
       <c r="AA224" s="1"/>
       <c r="AB224" s="1"/>
     </row>
-    <row r="225" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A225" s="1"/>
       <c r="B225" s="33"/>
       <c r="C225" s="73">
@@ -17443,7 +17436,7 @@
       <c r="AA225" s="1"/>
       <c r="AB225" s="1"/>
     </row>
-    <row r="226" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A226" s="1"/>
       <c r="B226" s="33"/>
       <c r="C226" s="73">
@@ -17512,7 +17505,7 @@
       <c r="AA226" s="1"/>
       <c r="AB226" s="1"/>
     </row>
-    <row r="227" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A227" s="1"/>
       <c r="B227" s="33"/>
       <c r="C227" s="73">
@@ -17579,7 +17572,7 @@
       <c r="AA227" s="1"/>
       <c r="AB227" s="1"/>
     </row>
-    <row r="228" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A228" s="1"/>
       <c r="B228" s="33"/>
       <c r="C228" s="73">
@@ -17646,7 +17639,7 @@
       <c r="AA228" s="1"/>
       <c r="AB228" s="1"/>
     </row>
-    <row r="229" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A229" s="1"/>
       <c r="B229" s="33"/>
       <c r="C229" s="73">
@@ -17713,7 +17706,7 @@
       <c r="AA229" s="1"/>
       <c r="AB229" s="1"/>
     </row>
-    <row r="230" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A230" s="1"/>
       <c r="B230" s="33"/>
       <c r="C230" s="73">
@@ -17782,7 +17775,7 @@
       <c r="AA230" s="1"/>
       <c r="AB230" s="1"/>
     </row>
-    <row r="231" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A231" s="1"/>
       <c r="B231" s="33"/>
       <c r="C231" s="73">
@@ -17851,7 +17844,7 @@
       <c r="AA231" s="1"/>
       <c r="AB231" s="1"/>
     </row>
-    <row r="232" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A232" s="1"/>
       <c r="B232" s="33"/>
       <c r="C232" s="73">
@@ -17918,7 +17911,7 @@
       <c r="AA232" s="1"/>
       <c r="AB232" s="1"/>
     </row>
-    <row r="233" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A233" s="1"/>
       <c r="B233" s="33"/>
       <c r="C233" s="73">
@@ -17985,7 +17978,7 @@
       <c r="AA233" s="1"/>
       <c r="AB233" s="1"/>
     </row>
-    <row r="234" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A234" s="1"/>
       <c r="B234" s="33"/>
       <c r="C234" s="73">
@@ -18052,7 +18045,7 @@
       <c r="AA234" s="1"/>
       <c r="AB234" s="1"/>
     </row>
-    <row r="235" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A235" s="1"/>
       <c r="B235" s="33"/>
       <c r="C235" s="73">
@@ -18122,7 +18115,7 @@
       <c r="AA235" s="1"/>
       <c r="AB235" s="1"/>
     </row>
-    <row r="236" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A236" s="1"/>
       <c r="B236" s="33"/>
       <c r="C236" s="73">
@@ -18189,7 +18182,7 @@
       <c r="AA236" s="1"/>
       <c r="AB236" s="1"/>
     </row>
-    <row r="237" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A237" s="1"/>
       <c r="B237" s="33"/>
       <c r="C237" s="73">
@@ -18252,7 +18245,7 @@
       <c r="AA237" s="1"/>
       <c r="AB237" s="1"/>
     </row>
-    <row r="238" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A238" s="1"/>
       <c r="B238" s="33"/>
       <c r="C238" s="73">
@@ -18315,7 +18308,7 @@
       <c r="AA238" s="1"/>
       <c r="AB238" s="1"/>
     </row>
-    <row r="239" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A239" s="1"/>
       <c r="B239" s="33"/>
       <c r="C239" s="73">
@@ -18382,7 +18375,7 @@
       <c r="AA239" s="1"/>
       <c r="AB239" s="1"/>
     </row>
-    <row r="240" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A240" s="1"/>
       <c r="B240" s="33"/>
       <c r="C240" s="73">
@@ -18451,7 +18444,7 @@
       <c r="AA240" s="1"/>
       <c r="AB240" s="1"/>
     </row>
-    <row r="241" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A241" s="1"/>
       <c r="B241" s="33"/>
       <c r="C241" s="73">
@@ -18518,7 +18511,7 @@
       <c r="AA241" s="1"/>
       <c r="AB241" s="1"/>
     </row>
-    <row r="242" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A242" s="1"/>
       <c r="B242" s="33"/>
       <c r="C242" s="73">
@@ -18585,7 +18578,7 @@
       <c r="AA242" s="1"/>
       <c r="AB242" s="1"/>
     </row>
-    <row r="243" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A243" s="1"/>
       <c r="B243" s="33"/>
       <c r="C243" s="73">
@@ -18652,7 +18645,7 @@
       <c r="AA243" s="1"/>
       <c r="AB243" s="1"/>
     </row>
-    <row r="244" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A244" s="1"/>
       <c r="B244" s="33"/>
       <c r="C244" s="73">
@@ -18719,7 +18712,7 @@
       <c r="AA244" s="1"/>
       <c r="AB244" s="1"/>
     </row>
-    <row r="245" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A245" s="1"/>
       <c r="B245" s="33"/>
       <c r="C245" s="73">
@@ -18788,7 +18781,7 @@
       <c r="AA245" s="1"/>
       <c r="AB245" s="1"/>
     </row>
-    <row r="246" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A246" s="1"/>
       <c r="B246" s="33"/>
       <c r="C246" s="73">
@@ -18855,7 +18848,7 @@
       <c r="AA246" s="1"/>
       <c r="AB246" s="1"/>
     </row>
-    <row r="247" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A247" s="1"/>
       <c r="B247" s="33"/>
       <c r="C247" s="73">
@@ -18922,7 +18915,7 @@
       <c r="AA247" s="1"/>
       <c r="AB247" s="1"/>
     </row>
-    <row r="248" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A248" s="1"/>
       <c r="B248" s="33"/>
       <c r="C248" s="73">
@@ -18989,7 +18982,7 @@
       <c r="AA248" s="1"/>
       <c r="AB248" s="1"/>
     </row>
-    <row r="249" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A249" s="1"/>
       <c r="B249" s="33"/>
       <c r="C249" s="73">
@@ -19056,7 +19049,7 @@
       <c r="AA249" s="1"/>
       <c r="AB249" s="1"/>
     </row>
-    <row r="250" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A250" s="1"/>
       <c r="B250" s="33"/>
       <c r="C250" s="73">
@@ -19125,7 +19118,7 @@
       <c r="AA250" s="1"/>
       <c r="AB250" s="1"/>
     </row>
-    <row r="251" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A251" s="1"/>
       <c r="B251" s="33"/>
       <c r="C251" s="73">
@@ -19192,7 +19185,7 @@
       <c r="AA251" s="1"/>
       <c r="AB251" s="1"/>
     </row>
-    <row r="252" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A252" s="1"/>
       <c r="B252" s="33"/>
       <c r="C252" s="73">
@@ -19259,7 +19252,7 @@
       <c r="AA252" s="1"/>
       <c r="AB252" s="1"/>
     </row>
-    <row r="253" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A253" s="1"/>
       <c r="B253" s="33"/>
       <c r="C253" s="73">
@@ -19326,7 +19319,7 @@
       <c r="AA253" s="1"/>
       <c r="AB253" s="1"/>
     </row>
-    <row r="254" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A254" s="1"/>
       <c r="B254" s="33"/>
       <c r="C254" s="73">
@@ -19393,7 +19386,7 @@
       <c r="AA254" s="1"/>
       <c r="AB254" s="1"/>
     </row>
-    <row r="255" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A255" s="1"/>
       <c r="B255" s="33"/>
       <c r="C255" s="73">
@@ -19464,7 +19457,7 @@
       <c r="AA255" s="1"/>
       <c r="AB255" s="1"/>
     </row>
-    <row r="256" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A256" s="1"/>
       <c r="B256" s="33"/>
       <c r="C256" s="73">
@@ -19533,7 +19526,7 @@
       <c r="AA256" s="1"/>
       <c r="AB256" s="1"/>
     </row>
-    <row r="257" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A257" s="1"/>
       <c r="B257" s="33"/>
       <c r="C257" s="73">
@@ -19600,7 +19593,7 @@
       <c r="AA257" s="1"/>
       <c r="AB257" s="1"/>
     </row>
-    <row r="258" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A258" s="1"/>
       <c r="B258" s="33"/>
       <c r="C258" s="73">
@@ -19667,7 +19660,7 @@
       <c r="AA258" s="1"/>
       <c r="AB258" s="1"/>
     </row>
-    <row r="259" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A259" s="1"/>
       <c r="B259" s="33"/>
       <c r="C259" s="73">
@@ -19734,7 +19727,7 @@
       <c r="AA259" s="1"/>
       <c r="AB259" s="1"/>
     </row>
-    <row r="260" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A260" s="1"/>
       <c r="B260" s="33"/>
       <c r="C260" s="73">
@@ -19803,7 +19796,7 @@
       <c r="AA260" s="1"/>
       <c r="AB260" s="1"/>
     </row>
-    <row r="261" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A261" s="1"/>
       <c r="B261" s="33"/>
       <c r="C261" s="73">
@@ -19870,7 +19863,7 @@
       <c r="AA261" s="1"/>
       <c r="AB261" s="1"/>
     </row>
-    <row r="262" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A262" s="1"/>
       <c r="B262" s="33"/>
       <c r="C262" s="73">
@@ -19937,7 +19930,7 @@
       <c r="AA262" s="1"/>
       <c r="AB262" s="1"/>
     </row>
-    <row r="263" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A263" s="1"/>
       <c r="B263" s="33"/>
       <c r="C263" s="73">
@@ -20004,7 +19997,7 @@
       <c r="AA263" s="1"/>
       <c r="AB263" s="1"/>
     </row>
-    <row r="264" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A264" s="1"/>
       <c r="B264" s="33"/>
       <c r="C264" s="73">
@@ -20071,7 +20064,7 @@
       <c r="AA264" s="1"/>
       <c r="AB264" s="1"/>
     </row>
-    <row r="265" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A265" s="1"/>
       <c r="B265" s="33"/>
       <c r="C265" s="73">
@@ -20130,7 +20123,7 @@
       <c r="AA265" s="1"/>
       <c r="AB265" s="1"/>
     </row>
-    <row r="266" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A266" s="1"/>
       <c r="B266" s="33"/>
       <c r="C266" s="73">
@@ -20192,7 +20185,7 @@
       <c r="AA266" s="1"/>
       <c r="AB266" s="1"/>
     </row>
-    <row r="267" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A267" s="1"/>
       <c r="B267" s="33"/>
       <c r="C267" s="73">
@@ -20253,7 +20246,7 @@
       <c r="AA267" s="1"/>
       <c r="AB267" s="1"/>
     </row>
-    <row r="268" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A268" s="1"/>
       <c r="B268" s="33"/>
       <c r="C268" s="73">
@@ -20313,7 +20306,7 @@
       <c r="AA268" s="1"/>
       <c r="AB268" s="1"/>
     </row>
-    <row r="269" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A269" s="1"/>
       <c r="B269" s="33"/>
       <c r="C269" s="73">
@@ -20380,7 +20373,7 @@
       <c r="AA269" s="1"/>
       <c r="AB269" s="1"/>
     </row>
-    <row r="270" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A270" s="1"/>
       <c r="B270" s="33"/>
       <c r="C270" s="73">
@@ -20445,7 +20438,7 @@
       <c r="AA270" s="1"/>
       <c r="AB270" s="1"/>
     </row>
-    <row r="271" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A271" s="1"/>
       <c r="B271" s="33"/>
       <c r="C271" s="73">
@@ -20507,7 +20500,7 @@
       <c r="AA271" s="1"/>
       <c r="AB271" s="1"/>
     </row>
-    <row r="272" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A272" s="1"/>
       <c r="B272" s="33"/>
       <c r="C272" s="73">
@@ -20567,7 +20560,7 @@
       <c r="AA272" s="1"/>
       <c r="AB272" s="1"/>
     </row>
-    <row r="273" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A273" s="1"/>
       <c r="B273" s="33"/>
       <c r="C273" s="73">
@@ -20624,7 +20617,7 @@
       <c r="AA273" s="1"/>
       <c r="AB273" s="1"/>
     </row>
-    <row r="274" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A274" s="1"/>
       <c r="B274" s="33"/>
       <c r="C274" s="73">
@@ -20691,7 +20684,7 @@
       <c r="AA274" s="1"/>
       <c r="AB274" s="1"/>
     </row>
-    <row r="275" spans="1:28" s="122" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:28" s="122" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A275" s="1"/>
       <c r="B275" s="33"/>
       <c r="C275" s="73">
@@ -20724,7 +20717,7 @@
       <c r="AA275" s="1"/>
       <c r="AB275" s="1"/>
     </row>
-    <row r="276" spans="1:28" s="122" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:28" s="122" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A276" s="1"/>
       <c r="B276" s="33"/>
       <c r="C276" s="73">
@@ -20780,7 +20773,7 @@
       <c r="AA276" s="1"/>
       <c r="AB276" s="1"/>
     </row>
-    <row r="277" spans="1:28" s="131" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:28" s="131" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A277" s="1"/>
       <c r="B277" s="33"/>
       <c r="C277" s="73">
@@ -20833,7 +20826,7 @@
       <c r="AA277" s="1"/>
       <c r="AB277" s="1"/>
     </row>
-    <row r="278" spans="1:28" s="131" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:28" s="131" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A278" s="1"/>
       <c r="B278" s="33"/>
       <c r="C278" s="73">
@@ -20886,7 +20879,7 @@
       <c r="AA278" s="1"/>
       <c r="AB278" s="1"/>
     </row>
-    <row r="279" spans="1:28" s="122" customFormat="1" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:28" s="122" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A279" s="1"/>
       <c r="B279" s="33"/>
       <c r="C279" s="73">
@@ -20921,7 +20914,7 @@
       <c r="AA279" s="1"/>
       <c r="AB279" s="1"/>
     </row>
-    <row r="280" spans="1:28" s="122" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:28" s="122" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A280" s="1"/>
       <c r="B280" s="33"/>
       <c r="C280" s="73">
@@ -20971,7 +20964,7 @@
       <c r="AA280" s="1"/>
       <c r="AB280" s="1"/>
     </row>
-    <row r="281" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A281" s="1"/>
       <c r="B281" s="33"/>
       <c r="C281" s="73">
@@ -21029,7 +21022,7 @@
       <c r="AA281" s="1"/>
       <c r="AB281" s="1"/>
     </row>
-    <row r="282" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A282" s="1"/>
       <c r="B282" s="33"/>
       <c r="C282" s="73">
@@ -21087,7 +21080,7 @@
       <c r="AA282" s="1"/>
       <c r="AB282" s="1"/>
     </row>
-    <row r="283" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A283" s="1"/>
       <c r="B283" s="33"/>
       <c r="C283" s="73">
@@ -21140,7 +21133,7 @@
       <c r="AA283" s="1"/>
       <c r="AB283" s="1"/>
     </row>
-    <row r="284" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A284" s="1"/>
       <c r="B284" s="33"/>
       <c r="C284" s="73">
@@ -21192,7 +21185,7 @@
       <c r="AA284" s="1"/>
       <c r="AB284" s="1"/>
     </row>
-    <row r="285" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A285" s="1"/>
       <c r="B285" s="33"/>
       <c r="C285" s="73">
@@ -21247,7 +21240,7 @@
       <c r="AA285" s="1"/>
       <c r="AB285" s="1"/>
     </row>
-    <row r="286" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A286" s="1"/>
       <c r="B286" s="33"/>
       <c r="C286" s="73">
@@ -21301,7 +21294,7 @@
       <c r="AA286" s="1"/>
       <c r="AB286" s="1"/>
     </row>
-    <row r="287" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A287" s="1"/>
       <c r="B287" s="33"/>
       <c r="C287" s="73">
@@ -21355,7 +21348,7 @@
       <c r="AA287" s="1"/>
       <c r="AB287" s="1"/>
     </row>
-    <row r="288" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A288" s="1"/>
       <c r="B288" s="33"/>
       <c r="C288" s="73">
@@ -21405,7 +21398,7 @@
       <c r="AA288" s="1"/>
       <c r="AB288" s="1"/>
     </row>
-    <row r="289" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A289" s="1"/>
       <c r="B289" s="33"/>
       <c r="C289" s="73">
@@ -21455,7 +21448,7 @@
       <c r="AA289" s="1"/>
       <c r="AB289" s="1"/>
     </row>
-    <row r="290" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A290" s="1"/>
       <c r="B290" s="33"/>
       <c r="C290" s="73">
@@ -21508,7 +21501,7 @@
       <c r="AA290" s="1"/>
       <c r="AB290" s="1"/>
     </row>
-    <row r="291" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A291" s="1"/>
       <c r="B291" s="33"/>
       <c r="C291" s="73">
@@ -21562,7 +21555,7 @@
       <c r="AA291" s="1"/>
       <c r="AB291" s="1"/>
     </row>
-    <row r="292" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A292" s="1"/>
       <c r="B292" s="33"/>
       <c r="C292" s="73">
@@ -21616,7 +21609,7 @@
       <c r="AA292" s="1"/>
       <c r="AB292" s="1"/>
     </row>
-    <row r="293" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A293" s="1"/>
       <c r="B293" s="33"/>
       <c r="C293" s="73">
@@ -21666,7 +21659,7 @@
       <c r="AA293" s="1"/>
       <c r="AB293" s="1"/>
     </row>
-    <row r="294" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A294" s="1"/>
       <c r="B294" s="33"/>
       <c r="C294" s="73">
@@ -21716,7 +21709,7 @@
       <c r="AA294" s="1"/>
       <c r="AB294" s="1"/>
     </row>
-    <row r="295" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A295" s="1"/>
       <c r="B295" s="33"/>
       <c r="C295" s="73">
@@ -21769,7 +21762,7 @@
       <c r="AA295" s="1"/>
       <c r="AB295" s="1"/>
     </row>
-    <row r="296" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A296" s="1"/>
       <c r="B296" s="33"/>
       <c r="C296" s="73">
@@ -21821,7 +21814,7 @@
       <c r="AA296" s="1"/>
       <c r="AB296" s="1"/>
     </row>
-    <row r="297" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A297" s="1"/>
       <c r="B297" s="33"/>
       <c r="C297" s="73">
@@ -21873,7 +21866,7 @@
       <c r="AA297" s="1"/>
       <c r="AB297" s="1"/>
     </row>
-    <row r="298" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A298" s="1"/>
       <c r="B298" s="33"/>
       <c r="C298" s="73">
@@ -21922,7 +21915,7 @@
       <c r="AA298" s="1"/>
       <c r="AB298" s="1"/>
     </row>
-    <row r="299" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A299" s="1"/>
       <c r="B299" s="33"/>
       <c r="C299" s="73">
@@ -21969,7 +21962,7 @@
       <c r="AA299" s="1"/>
       <c r="AB299" s="1"/>
     </row>
-    <row r="300" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:28" s="122" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A300" s="1"/>
       <c r="B300" s="33"/>
       <c r="C300" s="73">
@@ -22022,7 +22015,7 @@
       <c r="AA300" s="1"/>
       <c r="AB300" s="1"/>
     </row>
-    <row r="301" spans="1:28" s="122" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:28" s="122" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A301" s="1"/>
       <c r="B301" s="33"/>
       <c r="C301" s="73">
@@ -22055,7 +22048,7 @@
       <c r="AA301" s="1"/>
       <c r="AB301" s="1"/>
     </row>
-    <row r="302" spans="1:28" s="95" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:28" s="95" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A302" s="1"/>
       <c r="B302" s="33"/>
       <c r="C302" s="73">
@@ -22088,7 +22081,7 @@
       <c r="AA302" s="1"/>
       <c r="AB302" s="1"/>
     </row>
-    <row r="303" spans="1:28" s="95" customFormat="1" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:28" s="95" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A303" s="1"/>
       <c r="B303" s="35"/>
       <c r="C303" s="76">
@@ -22123,7 +22116,7 @@
       <c r="AA303" s="1"/>
       <c r="AB303" s="1"/>
     </row>
-    <row r="304" spans="1:28" s="95" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:28" s="95" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A304" s="1"/>
       <c r="B304" s="19"/>
       <c r="C304" s="77">
@@ -22156,7 +22149,7 @@
       <c r="AA304" s="1"/>
       <c r="AB304" s="1"/>
     </row>
-    <row r="305" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A305" s="1"/>
       <c r="B305" s="1"/>
       <c r="C305" s="73">
@@ -22189,7 +22182,7 @@
       <c r="AA305" s="1"/>
       <c r="AB305" s="1"/>
     </row>
-    <row r="306" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A306" s="1"/>
       <c r="B306" s="1"/>
       <c r="C306" s="73">
@@ -22222,7 +22215,7 @@
       <c r="AA306" s="1"/>
       <c r="AB306" s="1"/>
     </row>
-    <row r="307" spans="1:28" s="97" customFormat="1" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="307" spans="1:28" s="97" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A307" s="1"/>
       <c r="B307" s="20"/>
       <c r="C307" s="74">
@@ -22255,7 +22248,7 @@
       <c r="AA307" s="1"/>
       <c r="AB307" s="1"/>
     </row>
-    <row r="308" spans="1:28" s="97" customFormat="1" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:28" s="97" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A308" s="1"/>
       <c r="B308" s="34" t="s">
         <v>21</v>
@@ -22290,7 +22283,7 @@
       <c r="AA308" s="1"/>
       <c r="AB308" s="1"/>
     </row>
-    <row r="309" spans="1:28" s="97" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:28" s="97" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A309" s="1"/>
       <c r="B309" s="33"/>
       <c r="C309" s="73">
@@ -22323,7 +22316,7 @@
       <c r="AA309" s="1"/>
       <c r="AB309" s="1"/>
     </row>
-    <row r="310" spans="1:28" s="97" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:28" s="97" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A310" s="1"/>
       <c r="B310" s="33"/>
       <c r="C310" s="73">
@@ -22360,7 +22353,7 @@
       <c r="AA310" s="1"/>
       <c r="AB310" s="1"/>
     </row>
-    <row r="311" spans="1:28" s="97" customFormat="1" ht="20.149999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:28" s="97" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A311" s="1"/>
       <c r="B311" s="33"/>
       <c r="C311" s="73">
@@ -22397,7 +22390,7 @@
       <c r="AA311" s="1"/>
       <c r="AB311" s="1"/>
     </row>
-    <row r="312" spans="1:28" s="97" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:28" s="97" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A312" s="1"/>
       <c r="B312" s="33"/>
       <c r="C312" s="73">
@@ -22430,7 +22423,7 @@
       <c r="AA312" s="1"/>
       <c r="AB312" s="1"/>
     </row>
-    <row r="313" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A313" s="1"/>
       <c r="B313" s="33"/>
       <c r="C313" s="73">
@@ -22463,7 +22456,7 @@
       <c r="AA313" s="1"/>
       <c r="AB313" s="1"/>
     </row>
-    <row r="314" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A314" s="1"/>
       <c r="B314" s="33"/>
       <c r="C314" s="73">
@@ -22502,7 +22495,7 @@
       <c r="AA314" s="1"/>
       <c r="AB314" s="1"/>
     </row>
-    <row r="315" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A315" s="1"/>
       <c r="B315" s="33"/>
       <c r="C315" s="73">
@@ -22541,7 +22534,7 @@
       <c r="AA315" s="1"/>
       <c r="AB315" s="1"/>
     </row>
-    <row r="316" spans="1:28" s="97" customFormat="1" ht="28" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:28" s="97" customFormat="1" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A316" s="1"/>
       <c r="B316" s="33"/>
       <c r="C316" s="73">
@@ -22584,7 +22577,7 @@
       <c r="AA316" s="1"/>
       <c r="AB316" s="1"/>
     </row>
-    <row r="317" spans="1:28" s="97" customFormat="1" ht="11.5" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:28" s="97" customFormat="1" ht="11.45" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A317" s="1"/>
       <c r="B317" s="33" t="s">
         <v>20</v>
@@ -22625,7 +22618,7 @@
       <c r="AA317" s="1"/>
       <c r="AB317" s="1"/>
     </row>
-    <row r="318" spans="1:28" s="97" customFormat="1" ht="13" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:28" s="97" customFormat="1" ht="12.95" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A318" s="1"/>
       <c r="B318" s="33"/>
       <c r="C318" s="73">
@@ -22658,7 +22651,7 @@
       <c r="AA318" s="1"/>
       <c r="AB318" s="1"/>
     </row>
-    <row r="319" spans="1:28" s="97" customFormat="1" ht="8.5" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:28" s="97" customFormat="1" ht="8.4499999999999993" customHeight="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A319" s="1"/>
       <c r="B319" s="33" t="s">
         <v>19</v>
@@ -22695,7 +22688,7 @@
       <c r="AA319" s="1"/>
       <c r="AB319" s="1"/>
     </row>
-    <row r="320" spans="1:28" s="97" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:28" s="97" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A320" s="1"/>
       <c r="B320" s="33"/>
       <c r="C320" s="73">
@@ -22730,7 +22723,7 @@
       <c r="AA320" s="1"/>
       <c r="AB320" s="1"/>
     </row>
-    <row r="321" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:28" s="97" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A321" s="1"/>
       <c r="B321" s="33"/>
       <c r="C321" s="73">
@@ -22777,7 +22770,7 @@
       <c r="AA321" s="1"/>
       <c r="AB321" s="1"/>
     </row>
-    <row r="322" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A322" s="1"/>
       <c r="B322" s="33"/>
       <c r="C322" s="73"/>
@@ -22816,7 +22809,7 @@
       <c r="AA322" s="1"/>
       <c r="AB322" s="1"/>
     </row>
-    <row r="323" spans="1:28" s="97" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:28" s="97" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A323" s="1"/>
       <c r="B323" s="33"/>
       <c r="C323" s="73">
@@ -22859,7 +22852,7 @@
       <c r="AA323" s="1"/>
       <c r="AB323" s="1"/>
     </row>
-    <row r="324" spans="1:28" s="142" customFormat="1" ht="14.5" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:28" s="142" customFormat="1" ht="14.45" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A324" s="1"/>
       <c r="B324" s="33"/>
       <c r="C324" s="73"/>
@@ -22899,7 +22892,7 @@
       <c r="AA324" s="1"/>
       <c r="AB324" s="1"/>
     </row>
-    <row r="325" spans="1:28" s="120" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:28" s="120" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A325" s="1"/>
       <c r="B325" s="33"/>
       <c r="C325" s="73">
@@ -22940,7 +22933,7 @@
       <c r="AA325" s="1"/>
       <c r="AB325" s="1"/>
     </row>
-    <row r="326" spans="1:28" s="97" customFormat="1" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:28" s="97" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A326" s="1"/>
       <c r="B326" s="33"/>
       <c r="C326" s="73">
@@ -22975,7 +22968,7 @@
       <c r="AA326" s="1"/>
       <c r="AB326" s="1"/>
     </row>
-    <row r="327" spans="1:28" s="142" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:28" s="142" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A327" s="1"/>
       <c r="B327" s="33"/>
       <c r="C327" s="73">
@@ -23010,7 +23003,7 @@
       <c r="AA327" s="1"/>
       <c r="AB327" s="1"/>
     </row>
-    <row r="328" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A328" s="1"/>
       <c r="B328" s="33"/>
       <c r="C328" s="73">
@@ -23045,7 +23038,7 @@
       <c r="AA328" s="1"/>
       <c r="AB328" s="1"/>
     </row>
-    <row r="329" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A329" s="1"/>
       <c r="B329" s="33"/>
       <c r="C329" s="73">
@@ -23090,7 +23083,7 @@
       <c r="AA329" s="1"/>
       <c r="AB329" s="1"/>
     </row>
-    <row r="330" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A330" s="1"/>
       <c r="B330" s="33"/>
       <c r="C330" s="73">
@@ -23137,7 +23130,7 @@
       <c r="AA330" s="1"/>
       <c r="AB330" s="1"/>
     </row>
-    <row r="331" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A331" s="1"/>
       <c r="B331" s="33"/>
       <c r="C331" s="73">
@@ -23189,7 +23182,7 @@
       <c r="AA331" s="1"/>
       <c r="AB331" s="1"/>
     </row>
-    <row r="332" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A332" s="1"/>
       <c r="B332" s="33"/>
       <c r="C332" s="73"/>
@@ -23239,7 +23232,7 @@
       <c r="AA332" s="1"/>
       <c r="AB332" s="1"/>
     </row>
-    <row r="333" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A333" s="1"/>
       <c r="B333" s="33"/>
       <c r="C333" s="73">
@@ -23288,7 +23281,7 @@
       <c r="AA333" s="1"/>
       <c r="AB333" s="1"/>
     </row>
-    <row r="334" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A334" s="1"/>
       <c r="B334" s="33"/>
       <c r="C334" s="73"/>
@@ -23332,7 +23325,7 @@
       <c r="AA334" s="1"/>
       <c r="AB334" s="1"/>
     </row>
-    <row r="335" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A335" s="1"/>
       <c r="B335" s="33"/>
       <c r="C335" s="73">
@@ -23371,7 +23364,7 @@
       <c r="AA335" s="1"/>
       <c r="AB335" s="1"/>
     </row>
-    <row r="336" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A336" s="1"/>
       <c r="B336" s="33"/>
       <c r="C336" s="73">
@@ -23410,7 +23403,7 @@
       <c r="AA336" s="1"/>
       <c r="AB336" s="1"/>
     </row>
-    <row r="337" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A337" s="1"/>
       <c r="B337" s="33"/>
       <c r="C337" s="73">
@@ -23451,7 +23444,7 @@
       <c r="AA337" s="1"/>
       <c r="AB337" s="1"/>
     </row>
-    <row r="338" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A338" s="1"/>
       <c r="B338" s="33"/>
       <c r="C338" s="73"/>
@@ -23492,7 +23485,7 @@
       <c r="AA338" s="1"/>
       <c r="AB338" s="1"/>
     </row>
-    <row r="339" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A339" s="1"/>
       <c r="B339" s="33"/>
       <c r="C339" s="73"/>
@@ -23522,7 +23515,7 @@
       <c r="AA339" s="1"/>
       <c r="AB339" s="1"/>
     </row>
-    <row r="340" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A340" s="1"/>
       <c r="B340" s="33"/>
       <c r="C340" s="73">
@@ -23557,7 +23550,7 @@
       <c r="AA340" s="1"/>
       <c r="AB340" s="1"/>
     </row>
-    <row r="341" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A341" s="1"/>
       <c r="B341" s="33"/>
       <c r="C341" s="73">
@@ -23598,7 +23591,7 @@
       <c r="AA341" s="1"/>
       <c r="AB341" s="1"/>
     </row>
-    <row r="342" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A342" s="1"/>
       <c r="B342" s="33"/>
       <c r="C342" s="73">
@@ -23641,7 +23634,7 @@
       <c r="AA342" s="1"/>
       <c r="AB342" s="1"/>
     </row>
-    <row r="343" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A343" s="1"/>
       <c r="B343" s="33"/>
       <c r="C343" s="73">
@@ -23689,7 +23682,7 @@
       <c r="AA343" s="1"/>
       <c r="AB343" s="1"/>
     </row>
-    <row r="344" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A344" s="1"/>
       <c r="B344" s="33"/>
       <c r="C344" s="73"/>
@@ -23733,7 +23726,7 @@
       <c r="AA344" s="1"/>
       <c r="AB344" s="1"/>
     </row>
-    <row r="345" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A345" s="1"/>
       <c r="B345" s="33"/>
       <c r="C345" s="73">
@@ -23778,7 +23771,7 @@
       <c r="AA345" s="1"/>
       <c r="AB345" s="1"/>
     </row>
-    <row r="346" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A346" s="1"/>
       <c r="B346" s="33"/>
       <c r="C346" s="73">
@@ -23811,7 +23804,7 @@
       <c r="AA346" s="1"/>
       <c r="AB346" s="1"/>
     </row>
-    <row r="347" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A347" s="1"/>
       <c r="B347" s="33"/>
       <c r="C347" s="73">
@@ -23846,7 +23839,7 @@
       <c r="AA347" s="1"/>
       <c r="AB347" s="1"/>
     </row>
-    <row r="348" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A348" s="1"/>
       <c r="B348" s="33"/>
       <c r="C348" s="73">
@@ -23881,7 +23874,7 @@
       <c r="AA348" s="1"/>
       <c r="AB348" s="1"/>
     </row>
-    <row r="349" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A349" s="1"/>
       <c r="B349" s="33"/>
       <c r="C349" s="73">
@@ -23916,7 +23909,7 @@
       <c r="AA349" s="1"/>
       <c r="AB349" s="1"/>
     </row>
-    <row r="350" spans="1:28" s="142" customFormat="1" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:28" s="142" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A350" s="1"/>
       <c r="B350" s="33"/>
       <c r="C350" s="73">
@@ -23951,7 +23944,7 @@
       <c r="AA350" s="1"/>
       <c r="AB350" s="1"/>
     </row>
-    <row r="351" spans="1:28" s="131" customFormat="1" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:28" s="131" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A351" s="1"/>
       <c r="B351" s="33"/>
       <c r="C351" s="73">
@@ -23984,7 +23977,7 @@
       <c r="AA351" s="1"/>
       <c r="AB351" s="1"/>
     </row>
-    <row r="352" spans="1:28" s="131" customFormat="1" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:28" s="131" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A352" s="1"/>
       <c r="B352" s="35"/>
       <c r="C352" s="76">
@@ -24019,7 +24012,7 @@
       <c r="AA352" s="1"/>
       <c r="AB352" s="1"/>
     </row>
-    <row r="353" spans="1:28" s="131" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:28" s="131" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A353" s="1"/>
       <c r="B353" s="19"/>
       <c r="C353" s="77">
@@ -24052,7 +24045,7 @@
       <c r="AA353" s="1"/>
       <c r="AB353" s="1"/>
     </row>
-    <row r="354" spans="1:28" s="131" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:28" s="131" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A354" s="1"/>
       <c r="B354" s="1"/>
       <c r="C354" s="73">
@@ -24085,7 +24078,7 @@
       <c r="AA354" s="1"/>
       <c r="AB354" s="1"/>
     </row>
-    <row r="355" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A355" s="1"/>
       <c r="B355" s="1"/>
       <c r="C355" s="66"/>
@@ -24115,7 +24108,7 @@
       <c r="AA355" s="1"/>
       <c r="AB355" s="1"/>
     </row>
-    <row r="356" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A356" s="1"/>
       <c r="B356" s="1"/>
       <c r="C356" s="66"/>
@@ -24145,7 +24138,7 @@
       <c r="AA356" s="1"/>
       <c r="AB356" s="1"/>
     </row>
-    <row r="357" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A357" s="1"/>
       <c r="B357" s="1"/>
       <c r="C357" s="66"/>
@@ -24175,7 +24168,7 @@
       <c r="AA357" s="1"/>
       <c r="AB357" s="1"/>
     </row>
-    <row r="358" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A358" s="1"/>
       <c r="B358" s="1"/>
       <c r="C358" s="66"/>
@@ -24205,7 +24198,7 @@
       <c r="AA358" s="1"/>
       <c r="AB358" s="1"/>
     </row>
-    <row r="359" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A359" s="1"/>
       <c r="B359" s="1"/>
       <c r="C359" s="66"/>
@@ -24235,7 +24228,7 @@
       <c r="AA359" s="1"/>
       <c r="AB359" s="1"/>
     </row>
-    <row r="360" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A360" s="1"/>
       <c r="B360" s="1"/>
       <c r="C360" s="66"/>
@@ -24265,7 +24258,7 @@
       <c r="AA360" s="1"/>
       <c r="AB360" s="1"/>
     </row>
-    <row r="361" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C361" s="72" t="s">
         <v>4</v>
       </c>
@@ -24295,22 +24288,22 @@
       <selection activeCell="U37" sqref="U37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" customWidth="1"/>
-    <col min="2" max="2" width="2.7265625" customWidth="1"/>
-    <col min="3" max="3" width="4.7265625" customWidth="1" outlineLevel="2"/>
-    <col min="4" max="4" width="1.7265625" customWidth="1"/>
-    <col min="5" max="6" width="9.1796875" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="1.7265625" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="15.7265625" customWidth="1"/>
-    <col min="12" max="12" width="9.1796875" customWidth="1"/>
-    <col min="26" max="26" width="1.7265625" customWidth="1"/>
-    <col min="27" max="28" width="4.7265625" customWidth="1"/>
-    <col min="30" max="30" width="46.1796875" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="4" max="4" width="1.7109375" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="1.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" customWidth="1"/>
+    <col min="26" max="26" width="1.7109375" customWidth="1"/>
+    <col min="27" max="28" width="4.7109375" customWidth="1"/>
+    <col min="30" max="30" width="46.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="66"/>
@@ -24342,7 +24335,7 @@
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
     </row>
-    <row r="2" spans="1:30" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="67">
@@ -24377,7 +24370,7 @@
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
-    <row r="3" spans="1:30" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:30" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="20"/>
       <c r="C3" s="68">
@@ -24412,7 +24405,7 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
     </row>
-    <row r="4" spans="1:30" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="34" t="s">
         <v>21</v>
@@ -24449,7 +24442,7 @@
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
     </row>
-    <row r="5" spans="1:30" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:30" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="33"/>
       <c r="C5" s="67">
@@ -24526,7 +24519,7 @@
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" spans="1:30" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="33"/>
       <c r="C6" s="67">
@@ -24566,7 +24559,7 @@
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
     </row>
-    <row r="7" spans="1:30" ht="20.149999999999999" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:30" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="33"/>
       <c r="C7" s="67">
@@ -24607,7 +24600,7 @@
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
     </row>
-    <row r="8" spans="1:30" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="33"/>
       <c r="C8" s="67">
@@ -24642,7 +24635,7 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
     </row>
-    <row r="9" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="33"/>
       <c r="C9" s="67">
@@ -24677,7 +24670,7 @@
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
     </row>
-    <row r="10" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="33"/>
       <c r="C10" s="67">
@@ -24712,7 +24705,7 @@
       <c r="AC10" s="1"/>
       <c r="AD10" s="1"/>
     </row>
-    <row r="11" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="33"/>
       <c r="C11" s="67">
@@ -24747,7 +24740,7 @@
       <c r="AC11" s="1"/>
       <c r="AD11" s="1"/>
     </row>
-    <row r="12" spans="1:30" ht="28" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:30" ht="30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="33"/>
       <c r="C12" s="67">
@@ -24786,7 +24779,7 @@
       <c r="AC12" s="1"/>
       <c r="AD12" s="1"/>
     </row>
-    <row r="13" spans="1:30" ht="11.5" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:30" ht="11.45" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="33" t="s">
         <v>20</v>
@@ -24823,7 +24816,7 @@
       <c r="AC13" s="1"/>
       <c r="AD13" s="1"/>
     </row>
-    <row r="14" spans="1:30" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:30" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="33"/>
       <c r="C14" s="67">
@@ -24858,7 +24851,7 @@
       <c r="AC14" s="1"/>
       <c r="AD14" s="1"/>
     </row>
-    <row r="15" spans="1:30" outlineLevel="4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:30" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="33" t="s">
         <v>19</v>
@@ -24897,7 +24890,7 @@
       <c r="AC15" s="1"/>
       <c r="AD15" s="1"/>
     </row>
-    <row r="16" spans="1:30" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="33"/>
       <c r="C16" s="67">
@@ -24934,7 +24927,7 @@
       <c r="AC16" s="1"/>
       <c r="AD16" s="1"/>
     </row>
-    <row r="17" spans="1:30" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="33"/>
       <c r="C17" s="67">
@@ -24971,7 +24964,7 @@
       <c r="AC17" s="1"/>
       <c r="AD17" s="1"/>
     </row>
-    <row r="18" spans="1:30" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:30" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="33"/>
       <c r="C18" s="67">
@@ -25012,7 +25005,7 @@
       <c r="AC18" s="1"/>
       <c r="AD18" s="1"/>
     </row>
-    <row r="19" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="33"/>
       <c r="C19" s="67">
@@ -25047,7 +25040,7 @@
       <c r="AC19" s="1"/>
       <c r="AD19" s="1"/>
     </row>
-    <row r="20" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="33"/>
       <c r="C20" s="67">
@@ -25082,7 +25075,7 @@
       <c r="AC20" s="1"/>
       <c r="AD20" s="1"/>
     </row>
-    <row r="21" spans="1:30" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:30" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="33"/>
       <c r="C21" s="67">
@@ -25123,7 +25116,7 @@
       <c r="AC21" s="1"/>
       <c r="AD21" s="1"/>
     </row>
-    <row r="22" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="33"/>
       <c r="C22" s="67">
@@ -25158,7 +25151,7 @@
       <c r="AC22" s="1"/>
       <c r="AD22" s="1"/>
     </row>
-    <row r="23" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="33"/>
       <c r="C23" s="67">
@@ -25193,7 +25186,7 @@
       <c r="AC23" s="1"/>
       <c r="AD23" s="1"/>
     </row>
-    <row r="24" spans="1:30" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="33"/>
       <c r="C24" s="67">
@@ -25230,7 +25223,7 @@
       <c r="AC24" s="1"/>
       <c r="AD24" s="1"/>
     </row>
-    <row r="25" spans="1:30" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="33"/>
       <c r="C25" s="67">
@@ -25267,7 +25260,7 @@
       <c r="AC25" s="1"/>
       <c r="AD25" s="1"/>
     </row>
-    <row r="26" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="33"/>
       <c r="C26" s="67">
@@ -25316,7 +25309,7 @@
       <c r="AC26" s="1"/>
       <c r="AD26" s="1"/>
     </row>
-    <row r="27" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="33"/>
       <c r="C27" s="67">
@@ -25355,7 +25348,7 @@
       <c r="AC27" s="1"/>
       <c r="AD27" s="1"/>
     </row>
-    <row r="28" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="33"/>
       <c r="C28" s="67">
@@ -25394,7 +25387,7 @@
       <c r="AC28" s="1"/>
       <c r="AD28" s="1"/>
     </row>
-    <row r="29" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="33"/>
       <c r="C29" s="67">
@@ -25433,7 +25426,7 @@
       <c r="AC29" s="1"/>
       <c r="AD29" s="1"/>
     </row>
-    <row r="30" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="33"/>
       <c r="C30" s="67">
@@ -25472,7 +25465,7 @@
       <c r="AC30" s="1"/>
       <c r="AD30" s="1"/>
     </row>
-    <row r="31" spans="1:30" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="33"/>
       <c r="C31" s="67">
@@ -25509,7 +25502,7 @@
       <c r="AC31" s="1"/>
       <c r="AD31" s="1"/>
     </row>
-    <row r="32" spans="1:30" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="33"/>
       <c r="C32" s="67">
@@ -25546,7 +25539,7 @@
       <c r="AC32" s="1"/>
       <c r="AD32" s="1"/>
     </row>
-    <row r="33" spans="1:30" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:30" ht="15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="33"/>
       <c r="C33" s="67">
@@ -25607,7 +25600,7 @@
       <c r="AC33" s="1"/>
       <c r="AD33" s="1"/>
     </row>
-    <row r="34" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="33"/>
       <c r="C34" s="67">
@@ -25672,7 +25665,7 @@
       <c r="AC34" s="1"/>
       <c r="AD34" s="1"/>
     </row>
-    <row r="35" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="33"/>
       <c r="C35" s="67">
@@ -25707,7 +25700,7 @@
       <c r="AC35" s="1"/>
       <c r="AD35" s="1"/>
     </row>
-    <row r="36" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="33"/>
       <c r="C36" s="67">
@@ -25742,7 +25735,7 @@
       <c r="AC36" s="1"/>
       <c r="AD36" s="1"/>
     </row>
-    <row r="37" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:30" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="33"/>
       <c r="C37" s="67">
@@ -25777,7 +25770,7 @@
       <c r="AC37" s="1"/>
       <c r="AD37" s="1"/>
     </row>
-    <row r="38" spans="1:30" ht="5.15" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="33"/>
       <c r="C38" s="67">
@@ -25814,7 +25807,7 @@
       <c r="AC38" s="1"/>
       <c r="AD38" s="1"/>
     </row>
-    <row r="39" spans="1:30" ht="5.15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="33"/>
       <c r="C39" s="67">
@@ -25849,7 +25842,7 @@
       <c r="AC39" s="1"/>
       <c r="AD39" s="1"/>
     </row>
-    <row r="40" spans="1:30" ht="5.15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:30" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="35"/>
       <c r="C40" s="70">
@@ -25886,7 +25879,7 @@
       <c r="AC40" s="1"/>
       <c r="AD40" s="1"/>
     </row>
-    <row r="41" spans="1:30" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:30" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="19"/>
       <c r="C41" s="71">
@@ -25921,7 +25914,7 @@
       <c r="AC41" s="1"/>
       <c r="AD41" s="1"/>
     </row>
-    <row r="42" spans="1:30" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="67">
@@ -25956,7 +25949,7 @@
       <c r="AC42" s="1"/>
       <c r="AD42" s="1"/>
     </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="66"/>
@@ -25988,7 +25981,7 @@
       <c r="AC43" s="1"/>
       <c r="AD43" s="1"/>
     </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="66"/>
@@ -26020,7 +26013,7 @@
       <c r="AC44" s="1"/>
       <c r="AD44" s="1"/>
     </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="66"/>
@@ -26052,7 +26045,7 @@
       <c r="AC45" s="1"/>
       <c r="AD45" s="1"/>
     </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="66"/>
@@ -26084,7 +26077,7 @@
       <c r="AC46" s="1"/>
       <c r="AD46" s="1"/>
     </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="66"/>
@@ -26116,7 +26109,7 @@
       <c r="AC47" s="1"/>
       <c r="AD47" s="1"/>
     </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="66"/>
@@ -26148,7 +26141,7 @@
       <c r="AC48" s="1"/>
       <c r="AD48" s="1"/>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C49" s="72" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
add comments and version control comments xl
</commit_message>
<xml_diff>
--- a/Structural.xlsx
+++ b/Structural.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DFBCA05-CBBE-4EFE-AA88-A865F8167B74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA31942-0D89-4463-8FD8-07B001082C58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
@@ -2445,11 +2445,6 @@
 1: 1Apr19-Created the version control table</t>
   </si>
   <si>
-    <t>25Apr21: Moved inputs from Property.xlsx
-                   Moved FVP &amp; N inputs from Stock
-1: 1Apr19-Created the version control table</t>
-  </si>
-  <si>
     <t>nut spread</t>
   </si>
   <si>
@@ -2556,6 +2551,13 @@
   </si>
   <si>
     <t>mortality</t>
+  </si>
+  <si>
+    <t>27Apr21: add named ranges to inputs copied from pinp.
+                   Add REV inputs
+25Apr21: Moved inputs from Property.xlsx
+                   Moved FVP &amp; N inputs from Stock
+1: 1Apr19-Created the version control table</t>
   </si>
 </sst>
 </file>
@@ -8154,7 +8156,7 @@
   </sheetPr>
   <dimension ref="A1:AE312"/>
   <sheetViews>
-    <sheetView topLeftCell="B267" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C305" sqref="C305"/>
     </sheetView>
   </sheetViews>
@@ -23147,8 +23149,8 @@
   </sheetPr>
   <dimension ref="A1:AB157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="L143" sqref="L143"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18:T18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -23808,7 +23810,7 @@
         <v>44311.763956365699</v>
       </c>
       <c r="J18" s="185" t="s">
-        <v>285</v>
+        <v>314</v>
       </c>
       <c r="K18" s="186"/>
       <c r="L18" s="186"/>
@@ -26814,24 +26816,24 @@
       <c r="H98" s="2"/>
       <c r="I98" s="174"/>
       <c r="J98" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="K98" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="K98" s="2" t="s">
-        <v>287</v>
-      </c>
       <c r="L98" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="M98" s="2" t="s">
         <v>286</v>
-      </c>
-      <c r="M98" s="2" t="s">
-        <v>287</v>
       </c>
       <c r="N98" s="2"/>
       <c r="O98" s="2"/>
       <c r="P98" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q98" s="2" t="s">
         <v>286</v>
-      </c>
-      <c r="Q98" s="2" t="s">
-        <v>287</v>
       </c>
       <c r="R98" s="2"/>
       <c r="S98" s="2"/>
@@ -26859,10 +26861,10 @@
       <c r="F99" s="5"/>
       <c r="G99" s="4"/>
       <c r="H99" s="175" t="s">
+        <v>287</v>
+      </c>
+      <c r="I99" s="176" t="s">
         <v>288</v>
-      </c>
-      <c r="I99" s="176" t="s">
-        <v>289</v>
       </c>
       <c r="J99" s="177">
         <v>0</v>
@@ -26911,7 +26913,7 @@
       <c r="G100" s="4"/>
       <c r="H100" s="175"/>
       <c r="I100" s="176" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J100" s="175"/>
       <c r="K100" s="175"/>
@@ -26956,7 +26958,7 @@
       <c r="G101" s="4"/>
       <c r="H101" s="175"/>
       <c r="I101" s="176" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J101" s="175"/>
       <c r="K101" s="175"/>
@@ -27001,7 +27003,7 @@
       <c r="G102" s="4"/>
       <c r="H102" s="175"/>
       <c r="I102" s="176" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J102" s="175"/>
       <c r="K102" s="175"/>
@@ -27046,7 +27048,7 @@
       <c r="G103" s="4"/>
       <c r="H103" s="175"/>
       <c r="I103" s="176" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J103" s="175"/>
       <c r="K103" s="175"/>
@@ -27091,7 +27093,7 @@
       <c r="G104" s="4"/>
       <c r="H104" s="175"/>
       <c r="I104" s="176" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="J104" s="175"/>
       <c r="K104" s="175"/>
@@ -27136,7 +27138,7 @@
       <c r="G105" s="4"/>
       <c r="H105" s="175"/>
       <c r="I105" s="176" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="J105" s="175"/>
       <c r="K105" s="175"/>
@@ -27181,7 +27183,7 @@
       <c r="G106" s="4"/>
       <c r="H106" s="175"/>
       <c r="I106" s="176" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="J106" s="175"/>
       <c r="K106" s="175"/>
@@ -27289,7 +27291,7 @@
       <c r="F109" s="5"/>
       <c r="G109" s="4"/>
       <c r="H109" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I109" s="2"/>
       <c r="J109" s="100" t="s">
@@ -27332,42 +27334,42 @@
       <c r="H110" s="2"/>
       <c r="I110" s="2"/>
       <c r="J110" s="100" t="s">
+        <v>297</v>
+      </c>
+      <c r="K110" s="100" t="s">
         <v>298</v>
       </c>
-      <c r="K110" s="100" t="s">
+      <c r="L110" s="100" t="s">
         <v>299</v>
       </c>
-      <c r="L110" s="100" t="s">
+      <c r="M110" s="100" t="s">
         <v>300</v>
-      </c>
-      <c r="M110" s="100" t="s">
-        <v>301</v>
       </c>
       <c r="N110" s="2"/>
       <c r="O110" s="100" t="s">
+        <v>297</v>
+      </c>
+      <c r="P110" s="100" t="s">
         <v>298</v>
       </c>
-      <c r="P110" s="100" t="s">
+      <c r="Q110" s="100" t="s">
         <v>299</v>
       </c>
-      <c r="Q110" s="100" t="s">
+      <c r="R110" s="100" t="s">
         <v>300</v>
-      </c>
-      <c r="R110" s="100" t="s">
-        <v>301</v>
       </c>
       <c r="S110" s="2"/>
       <c r="T110" s="100" t="s">
+        <v>297</v>
+      </c>
+      <c r="U110" s="100" t="s">
         <v>298</v>
       </c>
-      <c r="U110" s="100" t="s">
+      <c r="V110" s="100" t="s">
         <v>299</v>
       </c>
-      <c r="V110" s="100" t="s">
+      <c r="W110" s="100" t="s">
         <v>300</v>
-      </c>
-      <c r="W110" s="100" t="s">
-        <v>301</v>
       </c>
       <c r="X110" s="4"/>
       <c r="Y110" s="16"/>
@@ -27389,7 +27391,7 @@
       <c r="F111" s="5"/>
       <c r="G111" s="4"/>
       <c r="H111" s="179" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I111" s="2"/>
       <c r="J111" s="180">
@@ -27450,7 +27452,7 @@
       <c r="F112" s="5"/>
       <c r="G112" s="4"/>
       <c r="H112" s="179" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="I112" s="2"/>
       <c r="J112" s="2"/>
@@ -27503,7 +27505,7 @@
       <c r="F113" s="5"/>
       <c r="G113" s="4"/>
       <c r="H113" s="179" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I113" s="2"/>
       <c r="J113" s="2"/>
@@ -28176,7 +28178,7 @@
       <c r="F132" s="5"/>
       <c r="G132" s="4"/>
       <c r="H132" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I132" s="31" t="b">
         <v>0</v>
@@ -28240,7 +28242,7 @@
       <c r="F134" s="5"/>
       <c r="G134" s="4"/>
       <c r="H134" s="26" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I134" s="31">
         <v>0</v>
@@ -28347,10 +28349,10 @@
       <c r="F137" s="5"/>
       <c r="G137" s="4"/>
       <c r="H137" s="64" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I137" s="64" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J137" s="2"/>
       <c r="K137" s="2"/>
@@ -28386,7 +28388,7 @@
       <c r="F138" s="5"/>
       <c r="G138" s="4"/>
       <c r="H138" s="31" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="I138" s="31" t="b">
         <v>0</v>
@@ -28425,7 +28427,7 @@
       <c r="F139" s="5"/>
       <c r="G139" s="4"/>
       <c r="H139" s="31" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I139" s="31" t="b">
         <v>0</v>
@@ -28464,7 +28466,7 @@
       <c r="F140" s="5"/>
       <c r="G140" s="4"/>
       <c r="H140" s="31" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I140" s="31" t="b">
         <v>0</v>
@@ -28503,7 +28505,7 @@
       <c r="F141" s="5"/>
       <c r="G141" s="4"/>
       <c r="H141" s="31" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="I141" s="31" t="b">
         <v>0</v>
@@ -28542,7 +28544,7 @@
       <c r="F142" s="5"/>
       <c r="G142" s="4"/>
       <c r="H142" s="31" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I142" s="31" t="b">
         <v>0</v>
@@ -28581,7 +28583,7 @@
       <c r="F143" s="5"/>
       <c r="G143" s="4"/>
       <c r="H143" s="31" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="I143" s="31" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
combine offs fvps they can all be changed
</commit_message>
<xml_diff>
--- a/Structural.xlsx
+++ b/Structural.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DDCA022-C9AA-4594-83E1-79291B931577}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635129C4-D2FE-4242-A343-4ACFF4426150}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -50,25 +50,25 @@
     <definedName name="i_b0_pos">Stock!$I$54</definedName>
     <definedName name="i_b1_pos">Stock!$I$55</definedName>
     <definedName name="i_btrt_idx_offs">Stock!$L$276:$Q$276</definedName>
-    <definedName name="i_condensefvp_type3">Stock!$J$334</definedName>
+    <definedName name="i_condensefvp_type3">StructuralSA!$J$63</definedName>
     <definedName name="i_d_pos">Stock!$I$56</definedName>
     <definedName name="i_date_assetvalue" localSheetId="0">General!$I$68</definedName>
     <definedName name="i_density_n0" localSheetId="2">StructuralSA!$K$93</definedName>
     <definedName name="i_density_n1" localSheetId="2">StructuralSA!$M$93:$M$99</definedName>
     <definedName name="i_density_n3" localSheetId="2">StructuralSA!$Q$93:$Q$100</definedName>
     <definedName name="i_dvp_mask_f1">StructuralSA!$M$53:$O$53</definedName>
-    <definedName name="i_dvp_mask_f3">StructuralSA!$M$62</definedName>
+    <definedName name="i_dvp_mask_f3">StructuralSA!$J$62:$M$62</definedName>
     <definedName name="i_e0_pos">Stock!$I$57</definedName>
     <definedName name="i_e1_pos">Stock!$I$58</definedName>
     <definedName name="i_feedsupply_itn_max">Stock!$I$80</definedName>
     <definedName name="i_fixed_dvp_mask_f1">Stock!$J$322:$L$322</definedName>
-    <definedName name="i_fixed_dvp_mask_f3">Stock!$J$333:$L$333</definedName>
+    <definedName name="i_fixed_dvp_mask_f3">Stock!#REF!</definedName>
     <definedName name="i_fixed_fvp_is_rdvp_f1">Stock!$J$323:$L$323</definedName>
     <definedName name="i_fixed_fvp_mask_dams">Stock!$J$320:$L$320</definedName>
-    <definedName name="i_fixed_fvp_mask_offs">Stock!$J$332:$L$332</definedName>
+    <definedName name="i_fixed_fvp_mask_offs">Stock!#REF!</definedName>
     <definedName name="i_fvp_is_rdvp_f1">StructuralSA!$M$54:$O$54</definedName>
     <definedName name="i_fvp_mask_dams">StructuralSA!$M$52:$O$52</definedName>
-    <definedName name="i_fvp_mask_offs">StructuralSA!$M$61</definedName>
+    <definedName name="i_fvp_mask_offs">StructuralSA!$J$61:$M$61</definedName>
     <definedName name="i_fvp4_date_i">StructuralSA!$O$55:$O$56</definedName>
     <definedName name="i_i_pos">Stock!$I$59</definedName>
     <definedName name="i_initial_b1">Stock!$L$163:$V$163</definedName>
@@ -1144,78 +1144,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="H332" authorId="0" shapeId="0" xr:uid="{6E1B67F4-BA96-4619-801B-47B8B30D7DE5}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Michael Young (21512438):</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-is the fvp being included in the model?</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H333" authorId="0" shapeId="0" xr:uid="{F8701BF3-886C-419F-AAF3-B4244F73A42F}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Michael Young (21512438):</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-is the fvp also a dvp?</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H334" authorId="0" shapeId="0" xr:uid="{2E6D080D-9B0F-4D90-8531-D9D2DD0BED71}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Michael Young (21512438):</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-DVP when condensing happens. For offs this can be any dvp.</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -1392,6 +1320,30 @@
           </rPr>
           <t xml:space="preserve">
 is the fvp also a dvp?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H63" authorId="0" shapeId="0" xr:uid="{496180E6-8141-4CF1-904D-19BDEBD21322}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Michael Young (21512438):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+DVP when condensing happens. For offs this can be any dvp.</t>
         </r>
       </text>
     </comment>
@@ -1622,7 +1574,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="312">
   <si>
     <t>Controls for this worksheet</t>
   </si>
@@ -8263,10 +8215,10 @@
   <sheetPr codeName="Sheet1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AE348"/>
+  <dimension ref="A1:AE343"/>
   <sheetViews>
-    <sheetView topLeftCell="B314" workbookViewId="0">
-      <selection activeCell="J333" sqref="J333:L333"/>
+    <sheetView tabSelected="1" topLeftCell="B314" workbookViewId="0">
+      <selection activeCell="B330" sqref="A330:XFD334"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -23955,30 +23907,22 @@
       <c r="AA329" s="1"/>
       <c r="AB329" s="1"/>
     </row>
-    <row r="330" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A330" s="1"/>
       <c r="B330" s="33"/>
       <c r="C330" s="73">
-        <f>INT($C$40)+2</f>
-        <v>3</v>
+        <f>INT($C$40)+3</f>
+        <v>4</v>
       </c>
       <c r="D330" s="4"/>
       <c r="E330" s="5"/>
       <c r="F330" s="5"/>
       <c r="G330" s="4"/>
-      <c r="H330" s="100" t="s">
-        <v>250</v>
-      </c>
+      <c r="H330" s="2"/>
       <c r="I330" s="2"/>
-      <c r="J330" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="K330" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="L330" s="2" t="s">
-        <v>253</v>
-      </c>
+      <c r="J330" s="2"/>
+      <c r="K330" s="2"/>
+      <c r="L330" s="2"/>
       <c r="M330" s="2"/>
       <c r="N330" s="2"/>
       <c r="O330" s="2"/>
@@ -23996,340 +23940,302 @@
       <c r="AA330" s="1"/>
       <c r="AB330" s="1"/>
     </row>
-    <row r="331" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:28" s="142" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A331" s="1"/>
       <c r="B331" s="33"/>
       <c r="C331" s="73">
-        <f>INT($C$40)+3</f>
-        <v>4</v>
+        <f>INT($C$40)+3.005</f>
+        <v>4.0049999999999999</v>
       </c>
       <c r="D331" s="4"/>
-      <c r="E331" s="5"/>
-      <c r="F331" s="5"/>
+      <c r="E331" s="4"/>
+      <c r="F331" s="4"/>
       <c r="G331" s="4"/>
-      <c r="H331" s="2"/>
-      <c r="I331" s="2"/>
-      <c r="J331" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="K331" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="L331" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="M331" s="2"/>
-      <c r="N331" s="2"/>
-      <c r="O331" s="2"/>
-      <c r="P331" s="2"/>
-      <c r="Q331" s="2"/>
-      <c r="R331" s="2"/>
-      <c r="S331" s="2"/>
-      <c r="T331" s="2"/>
-      <c r="U331" s="2"/>
-      <c r="V331" s="2"/>
-      <c r="W331" s="2"/>
-      <c r="X331" s="4"/>
+      <c r="H331" s="83"/>
+      <c r="I331" s="83"/>
+      <c r="J331" s="83"/>
+      <c r="K331" s="83"/>
+      <c r="L331" s="83"/>
+      <c r="M331" s="83"/>
+      <c r="N331" s="83"/>
+      <c r="O331" s="83"/>
+      <c r="P331" s="83"/>
+      <c r="Q331" s="83"/>
+      <c r="R331" s="83"/>
+      <c r="S331" s="83"/>
+      <c r="T331" s="83"/>
+      <c r="U331" s="83"/>
+      <c r="V331" s="83"/>
+      <c r="W331" s="83"/>
+      <c r="X331" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="Y331" s="16"/>
       <c r="Z331" s="1"/>
       <c r="AA331" s="1"/>
       <c r="AB331" s="1"/>
     </row>
-    <row r="332" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:28" s="142" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A332" s="1"/>
       <c r="B332" s="33"/>
       <c r="C332" s="73">
-        <f>INT($C$40)+3</f>
-        <v>4</v>
+        <f>INT($C$40)+2.005</f>
+        <v>3.0049999999999999</v>
       </c>
       <c r="D332" s="4"/>
-      <c r="E332" s="5"/>
-      <c r="F332" s="5"/>
+      <c r="E332" s="4"/>
+      <c r="F332" s="4"/>
       <c r="G332" s="4"/>
-      <c r="H332" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="I332" s="2"/>
-      <c r="J332" s="31" t="b">
-        <v>1</v>
-      </c>
-      <c r="K332" s="31" t="b">
-        <v>1</v>
-      </c>
-      <c r="L332" s="31" t="b">
-        <v>1</v>
-      </c>
-      <c r="M332" s="2"/>
-      <c r="N332" s="2"/>
-      <c r="O332" s="2"/>
-      <c r="P332" s="2"/>
-      <c r="Q332" s="2"/>
-      <c r="R332" s="2"/>
-      <c r="S332" s="2"/>
-      <c r="T332" s="2"/>
-      <c r="U332" s="2"/>
-      <c r="V332" s="2"/>
-      <c r="W332" s="2"/>
+      <c r="H332" s="4"/>
+      <c r="I332" s="4"/>
+      <c r="J332" s="4"/>
+      <c r="K332" s="4"/>
+      <c r="L332" s="4"/>
+      <c r="M332" s="4"/>
+      <c r="N332" s="4"/>
+      <c r="O332" s="4"/>
+      <c r="P332" s="4"/>
+      <c r="Q332" s="4"/>
+      <c r="R332" s="4"/>
+      <c r="S332" s="4"/>
+      <c r="T332" s="4"/>
+      <c r="U332" s="4"/>
+      <c r="V332" s="4"/>
+      <c r="W332" s="4"/>
       <c r="X332" s="4"/>
       <c r="Y332" s="16"/>
       <c r="Z332" s="1"/>
       <c r="AA332" s="1"/>
       <c r="AB332" s="1"/>
     </row>
-    <row r="333" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:28" s="142" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A333" s="1"/>
-      <c r="B333" s="33"/>
-      <c r="C333" s="73">
-        <f>INT(C$40+3)</f>
-        <v>4</v>
-      </c>
-      <c r="D333" s="4"/>
-      <c r="E333" s="5"/>
-      <c r="F333" s="5"/>
-      <c r="G333" s="4"/>
-      <c r="H333" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="I333" s="2"/>
-      <c r="J333" s="31" t="b">
-        <v>1</v>
-      </c>
-      <c r="K333" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="L333" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="M333" s="2"/>
-      <c r="N333" s="2"/>
-      <c r="O333" s="2"/>
-      <c r="P333" s="2"/>
-      <c r="Q333" s="2"/>
-      <c r="R333" s="2"/>
-      <c r="S333" s="2"/>
-      <c r="T333" s="2"/>
-      <c r="U333" s="2"/>
-      <c r="V333" s="2"/>
-      <c r="W333" s="2"/>
-      <c r="X333" s="4"/>
-      <c r="Y333" s="16"/>
+      <c r="B333" s="35"/>
+      <c r="C333" s="76">
+        <f>INT($C$40)+1.005</f>
+        <v>2.0049999999999999</v>
+      </c>
+      <c r="D333" s="17"/>
+      <c r="E333" s="17"/>
+      <c r="F333" s="17"/>
+      <c r="G333" s="17"/>
+      <c r="H333" s="17"/>
+      <c r="I333" s="17"/>
+      <c r="J333" s="17"/>
+      <c r="K333" s="17"/>
+      <c r="L333" s="17"/>
+      <c r="M333" s="17"/>
+      <c r="N333" s="17"/>
+      <c r="O333" s="17"/>
+      <c r="P333" s="17"/>
+      <c r="Q333" s="17"/>
+      <c r="R333" s="17"/>
+      <c r="S333" s="17"/>
+      <c r="T333" s="17"/>
+      <c r="U333" s="17"/>
+      <c r="V333" s="17"/>
+      <c r="W333" s="17"/>
+      <c r="X333" s="17"/>
+      <c r="Y333" s="18" t="s">
+        <v>1</v>
+      </c>
       <c r="Z333" s="1"/>
       <c r="AA333" s="1"/>
       <c r="AB333" s="1"/>
     </row>
-    <row r="334" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:28" s="142" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A334" s="1"/>
-      <c r="B334" s="33"/>
-      <c r="C334" s="73">
-        <f>INT(C$40+3)</f>
-        <v>4</v>
-      </c>
-      <c r="D334" s="4"/>
-      <c r="E334" s="5"/>
-      <c r="F334" s="5"/>
-      <c r="G334" s="4"/>
-      <c r="H334" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="I334" s="2"/>
-      <c r="J334" s="31">
-        <v>0</v>
-      </c>
-      <c r="K334" s="2"/>
-      <c r="L334" s="2"/>
-      <c r="M334" s="2"/>
-      <c r="N334" s="2"/>
-      <c r="O334" s="2"/>
-      <c r="P334" s="2"/>
-      <c r="Q334" s="2"/>
-      <c r="R334" s="2"/>
-      <c r="S334" s="2"/>
-      <c r="T334" s="2"/>
-      <c r="U334" s="2"/>
-      <c r="V334" s="2"/>
-      <c r="W334" s="2"/>
-      <c r="X334" s="4"/>
-      <c r="Y334" s="16"/>
+      <c r="B334" s="19"/>
+      <c r="C334" s="77">
+        <f>INT($C$40)+0.005</f>
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="D334" s="19"/>
+      <c r="E334" s="19"/>
+      <c r="F334" s="19"/>
+      <c r="G334" s="19"/>
+      <c r="H334" s="19"/>
+      <c r="I334" s="19"/>
+      <c r="J334" s="19"/>
+      <c r="K334" s="19"/>
+      <c r="L334" s="19"/>
+      <c r="M334" s="19"/>
+      <c r="N334" s="19"/>
+      <c r="O334" s="19"/>
+      <c r="P334" s="19"/>
+      <c r="Q334" s="19"/>
+      <c r="R334" s="19"/>
+      <c r="S334" s="19"/>
+      <c r="T334" s="19"/>
+      <c r="U334" s="19"/>
+      <c r="V334" s="19"/>
+      <c r="W334" s="19"/>
+      <c r="X334" s="19"/>
+      <c r="Y334" s="19"/>
       <c r="Z334" s="1"/>
       <c r="AA334" s="1"/>
       <c r="AB334" s="1"/>
     </row>
-    <row r="335" spans="1:28" s="142" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A335" s="1"/>
-      <c r="B335" s="33"/>
+      <c r="B335" s="1"/>
       <c r="C335" s="73">
-        <f>INT($C$40)+3</f>
-        <v>4</v>
-      </c>
-      <c r="D335" s="4"/>
-      <c r="E335" s="5"/>
-      <c r="F335" s="5"/>
-      <c r="G335" s="4"/>
-      <c r="H335" s="2"/>
-      <c r="I335" s="2"/>
-      <c r="J335" s="2"/>
-      <c r="K335" s="2"/>
-      <c r="L335" s="2"/>
-      <c r="M335" s="2"/>
-      <c r="N335" s="2"/>
-      <c r="O335" s="2"/>
-      <c r="P335" s="2"/>
-      <c r="Q335" s="2"/>
-      <c r="R335" s="2"/>
-      <c r="S335" s="2"/>
-      <c r="T335" s="2"/>
-      <c r="U335" s="2"/>
-      <c r="V335" s="2"/>
-      <c r="W335" s="2"/>
-      <c r="X335" s="4"/>
-      <c r="Y335" s="16"/>
+        <f>INT($C$40)+2</f>
+        <v>3</v>
+      </c>
+      <c r="D335" s="1"/>
+      <c r="E335" s="1"/>
+      <c r="F335" s="1"/>
+      <c r="G335" s="1"/>
+      <c r="H335" s="1"/>
+      <c r="I335" s="1"/>
+      <c r="J335" s="1"/>
+      <c r="K335" s="1"/>
+      <c r="L335" s="1"/>
+      <c r="M335" s="1"/>
+      <c r="N335" s="1"/>
+      <c r="O335" s="1"/>
+      <c r="P335" s="1"/>
+      <c r="Q335" s="1"/>
+      <c r="R335" s="1"/>
+      <c r="S335" s="1"/>
+      <c r="T335" s="1"/>
+      <c r="U335" s="1"/>
+      <c r="V335" s="1"/>
+      <c r="W335" s="1"/>
+      <c r="X335" s="1"/>
+      <c r="Y335" s="1"/>
       <c r="Z335" s="1"/>
       <c r="AA335" s="1"/>
       <c r="AB335" s="1"/>
     </row>
-    <row r="336" spans="1:28" s="142" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A336" s="1"/>
-      <c r="B336" s="33"/>
+      <c r="B336" s="1"/>
       <c r="C336" s="73">
-        <f>INT($C$40)+3.005</f>
-        <v>4.0049999999999999</v>
-      </c>
-      <c r="D336" s="4"/>
-      <c r="E336" s="4"/>
-      <c r="F336" s="4"/>
-      <c r="G336" s="4"/>
-      <c r="H336" s="83"/>
-      <c r="I336" s="83"/>
-      <c r="J336" s="83"/>
-      <c r="K336" s="83"/>
-      <c r="L336" s="83"/>
-      <c r="M336" s="83"/>
-      <c r="N336" s="83"/>
-      <c r="O336" s="83"/>
-      <c r="P336" s="83"/>
-      <c r="Q336" s="83"/>
-      <c r="R336" s="83"/>
-      <c r="S336" s="83"/>
-      <c r="T336" s="83"/>
-      <c r="U336" s="83"/>
-      <c r="V336" s="83"/>
-      <c r="W336" s="83"/>
-      <c r="X336" s="4" t="s">
+        <f>INT($C$140)+2</f>
         <v>3</v>
       </c>
-      <c r="Y336" s="16"/>
+      <c r="D336" s="1"/>
+      <c r="E336" s="1"/>
+      <c r="F336" s="1"/>
+      <c r="G336" s="1"/>
+      <c r="H336" s="1"/>
+      <c r="I336" s="1"/>
+      <c r="J336" s="1"/>
+      <c r="K336" s="1"/>
+      <c r="L336" s="1"/>
+      <c r="M336" s="1"/>
+      <c r="N336" s="1"/>
+      <c r="O336" s="1"/>
+      <c r="P336" s="1"/>
+      <c r="Q336" s="1"/>
+      <c r="R336" s="1"/>
+      <c r="S336" s="1"/>
+      <c r="T336" s="1"/>
+      <c r="U336" s="1"/>
+      <c r="V336" s="1"/>
+      <c r="W336" s="1"/>
+      <c r="X336" s="1"/>
+      <c r="Y336" s="1"/>
       <c r="Z336" s="1"/>
       <c r="AA336" s="1"/>
       <c r="AB336" s="1"/>
     </row>
-    <row r="337" spans="1:28" s="142" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A337" s="1"/>
-      <c r="B337" s="33"/>
-      <c r="C337" s="73">
-        <f>INT($C$40)+2.005</f>
-        <v>3.0049999999999999</v>
-      </c>
-      <c r="D337" s="4"/>
-      <c r="E337" s="4"/>
-      <c r="F337" s="4"/>
-      <c r="G337" s="4"/>
-      <c r="H337" s="4"/>
-      <c r="I337" s="4"/>
-      <c r="J337" s="4"/>
-      <c r="K337" s="4"/>
-      <c r="L337" s="4"/>
-      <c r="M337" s="4"/>
-      <c r="N337" s="4"/>
-      <c r="O337" s="4"/>
-      <c r="P337" s="4"/>
-      <c r="Q337" s="4"/>
-      <c r="R337" s="4"/>
-      <c r="S337" s="4"/>
-      <c r="T337" s="4"/>
-      <c r="U337" s="4"/>
-      <c r="V337" s="4"/>
-      <c r="W337" s="4"/>
-      <c r="X337" s="4"/>
-      <c r="Y337" s="16"/>
+      <c r="B337" s="1"/>
+      <c r="C337" s="66"/>
+      <c r="D337" s="1"/>
+      <c r="E337" s="1"/>
+      <c r="F337" s="1"/>
+      <c r="G337" s="1"/>
+      <c r="H337" s="1"/>
+      <c r="I337" s="1"/>
+      <c r="J337" s="1"/>
+      <c r="K337" s="1"/>
+      <c r="L337" s="1"/>
+      <c r="M337" s="1"/>
+      <c r="N337" s="1"/>
+      <c r="O337" s="1"/>
+      <c r="P337" s="1"/>
+      <c r="Q337" s="1"/>
+      <c r="R337" s="1"/>
+      <c r="S337" s="1"/>
+      <c r="T337" s="1"/>
+      <c r="U337" s="1"/>
+      <c r="V337" s="1"/>
+      <c r="W337" s="1"/>
+      <c r="X337" s="1"/>
+      <c r="Y337" s="1"/>
       <c r="Z337" s="1"/>
       <c r="AA337" s="1"/>
       <c r="AB337" s="1"/>
     </row>
-    <row r="338" spans="1:28" s="142" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A338" s="1"/>
-      <c r="B338" s="35"/>
-      <c r="C338" s="76">
-        <f>INT($C$40)+1.005</f>
-        <v>2.0049999999999999</v>
-      </c>
-      <c r="D338" s="17"/>
-      <c r="E338" s="17"/>
-      <c r="F338" s="17"/>
-      <c r="G338" s="17"/>
-      <c r="H338" s="17"/>
-      <c r="I338" s="17"/>
-      <c r="J338" s="17"/>
-      <c r="K338" s="17"/>
-      <c r="L338" s="17"/>
-      <c r="M338" s="17"/>
-      <c r="N338" s="17"/>
-      <c r="O338" s="17"/>
-      <c r="P338" s="17"/>
-      <c r="Q338" s="17"/>
-      <c r="R338" s="17"/>
-      <c r="S338" s="17"/>
-      <c r="T338" s="17"/>
-      <c r="U338" s="17"/>
-      <c r="V338" s="17"/>
-      <c r="W338" s="17"/>
-      <c r="X338" s="17"/>
-      <c r="Y338" s="18" t="s">
-        <v>1</v>
-      </c>
+      <c r="B338" s="1"/>
+      <c r="C338" s="66"/>
+      <c r="D338" s="1"/>
+      <c r="E338" s="1"/>
+      <c r="F338" s="1"/>
+      <c r="G338" s="1"/>
+      <c r="H338" s="1"/>
+      <c r="I338" s="1"/>
+      <c r="J338" s="1"/>
+      <c r="K338" s="1"/>
+      <c r="L338" s="1"/>
+      <c r="M338" s="1"/>
+      <c r="N338" s="1"/>
+      <c r="O338" s="1"/>
+      <c r="P338" s="1"/>
+      <c r="Q338" s="1"/>
+      <c r="R338" s="1"/>
+      <c r="S338" s="1"/>
+      <c r="T338" s="1"/>
+      <c r="U338" s="1"/>
+      <c r="V338" s="1"/>
+      <c r="W338" s="1"/>
+      <c r="X338" s="1"/>
+      <c r="Y338" s="1"/>
       <c r="Z338" s="1"/>
       <c r="AA338" s="1"/>
       <c r="AB338" s="1"/>
     </row>
-    <row r="339" spans="1:28" s="142" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A339" s="1"/>
-      <c r="B339" s="19"/>
-      <c r="C339" s="77">
-        <f>INT($C$40)+0.005</f>
-        <v>1.0049999999999999</v>
-      </c>
-      <c r="D339" s="19"/>
-      <c r="E339" s="19"/>
-      <c r="F339" s="19"/>
-      <c r="G339" s="19"/>
-      <c r="H339" s="19"/>
-      <c r="I339" s="19"/>
-      <c r="J339" s="19"/>
-      <c r="K339" s="19"/>
-      <c r="L339" s="19"/>
-      <c r="M339" s="19"/>
-      <c r="N339" s="19"/>
-      <c r="O339" s="19"/>
-      <c r="P339" s="19"/>
-      <c r="Q339" s="19"/>
-      <c r="R339" s="19"/>
-      <c r="S339" s="19"/>
-      <c r="T339" s="19"/>
-      <c r="U339" s="19"/>
-      <c r="V339" s="19"/>
-      <c r="W339" s="19"/>
-      <c r="X339" s="19"/>
-      <c r="Y339" s="19"/>
+      <c r="B339" s="1"/>
+      <c r="C339" s="66"/>
+      <c r="D339" s="1"/>
+      <c r="E339" s="1"/>
+      <c r="F339" s="1"/>
+      <c r="G339" s="1"/>
+      <c r="H339" s="1"/>
+      <c r="I339" s="1"/>
+      <c r="J339" s="1"/>
+      <c r="K339" s="1"/>
+      <c r="L339" s="1"/>
+      <c r="M339" s="1"/>
+      <c r="N339" s="1"/>
+      <c r="O339" s="1"/>
+      <c r="P339" s="1"/>
+      <c r="Q339" s="1"/>
+      <c r="R339" s="1"/>
+      <c r="S339" s="1"/>
+      <c r="T339" s="1"/>
+      <c r="U339" s="1"/>
+      <c r="V339" s="1"/>
+      <c r="W339" s="1"/>
+      <c r="X339" s="1"/>
+      <c r="Y339" s="1"/>
       <c r="Z339" s="1"/>
       <c r="AA339" s="1"/>
       <c r="AB339" s="1"/>
     </row>
-    <row r="340" spans="1:28" s="142" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A340" s="1"/>
       <c r="B340" s="1"/>
-      <c r="C340" s="73">
-        <f>INT($C$40)+2</f>
-        <v>3</v>
-      </c>
+      <c r="C340" s="66"/>
       <c r="D340" s="1"/>
       <c r="E340" s="1"/>
       <c r="F340" s="1"/>
@@ -24356,13 +24262,10 @@
       <c r="AA340" s="1"/>
       <c r="AB340" s="1"/>
     </row>
-    <row r="341" spans="1:28" s="95" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A341" s="1"/>
       <c r="B341" s="1"/>
-      <c r="C341" s="73">
-        <f>INT($C$140)+2</f>
-        <v>3</v>
-      </c>
+      <c r="C341" s="66"/>
       <c r="D341" s="1"/>
       <c r="E341" s="1"/>
       <c r="F341" s="1"/>
@@ -24420,157 +24323,7 @@
       <c r="AB342" s="1"/>
     </row>
     <row r="343" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A343" s="1"/>
-      <c r="B343" s="1"/>
-      <c r="C343" s="66"/>
-      <c r="D343" s="1"/>
-      <c r="E343" s="1"/>
-      <c r="F343" s="1"/>
-      <c r="G343" s="1"/>
-      <c r="H343" s="1"/>
-      <c r="I343" s="1"/>
-      <c r="J343" s="1"/>
-      <c r="K343" s="1"/>
-      <c r="L343" s="1"/>
-      <c r="M343" s="1"/>
-      <c r="N343" s="1"/>
-      <c r="O343" s="1"/>
-      <c r="P343" s="1"/>
-      <c r="Q343" s="1"/>
-      <c r="R343" s="1"/>
-      <c r="S343" s="1"/>
-      <c r="T343" s="1"/>
-      <c r="U343" s="1"/>
-      <c r="V343" s="1"/>
-      <c r="W343" s="1"/>
-      <c r="X343" s="1"/>
-      <c r="Y343" s="1"/>
-      <c r="Z343" s="1"/>
-      <c r="AA343" s="1"/>
-      <c r="AB343" s="1"/>
-    </row>
-    <row r="344" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A344" s="1"/>
-      <c r="B344" s="1"/>
-      <c r="C344" s="66"/>
-      <c r="D344" s="1"/>
-      <c r="E344" s="1"/>
-      <c r="F344" s="1"/>
-      <c r="G344" s="1"/>
-      <c r="H344" s="1"/>
-      <c r="I344" s="1"/>
-      <c r="J344" s="1"/>
-      <c r="K344" s="1"/>
-      <c r="L344" s="1"/>
-      <c r="M344" s="1"/>
-      <c r="N344" s="1"/>
-      <c r="O344" s="1"/>
-      <c r="P344" s="1"/>
-      <c r="Q344" s="1"/>
-      <c r="R344" s="1"/>
-      <c r="S344" s="1"/>
-      <c r="T344" s="1"/>
-      <c r="U344" s="1"/>
-      <c r="V344" s="1"/>
-      <c r="W344" s="1"/>
-      <c r="X344" s="1"/>
-      <c r="Y344" s="1"/>
-      <c r="Z344" s="1"/>
-      <c r="AA344" s="1"/>
-      <c r="AB344" s="1"/>
-    </row>
-    <row r="345" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A345" s="1"/>
-      <c r="B345" s="1"/>
-      <c r="C345" s="66"/>
-      <c r="D345" s="1"/>
-      <c r="E345" s="1"/>
-      <c r="F345" s="1"/>
-      <c r="G345" s="1"/>
-      <c r="H345" s="1"/>
-      <c r="I345" s="1"/>
-      <c r="J345" s="1"/>
-      <c r="K345" s="1"/>
-      <c r="L345" s="1"/>
-      <c r="M345" s="1"/>
-      <c r="N345" s="1"/>
-      <c r="O345" s="1"/>
-      <c r="P345" s="1"/>
-      <c r="Q345" s="1"/>
-      <c r="R345" s="1"/>
-      <c r="S345" s="1"/>
-      <c r="T345" s="1"/>
-      <c r="U345" s="1"/>
-      <c r="V345" s="1"/>
-      <c r="W345" s="1"/>
-      <c r="X345" s="1"/>
-      <c r="Y345" s="1"/>
-      <c r="Z345" s="1"/>
-      <c r="AA345" s="1"/>
-      <c r="AB345" s="1"/>
-    </row>
-    <row r="346" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A346" s="1"/>
-      <c r="B346" s="1"/>
-      <c r="C346" s="66"/>
-      <c r="D346" s="1"/>
-      <c r="E346" s="1"/>
-      <c r="F346" s="1"/>
-      <c r="G346" s="1"/>
-      <c r="H346" s="1"/>
-      <c r="I346" s="1"/>
-      <c r="J346" s="1"/>
-      <c r="K346" s="1"/>
-      <c r="L346" s="1"/>
-      <c r="M346" s="1"/>
-      <c r="N346" s="1"/>
-      <c r="O346" s="1"/>
-      <c r="P346" s="1"/>
-      <c r="Q346" s="1"/>
-      <c r="R346" s="1"/>
-      <c r="S346" s="1"/>
-      <c r="T346" s="1"/>
-      <c r="U346" s="1"/>
-      <c r="V346" s="1"/>
-      <c r="W346" s="1"/>
-      <c r="X346" s="1"/>
-      <c r="Y346" s="1"/>
-      <c r="Z346" s="1"/>
-      <c r="AA346" s="1"/>
-      <c r="AB346" s="1"/>
-    </row>
-    <row r="347" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A347" s="1"/>
-      <c r="B347" s="1"/>
-      <c r="C347" s="66"/>
-      <c r="D347" s="1"/>
-      <c r="E347" s="1"/>
-      <c r="F347" s="1"/>
-      <c r="G347" s="1"/>
-      <c r="H347" s="1"/>
-      <c r="I347" s="1"/>
-      <c r="J347" s="1"/>
-      <c r="K347" s="1"/>
-      <c r="L347" s="1"/>
-      <c r="M347" s="1"/>
-      <c r="N347" s="1"/>
-      <c r="O347" s="1"/>
-      <c r="P347" s="1"/>
-      <c r="Q347" s="1"/>
-      <c r="R347" s="1"/>
-      <c r="S347" s="1"/>
-      <c r="T347" s="1"/>
-      <c r="U347" s="1"/>
-      <c r="V347" s="1"/>
-      <c r="W347" s="1"/>
-      <c r="X347" s="1"/>
-      <c r="Y347" s="1"/>
-      <c r="Z347" s="1"/>
-      <c r="AA347" s="1"/>
-      <c r="AB347" s="1"/>
-    </row>
-    <row r="348" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C348" s="72" t="s">
+      <c r="C343" s="72" t="s">
         <v>4</v>
       </c>
     </row>
@@ -24594,8 +24347,8 @@
   </sheetPr>
   <dimension ref="A1:AB151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H59" sqref="H59"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="M61" sqref="M61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -26727,9 +26480,15 @@
         <v>250</v>
       </c>
       <c r="I59" s="2"/>
-      <c r="J59" s="2"/>
-      <c r="K59" s="2"/>
-      <c r="L59" s="2"/>
+      <c r="J59" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="K59" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="L59" s="2" t="s">
+        <v>253</v>
+      </c>
       <c r="M59" s="2" t="s">
         <v>241</v>
       </c>
@@ -26762,9 +26521,15 @@
       <c r="G60" s="4"/>
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
-      <c r="J60" s="2"/>
-      <c r="K60" s="2"/>
-      <c r="L60" s="2"/>
+      <c r="J60" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="K60" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="L60" s="2" t="s">
+        <v>235</v>
+      </c>
       <c r="M60" s="2" t="s">
         <v>236</v>
       </c>
@@ -26799,9 +26564,15 @@
         <v>238</v>
       </c>
       <c r="I61" s="2"/>
-      <c r="J61" s="2"/>
-      <c r="K61" s="2"/>
-      <c r="L61" s="2"/>
+      <c r="J61" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="K61" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="L61" s="31" t="b">
+        <v>1</v>
+      </c>
       <c r="M61" s="31" t="b">
         <v>0</v>
       </c>
@@ -26836,9 +26607,15 @@
         <v>239</v>
       </c>
       <c r="I62" s="2"/>
-      <c r="J62" s="2"/>
-      <c r="K62" s="2"/>
-      <c r="L62" s="2"/>
+      <c r="J62" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="K62" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="L62" s="31" t="b">
+        <v>0</v>
+      </c>
       <c r="M62" s="31" t="b">
         <v>0</v>
       </c>
@@ -26869,9 +26646,13 @@
       <c r="E63" s="5"/>
       <c r="F63" s="5"/>
       <c r="G63" s="4"/>
-      <c r="H63" s="2"/>
+      <c r="H63" s="2" t="s">
+        <v>249</v>
+      </c>
       <c r="I63" s="2"/>
-      <c r="J63" s="2"/>
+      <c r="J63" s="31">
+        <v>0</v>
+      </c>
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
       <c r="M63" s="2"/>
@@ -27666,7 +27447,7 @@
       </c>
       <c r="P85" s="121">
         <f>i_w_start_len3*i_n3_len^P88</f>
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="Q85" s="2"/>
       <c r="R85" s="2"/>
@@ -27794,7 +27575,7 @@
       <c r="O88" s="2"/>
       <c r="P88" s="121">
         <f>COUNTIF(J61:M61,TRUE)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q88" s="115"/>
       <c r="R88" s="193"/>

</xml_diff>

<commit_message>
change pool name structure.xl and add comment to code.
</commit_message>
<xml_diff>
--- a/Structural.xlsx
+++ b/Structural.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635129C4-D2FE-4242-A343-4ACFF4426150}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4A3B0B-417C-400C-8C0F-19C0C8DEEC86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -1574,7 +1574,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="313">
   <si>
     <t>Controls for this worksheet</t>
   </si>
@@ -2208,9 +2208,6 @@
     <t>Graz25</t>
   </si>
   <si>
-    <t>Graz75</t>
-  </si>
-  <si>
     <t>Graz100</t>
   </si>
   <si>
@@ -2553,6 +2550,13 @@
 25Apr21: Moved inputs from Property.xlsx
                    Moved FVP &amp; N inputs from Stock
 1: 1Apr19-Created the version control table</t>
+  </si>
+  <si>
+    <t>Graz50</t>
+  </si>
+  <si>
+    <t>28Apr21 change grazing pool names
+1: 1Apr19-Blank worksheet</t>
   </si>
 </sst>
 </file>
@@ -5145,8 +5149,8 @@
   </sheetPr>
   <dimension ref="A1:AT84"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="I62" sqref="I62:M62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21:T21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -5911,7 +5915,7 @@
         <v>1</v>
       </c>
       <c r="J21" s="188" t="s">
-        <v>35</v>
+        <v>312</v>
       </c>
       <c r="K21" s="189"/>
       <c r="L21" s="189"/>
@@ -7235,10 +7239,10 @@
         <v>209</v>
       </c>
       <c r="K58" s="101" t="s">
+        <v>311</v>
+      </c>
+      <c r="L58" s="101" t="s">
         <v>210</v>
-      </c>
-      <c r="L58" s="101" t="s">
-        <v>211</v>
       </c>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
@@ -7272,13 +7276,13 @@
         <v>202</v>
       </c>
       <c r="I59" s="101" t="s">
+        <v>211</v>
+      </c>
+      <c r="J59" s="101" t="s">
         <v>212</v>
       </c>
-      <c r="J59" s="101" t="s">
+      <c r="K59" s="101" t="s">
         <v>213</v>
-      </c>
-      <c r="K59" s="101" t="s">
-        <v>214</v>
       </c>
       <c r="L59" s="144"/>
       <c r="M59" s="2"/>
@@ -7343,22 +7347,22 @@
       <c r="F61" s="5"/>
       <c r="G61" s="4"/>
       <c r="H61" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I61" s="101" t="s">
+        <v>258</v>
+      </c>
+      <c r="J61" s="101" t="s">
         <v>259</v>
       </c>
-      <c r="J61" s="101" t="s">
+      <c r="K61" s="101" t="s">
         <v>260</v>
       </c>
-      <c r="K61" s="101" t="s">
+      <c r="L61" s="101" t="s">
         <v>261</v>
       </c>
-      <c r="L61" s="101" t="s">
-        <v>262</v>
-      </c>
       <c r="M61" s="101" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="N61" s="2"/>
       <c r="O61" s="2"/>
@@ -7385,7 +7389,7 @@
       <c r="F62" s="5"/>
       <c r="G62" s="4"/>
       <c r="H62" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I62" s="101" t="b">
         <v>1</v>
@@ -7463,7 +7467,7 @@
       <c r="F64" s="5"/>
       <c r="G64" s="4"/>
       <c r="H64" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I64" s="101">
         <v>6</v>
@@ -7533,7 +7537,7 @@
       <c r="F66" s="5"/>
       <c r="G66" s="4"/>
       <c r="H66" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I66" s="101">
         <v>1</v>
@@ -8217,7 +8221,7 @@
   </sheetPr>
   <dimension ref="A1:AE343"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B314" workbookViewId="0">
+    <sheetView topLeftCell="B314" workbookViewId="0">
       <selection activeCell="B330" sqref="A330:XFD334"/>
     </sheetView>
   </sheetViews>
@@ -8876,7 +8880,7 @@
         <v>44311.756953009302</v>
       </c>
       <c r="J18" s="185" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K18" s="186"/>
       <c r="L18" s="186"/>
@@ -8981,7 +8985,7 @@
         <v>44300</v>
       </c>
       <c r="J21" s="188" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K21" s="189"/>
       <c r="L21" s="189"/>
@@ -10072,7 +10076,7 @@
       <c r="F52" s="5"/>
       <c r="G52" s="4"/>
       <c r="H52" s="36" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I52" s="31">
         <v>-6</v>
@@ -10109,7 +10113,7 @@
       <c r="F53" s="5"/>
       <c r="G53" s="4"/>
       <c r="H53" s="36" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I53" s="31">
         <v>-14</v>
@@ -10146,7 +10150,7 @@
       <c r="F54" s="5"/>
       <c r="G54" s="4"/>
       <c r="H54" s="36" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I54" s="31">
         <v>-4</v>
@@ -10183,7 +10187,7 @@
       <c r="F55" s="5"/>
       <c r="G55" s="4"/>
       <c r="H55" s="36" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I55" s="31">
         <v>-12</v>
@@ -10220,7 +10224,7 @@
       <c r="F56" s="5"/>
       <c r="G56" s="4"/>
       <c r="H56" s="36" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I56" s="31">
         <v>-7</v>
@@ -10257,7 +10261,7 @@
       <c r="F57" s="5"/>
       <c r="G57" s="4"/>
       <c r="H57" s="133" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I57" s="31">
         <v>-5</v>
@@ -10294,7 +10298,7 @@
       <c r="F58" s="5"/>
       <c r="G58" s="4"/>
       <c r="H58" s="133" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I58" s="31">
         <v>-13</v>
@@ -10331,7 +10335,7 @@
       <c r="F59" s="5"/>
       <c r="G59" s="4"/>
       <c r="H59" s="36" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I59" s="31">
         <v>-8</v>
@@ -10479,7 +10483,7 @@
       <c r="F63" s="5"/>
       <c r="G63" s="4"/>
       <c r="H63" s="133" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I63" s="31">
         <v>-11</v>
@@ -10516,7 +10520,7 @@
       <c r="F64" s="5"/>
       <c r="G64" s="4"/>
       <c r="H64" s="133" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I64" s="31">
         <v>-15</v>
@@ -10553,7 +10557,7 @@
       <c r="F65" s="5"/>
       <c r="G65" s="4"/>
       <c r="H65" s="133" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I65" s="31">
         <v>-10</v>
@@ -10592,7 +10596,7 @@
       <c r="F66" s="5"/>
       <c r="G66" s="4"/>
       <c r="H66" s="133" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I66" s="31">
         <v>-3</v>
@@ -10629,7 +10633,7 @@
       <c r="F67" s="5"/>
       <c r="G67" s="4"/>
       <c r="H67" s="133" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I67" s="31">
         <v>-2</v>
@@ -10666,7 +10670,7 @@
       <c r="F68" s="5"/>
       <c r="G68" s="4"/>
       <c r="H68" s="133" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I68" s="31">
         <v>-9</v>
@@ -10782,7 +10786,7 @@
         <v>88</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="L71" s="2"/>
       <c r="M71" s="2"/>
@@ -10823,7 +10827,7 @@
         <v>88</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="L72" s="2"/>
       <c r="M72" s="2"/>
@@ -10888,7 +10892,7 @@
       <c r="F74" s="5"/>
       <c r="G74" s="4"/>
       <c r="H74" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I74" s="31">
         <v>8</v>
@@ -14193,7 +14197,7 @@
       <c r="F157" s="5"/>
       <c r="G157" s="4"/>
       <c r="H157" s="64" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I157" s="2"/>
       <c r="J157" s="2"/>
@@ -17237,37 +17241,37 @@
       <c r="J210" s="49"/>
       <c r="K210" s="49"/>
       <c r="L210" s="152" t="s">
+        <v>265</v>
+      </c>
+      <c r="M210" s="153" t="s">
         <v>266</v>
       </c>
-      <c r="M210" s="153" t="s">
+      <c r="N210" s="153" t="s">
         <v>267</v>
       </c>
-      <c r="N210" s="153" t="s">
+      <c r="O210" s="153" t="s">
         <v>268</v>
       </c>
-      <c r="O210" s="153" t="s">
+      <c r="P210" s="153" t="s">
         <v>269</v>
       </c>
-      <c r="P210" s="153" t="s">
+      <c r="Q210" s="153" t="s">
         <v>270</v>
       </c>
-      <c r="Q210" s="153" t="s">
+      <c r="R210" s="153" t="s">
         <v>271</v>
       </c>
-      <c r="R210" s="153" t="s">
+      <c r="S210" s="153" t="s">
         <v>272</v>
       </c>
-      <c r="S210" s="153" t="s">
+      <c r="T210" s="153" t="s">
         <v>273</v>
       </c>
-      <c r="T210" s="153" t="s">
+      <c r="U210" s="153" t="s">
         <v>274</v>
       </c>
-      <c r="U210" s="153" t="s">
+      <c r="V210" s="154" t="s">
         <v>275</v>
-      </c>
-      <c r="V210" s="154" t="s">
-        <v>276</v>
       </c>
       <c r="W210" s="94"/>
       <c r="X210" s="4"/>
@@ -17462,7 +17466,7 @@
         <v>121</v>
       </c>
       <c r="I214" s="54" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="J214" s="54" t="s">
         <v>111</v>
@@ -20294,7 +20298,7 @@
       <c r="G256" s="4"/>
       <c r="H256" s="26"/>
       <c r="I256" s="103" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="J256" s="103"/>
       <c r="K256" s="56">
@@ -23273,13 +23277,13 @@
       <c r="H313" s="29"/>
       <c r="I313" s="29"/>
       <c r="J313" s="184" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K313" s="184" t="s">
         <v>98</v>
       </c>
       <c r="L313" s="184" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="M313" s="184"/>
       <c r="N313" s="184"/>
@@ -23312,13 +23316,13 @@
       <c r="H314" s="29"/>
       <c r="I314" s="29"/>
       <c r="J314" s="184" t="s">
+        <v>232</v>
+      </c>
+      <c r="K314" s="184" t="s">
         <v>233</v>
       </c>
-      <c r="K314" s="184" t="s">
+      <c r="L314" s="184" t="s">
         <v>234</v>
-      </c>
-      <c r="L314" s="184" t="s">
-        <v>235</v>
       </c>
       <c r="M314" s="184"/>
       <c r="N314" s="184"/>
@@ -23503,7 +23507,7 @@
       <c r="F319" s="5"/>
       <c r="G319" s="4"/>
       <c r="H319" s="100" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I319" s="2"/>
       <c r="J319" s="2"/>
@@ -23538,7 +23542,7 @@
       <c r="F320" s="5"/>
       <c r="G320" s="4"/>
       <c r="H320" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I320" s="2"/>
       <c r="J320" s="31" t="b">
@@ -23579,7 +23583,7 @@
       <c r="F321" s="5"/>
       <c r="G321" s="4"/>
       <c r="H321" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I321" s="2"/>
       <c r="J321" s="121">
@@ -23620,7 +23624,7 @@
       <c r="F322" s="5"/>
       <c r="G322" s="4"/>
       <c r="H322" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I322" s="2"/>
       <c r="J322" s="31" t="b">
@@ -23661,7 +23665,7 @@
       <c r="F323" s="5"/>
       <c r="G323" s="4"/>
       <c r="H323" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I323" s="2"/>
       <c r="J323" s="31" t="b">
@@ -23702,7 +23706,7 @@
       <c r="F324" s="5"/>
       <c r="G324" s="4"/>
       <c r="H324" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I324" s="2"/>
       <c r="J324" s="2"/>
@@ -23772,13 +23776,13 @@
       <c r="H326" s="2"/>
       <c r="I326" s="147"/>
       <c r="J326" s="148" t="s">
+        <v>255</v>
+      </c>
+      <c r="K326" s="148" t="s">
         <v>256</v>
       </c>
-      <c r="K326" s="148" t="s">
+      <c r="L326" s="148" t="s">
         <v>257</v>
-      </c>
-      <c r="L326" s="148" t="s">
-        <v>258</v>
       </c>
       <c r="M326" s="2"/>
       <c r="N326" s="2"/>
@@ -23809,7 +23813,7 @@
       <c r="F327" s="5"/>
       <c r="G327" s="4"/>
       <c r="H327" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I327" s="147"/>
       <c r="J327" s="31">
@@ -25008,7 +25012,7 @@
         <v>44311.763956365699</v>
       </c>
       <c r="J18" s="185" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K18" s="186"/>
       <c r="L18" s="186"/>
@@ -25964,13 +25968,13 @@
       <c r="K45" s="29"/>
       <c r="L45" s="29"/>
       <c r="M45" s="184" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="N45" s="184" t="s">
         <v>99</v>
       </c>
       <c r="O45" s="184" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="P45" s="184"/>
       <c r="Q45" s="184"/>
@@ -26003,13 +26007,13 @@
       <c r="K46" s="29"/>
       <c r="L46" s="29"/>
       <c r="M46" s="184" t="s">
+        <v>235</v>
+      </c>
+      <c r="N46" s="184" t="s">
         <v>236</v>
       </c>
-      <c r="N46" s="184" t="s">
-        <v>237</v>
-      </c>
       <c r="O46" s="184" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="P46" s="184"/>
       <c r="Q46" s="184"/>
@@ -26181,7 +26185,7 @@
       <c r="F51" s="5"/>
       <c r="G51" s="4"/>
       <c r="H51" s="100" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
@@ -26216,7 +26220,7 @@
       <c r="F52" s="5"/>
       <c r="G52" s="4"/>
       <c r="H52" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
@@ -26257,7 +26261,7 @@
       <c r="F53" s="5"/>
       <c r="G53" s="4"/>
       <c r="H53" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
@@ -26298,7 +26302,7 @@
       <c r="F54" s="5"/>
       <c r="G54" s="4"/>
       <c r="H54" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
@@ -26339,7 +26343,7 @@
       <c r="F55" s="5"/>
       <c r="G55" s="4"/>
       <c r="H55" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
@@ -26477,20 +26481,20 @@
       <c r="F59" s="5"/>
       <c r="G59" s="4"/>
       <c r="H59" s="100" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I59" s="2"/>
       <c r="J59" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="K59" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="K59" s="2" t="s">
+      <c r="L59" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="L59" s="2" t="s">
-        <v>253</v>
-      </c>
       <c r="M59" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="N59" s="2"/>
       <c r="O59" s="2"/>
@@ -26522,16 +26526,16 @@
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
       <c r="J60" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="K60" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="K60" s="2" t="s">
+      <c r="L60" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="L60" s="2" t="s">
+      <c r="M60" s="2" t="s">
         <v>235</v>
-      </c>
-      <c r="M60" s="2" t="s">
-        <v>236</v>
       </c>
       <c r="N60" s="2"/>
       <c r="O60" s="2"/>
@@ -26561,7 +26565,7 @@
       <c r="F61" s="5"/>
       <c r="G61" s="4"/>
       <c r="H61" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I61" s="2"/>
       <c r="J61" s="31" t="b">
@@ -26604,7 +26608,7 @@
       <c r="F62" s="5"/>
       <c r="G62" s="4"/>
       <c r="H62" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I62" s="2"/>
       <c r="J62" s="31" t="b">
@@ -26647,7 +26651,7 @@
       <c r="F63" s="5"/>
       <c r="G63" s="4"/>
       <c r="H63" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I63" s="2"/>
       <c r="J63" s="31">
@@ -27715,24 +27719,24 @@
       <c r="H92" s="2"/>
       <c r="I92" s="174"/>
       <c r="J92" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="K92" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="K92" s="2" t="s">
-        <v>282</v>
-      </c>
       <c r="L92" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="M92" s="2" t="s">
         <v>281</v>
-      </c>
-      <c r="M92" s="2" t="s">
-        <v>282</v>
       </c>
       <c r="N92" s="2"/>
       <c r="O92" s="2"/>
       <c r="P92" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q92" s="2" t="s">
         <v>281</v>
-      </c>
-      <c r="Q92" s="2" t="s">
-        <v>282</v>
       </c>
       <c r="R92" s="2"/>
       <c r="S92" s="2"/>
@@ -27760,10 +27764,10 @@
       <c r="F93" s="5"/>
       <c r="G93" s="4"/>
       <c r="H93" s="175" t="s">
+        <v>282</v>
+      </c>
+      <c r="I93" s="176" t="s">
         <v>283</v>
-      </c>
-      <c r="I93" s="176" t="s">
-        <v>284</v>
       </c>
       <c r="J93" s="177">
         <v>0</v>
@@ -27812,7 +27816,7 @@
       <c r="G94" s="4"/>
       <c r="H94" s="175"/>
       <c r="I94" s="176" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J94" s="175"/>
       <c r="K94" s="175"/>
@@ -27857,7 +27861,7 @@
       <c r="G95" s="4"/>
       <c r="H95" s="175"/>
       <c r="I95" s="176" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J95" s="175"/>
       <c r="K95" s="175"/>
@@ -27902,7 +27906,7 @@
       <c r="G96" s="4"/>
       <c r="H96" s="175"/>
       <c r="I96" s="176" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J96" s="175"/>
       <c r="K96" s="175"/>
@@ -27947,7 +27951,7 @@
       <c r="G97" s="4"/>
       <c r="H97" s="175"/>
       <c r="I97" s="176" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J97" s="175"/>
       <c r="K97" s="175"/>
@@ -27992,7 +27996,7 @@
       <c r="G98" s="4"/>
       <c r="H98" s="175"/>
       <c r="I98" s="176" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J98" s="175"/>
       <c r="K98" s="175"/>
@@ -28037,7 +28041,7 @@
       <c r="G99" s="4"/>
       <c r="H99" s="175"/>
       <c r="I99" s="176" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J99" s="175"/>
       <c r="K99" s="175"/>
@@ -28082,7 +28086,7 @@
       <c r="G100" s="4"/>
       <c r="H100" s="175"/>
       <c r="I100" s="176" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J100" s="175"/>
       <c r="K100" s="175"/>
@@ -28190,7 +28194,7 @@
       <c r="F103" s="5"/>
       <c r="G103" s="4"/>
       <c r="H103" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I103" s="2"/>
       <c r="J103" s="100" t="s">
@@ -28233,42 +28237,42 @@
       <c r="H104" s="2"/>
       <c r="I104" s="2"/>
       <c r="J104" s="100" t="s">
+        <v>292</v>
+      </c>
+      <c r="K104" s="100" t="s">
         <v>293</v>
       </c>
-      <c r="K104" s="100" t="s">
+      <c r="L104" s="100" t="s">
         <v>294</v>
       </c>
-      <c r="L104" s="100" t="s">
+      <c r="M104" s="100" t="s">
         <v>295</v>
-      </c>
-      <c r="M104" s="100" t="s">
-        <v>296</v>
       </c>
       <c r="N104" s="2"/>
       <c r="O104" s="100" t="s">
+        <v>292</v>
+      </c>
+      <c r="P104" s="100" t="s">
         <v>293</v>
       </c>
-      <c r="P104" s="100" t="s">
+      <c r="Q104" s="100" t="s">
         <v>294</v>
       </c>
-      <c r="Q104" s="100" t="s">
+      <c r="R104" s="100" t="s">
         <v>295</v>
-      </c>
-      <c r="R104" s="100" t="s">
-        <v>296</v>
       </c>
       <c r="S104" s="2"/>
       <c r="T104" s="100" t="s">
+        <v>292</v>
+      </c>
+      <c r="U104" s="100" t="s">
         <v>293</v>
       </c>
-      <c r="U104" s="100" t="s">
+      <c r="V104" s="100" t="s">
         <v>294</v>
       </c>
-      <c r="V104" s="100" t="s">
+      <c r="W104" s="100" t="s">
         <v>295</v>
-      </c>
-      <c r="W104" s="100" t="s">
-        <v>296</v>
       </c>
       <c r="X104" s="4"/>
       <c r="Y104" s="16"/>
@@ -28290,7 +28294,7 @@
       <c r="F105" s="5"/>
       <c r="G105" s="4"/>
       <c r="H105" s="179" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I105" s="2"/>
       <c r="J105" s="180">
@@ -28351,7 +28355,7 @@
       <c r="F106" s="5"/>
       <c r="G106" s="4"/>
       <c r="H106" s="179" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I106" s="2"/>
       <c r="J106" s="2"/>
@@ -28404,7 +28408,7 @@
       <c r="F107" s="5"/>
       <c r="G107" s="4"/>
       <c r="H107" s="179" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I107" s="2"/>
       <c r="J107" s="2"/>
@@ -29077,7 +29081,7 @@
       <c r="F126" s="5"/>
       <c r="G126" s="4"/>
       <c r="H126" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I126" s="31" t="b">
         <v>0</v>
@@ -29141,7 +29145,7 @@
       <c r="F128" s="5"/>
       <c r="G128" s="4"/>
       <c r="H128" s="26" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I128" s="31">
         <v>0</v>
@@ -29248,10 +29252,10 @@
       <c r="F131" s="5"/>
       <c r="G131" s="4"/>
       <c r="H131" s="64" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="I131" s="64" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="J131" s="2"/>
       <c r="K131" s="2"/>
@@ -29287,7 +29291,7 @@
       <c r="F132" s="5"/>
       <c r="G132" s="4"/>
       <c r="H132" s="31" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I132" s="31" t="b">
         <v>0</v>
@@ -29326,7 +29330,7 @@
       <c r="F133" s="5"/>
       <c r="G133" s="4"/>
       <c r="H133" s="31" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I133" s="31" t="b">
         <v>0</v>
@@ -29365,7 +29369,7 @@
       <c r="F134" s="5"/>
       <c r="G134" s="4"/>
       <c r="H134" s="31" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I134" s="31" t="b">
         <v>0</v>
@@ -29404,7 +29408,7 @@
       <c r="F135" s="5"/>
       <c r="G135" s="4"/>
       <c r="H135" s="31" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I135" s="31" t="b">
         <v>0</v>
@@ -29443,7 +29447,7 @@
       <c r="F136" s="5"/>
       <c r="G136" s="4"/>
       <c r="H136" s="31" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I136" s="31" t="b">
         <v>0</v>
@@ -29482,7 +29486,7 @@
       <c r="F137" s="5"/>
       <c r="G137" s="4"/>
       <c r="H137" s="31" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="I137" s="31" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
finish adding lcw REV
</commit_message>
<xml_diff>
--- a/Structural.xlsx
+++ b/Structural.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4A3B0B-417C-400C-8C0F-19C0C8DEEC86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF6A3C3-28B9-47E2-A60F-17E398A2EEEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -138,8 +138,8 @@
     <definedName name="rdvp_type_r">Stock!$J$327:$L$327</definedName>
     <definedName name="rev_create" localSheetId="2">StructuralSA!$I$126</definedName>
     <definedName name="rev_number" localSheetId="2">StructuralSA!$I$128</definedName>
-    <definedName name="rev_trait_inc" localSheetId="2">StructuralSA!$I$132:$I$137</definedName>
-    <definedName name="rev_trait_name" localSheetId="2">StructuralSA!$H$132:$H$137</definedName>
+    <definedName name="rev_trait_inc" localSheetId="2">StructuralSA!$I$132:$I$138</definedName>
+    <definedName name="rev_trait_name" localSheetId="2">StructuralSA!$H$132:$H$138</definedName>
     <definedName name="sheep_pools" localSheetId="0">General!$I$61:$M$61</definedName>
     <definedName name="worker_levels" localSheetId="0">General!$I$51:$K$51</definedName>
     <definedName name="ZA.Gridlines" localSheetId="3">Admin!$L$29</definedName>
@@ -1574,7 +1574,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="314">
   <si>
     <t>Controls for this worksheet</t>
   </si>
@@ -2557,6 +2557,9 @@
   <si>
     <t>28Apr21 change grazing pool names
 1: 1Apr19-Blank worksheet</t>
+  </si>
+  <si>
+    <t>lwc</t>
   </si>
 </sst>
 </file>
@@ -5149,7 +5152,7 @@
   </sheetPr>
   <dimension ref="A1:AT84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J21" sqref="J21:T21"/>
     </sheetView>
   </sheetViews>
@@ -24349,10 +24352,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AB151"/>
+  <dimension ref="A1:AB152"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="M61" sqref="M61"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="H138" sqref="H138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -29437,7 +29440,7 @@
       <c r="A136" s="1"/>
       <c r="B136" s="33"/>
       <c r="C136" s="73">
-        <f t="shared" ref="C136:C139" si="4">INT(C$74+3)</f>
+        <f t="shared" ref="C136:C140" si="4">INT(C$74+3)</f>
         <v>4</v>
       </c>
       <c r="D136" s="4"/>
@@ -29475,14 +29478,9 @@
     <row r="137" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A137" s="1"/>
       <c r="B137" s="33"/>
-      <c r="C137" s="73">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
+      <c r="C137" s="73"/>
       <c r="D137" s="4"/>
-      <c r="E137" s="5">
-        <v>5</v>
-      </c>
+      <c r="E137" s="5"/>
       <c r="F137" s="5"/>
       <c r="G137" s="4"/>
       <c r="H137" s="31" t="s">
@@ -29520,12 +29518,16 @@
       </c>
       <c r="D138" s="4"/>
       <c r="E138" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F138" s="5"/>
       <c r="G138" s="4"/>
-      <c r="H138" s="175"/>
-      <c r="I138" s="175"/>
+      <c r="H138" s="31" t="s">
+        <v>313</v>
+      </c>
+      <c r="I138" s="31" t="b">
+        <v>0</v>
+      </c>
       <c r="J138" s="175"/>
       <c r="K138" s="175"/>
       <c r="L138" s="175"/>
@@ -29555,7 +29557,7 @@
       </c>
       <c r="D139" s="4"/>
       <c r="E139" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F139" s="5"/>
       <c r="G139" s="4"/>
@@ -29581,47 +29583,47 @@
       <c r="AA139" s="1"/>
       <c r="AB139" s="1"/>
     </row>
-    <row r="140" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
       <c r="B140" s="33"/>
       <c r="C140" s="73">
-        <f>INT($C$74)+3.005</f>
-        <v>4.0049999999999999</v>
+        <f t="shared" si="4"/>
+        <v>4</v>
       </c>
       <c r="D140" s="4"/>
-      <c r="E140" s="4"/>
-      <c r="F140" s="4"/>
+      <c r="E140" s="5">
+        <v>7</v>
+      </c>
+      <c r="F140" s="5"/>
       <c r="G140" s="4"/>
-      <c r="H140" s="4"/>
-      <c r="I140" s="4"/>
-      <c r="J140" s="4"/>
-      <c r="K140" s="4"/>
-      <c r="L140" s="4"/>
-      <c r="M140" s="4"/>
-      <c r="N140" s="4"/>
-      <c r="O140" s="4"/>
-      <c r="P140" s="4"/>
-      <c r="Q140" s="4"/>
-      <c r="R140" s="4"/>
-      <c r="S140" s="4"/>
-      <c r="T140" s="4"/>
-      <c r="U140" s="4"/>
-      <c r="V140" s="4"/>
-      <c r="W140" s="4"/>
-      <c r="X140" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="H140" s="175"/>
+      <c r="I140" s="175"/>
+      <c r="J140" s="175"/>
+      <c r="K140" s="175"/>
+      <c r="L140" s="175"/>
+      <c r="M140" s="175"/>
+      <c r="N140" s="175"/>
+      <c r="O140" s="175"/>
+      <c r="P140" s="175"/>
+      <c r="Q140" s="175"/>
+      <c r="R140" s="175"/>
+      <c r="S140" s="2"/>
+      <c r="T140" s="2"/>
+      <c r="U140" s="2"/>
+      <c r="V140" s="2"/>
+      <c r="W140" s="2"/>
+      <c r="X140" s="4"/>
       <c r="Y140" s="16"/>
       <c r="Z140" s="1"/>
       <c r="AA140" s="1"/>
       <c r="AB140" s="1"/>
     </row>
-    <row r="141" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
       <c r="B141" s="33"/>
       <c r="C141" s="73">
-        <f>INT($C$74)+2.005</f>
-        <v>3.0049999999999999</v>
+        <f>INT($C$74)+3.005</f>
+        <v>4.0049999999999999</v>
       </c>
       <c r="D141" s="4"/>
       <c r="E141" s="4"/>
@@ -29643,117 +29645,122 @@
       <c r="U141" s="4"/>
       <c r="V141" s="4"/>
       <c r="W141" s="4"/>
-      <c r="X141" s="4"/>
+      <c r="X141" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="Y141" s="16"/>
       <c r="Z141" s="1"/>
       <c r="AA141" s="1"/>
       <c r="AB141" s="1"/>
     </row>
-    <row r="142" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
-      <c r="B142" s="35"/>
-      <c r="C142" s="76">
-        <f>INT($C$74)+1.005</f>
-        <v>2.0049999999999999</v>
-      </c>
-      <c r="D142" s="17"/>
-      <c r="E142" s="17"/>
-      <c r="F142" s="17"/>
-      <c r="G142" s="17"/>
-      <c r="H142" s="17"/>
-      <c r="I142" s="17"/>
-      <c r="J142" s="17"/>
-      <c r="K142" s="17"/>
-      <c r="L142" s="17"/>
-      <c r="M142" s="17"/>
-      <c r="N142" s="17"/>
-      <c r="O142" s="17"/>
-      <c r="P142" s="17"/>
-      <c r="Q142" s="17"/>
-      <c r="R142" s="17"/>
-      <c r="S142" s="17"/>
-      <c r="T142" s="17"/>
-      <c r="U142" s="17"/>
-      <c r="V142" s="17"/>
-      <c r="W142" s="17"/>
-      <c r="X142" s="17"/>
-      <c r="Y142" s="18" t="s">
-        <v>1</v>
-      </c>
+      <c r="B142" s="33"/>
+      <c r="C142" s="73">
+        <f>INT($C$74)+2.005</f>
+        <v>3.0049999999999999</v>
+      </c>
+      <c r="D142" s="4"/>
+      <c r="E142" s="4"/>
+      <c r="F142" s="4"/>
+      <c r="G142" s="4"/>
+      <c r="H142" s="4"/>
+      <c r="I142" s="4"/>
+      <c r="J142" s="4"/>
+      <c r="K142" s="4"/>
+      <c r="L142" s="4"/>
+      <c r="M142" s="4"/>
+      <c r="N142" s="4"/>
+      <c r="O142" s="4"/>
+      <c r="P142" s="4"/>
+      <c r="Q142" s="4"/>
+      <c r="R142" s="4"/>
+      <c r="S142" s="4"/>
+      <c r="T142" s="4"/>
+      <c r="U142" s="4"/>
+      <c r="V142" s="4"/>
+      <c r="W142" s="4"/>
+      <c r="X142" s="4"/>
+      <c r="Y142" s="16"/>
       <c r="Z142" s="1"/>
       <c r="AA142" s="1"/>
       <c r="AB142" s="1"/>
     </row>
-    <row r="143" spans="1:28" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
-      <c r="B143" s="19"/>
-      <c r="C143" s="77">
-        <f>INT($C$74)+0.005</f>
-        <v>1.0049999999999999</v>
-      </c>
-      <c r="D143" s="19"/>
-      <c r="E143" s="19"/>
-      <c r="F143" s="19"/>
-      <c r="G143" s="19"/>
-      <c r="H143" s="19"/>
-      <c r="I143" s="19"/>
-      <c r="J143" s="19"/>
-      <c r="K143" s="19"/>
-      <c r="L143" s="19"/>
-      <c r="M143" s="19"/>
-      <c r="N143" s="19"/>
-      <c r="O143" s="19"/>
-      <c r="P143" s="19"/>
-      <c r="Q143" s="19"/>
-      <c r="R143" s="19"/>
-      <c r="S143" s="19"/>
-      <c r="T143" s="19"/>
-      <c r="U143" s="19"/>
-      <c r="V143" s="19"/>
-      <c r="W143" s="19"/>
-      <c r="X143" s="19"/>
-      <c r="Y143" s="19"/>
+      <c r="B143" s="35"/>
+      <c r="C143" s="76">
+        <f>INT($C$74)+1.005</f>
+        <v>2.0049999999999999</v>
+      </c>
+      <c r="D143" s="17"/>
+      <c r="E143" s="17"/>
+      <c r="F143" s="17"/>
+      <c r="G143" s="17"/>
+      <c r="H143" s="17"/>
+      <c r="I143" s="17"/>
+      <c r="J143" s="17"/>
+      <c r="K143" s="17"/>
+      <c r="L143" s="17"/>
+      <c r="M143" s="17"/>
+      <c r="N143" s="17"/>
+      <c r="O143" s="17"/>
+      <c r="P143" s="17"/>
+      <c r="Q143" s="17"/>
+      <c r="R143" s="17"/>
+      <c r="S143" s="17"/>
+      <c r="T143" s="17"/>
+      <c r="U143" s="17"/>
+      <c r="V143" s="17"/>
+      <c r="W143" s="17"/>
+      <c r="X143" s="17"/>
+      <c r="Y143" s="18" t="s">
+        <v>1</v>
+      </c>
       <c r="Z143" s="1"/>
       <c r="AA143" s="1"/>
       <c r="AB143" s="1"/>
     </row>
-    <row r="144" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:28" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
-      <c r="B144" s="1"/>
-      <c r="C144" s="73">
-        <f>INT($C$74)+2</f>
-        <v>3</v>
-      </c>
-      <c r="D144" s="1"/>
-      <c r="E144" s="1"/>
-      <c r="F144" s="1"/>
-      <c r="G144" s="1"/>
-      <c r="H144" s="1"/>
-      <c r="I144" s="1"/>
-      <c r="J144" s="1"/>
-      <c r="K144" s="1"/>
-      <c r="L144" s="1"/>
-      <c r="M144" s="1"/>
-      <c r="N144" s="1"/>
-      <c r="O144" s="1"/>
-      <c r="P144" s="1"/>
-      <c r="Q144" s="1"/>
-      <c r="R144" s="1"/>
-      <c r="S144" s="1"/>
-      <c r="T144" s="1"/>
-      <c r="U144" s="1"/>
-      <c r="V144" s="1"/>
-      <c r="W144" s="1"/>
-      <c r="X144" s="1"/>
-      <c r="Y144" s="1"/>
+      <c r="B144" s="19"/>
+      <c r="C144" s="77">
+        <f>INT($C$74)+0.005</f>
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="D144" s="19"/>
+      <c r="E144" s="19"/>
+      <c r="F144" s="19"/>
+      <c r="G144" s="19"/>
+      <c r="H144" s="19"/>
+      <c r="I144" s="19"/>
+      <c r="J144" s="19"/>
+      <c r="K144" s="19"/>
+      <c r="L144" s="19"/>
+      <c r="M144" s="19"/>
+      <c r="N144" s="19"/>
+      <c r="O144" s="19"/>
+      <c r="P144" s="19"/>
+      <c r="Q144" s="19"/>
+      <c r="R144" s="19"/>
+      <c r="S144" s="19"/>
+      <c r="T144" s="19"/>
+      <c r="U144" s="19"/>
+      <c r="V144" s="19"/>
+      <c r="W144" s="19"/>
+      <c r="X144" s="19"/>
+      <c r="Y144" s="19"/>
       <c r="Z144" s="1"/>
       <c r="AA144" s="1"/>
       <c r="AB144" s="1"/>
     </row>
-    <row r="145" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
-      <c r="C145" s="66"/>
+      <c r="C145" s="73">
+        <f>INT($C$74)+2</f>
+        <v>3</v>
+      </c>
       <c r="D145" s="1"/>
       <c r="E145" s="1"/>
       <c r="F145" s="1"/>
@@ -29931,7 +29938,37 @@
       <c r="AB150" s="1"/>
     </row>
     <row r="151" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C151" s="72" t="s">
+      <c r="A151" s="1"/>
+      <c r="B151" s="1"/>
+      <c r="C151" s="66"/>
+      <c r="D151" s="1"/>
+      <c r="E151" s="1"/>
+      <c r="F151" s="1"/>
+      <c r="G151" s="1"/>
+      <c r="H151" s="1"/>
+      <c r="I151" s="1"/>
+      <c r="J151" s="1"/>
+      <c r="K151" s="1"/>
+      <c r="L151" s="1"/>
+      <c r="M151" s="1"/>
+      <c r="N151" s="1"/>
+      <c r="O151" s="1"/>
+      <c r="P151" s="1"/>
+      <c r="Q151" s="1"/>
+      <c r="R151" s="1"/>
+      <c r="S151" s="1"/>
+      <c r="T151" s="1"/>
+      <c r="U151" s="1"/>
+      <c r="V151" s="1"/>
+      <c r="W151" s="1"/>
+      <c r="X151" s="1"/>
+      <c r="Y151" s="1"/>
+      <c r="Z151" s="1"/>
+      <c r="AA151" s="1"/>
+      <c r="AB151" s="1"/>
+    </row>
+    <row r="152" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="C152" s="72" t="s">
         <v>4</v>
       </c>
     </row>
@@ -29943,127 +29980,127 @@
   </mergeCells>
   <conditionalFormatting sqref="P107">
     <cfRule type="expression" dxfId="24" priority="33">
-      <formula>(#REF!&gt;=L$343)</formula>
+      <formula>(#REF!&gt;=L$344)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q107 U107">
     <cfRule type="expression" dxfId="23" priority="34">
-      <formula>(#REF!&gt;=L$343)</formula>
+      <formula>(#REF!&gt;=L$344)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R107">
     <cfRule type="expression" dxfId="22" priority="35">
-      <formula>(#REF!&gt;=L$343)</formula>
+      <formula>(#REF!&gt;=L$344)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W107">
     <cfRule type="expression" dxfId="21" priority="36">
-      <formula>(#REF!&gt;=P$343)</formula>
+      <formula>(#REF!&gt;=P$344)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V107">
     <cfRule type="expression" dxfId="20" priority="37">
-      <formula>(#REF!&gt;=P$343)</formula>
+      <formula>(#REF!&gt;=P$344)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P106">
     <cfRule type="expression" dxfId="19" priority="38">
-      <formula>(#REF!&gt;=L$343)</formula>
+      <formula>(#REF!&gt;=L$344)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q106 U105:U106">
     <cfRule type="expression" dxfId="18" priority="39">
-      <formula>(#REF!&gt;=L$343)</formula>
+      <formula>(#REF!&gt;=L$344)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R106">
     <cfRule type="expression" dxfId="17" priority="40">
-      <formula>(#REF!&gt;=L$343)</formula>
+      <formula>(#REF!&gt;=L$344)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W106">
     <cfRule type="expression" dxfId="16" priority="41">
-      <formula>(#REF!&gt;=P$343)</formula>
+      <formula>(#REF!&gt;=P$344)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V106">
     <cfRule type="expression" dxfId="15" priority="42">
-      <formula>(#REF!&gt;=P$343)</formula>
+      <formula>(#REF!&gt;=P$344)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K105">
     <cfRule type="expression" dxfId="14" priority="43">
-      <formula>(#REF!&gt;=J$343)</formula>
+      <formula>(#REF!&gt;=J$344)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M105">
     <cfRule type="expression" dxfId="13" priority="44">
-      <formula>(#REF!&gt;=J$343)</formula>
+      <formula>(#REF!&gt;=J$344)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L105">
     <cfRule type="expression" dxfId="12" priority="45">
-      <formula>(#REF!&gt;=J$343)</formula>
+      <formula>(#REF!&gt;=J$344)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P105">
     <cfRule type="expression" dxfId="11" priority="46">
-      <formula>(#REF!&gt;=L$343)</formula>
+      <formula>(#REF!&gt;=L$344)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q105">
     <cfRule type="expression" dxfId="10" priority="47">
-      <formula>(#REF!&gt;=L$343)</formula>
+      <formula>(#REF!&gt;=L$344)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R105">
     <cfRule type="expression" dxfId="9" priority="48">
-      <formula>(#REF!&gt;=L$343)</formula>
+      <formula>(#REF!&gt;=L$344)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W105">
     <cfRule type="expression" dxfId="8" priority="49">
-      <formula>(#REF!&gt;=P$343)</formula>
+      <formula>(#REF!&gt;=P$344)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V105">
     <cfRule type="expression" dxfId="7" priority="50">
-      <formula>(#REF!&gt;=P$343)</formula>
+      <formula>(#REF!&gt;=P$344)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O107">
     <cfRule type="expression" dxfId="6" priority="29">
-      <formula>(#REF!&gt;=K$343)</formula>
+      <formula>(#REF!&gt;=K$344)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O106">
     <cfRule type="expression" dxfId="5" priority="30">
-      <formula>(#REF!&gt;=K$343)</formula>
+      <formula>(#REF!&gt;=K$344)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O105">
     <cfRule type="expression" dxfId="4" priority="31">
-      <formula>(#REF!&gt;=K$343)</formula>
+      <formula>(#REF!&gt;=K$344)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T107">
     <cfRule type="expression" dxfId="3" priority="26">
-      <formula>(#REF!&gt;=P$343)</formula>
+      <formula>(#REF!&gt;=P$344)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T106">
     <cfRule type="expression" dxfId="2" priority="27">
-      <formula>(#REF!&gt;=P$343)</formula>
+      <formula>(#REF!&gt;=P$344)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T105">
     <cfRule type="expression" dxfId="1" priority="28">
-      <formula>(#REF!&gt;=P$343)</formula>
+      <formula>(#REF!&gt;=P$344)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I105:J107 I103:I104 K106:M107">
     <cfRule type="expression" dxfId="0" priority="56">
-      <formula>($E103&gt;=I$343)</formula>
+      <formula>($E103&gt;=I$344)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Altered the standard feed supply in Property Formatting in Universal & Structure
</commit_message>
<xml_diff>
--- a/Structural.xlsx
+++ b/Structural.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF6A3C3-28B9-47E2-A60F-17E398A2EEEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D915166-F6EA-4EB9-9441-6442060FC70A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -157,14 +157,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -2544,14 +2536,6 @@
 1: 1Apr19-Created the version control table</t>
   </si>
   <si>
-    <t>27Apr21: add named ranges to inputs copied from pinp.
-                   Add REV inputs
-                    Split fvp inputs
-25Apr21: Moved inputs from Property.xlsx
-                   Moved FVP &amp; N inputs from Stock
-1: 1Apr19-Created the version control table</t>
-  </si>
-  <si>
     <t>Graz50</t>
   </si>
   <si>
@@ -2560,6 +2544,15 @@
   </si>
   <si>
     <t>lwc</t>
+  </si>
+  <si>
+    <t>29Apr21: Added the fixed DVPs to the formula for the number of dam FVPs
+27Apr21: add named ranges to inputs copied from pinp.
+                   Add REV inputs
+                    Split fvp inputs
+25Apr21: Moved inputs from Property.xlsx
+                   Moved FVP &amp; N inputs from Stock
+1: 1Apr19-Created the version control table</t>
   </si>
 </sst>
 </file>
@@ -5918,7 +5911,7 @@
         <v>1</v>
       </c>
       <c r="J21" s="188" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K21" s="189"/>
       <c r="L21" s="189"/>
@@ -7242,7 +7235,7 @@
         <v>209</v>
       </c>
       <c r="K58" s="101" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="L58" s="101" t="s">
         <v>210</v>
@@ -8224,8 +8217,11 @@
   </sheetPr>
   <dimension ref="A1:AE343"/>
   <sheetViews>
-    <sheetView topLeftCell="B314" workbookViewId="0">
-      <selection activeCell="B330" sqref="A330:XFD334"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="8" ySplit="33" topLeftCell="I34" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
+      <selection pane="bottomRight" activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -8446,7 +8442,7 @@
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
     </row>
-    <row r="6" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="20.100000000000001" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="33"/>
       <c r="C6" s="67">
@@ -8484,7 +8480,7 @@
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
     </row>
-    <row r="7" spans="1:28" ht="20.100000000000001" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="33"/>
       <c r="C7" s="67">
@@ -8793,7 +8789,7 @@
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
     </row>
-    <row r="16" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="33" t="s">
         <v>19</v>
@@ -8830,7 +8826,7 @@
       <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>
     </row>
-    <row r="17" spans="1:28" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="33"/>
       <c r="C17" s="67">
@@ -8865,7 +8861,7 @@
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
     </row>
-    <row r="18" spans="1:28" ht="45" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" ht="45" hidden="1" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="33"/>
       <c r="C18" s="67">
@@ -8970,7 +8966,7 @@
       <c r="AA20" s="1"/>
       <c r="AB20" s="1"/>
     </row>
-    <row r="21" spans="1:28" ht="45" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" ht="45" hidden="1" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="33"/>
       <c r="C21" s="67">
@@ -9408,7 +9404,7 @@
       <c r="AA32" s="1"/>
       <c r="AB32" s="1"/>
     </row>
-    <row r="33" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="35"/>
       <c r="C33" s="70">
@@ -24349,13 +24345,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC76D6D2-A3AB-40A8-BB6F-FAC5176C31EB}">
-  <sheetPr>
+  <sheetPr codeName="Sheet3">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:AB152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="H138" sqref="H138"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="8" ySplit="33" topLeftCell="I34" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
+      <selection pane="bottomRight" activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -24376,7 +24375,7 @@
     <col min="29" max="16384" width="8.7109375" style="142"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="66"/>
@@ -24406,7 +24405,7 @@
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
     </row>
-    <row r="2" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="67">
@@ -24616,7 +24615,7 @@
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
     </row>
-    <row r="7" spans="1:28" ht="20.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" ht="20.100000000000001" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="33"/>
       <c r="C7" s="67">
@@ -24655,7 +24654,7 @@
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
     </row>
-    <row r="8" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="33"/>
       <c r="C8" s="67">
@@ -24688,7 +24687,7 @@
       <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
     </row>
-    <row r="9" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="33"/>
       <c r="C9" s="67">
@@ -24721,7 +24720,7 @@
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
     </row>
-    <row r="10" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="33"/>
       <c r="C10" s="67">
@@ -24754,7 +24753,7 @@
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
     </row>
-    <row r="11" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="33"/>
       <c r="C11" s="67">
@@ -24787,7 +24786,7 @@
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
     </row>
-    <row r="12" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="33"/>
       <c r="C12" s="67">
@@ -24824,7 +24823,7 @@
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
     </row>
-    <row r="13" spans="1:28" ht="11.45" customHeight="1" outlineLevel="3" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" ht="11.45" hidden="1" customHeight="1" outlineLevel="3" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="33" t="s">
         <v>20</v>
@@ -25012,10 +25011,10 @@
         <v>16</v>
       </c>
       <c r="I18" s="151">
-        <v>44311.763956365699</v>
+        <v>44315.6845902778</v>
       </c>
       <c r="J18" s="185" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="K18" s="186"/>
       <c r="L18" s="186"/>
@@ -25849,7 +25848,7 @@
       <c r="AA41" s="1"/>
       <c r="AB41" s="1"/>
     </row>
-    <row r="42" spans="1:28" s="97" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:28" s="97" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="33"/>
       <c r="C42" s="73">
@@ -25882,7 +25881,7 @@
       <c r="AA42" s="1"/>
       <c r="AB42" s="1"/>
     </row>
-    <row r="43" spans="1:28" s="97" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:28" s="97" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="33"/>
       <c r="C43" s="73">
@@ -25915,7 +25914,7 @@
       <c r="AA43" s="1"/>
       <c r="AB43" s="1"/>
     </row>
-    <row r="44" spans="1:28" s="97" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:28" s="97" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="33"/>
       <c r="C44" s="73">
@@ -26815,7 +26814,7 @@
       <c r="AA67" s="1"/>
       <c r="AB67" s="1"/>
     </row>
-    <row r="68" spans="1:28" s="131" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:28" s="131" customFormat="1" ht="5.0999999999999996" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="19"/>
       <c r="C68" s="77">
@@ -26848,7 +26847,7 @@
       <c r="AA68" s="1"/>
       <c r="AB68" s="1"/>
     </row>
-    <row r="69" spans="1:28" s="131" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:28" s="131" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="73">
@@ -26881,7 +26880,7 @@
       <c r="AA69" s="1"/>
       <c r="AB69" s="1"/>
     </row>
-    <row r="70" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:28" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="73">
@@ -27089,7 +27088,7 @@
       <c r="AA75" s="1"/>
       <c r="AB75" s="1"/>
     </row>
-    <row r="76" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="33"/>
       <c r="C76" s="73">
@@ -27122,7 +27121,7 @@
       <c r="AA76" s="1"/>
       <c r="AB76" s="1"/>
     </row>
-    <row r="77" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="33"/>
       <c r="C77" s="73">
@@ -27155,7 +27154,7 @@
       <c r="AA77" s="1"/>
       <c r="AB77" s="1"/>
     </row>
-    <row r="78" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="33"/>
       <c r="C78" s="73">
@@ -27443,7 +27442,7 @@
       <c r="K85" s="2"/>
       <c r="L85" s="121">
         <f>i_w_start_len1*i_n1_len^L88</f>
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="M85" s="2"/>
       <c r="N85" s="116" t="s">
@@ -27574,8 +27573,8 @@
       </c>
       <c r="K88" s="2"/>
       <c r="L88" s="121">
-        <f>COUNTIF(J52:O52,TRUE)</f>
-        <v>0</v>
+        <f>COUNTIF(i_fixed_fvp_mask_dams,TRUE)+COUNTIF(i_fvp_mask_dams,TRUE)</f>
+        <v>3</v>
       </c>
       <c r="M88" s="2"/>
       <c r="N88" s="2"/>
@@ -28586,7 +28585,7 @@
       <c r="AA111" s="1"/>
       <c r="AB111" s="1"/>
     </row>
-    <row r="112" spans="1:28" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:28" ht="5.0999999999999996" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="19"/>
       <c r="C112" s="77">
@@ -28619,7 +28618,7 @@
       <c r="AA112" s="1"/>
       <c r="AB112" s="1"/>
     </row>
-    <row r="113" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:28" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="73">
@@ -28652,7 +28651,7 @@
       <c r="AA113" s="1"/>
       <c r="AB113" s="1"/>
     </row>
-    <row r="114" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:28" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="73">
@@ -29139,7 +29138,7 @@
       <c r="AA127" s="1"/>
       <c r="AB127" s="1"/>
     </row>
-    <row r="128" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:28" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
       <c r="B128" s="33"/>
       <c r="C128" s="73"/>
@@ -29173,7 +29172,7 @@
       <c r="AA128" s="1"/>
       <c r="AB128" s="1"/>
     </row>
-    <row r="129" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
       <c r="B129" s="33"/>
       <c r="C129" s="73">
@@ -29523,7 +29522,7 @@
       <c r="F138" s="5"/>
       <c r="G138" s="4"/>
       <c r="H138" s="31" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I138" s="31" t="b">
         <v>0</v>
@@ -29721,7 +29720,7 @@
       <c r="AA143" s="1"/>
       <c r="AB143" s="1"/>
     </row>
-    <row r="144" spans="1:28" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:28" ht="5.0999999999999996" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
       <c r="B144" s="19"/>
       <c r="C144" s="77">
@@ -29754,7 +29753,7 @@
       <c r="AA144" s="1"/>
       <c r="AB144" s="1"/>
     </row>
-    <row r="145" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:28" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="73">

</xml_diff>

<commit_message>
Alter extra FVP date (for GEPEP calibration)
</commit_message>
<xml_diff>
--- a/Structural.xlsx
+++ b/Structural.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{447D11BE-40DD-43B3-AC3F-F08AD28901D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03DA4106-41F4-4892-A12B-3BDE1A21D366}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -157,14 +157,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -378,7 +370,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Michael Young (21512438):</t>
         </r>
@@ -387,7 +379,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 confinement must be last</t>
@@ -754,7 +746,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>John:</t>
         </r>
@@ -763,7 +755,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 This table is only used for the feed supply only.
@@ -1227,7 +1219,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O55" authorId="1" shapeId="0" xr:uid="{03367603-CB1F-4742-BCDF-5211165287E6}">
+    <comment ref="O55" authorId="1" shapeId="0" xr:uid="{ADB63854-4700-4EFC-9C28-7DD675173D98}">
       <text>
         <r>
           <rPr>
@@ -1331,7 +1323,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Michael Young (21512438):</t>
         </r>
@@ -1340,7 +1332,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 DVP when condensing happens. For offs this can be any dvp.</t>
@@ -1529,7 +1521,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Michael Young (21512438):</t>
         </r>
@@ -1538,7 +1530,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 These can be controlled using SAV. When true these traits will be updated with the values from the std trial.</t>
@@ -1574,7 +1566,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="317">
   <si>
     <t>Controls for this worksheet</t>
   </si>
@@ -2557,7 +2549,8 @@
     <t>random</t>
   </si>
   <si>
-    <t>4May21: add random rev
+    <t>5May21: Adjust the extra FVP date for TOL[0] (for GEPEP calibration)
+4May21: add random rev
 29Apr21: Added the fixed DVPs to the formula for the number of dam FVPs
 27Apr21: add named ranges to inputs copied from pinp.
                    Add REV inputs
@@ -2565,6 +2558,12 @@
 25Apr21: Moved inputs from Property.xlsx
                    Moved FVP &amp; N inputs from Stock
 1: 1Apr19-Created the version control table</t>
+  </si>
+  <si>
+    <t>User defined FVP date - TOL[0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                   - TOL[1]</t>
   </si>
 </sst>
 </file>
@@ -2574,7 +2573,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2765,19 +2764,6 @@
       <color rgb="FF0000FF"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="35">
@@ -24363,10 +24349,10 @@
   <dimension ref="A1:AB153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="8" ySplit="33" topLeftCell="I88" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="33" topLeftCell="I34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
-      <selection pane="bottomRight" activeCell="J18" sqref="J18:T18"/>
+      <selection pane="bottomRight" activeCell="O55" sqref="O55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -25023,7 +25009,7 @@
         <v>16</v>
       </c>
       <c r="I18" s="151">
-        <v>44315.6845902778</v>
+        <v>44321.657764930598</v>
       </c>
       <c r="J18" s="185" t="s">
         <v>314</v>
@@ -26357,7 +26343,7 @@
       <c r="F55" s="5"/>
       <c r="G55" s="4"/>
       <c r="H55" s="2" t="s">
-        <v>244</v>
+        <v>315</v>
       </c>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
@@ -26366,7 +26352,7 @@
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
       <c r="O55" s="146">
-        <v>43755</v>
+        <v>43748</v>
       </c>
       <c r="P55" s="2"/>
       <c r="Q55" s="2"/>
@@ -26393,7 +26379,9 @@
       <c r="E56" s="5"/>
       <c r="F56" s="5"/>
       <c r="G56" s="4"/>
-      <c r="H56" s="2"/>
+      <c r="H56" s="2" t="s">
+        <v>316</v>
+      </c>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>

</xml_diff>

<commit_message>
Increase dams to N8 (F3N8 is same size as F4N5)
</commit_message>
<xml_diff>
--- a/Structural.xlsx
+++ b/Structural.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{258D0C3D-D58E-47E5-AD8F-A92DD33E11DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC83C702-EAB0-491E-B3EF-EA76562EC677}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="75" yWindow="1065" windowWidth="27870" windowHeight="15135" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27975" windowHeight="16440" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -54,7 +54,7 @@
     <definedName name="i_d_pos">Stock!$I$56</definedName>
     <definedName name="i_date_assetvalue" localSheetId="0">General!$I$68</definedName>
     <definedName name="i_density_n0" localSheetId="2">StructuralSA!$K$94</definedName>
-    <definedName name="i_density_n1" localSheetId="2">StructuralSA!$M$94:$M$100</definedName>
+    <definedName name="i_density_n1" localSheetId="2">StructuralSA!$M$94:$M$101</definedName>
     <definedName name="i_density_n3" localSheetId="2">StructuralSA!$Q$94:$Q$101</definedName>
     <definedName name="i_dvp_mask_f1">StructuralSA!$M$53:$O$53</definedName>
     <definedName name="i_dvp_mask_f3">StructuralSA!$J$63:$M$63</definedName>
@@ -104,7 +104,7 @@
     <definedName name="i_n3_matrix_len">StructuralSA!$P$90</definedName>
     <definedName name="i_numbers_min_b1">Stock!$L$164:$V$164</definedName>
     <definedName name="i_nut_spread_n0" localSheetId="2">StructuralSA!$J$94</definedName>
-    <definedName name="i_nut_spread_n1" localSheetId="2">StructuralSA!$L$94:$L$100</definedName>
+    <definedName name="i_nut_spread_n1" localSheetId="2">StructuralSA!$L$94:$L$101</definedName>
     <definedName name="i_nut_spread_n3" localSheetId="2">StructuralSA!$P$94:$P$101</definedName>
     <definedName name="i_p_pos">Stock!$I$64</definedName>
     <definedName name="i_prejoin_offset">Stock!$I$74</definedName>
@@ -151,7 +151,6 @@
     <definedName name="ZA.ZoomSheet" localSheetId="3">Admin!$O$26</definedName>
   </definedNames>
   <calcPr calcId="191029" refMode="R1C1"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1695,9 +1694,6 @@
     <t>1: 2Apr19-Standards &amp; Cell styles</t>
   </si>
   <si>
-    <t>1: 1Apr19-Blank worksheet</t>
-  </si>
-  <si>
     <t>Number</t>
   </si>
   <si>
@@ -2561,18 +2557,6 @@
     <t xml:space="preserve">                                   - TOL[2]</t>
   </si>
   <si>
-    <t>16May21: Add extra TOL to the extra FVP date
-5May21: Adjust the extra FVP date for TOL[0] (for GEPEP calibration)
-4May21: add random rev
-29Apr21: Added the fixed DVPs to the formula for the number of dam FVPs
-27Apr21: add named ranges to inputs copied from pinp.
-                   Add REV inputs
-                    Split fvp inputs
-25Apr21: Moved inputs from Property.xlsx
-                   Moved FVP &amp; N inputs from Stock
-1: 1Apr19-Created the version control table</t>
-  </si>
-  <si>
     <t>FVP type</t>
   </si>
   <si>
@@ -2587,6 +2571,23 @@
 31Mar21: Change the index for the k2 cluster (for the seasonality model)
 29Mar21: Changed to FVP3, 1N for dams, 3N for Offs
 22Mar21: Alter the initial weight &amp; wool spread for the weaners
+1: 1Apr19-Blank worksheet</t>
+  </si>
+  <si>
+    <t>20May21: Add extra N for dams (now 8)
+16May21: Add extra TOL to the extra FVP date
+5May21: Adjust the extra FVP date for TOL[0] (for GEPEP calibration)
+4May21: add random rev
+29Apr21: Added the fixed DVPs to the formula for the number of dam FVPs
+27Apr21: add named ranges to inputs copied from pinp.
+                   Add REV inputs
+                    Split fvp inputs
+25Apr21: Moved inputs from Property.xlsx
+                   Moved FVP &amp; N inputs from Stock
+1: 1Apr19-Created the version control table</t>
+  </si>
+  <si>
+    <t>20May21: Make the extra nut_spread_g1 = 0.1
 1: 1Apr19-Blank worksheet</t>
   </si>
 </sst>
@@ -5406,7 +5407,7 @@
       </c>
       <c r="G6" s="12"/>
       <c r="H6" s="44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
@@ -5613,7 +5614,7 @@
       <c r="G12" s="3"/>
       <c r="H12" s="29"/>
       <c r="I12" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J12" s="29" t="s">
         <v>5</v>
@@ -5787,7 +5788,7 @@
       <c r="F17" s="5"/>
       <c r="G17" s="4"/>
       <c r="H17" s="50" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -5828,7 +5829,7 @@
         <v>2</v>
       </c>
       <c r="J18" s="185" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K18" s="186"/>
       <c r="L18" s="186"/>
@@ -5933,7 +5934,7 @@
         <v>1</v>
       </c>
       <c r="J21" s="188" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="K21" s="189"/>
       <c r="L21" s="189"/>
@@ -6641,7 +6642,7 @@
       </c>
       <c r="G41" s="13"/>
       <c r="H41" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I41" s="7"/>
       <c r="J41" s="7"/>
@@ -6907,7 +6908,7 @@
         <v>4</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
@@ -6981,16 +6982,16 @@
       <c r="F51" s="5"/>
       <c r="G51" s="4"/>
       <c r="H51" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="I51" s="101" t="s">
         <v>191</v>
       </c>
-      <c r="I51" s="101" t="s">
+      <c r="J51" s="101" t="s">
         <v>192</v>
       </c>
-      <c r="J51" s="101" t="s">
+      <c r="K51" s="101" t="s">
         <v>193</v>
-      </c>
-      <c r="K51" s="101" t="s">
-        <v>194</v>
       </c>
       <c r="L51" s="144"/>
       <c r="M51" s="2"/>
@@ -7055,13 +7056,13 @@
       <c r="F53" s="5"/>
       <c r="G53" s="4"/>
       <c r="H53" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="I53" s="101" t="s">
         <v>195</v>
       </c>
-      <c r="I53" s="101" t="s">
+      <c r="J53" s="101" t="s">
         <v>196</v>
-      </c>
-      <c r="J53" s="101" t="s">
-        <v>197</v>
       </c>
       <c r="K53" s="144"/>
       <c r="L53" s="144"/>
@@ -7127,16 +7128,16 @@
       <c r="F55" s="5"/>
       <c r="G55" s="4"/>
       <c r="H55" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I55" s="101" t="s">
+        <v>202</v>
+      </c>
+      <c r="J55" s="101" t="s">
         <v>203</v>
       </c>
-      <c r="J55" s="101" t="s">
+      <c r="K55" s="101" t="s">
         <v>204</v>
-      </c>
-      <c r="K55" s="101" t="s">
-        <v>205</v>
       </c>
       <c r="L55" s="144"/>
       <c r="M55" s="2"/>
@@ -7168,7 +7169,7 @@
       <c r="F56" s="5"/>
       <c r="G56" s="4"/>
       <c r="H56" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I56" s="101" t="b">
         <v>1</v>
@@ -7209,13 +7210,13 @@
       <c r="F57" s="5"/>
       <c r="G57" s="4"/>
       <c r="H57" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I57" s="101" t="s">
+        <v>205</v>
+      </c>
+      <c r="J57" s="101" t="s">
         <v>206</v>
-      </c>
-      <c r="J57" s="101" t="s">
-        <v>207</v>
       </c>
       <c r="K57" s="144"/>
       <c r="L57" s="144"/>
@@ -7248,19 +7249,19 @@
       <c r="F58" s="5"/>
       <c r="G58" s="4"/>
       <c r="H58" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I58" s="101" t="s">
+        <v>207</v>
+      </c>
+      <c r="J58" s="101" t="s">
         <v>208</v>
       </c>
-      <c r="J58" s="101" t="s">
+      <c r="K58" s="101" t="s">
+        <v>306</v>
+      </c>
+      <c r="L58" s="101" t="s">
         <v>209</v>
-      </c>
-      <c r="K58" s="101" t="s">
-        <v>307</v>
-      </c>
-      <c r="L58" s="101" t="s">
-        <v>210</v>
       </c>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
@@ -7291,16 +7292,16 @@
       <c r="F59" s="5"/>
       <c r="G59" s="4"/>
       <c r="H59" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I59" s="101" t="s">
+        <v>210</v>
+      </c>
+      <c r="J59" s="101" t="s">
         <v>211</v>
       </c>
-      <c r="J59" s="101" t="s">
+      <c r="K59" s="101" t="s">
         <v>212</v>
-      </c>
-      <c r="K59" s="101" t="s">
-        <v>213</v>
       </c>
       <c r="L59" s="144"/>
       <c r="M59" s="2"/>
@@ -7365,22 +7366,22 @@
       <c r="F61" s="5"/>
       <c r="G61" s="4"/>
       <c r="H61" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I61" s="101" t="s">
+        <v>255</v>
+      </c>
+      <c r="J61" s="101" t="s">
         <v>256</v>
       </c>
-      <c r="J61" s="101" t="s">
+      <c r="K61" s="101" t="s">
         <v>257</v>
       </c>
-      <c r="K61" s="101" t="s">
+      <c r="L61" s="101" t="s">
         <v>258</v>
       </c>
-      <c r="L61" s="101" t="s">
-        <v>259</v>
-      </c>
       <c r="M61" s="101" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="N61" s="2"/>
       <c r="O61" s="2"/>
@@ -7407,7 +7408,7 @@
       <c r="F62" s="5"/>
       <c r="G62" s="4"/>
       <c r="H62" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I62" s="101" t="b">
         <v>1</v>
@@ -7485,7 +7486,7 @@
       <c r="F64" s="5"/>
       <c r="G64" s="4"/>
       <c r="H64" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I64" s="101">
         <v>6</v>
@@ -7555,7 +7556,7 @@
       <c r="F66" s="5"/>
       <c r="G66" s="4"/>
       <c r="H66" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I66" s="101">
         <v>1</v>
@@ -7625,14 +7626,14 @@
       <c r="F68" s="5"/>
       <c r="G68" s="4"/>
       <c r="H68" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I68" s="140">
         <v>43466</v>
       </c>
       <c r="J68" s="2"/>
       <c r="K68" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L68" s="2"/>
       <c r="M68" s="2"/>
@@ -7681,25 +7682,25 @@
       <c r="F69" s="5"/>
       <c r="G69" s="4"/>
       <c r="H69" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="I69" s="140" t="s">
         <v>184</v>
       </c>
-      <c r="I69" s="140" t="s">
+      <c r="J69" s="140" t="s">
         <v>185</v>
       </c>
-      <c r="J69" s="140" t="s">
+      <c r="K69" s="140" t="s">
         <v>186</v>
       </c>
-      <c r="K69" s="140" t="s">
+      <c r="L69" s="140" t="s">
         <v>187</v>
       </c>
-      <c r="L69" s="140" t="s">
+      <c r="M69" s="140" t="s">
         <v>188</v>
       </c>
-      <c r="M69" s="140" t="s">
+      <c r="N69" s="140" t="s">
         <v>189</v>
-      </c>
-      <c r="N69" s="140" t="s">
-        <v>190</v>
       </c>
       <c r="O69" s="2"/>
       <c r="P69" s="2"/>
@@ -8479,7 +8480,7 @@
       </c>
       <c r="G6" s="12"/>
       <c r="H6" s="44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
@@ -8686,7 +8687,7 @@
       <c r="G12" s="3"/>
       <c r="H12" s="29"/>
       <c r="I12" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J12" s="29" t="s">
         <v>5</v>
@@ -8860,7 +8861,7 @@
       <c r="F17" s="5"/>
       <c r="G17" s="4"/>
       <c r="H17" s="50" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -8901,7 +8902,7 @@
         <v>44311.756953009302</v>
       </c>
       <c r="J18" s="185" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="K18" s="186"/>
       <c r="L18" s="186"/>
@@ -9006,7 +9007,7 @@
         <v>44332.897875578703</v>
       </c>
       <c r="J21" s="188" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="K21" s="189"/>
       <c r="L21" s="189"/>
@@ -9880,21 +9881,21 @@
       <c r="G46" s="3"/>
       <c r="H46" s="29"/>
       <c r="I46" s="29" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J46" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K46" s="29"/>
       <c r="L46" s="29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M46" s="29"/>
       <c r="N46" s="29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O46" s="29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P46" s="29"/>
       <c r="Q46" s="29"/>
@@ -9988,7 +9989,7 @@
         <v>5</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
@@ -10062,7 +10063,7 @@
       <c r="F51" s="5"/>
       <c r="G51" s="4"/>
       <c r="H51" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
@@ -10097,7 +10098,7 @@
       <c r="F52" s="5"/>
       <c r="G52" s="4"/>
       <c r="H52" s="36" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I52" s="31">
         <v>-6</v>
@@ -10134,7 +10135,7 @@
       <c r="F53" s="5"/>
       <c r="G53" s="4"/>
       <c r="H53" s="36" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I53" s="31">
         <v>-14</v>
@@ -10171,7 +10172,7 @@
       <c r="F54" s="5"/>
       <c r="G54" s="4"/>
       <c r="H54" s="36" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I54" s="31">
         <v>-4</v>
@@ -10208,7 +10209,7 @@
       <c r="F55" s="5"/>
       <c r="G55" s="4"/>
       <c r="H55" s="36" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I55" s="31">
         <v>-12</v>
@@ -10245,7 +10246,7 @@
       <c r="F56" s="5"/>
       <c r="G56" s="4"/>
       <c r="H56" s="36" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I56" s="31">
         <v>-7</v>
@@ -10282,7 +10283,7 @@
       <c r="F57" s="5"/>
       <c r="G57" s="4"/>
       <c r="H57" s="133" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I57" s="31">
         <v>-5</v>
@@ -10319,7 +10320,7 @@
       <c r="F58" s="5"/>
       <c r="G58" s="4"/>
       <c r="H58" s="133" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I58" s="31">
         <v>-13</v>
@@ -10356,7 +10357,7 @@
       <c r="F59" s="5"/>
       <c r="G59" s="4"/>
       <c r="H59" s="36" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I59" s="31">
         <v>-8</v>
@@ -10393,7 +10394,7 @@
       <c r="F60" s="5"/>
       <c r="G60" s="4"/>
       <c r="H60" s="133" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I60" s="31">
         <v>-17</v>
@@ -10430,7 +10431,7 @@
       <c r="F61" s="5"/>
       <c r="G61" s="4"/>
       <c r="H61" s="133" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I61" s="31">
         <v>-18</v>
@@ -10467,7 +10468,7 @@
       <c r="F62" s="5"/>
       <c r="G62" s="4"/>
       <c r="H62" s="133" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I62" s="31">
         <v>-17</v>
@@ -10504,7 +10505,7 @@
       <c r="F63" s="5"/>
       <c r="G63" s="4"/>
       <c r="H63" s="133" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I63" s="31">
         <v>-11</v>
@@ -10541,7 +10542,7 @@
       <c r="F64" s="5"/>
       <c r="G64" s="4"/>
       <c r="H64" s="133" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I64" s="31">
         <v>-15</v>
@@ -10578,13 +10579,13 @@
       <c r="F65" s="5"/>
       <c r="G65" s="4"/>
       <c r="H65" s="133" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I65" s="31">
         <v>-10</v>
       </c>
       <c r="J65" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
@@ -10617,7 +10618,7 @@
       <c r="F66" s="5"/>
       <c r="G66" s="4"/>
       <c r="H66" s="133" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I66" s="31">
         <v>-3</v>
@@ -10654,7 +10655,7 @@
       <c r="F67" s="5"/>
       <c r="G67" s="4"/>
       <c r="H67" s="133" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I67" s="31">
         <v>-2</v>
@@ -10691,7 +10692,7 @@
       <c r="F68" s="5"/>
       <c r="G68" s="4"/>
       <c r="H68" s="133" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I68" s="31">
         <v>-9</v>
@@ -10761,7 +10762,7 @@
       <c r="F70" s="5"/>
       <c r="G70" s="4"/>
       <c r="H70" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I70" s="31">
         <v>52</v>
@@ -10798,16 +10799,16 @@
       <c r="F71" s="5"/>
       <c r="G71" s="4"/>
       <c r="H71" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I71" s="31">
         <v>7.25</v>
       </c>
       <c r="J71" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="L71" s="2"/>
       <c r="M71" s="2"/>
@@ -10839,16 +10840,16 @@
       <c r="F72" s="5"/>
       <c r="G72" s="4"/>
       <c r="H72" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I72" s="31">
         <v>4.25</v>
       </c>
       <c r="J72" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="L72" s="2"/>
       <c r="M72" s="2"/>
@@ -10913,13 +10914,13 @@
       <c r="F74" s="5"/>
       <c r="G74" s="4"/>
       <c r="H74" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I74" s="31">
         <v>8</v>
       </c>
       <c r="J74" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K74" s="2"/>
       <c r="L74" s="2"/>
@@ -10985,7 +10986,7 @@
       <c r="F76" s="5"/>
       <c r="G76" s="4"/>
       <c r="H76" s="53" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I76" s="53"/>
       <c r="J76" s="2"/>
@@ -11020,16 +11021,16 @@
       <c r="F77" s="5"/>
       <c r="G77" s="4"/>
       <c r="H77" s="98" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I77" s="31">
         <v>1</v>
       </c>
       <c r="J77" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L77" s="2"/>
       <c r="M77" s="2"/>
@@ -11061,16 +11062,16 @@
       <c r="F78" s="5"/>
       <c r="G78" s="4"/>
       <c r="H78" s="98" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I78" s="31">
         <v>1</v>
       </c>
       <c r="J78" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K78" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L78" s="2"/>
       <c r="M78" s="2"/>
@@ -11135,7 +11136,7 @@
       <c r="F80" s="5"/>
       <c r="G80" s="4"/>
       <c r="H80" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I80" s="31">
         <v>10</v>
@@ -11683,17 +11684,17 @@
       <c r="H96" s="29"/>
       <c r="I96" s="29"/>
       <c r="J96" s="29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K96" s="65" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L96" s="65"/>
       <c r="M96" s="65"/>
       <c r="N96" s="65"/>
       <c r="O96" s="29"/>
       <c r="P96" s="65" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q96" s="65"/>
       <c r="R96" s="65"/>
@@ -11722,29 +11723,29 @@
       <c r="H97" s="29"/>
       <c r="I97" s="29"/>
       <c r="J97" s="29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K97" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="L97" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="L97" s="29" t="s">
+      <c r="M97" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="M97" s="29" t="s">
-        <v>73</v>
-      </c>
       <c r="N97" s="29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="O97" s="29"/>
       <c r="P97" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q97" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="Q97" s="29" t="s">
+      <c r="R97" s="29" t="s">
         <v>43</v>
-      </c>
-      <c r="R97" s="29" t="s">
-        <v>44</v>
       </c>
       <c r="S97" s="29"/>
       <c r="T97" s="29"/>
@@ -11835,7 +11836,7 @@
         <v>5</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E100" s="5"/>
       <c r="F100" s="5"/>
@@ -11909,13 +11910,13 @@
       <c r="F102" s="5"/>
       <c r="G102" s="4"/>
       <c r="H102" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I102" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J102" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K102" s="31" t="b">
         <v>1</v>
@@ -11962,11 +11963,11 @@
       <c r="F103" s="5"/>
       <c r="G103" s="4"/>
       <c r="H103" s="116" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I103" s="2"/>
       <c r="J103" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K103" s="31" t="b">
         <v>0</v>
@@ -12013,11 +12014,11 @@
       <c r="F104" s="5"/>
       <c r="G104" s="4"/>
       <c r="H104" s="116" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I104" s="2"/>
       <c r="J104" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K104" s="31" t="b">
         <v>0</v>
@@ -12098,10 +12099,10 @@
       <c r="G106" s="4"/>
       <c r="H106" s="2"/>
       <c r="I106" s="26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J106" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K106" s="31" t="b">
         <v>1</v>
@@ -12150,7 +12151,7 @@
       <c r="H107" s="2"/>
       <c r="I107" s="2"/>
       <c r="J107" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K107" s="31" t="b">
         <v>0</v>
@@ -12199,7 +12200,7 @@
       <c r="H108" s="2"/>
       <c r="I108" s="2"/>
       <c r="J108" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K108" s="31" t="b">
         <v>0</v>
@@ -12248,7 +12249,7 @@
       <c r="H109" s="2"/>
       <c r="I109" s="2"/>
       <c r="J109" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K109" s="31" t="b">
         <v>0</v>
@@ -12329,10 +12330,10 @@
       <c r="G111" s="4"/>
       <c r="H111" s="2"/>
       <c r="I111" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J111" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K111" s="31" t="b">
         <v>1</v>
@@ -12381,7 +12382,7 @@
       <c r="H112" s="2"/>
       <c r="I112" s="2"/>
       <c r="J112" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K112" s="31" t="b">
         <v>0</v>
@@ -12430,7 +12431,7 @@
       <c r="H113" s="2"/>
       <c r="I113" s="2"/>
       <c r="J113" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K113" s="31" t="b">
         <v>0</v>
@@ -12479,7 +12480,7 @@
       <c r="H114" s="2"/>
       <c r="I114" s="2"/>
       <c r="J114" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K114" s="31" t="b">
         <v>0</v>
@@ -12560,10 +12561,10 @@
       <c r="G116" s="4"/>
       <c r="H116" s="2"/>
       <c r="I116" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J116" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K116" s="31" t="b">
         <v>1</v>
@@ -12612,7 +12613,7 @@
       <c r="H117" s="2"/>
       <c r="I117" s="2"/>
       <c r="J117" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K117" s="31" t="b">
         <v>0</v>
@@ -12661,7 +12662,7 @@
       <c r="H118" s="2"/>
       <c r="I118" s="2"/>
       <c r="J118" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K118" s="31" t="b">
         <v>0</v>
@@ -12710,7 +12711,7 @@
       <c r="H119" s="2"/>
       <c r="I119" s="2"/>
       <c r="J119" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K119" s="31" t="b">
         <v>0</v>
@@ -12793,7 +12794,7 @@
       <c r="I121" s="2"/>
       <c r="J121" s="2"/>
       <c r="K121" s="52" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L121" s="52"/>
       <c r="M121" s="52"/>
@@ -12828,16 +12829,16 @@
       <c r="I122" s="2"/>
       <c r="J122" s="2"/>
       <c r="K122" s="36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L122" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="M122" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="M122" s="36" t="s">
+      <c r="N122" s="36" t="s">
         <v>39</v>
-      </c>
-      <c r="N122" s="36" t="s">
-        <v>40</v>
       </c>
       <c r="O122" s="2"/>
       <c r="P122" s="2"/>
@@ -12866,13 +12867,13 @@
       <c r="F123" s="5"/>
       <c r="G123" s="4"/>
       <c r="H123" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I123" s="26" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J123" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K123" s="31">
         <v>0</v>
@@ -12914,11 +12915,11 @@
       <c r="F124" s="5"/>
       <c r="G124" s="4"/>
       <c r="H124" s="116" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I124" s="2"/>
       <c r="J124" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K124" s="31">
         <v>1</v>
@@ -12962,7 +12963,7 @@
       <c r="H125" s="2"/>
       <c r="I125" s="2"/>
       <c r="J125" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K125" s="31">
         <v>2</v>
@@ -13036,13 +13037,13 @@
       <c r="F127" s="5"/>
       <c r="G127" s="4"/>
       <c r="H127" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="I127" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="I127" s="26" t="s">
-        <v>162</v>
-      </c>
       <c r="J127" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K127" s="31" t="b">
         <v>1</v>
@@ -13083,11 +13084,11 @@
       <c r="F128" s="5"/>
       <c r="G128" s="4"/>
       <c r="H128" s="116" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I128" s="2"/>
       <c r="J128" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K128" s="31" t="b">
         <v>1</v>
@@ -13130,7 +13131,7 @@
       <c r="H129" s="2"/>
       <c r="I129" s="2"/>
       <c r="J129" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K129" s="31" t="b">
         <v>1</v>
@@ -13651,7 +13652,7 @@
       <c r="J144" s="29"/>
       <c r="K144" s="29"/>
       <c r="L144" s="65" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M144" s="65"/>
       <c r="N144" s="65"/>
@@ -13686,7 +13687,7 @@
       <c r="J145" s="29"/>
       <c r="K145" s="29"/>
       <c r="L145" s="65" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M145" s="65"/>
       <c r="N145" s="65"/>
@@ -13721,10 +13722,10 @@
       <c r="J146" s="29"/>
       <c r="K146" s="145"/>
       <c r="L146" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M146" s="29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N146" s="29">
         <v>11</v>
@@ -13860,7 +13861,7 @@
         <v>5</v>
       </c>
       <c r="D149" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E149" s="5"/>
       <c r="F149" s="5"/>
@@ -13934,7 +13935,7 @@
       <c r="F151" s="5"/>
       <c r="G151" s="4"/>
       <c r="H151" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I151" s="2"/>
       <c r="J151" s="2"/>
@@ -13969,10 +13970,10 @@
       <c r="F152" s="5"/>
       <c r="G152" s="4"/>
       <c r="H152" s="26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I152" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J152" s="2"/>
       <c r="K152" s="2"/>
@@ -14009,10 +14010,10 @@
       <c r="G153" s="4"/>
       <c r="H153" s="26"/>
       <c r="I153" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J153" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K153" s="2"/>
       <c r="L153" s="31">
@@ -14068,7 +14069,7 @@
       <c r="G154" s="4"/>
       <c r="H154" s="26"/>
       <c r="I154" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J154" s="2"/>
       <c r="K154" s="2"/>
@@ -14125,7 +14126,7 @@
       <c r="G155" s="4"/>
       <c r="H155" s="26"/>
       <c r="I155" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J155" s="2"/>
       <c r="K155" s="2"/>
@@ -14161,7 +14162,7 @@
       <c r="F156" s="5"/>
       <c r="G156" s="4"/>
       <c r="H156" s="64" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I156" s="2"/>
       <c r="J156" s="2"/>
@@ -14218,7 +14219,7 @@
       <c r="F157" s="5"/>
       <c r="G157" s="4"/>
       <c r="H157" s="64" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I157" s="2"/>
       <c r="J157" s="2"/>
@@ -14275,7 +14276,7 @@
       <c r="F158" s="5"/>
       <c r="G158" s="4"/>
       <c r="H158" s="64" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I158" s="2"/>
       <c r="J158" s="2"/>
@@ -14332,7 +14333,7 @@
       <c r="F159" s="5"/>
       <c r="G159" s="4"/>
       <c r="H159" s="64" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I159" s="2"/>
       <c r="J159" s="2"/>
@@ -14389,7 +14390,7 @@
       <c r="F160" s="5"/>
       <c r="G160" s="4"/>
       <c r="H160" s="64" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I160" s="2"/>
       <c r="J160" s="2"/>
@@ -14446,7 +14447,7 @@
       <c r="F161" s="5"/>
       <c r="G161" s="4"/>
       <c r="H161" s="64" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I161" s="2"/>
       <c r="J161" s="2"/>
@@ -14503,7 +14504,7 @@
       <c r="F162" s="5"/>
       <c r="G162" s="4"/>
       <c r="H162" s="64" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I162" s="2"/>
       <c r="J162" s="2"/>
@@ -14560,7 +14561,7 @@
       <c r="F163" s="5"/>
       <c r="G163" s="4"/>
       <c r="H163" s="64" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I163" s="2"/>
       <c r="J163" s="2"/>
@@ -14620,7 +14621,7 @@
       <c r="F164" s="5"/>
       <c r="G164" s="4"/>
       <c r="H164" s="64" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I164" s="2"/>
       <c r="J164" s="2"/>
@@ -14713,7 +14714,7 @@
       <c r="F166" s="5"/>
       <c r="G166" s="4"/>
       <c r="H166" s="59" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I166" s="60" t="str">
         <f>"("&amp;ROWS(ia_k2_mlsb1)-2&amp;","&amp;COLUMNS(ia_k2_mlsb1)-1&amp;"): ia_k2_mlsb1(pointers) = input"</f>
@@ -14722,10 +14723,10 @@
       <c r="J166" s="49"/>
       <c r="K166" s="49"/>
       <c r="L166" s="94" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M166" s="94" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N166" s="94">
         <v>11</v>
@@ -14814,16 +14815,16 @@
       <c r="F168" s="5"/>
       <c r="G168" s="4"/>
       <c r="H168" s="117" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I168" s="54" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J168" s="54" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K168" s="54" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L168" s="31">
         <f>COUNTA($I$169:$I$209)</f>
@@ -14837,7 +14838,7 @@
         <v>5</v>
       </c>
       <c r="O168" s="106" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P168" s="106"/>
       <c r="Q168" s="106"/>
@@ -14868,7 +14869,7 @@
       <c r="F169" s="5"/>
       <c r="G169" s="4"/>
       <c r="H169" s="64" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I169" s="57">
         <v>0</v>
@@ -14931,11 +14932,11 @@
       <c r="F170" s="5"/>
       <c r="G170" s="4"/>
       <c r="H170" s="64" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I170" s="103"/>
       <c r="J170" s="103" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K170" s="56">
         <v>1</v>
@@ -14992,7 +14993,7 @@
       <c r="F171" s="5"/>
       <c r="G171" s="4"/>
       <c r="H171" s="64" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I171" s="103"/>
       <c r="J171" s="103"/>
@@ -15051,7 +15052,7 @@
       <c r="F172" s="5"/>
       <c r="G172" s="4"/>
       <c r="H172" s="64" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I172" s="103"/>
       <c r="J172" s="103"/>
@@ -15110,7 +15111,7 @@
       <c r="F173" s="5"/>
       <c r="G173" s="4"/>
       <c r="H173" s="64" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I173" s="103"/>
       <c r="J173" s="103"/>
@@ -15169,7 +15170,7 @@
       <c r="F174" s="5"/>
       <c r="G174" s="4"/>
       <c r="H174" s="113" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I174" s="79"/>
       <c r="J174" s="61">
@@ -15230,11 +15231,11 @@
       <c r="F175" s="5"/>
       <c r="G175" s="4"/>
       <c r="H175" s="113" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I175" s="79"/>
       <c r="J175" s="56" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K175" s="56">
         <v>1</v>
@@ -15291,7 +15292,7 @@
       <c r="F176" s="5"/>
       <c r="G176" s="4"/>
       <c r="H176" s="113" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I176" s="79"/>
       <c r="J176" s="56"/>
@@ -15350,7 +15351,7 @@
       <c r="F177" s="5"/>
       <c r="G177" s="4"/>
       <c r="H177" s="64" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I177" s="79"/>
       <c r="J177" s="56"/>
@@ -15409,7 +15410,7 @@
       <c r="F178" s="5"/>
       <c r="G178" s="4"/>
       <c r="H178" s="113" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I178" s="79"/>
       <c r="J178" s="63"/>
@@ -15468,7 +15469,7 @@
       <c r="F179" s="5"/>
       <c r="G179" s="4"/>
       <c r="H179" s="113" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I179" s="103"/>
       <c r="J179" s="61">
@@ -15529,11 +15530,11 @@
       <c r="F180" s="5"/>
       <c r="G180" s="4"/>
       <c r="H180" s="113" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I180" s="103"/>
       <c r="J180" s="56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K180" s="56">
         <v>1</v>
@@ -15590,7 +15591,7 @@
       <c r="F181" s="5"/>
       <c r="G181" s="4"/>
       <c r="H181" s="113" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I181" s="103"/>
       <c r="J181" s="56"/>
@@ -15706,7 +15707,7 @@
       <c r="F183" s="5"/>
       <c r="G183" s="4"/>
       <c r="H183" s="64" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I183" s="103"/>
       <c r="J183" s="63"/>
@@ -15765,7 +15766,7 @@
       <c r="F184" s="5"/>
       <c r="G184" s="4"/>
       <c r="H184" s="113" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I184" s="79"/>
       <c r="J184" s="61">
@@ -15826,11 +15827,11 @@
       <c r="F185" s="5"/>
       <c r="G185" s="4"/>
       <c r="H185" s="113" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I185" s="79"/>
       <c r="J185" s="56" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K185" s="56">
         <v>1</v>
@@ -15887,7 +15888,7 @@
       <c r="F186" s="5"/>
       <c r="G186" s="4"/>
       <c r="H186" s="113" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I186" s="79"/>
       <c r="J186" s="56"/>
@@ -15946,7 +15947,7 @@
       <c r="F187" s="5"/>
       <c r="G187" s="4"/>
       <c r="H187" s="113" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I187" s="79"/>
       <c r="J187" s="56"/>
@@ -16005,7 +16006,7 @@
       <c r="F188" s="5"/>
       <c r="G188" s="4"/>
       <c r="H188" s="113" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I188" s="62"/>
       <c r="J188" s="63"/>
@@ -16064,7 +16065,7 @@
       <c r="F189" s="5"/>
       <c r="G189" s="4"/>
       <c r="H189" s="113" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I189" s="112">
         <v>1</v>
@@ -16127,7 +16128,7 @@
       <c r="F190" s="5"/>
       <c r="G190" s="4"/>
       <c r="H190" s="113" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I190" s="103"/>
       <c r="J190" s="103"/>
@@ -17253,7 +17254,7 @@
       <c r="F210" s="5"/>
       <c r="G210" s="4"/>
       <c r="H210" s="59" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I210" s="60" t="str">
         <f>"("&amp;ROWS(ia_ppk2g1_rlsb1)-2&amp;","&amp;COLUMNS(ia_ppk2g1_rlsb1)-1&amp;"): ia_ppk2_vlsb1(pointers) = input"</f>
@@ -17262,37 +17263,37 @@
       <c r="J210" s="49"/>
       <c r="K210" s="49"/>
       <c r="L210" s="152" t="s">
+        <v>262</v>
+      </c>
+      <c r="M210" s="153" t="s">
         <v>263</v>
       </c>
-      <c r="M210" s="153" t="s">
+      <c r="N210" s="153" t="s">
         <v>264</v>
       </c>
-      <c r="N210" s="153" t="s">
+      <c r="O210" s="153" t="s">
         <v>265</v>
       </c>
-      <c r="O210" s="153" t="s">
+      <c r="P210" s="153" t="s">
         <v>266</v>
       </c>
-      <c r="P210" s="153" t="s">
+      <c r="Q210" s="153" t="s">
         <v>267</v>
       </c>
-      <c r="Q210" s="153" t="s">
+      <c r="R210" s="153" t="s">
         <v>268</v>
       </c>
-      <c r="R210" s="153" t="s">
+      <c r="S210" s="153" t="s">
         <v>269</v>
       </c>
-      <c r="S210" s="153" t="s">
+      <c r="T210" s="153" t="s">
         <v>270</v>
       </c>
-      <c r="T210" s="153" t="s">
+      <c r="U210" s="153" t="s">
         <v>271</v>
       </c>
-      <c r="U210" s="153" t="s">
+      <c r="V210" s="154" t="s">
         <v>272</v>
-      </c>
-      <c r="V210" s="154" t="s">
-        <v>273</v>
       </c>
       <c r="W210" s="94"/>
       <c r="X210" s="4"/>
@@ -17484,16 +17485,16 @@
       <c r="F214" s="5"/>
       <c r="G214" s="4"/>
       <c r="H214" s="117" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I214" s="54" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J214" s="54" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K214" s="54" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L214" s="31">
         <v>3</v>
@@ -17507,7 +17508,7 @@
         <v>5</v>
       </c>
       <c r="O214" s="106" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="P214" s="106"/>
       <c r="Q214" s="106"/>
@@ -17535,7 +17536,7 @@
       <c r="F215" s="5"/>
       <c r="G215" s="4"/>
       <c r="H215" s="64" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I215" s="57">
         <v>0</v>
@@ -17607,13 +17608,13 @@
       <c r="F216" s="5"/>
       <c r="G216" s="4"/>
       <c r="H216" s="64" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I216" s="103" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J216" s="103" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K216" s="56">
         <v>1</v>
@@ -17747,7 +17748,7 @@
       <c r="F218" s="5"/>
       <c r="G218" s="4"/>
       <c r="H218" s="64" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I218" s="103"/>
       <c r="J218" s="103"/>
@@ -17816,7 +17817,7 @@
       <c r="F219" s="5"/>
       <c r="G219" s="4"/>
       <c r="H219" s="113" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I219" s="103"/>
       <c r="J219" s="103"/>
@@ -17885,7 +17886,7 @@
       <c r="F220" s="5"/>
       <c r="G220" s="4"/>
       <c r="H220" s="113" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I220" s="79"/>
       <c r="J220" s="61">
@@ -17956,11 +17957,11 @@
       <c r="F221" s="5"/>
       <c r="G221" s="4"/>
       <c r="H221" s="113" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I221" s="79"/>
       <c r="J221" s="56" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K221" s="56">
         <v>1</v>
@@ -18299,7 +18300,7 @@
       <c r="H226" s="26"/>
       <c r="I226" s="103"/>
       <c r="J226" s="56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K226" s="56">
         <v>1</v>
@@ -18638,7 +18639,7 @@
       <c r="H231" s="26"/>
       <c r="I231" s="79"/>
       <c r="J231" s="56" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K231" s="56">
         <v>1</v>
@@ -18977,7 +18978,7 @@
       <c r="G236" s="4"/>
       <c r="H236" s="26"/>
       <c r="I236" s="103" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J236" s="103"/>
       <c r="K236" s="56">
@@ -20319,7 +20320,7 @@
       <c r="G256" s="4"/>
       <c r="H256" s="26"/>
       <c r="I256" s="103" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="J256" s="103"/>
       <c r="K256" s="56">
@@ -21578,7 +21579,7 @@
       <c r="F276" s="5"/>
       <c r="G276" s="4"/>
       <c r="H276" s="59" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I276" s="60" t="str">
         <f>"("&amp;ROWS(ia_ppk5_lsb0)-2&amp;","&amp;COLUMNS(ia_ppk5_lsb0)-1&amp;"): ia_ppk5g3_lsb0(pointers) = input"</f>
@@ -21775,14 +21776,14 @@
       <c r="F280" s="5"/>
       <c r="G280" s="4"/>
       <c r="H280" s="117" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I280" s="54"/>
       <c r="J280" s="54" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K280" s="54" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L280" s="31">
         <f>i_len_l</f>
@@ -21797,7 +21798,7 @@
         <v>-4</v>
       </c>
       <c r="O280" s="110" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P280" s="106"/>
       <c r="Q280" s="106"/>
@@ -21825,10 +21826,10 @@
       <c r="F281" s="5"/>
       <c r="G281" s="4"/>
       <c r="H281" s="64" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I281" s="123" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J281" s="57">
         <v>0</v>
@@ -21883,13 +21884,13 @@
       <c r="F282" s="5"/>
       <c r="G282" s="4"/>
       <c r="H282" s="64" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I282" s="103" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J282" s="103" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K282" s="56">
         <v>1</v>
@@ -21942,7 +21943,7 @@
       <c r="G283" s="4"/>
       <c r="H283" s="64"/>
       <c r="I283" s="103" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J283" s="103"/>
       <c r="K283" s="56">
@@ -21995,7 +21996,7 @@
       <c r="G284" s="4"/>
       <c r="H284" s="64"/>
       <c r="I284" s="103" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J284" s="103"/>
       <c r="K284" s="56">
@@ -22047,7 +22048,7 @@
       <c r="G285" s="4"/>
       <c r="H285" s="64"/>
       <c r="I285" s="103" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J285" s="103"/>
       <c r="K285" s="63">
@@ -22157,7 +22158,7 @@
       <c r="H287" s="113"/>
       <c r="I287" s="79"/>
       <c r="J287" s="56" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K287" s="56">
         <v>1</v>
@@ -22418,7 +22419,7 @@
       <c r="H292" s="113"/>
       <c r="I292" s="103"/>
       <c r="J292" s="56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K292" s="56">
         <v>1</v>
@@ -22677,7 +22678,7 @@
       <c r="H297" s="113"/>
       <c r="I297" s="79"/>
       <c r="J297" s="56" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K297" s="56">
         <v>1</v>
@@ -23253,23 +23254,23 @@
       <c r="H312" s="29"/>
       <c r="I312" s="29"/>
       <c r="J312" s="149" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K312" s="149"/>
       <c r="L312" s="149" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M312" s="149" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N312" s="149" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O312" s="149" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P312" s="149" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q312" s="149"/>
       <c r="R312" s="29"/>
@@ -23298,13 +23299,13 @@
       <c r="H313" s="29"/>
       <c r="I313" s="29"/>
       <c r="J313" s="184" t="s">
+        <v>240</v>
+      </c>
+      <c r="K313" s="184" t="s">
+        <v>97</v>
+      </c>
+      <c r="L313" s="184" t="s">
         <v>241</v>
-      </c>
-      <c r="K313" s="184" t="s">
-        <v>98</v>
-      </c>
-      <c r="L313" s="184" t="s">
-        <v>242</v>
       </c>
       <c r="M313" s="184"/>
       <c r="N313" s="184"/>
@@ -23337,13 +23338,13 @@
       <c r="H314" s="29"/>
       <c r="I314" s="29"/>
       <c r="J314" s="184" t="s">
+        <v>231</v>
+      </c>
+      <c r="K314" s="184" t="s">
         <v>232</v>
       </c>
-      <c r="K314" s="184" t="s">
+      <c r="L314" s="184" t="s">
         <v>233</v>
-      </c>
-      <c r="L314" s="184" t="s">
-        <v>234</v>
       </c>
       <c r="M314" s="184"/>
       <c r="N314" s="184"/>
@@ -23378,26 +23379,26 @@
       <c r="H315" s="29"/>
       <c r="I315" s="29"/>
       <c r="J315" s="149" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K315" s="149"/>
       <c r="L315" s="149" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M315" s="149" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N315" s="149" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O315" s="149" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P315" s="149" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q315" s="149" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R315" s="29"/>
       <c r="S315" s="29"/>
@@ -23454,7 +23455,7 @@
         <v>5</v>
       </c>
       <c r="D317" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E317" s="5"/>
       <c r="F317" s="5"/>
@@ -23528,7 +23529,7 @@
       <c r="F319" s="5"/>
       <c r="G319" s="4"/>
       <c r="H319" s="100" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I319" s="2"/>
       <c r="J319" s="2"/>
@@ -23563,7 +23564,7 @@
       <c r="F320" s="5"/>
       <c r="G320" s="4"/>
       <c r="H320" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I320" s="2"/>
       <c r="J320" s="31" t="b">
@@ -23604,7 +23605,7 @@
       <c r="F321" s="5"/>
       <c r="G321" s="4"/>
       <c r="H321" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I321" s="2"/>
       <c r="J321" s="121">
@@ -23645,7 +23646,7 @@
       <c r="F322" s="5"/>
       <c r="G322" s="4"/>
       <c r="H322" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I322" s="2"/>
       <c r="J322" s="31" t="b">
@@ -23686,7 +23687,7 @@
       <c r="F323" s="5"/>
       <c r="G323" s="4"/>
       <c r="H323" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I323" s="2"/>
       <c r="J323" s="31" t="b">
@@ -23795,13 +23796,13 @@
       <c r="H326" s="2"/>
       <c r="I326" s="147"/>
       <c r="J326" s="148" t="s">
+        <v>252</v>
+      </c>
+      <c r="K326" s="148" t="s">
         <v>253</v>
       </c>
-      <c r="K326" s="148" t="s">
+      <c r="L326" s="148" t="s">
         <v>254</v>
-      </c>
-      <c r="L326" s="148" t="s">
-        <v>255</v>
       </c>
       <c r="M326" s="2"/>
       <c r="N326" s="2"/>
@@ -23832,7 +23833,7 @@
       <c r="F327" s="5"/>
       <c r="G327" s="4"/>
       <c r="H327" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I327" s="147"/>
       <c r="J327" s="31">
@@ -24371,10 +24372,10 @@
   <dimension ref="A1:AB154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="8" ySplit="33" topLeftCell="I42" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="33" topLeftCell="I85" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
-      <selection pane="bottomRight" activeCell="O55" sqref="O55:O57"/>
+      <selection pane="bottomRight" activeCell="J21" sqref="J21:T21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -24612,7 +24613,7 @@
       </c>
       <c r="G6" s="12"/>
       <c r="H6" s="44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
@@ -24819,7 +24820,7 @@
       <c r="G12" s="3"/>
       <c r="H12" s="29"/>
       <c r="I12" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J12" s="29" t="s">
         <v>5</v>
@@ -24993,7 +24994,7 @@
       <c r="F17" s="5"/>
       <c r="G17" s="4"/>
       <c r="H17" s="50" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -25031,10 +25032,10 @@
         <v>16</v>
       </c>
       <c r="I18" s="151">
-        <v>44332.873621527797</v>
+        <v>44336.775273148101</v>
       </c>
       <c r="J18" s="185" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="K18" s="186"/>
       <c r="L18" s="186"/>
@@ -25136,10 +25137,10 @@
         <v>17</v>
       </c>
       <c r="I21" s="23">
-        <v>1</v>
+        <v>44336.775756828698</v>
       </c>
       <c r="J21" s="188" t="s">
-        <v>35</v>
+        <v>316</v>
       </c>
       <c r="K21" s="189"/>
       <c r="L21" s="189"/>
@@ -25948,17 +25949,17 @@
       <c r="H44" s="29"/>
       <c r="I44" s="29"/>
       <c r="J44" s="149" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K44" s="149"/>
       <c r="L44" s="149" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M44" s="149"/>
       <c r="N44" s="29"/>
       <c r="O44" s="29"/>
       <c r="P44" s="149" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q44" s="149"/>
       <c r="R44" s="29"/>
@@ -25990,13 +25991,13 @@
       <c r="K45" s="29"/>
       <c r="L45" s="29"/>
       <c r="M45" s="184" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="N45" s="184" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="O45" s="184" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="P45" s="184"/>
       <c r="Q45" s="184"/>
@@ -26029,13 +26030,13 @@
       <c r="K46" s="29"/>
       <c r="L46" s="29"/>
       <c r="M46" s="184" t="s">
+        <v>234</v>
+      </c>
+      <c r="N46" s="184" t="s">
         <v>235</v>
       </c>
-      <c r="N46" s="184" t="s">
-        <v>236</v>
-      </c>
       <c r="O46" s="184" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="P46" s="184"/>
       <c r="Q46" s="184"/>
@@ -26073,10 +26074,10 @@
       <c r="N47" s="29"/>
       <c r="O47" s="29"/>
       <c r="P47" s="149" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q47" s="149" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R47" s="29"/>
       <c r="S47" s="29"/>
@@ -26133,7 +26134,7 @@
         <v>5</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
@@ -26207,7 +26208,7 @@
       <c r="F51" s="5"/>
       <c r="G51" s="4"/>
       <c r="H51" s="100" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
@@ -26242,7 +26243,7 @@
       <c r="F52" s="5"/>
       <c r="G52" s="4"/>
       <c r="H52" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
@@ -26283,7 +26284,7 @@
       <c r="F53" s="5"/>
       <c r="G53" s="4"/>
       <c r="H53" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
@@ -26324,7 +26325,7 @@
       <c r="F54" s="5"/>
       <c r="G54" s="4"/>
       <c r="H54" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
@@ -26365,7 +26366,7 @@
       <c r="F55" s="5"/>
       <c r="G55" s="4"/>
       <c r="H55" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
@@ -26402,7 +26403,7 @@
       <c r="F56" s="5"/>
       <c r="G56" s="4"/>
       <c r="H56" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
@@ -26439,7 +26440,7 @@
       <c r="F57" s="5"/>
       <c r="G57" s="4"/>
       <c r="H57" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
@@ -26542,20 +26543,20 @@
       <c r="F60" s="5"/>
       <c r="G60" s="4"/>
       <c r="H60" s="100" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I60" s="2"/>
       <c r="J60" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="K60" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="K60" s="2" t="s">
+      <c r="L60" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="L60" s="2" t="s">
-        <v>250</v>
-      </c>
       <c r="M60" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="N60" s="2"/>
       <c r="O60" s="2"/>
@@ -26587,16 +26588,16 @@
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
       <c r="J61" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="K61" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="K61" s="2" t="s">
+      <c r="L61" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="L61" s="2" t="s">
+      <c r="M61" s="2" t="s">
         <v>234</v>
-      </c>
-      <c r="M61" s="2" t="s">
-        <v>235</v>
       </c>
       <c r="N61" s="2"/>
       <c r="O61" s="2"/>
@@ -26626,7 +26627,7 @@
       <c r="F62" s="5"/>
       <c r="G62" s="4"/>
       <c r="H62" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I62" s="2"/>
       <c r="J62" s="31" t="b">
@@ -26669,7 +26670,7 @@
       <c r="F63" s="5"/>
       <c r="G63" s="4"/>
       <c r="H63" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I63" s="2"/>
       <c r="J63" s="31" t="b">
@@ -26712,7 +26713,7 @@
       <c r="F64" s="5"/>
       <c r="G64" s="4"/>
       <c r="H64" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I64" s="2"/>
       <c r="J64" s="31">
@@ -27227,17 +27228,17 @@
       <c r="H79" s="29"/>
       <c r="I79" s="29"/>
       <c r="J79" s="149" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K79" s="149"/>
       <c r="L79" s="149" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M79" s="149"/>
       <c r="N79" s="29"/>
       <c r="O79" s="29"/>
       <c r="P79" s="149" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q79" s="149"/>
       <c r="R79" s="29"/>
@@ -27266,17 +27267,17 @@
       <c r="H80" s="29"/>
       <c r="I80" s="29"/>
       <c r="J80" s="149" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K80" s="149"/>
       <c r="L80" s="149" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M80" s="149"/>
       <c r="N80" s="29"/>
       <c r="O80" s="29"/>
       <c r="P80" s="149" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q80" s="149"/>
       <c r="R80" s="29"/>
@@ -27305,21 +27306,21 @@
       <c r="H81" s="29"/>
       <c r="I81" s="29"/>
       <c r="J81" s="149" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K81" s="149"/>
       <c r="L81" s="149" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M81" s="149"/>
       <c r="N81" s="29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O81" s="29" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="P81" s="149" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q81" s="149"/>
       <c r="R81" s="29"/>
@@ -27350,17 +27351,17 @@
       <c r="H82" s="29"/>
       <c r="I82" s="29"/>
       <c r="J82" s="149" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K82" s="149"/>
       <c r="L82" s="149" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M82" s="149"/>
       <c r="N82" s="29"/>
       <c r="O82" s="29"/>
       <c r="P82" s="149" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q82" s="149"/>
       <c r="R82" s="29"/>
@@ -27418,7 +27419,7 @@
         <v>8</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E84" s="5"/>
       <c r="F84" s="5"/>
@@ -27492,7 +27493,7 @@
       <c r="F86" s="5"/>
       <c r="G86" s="4"/>
       <c r="H86" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I86" s="2"/>
       <c r="J86" s="36">
@@ -27505,7 +27506,7 @@
       </c>
       <c r="M86" s="2"/>
       <c r="N86" s="116" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O86" s="31">
         <v>10</v>
@@ -27539,7 +27540,7 @@
       <c r="F87" s="5"/>
       <c r="G87" s="4"/>
       <c r="H87" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I87" s="2"/>
       <c r="J87" s="121">
@@ -27581,7 +27582,7 @@
       <c r="F88" s="5"/>
       <c r="G88" s="4"/>
       <c r="H88" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I88" s="2"/>
       <c r="J88" s="36">
@@ -27599,7 +27600,7 @@
       </c>
       <c r="Q88" s="115"/>
       <c r="R88" s="190" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="S88" s="191"/>
       <c r="T88" s="191"/>
@@ -27624,7 +27625,7 @@
       <c r="F89" s="5"/>
       <c r="G89" s="4"/>
       <c r="H89" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I89" s="2"/>
       <c r="J89" s="31">
@@ -27667,7 +27668,7 @@
       <c r="F90" s="5"/>
       <c r="G90" s="4"/>
       <c r="H90" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I90" s="2"/>
       <c r="J90" s="31">
@@ -27780,24 +27781,24 @@
       <c r="H93" s="2"/>
       <c r="I93" s="174"/>
       <c r="J93" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="K93" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="K93" s="2" t="s">
-        <v>278</v>
-      </c>
       <c r="L93" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="M93" s="2" t="s">
         <v>277</v>
-      </c>
-      <c r="M93" s="2" t="s">
-        <v>278</v>
       </c>
       <c r="N93" s="2"/>
       <c r="O93" s="2"/>
       <c r="P93" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="Q93" s="2" t="s">
         <v>277</v>
-      </c>
-      <c r="Q93" s="2" t="s">
-        <v>278</v>
       </c>
       <c r="R93" s="2"/>
       <c r="S93" s="2"/>
@@ -27825,10 +27826,10 @@
       <c r="F94" s="5"/>
       <c r="G94" s="4"/>
       <c r="H94" s="175" t="s">
+        <v>278</v>
+      </c>
+      <c r="I94" s="176" t="s">
         <v>279</v>
-      </c>
-      <c r="I94" s="176" t="s">
-        <v>280</v>
       </c>
       <c r="J94" s="177">
         <v>0</v>
@@ -27877,7 +27878,7 @@
       <c r="G95" s="4"/>
       <c r="H95" s="175"/>
       <c r="I95" s="176" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J95" s="175"/>
       <c r="K95" s="175"/>
@@ -27922,7 +27923,7 @@
       <c r="G96" s="4"/>
       <c r="H96" s="175"/>
       <c r="I96" s="176" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J96" s="175"/>
       <c r="K96" s="175"/>
@@ -27967,7 +27968,7 @@
       <c r="G97" s="4"/>
       <c r="H97" s="175"/>
       <c r="I97" s="176" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J97" s="175"/>
       <c r="K97" s="175"/>
@@ -28012,7 +28013,7 @@
       <c r="G98" s="4"/>
       <c r="H98" s="175"/>
       <c r="I98" s="176" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J98" s="175"/>
       <c r="K98" s="175"/>
@@ -28057,7 +28058,7 @@
       <c r="G99" s="4"/>
       <c r="H99" s="175"/>
       <c r="I99" s="176" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J99" s="175"/>
       <c r="K99" s="175"/>
@@ -28102,7 +28103,7 @@
       <c r="G100" s="4"/>
       <c r="H100" s="175"/>
       <c r="I100" s="176" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J100" s="175"/>
       <c r="K100" s="175"/>
@@ -28147,12 +28148,16 @@
       <c r="G101" s="4"/>
       <c r="H101" s="175"/>
       <c r="I101" s="176" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J101" s="175"/>
       <c r="K101" s="175"/>
-      <c r="L101" s="175"/>
-      <c r="M101" s="175"/>
+      <c r="L101" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="M101" s="31">
+        <v>1</v>
+      </c>
       <c r="N101" s="2"/>
       <c r="O101" s="2"/>
       <c r="P101" s="31">
@@ -28255,25 +28260,25 @@
       <c r="F104" s="5"/>
       <c r="G104" s="4"/>
       <c r="H104" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I104" s="2"/>
       <c r="J104" s="100" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K104" s="100"/>
       <c r="L104" s="100"/>
       <c r="M104" s="100"/>
       <c r="N104" s="2"/>
       <c r="O104" s="100" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P104" s="2"/>
       <c r="Q104" s="2"/>
       <c r="R104" s="2"/>
       <c r="S104" s="2"/>
       <c r="T104" s="100" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="U104" s="2"/>
       <c r="V104" s="2"/>
@@ -28298,42 +28303,42 @@
       <c r="H105" s="2"/>
       <c r="I105" s="2"/>
       <c r="J105" s="100" t="s">
+        <v>288</v>
+      </c>
+      <c r="K105" s="100" t="s">
         <v>289</v>
       </c>
-      <c r="K105" s="100" t="s">
+      <c r="L105" s="100" t="s">
         <v>290</v>
       </c>
-      <c r="L105" s="100" t="s">
+      <c r="M105" s="100" t="s">
         <v>291</v>
-      </c>
-      <c r="M105" s="100" t="s">
-        <v>292</v>
       </c>
       <c r="N105" s="2"/>
       <c r="O105" s="100" t="s">
+        <v>288</v>
+      </c>
+      <c r="P105" s="100" t="s">
         <v>289</v>
       </c>
-      <c r="P105" s="100" t="s">
+      <c r="Q105" s="100" t="s">
         <v>290</v>
       </c>
-      <c r="Q105" s="100" t="s">
+      <c r="R105" s="100" t="s">
         <v>291</v>
-      </c>
-      <c r="R105" s="100" t="s">
-        <v>292</v>
       </c>
       <c r="S105" s="2"/>
       <c r="T105" s="100" t="s">
+        <v>288</v>
+      </c>
+      <c r="U105" s="100" t="s">
         <v>289</v>
       </c>
-      <c r="U105" s="100" t="s">
+      <c r="V105" s="100" t="s">
         <v>290</v>
       </c>
-      <c r="V105" s="100" t="s">
+      <c r="W105" s="100" t="s">
         <v>291</v>
-      </c>
-      <c r="W105" s="100" t="s">
-        <v>292</v>
       </c>
       <c r="X105" s="4"/>
       <c r="Y105" s="16"/>
@@ -28355,7 +28360,7 @@
       <c r="F106" s="5"/>
       <c r="G106" s="4"/>
       <c r="H106" s="179" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="I106" s="2"/>
       <c r="J106" s="180">
@@ -28416,7 +28421,7 @@
       <c r="F107" s="5"/>
       <c r="G107" s="4"/>
       <c r="H107" s="179" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="I107" s="2"/>
       <c r="J107" s="2"/>
@@ -28469,7 +28474,7 @@
       <c r="F108" s="5"/>
       <c r="G108" s="4"/>
       <c r="H108" s="179" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I108" s="2"/>
       <c r="J108" s="2"/>
@@ -29000,17 +29005,17 @@
       <c r="H123" s="29"/>
       <c r="I123" s="29"/>
       <c r="J123" s="149" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K123" s="149"/>
       <c r="L123" s="149" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M123" s="149"/>
       <c r="N123" s="29"/>
       <c r="O123" s="29"/>
       <c r="P123" s="149" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q123" s="149"/>
       <c r="R123" s="29"/>
@@ -29068,7 +29073,7 @@
         <v>8</v>
       </c>
       <c r="D125" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E125" s="5"/>
       <c r="F125" s="5"/>
@@ -29142,7 +29147,7 @@
       <c r="F127" s="5"/>
       <c r="G127" s="4"/>
       <c r="H127" s="26" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I127" s="31" t="b">
         <v>0</v>
@@ -29206,7 +29211,7 @@
       <c r="F129" s="5"/>
       <c r="G129" s="4"/>
       <c r="H129" s="26" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I129" s="31">
         <v>0</v>
@@ -29313,10 +29318,10 @@
       <c r="F132" s="5"/>
       <c r="G132" s="4"/>
       <c r="H132" s="64" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I132" s="64" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J132" s="2"/>
       <c r="K132" s="2"/>
@@ -29352,7 +29357,7 @@
       <c r="F133" s="5"/>
       <c r="G133" s="4"/>
       <c r="H133" s="31" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I133" s="31" t="b">
         <v>0</v>
@@ -29391,7 +29396,7 @@
       <c r="F134" s="5"/>
       <c r="G134" s="4"/>
       <c r="H134" s="31" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I134" s="31" t="b">
         <v>0</v>
@@ -29430,7 +29435,7 @@
       <c r="F135" s="5"/>
       <c r="G135" s="4"/>
       <c r="H135" s="31" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I135" s="31" t="b">
         <v>0</v>
@@ -29469,7 +29474,7 @@
       <c r="F136" s="5"/>
       <c r="G136" s="4"/>
       <c r="H136" s="31" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="I136" s="31" t="b">
         <v>0</v>
@@ -29508,7 +29513,7 @@
       <c r="F137" s="5"/>
       <c r="G137" s="4"/>
       <c r="H137" s="31" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I137" s="31" t="b">
         <v>0</v>
@@ -29542,7 +29547,7 @@
       <c r="F138" s="5"/>
       <c r="G138" s="4"/>
       <c r="H138" s="31" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I138" s="31" t="b">
         <v>0</v>
@@ -29576,7 +29581,7 @@
       <c r="F139" s="5"/>
       <c r="G139" s="4"/>
       <c r="H139" s="31" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="I139" s="31" t="b">
         <v>0</v>
@@ -29615,7 +29620,7 @@
       <c r="F140" s="5"/>
       <c r="G140" s="4"/>
       <c r="H140" s="31" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I140" s="31" t="b">
         <v>0</v>
@@ -30678,7 +30683,7 @@
       <c r="G12" s="3"/>
       <c r="H12" s="29"/>
       <c r="I12" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J12" s="29" t="s">
         <v>5</v>
@@ -30786,7 +30791,7 @@
         <v>5</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
@@ -30864,7 +30869,7 @@
       <c r="F17" s="5"/>
       <c r="G17" s="4"/>
       <c r="H17" s="50" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -31482,10 +31487,10 @@
         <v>23</v>
       </c>
       <c r="J33" s="80" t="s">
+        <v>48</v>
+      </c>
+      <c r="K33" s="81" t="s">
         <v>49</v>
-      </c>
-      <c r="K33" s="81" t="s">
-        <v>50</v>
       </c>
       <c r="L33" s="31" t="s">
         <v>25</v>
@@ -31538,49 +31543,49 @@
       <c r="G34" s="4"/>
       <c r="H34" s="2"/>
       <c r="I34" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="J34" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="J34" s="48" t="s">
+      <c r="K34" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="K34" s="45" t="s">
+      <c r="L34" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="L34" s="47" t="s">
+      <c r="M34" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="M34" s="46" t="s">
+      <c r="N34" s="84" t="s">
         <v>61</v>
       </c>
-      <c r="N34" s="84" t="s">
+      <c r="O34" s="85" t="s">
         <v>62</v>
       </c>
-      <c r="O34" s="85" t="s">
+      <c r="P34" s="86" t="s">
         <v>63</v>
       </c>
-      <c r="P34" s="86" t="s">
+      <c r="Q34" s="87" t="s">
         <v>64</v>
       </c>
-      <c r="Q34" s="87" t="s">
+      <c r="R34" s="88" t="s">
+        <v>51</v>
+      </c>
+      <c r="S34" s="89" t="s">
+        <v>52</v>
+      </c>
+      <c r="T34" s="90" t="s">
+        <v>53</v>
+      </c>
+      <c r="U34" s="91" t="s">
+        <v>54</v>
+      </c>
+      <c r="V34" s="92" t="s">
+        <v>55</v>
+      </c>
+      <c r="W34" s="93" t="s">
         <v>65</v>
-      </c>
-      <c r="R34" s="88" t="s">
-        <v>52</v>
-      </c>
-      <c r="S34" s="89" t="s">
-        <v>53</v>
-      </c>
-      <c r="T34" s="90" t="s">
-        <v>54</v>
-      </c>
-      <c r="U34" s="91" t="s">
-        <v>55</v>
-      </c>
-      <c r="V34" s="92" t="s">
-        <v>56</v>
-      </c>
-      <c r="W34" s="93" t="s">
-        <v>66</v>
       </c>
       <c r="X34" s="2"/>
       <c r="Y34" s="2"/>

</xml_diff>

<commit_message>
Change rangenames from fev to nv
</commit_message>
<xml_diff>
--- a/Structural.xlsx
+++ b/Structural.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BD0955-2F6C-493A-8F13-E93FD89437BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDBFE6C-D88C-4567-9D67-ACC9C1A9045E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="29610" yWindow="-90" windowWidth="28110" windowHeight="16440" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -60,8 +60,6 @@
     <definedName name="i_e0_pos">Stock!$I$48</definedName>
     <definedName name="i_e1_pos">Stock!$I$49</definedName>
     <definedName name="i_feedsupply_itn_max">Stock!$I$72</definedName>
-    <definedName name="i_fev_lower_p6">StructuralSA!$J$155:$S$155</definedName>
-    <definedName name="i_fev_upper_p6">StructuralSA!$J$156:$S$156</definedName>
     <definedName name="i_fixed_dvp_mask_f1">Stock!$J$314:$L$314</definedName>
     <definedName name="i_fixed_fvp_is_rdvp_f1">Stock!$J$315:$L$315</definedName>
     <definedName name="i_fixed_fvp_mask_dams">Stock!$J$312:$L$312</definedName>
@@ -108,6 +106,8 @@
     <definedName name="i_nut_spread_n0" localSheetId="2">StructuralSA!$J$85</definedName>
     <definedName name="i_nut_spread_n1" localSheetId="2">StructuralSA!$L$85:$L$92</definedName>
     <definedName name="i_nut_spread_n3" localSheetId="2">StructuralSA!$P$85:$P$92</definedName>
+    <definedName name="i_nv_lower_p6">StructuralSA!$J$155:$S$155</definedName>
+    <definedName name="i_nv_upper_p6">StructuralSA!$J$156:$S$156</definedName>
     <definedName name="i_p_pos">Stock!$I$55</definedName>
     <definedName name="i_prejoin_offset">Stock!$I$66</definedName>
     <definedName name="i_progeny_w2_len">StructuralSA!$O$77</definedName>
@@ -2650,7 +2650,55 @@
     <t>Triplets (7)</t>
   </si>
   <si>
-    <t>24Jun21: Add inputs for the user defined feed pools
+    <t>Number of feed pools</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Period definitions</t>
+  </si>
+  <si>
+    <t>Axis postions</t>
+  </si>
+  <si>
+    <t>+ the confinement feeding pool</t>
+  </si>
+  <si>
+    <t>Lower cutoff level between pools</t>
+  </si>
+  <si>
+    <t>Feed Period (p6)</t>
+  </si>
+  <si>
+    <t>Highest value</t>
+  </si>
+  <si>
+    <t>Number of feed pools (i_len_f) and the cut-offs for each feed period (i_fev_cutoff_fp6)</t>
+  </si>
+  <si>
+    <t>24Jun21: Delete feed pool inputs (because now calculated in the code).
+17Jul20: Added structural inputs table
+1Apr19: Created the version control table</t>
+  </si>
+  <si>
+    <t>28Apr21: change grazing pool names
+1Apr19: Blank worksheet</t>
+  </si>
+  <si>
+    <t>Latest</t>
+  </si>
+  <si>
+    <t>Lowest value</t>
+  </si>
+  <si>
+    <t>20May21: Make the extra nut_spread_g1 = 0.1
+1Apr19: Blank worksheet</t>
+  </si>
+  <si>
+    <t>30Jun21: Change rangename from fev to nv
+24Jun21: Fix the conditional formatting in the Initial LW section.  
+                  Add inputs for the user defined feed pools
 20May21: Add extra N for dams (now 8)
 16May21: Add extra TOL to the extra FVP date
 5May21: Adjust the extra FVP date for TOL[0] (for GEPEP calibration)
@@ -2662,52 +2710,6 @@
 25Apr21: Moved inputs from Property.xlsx
                    Moved FVP &amp; N inputs from Stock
 1: 1Apr19-Created the version control table</t>
-  </si>
-  <si>
-    <t>Number of feed pools</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Period definitions</t>
-  </si>
-  <si>
-    <t>Axis postions</t>
-  </si>
-  <si>
-    <t>+ the confinement feeding pool</t>
-  </si>
-  <si>
-    <t>Lower cutoff level between pools</t>
-  </si>
-  <si>
-    <t>Feed Period (p6)</t>
-  </si>
-  <si>
-    <t>Highest value</t>
-  </si>
-  <si>
-    <t>Number of feed pools (i_len_f) and the cut-offs for each feed period (i_fev_cutoff_fp6)</t>
-  </si>
-  <si>
-    <t>24Jun21: Delete feed pool inputs (because now calculated in the code).
-17Jul20: Added structural inputs table
-1Apr19: Created the version control table</t>
-  </si>
-  <si>
-    <t>28Apr21: change grazing pool names
-1Apr19: Blank worksheet</t>
-  </si>
-  <si>
-    <t>Latest</t>
-  </si>
-  <si>
-    <t>Lowest value</t>
-  </si>
-  <si>
-    <t>20May21: Make the extra nut_spread_g1 = 0.1
-1Apr19: Blank worksheet</t>
   </si>
 </sst>
 </file>
@@ -4405,6 +4407,18 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="32" xfId="11" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="25" xfId="3" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="25" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="25" xfId="3" quotePrefix="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="25" xfId="3" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="38" xfId="12" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -4456,18 +4470,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="25" xfId="3" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="25" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="25" xfId="3" quotePrefix="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="25" xfId="3" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="Accent2" xfId="33" builtinId="33" customBuiltin="1"/>
@@ -4515,161 +4517,7 @@
     <cellStyle name="Warning Text" xfId="21" builtinId="11" customBuiltin="1"/>
     <cellStyle name="WorksheetBackground" xfId="37" xr:uid="{D9586848-0E78-42E2-92FA-4C5FBD9E7440}"/>
   </cellStyles>
-  <dxfs count="25">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -4798,15 +4646,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
+      <xdr:colOff>114300</xdr:colOff>
       <xdr:row>82</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>94</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4821,7 +4669,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9753600" y="14630400"/>
+          <a:off x="11391900" y="13544550"/>
           <a:ext cx="4524375" cy="1866900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5649,7 +5497,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="29"/>
       <c r="I9" s="29" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J9" s="29" t="s">
         <v>5</v>
@@ -5797,19 +5645,19 @@
       <c r="I13" s="150">
         <v>44371.659649305599</v>
       </c>
-      <c r="J13" s="182" t="s">
-        <v>317</v>
-      </c>
-      <c r="K13" s="183"/>
-      <c r="L13" s="183"/>
-      <c r="M13" s="183"/>
-      <c r="N13" s="183"/>
-      <c r="O13" s="183"/>
-      <c r="P13" s="183"/>
-      <c r="Q13" s="183"/>
-      <c r="R13" s="183"/>
-      <c r="S13" s="183"/>
-      <c r="T13" s="184"/>
+      <c r="J13" s="186" t="s">
+        <v>316</v>
+      </c>
+      <c r="K13" s="187"/>
+      <c r="L13" s="187"/>
+      <c r="M13" s="187"/>
+      <c r="N13" s="187"/>
+      <c r="O13" s="187"/>
+      <c r="P13" s="187"/>
+      <c r="Q13" s="187"/>
+      <c r="R13" s="187"/>
+      <c r="S13" s="187"/>
+      <c r="T13" s="188"/>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
@@ -5836,19 +5684,19 @@
       <c r="I14" s="149">
         <v>44371.660335300898</v>
       </c>
-      <c r="J14" s="185" t="s">
-        <v>318</v>
-      </c>
-      <c r="K14" s="186"/>
-      <c r="L14" s="186"/>
-      <c r="M14" s="186"/>
-      <c r="N14" s="186"/>
-      <c r="O14" s="186"/>
-      <c r="P14" s="186"/>
-      <c r="Q14" s="186"/>
-      <c r="R14" s="186"/>
-      <c r="S14" s="186"/>
-      <c r="T14" s="186"/>
+      <c r="J14" s="189" t="s">
+        <v>317</v>
+      </c>
+      <c r="K14" s="190"/>
+      <c r="L14" s="190"/>
+      <c r="M14" s="190"/>
+      <c r="N14" s="190"/>
+      <c r="O14" s="190"/>
+      <c r="P14" s="190"/>
+      <c r="Q14" s="190"/>
+      <c r="R14" s="190"/>
+      <c r="S14" s="190"/>
+      <c r="T14" s="190"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
@@ -6811,7 +6659,7 @@
       <c r="A42" s="1"/>
       <c r="B42" s="33"/>
       <c r="C42" s="73">
-        <f>INT($C$31)+2</f>
+        <f t="shared" ref="C42:C59" si="1">INT($C$31)+2</f>
         <v>3</v>
       </c>
       <c r="D42" s="4"/>
@@ -6852,7 +6700,7 @@
       <c r="A43" s="1"/>
       <c r="B43" s="33"/>
       <c r="C43" s="73">
-        <f>INT($C$31)+2</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="D43" s="4"/>
@@ -6885,7 +6733,7 @@
       <c r="A44" s="1"/>
       <c r="B44" s="33"/>
       <c r="C44" s="73">
-        <f>INT($C$31)+2</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="D44" s="4"/>
@@ -6924,7 +6772,7 @@
       <c r="A45" s="1"/>
       <c r="B45" s="33"/>
       <c r="C45" s="73">
-        <f>INT($C$31)+2</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="D45" s="4"/>
@@ -6957,7 +6805,7 @@
       <c r="A46" s="1"/>
       <c r="B46" s="33"/>
       <c r="C46" s="73">
-        <f>INT($C$31)+2</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="D46" s="4"/>
@@ -6998,7 +6846,7 @@
       <c r="A47" s="1"/>
       <c r="B47" s="33"/>
       <c r="C47" s="73">
-        <f>INT($C$31)+2</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="D47" s="4"/>
@@ -7039,7 +6887,7 @@
       <c r="A48" s="1"/>
       <c r="B48" s="33"/>
       <c r="C48" s="73">
-        <f>INT($C$31)+2</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="D48" s="4"/>
@@ -7078,7 +6926,7 @@
       <c r="A49" s="1"/>
       <c r="B49" s="33"/>
       <c r="C49" s="73">
-        <f>INT($C$31)+2</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="D49" s="4"/>
@@ -7121,7 +6969,7 @@
       <c r="A50" s="1"/>
       <c r="B50" s="33"/>
       <c r="C50" s="73">
-        <f>INT($C$31)+2</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="D50" s="4"/>
@@ -7162,7 +7010,7 @@
       <c r="A51" s="1"/>
       <c r="B51" s="33"/>
       <c r="C51" s="73">
-        <f>INT($C$31)+2</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="D51" s="4"/>
@@ -7195,7 +7043,7 @@
       <c r="A52" s="1"/>
       <c r="B52" s="33"/>
       <c r="C52" s="73">
-        <f>INT($C$31)+2</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="D52" s="4"/>
@@ -7232,7 +7080,7 @@
       <c r="A53" s="1"/>
       <c r="B53" s="33"/>
       <c r="C53" s="73">
-        <f>INT($C$31)+2</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="D53" s="4"/>
@@ -7265,7 +7113,7 @@
       <c r="A54" s="1"/>
       <c r="B54" s="33"/>
       <c r="C54" s="73">
-        <f>INT($C$31)+2</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="D54" s="4"/>
@@ -7302,7 +7150,7 @@
       <c r="A55" s="1"/>
       <c r="B55" s="33"/>
       <c r="C55" s="73">
-        <f>INT($C$31)+2</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="D55" s="4"/>
@@ -7335,7 +7183,7 @@
       <c r="A56" s="1"/>
       <c r="B56" s="33"/>
       <c r="C56" s="73">
-        <f>INT($C$31)+2</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="D56" s="4"/>
@@ -7391,7 +7239,7 @@
       <c r="A57" s="1"/>
       <c r="B57" s="33"/>
       <c r="C57" s="73">
-        <f>INT($C$31)+2</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="D57" s="4"/>
@@ -7455,7 +7303,7 @@
       <c r="A58" s="1"/>
       <c r="B58" s="33"/>
       <c r="C58" s="73">
-        <f>INT($C$31)+2</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="D58" s="4"/>
@@ -7505,7 +7353,7 @@
       <c r="A59" s="1"/>
       <c r="B59" s="33"/>
       <c r="C59" s="73">
-        <f>INT($C$31)+2</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="D59" s="4"/>
@@ -7958,7 +7806,7 @@
   <dimension ref="A1:AE335"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <pane xSplit="9" ySplit="10" topLeftCell="J16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="10" topLeftCell="J304" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
@@ -8306,7 +8154,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="29"/>
       <c r="I9" s="29" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J9" s="29" t="s">
         <v>5</v>
@@ -8454,19 +8302,19 @@
       <c r="I13" s="150">
         <v>44311.756953009302</v>
       </c>
-      <c r="J13" s="182" t="s">
+      <c r="J13" s="186" t="s">
         <v>282</v>
       </c>
-      <c r="K13" s="183"/>
-      <c r="L13" s="183"/>
-      <c r="M13" s="183"/>
-      <c r="N13" s="183"/>
-      <c r="O13" s="183"/>
-      <c r="P13" s="183"/>
-      <c r="Q13" s="183"/>
-      <c r="R13" s="183"/>
-      <c r="S13" s="183"/>
-      <c r="T13" s="184"/>
+      <c r="K13" s="187"/>
+      <c r="L13" s="187"/>
+      <c r="M13" s="187"/>
+      <c r="N13" s="187"/>
+      <c r="O13" s="187"/>
+      <c r="P13" s="187"/>
+      <c r="Q13" s="187"/>
+      <c r="R13" s="187"/>
+      <c r="S13" s="187"/>
+      <c r="T13" s="188"/>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
@@ -8493,19 +8341,19 @@
       <c r="I14" s="149">
         <v>44355.378988657401</v>
       </c>
-      <c r="J14" s="185" t="s">
+      <c r="J14" s="189" t="s">
         <v>298</v>
       </c>
-      <c r="K14" s="186"/>
-      <c r="L14" s="186"/>
-      <c r="M14" s="186"/>
-      <c r="N14" s="186"/>
-      <c r="O14" s="186"/>
-      <c r="P14" s="186"/>
-      <c r="Q14" s="186"/>
-      <c r="R14" s="186"/>
-      <c r="S14" s="186"/>
-      <c r="T14" s="186"/>
+      <c r="K14" s="190"/>
+      <c r="L14" s="190"/>
+      <c r="M14" s="190"/>
+      <c r="N14" s="190"/>
+      <c r="O14" s="190"/>
+      <c r="P14" s="190"/>
+      <c r="Q14" s="190"/>
+      <c r="R14" s="190"/>
+      <c r="S14" s="190"/>
+      <c r="T14" s="190"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
@@ -9473,8 +9321,8 @@
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
       <c r="G42" s="4"/>
-      <c r="H42" s="199" t="s">
-        <v>311</v>
+      <c r="H42" s="183" t="s">
+        <v>310</v>
       </c>
       <c r="I42" s="36" t="s">
         <v>290</v>
@@ -10177,10 +10025,10 @@
       <c r="F61" s="5"/>
       <c r="G61" s="4"/>
       <c r="H61" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I61" s="36" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
@@ -23826,11 +23674,11 @@
   <dimension ref="A1:AB170"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <pane xSplit="9" ySplit="10" topLeftCell="J144" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="10" topLeftCell="J131" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="T154" sqref="T154"/>
+      <selection pane="bottomRight" activeCell="J13" sqref="J13:T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -23838,9 +23686,9 @@
     <col min="1" max="1" width="4.7109375" style="141" customWidth="1"/>
     <col min="2" max="2" width="2.7109375" style="141" customWidth="1"/>
     <col min="3" max="3" width="4.7109375" style="141" customWidth="1" outlineLevel="2"/>
-    <col min="4" max="4" width="1.7109375" style="141" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="9.7109375" style="141" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="1.7109375" style="141" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="1.7109375" style="141" customWidth="1"/>
+    <col min="5" max="6" width="9.7109375" style="141" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="1.7109375" style="141" customWidth="1" outlineLevel="1"/>
     <col min="8" max="8" width="37.28515625" style="141" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" style="141" customWidth="1"/>
     <col min="10" max="23" width="10.85546875" style="141" customWidth="1"/>
@@ -24176,7 +24024,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="29"/>
       <c r="I9" s="29" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J9" s="29" t="s">
         <v>5</v>
@@ -24322,21 +24170,21 @@
         <v>16</v>
       </c>
       <c r="I13" s="150">
-        <v>44371.556718634303</v>
-      </c>
-      <c r="J13" s="182" t="s">
-        <v>307</v>
-      </c>
-      <c r="K13" s="183"/>
-      <c r="L13" s="183"/>
-      <c r="M13" s="183"/>
-      <c r="N13" s="183"/>
-      <c r="O13" s="183"/>
-      <c r="P13" s="183"/>
-      <c r="Q13" s="183"/>
-      <c r="R13" s="183"/>
-      <c r="S13" s="183"/>
-      <c r="T13" s="184"/>
+        <v>44377.656706597198</v>
+      </c>
+      <c r="J13" s="186" t="s">
+        <v>321</v>
+      </c>
+      <c r="K13" s="187"/>
+      <c r="L13" s="187"/>
+      <c r="M13" s="187"/>
+      <c r="N13" s="187"/>
+      <c r="O13" s="187"/>
+      <c r="P13" s="187"/>
+      <c r="Q13" s="187"/>
+      <c r="R13" s="187"/>
+      <c r="S13" s="187"/>
+      <c r="T13" s="188"/>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
@@ -24363,19 +24211,19 @@
       <c r="I14" s="149">
         <v>44336.775273148101</v>
       </c>
-      <c r="J14" s="185" t="s">
-        <v>321</v>
-      </c>
-      <c r="K14" s="186"/>
-      <c r="L14" s="186"/>
-      <c r="M14" s="186"/>
-      <c r="N14" s="186"/>
-      <c r="O14" s="186"/>
-      <c r="P14" s="186"/>
-      <c r="Q14" s="186"/>
-      <c r="R14" s="186"/>
-      <c r="S14" s="186"/>
-      <c r="T14" s="186"/>
+      <c r="J14" s="189" t="s">
+        <v>320</v>
+      </c>
+      <c r="K14" s="190"/>
+      <c r="L14" s="190"/>
+      <c r="M14" s="190"/>
+      <c r="N14" s="190"/>
+      <c r="O14" s="190"/>
+      <c r="P14" s="190"/>
+      <c r="Q14" s="190"/>
+      <c r="R14" s="190"/>
+      <c r="S14" s="190"/>
+      <c r="T14" s="190"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
@@ -26757,14 +26605,14 @@
         <v>3</v>
       </c>
       <c r="Q79" s="115"/>
-      <c r="R79" s="187" t="s">
+      <c r="R79" s="191" t="s">
         <v>139</v>
       </c>
-      <c r="S79" s="188"/>
-      <c r="T79" s="188"/>
-      <c r="U79" s="188"/>
-      <c r="V79" s="188"/>
-      <c r="W79" s="189"/>
+      <c r="S79" s="192"/>
+      <c r="T79" s="192"/>
+      <c r="U79" s="192"/>
+      <c r="V79" s="192"/>
+      <c r="W79" s="193"/>
       <c r="X79" s="4"/>
       <c r="Y79" s="16"/>
       <c r="Z79" s="1"/>
@@ -26802,12 +26650,12 @@
         <v>3</v>
       </c>
       <c r="Q80" s="115"/>
-      <c r="R80" s="190"/>
-      <c r="S80" s="191"/>
-      <c r="T80" s="191"/>
-      <c r="U80" s="191"/>
-      <c r="V80" s="191"/>
-      <c r="W80" s="192"/>
+      <c r="R80" s="194"/>
+      <c r="S80" s="195"/>
+      <c r="T80" s="195"/>
+      <c r="U80" s="195"/>
+      <c r="V80" s="195"/>
+      <c r="W80" s="196"/>
       <c r="X80" s="4"/>
       <c r="Y80" s="16"/>
       <c r="Z80" s="1"/>
@@ -26843,12 +26691,12 @@
         <v>1</v>
       </c>
       <c r="Q81" s="2"/>
-      <c r="R81" s="193"/>
-      <c r="S81" s="194"/>
-      <c r="T81" s="194"/>
-      <c r="U81" s="194"/>
-      <c r="V81" s="194"/>
-      <c r="W81" s="195"/>
+      <c r="R81" s="197"/>
+      <c r="S81" s="198"/>
+      <c r="T81" s="198"/>
+      <c r="U81" s="198"/>
+      <c r="V81" s="198"/>
+      <c r="W81" s="199"/>
       <c r="X81" s="4"/>
       <c r="Y81" s="16"/>
       <c r="Z81" s="1"/>
@@ -27574,7 +27422,7 @@
       </c>
       <c r="D98" s="4"/>
       <c r="E98" s="5">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="F98" s="5"/>
       <c r="G98" s="4"/>
@@ -27627,7 +27475,7 @@
       </c>
       <c r="D99" s="4"/>
       <c r="E99" s="5">
-        <v>54</v>
+        <v>2</v>
       </c>
       <c r="F99" s="5"/>
       <c r="G99" s="4"/>
@@ -29241,7 +29089,7 @@
       </c>
       <c r="G144" s="13"/>
       <c r="H144" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I144" s="7"/>
       <c r="J144" s="7"/>
@@ -29311,7 +29159,7 @@
       <c r="H146" s="29"/>
       <c r="I146" s="29"/>
       <c r="J146" s="65" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="K146" s="65"/>
       <c r="L146" s="65"/>
@@ -29537,13 +29385,13 @@
       <c r="F152" s="5"/>
       <c r="G152" s="4"/>
       <c r="H152" s="64" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I152" s="31">
         <v>4</v>
       </c>
-      <c r="J152" s="200" t="s">
-        <v>312</v>
+      <c r="J152" s="184" t="s">
+        <v>311</v>
       </c>
       <c r="K152" s="2"/>
       <c r="L152" s="2"/>
@@ -29575,7 +29423,7 @@
       <c r="E153" s="5"/>
       <c r="F153" s="5"/>
       <c r="G153" s="4"/>
-      <c r="H153" s="198"/>
+      <c r="H153" s="182"/>
       <c r="I153" s="2"/>
       <c r="J153" s="2"/>
       <c r="K153" s="2"/>
@@ -29609,7 +29457,7 @@
       <c r="F154" s="5"/>
       <c r="G154" s="4"/>
       <c r="H154" s="64" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I154" s="2"/>
       <c r="J154" s="2"/>
@@ -29643,8 +29491,8 @@
       <c r="E155" s="5"/>
       <c r="F155" s="5"/>
       <c r="G155" s="4"/>
-      <c r="H155" s="201" t="s">
-        <v>320</v>
+      <c r="H155" s="185" t="s">
+        <v>319</v>
       </c>
       <c r="I155" s="2"/>
       <c r="J155" s="31">
@@ -29698,8 +29546,8 @@
       <c r="E156" s="5"/>
       <c r="F156" s="5"/>
       <c r="G156" s="4"/>
-      <c r="H156" s="201" t="s">
-        <v>315</v>
+      <c r="H156" s="185" t="s">
+        <v>314</v>
       </c>
       <c r="I156" s="2"/>
       <c r="J156" s="31">
@@ -30169,129 +30017,19 @@
     <mergeCell ref="R79:W81"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
-  <conditionalFormatting sqref="P99">
-    <cfRule type="expression" dxfId="24" priority="35">
-      <formula>(#REF!&gt;=L$362)</formula>
+  <conditionalFormatting sqref="J97:M99">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>($E97&gt;=$J$78)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q99 U99">
-    <cfRule type="expression" dxfId="23" priority="36">
-      <formula>(#REF!&gt;=L$362)</formula>
+  <conditionalFormatting sqref="O97:R99">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>($E97&gt;=$L$78)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R99">
-    <cfRule type="expression" dxfId="22" priority="37">
-      <formula>(#REF!&gt;=L$362)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="W99">
-    <cfRule type="expression" dxfId="21" priority="38">
-      <formula>(#REF!&gt;=P$362)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V99">
-    <cfRule type="expression" dxfId="20" priority="39">
-      <formula>(#REF!&gt;=P$362)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P98">
-    <cfRule type="expression" dxfId="19" priority="40">
-      <formula>(#REF!&gt;=L$362)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q98 U97:U98">
-    <cfRule type="expression" dxfId="18" priority="41">
-      <formula>(#REF!&gt;=L$362)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R98">
-    <cfRule type="expression" dxfId="17" priority="42">
-      <formula>(#REF!&gt;=L$362)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="W98">
-    <cfRule type="expression" dxfId="16" priority="43">
-      <formula>(#REF!&gt;=P$362)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V98">
-    <cfRule type="expression" dxfId="15" priority="44">
-      <formula>(#REF!&gt;=P$362)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K97">
-    <cfRule type="expression" dxfId="14" priority="45">
-      <formula>(#REF!&gt;=J$362)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M97">
-    <cfRule type="expression" dxfId="13" priority="46">
-      <formula>(#REF!&gt;=J$362)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L97">
-    <cfRule type="expression" dxfId="12" priority="47">
-      <formula>(#REF!&gt;=J$362)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P97">
-    <cfRule type="expression" dxfId="11" priority="48">
-      <formula>(#REF!&gt;=L$362)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q97">
-    <cfRule type="expression" dxfId="10" priority="49">
-      <formula>(#REF!&gt;=L$362)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R97">
-    <cfRule type="expression" dxfId="9" priority="50">
-      <formula>(#REF!&gt;=L$362)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="W97">
-    <cfRule type="expression" dxfId="8" priority="51">
-      <formula>(#REF!&gt;=P$362)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V97">
-    <cfRule type="expression" dxfId="7" priority="52">
-      <formula>(#REF!&gt;=P$362)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O99">
-    <cfRule type="expression" dxfId="6" priority="31">
-      <formula>(#REF!&gt;=K$362)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O98">
-    <cfRule type="expression" dxfId="5" priority="32">
-      <formula>(#REF!&gt;=K$362)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O97">
-    <cfRule type="expression" dxfId="4" priority="33">
-      <formula>(#REF!&gt;=K$362)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T99">
-    <cfRule type="expression" dxfId="3" priority="28">
-      <formula>(#REF!&gt;=P$362)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T98">
-    <cfRule type="expression" dxfId="2" priority="29">
-      <formula>(#REF!&gt;=P$362)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T97">
-    <cfRule type="expression" dxfId="1" priority="30">
-      <formula>(#REF!&gt;=P$362)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I95:I96 I97:J99 K98:M99">
-    <cfRule type="expression" dxfId="0" priority="84">
-      <formula>($E95&gt;=I$362)</formula>
+  <conditionalFormatting sqref="T97:W99">
+    <cfRule type="expression" dxfId="0" priority="86">
+      <formula>($E97&gt;=$P$78)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -31005,23 +30743,23 @@
       <c r="I18" s="31">
         <v>1</v>
       </c>
-      <c r="J18" s="196" t="s">
+      <c r="J18" s="200" t="s">
         <v>22</v>
       </c>
-      <c r="K18" s="196"/>
-      <c r="L18" s="196"/>
-      <c r="M18" s="196"/>
-      <c r="N18" s="196"/>
-      <c r="O18" s="196"/>
-      <c r="P18" s="196"/>
-      <c r="Q18" s="196"/>
-      <c r="R18" s="196"/>
-      <c r="S18" s="196"/>
-      <c r="T18" s="196"/>
-      <c r="U18" s="196"/>
-      <c r="V18" s="196"/>
-      <c r="W18" s="196"/>
-      <c r="X18" s="196"/>
+      <c r="K18" s="200"/>
+      <c r="L18" s="200"/>
+      <c r="M18" s="200"/>
+      <c r="N18" s="200"/>
+      <c r="O18" s="200"/>
+      <c r="P18" s="200"/>
+      <c r="Q18" s="200"/>
+      <c r="R18" s="200"/>
+      <c r="S18" s="200"/>
+      <c r="T18" s="200"/>
+      <c r="U18" s="200"/>
+      <c r="V18" s="200"/>
+      <c r="W18" s="200"/>
+      <c r="X18" s="200"/>
       <c r="Y18" s="2"/>
       <c r="Z18" s="4"/>
       <c r="AA18" s="16"/>
@@ -31116,23 +30854,23 @@
       <c r="I21" s="23">
         <v>1</v>
       </c>
-      <c r="J21" s="185" t="s">
+      <c r="J21" s="189" t="s">
         <v>34</v>
       </c>
-      <c r="K21" s="186"/>
-      <c r="L21" s="186"/>
-      <c r="M21" s="186"/>
-      <c r="N21" s="186"/>
-      <c r="O21" s="186"/>
-      <c r="P21" s="186"/>
-      <c r="Q21" s="186"/>
-      <c r="R21" s="186"/>
-      <c r="S21" s="186"/>
-      <c r="T21" s="186"/>
-      <c r="U21" s="186"/>
-      <c r="V21" s="186"/>
-      <c r="W21" s="186"/>
-      <c r="X21" s="197"/>
+      <c r="K21" s="190"/>
+      <c r="L21" s="190"/>
+      <c r="M21" s="190"/>
+      <c r="N21" s="190"/>
+      <c r="O21" s="190"/>
+      <c r="P21" s="190"/>
+      <c r="Q21" s="190"/>
+      <c r="R21" s="190"/>
+      <c r="S21" s="190"/>
+      <c r="T21" s="190"/>
+      <c r="U21" s="190"/>
+      <c r="V21" s="190"/>
+      <c r="W21" s="190"/>
+      <c r="X21" s="201"/>
       <c r="Y21" s="2"/>
       <c r="Z21" s="4"/>
       <c r="AA21" s="16"/>

</xml_diff>

<commit_message>
new cashflow structure (seems to be working 8k profit difference to old version but working capital con is not hooked up)
</commit_message>
<xml_diff>
--- a/Structural.xlsx
+++ b/Structural.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\Models\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A6276BC-995C-4E18-AADB-A1A959829EEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{035A5233-F855-4DE6-BEFA-AEFC1AB2C32F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
@@ -57,6 +57,7 @@
     <definedName name="i_dvp_mask_f3">StructuralSA!$J$53:$L$53</definedName>
     <definedName name="i_e0_pos">Stock!$I$48</definedName>
     <definedName name="i_e1_pos">Stock!$I$49</definedName>
+    <definedName name="i_enterprises_c0" localSheetId="0">General!$I$56:$J$56</definedName>
     <definedName name="i_feedsupply_itn_max">Stock!$I$72</definedName>
     <definedName name="i_fixed_dvp_mask_f1">Stock!$J$314:$L$314</definedName>
     <definedName name="i_fixed_fvp_mask_dams">Stock!$J$312:$L$312</definedName>
@@ -1570,7 +1571,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="314">
   <si>
     <t>Controls for this worksheet</t>
   </si>
@@ -2609,6 +2610,15 @@
 30Mar21: Added inputs for % dry and number dams mated
 2: 17Jul20-Added structural inputs table
 1: 1Apr19-Created the version control table</t>
+  </si>
+  <si>
+    <t>enterprises</t>
+  </si>
+  <si>
+    <t>stk</t>
+  </si>
+  <si>
+    <t>crp</t>
   </si>
 </sst>
 </file>
@@ -5047,7 +5057,7 @@
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="N49" sqref="N49"/>
+      <selection pane="bottomRight" activeCell="I56" sqref="I56:J56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -7086,9 +7096,15 @@
       <c r="E56" s="5"/>
       <c r="F56" s="5"/>
       <c r="G56" s="4"/>
-      <c r="H56" s="2"/>
-      <c r="I56" s="2"/>
-      <c r="J56" s="2"/>
+      <c r="H56" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="I56" s="101" t="s">
+        <v>312</v>
+      </c>
+      <c r="J56" s="101" t="s">
+        <v>313</v>
+      </c>
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
       <c r="M56" s="2"/>

</xml_diff>

<commit_message>
Add confinement to the inputs
</commit_message>
<xml_diff>
--- a/Structural.xlsx
+++ b/Structural.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\Models\AFO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{035A5233-F855-4DE6-BEFA-AEFC1AB2C32F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D00D9423-4D5C-4344-90E9-F78BB70E51A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="29895" yWindow="600" windowWidth="27705" windowHeight="15630" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -48,11 +48,14 @@
     <definedName name="i_b0_pos">Stock!$I$45</definedName>
     <definedName name="i_b1_pos">Stock!$I$46</definedName>
     <definedName name="i_btrt_idx_offs">Stock!$L$268:$Q$268</definedName>
+    <definedName name="i_confinement_n0">StructuralSA!$K$83</definedName>
+    <definedName name="i_confinement_n1">StructuralSA!$N$83:$N$90</definedName>
+    <definedName name="i_confinement_n3">StructuralSA!$T$83:$T$90</definedName>
     <definedName name="i_core_dvp_types_f1" localSheetId="1">Stock!$J$313:$L$313</definedName>
     <definedName name="i_d_pos">Stock!$I$47</definedName>
-    <definedName name="i_density_n0" localSheetId="2">StructuralSA!$K$83</definedName>
-    <definedName name="i_density_n1" localSheetId="2">StructuralSA!$M$83:$M$90</definedName>
-    <definedName name="i_density_n3" localSheetId="2">StructuralSA!$Q$83:$Q$90</definedName>
+    <definedName name="i_density_n0" localSheetId="2">StructuralSA!$L$83</definedName>
+    <definedName name="i_density_n1" localSheetId="2">StructuralSA!$O$83:$O$90</definedName>
+    <definedName name="i_density_n3" localSheetId="2">StructuralSA!$U$83:$U$90</definedName>
     <definedName name="i_dvp_mask_f1">StructuralSA!$N$44:$O$44</definedName>
     <definedName name="i_dvp_mask_f3">StructuralSA!$J$53:$L$53</definedName>
     <definedName name="i_e0_pos">Stock!$I$48</definedName>
@@ -94,25 +97,25 @@
     <definedName name="i_n_r1type">Stock!$L$206</definedName>
     <definedName name="i_n0_len">StructuralSA!$J$77</definedName>
     <definedName name="i_n0_matrix_len">StructuralSA!$J$79</definedName>
-    <definedName name="i_n1_len">StructuralSA!$L$77</definedName>
-    <definedName name="i_n1_matrix_len">StructuralSA!$L$79</definedName>
-    <definedName name="i_n2_len">StructuralSA!$L$77</definedName>
-    <definedName name="i_n3_len">StructuralSA!$P$77</definedName>
-    <definedName name="i_n3_matrix_len">StructuralSA!$P$79</definedName>
+    <definedName name="i_n1_len">StructuralSA!$M$77</definedName>
+    <definedName name="i_n1_matrix_len">StructuralSA!$M$79</definedName>
+    <definedName name="i_n2_len">StructuralSA!$M$77</definedName>
+    <definedName name="i_n3_len">StructuralSA!$S$77</definedName>
+    <definedName name="i_n3_matrix_len">StructuralSA!$S$79</definedName>
     <definedName name="i_numbers_min_b1">Stock!$L$156:$V$156</definedName>
     <definedName name="i_nut_spread_n0" localSheetId="2">StructuralSA!$J$83</definedName>
-    <definedName name="i_nut_spread_n1" localSheetId="2">StructuralSA!$L$83:$L$90</definedName>
-    <definedName name="i_nut_spread_n3" localSheetId="2">StructuralSA!$P$83:$P$90</definedName>
+    <definedName name="i_nut_spread_n1" localSheetId="2">StructuralSA!$M$83:$M$90</definedName>
+    <definedName name="i_nut_spread_n3" localSheetId="2">StructuralSA!$S$83:$S$90</definedName>
     <definedName name="i_nv_lower_p6">StructuralSA!$J$153:$S$153</definedName>
     <definedName name="i_nv_upper_p6">StructuralSA!$J$154:$S$154</definedName>
     <definedName name="i_p_pos">Stock!$I$55</definedName>
     <definedName name="i_prejoin_offset">Stock!$I$66</definedName>
-    <definedName name="i_progeny_w2_len">StructuralSA!$O$75</definedName>
+    <definedName name="i_progeny_w2_len">StructuralSA!$Q$75</definedName>
     <definedName name="i_sim_periods_year">Stock!$I$62</definedName>
     <definedName name="i_transfer_exists_tg1">Stock!$K$119:$N$121</definedName>
     <definedName name="i_w_pos">Stock!$I$56</definedName>
-    <definedName name="i_w_start_len1">StructuralSA!$L$76</definedName>
-    <definedName name="i_w_start_len3">StructuralSA!$P$76</definedName>
+    <definedName name="i_w_start_len1">StructuralSA!$M$76</definedName>
+    <definedName name="i_w_start_len3">StructuralSA!$S$76</definedName>
     <definedName name="i_w0_len">StructuralSA!$J$75</definedName>
     <definedName name="i_x_pos">Stock!$I$57</definedName>
     <definedName name="i_y_pos">Stock!$I$58</definedName>
@@ -156,9 +159,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1293,7 +1294,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L76" authorId="0" shapeId="0" xr:uid="{957206BF-28F7-4DCB-855B-7955BBC3DD41}">
+    <comment ref="M76" authorId="0" shapeId="0" xr:uid="{957206BF-28F7-4DCB-855B-7955BBC3DD41}">
       <text>
         <r>
           <rPr>
@@ -1318,7 +1319,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P76" authorId="0" shapeId="0" xr:uid="{D3F3BA59-396C-4A97-891A-8BB313E15EEB}">
+    <comment ref="S76" authorId="0" shapeId="0" xr:uid="{D3F3BA59-396C-4A97-891A-8BB313E15EEB}">
       <text>
         <r>
           <rPr>
@@ -1340,6 +1341,31 @@
           <t xml:space="preserve">
 This can only be 2 or 3.
 if you want more than 3 you will need to modify f_condense</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H78" authorId="1" shapeId="0" xr:uid="{2126B92C-6ACE-4F21-831E-B8B538AEDA39}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>John:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+In version 1 the year is split into fvp_periods &amp; each inlcudes all the nutrition levels. At the end of the fvp_period the profile splits into each of the nutrition levels for the next period.
+i.e. at the end of a feed variation period the profiles don't collapse back to common starting weights in the next period, like they do for the decision variable periods.</t>
         </r>
       </text>
     </comment>
@@ -1370,7 +1396,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K82" authorId="1" shapeId="0" xr:uid="{C8F7BE02-A498-419E-B390-39EA169EF5C2}">
+    <comment ref="L82" authorId="1" shapeId="0" xr:uid="{C8F7BE02-A498-419E-B390-39EA169EF5C2}">
       <text>
         <r>
           <rPr>
@@ -1391,6 +1417,30 @@
           </rPr>
           <t xml:space="preserve">
 Scalar of the stock density entered in the MIDAS feed periods.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S89" authorId="1" shapeId="0" xr:uid="{7104E76F-9C27-4C3A-B5E1-62B91C191243}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>John:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+A large number to ensure that the NV is at the maximum value, to represent an ad lib ration.</t>
         </r>
       </text>
     </comment>
@@ -1571,7 +1621,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="314">
   <si>
     <t>Controls for this worksheet</t>
   </si>
@@ -1988,10 +2038,6 @@
   </si>
   <si>
     <t>if e1 is not identified then all in k2[0:10]</t>
-  </si>
-  <si>
-    <t>In version 1 the year is split into fvp_periods &amp; each inlcudes all the nutrition levels. At the end of the fvp_period the profile splits into each of the nutrition levels for the next period.
-i.e. at the end of a feed variation period the profiles don't collapse back to common starting weights in the next period, like they do for the decision variable periods.</t>
   </si>
   <si>
     <t>The post processing cluster (k2) for this LSLN (add 11*index_e1 if scan=4)</t>
@@ -2586,23 +2632,6 @@
     <t>is DVP</t>
   </si>
   <si>
-    <t>11/Jul/21: dvp/fvp updates -  to go with node structure (remove season dvp/fvp)
-30Jun21: Change rangename from fev to nv
-24Jun21: Fix the conditional formatting in the Initial LW section.  
-                  Add inputs for the user defined feed pools
-20May21: Add extra N for dams (now 8)
-16May21: Add extra TOL to the extra FVP date
-5May21: Adjust the extra FVP date for TOL[0] (for GEPEP calibration)
-4May21: add random rev
-29Apr21: Added the fixed DVPs to the formula for the number of dam FVPs
-27Apr21: add named ranges to inputs copied from pinp.
-                   Add REV inputs
-                    Split fvp inputs
-25Apr21: Moved inputs from Property.xlsx
-                   Moved FVP &amp; N inputs from Stock
-1: 1Apr19-Created the version control table</t>
-  </si>
-  <si>
     <t>11/Jul/21: dvp/fvp updates 
 27Apr21: Split fvp inputs
 25Apr21: Deleted range names i_w1_len &amp; w3
@@ -2620,6 +2649,27 @@
   <si>
     <t>crp</t>
   </si>
+  <si>
+    <t>Confinement</t>
+  </si>
+  <si>
+    <t>26Nov21: Add confinement to the nutspread inputs.
+11Jul21: dvp/fvp updates -  to go with node structure (remove season dvp/fvp)
+30Jun21: Change rangename from fev to nv
+24Jun21: Fix the conditional formatting in the Initial LW section.  
+                  Add inputs for the user defined feed pools
+20May21: Add extra N for dams (now 8)
+16May21: Add extra TOL to the extra FVP date
+5May21: Adjust the extra FVP date for TOL[0] (for GEPEP calibration)
+4May21: add random rev
+29Apr21: Added the fixed DVPs to the formula for the number of dam FVPs
+27Apr21: add named ranges to inputs copied from pinp.
+                   Add REV inputs
+                    Split fvp inputs
+25Apr21: Moved inputs from Property.xlsx
+                   Moved FVP &amp; N inputs from Stock
+1: 1Apr19-Created the version control table</t>
+  </si>
 </sst>
 </file>
 
@@ -2628,7 +2678,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2807,12 +2857,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
     <font>
       <sz val="9"/>
@@ -3032,7 +3076,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="60">
+  <borders count="55">
     <border>
       <left/>
       <right/>
@@ -3545,61 +3589,8 @@
         <color theme="0" tint="-0.24994659260841701"/>
       </left>
       <right/>
-      <top style="hair">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="hair">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="hair">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </right>
-      <top style="hair">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </left>
-      <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="hair">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="hair">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </right>
-      <top/>
-      <bottom style="hair">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -3769,7 +3760,7 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" applyNumberFormat="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="55" applyNumberFormat="0" applyFont="0" applyAlignment="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="50" applyNumberFormat="0" applyFont="0" applyAlignment="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="24" applyNumberFormat="0" applyFont="0" applyAlignment="0">
@@ -3859,7 +3850,7 @@
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="201">
+  <cellXfs count="193">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="25" xfId="3">
@@ -3956,7 +3947,7 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="8" applyBorder="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="55" xfId="13">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="50" xfId="13">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="1" applyBorder="1">
@@ -4159,7 +4150,7 @@
     <xf numFmtId="0" fontId="15" fillId="8" borderId="29" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="55" xfId="13" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="50" xfId="13" applyFont="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="24" xfId="16" applyFont="1">
@@ -4186,7 +4177,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="28" fillId="10" borderId="0" xfId="18" applyFont="1">
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" xfId="18" applyFont="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -4200,7 +4191,7 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="25" xfId="3" applyNumberFormat="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="46" xfId="11" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="43" xfId="11" applyBorder="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="11" borderId="1" xfId="12" applyNumberFormat="1">
@@ -4222,16 +4213,16 @@
     <xf numFmtId="15" fontId="1" fillId="11" borderId="1" xfId="12" applyNumberFormat="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="49" xfId="7" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="44" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="18" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="50" xfId="7" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="45" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="51" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="46" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="10" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4240,10 +4231,10 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="52" xfId="7" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="47" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="53" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="48" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="10" borderId="16" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4252,22 +4243,22 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="16" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="54" xfId="7" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="49" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="56" xfId="12" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="51" xfId="12" applyBorder="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="57" xfId="13" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="52" xfId="13" applyFont="1" applyBorder="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="58" xfId="13" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="53" xfId="13" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="55" xfId="13" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="50" xfId="13" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="59" xfId="13" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="54" xfId="13" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="27" xfId="41" applyBorder="1" applyAlignment="1">
@@ -4279,10 +4270,10 @@
     <xf numFmtId="0" fontId="16" fillId="34" borderId="33" xfId="41" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="51" xfId="7" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="46" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="53" xfId="7" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="48" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="43" applyBorder="1">
@@ -4342,39 +4333,15 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="43" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="44" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="36" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="12" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="23" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="25" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -4551,16 +4518,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>80</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>114301</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>154781</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>91</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>357187</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4575,8 +4542,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11391900" y="13544550"/>
-          <a:ext cx="4524375" cy="1866900"/>
+          <a:off x="13032582" y="10941844"/>
+          <a:ext cx="3886199" cy="1083469"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4616,7 +4583,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-AU" sz="1000" baseline="0"/>
-            <a:t> of nut spread is controlled in the table above.</a:t>
+            <a:t> of nut spread is controlled in this table.</a:t>
           </a:r>
           <a:endParaRPr lang="en-AU" sz="1000"/>
         </a:p>
@@ -4627,19 +4594,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-AU" sz="1000" baseline="0"/>
-            <a:t> when there is 2n:</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-AU" sz="1000" baseline="0"/>
-            <a:t>High spread</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-AU" sz="1000" baseline="0"/>
-            <a:t>Low </a:t>
+            <a:t> when there is 2n: High spread, Low </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-AU" sz="1000" baseline="0">
@@ -4658,13 +4613,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-AU" sz="1000" baseline="0"/>
-            <a:t>When there is 3n or greater:</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-AU" sz="1000" baseline="0"/>
-            <a:t>Medium </a:t>
+            <a:t>When there is 3n or greater: Medium </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-AU" sz="1000" baseline="0">
@@ -4676,11 +4625,8 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>spread</a:t>
+            <a:t>spread, </a:t>
           </a:r>
-          <a:endParaRPr lang="en-AU" sz="1000" baseline="0"/>
-        </a:p>
-        <a:p>
           <a:r>
             <a:rPr lang="en-AU" sz="1000" baseline="0"/>
             <a:t>High </a:t>
@@ -4695,11 +4641,8 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>spread</a:t>
+            <a:t>spread, </a:t>
           </a:r>
-          <a:endParaRPr lang="en-AU" sz="1000" baseline="0"/>
-        </a:p>
-        <a:p>
           <a:r>
             <a:rPr lang="en-AU" sz="1000" baseline="0"/>
             <a:t>Low </a:t>
@@ -4739,7 +4682,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Note: the order of the dams nut spread affects LTW effects because Offspring use LTW adjustments from dams w[0] (because w[0] is the best estimate of the optimum profile. </a:t>
+            <a:t>Note: the order of the dams nut spread affects LTW effects because Offspring use LTW adjustments from dams w[0] (because w[0] is the best estimate of the optimum profile). </a:t>
           </a:r>
           <a:endParaRPr lang="en-AU" sz="1000"/>
         </a:p>
@@ -5052,8 +4995,8 @@
   </sheetPr>
   <dimension ref="A1:AT69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <pane xSplit="9" ySplit="10" topLeftCell="J40" activePane="bottomRight" state="frozen"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <pane xSplit="9" ySplit="10" topLeftCell="J16" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
@@ -5403,7 +5346,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="29"/>
       <c r="I9" s="29" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J9" s="29" t="s">
         <v>5</v>
@@ -5552,7 +5495,7 @@
         <v>44371.659649305599</v>
       </c>
       <c r="J13" s="185" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K13" s="186"/>
       <c r="L13" s="186"/>
@@ -5591,7 +5534,7 @@
         <v>44371.660335300898</v>
       </c>
       <c r="J14" s="188" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="K14" s="189"/>
       <c r="L14" s="189"/>
@@ -6573,16 +6516,16 @@
       <c r="F42" s="5"/>
       <c r="G42" s="4"/>
       <c r="H42" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="I42" s="101" t="s">
         <v>165</v>
       </c>
-      <c r="I42" s="101" t="s">
+      <c r="J42" s="101" t="s">
         <v>166</v>
       </c>
-      <c r="J42" s="101" t="s">
+      <c r="K42" s="101" t="s">
         <v>167</v>
-      </c>
-      <c r="K42" s="101" t="s">
-        <v>168</v>
       </c>
       <c r="L42" s="142"/>
       <c r="M42" s="2"/>
@@ -6647,13 +6590,13 @@
       <c r="F44" s="5"/>
       <c r="G44" s="4"/>
       <c r="H44" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I44" s="101" t="s">
         <v>169</v>
       </c>
-      <c r="I44" s="101" t="s">
+      <c r="J44" s="101" t="s">
         <v>170</v>
-      </c>
-      <c r="J44" s="101" t="s">
-        <v>171</v>
       </c>
       <c r="K44" s="142"/>
       <c r="L44" s="142"/>
@@ -6719,16 +6662,16 @@
       <c r="F46" s="5"/>
       <c r="G46" s="4"/>
       <c r="H46" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I46" s="101" t="s">
+        <v>176</v>
+      </c>
+      <c r="J46" s="101" t="s">
         <v>177</v>
       </c>
-      <c r="J46" s="101" t="s">
+      <c r="K46" s="101" t="s">
         <v>178</v>
-      </c>
-      <c r="K46" s="101" t="s">
-        <v>179</v>
       </c>
       <c r="L46" s="142"/>
       <c r="M46" s="2"/>
@@ -6760,7 +6703,7 @@
       <c r="F47" s="5"/>
       <c r="G47" s="4"/>
       <c r="H47" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I47" s="101" t="b">
         <v>1</v>
@@ -6801,13 +6744,13 @@
       <c r="F48" s="5"/>
       <c r="G48" s="4"/>
       <c r="H48" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I48" s="101" t="s">
+        <v>179</v>
+      </c>
+      <c r="J48" s="101" t="s">
         <v>180</v>
-      </c>
-      <c r="J48" s="101" t="s">
-        <v>181</v>
       </c>
       <c r="K48" s="142"/>
       <c r="L48" s="142"/>
@@ -6840,19 +6783,19 @@
       <c r="F49" s="5"/>
       <c r="G49" s="4"/>
       <c r="H49" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I49" s="101" t="s">
+        <v>181</v>
+      </c>
+      <c r="J49" s="101" t="s">
         <v>182</v>
       </c>
-      <c r="J49" s="101" t="s">
+      <c r="K49" s="101" t="s">
+        <v>268</v>
+      </c>
+      <c r="L49" s="101" t="s">
         <v>183</v>
-      </c>
-      <c r="K49" s="101" t="s">
-        <v>269</v>
-      </c>
-      <c r="L49" s="101" t="s">
-        <v>184</v>
       </c>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -6883,16 +6826,16 @@
       <c r="F50" s="5"/>
       <c r="G50" s="4"/>
       <c r="H50" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I50" s="101" t="s">
+        <v>184</v>
+      </c>
+      <c r="J50" s="101" t="s">
         <v>185</v>
       </c>
-      <c r="J50" s="101" t="s">
+      <c r="K50" s="101" t="s">
         <v>186</v>
-      </c>
-      <c r="K50" s="101" t="s">
-        <v>187</v>
       </c>
       <c r="L50" s="142"/>
       <c r="M50" s="2"/>
@@ -6957,7 +6900,7 @@
       <c r="F52" s="5"/>
       <c r="G52" s="4"/>
       <c r="H52" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I52" s="101">
         <v>6</v>
@@ -7027,7 +6970,7 @@
       <c r="F54" s="5"/>
       <c r="G54" s="4"/>
       <c r="H54" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I54" s="101">
         <v>1</v>
@@ -7097,13 +7040,13 @@
       <c r="F56" s="5"/>
       <c r="G56" s="4"/>
       <c r="H56" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="I56" s="101" t="s">
+        <v>310</v>
+      </c>
+      <c r="J56" s="101" t="s">
         <v>311</v>
-      </c>
-      <c r="I56" s="101" t="s">
-        <v>312</v>
-      </c>
-      <c r="J56" s="101" t="s">
-        <v>313</v>
       </c>
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
@@ -7548,11 +7491,11 @@
   <dimension ref="A1:AE334"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <pane xSplit="9" ySplit="10" topLeftCell="J301" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="10" topLeftCell="J305" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="J13" sqref="J13:T13"/>
+      <selection pane="bottomRight" activeCell="J315" sqref="J315"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -7896,7 +7839,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="29"/>
       <c r="I9" s="29" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J9" s="29" t="s">
         <v>5</v>
@@ -8045,7 +7988,7 @@
         <v>44311.756953009302</v>
       </c>
       <c r="J13" s="185" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="K13" s="186"/>
       <c r="L13" s="186"/>
@@ -8066,7 +8009,7 @@
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
     </row>
-    <row r="14" spans="1:28" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" ht="45" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="33"/>
       <c r="C14" s="67">
@@ -8084,7 +8027,7 @@
         <v>44355.378988657401</v>
       </c>
       <c r="J14" s="188" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K14" s="189"/>
       <c r="L14" s="189"/>
@@ -8105,7 +8048,7 @@
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
     </row>
-    <row r="15" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="33"/>
       <c r="C15" s="67">
@@ -8140,7 +8083,7 @@
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
     </row>
-    <row r="16" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="33"/>
       <c r="C16" s="67">
@@ -8175,7 +8118,7 @@
       <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>
     </row>
-    <row r="17" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="33"/>
       <c r="C17" s="67">
@@ -8222,7 +8165,7 @@
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
     </row>
-    <row r="18" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="33"/>
       <c r="C18" s="67">
@@ -8259,7 +8202,7 @@
       <c r="AA18" s="1"/>
       <c r="AB18" s="1"/>
     </row>
-    <row r="19" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="33"/>
       <c r="C19" s="67">
@@ -8296,7 +8239,7 @@
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
     </row>
-    <row r="20" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="33"/>
       <c r="C20" s="67">
@@ -8333,7 +8276,7 @@
       <c r="AA20" s="1"/>
       <c r="AB20" s="1"/>
     </row>
-    <row r="21" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="33"/>
       <c r="C21" s="67">
@@ -8370,7 +8313,7 @@
       <c r="AA21" s="1"/>
       <c r="AB21" s="1"/>
     </row>
-    <row r="22" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="33"/>
       <c r="C22" s="67">
@@ -8405,7 +8348,7 @@
       <c r="AA22" s="1"/>
       <c r="AB22" s="1"/>
     </row>
-    <row r="23" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="33"/>
       <c r="C23" s="67">
@@ -9064,13 +9007,13 @@
       <c r="F42" s="5"/>
       <c r="G42" s="4"/>
       <c r="H42" s="182" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I42" s="36" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
@@ -9103,7 +9046,7 @@
       <c r="F43" s="5"/>
       <c r="G43" s="4"/>
       <c r="H43" s="113" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I43" s="31">
         <v>-6</v>
@@ -9140,7 +9083,7 @@
       <c r="F44" s="5"/>
       <c r="G44" s="4"/>
       <c r="H44" s="113" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I44" s="31">
         <v>-14</v>
@@ -9177,7 +9120,7 @@
       <c r="F45" s="5"/>
       <c r="G45" s="4"/>
       <c r="H45" s="113" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I45" s="31">
         <v>-4</v>
@@ -9214,7 +9157,7 @@
       <c r="F46" s="5"/>
       <c r="G46" s="4"/>
       <c r="H46" s="113" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I46" s="31">
         <v>-12</v>
@@ -9251,7 +9194,7 @@
       <c r="F47" s="5"/>
       <c r="G47" s="4"/>
       <c r="H47" s="113" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I47" s="31">
         <v>-7</v>
@@ -9288,7 +9231,7 @@
       <c r="F48" s="5"/>
       <c r="G48" s="4"/>
       <c r="H48" s="113" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I48" s="31">
         <v>-5</v>
@@ -9325,7 +9268,7 @@
       <c r="F49" s="5"/>
       <c r="G49" s="4"/>
       <c r="H49" s="113" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I49" s="31">
         <v>-13</v>
@@ -9362,7 +9305,7 @@
       <c r="F50" s="5"/>
       <c r="G50" s="4"/>
       <c r="H50" s="113" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I50" s="31">
         <v>-8</v>
@@ -9399,7 +9342,7 @@
       <c r="F51" s="5"/>
       <c r="G51" s="4"/>
       <c r="H51" s="113" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I51" s="31">
         <v>-17</v>
@@ -9436,7 +9379,7 @@
       <c r="F52" s="5"/>
       <c r="G52" s="4"/>
       <c r="H52" s="113" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I52" s="31">
         <v>-18</v>
@@ -9473,7 +9416,7 @@
       <c r="F53" s="5"/>
       <c r="G53" s="4"/>
       <c r="H53" s="113" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I53" s="31">
         <v>-17</v>
@@ -9510,7 +9453,7 @@
       <c r="F54" s="5"/>
       <c r="G54" s="4"/>
       <c r="H54" s="113" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I54" s="31">
         <v>-11</v>
@@ -9547,7 +9490,7 @@
       <c r="F55" s="5"/>
       <c r="G55" s="4"/>
       <c r="H55" s="113" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I55" s="31">
         <v>-15</v>
@@ -9584,7 +9527,7 @@
       <c r="F56" s="5"/>
       <c r="G56" s="4"/>
       <c r="H56" s="113" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I56" s="31">
         <v>-10</v>
@@ -9623,7 +9566,7 @@
       <c r="F57" s="5"/>
       <c r="G57" s="4"/>
       <c r="H57" s="113" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I57" s="31">
         <v>-3</v>
@@ -9660,7 +9603,7 @@
       <c r="F58" s="5"/>
       <c r="G58" s="4"/>
       <c r="H58" s="113" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I58" s="31">
         <v>-2</v>
@@ -9697,7 +9640,7 @@
       <c r="F59" s="5"/>
       <c r="G59" s="4"/>
       <c r="H59" s="113" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I59" s="31">
         <v>-9</v>
@@ -9767,10 +9710,10 @@
       <c r="F61" s="5"/>
       <c r="G61" s="4"/>
       <c r="H61" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I61" s="36" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
@@ -9841,7 +9784,7 @@
       <c r="F63" s="5"/>
       <c r="G63" s="4"/>
       <c r="H63" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I63" s="31">
         <v>7.25</v>
@@ -9850,7 +9793,7 @@
         <v>86</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L63" s="2"/>
       <c r="M63" s="2"/>
@@ -9882,7 +9825,7 @@
       <c r="F64" s="5"/>
       <c r="G64" s="4"/>
       <c r="H64" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I64" s="31">
         <v>4.25</v>
@@ -9891,7 +9834,7 @@
         <v>86</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L64" s="2"/>
       <c r="M64" s="2"/>
@@ -9956,7 +9899,7 @@
       <c r="F66" s="5"/>
       <c r="G66" s="4"/>
       <c r="H66" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I66" s="31">
         <v>8</v>
@@ -11005,7 +10948,7 @@
       <c r="F95" s="5"/>
       <c r="G95" s="4"/>
       <c r="H95" s="116" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I95" s="2"/>
       <c r="J95" s="2" t="s">
@@ -11056,7 +10999,7 @@
       <c r="F96" s="5"/>
       <c r="G96" s="4"/>
       <c r="H96" s="116" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I96" s="2"/>
       <c r="J96" s="2" t="s">
@@ -11909,10 +11852,10 @@
       <c r="F115" s="5"/>
       <c r="G115" s="4"/>
       <c r="H115" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I115" s="26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J115" s="2" t="s">
         <v>41</v>
@@ -11957,7 +11900,7 @@
       <c r="F116" s="5"/>
       <c r="G116" s="4"/>
       <c r="H116" s="116" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I116" s="2"/>
       <c r="J116" s="2" t="s">
@@ -12079,10 +12022,10 @@
       <c r="F119" s="5"/>
       <c r="G119" s="4"/>
       <c r="H119" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="I119" s="26" t="s">
         <v>144</v>
-      </c>
-      <c r="I119" s="26" t="s">
-        <v>145</v>
       </c>
       <c r="J119" s="2" t="s">
         <v>41</v>
@@ -12126,7 +12069,7 @@
       <c r="F120" s="5"/>
       <c r="G120" s="4"/>
       <c r="H120" s="116" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I120" s="2"/>
       <c r="J120" s="2" t="s">
@@ -13261,7 +13204,7 @@
       <c r="F149" s="5"/>
       <c r="G149" s="4"/>
       <c r="H149" s="64" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I149" s="2"/>
       <c r="J149" s="2"/>
@@ -13318,7 +13261,7 @@
       <c r="F150" s="5"/>
       <c r="G150" s="4"/>
       <c r="H150" s="64" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I150" s="2"/>
       <c r="J150" s="2"/>
@@ -13432,7 +13375,7 @@
       <c r="F152" s="5"/>
       <c r="G152" s="4"/>
       <c r="H152" s="64" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I152" s="2"/>
       <c r="J152" s="2"/>
@@ -13663,7 +13606,7 @@
       <c r="F156" s="5"/>
       <c r="G156" s="4"/>
       <c r="H156" s="64" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I156" s="2"/>
       <c r="J156" s="2"/>
@@ -13756,7 +13699,7 @@
       <c r="F158" s="5"/>
       <c r="G158" s="4"/>
       <c r="H158" s="59" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I158" s="60" t="str">
         <f>"("&amp;ROWS(ia_k2_mlsb1)-2&amp;","&amp;COLUMNS(ia_k2_mlsb1)-1&amp;"): ia_k2_mlsb1(pointers) = input"</f>
@@ -13978,7 +13921,7 @@
       </c>
       <c r="I162" s="103"/>
       <c r="J162" s="103" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K162" s="56">
         <v>1</v>
@@ -14277,7 +14220,7 @@
       </c>
       <c r="I167" s="79"/>
       <c r="J167" s="56" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K167" s="56">
         <v>1</v>
@@ -14749,7 +14692,7 @@
       <c r="F175" s="5"/>
       <c r="G175" s="4"/>
       <c r="H175" s="64" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="I175" s="103"/>
       <c r="J175" s="63"/>
@@ -14808,7 +14751,7 @@
       <c r="F176" s="5"/>
       <c r="G176" s="4"/>
       <c r="H176" s="113" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I176" s="79"/>
       <c r="J176" s="61">
@@ -14869,11 +14812,11 @@
       <c r="F177" s="5"/>
       <c r="G177" s="4"/>
       <c r="H177" s="113" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I177" s="79"/>
       <c r="J177" s="56" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K177" s="56">
         <v>1</v>
@@ -14930,7 +14873,7 @@
       <c r="F178" s="5"/>
       <c r="G178" s="4"/>
       <c r="H178" s="113" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I178" s="79"/>
       <c r="J178" s="56"/>
@@ -14989,7 +14932,7 @@
       <c r="F179" s="5"/>
       <c r="G179" s="4"/>
       <c r="H179" s="113" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I179" s="79"/>
       <c r="J179" s="56"/>
@@ -15048,7 +14991,7 @@
       <c r="F180" s="5"/>
       <c r="G180" s="4"/>
       <c r="H180" s="113" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I180" s="62"/>
       <c r="J180" s="63"/>
@@ -15107,7 +15050,7 @@
       <c r="F181" s="5"/>
       <c r="G181" s="4"/>
       <c r="H181" s="113" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I181" s="112">
         <v>1</v>
@@ -15170,7 +15113,7 @@
       <c r="F182" s="5"/>
       <c r="G182" s="4"/>
       <c r="H182" s="113" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I182" s="103"/>
       <c r="J182" s="103"/>
@@ -15229,7 +15172,7 @@
       <c r="F183" s="5"/>
       <c r="G183" s="4"/>
       <c r="H183" s="113" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I183" s="103"/>
       <c r="J183" s="103"/>
@@ -16298,7 +16241,7 @@
       <c r="F202" s="5"/>
       <c r="G202" s="4"/>
       <c r="H202" s="59" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I202" s="60" t="str">
         <f>"("&amp;ROWS(ia_ppk2g1_rlsb1)-2&amp;","&amp;COLUMNS(ia_ppk2g1_rlsb1)-1&amp;"): ia_ppk2_vlsb1(pointers) = input"</f>
@@ -16307,37 +16250,37 @@
       <c r="J202" s="49"/>
       <c r="K202" s="49"/>
       <c r="L202" s="150" t="s">
+        <v>227</v>
+      </c>
+      <c r="M202" s="151" t="s">
         <v>228</v>
       </c>
-      <c r="M202" s="151" t="s">
+      <c r="N202" s="151" t="s">
         <v>229</v>
       </c>
-      <c r="N202" s="151" t="s">
+      <c r="O202" s="151" t="s">
         <v>230</v>
       </c>
-      <c r="O202" s="151" t="s">
+      <c r="P202" s="151" t="s">
         <v>231</v>
       </c>
-      <c r="P202" s="151" t="s">
+      <c r="Q202" s="151" t="s">
         <v>232</v>
       </c>
-      <c r="Q202" s="151" t="s">
+      <c r="R202" s="151" t="s">
         <v>233</v>
       </c>
-      <c r="R202" s="151" t="s">
+      <c r="S202" s="151" t="s">
         <v>234</v>
       </c>
-      <c r="S202" s="151" t="s">
+      <c r="T202" s="151" t="s">
         <v>235</v>
       </c>
-      <c r="T202" s="151" t="s">
+      <c r="U202" s="151" t="s">
         <v>236</v>
       </c>
-      <c r="U202" s="151" t="s">
+      <c r="V202" s="152" t="s">
         <v>237</v>
-      </c>
-      <c r="V202" s="152" t="s">
-        <v>238</v>
       </c>
       <c r="W202" s="94"/>
       <c r="X202" s="4"/>
@@ -16532,7 +16475,7 @@
         <v>117</v>
       </c>
       <c r="I206" s="54" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J206" s="54" t="s">
         <v>108</v>
@@ -16552,7 +16495,7 @@
         <v>5</v>
       </c>
       <c r="O206" s="106" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="P206" s="106"/>
       <c r="Q206" s="106"/>
@@ -16655,10 +16598,10 @@
         <v>130</v>
       </c>
       <c r="I208" s="103" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J208" s="103" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K208" s="56">
         <v>1</v>
@@ -17005,7 +16948,7 @@
       </c>
       <c r="I213" s="79"/>
       <c r="J213" s="56" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K213" s="56">
         <v>1</v>
@@ -17683,7 +17626,7 @@
       <c r="H223" s="26"/>
       <c r="I223" s="79"/>
       <c r="J223" s="56" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K223" s="56">
         <v>1</v>
@@ -18022,7 +17965,7 @@
       <c r="G228" s="4"/>
       <c r="H228" s="26"/>
       <c r="I228" s="103" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J228" s="103"/>
       <c r="K228" s="56">
@@ -19364,7 +19307,7 @@
       <c r="G248" s="4"/>
       <c r="H248" s="26"/>
       <c r="I248" s="103" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J248" s="103"/>
       <c r="K248" s="56">
@@ -20873,7 +20816,7 @@
         <v>131</v>
       </c>
       <c r="I273" s="123" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J273" s="57">
         <v>0</v>
@@ -20931,10 +20874,10 @@
         <v>132</v>
       </c>
       <c r="I274" s="103" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J274" s="103" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K274" s="56">
         <v>1</v>
@@ -20987,7 +20930,7 @@
       <c r="G275" s="4"/>
       <c r="H275" s="64"/>
       <c r="I275" s="103" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J275" s="103"/>
       <c r="K275" s="56">
@@ -21040,7 +20983,7 @@
       <c r="G276" s="4"/>
       <c r="H276" s="64"/>
       <c r="I276" s="103" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J276" s="103"/>
       <c r="K276" s="56">
@@ -21092,7 +21035,7 @@
       <c r="G277" s="4"/>
       <c r="H277" s="64"/>
       <c r="I277" s="103" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J277" s="103"/>
       <c r="K277" s="63">
@@ -21202,7 +21145,7 @@
       <c r="H279" s="113"/>
       <c r="I279" s="79"/>
       <c r="J279" s="56" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K279" s="56">
         <v>1</v>
@@ -21722,7 +21665,7 @@
       <c r="H289" s="113"/>
       <c r="I289" s="79"/>
       <c r="J289" s="56" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K289" s="56">
         <v>1</v>
@@ -22343,13 +22286,13 @@
       <c r="H305" s="29"/>
       <c r="I305" s="29"/>
       <c r="J305" s="180" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K305" s="180" t="s">
         <v>96</v>
       </c>
       <c r="L305" s="180" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="M305" s="180"/>
       <c r="N305" s="180"/>
@@ -22382,13 +22325,13 @@
       <c r="H306" s="29"/>
       <c r="I306" s="29"/>
       <c r="J306" s="180" t="s">
+        <v>204</v>
+      </c>
+      <c r="K306" s="180" t="s">
         <v>205</v>
       </c>
-      <c r="K306" s="180" t="s">
+      <c r="L306" s="180" t="s">
         <v>206</v>
-      </c>
-      <c r="L306" s="180" t="s">
-        <v>207</v>
       </c>
       <c r="M306" s="180"/>
       <c r="N306" s="180"/>
@@ -22573,7 +22516,7 @@
       <c r="F311" s="5"/>
       <c r="G311" s="4"/>
       <c r="H311" s="100" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I311" s="2"/>
       <c r="J311" s="2"/>
@@ -22608,7 +22551,7 @@
       <c r="F312" s="5"/>
       <c r="G312" s="4"/>
       <c r="H312" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I312" s="2"/>
       <c r="J312" s="31" t="b">
@@ -22649,7 +22592,7 @@
       <c r="F313" s="5"/>
       <c r="G313" s="4"/>
       <c r="H313" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="I313" s="2"/>
       <c r="J313" s="121">
@@ -22690,7 +22633,7 @@
       <c r="F314" s="5"/>
       <c r="G314" s="4"/>
       <c r="H314" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I314" s="2"/>
       <c r="J314" s="31" t="b">
@@ -22799,13 +22742,13 @@
       <c r="H317" s="2"/>
       <c r="I317" s="145"/>
       <c r="J317" s="146" t="s">
+        <v>221</v>
+      </c>
+      <c r="K317" s="146" t="s">
         <v>222</v>
       </c>
-      <c r="K317" s="146" t="s">
+      <c r="L317" s="146" t="s">
         <v>223</v>
-      </c>
-      <c r="L317" s="146" t="s">
-        <v>224</v>
       </c>
       <c r="M317" s="2"/>
       <c r="N317" s="2"/>
@@ -22836,7 +22779,7 @@
       <c r="F318" s="5"/>
       <c r="G318" s="4"/>
       <c r="H318" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I318" s="145"/>
       <c r="J318" s="31">
@@ -23374,12 +23317,12 @@
   </sheetPr>
   <dimension ref="A1:AB168"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="9" ySplit="10" topLeftCell="J16" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="9" ySplit="10" topLeftCell="J66" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="J13" sqref="J13:T13"/>
+      <selection pane="bottomRight" activeCell="J93" activeCellId="2" sqref="T93:W93 O93:R93 J93:M93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -23391,7 +23334,7 @@
     <col min="5" max="6" width="9.7109375" style="140" customWidth="1" outlineLevel="1"/>
     <col min="7" max="7" width="1.7109375" style="140" customWidth="1" outlineLevel="1"/>
     <col min="8" max="8" width="37.28515625" style="140" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" style="140" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="140" customWidth="1"/>
     <col min="10" max="14" width="10.85546875" style="140" customWidth="1"/>
     <col min="15" max="15" width="12.140625" style="140" bestFit="1" customWidth="1"/>
     <col min="16" max="23" width="10.85546875" style="140" customWidth="1"/>
@@ -23727,7 +23670,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="29"/>
       <c r="I9" s="29" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J9" s="29" t="s">
         <v>5</v>
@@ -23873,10 +23816,10 @@
         <v>16</v>
       </c>
       <c r="I13" s="149">
-        <v>44377.656706597198</v>
+        <v>44526.640759722199</v>
       </c>
       <c r="J13" s="185" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="K13" s="186"/>
       <c r="L13" s="186"/>
@@ -23897,7 +23840,7 @@
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
     </row>
-    <row r="14" spans="1:28" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" ht="45" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="33"/>
       <c r="C14" s="67">
@@ -23915,7 +23858,7 @@
         <v>44336.775273148101</v>
       </c>
       <c r="J14" s="188" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="K14" s="189"/>
       <c r="L14" s="189"/>
@@ -23936,7 +23879,7 @@
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
     </row>
-    <row r="15" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="33"/>
       <c r="C15" s="67">
@@ -23971,7 +23914,7 @@
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
     </row>
-    <row r="16" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="33"/>
       <c r="C16" s="67">
@@ -24006,7 +23949,7 @@
       <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>
     </row>
-    <row r="17" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="33"/>
       <c r="C17" s="67">
@@ -24053,7 +23996,7 @@
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
     </row>
-    <row r="18" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="33"/>
       <c r="C18" s="67">
@@ -24090,7 +24033,7 @@
       <c r="AA18" s="1"/>
       <c r="AB18" s="1"/>
     </row>
-    <row r="19" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="33"/>
       <c r="C19" s="67">
@@ -24127,7 +24070,7 @@
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
     </row>
-    <row r="20" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="33"/>
       <c r="C20" s="67">
@@ -24164,7 +24107,7 @@
       <c r="AA20" s="1"/>
       <c r="AB20" s="1"/>
     </row>
-    <row r="21" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="33"/>
       <c r="C21" s="67">
@@ -24201,7 +24144,7 @@
       <c r="AA21" s="1"/>
       <c r="AB21" s="1"/>
     </row>
-    <row r="22" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="33"/>
       <c r="C22" s="67">
@@ -24236,7 +24179,7 @@
       <c r="AA22" s="1"/>
       <c r="AB22" s="1"/>
     </row>
-    <row r="23" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" ht="5.0999999999999996" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="33"/>
       <c r="C23" s="67">
@@ -24704,7 +24647,7 @@
         <v>97</v>
       </c>
       <c r="O36" s="180" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="P36" s="180"/>
       <c r="Q36" s="180"/>
@@ -24738,10 +24681,10 @@
       <c r="L37" s="29"/>
       <c r="M37" s="180"/>
       <c r="N37" s="180" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="O37" s="180" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="P37" s="180"/>
       <c r="Q37" s="180"/>
@@ -24913,7 +24856,7 @@
       <c r="F42" s="5"/>
       <c r="G42" s="4"/>
       <c r="H42" s="100" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
@@ -24948,7 +24891,7 @@
       <c r="F43" s="5"/>
       <c r="G43" s="4"/>
       <c r="H43" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
@@ -24987,7 +24930,7 @@
       <c r="F44" s="5"/>
       <c r="G44" s="4"/>
       <c r="H44" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
@@ -25026,7 +24969,7 @@
       <c r="F45" s="5"/>
       <c r="G45" s="4"/>
       <c r="H45" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
@@ -25063,7 +25006,7 @@
       <c r="F46" s="5"/>
       <c r="G46" s="4"/>
       <c r="H46" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
@@ -25100,7 +25043,7 @@
       <c r="F47" s="5"/>
       <c r="G47" s="4"/>
       <c r="H47" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
@@ -25203,17 +25146,17 @@
       <c r="F50" s="5"/>
       <c r="G50" s="4"/>
       <c r="H50" s="100" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I50" s="2"/>
       <c r="J50" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="K50" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="K50" s="2" t="s">
+      <c r="L50" s="2" t="s">
         <v>219</v>
-      </c>
-      <c r="L50" s="2" t="s">
-        <v>220</v>
       </c>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -25246,13 +25189,13 @@
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
       <c r="J51" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="K51" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="K51" s="2" t="s">
+      <c r="L51" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="L51" s="2" t="s">
-        <v>207</v>
       </c>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
@@ -25283,7 +25226,7 @@
       <c r="F52" s="5"/>
       <c r="G52" s="4"/>
       <c r="H52" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I52" s="2"/>
       <c r="J52" s="31" t="b">
@@ -25324,7 +25267,7 @@
       <c r="F53" s="5"/>
       <c r="G53" s="4"/>
       <c r="H53" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I53" s="2"/>
       <c r="J53" s="31" t="b">
@@ -25845,21 +25788,21 @@
       <c r="J68" s="147" t="s">
         <v>44</v>
       </c>
-      <c r="K68" s="147"/>
-      <c r="L68" s="147" t="s">
+      <c r="K68" s="29"/>
+      <c r="L68" s="147"/>
+      <c r="M68" s="147" t="s">
         <v>44</v>
       </c>
-      <c r="M68" s="147"/>
       <c r="N68" s="29"/>
-      <c r="O68" s="29"/>
-      <c r="P68" s="147" t="s">
+      <c r="O68" s="147"/>
+      <c r="P68" s="29"/>
+      <c r="Q68" s="29"/>
+      <c r="R68" s="29"/>
+      <c r="S68" s="147" t="s">
         <v>44</v>
       </c>
-      <c r="Q68" s="147"/>
-      <c r="R68" s="29"/>
-      <c r="S68" s="29"/>
       <c r="T68" s="29"/>
-      <c r="U68" s="29"/>
+      <c r="U68" s="147"/>
       <c r="V68" s="29"/>
       <c r="W68" s="29"/>
       <c r="X68" s="3"/>
@@ -25884,21 +25827,21 @@
       <c r="J69" s="147" t="s">
         <v>44</v>
       </c>
-      <c r="K69" s="147"/>
-      <c r="L69" s="147" t="s">
+      <c r="K69" s="29"/>
+      <c r="L69" s="147"/>
+      <c r="M69" s="147" t="s">
         <v>44</v>
       </c>
-      <c r="M69" s="147"/>
       <c r="N69" s="29"/>
-      <c r="O69" s="29"/>
-      <c r="P69" s="147" t="s">
+      <c r="O69" s="147"/>
+      <c r="P69" s="29"/>
+      <c r="Q69" s="29"/>
+      <c r="R69" s="29"/>
+      <c r="S69" s="147" t="s">
         <v>44</v>
       </c>
-      <c r="Q69" s="147"/>
-      <c r="R69" s="29"/>
-      <c r="S69" s="29"/>
       <c r="T69" s="29"/>
-      <c r="U69" s="29"/>
+      <c r="U69" s="147"/>
       <c r="V69" s="29"/>
       <c r="W69" s="29"/>
       <c r="X69" s="3"/>
@@ -25923,25 +25866,25 @@
       <c r="J70" s="147" t="s">
         <v>72</v>
       </c>
-      <c r="K70" s="147"/>
-      <c r="L70" s="147" t="s">
+      <c r="K70" s="65"/>
+      <c r="L70" s="147"/>
+      <c r="M70" s="147" t="s">
         <v>73</v>
       </c>
-      <c r="M70" s="147"/>
-      <c r="N70" s="29" t="s">
+      <c r="N70" s="65"/>
+      <c r="O70" s="147"/>
+      <c r="P70" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="O70" s="29" t="s">
-        <v>149</v>
-      </c>
-      <c r="P70" s="147" t="s">
+      <c r="Q70" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="R70" s="29"/>
+      <c r="S70" s="147" t="s">
         <v>75</v>
       </c>
-      <c r="Q70" s="147"/>
-      <c r="R70" s="29"/>
-      <c r="S70" s="29"/>
-      <c r="T70" s="29"/>
-      <c r="U70" s="29"/>
+      <c r="T70" s="65"/>
+      <c r="U70" s="147"/>
       <c r="V70" s="29"/>
       <c r="W70" s="29"/>
       <c r="X70" s="3"/>
@@ -25968,21 +25911,21 @@
       <c r="J71" s="147" t="s">
         <v>44</v>
       </c>
-      <c r="K71" s="147"/>
-      <c r="L71" s="147" t="s">
+      <c r="K71" s="29"/>
+      <c r="L71" s="147"/>
+      <c r="M71" s="147" t="s">
         <v>44</v>
       </c>
-      <c r="M71" s="147"/>
       <c r="N71" s="29"/>
-      <c r="O71" s="29"/>
-      <c r="P71" s="147" t="s">
+      <c r="O71" s="147"/>
+      <c r="P71" s="29"/>
+      <c r="Q71" s="29"/>
+      <c r="R71" s="29"/>
+      <c r="S71" s="147" t="s">
         <v>44</v>
       </c>
-      <c r="Q71" s="147"/>
-      <c r="R71" s="29"/>
-      <c r="S71" s="29"/>
       <c r="T71" s="29"/>
-      <c r="U71" s="29"/>
+      <c r="U71" s="147"/>
       <c r="V71" s="29"/>
       <c r="W71" s="29"/>
       <c r="X71" s="3"/>
@@ -26115,24 +26058,24 @@
         <v>1</v>
       </c>
       <c r="K75" s="2"/>
-      <c r="L75" s="121">
-        <f>i_w_start_len1*i_n1_len^L78</f>
+      <c r="L75" s="2"/>
+      <c r="M75" s="121">
+        <f>i_w_start_len1*i_n1_len^M78</f>
         <v>81</v>
       </c>
-      <c r="M75" s="2"/>
-      <c r="N75" s="116" t="s">
-        <v>150</v>
-      </c>
-      <c r="O75" s="31">
+      <c r="N75" s="2"/>
+      <c r="O75" s="2"/>
+      <c r="P75" s="116" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q75" s="31">
         <v>10</v>
       </c>
-      <c r="P75" s="121">
-        <f>i_w_start_len3*i_n3_len^P78</f>
+      <c r="R75" s="2"/>
+      <c r="S75" s="121">
+        <f>i_w_start_len3*i_n3_len^S78</f>
         <v>81</v>
       </c>
-      <c r="Q75" s="2"/>
-      <c r="R75" s="2"/>
-      <c r="S75" s="2"/>
       <c r="T75" s="2"/>
       <c r="U75" s="2"/>
       <c r="V75" s="2"/>
@@ -26163,18 +26106,18 @@
         <v>1</v>
       </c>
       <c r="K76" s="2"/>
-      <c r="L76" s="31">
+      <c r="L76" s="2"/>
+      <c r="M76" s="31">
         <v>3</v>
       </c>
-      <c r="M76" s="2"/>
       <c r="N76" s="2"/>
       <c r="O76" s="2"/>
-      <c r="P76" s="31">
-        <v>3</v>
-      </c>
+      <c r="P76" s="2"/>
       <c r="Q76" s="2"/>
       <c r="R76" s="2"/>
-      <c r="S76" s="2"/>
+      <c r="S76" s="31">
+        <v>3</v>
+      </c>
       <c r="T76" s="2"/>
       <c r="U76" s="2"/>
       <c r="V76" s="2"/>
@@ -26203,25 +26146,23 @@
       <c r="J77" s="36">
         <v>1</v>
       </c>
-      <c r="K77" s="115"/>
-      <c r="L77" s="31">
+      <c r="K77" s="2"/>
+      <c r="L77" s="115"/>
+      <c r="M77" s="31">
         <v>3</v>
       </c>
-      <c r="M77" s="115"/>
       <c r="N77" s="2"/>
-      <c r="O77" s="2"/>
-      <c r="P77" s="31">
+      <c r="O77" s="115"/>
+      <c r="P77" s="2"/>
+      <c r="Q77" s="2"/>
+      <c r="R77" s="2"/>
+      <c r="S77" s="31">
         <v>3</v>
       </c>
-      <c r="Q77" s="115"/>
-      <c r="R77" s="190" t="s">
-        <v>139</v>
-      </c>
-      <c r="S77" s="191"/>
-      <c r="T77" s="191"/>
-      <c r="U77" s="191"/>
-      <c r="V77" s="191"/>
-      <c r="W77" s="192"/>
+      <c r="T77" s="2"/>
+      <c r="U77" s="115"/>
+      <c r="V77" s="2"/>
+      <c r="W77" s="2"/>
       <c r="X77" s="4"/>
       <c r="Y77" s="16"/>
       <c r="Z77" s="1"/>
@@ -26247,24 +26188,24 @@
         <v>1</v>
       </c>
       <c r="K78" s="2"/>
-      <c r="L78" s="121">
+      <c r="L78" s="2"/>
+      <c r="M78" s="121">
         <f>COUNTIF(i_fixed_fvp_mask_dams,TRUE)+COUNTIF(i_fvp_mask_dams,TRUE)</f>
         <v>3</v>
       </c>
-      <c r="M78" s="2"/>
       <c r="N78" s="2"/>
       <c r="O78" s="2"/>
-      <c r="P78" s="121">
+      <c r="P78" s="2"/>
+      <c r="Q78" s="2"/>
+      <c r="R78" s="2"/>
+      <c r="S78" s="121">
         <f>COUNTIF(J52:L52,TRUE)</f>
         <v>3</v>
       </c>
-      <c r="Q78" s="115"/>
-      <c r="R78" s="193"/>
-      <c r="S78" s="194"/>
-      <c r="T78" s="194"/>
-      <c r="U78" s="194"/>
-      <c r="V78" s="194"/>
-      <c r="W78" s="195"/>
+      <c r="T78" s="2"/>
+      <c r="U78" s="115"/>
+      <c r="V78" s="2"/>
+      <c r="W78" s="2"/>
       <c r="X78" s="4"/>
       <c r="Y78" s="16"/>
       <c r="Z78" s="1"/>
@@ -26290,22 +26231,22 @@
         <v>1</v>
       </c>
       <c r="K79" s="2"/>
-      <c r="L79" s="31">
-        <v>1</v>
-      </c>
-      <c r="M79" s="2"/>
+      <c r="L79" s="2"/>
+      <c r="M79" s="31">
+        <v>1</v>
+      </c>
       <c r="N79" s="2"/>
       <c r="O79" s="2"/>
-      <c r="P79" s="31">
-        <v>1</v>
-      </c>
+      <c r="P79" s="2"/>
       <c r="Q79" s="2"/>
-      <c r="R79" s="196"/>
-      <c r="S79" s="197"/>
-      <c r="T79" s="197"/>
-      <c r="U79" s="197"/>
-      <c r="V79" s="197"/>
-      <c r="W79" s="198"/>
+      <c r="R79" s="2"/>
+      <c r="S79" s="31">
+        <v>1</v>
+      </c>
+      <c r="T79" s="2"/>
+      <c r="U79" s="2"/>
+      <c r="V79" s="2"/>
+      <c r="W79" s="2"/>
       <c r="X79" s="4"/>
       <c r="Y79" s="16"/>
       <c r="Z79" s="1"/>
@@ -26394,33 +26335,39 @@
       <c r="F82" s="5"/>
       <c r="G82" s="4"/>
       <c r="H82" s="172" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I82" s="2"/>
       <c r="J82" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="K82" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
+      </c>
+      <c r="K82" s="36" t="s">
+        <v>312</v>
       </c>
       <c r="L82" s="2" t="s">
         <v>240</v>
       </c>
       <c r="M82" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="N82" s="2"/>
-      <c r="O82" s="2"/>
-      <c r="P82" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="N82" s="36" t="s">
+        <v>312</v>
+      </c>
+      <c r="O82" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="Q82" s="2" t="s">
-        <v>241</v>
-      </c>
+      <c r="P82" s="2"/>
+      <c r="Q82" s="2"/>
       <c r="R82" s="2"/>
-      <c r="S82" s="2"/>
-      <c r="T82" s="2"/>
-      <c r="U82" s="2"/>
+      <c r="S82" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="T82" s="36" t="s">
+        <v>312</v>
+      </c>
+      <c r="U82" s="2" t="s">
+        <v>240</v>
+      </c>
       <c r="V82" s="2"/>
       <c r="W82" s="2"/>
       <c r="X82" s="4"/>
@@ -26443,33 +26390,39 @@
       <c r="F83" s="5"/>
       <c r="G83" s="4"/>
       <c r="H83" s="175" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I83" s="2"/>
       <c r="J83" s="173">
         <v>0</v>
       </c>
-      <c r="K83" s="31">
-        <v>1</v>
+      <c r="K83" s="173" t="b">
+        <v>0</v>
       </c>
       <c r="L83" s="31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M83" s="31">
-        <v>1</v>
-      </c>
-      <c r="N83" s="2"/>
-      <c r="O83" s="172"/>
-      <c r="P83" s="31">
-        <v>0</v>
-      </c>
-      <c r="Q83" s="173">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="N83" s="173" t="b">
+        <v>0</v>
+      </c>
+      <c r="O83" s="31">
+        <v>1</v>
+      </c>
+      <c r="P83" s="2"/>
+      <c r="Q83" s="172"/>
       <c r="R83" s="2"/>
-      <c r="S83" s="2"/>
-      <c r="T83" s="2"/>
-      <c r="U83" s="2"/>
+      <c r="S83" s="31">
+        <v>0</v>
+      </c>
+      <c r="T83" s="173" t="b">
+        <v>0</v>
+      </c>
+      <c r="U83" s="173">
+        <v>1</v>
+      </c>
       <c r="V83" s="2"/>
       <c r="W83" s="2"/>
       <c r="X83" s="4"/>
@@ -26492,29 +26445,33 @@
       <c r="F84" s="5"/>
       <c r="G84" s="4"/>
       <c r="H84" s="175" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I84" s="2"/>
       <c r="J84" s="172"/>
-      <c r="K84" s="172"/>
-      <c r="L84" s="31">
-        <v>1</v>
-      </c>
+      <c r="K84" s="2"/>
+      <c r="L84" s="172"/>
       <c r="M84" s="31">
         <v>1</v>
       </c>
-      <c r="N84" s="2"/>
-      <c r="O84" s="172"/>
-      <c r="P84" s="31">
-        <v>1</v>
-      </c>
-      <c r="Q84" s="173">
-        <v>1</v>
-      </c>
+      <c r="N84" s="173" t="b">
+        <v>0</v>
+      </c>
+      <c r="O84" s="31">
+        <v>1</v>
+      </c>
+      <c r="P84" s="2"/>
+      <c r="Q84" s="172"/>
       <c r="R84" s="2"/>
-      <c r="S84" s="2"/>
-      <c r="T84" s="2"/>
-      <c r="U84" s="2"/>
+      <c r="S84" s="31">
+        <v>1</v>
+      </c>
+      <c r="T84" s="173" t="b">
+        <v>0</v>
+      </c>
+      <c r="U84" s="173">
+        <v>1</v>
+      </c>
       <c r="V84" s="2"/>
       <c r="W84" s="2"/>
       <c r="X84" s="4"/>
@@ -26537,29 +26494,33 @@
       <c r="F85" s="5"/>
       <c r="G85" s="4"/>
       <c r="H85" s="175" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I85" s="2"/>
       <c r="J85" s="172"/>
-      <c r="K85" s="172"/>
-      <c r="L85" s="31">
+      <c r="K85" s="2"/>
+      <c r="L85" s="172"/>
+      <c r="M85" s="31">
         <v>-1</v>
       </c>
-      <c r="M85" s="31">
-        <v>1</v>
-      </c>
-      <c r="N85" s="2"/>
-      <c r="O85" s="172"/>
-      <c r="P85" s="31">
+      <c r="N85" s="173" t="b">
+        <v>0</v>
+      </c>
+      <c r="O85" s="31">
+        <v>1</v>
+      </c>
+      <c r="P85" s="2"/>
+      <c r="Q85" s="172"/>
+      <c r="R85" s="2"/>
+      <c r="S85" s="31">
         <v>-1</v>
       </c>
-      <c r="Q85" s="173">
-        <v>1</v>
-      </c>
-      <c r="R85" s="2"/>
-      <c r="S85" s="2"/>
-      <c r="T85" s="2"/>
-      <c r="U85" s="2"/>
+      <c r="T85" s="173" t="b">
+        <v>0</v>
+      </c>
+      <c r="U85" s="173">
+        <v>1</v>
+      </c>
       <c r="V85" s="2"/>
       <c r="W85" s="2"/>
       <c r="X85" s="4"/>
@@ -26582,29 +26543,33 @@
       <c r="F86" s="5"/>
       <c r="G86" s="4"/>
       <c r="H86" s="175" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I86" s="2"/>
       <c r="J86" s="172"/>
-      <c r="K86" s="172"/>
-      <c r="L86" s="31">
+      <c r="K86" s="2"/>
+      <c r="L86" s="172"/>
+      <c r="M86" s="31">
         <v>0.5</v>
       </c>
-      <c r="M86" s="31">
-        <v>1</v>
-      </c>
-      <c r="N86" s="2"/>
-      <c r="O86" s="2"/>
-      <c r="P86" s="31">
+      <c r="N86" s="173" t="b">
+        <v>0</v>
+      </c>
+      <c r="O86" s="31">
+        <v>1</v>
+      </c>
+      <c r="P86" s="2"/>
+      <c r="Q86" s="2"/>
+      <c r="R86" s="2"/>
+      <c r="S86" s="31">
         <v>0.33300000000000002</v>
       </c>
-      <c r="Q86" s="31">
-        <v>1</v>
-      </c>
-      <c r="R86" s="2"/>
-      <c r="S86" s="2"/>
-      <c r="T86" s="2"/>
-      <c r="U86" s="2"/>
+      <c r="T86" s="173" t="b">
+        <v>0</v>
+      </c>
+      <c r="U86" s="31">
+        <v>1</v>
+      </c>
       <c r="V86" s="2"/>
       <c r="W86" s="2"/>
       <c r="X86" s="4"/>
@@ -26627,29 +26592,33 @@
       <c r="F87" s="5"/>
       <c r="G87" s="4"/>
       <c r="H87" s="175" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I87" s="2"/>
       <c r="J87" s="172"/>
-      <c r="K87" s="172"/>
-      <c r="L87" s="31">
+      <c r="K87" s="2"/>
+      <c r="L87" s="172"/>
+      <c r="M87" s="31">
         <v>-0.5</v>
       </c>
-      <c r="M87" s="31">
-        <v>1</v>
-      </c>
-      <c r="N87" s="2"/>
-      <c r="O87" s="2"/>
-      <c r="P87" s="31">
+      <c r="N87" s="173" t="b">
+        <v>0</v>
+      </c>
+      <c r="O87" s="31">
+        <v>1</v>
+      </c>
+      <c r="P87" s="2"/>
+      <c r="Q87" s="2"/>
+      <c r="R87" s="2"/>
+      <c r="S87" s="31">
         <v>0.66600000000000004</v>
       </c>
-      <c r="Q87" s="31">
-        <v>1</v>
-      </c>
-      <c r="R87" s="2"/>
-      <c r="S87" s="2"/>
-      <c r="T87" s="2"/>
-      <c r="U87" s="2"/>
+      <c r="T87" s="173" t="b">
+        <v>0</v>
+      </c>
+      <c r="U87" s="31">
+        <v>1</v>
+      </c>
       <c r="V87" s="2"/>
       <c r="W87" s="2"/>
       <c r="X87" s="4"/>
@@ -26672,29 +26641,33 @@
       <c r="F88" s="5"/>
       <c r="G88" s="4"/>
       <c r="H88" s="175" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I88" s="2"/>
       <c r="J88" s="172"/>
-      <c r="K88" s="172"/>
-      <c r="L88" s="31">
+      <c r="K88" s="2"/>
+      <c r="L88" s="172"/>
+      <c r="M88" s="31">
         <v>0.2</v>
       </c>
-      <c r="M88" s="31">
-        <v>1</v>
-      </c>
-      <c r="N88" s="2"/>
-      <c r="O88" s="2"/>
-      <c r="P88" s="31">
+      <c r="N88" s="173" t="b">
+        <v>0</v>
+      </c>
+      <c r="O88" s="31">
+        <v>1</v>
+      </c>
+      <c r="P88" s="2"/>
+      <c r="Q88" s="2"/>
+      <c r="R88" s="2"/>
+      <c r="S88" s="31">
         <v>-0.5</v>
       </c>
-      <c r="Q88" s="31">
-        <v>1</v>
-      </c>
-      <c r="R88" s="2"/>
-      <c r="S88" s="2"/>
-      <c r="T88" s="2"/>
-      <c r="U88" s="2"/>
+      <c r="T88" s="173" t="b">
+        <v>0</v>
+      </c>
+      <c r="U88" s="31">
+        <v>1</v>
+      </c>
       <c r="V88" s="2"/>
       <c r="W88" s="2"/>
       <c r="X88" s="4"/>
@@ -26717,29 +26690,33 @@
       <c r="F89" s="5"/>
       <c r="G89" s="4"/>
       <c r="H89" s="175" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I89" s="2"/>
       <c r="J89" s="172"/>
-      <c r="K89" s="172"/>
-      <c r="L89" s="31">
+      <c r="K89" s="2"/>
+      <c r="L89" s="172"/>
+      <c r="M89" s="31">
         <v>-0.2</v>
       </c>
-      <c r="M89" s="31">
-        <v>1</v>
-      </c>
-      <c r="N89" s="2"/>
-      <c r="O89" s="2"/>
-      <c r="P89" s="31">
-        <v>3.9</v>
-      </c>
-      <c r="Q89" s="31">
+      <c r="N89" s="173" t="b">
+        <v>0</v>
+      </c>
+      <c r="O89" s="31">
+        <v>1</v>
+      </c>
+      <c r="P89" s="2"/>
+      <c r="Q89" s="2"/>
+      <c r="R89" s="2"/>
+      <c r="S89" s="31">
+        <v>10</v>
+      </c>
+      <c r="T89" s="173" t="b">
+        <v>1</v>
+      </c>
+      <c r="U89" s="31">
         <v>300</v>
       </c>
-      <c r="R89" s="2"/>
-      <c r="S89" s="2"/>
-      <c r="T89" s="2"/>
-      <c r="U89" s="2"/>
       <c r="V89" s="2"/>
       <c r="W89" s="2"/>
       <c r="X89" s="4"/>
@@ -26762,29 +26739,33 @@
       <c r="F90" s="5"/>
       <c r="G90" s="4"/>
       <c r="H90" s="175" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I90" s="2"/>
       <c r="J90" s="172"/>
-      <c r="K90" s="172"/>
-      <c r="L90" s="31">
+      <c r="K90" s="2"/>
+      <c r="L90" s="172"/>
+      <c r="M90" s="31">
         <v>0.1</v>
       </c>
-      <c r="M90" s="31">
-        <v>1</v>
-      </c>
-      <c r="N90" s="2"/>
-      <c r="O90" s="2"/>
-      <c r="P90" s="31">
-        <v>3.5</v>
-      </c>
-      <c r="Q90" s="31">
+      <c r="N90" s="173" t="b">
+        <v>0</v>
+      </c>
+      <c r="O90" s="31">
+        <v>1</v>
+      </c>
+      <c r="P90" s="2"/>
+      <c r="Q90" s="2"/>
+      <c r="R90" s="2"/>
+      <c r="S90" s="31">
+        <v>0</v>
+      </c>
+      <c r="T90" s="173" t="b">
+        <v>1</v>
+      </c>
+      <c r="U90" s="31">
         <v>100</v>
       </c>
-      <c r="R90" s="2"/>
-      <c r="S90" s="2"/>
-      <c r="T90" s="2"/>
-      <c r="U90" s="2"/>
       <c r="V90" s="2"/>
       <c r="W90" s="2"/>
       <c r="X90" s="4"/>
@@ -26875,29 +26856,29 @@
       <c r="F93" s="5"/>
       <c r="G93" s="4"/>
       <c r="H93" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I93" s="2"/>
-      <c r="J93" s="100" t="s">
+      <c r="J93" s="192" t="s">
         <v>72</v>
       </c>
-      <c r="K93" s="100"/>
-      <c r="L93" s="100"/>
-      <c r="M93" s="100"/>
+      <c r="K93" s="192"/>
+      <c r="L93" s="192"/>
+      <c r="M93" s="192"/>
       <c r="N93" s="2"/>
-      <c r="O93" s="100" t="s">
+      <c r="O93" s="192" t="s">
         <v>73</v>
       </c>
-      <c r="P93" s="2"/>
-      <c r="Q93" s="2"/>
-      <c r="R93" s="2"/>
+      <c r="P93" s="52"/>
+      <c r="Q93" s="52"/>
+      <c r="R93" s="52"/>
       <c r="S93" s="2"/>
-      <c r="T93" s="100" t="s">
+      <c r="T93" s="192" t="s">
         <v>75</v>
       </c>
-      <c r="U93" s="2"/>
-      <c r="V93" s="2"/>
-      <c r="W93" s="2"/>
+      <c r="U93" s="52"/>
+      <c r="V93" s="52"/>
+      <c r="W93" s="52"/>
       <c r="X93" s="4"/>
       <c r="Y93" s="16"/>
       <c r="Z93" s="1"/>
@@ -26918,42 +26899,42 @@
       <c r="H94" s="2"/>
       <c r="I94" s="2"/>
       <c r="J94" s="100" t="s">
+        <v>251</v>
+      </c>
+      <c r="K94" s="100" t="s">
         <v>252</v>
       </c>
-      <c r="K94" s="100" t="s">
+      <c r="L94" s="100" t="s">
         <v>253</v>
       </c>
-      <c r="L94" s="100" t="s">
+      <c r="M94" s="100" t="s">
         <v>254</v>
-      </c>
-      <c r="M94" s="100" t="s">
-        <v>255</v>
       </c>
       <c r="N94" s="2"/>
       <c r="O94" s="100" t="s">
+        <v>251</v>
+      </c>
+      <c r="P94" s="100" t="s">
         <v>252</v>
       </c>
-      <c r="P94" s="100" t="s">
+      <c r="Q94" s="100" t="s">
         <v>253</v>
       </c>
-      <c r="Q94" s="100" t="s">
+      <c r="R94" s="100" t="s">
         <v>254</v>
-      </c>
-      <c r="R94" s="100" t="s">
-        <v>255</v>
       </c>
       <c r="S94" s="2"/>
       <c r="T94" s="100" t="s">
+        <v>251</v>
+      </c>
+      <c r="U94" s="100" t="s">
         <v>252</v>
       </c>
-      <c r="U94" s="100" t="s">
+      <c r="V94" s="100" t="s">
         <v>253</v>
       </c>
-      <c r="V94" s="100" t="s">
+      <c r="W94" s="100" t="s">
         <v>254</v>
-      </c>
-      <c r="W94" s="100" t="s">
-        <v>255</v>
       </c>
       <c r="X94" s="4"/>
       <c r="Y94" s="16"/>
@@ -26975,7 +26956,7 @@
       <c r="F95" s="5"/>
       <c r="G95" s="4"/>
       <c r="H95" s="175" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I95" s="2"/>
       <c r="J95" s="176">
@@ -27036,7 +27017,7 @@
       <c r="F96" s="5"/>
       <c r="G96" s="4"/>
       <c r="H96" s="175" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I96" s="2"/>
       <c r="J96" s="2"/>
@@ -27089,7 +27070,7 @@
       <c r="F97" s="5"/>
       <c r="G97" s="4"/>
       <c r="H97" s="175" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I97" s="2"/>
       <c r="J97" s="2"/>
@@ -27762,7 +27743,7 @@
       <c r="F116" s="5"/>
       <c r="G116" s="4"/>
       <c r="H116" s="26" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I116" s="31" t="b">
         <v>0</v>
@@ -27832,7 +27813,7 @@
       <c r="F118" s="5"/>
       <c r="G118" s="4"/>
       <c r="H118" s="26" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I118" s="31">
         <v>0</v>
@@ -27939,10 +27920,10 @@
       <c r="F121" s="5"/>
       <c r="G121" s="4"/>
       <c r="H121" s="64" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I121" s="64" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J121" s="2"/>
       <c r="K121" s="2"/>
@@ -27978,7 +27959,7 @@
       <c r="F122" s="5"/>
       <c r="G122" s="4"/>
       <c r="H122" s="31" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="I122" s="31" t="b">
         <v>0</v>
@@ -28017,7 +27998,7 @@
       <c r="F123" s="5"/>
       <c r="G123" s="4"/>
       <c r="H123" s="31" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I123" s="31" t="b">
         <v>0</v>
@@ -28056,7 +28037,7 @@
       <c r="F124" s="5"/>
       <c r="G124" s="4"/>
       <c r="H124" s="31" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I124" s="31" t="b">
         <v>0</v>
@@ -28095,7 +28076,7 @@
       <c r="F125" s="5"/>
       <c r="G125" s="4"/>
       <c r="H125" s="31" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I125" s="31" t="b">
         <v>0</v>
@@ -28134,7 +28115,7 @@
       <c r="F126" s="5"/>
       <c r="G126" s="4"/>
       <c r="H126" s="31" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I126" s="31" t="b">
         <v>0</v>
@@ -28173,7 +28154,7 @@
       <c r="F127" s="5"/>
       <c r="G127" s="4"/>
       <c r="H127" s="31" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I127" s="31" t="b">
         <v>0</v>
@@ -28212,7 +28193,7 @@
       <c r="F128" s="5"/>
       <c r="G128" s="4"/>
       <c r="H128" s="31" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I128" s="31" t="b">
         <v>0</v>
@@ -28251,7 +28232,7 @@
       <c r="F129" s="5"/>
       <c r="G129" s="4"/>
       <c r="H129" s="31" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I129" s="31" t="b">
         <v>0</v>
@@ -28698,7 +28679,7 @@
       </c>
       <c r="G142" s="13"/>
       <c r="H142" s="8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I142" s="7"/>
       <c r="J142" s="7"/>
@@ -28768,7 +28749,7 @@
       <c r="H144" s="29"/>
       <c r="I144" s="29"/>
       <c r="J144" s="65" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="K144" s="65"/>
       <c r="L144" s="65"/>
@@ -28994,13 +28975,13 @@
       <c r="F150" s="5"/>
       <c r="G150" s="4"/>
       <c r="H150" s="64" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="I150" s="31">
         <v>4</v>
       </c>
       <c r="J150" s="183" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K150" s="2"/>
       <c r="L150" s="2"/>
@@ -29066,7 +29047,7 @@
       <c r="F152" s="5"/>
       <c r="G152" s="4"/>
       <c r="H152" s="64" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I152" s="2"/>
       <c r="J152" s="2"/>
@@ -29101,7 +29082,7 @@
       <c r="F153" s="5"/>
       <c r="G153" s="4"/>
       <c r="H153" s="184" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I153" s="2"/>
       <c r="J153" s="31">
@@ -29156,7 +29137,7 @@
       <c r="F154" s="5"/>
       <c r="G154" s="4"/>
       <c r="H154" s="184" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I154" s="2"/>
       <c r="J154" s="31">
@@ -29620,10 +29601,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="J13:T13"/>
     <mergeCell ref="J14:T14"/>
-    <mergeCell ref="R77:W79"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <conditionalFormatting sqref="J95:M97">
@@ -29632,13 +29612,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O95:R97">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>($E95&gt;=$L$76)</formula>
+    <cfRule type="expression" dxfId="1" priority="89">
+      <formula>($E95&gt;=$M$76)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T95:W97">
-    <cfRule type="expression" dxfId="0" priority="86">
-      <formula>($E95&gt;=$P$76)</formula>
+    <cfRule type="expression" dxfId="0" priority="90">
+      <formula>($E95&gt;=$S$76)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -30352,23 +30332,23 @@
       <c r="I18" s="31">
         <v>1</v>
       </c>
-      <c r="J18" s="199" t="s">
+      <c r="J18" s="190" t="s">
         <v>22</v>
       </c>
-      <c r="K18" s="199"/>
-      <c r="L18" s="199"/>
-      <c r="M18" s="199"/>
-      <c r="N18" s="199"/>
-      <c r="O18" s="199"/>
-      <c r="P18" s="199"/>
-      <c r="Q18" s="199"/>
-      <c r="R18" s="199"/>
-      <c r="S18" s="199"/>
-      <c r="T18" s="199"/>
-      <c r="U18" s="199"/>
-      <c r="V18" s="199"/>
-      <c r="W18" s="199"/>
-      <c r="X18" s="199"/>
+      <c r="K18" s="190"/>
+      <c r="L18" s="190"/>
+      <c r="M18" s="190"/>
+      <c r="N18" s="190"/>
+      <c r="O18" s="190"/>
+      <c r="P18" s="190"/>
+      <c r="Q18" s="190"/>
+      <c r="R18" s="190"/>
+      <c r="S18" s="190"/>
+      <c r="T18" s="190"/>
+      <c r="U18" s="190"/>
+      <c r="V18" s="190"/>
+      <c r="W18" s="190"/>
+      <c r="X18" s="190"/>
       <c r="Y18" s="2"/>
       <c r="Z18" s="4"/>
       <c r="AA18" s="16"/>
@@ -30479,7 +30459,7 @@
       <c r="U21" s="189"/>
       <c r="V21" s="189"/>
       <c r="W21" s="189"/>
-      <c r="X21" s="200"/>
+      <c r="X21" s="191"/>
       <c r="Y21" s="2"/>
       <c r="Z21" s="4"/>
       <c r="AA21" s="16"/>

</xml_diff>

<commit_message>
add fs pkl controls
</commit_message>
<xml_diff>
--- a/Structural.xlsx
+++ b/Structural.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\Models\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D00D9423-4D5C-4344-90E9-F78BB70E51A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9236B91-63B7-4EC6-90FC-F64C882F6FFE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29895" yWindow="600" windowWidth="27705" windowHeight="15630" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -27,6 +27,9 @@
     <definedName name="a_nyatf_b1">Stock!$L$154:$V$154</definedName>
     <definedName name="dry_groups" localSheetId="0">General!$I$48:$J$48</definedName>
     <definedName name="foo_levels" localSheetId="0">General!$I$50:$K$50</definedName>
+    <definedName name="fs_create" localSheetId="2">StructuralSA!$O$117</definedName>
+    <definedName name="fs_number" localSheetId="2">StructuralSA!$O$118</definedName>
+    <definedName name="fs_use_pkl" localSheetId="2">StructuralSA!$O$116</definedName>
     <definedName name="grain_pools" localSheetId="0">General!$I$44:$J$44</definedName>
     <definedName name="grazing_int" localSheetId="0">General!$I$49:$L$49</definedName>
     <definedName name="i_a0_pos">Stock!$I$43</definedName>
@@ -159,7 +162,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1420,6 +1426,54 @@
         </r>
       </text>
     </comment>
+    <comment ref="N82" authorId="0" shapeId="0" xr:uid="{E340AD6E-11C9-44BF-82E3-7B07708AECC7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Michael Young (21512438):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This control allows confinement to occur if it is turned on for the given p6 period (controlled in feedsupply in property inputs)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T82" authorId="0" shapeId="0" xr:uid="{D3F46B65-AA6B-45FC-BB7B-0F0F7648D80A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Michael Young (21512438):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This control allows confinement to occur if it is turned on for the given p6 period (controlled in feedsupply in property inputs)</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="S89" authorId="1" shapeId="0" xr:uid="{7104E76F-9C27-4C3A-B5E1-62B91C191243}">
       <text>
         <r>
@@ -1468,6 +1522,54 @@
         </r>
       </text>
     </comment>
+    <comment ref="N116" authorId="0" shapeId="0" xr:uid="{A9138754-B6ED-47ED-AB84-13224D267758}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Young (21512438):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Controls if a trial uses the pkl feedsupply or used the excel input feedsupply.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N117" authorId="0" shapeId="0" xr:uid="{4842D124-AE7E-42FA-B06C-37867218491F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Young (21512438):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This is to controls if the feedsupply from a given trial is saved (typically this will be False except for a group of trials used to determine optimal fs).</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="H118" authorId="0" shapeId="0" xr:uid="{F11FB435-94C6-4D6B-8CF5-C6375FFCCDEC}">
       <text>
         <r>
@@ -1489,6 +1591,30 @@
           </rPr>
           <t xml:space="preserve">
 This number is appended to the std REV pickle file. This is required so multiple REVs can be run similtaneously.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N118" authorId="0" shapeId="0" xr:uid="{1D224ECA-F2E2-44DB-A203-7D8A825CE404}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Young (21512438):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This number is appended to the std fs pickle file. This is required so multiple fs can be stored similtaneously.</t>
         </r>
       </text>
     </comment>
@@ -1621,7 +1747,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="317">
   <si>
     <t>Controls for this worksheet</t>
   </si>
@@ -2670,6 +2796,15 @@
                    Moved FVP &amp; N inputs from Stock
 1: 1Apr19-Created the version control table</t>
   </si>
+  <si>
+    <t>fs_use_pkl</t>
+  </si>
+  <si>
+    <t>fs_create</t>
+  </si>
+  <si>
+    <t>fs_number</t>
+  </si>
 </sst>
 </file>
 
@@ -2678,7 +2813,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2871,6 +3006,19 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="35">
@@ -4316,6 +4464,9 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="25" xfId="3" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="25" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="38" xfId="12" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -4339,9 +4490,6 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="23" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="25" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -5494,19 +5642,19 @@
       <c r="I13" s="149">
         <v>44371.659649305599</v>
       </c>
-      <c r="J13" s="185" t="s">
+      <c r="J13" s="186" t="s">
         <v>301</v>
       </c>
-      <c r="K13" s="186"/>
-      <c r="L13" s="186"/>
-      <c r="M13" s="186"/>
-      <c r="N13" s="186"/>
-      <c r="O13" s="186"/>
-      <c r="P13" s="186"/>
-      <c r="Q13" s="186"/>
-      <c r="R13" s="186"/>
-      <c r="S13" s="186"/>
-      <c r="T13" s="187"/>
+      <c r="K13" s="187"/>
+      <c r="L13" s="187"/>
+      <c r="M13" s="187"/>
+      <c r="N13" s="187"/>
+      <c r="O13" s="187"/>
+      <c r="P13" s="187"/>
+      <c r="Q13" s="187"/>
+      <c r="R13" s="187"/>
+      <c r="S13" s="187"/>
+      <c r="T13" s="188"/>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
@@ -5533,19 +5681,19 @@
       <c r="I14" s="148">
         <v>44371.660335300898</v>
       </c>
-      <c r="J14" s="188" t="s">
+      <c r="J14" s="189" t="s">
         <v>302</v>
       </c>
-      <c r="K14" s="189"/>
-      <c r="L14" s="189"/>
-      <c r="M14" s="189"/>
-      <c r="N14" s="189"/>
-      <c r="O14" s="189"/>
-      <c r="P14" s="189"/>
-      <c r="Q14" s="189"/>
-      <c r="R14" s="189"/>
-      <c r="S14" s="189"/>
-      <c r="T14" s="189"/>
+      <c r="K14" s="190"/>
+      <c r="L14" s="190"/>
+      <c r="M14" s="190"/>
+      <c r="N14" s="190"/>
+      <c r="O14" s="190"/>
+      <c r="P14" s="190"/>
+      <c r="Q14" s="190"/>
+      <c r="R14" s="190"/>
+      <c r="S14" s="190"/>
+      <c r="T14" s="190"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
@@ -7491,11 +7639,11 @@
   <dimension ref="A1:AE334"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <pane xSplit="9" ySplit="10" topLeftCell="J305" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="10" topLeftCell="J144" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="J315" sqref="J315"/>
+      <selection pane="bottomRight" activeCell="L156" sqref="L156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -7987,19 +8135,19 @@
       <c r="I13" s="149">
         <v>44311.756953009302</v>
       </c>
-      <c r="J13" s="185" t="s">
+      <c r="J13" s="186" t="s">
         <v>308</v>
       </c>
-      <c r="K13" s="186"/>
-      <c r="L13" s="186"/>
-      <c r="M13" s="186"/>
-      <c r="N13" s="186"/>
-      <c r="O13" s="186"/>
-      <c r="P13" s="186"/>
-      <c r="Q13" s="186"/>
-      <c r="R13" s="186"/>
-      <c r="S13" s="186"/>
-      <c r="T13" s="187"/>
+      <c r="K13" s="187"/>
+      <c r="L13" s="187"/>
+      <c r="M13" s="187"/>
+      <c r="N13" s="187"/>
+      <c r="O13" s="187"/>
+      <c r="P13" s="187"/>
+      <c r="Q13" s="187"/>
+      <c r="R13" s="187"/>
+      <c r="S13" s="187"/>
+      <c r="T13" s="188"/>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
@@ -8026,19 +8174,19 @@
       <c r="I14" s="148">
         <v>44355.378988657401</v>
       </c>
-      <c r="J14" s="188" t="s">
+      <c r="J14" s="189" t="s">
         <v>283</v>
       </c>
-      <c r="K14" s="189"/>
-      <c r="L14" s="189"/>
-      <c r="M14" s="189"/>
-      <c r="N14" s="189"/>
-      <c r="O14" s="189"/>
-      <c r="P14" s="189"/>
-      <c r="Q14" s="189"/>
-      <c r="R14" s="189"/>
-      <c r="S14" s="189"/>
-      <c r="T14" s="189"/>
+      <c r="K14" s="190"/>
+      <c r="L14" s="190"/>
+      <c r="M14" s="190"/>
+      <c r="N14" s="190"/>
+      <c r="O14" s="190"/>
+      <c r="P14" s="190"/>
+      <c r="Q14" s="190"/>
+      <c r="R14" s="190"/>
+      <c r="S14" s="190"/>
+      <c r="T14" s="190"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
@@ -23318,11 +23466,11 @@
   <dimension ref="A1:AB168"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="9" ySplit="10" topLeftCell="J66" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="10" topLeftCell="J96" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="J93" activeCellId="2" sqref="T93:W93 O93:R93 J93:M93"/>
+      <selection pane="bottomRight" activeCell="O118" sqref="O118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -23818,19 +23966,19 @@
       <c r="I13" s="149">
         <v>44526.640759722199</v>
       </c>
-      <c r="J13" s="185" t="s">
+      <c r="J13" s="186" t="s">
         <v>313</v>
       </c>
-      <c r="K13" s="186"/>
-      <c r="L13" s="186"/>
-      <c r="M13" s="186"/>
-      <c r="N13" s="186"/>
-      <c r="O13" s="186"/>
-      <c r="P13" s="186"/>
-      <c r="Q13" s="186"/>
-      <c r="R13" s="186"/>
-      <c r="S13" s="186"/>
-      <c r="T13" s="187"/>
+      <c r="K13" s="187"/>
+      <c r="L13" s="187"/>
+      <c r="M13" s="187"/>
+      <c r="N13" s="187"/>
+      <c r="O13" s="187"/>
+      <c r="P13" s="187"/>
+      <c r="Q13" s="187"/>
+      <c r="R13" s="187"/>
+      <c r="S13" s="187"/>
+      <c r="T13" s="188"/>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
@@ -23857,19 +24005,19 @@
       <c r="I14" s="148">
         <v>44336.775273148101</v>
       </c>
-      <c r="J14" s="188" t="s">
+      <c r="J14" s="189" t="s">
         <v>305</v>
       </c>
-      <c r="K14" s="189"/>
-      <c r="L14" s="189"/>
-      <c r="M14" s="189"/>
-      <c r="N14" s="189"/>
-      <c r="O14" s="189"/>
-      <c r="P14" s="189"/>
-      <c r="Q14" s="189"/>
-      <c r="R14" s="189"/>
-      <c r="S14" s="189"/>
-      <c r="T14" s="189"/>
+      <c r="K14" s="190"/>
+      <c r="L14" s="190"/>
+      <c r="M14" s="190"/>
+      <c r="N14" s="190"/>
+      <c r="O14" s="190"/>
+      <c r="P14" s="190"/>
+      <c r="Q14" s="190"/>
+      <c r="R14" s="190"/>
+      <c r="S14" s="190"/>
+      <c r="T14" s="190"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
@@ -26859,21 +27007,21 @@
         <v>250</v>
       </c>
       <c r="I93" s="2"/>
-      <c r="J93" s="192" t="s">
+      <c r="J93" s="185" t="s">
         <v>72</v>
       </c>
-      <c r="K93" s="192"/>
-      <c r="L93" s="192"/>
-      <c r="M93" s="192"/>
+      <c r="K93" s="185"/>
+      <c r="L93" s="185"/>
+      <c r="M93" s="185"/>
       <c r="N93" s="2"/>
-      <c r="O93" s="192" t="s">
+      <c r="O93" s="185" t="s">
         <v>73</v>
       </c>
       <c r="P93" s="52"/>
       <c r="Q93" s="52"/>
       <c r="R93" s="52"/>
       <c r="S93" s="2"/>
-      <c r="T93" s="192" t="s">
+      <c r="T93" s="185" t="s">
         <v>75</v>
       </c>
       <c r="U93" s="52"/>
@@ -27458,8 +27606,8 @@
       <c r="F108" s="25"/>
       <c r="G108" s="12"/>
       <c r="H108" s="171" t="str">
-        <f>COUNTIFS($B$1:$B108, "«")&amp;" REV trait info"</f>
-        <v>4 REV trait info</v>
+        <f>COUNTIFS($B$1:$B108, "«")&amp;" REV trait info and pkl feedsupply controls"</f>
+        <v>4 REV trait info and pkl feedsupply controls</v>
       </c>
       <c r="I108" s="6"/>
       <c r="J108" s="6"/>
@@ -27752,8 +27900,12 @@
       <c r="K116" s="36"/>
       <c r="L116" s="36"/>
       <c r="M116" s="36"/>
-      <c r="N116" s="36"/>
-      <c r="O116" s="36"/>
+      <c r="N116" s="36" t="s">
+        <v>314</v>
+      </c>
+      <c r="O116" s="31" t="b">
+        <v>0</v>
+      </c>
       <c r="P116" s="36"/>
       <c r="Q116" s="36"/>
       <c r="R116" s="2"/>
@@ -27785,8 +27937,12 @@
       <c r="K117" s="36"/>
       <c r="L117" s="36"/>
       <c r="M117" s="36"/>
-      <c r="N117" s="36"/>
-      <c r="O117" s="36"/>
+      <c r="N117" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="O117" s="31" t="b">
+        <v>0</v>
+      </c>
       <c r="P117" s="36"/>
       <c r="Q117" s="36"/>
       <c r="R117" s="2"/>
@@ -27822,8 +27978,12 @@
       <c r="K118" s="36"/>
       <c r="L118" s="36"/>
       <c r="M118" s="36"/>
-      <c r="N118" s="36"/>
-      <c r="O118" s="36"/>
+      <c r="N118" s="26" t="s">
+        <v>316</v>
+      </c>
+      <c r="O118" s="31">
+        <v>0</v>
+      </c>
       <c r="P118" s="36"/>
       <c r="Q118" s="36"/>
       <c r="R118" s="2"/>
@@ -30332,23 +30492,23 @@
       <c r="I18" s="31">
         <v>1</v>
       </c>
-      <c r="J18" s="190" t="s">
+      <c r="J18" s="191" t="s">
         <v>22</v>
       </c>
-      <c r="K18" s="190"/>
-      <c r="L18" s="190"/>
-      <c r="M18" s="190"/>
-      <c r="N18" s="190"/>
-      <c r="O18" s="190"/>
-      <c r="P18" s="190"/>
-      <c r="Q18" s="190"/>
-      <c r="R18" s="190"/>
-      <c r="S18" s="190"/>
-      <c r="T18" s="190"/>
-      <c r="U18" s="190"/>
-      <c r="V18" s="190"/>
-      <c r="W18" s="190"/>
-      <c r="X18" s="190"/>
+      <c r="K18" s="191"/>
+      <c r="L18" s="191"/>
+      <c r="M18" s="191"/>
+      <c r="N18" s="191"/>
+      <c r="O18" s="191"/>
+      <c r="P18" s="191"/>
+      <c r="Q18" s="191"/>
+      <c r="R18" s="191"/>
+      <c r="S18" s="191"/>
+      <c r="T18" s="191"/>
+      <c r="U18" s="191"/>
+      <c r="V18" s="191"/>
+      <c r="W18" s="191"/>
+      <c r="X18" s="191"/>
       <c r="Y18" s="2"/>
       <c r="Z18" s="4"/>
       <c r="AA18" s="16"/>
@@ -30443,23 +30603,23 @@
       <c r="I21" s="23">
         <v>1</v>
       </c>
-      <c r="J21" s="188" t="s">
+      <c r="J21" s="189" t="s">
         <v>34</v>
       </c>
-      <c r="K21" s="189"/>
-      <c r="L21" s="189"/>
-      <c r="M21" s="189"/>
-      <c r="N21" s="189"/>
-      <c r="O21" s="189"/>
-      <c r="P21" s="189"/>
-      <c r="Q21" s="189"/>
-      <c r="R21" s="189"/>
-      <c r="S21" s="189"/>
-      <c r="T21" s="189"/>
-      <c r="U21" s="189"/>
-      <c r="V21" s="189"/>
-      <c r="W21" s="189"/>
-      <c r="X21" s="191"/>
+      <c r="K21" s="190"/>
+      <c r="L21" s="190"/>
+      <c r="M21" s="190"/>
+      <c r="N21" s="190"/>
+      <c r="O21" s="190"/>
+      <c r="P21" s="190"/>
+      <c r="Q21" s="190"/>
+      <c r="R21" s="190"/>
+      <c r="S21" s="190"/>
+      <c r="T21" s="190"/>
+      <c r="U21" s="190"/>
+      <c r="V21" s="190"/>
+      <c r="W21" s="190"/>
+      <c r="X21" s="192"/>
       <c r="Y21" s="2"/>
       <c r="Z21" s="4"/>
       <c r="AA21" s="16"/>

</xml_diff>

<commit_message>
fix drys retained, remove min b1 numbers since they were 0 and add some comments
</commit_message>
<xml_diff>
--- a/Structural.xlsx
+++ b/Structural.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\Models\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9236B91-63B7-4EC6-90FC-F64C882F6FFE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D939640E-09BB-4FE3-A7DA-57BA1F88758A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -105,7 +105,6 @@
     <definedName name="i_n2_len">StructuralSA!$M$77</definedName>
     <definedName name="i_n3_len">StructuralSA!$S$77</definedName>
     <definedName name="i_n3_matrix_len">StructuralSA!$S$79</definedName>
-    <definedName name="i_numbers_min_b1">Stock!$L$156:$V$156</definedName>
     <definedName name="i_nut_spread_n0" localSheetId="2">StructuralSA!$J$83</definedName>
     <definedName name="i_nut_spread_n1" localSheetId="2">StructuralSA!$M$83:$M$90</definedName>
     <definedName name="i_nut_spread_n3" localSheetId="2">StructuralSA!$S$83:$S$90</definedName>
@@ -1747,7 +1746,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="316">
   <si>
     <t>Controls for this worksheet</t>
   </si>
@@ -2170,9 +2169,6 @@
   </si>
   <si>
     <t>a_prepost_b1</t>
-  </si>
-  <si>
-    <t>Minimum numbers</t>
   </si>
   <si>
     <t>Mated</t>
@@ -2665,23 +2661,6 @@
     <t>The slices of the 'k2 input cluster' are:</t>
   </si>
   <si>
-    <t>8Jun21: Change definition of the 'k2 input cluster' to include NM so these animals can be differentially fed.
-                 Add comments about difference between 'k2 input cluster' and 'k2 post processing cluster'
-                 Added comment about including the axis length inputs in the first table
-16May21: Remove heading user defined date
-14Apr21: MRY changes for EV pools and confinement (removed about confinement patterns being included)
-12Apr21: Change back to 3N for analysis
-                  1N for LW profile comparisons
-10Apr21: Altered k2 cluster for scan 0 to allocate all ewes to the 11 slice
-                   Changed inputs for GBAL because it can't be represented in the matrix
-4Apr21: Change to 3FVP with 3N
-2Apr21: Change to 3N for dams &amp; 5FVP
-31Mar21: Change the index for the k2 cluster (for the seasonality model)
-29Mar21: Changed to FVP3, 1N for dams, 3N for Offs
-22Mar21: Alter the initial weight &amp; wool spread for the weaners
-1: 1Apr19-Blank worksheet</t>
-  </si>
-  <si>
     <t>Not mated (1)</t>
   </si>
   <si>
@@ -2804,6 +2783,24 @@
   </si>
   <si>
     <t>fs_number</t>
+  </si>
+  <si>
+    <t>2Dec21 remove min numbers b1. it wasnt doing anything in the code.
+8Jun21: Change definition of the 'k2 input cluster' to include NM so these animals can be differentially fed.
+                 Add comments about difference between 'k2 input cluster' and 'k2 post processing cluster'
+                 Added comment about including the axis length inputs in the first table
+16May21: Remove heading user defined date
+14Apr21: MRY changes for EV pools and confinement (removed about confinement patterns being included)
+12Apr21: Change back to 3N for analysis
+                  1N for LW profile comparisons
+10Apr21: Altered k2 cluster for scan 0 to allocate all ewes to the 11 slice
+                   Changed inputs for GBAL because it can't be represented in the matrix
+4Apr21: Change to 3FVP with 3N
+2Apr21: Change to 3N for dams &amp; 5FVP
+31Mar21: Change the index for the k2 cluster (for the seasonality model)
+29Mar21: Changed to FVP3, 1N for dams, 3N for Offs
+22Mar21: Alter the initial weight &amp; wool spread for the weaners
+1: 1Apr19-Blank worksheet</t>
   </si>
 </sst>
 </file>
@@ -5494,7 +5491,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="29"/>
       <c r="I9" s="29" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="J9" s="29" t="s">
         <v>5</v>
@@ -5643,7 +5640,7 @@
         <v>44371.659649305599</v>
       </c>
       <c r="J13" s="186" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="K13" s="187"/>
       <c r="L13" s="187"/>
@@ -5682,7 +5679,7 @@
         <v>44371.660335300898</v>
       </c>
       <c r="J14" s="189" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="K14" s="190"/>
       <c r="L14" s="190"/>
@@ -6664,16 +6661,16 @@
       <c r="F42" s="5"/>
       <c r="G42" s="4"/>
       <c r="H42" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="I42" s="101" t="s">
         <v>164</v>
       </c>
-      <c r="I42" s="101" t="s">
+      <c r="J42" s="101" t="s">
         <v>165</v>
       </c>
-      <c r="J42" s="101" t="s">
+      <c r="K42" s="101" t="s">
         <v>166</v>
-      </c>
-      <c r="K42" s="101" t="s">
-        <v>167</v>
       </c>
       <c r="L42" s="142"/>
       <c r="M42" s="2"/>
@@ -6738,13 +6735,13 @@
       <c r="F44" s="5"/>
       <c r="G44" s="4"/>
       <c r="H44" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="I44" s="101" t="s">
         <v>168</v>
       </c>
-      <c r="I44" s="101" t="s">
+      <c r="J44" s="101" t="s">
         <v>169</v>
-      </c>
-      <c r="J44" s="101" t="s">
-        <v>170</v>
       </c>
       <c r="K44" s="142"/>
       <c r="L44" s="142"/>
@@ -6810,16 +6807,16 @@
       <c r="F46" s="5"/>
       <c r="G46" s="4"/>
       <c r="H46" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I46" s="101" t="s">
+        <v>175</v>
+      </c>
+      <c r="J46" s="101" t="s">
         <v>176</v>
       </c>
-      <c r="J46" s="101" t="s">
+      <c r="K46" s="101" t="s">
         <v>177</v>
-      </c>
-      <c r="K46" s="101" t="s">
-        <v>178</v>
       </c>
       <c r="L46" s="142"/>
       <c r="M46" s="2"/>
@@ -6851,7 +6848,7 @@
       <c r="F47" s="5"/>
       <c r="G47" s="4"/>
       <c r="H47" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I47" s="101" t="b">
         <v>1</v>
@@ -6892,13 +6889,13 @@
       <c r="F48" s="5"/>
       <c r="G48" s="4"/>
       <c r="H48" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I48" s="101" t="s">
+        <v>178</v>
+      </c>
+      <c r="J48" s="101" t="s">
         <v>179</v>
-      </c>
-      <c r="J48" s="101" t="s">
-        <v>180</v>
       </c>
       <c r="K48" s="142"/>
       <c r="L48" s="142"/>
@@ -6931,19 +6928,19 @@
       <c r="F49" s="5"/>
       <c r="G49" s="4"/>
       <c r="H49" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I49" s="101" t="s">
+        <v>180</v>
+      </c>
+      <c r="J49" s="101" t="s">
         <v>181</v>
       </c>
-      <c r="J49" s="101" t="s">
+      <c r="K49" s="101" t="s">
+        <v>267</v>
+      </c>
+      <c r="L49" s="101" t="s">
         <v>182</v>
-      </c>
-      <c r="K49" s="101" t="s">
-        <v>268</v>
-      </c>
-      <c r="L49" s="101" t="s">
-        <v>183</v>
       </c>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -6974,16 +6971,16 @@
       <c r="F50" s="5"/>
       <c r="G50" s="4"/>
       <c r="H50" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I50" s="101" t="s">
+        <v>183</v>
+      </c>
+      <c r="J50" s="101" t="s">
         <v>184</v>
       </c>
-      <c r="J50" s="101" t="s">
+      <c r="K50" s="101" t="s">
         <v>185</v>
-      </c>
-      <c r="K50" s="101" t="s">
-        <v>186</v>
       </c>
       <c r="L50" s="142"/>
       <c r="M50" s="2"/>
@@ -7048,7 +7045,7 @@
       <c r="F52" s="5"/>
       <c r="G52" s="4"/>
       <c r="H52" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I52" s="101">
         <v>6</v>
@@ -7118,7 +7115,7 @@
       <c r="F54" s="5"/>
       <c r="G54" s="4"/>
       <c r="H54" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I54" s="101">
         <v>1</v>
@@ -7188,13 +7185,13 @@
       <c r="F56" s="5"/>
       <c r="G56" s="4"/>
       <c r="H56" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="I56" s="101" t="s">
+        <v>308</v>
+      </c>
+      <c r="J56" s="101" t="s">
         <v>309</v>
-      </c>
-      <c r="I56" s="101" t="s">
-        <v>310</v>
-      </c>
-      <c r="J56" s="101" t="s">
-        <v>311</v>
       </c>
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
@@ -7638,12 +7635,12 @@
   </sheetPr>
   <dimension ref="A1:AE334"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
       <pane xSplit="9" ySplit="10" topLeftCell="J144" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="L156" sqref="L156"/>
+      <selection pane="bottomRight" activeCell="J14" sqref="J14:T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -7987,7 +7984,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="29"/>
       <c r="I9" s="29" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="J9" s="29" t="s">
         <v>5</v>
@@ -8136,7 +8133,7 @@
         <v>44311.756953009302</v>
       </c>
       <c r="J13" s="186" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="K13" s="187"/>
       <c r="L13" s="187"/>
@@ -8175,7 +8172,7 @@
         <v>44355.378988657401</v>
       </c>
       <c r="J14" s="189" t="s">
-        <v>283</v>
+        <v>315</v>
       </c>
       <c r="K14" s="190"/>
       <c r="L14" s="190"/>
@@ -9155,13 +9152,13 @@
       <c r="F42" s="5"/>
       <c r="G42" s="4"/>
       <c r="H42" s="182" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="I42" s="36" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
@@ -9194,7 +9191,7 @@
       <c r="F43" s="5"/>
       <c r="G43" s="4"/>
       <c r="H43" s="113" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I43" s="31">
         <v>-6</v>
@@ -9231,7 +9228,7 @@
       <c r="F44" s="5"/>
       <c r="G44" s="4"/>
       <c r="H44" s="113" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I44" s="31">
         <v>-14</v>
@@ -9268,7 +9265,7 @@
       <c r="F45" s="5"/>
       <c r="G45" s="4"/>
       <c r="H45" s="113" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I45" s="31">
         <v>-4</v>
@@ -9305,7 +9302,7 @@
       <c r="F46" s="5"/>
       <c r="G46" s="4"/>
       <c r="H46" s="113" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I46" s="31">
         <v>-12</v>
@@ -9342,7 +9339,7 @@
       <c r="F47" s="5"/>
       <c r="G47" s="4"/>
       <c r="H47" s="113" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I47" s="31">
         <v>-7</v>
@@ -9379,7 +9376,7 @@
       <c r="F48" s="5"/>
       <c r="G48" s="4"/>
       <c r="H48" s="113" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I48" s="31">
         <v>-5</v>
@@ -9416,7 +9413,7 @@
       <c r="F49" s="5"/>
       <c r="G49" s="4"/>
       <c r="H49" s="113" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I49" s="31">
         <v>-13</v>
@@ -9453,7 +9450,7 @@
       <c r="F50" s="5"/>
       <c r="G50" s="4"/>
       <c r="H50" s="113" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I50" s="31">
         <v>-8</v>
@@ -9490,7 +9487,7 @@
       <c r="F51" s="5"/>
       <c r="G51" s="4"/>
       <c r="H51" s="113" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I51" s="31">
         <v>-17</v>
@@ -9527,7 +9524,7 @@
       <c r="F52" s="5"/>
       <c r="G52" s="4"/>
       <c r="H52" s="113" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I52" s="31">
         <v>-18</v>
@@ -9564,7 +9561,7 @@
       <c r="F53" s="5"/>
       <c r="G53" s="4"/>
       <c r="H53" s="113" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I53" s="31">
         <v>-17</v>
@@ -9601,7 +9598,7 @@
       <c r="F54" s="5"/>
       <c r="G54" s="4"/>
       <c r="H54" s="113" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I54" s="31">
         <v>-11</v>
@@ -9638,7 +9635,7 @@
       <c r="F55" s="5"/>
       <c r="G55" s="4"/>
       <c r="H55" s="113" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I55" s="31">
         <v>-15</v>
@@ -9675,7 +9672,7 @@
       <c r="F56" s="5"/>
       <c r="G56" s="4"/>
       <c r="H56" s="113" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I56" s="31">
         <v>-10</v>
@@ -9714,7 +9711,7 @@
       <c r="F57" s="5"/>
       <c r="G57" s="4"/>
       <c r="H57" s="113" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I57" s="31">
         <v>-3</v>
@@ -9751,7 +9748,7 @@
       <c r="F58" s="5"/>
       <c r="G58" s="4"/>
       <c r="H58" s="113" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I58" s="31">
         <v>-2</v>
@@ -9788,7 +9785,7 @@
       <c r="F59" s="5"/>
       <c r="G59" s="4"/>
       <c r="H59" s="113" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I59" s="31">
         <v>-9</v>
@@ -9858,10 +9855,10 @@
       <c r="F61" s="5"/>
       <c r="G61" s="4"/>
       <c r="H61" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="I61" s="36" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
@@ -9932,7 +9929,7 @@
       <c r="F63" s="5"/>
       <c r="G63" s="4"/>
       <c r="H63" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I63" s="31">
         <v>7.25</v>
@@ -9941,7 +9938,7 @@
         <v>86</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="L63" s="2"/>
       <c r="M63" s="2"/>
@@ -9973,7 +9970,7 @@
       <c r="F64" s="5"/>
       <c r="G64" s="4"/>
       <c r="H64" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I64" s="31">
         <v>4.25</v>
@@ -9982,7 +9979,7 @@
         <v>86</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L64" s="2"/>
       <c r="M64" s="2"/>
@@ -10047,7 +10044,7 @@
       <c r="F66" s="5"/>
       <c r="G66" s="4"/>
       <c r="H66" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I66" s="31">
         <v>8</v>
@@ -11096,7 +11093,7 @@
       <c r="F95" s="5"/>
       <c r="G95" s="4"/>
       <c r="H95" s="116" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I95" s="2"/>
       <c r="J95" s="2" t="s">
@@ -11147,7 +11144,7 @@
       <c r="F96" s="5"/>
       <c r="G96" s="4"/>
       <c r="H96" s="116" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I96" s="2"/>
       <c r="J96" s="2" t="s">
@@ -12000,10 +11997,10 @@
       <c r="F115" s="5"/>
       <c r="G115" s="4"/>
       <c r="H115" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I115" s="26" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J115" s="2" t="s">
         <v>41</v>
@@ -12048,7 +12045,7 @@
       <c r="F116" s="5"/>
       <c r="G116" s="4"/>
       <c r="H116" s="116" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I116" s="2"/>
       <c r="J116" s="2" t="s">
@@ -12170,10 +12167,10 @@
       <c r="F119" s="5"/>
       <c r="G119" s="4"/>
       <c r="H119" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="I119" s="26" t="s">
         <v>143</v>
-      </c>
-      <c r="I119" s="26" t="s">
-        <v>144</v>
       </c>
       <c r="J119" s="2" t="s">
         <v>41</v>
@@ -12217,7 +12214,7 @@
       <c r="F120" s="5"/>
       <c r="G120" s="4"/>
       <c r="H120" s="116" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I120" s="2"/>
       <c r="J120" s="2" t="s">
@@ -13352,7 +13349,7 @@
       <c r="F149" s="5"/>
       <c r="G149" s="4"/>
       <c r="H149" s="64" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I149" s="2"/>
       <c r="J149" s="2"/>
@@ -13409,7 +13406,7 @@
       <c r="F150" s="5"/>
       <c r="G150" s="4"/>
       <c r="H150" s="64" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I150" s="2"/>
       <c r="J150" s="2"/>
@@ -13753,45 +13750,21 @@
       <c r="E156" s="5"/>
       <c r="F156" s="5"/>
       <c r="G156" s="4"/>
-      <c r="H156" s="64" t="s">
-        <v>141</v>
-      </c>
+      <c r="H156" s="64"/>
       <c r="I156" s="2"/>
       <c r="J156" s="2"/>
       <c r="K156" s="2"/>
-      <c r="L156" s="31">
-        <v>0</v>
-      </c>
-      <c r="M156" s="31">
-        <v>0</v>
-      </c>
-      <c r="N156" s="31">
-        <v>0</v>
-      </c>
-      <c r="O156" s="31">
-        <v>0</v>
-      </c>
-      <c r="P156" s="31">
-        <v>0</v>
-      </c>
-      <c r="Q156" s="31">
-        <v>0</v>
-      </c>
-      <c r="R156" s="31">
-        <v>0</v>
-      </c>
-      <c r="S156" s="31">
-        <v>0</v>
-      </c>
-      <c r="T156" s="31">
-        <v>0</v>
-      </c>
-      <c r="U156" s="31">
-        <v>0</v>
-      </c>
-      <c r="V156" s="31">
-        <v>0</v>
-      </c>
+      <c r="L156" s="2"/>
+      <c r="M156" s="2"/>
+      <c r="N156" s="2"/>
+      <c r="O156" s="2"/>
+      <c r="P156" s="2"/>
+      <c r="Q156" s="2"/>
+      <c r="R156" s="2"/>
+      <c r="S156" s="2"/>
+      <c r="T156" s="2"/>
+      <c r="U156" s="2"/>
+      <c r="V156" s="2"/>
       <c r="W156" s="2"/>
       <c r="X156" s="4"/>
       <c r="Y156" s="16"/>
@@ -13847,7 +13820,7 @@
       <c r="F158" s="5"/>
       <c r="G158" s="4"/>
       <c r="H158" s="59" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I158" s="60" t="str">
         <f>"("&amp;ROWS(ia_k2_mlsb1)-2&amp;","&amp;COLUMNS(ia_k2_mlsb1)-1&amp;"): ia_k2_mlsb1(pointers) = input"</f>
@@ -14069,7 +14042,7 @@
       </c>
       <c r="I162" s="103"/>
       <c r="J162" s="103" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K162" s="56">
         <v>1</v>
@@ -14368,7 +14341,7 @@
       </c>
       <c r="I167" s="79"/>
       <c r="J167" s="56" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K167" s="56">
         <v>1</v>
@@ -14840,7 +14813,7 @@
       <c r="F175" s="5"/>
       <c r="G175" s="4"/>
       <c r="H175" s="64" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I175" s="103"/>
       <c r="J175" s="63"/>
@@ -14899,7 +14872,7 @@
       <c r="F176" s="5"/>
       <c r="G176" s="4"/>
       <c r="H176" s="113" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="I176" s="79"/>
       <c r="J176" s="61">
@@ -14960,11 +14933,11 @@
       <c r="F177" s="5"/>
       <c r="G177" s="4"/>
       <c r="H177" s="113" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="I177" s="79"/>
       <c r="J177" s="56" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K177" s="56">
         <v>1</v>
@@ -15021,7 +14994,7 @@
       <c r="F178" s="5"/>
       <c r="G178" s="4"/>
       <c r="H178" s="113" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="I178" s="79"/>
       <c r="J178" s="56"/>
@@ -15080,7 +15053,7 @@
       <c r="F179" s="5"/>
       <c r="G179" s="4"/>
       <c r="H179" s="113" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="I179" s="79"/>
       <c r="J179" s="56"/>
@@ -15139,7 +15112,7 @@
       <c r="F180" s="5"/>
       <c r="G180" s="4"/>
       <c r="H180" s="113" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="I180" s="62"/>
       <c r="J180" s="63"/>
@@ -15198,7 +15171,7 @@
       <c r="F181" s="5"/>
       <c r="G181" s="4"/>
       <c r="H181" s="113" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="I181" s="112">
         <v>1</v>
@@ -15261,7 +15234,7 @@
       <c r="F182" s="5"/>
       <c r="G182" s="4"/>
       <c r="H182" s="113" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="I182" s="103"/>
       <c r="J182" s="103"/>
@@ -15320,7 +15293,7 @@
       <c r="F183" s="5"/>
       <c r="G183" s="4"/>
       <c r="H183" s="113" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="I183" s="103"/>
       <c r="J183" s="103"/>
@@ -16389,7 +16362,7 @@
       <c r="F202" s="5"/>
       <c r="G202" s="4"/>
       <c r="H202" s="59" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I202" s="60" t="str">
         <f>"("&amp;ROWS(ia_ppk2g1_rlsb1)-2&amp;","&amp;COLUMNS(ia_ppk2g1_rlsb1)-1&amp;"): ia_ppk2_vlsb1(pointers) = input"</f>
@@ -16398,37 +16371,37 @@
       <c r="J202" s="49"/>
       <c r="K202" s="49"/>
       <c r="L202" s="150" t="s">
+        <v>226</v>
+      </c>
+      <c r="M202" s="151" t="s">
         <v>227</v>
       </c>
-      <c r="M202" s="151" t="s">
+      <c r="N202" s="151" t="s">
         <v>228</v>
       </c>
-      <c r="N202" s="151" t="s">
+      <c r="O202" s="151" t="s">
         <v>229</v>
       </c>
-      <c r="O202" s="151" t="s">
+      <c r="P202" s="151" t="s">
         <v>230</v>
       </c>
-      <c r="P202" s="151" t="s">
+      <c r="Q202" s="151" t="s">
         <v>231</v>
       </c>
-      <c r="Q202" s="151" t="s">
+      <c r="R202" s="151" t="s">
         <v>232</v>
       </c>
-      <c r="R202" s="151" t="s">
+      <c r="S202" s="151" t="s">
         <v>233</v>
       </c>
-      <c r="S202" s="151" t="s">
+      <c r="T202" s="151" t="s">
         <v>234</v>
       </c>
-      <c r="T202" s="151" t="s">
+      <c r="U202" s="151" t="s">
         <v>235</v>
       </c>
-      <c r="U202" s="151" t="s">
+      <c r="V202" s="152" t="s">
         <v>236</v>
-      </c>
-      <c r="V202" s="152" t="s">
-        <v>237</v>
       </c>
       <c r="W202" s="94"/>
       <c r="X202" s="4"/>
@@ -16623,7 +16596,7 @@
         <v>117</v>
       </c>
       <c r="I206" s="54" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J206" s="54" t="s">
         <v>108</v>
@@ -16746,10 +16719,10 @@
         <v>130</v>
       </c>
       <c r="I208" s="103" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J208" s="103" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K208" s="56">
         <v>1</v>
@@ -17096,7 +17069,7 @@
       </c>
       <c r="I213" s="79"/>
       <c r="J213" s="56" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K213" s="56">
         <v>1</v>
@@ -17774,7 +17747,7 @@
       <c r="H223" s="26"/>
       <c r="I223" s="79"/>
       <c r="J223" s="56" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K223" s="56">
         <v>1</v>
@@ -18113,7 +18086,7 @@
       <c r="G228" s="4"/>
       <c r="H228" s="26"/>
       <c r="I228" s="103" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J228" s="103"/>
       <c r="K228" s="56">
@@ -19455,7 +19428,7 @@
       <c r="G248" s="4"/>
       <c r="H248" s="26"/>
       <c r="I248" s="103" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J248" s="103"/>
       <c r="K248" s="56">
@@ -20964,7 +20937,7 @@
         <v>131</v>
       </c>
       <c r="I273" s="123" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J273" s="57">
         <v>0</v>
@@ -21022,10 +20995,10 @@
         <v>132</v>
       </c>
       <c r="I274" s="103" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J274" s="103" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K274" s="56">
         <v>1</v>
@@ -21078,7 +21051,7 @@
       <c r="G275" s="4"/>
       <c r="H275" s="64"/>
       <c r="I275" s="103" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J275" s="103"/>
       <c r="K275" s="56">
@@ -21131,7 +21104,7 @@
       <c r="G276" s="4"/>
       <c r="H276" s="64"/>
       <c r="I276" s="103" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J276" s="103"/>
       <c r="K276" s="56">
@@ -21183,7 +21156,7 @@
       <c r="G277" s="4"/>
       <c r="H277" s="64"/>
       <c r="I277" s="103" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J277" s="103"/>
       <c r="K277" s="63">
@@ -21293,7 +21266,7 @@
       <c r="H279" s="113"/>
       <c r="I279" s="79"/>
       <c r="J279" s="56" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K279" s="56">
         <v>1</v>
@@ -21813,7 +21786,7 @@
       <c r="H289" s="113"/>
       <c r="I289" s="79"/>
       <c r="J289" s="56" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K289" s="56">
         <v>1</v>
@@ -22434,13 +22407,13 @@
       <c r="H305" s="29"/>
       <c r="I305" s="29"/>
       <c r="J305" s="180" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K305" s="180" t="s">
         <v>96</v>
       </c>
       <c r="L305" s="180" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="M305" s="180"/>
       <c r="N305" s="180"/>
@@ -22473,13 +22446,13 @@
       <c r="H306" s="29"/>
       <c r="I306" s="29"/>
       <c r="J306" s="180" t="s">
+        <v>203</v>
+      </c>
+      <c r="K306" s="180" t="s">
         <v>204</v>
       </c>
-      <c r="K306" s="180" t="s">
+      <c r="L306" s="180" t="s">
         <v>205</v>
-      </c>
-      <c r="L306" s="180" t="s">
-        <v>206</v>
       </c>
       <c r="M306" s="180"/>
       <c r="N306" s="180"/>
@@ -22664,7 +22637,7 @@
       <c r="F311" s="5"/>
       <c r="G311" s="4"/>
       <c r="H311" s="100" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I311" s="2"/>
       <c r="J311" s="2"/>
@@ -22699,7 +22672,7 @@
       <c r="F312" s="5"/>
       <c r="G312" s="4"/>
       <c r="H312" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="I312" s="2"/>
       <c r="J312" s="31" t="b">
@@ -22740,7 +22713,7 @@
       <c r="F313" s="5"/>
       <c r="G313" s="4"/>
       <c r="H313" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I313" s="2"/>
       <c r="J313" s="121">
@@ -22781,7 +22754,7 @@
       <c r="F314" s="5"/>
       <c r="G314" s="4"/>
       <c r="H314" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="I314" s="2"/>
       <c r="J314" s="31" t="b">
@@ -22890,13 +22863,13 @@
       <c r="H317" s="2"/>
       <c r="I317" s="145"/>
       <c r="J317" s="146" t="s">
+        <v>220</v>
+      </c>
+      <c r="K317" s="146" t="s">
         <v>221</v>
       </c>
-      <c r="K317" s="146" t="s">
+      <c r="L317" s="146" t="s">
         <v>222</v>
-      </c>
-      <c r="L317" s="146" t="s">
-        <v>223</v>
       </c>
       <c r="M317" s="2"/>
       <c r="N317" s="2"/>
@@ -22927,7 +22900,7 @@
       <c r="F318" s="5"/>
       <c r="G318" s="4"/>
       <c r="H318" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I318" s="145"/>
       <c r="J318" s="31">
@@ -23465,8 +23438,8 @@
   </sheetPr>
   <dimension ref="A1:AB168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="9" ySplit="10" topLeftCell="J96" activePane="bottomRight" state="frozen"/>
+    <sheetView topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="9" ySplit="10" topLeftCell="J16" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
@@ -23818,7 +23791,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="29"/>
       <c r="I9" s="29" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="J9" s="29" t="s">
         <v>5</v>
@@ -23967,7 +23940,7 @@
         <v>44526.640759722199</v>
       </c>
       <c r="J13" s="186" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="K13" s="187"/>
       <c r="L13" s="187"/>
@@ -24006,7 +23979,7 @@
         <v>44336.775273148101</v>
       </c>
       <c r="J14" s="189" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="K14" s="190"/>
       <c r="L14" s="190"/>
@@ -24795,7 +24768,7 @@
         <v>97</v>
       </c>
       <c r="O36" s="180" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="P36" s="180"/>
       <c r="Q36" s="180"/>
@@ -24829,10 +24802,10 @@
       <c r="L37" s="29"/>
       <c r="M37" s="180"/>
       <c r="N37" s="180" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="O37" s="180" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="P37" s="180"/>
       <c r="Q37" s="180"/>
@@ -25004,7 +24977,7 @@
       <c r="F42" s="5"/>
       <c r="G42" s="4"/>
       <c r="H42" s="100" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
@@ -25039,7 +25012,7 @@
       <c r="F43" s="5"/>
       <c r="G43" s="4"/>
       <c r="H43" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
@@ -25078,7 +25051,7 @@
       <c r="F44" s="5"/>
       <c r="G44" s="4"/>
       <c r="H44" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
@@ -25117,7 +25090,7 @@
       <c r="F45" s="5"/>
       <c r="G45" s="4"/>
       <c r="H45" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
@@ -25154,7 +25127,7 @@
       <c r="F46" s="5"/>
       <c r="G46" s="4"/>
       <c r="H46" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
@@ -25191,7 +25164,7 @@
       <c r="F47" s="5"/>
       <c r="G47" s="4"/>
       <c r="H47" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
@@ -25294,17 +25267,17 @@
       <c r="F50" s="5"/>
       <c r="G50" s="4"/>
       <c r="H50" s="100" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I50" s="2"/>
       <c r="J50" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="K50" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="K50" s="2" t="s">
+      <c r="L50" s="2" t="s">
         <v>218</v>
-      </c>
-      <c r="L50" s="2" t="s">
-        <v>219</v>
       </c>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -25337,13 +25310,13 @@
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
       <c r="J51" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="K51" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="K51" s="2" t="s">
+      <c r="L51" s="2" t="s">
         <v>205</v>
-      </c>
-      <c r="L51" s="2" t="s">
-        <v>206</v>
       </c>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
@@ -25374,7 +25347,7 @@
       <c r="F52" s="5"/>
       <c r="G52" s="4"/>
       <c r="H52" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I52" s="2"/>
       <c r="J52" s="31" t="b">
@@ -25415,7 +25388,7 @@
       <c r="F53" s="5"/>
       <c r="G53" s="4"/>
       <c r="H53" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I53" s="2"/>
       <c r="J53" s="31" t="b">
@@ -26025,7 +25998,7 @@
         <v>106</v>
       </c>
       <c r="Q70" s="29" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="R70" s="29"/>
       <c r="S70" s="147" t="s">
@@ -26214,7 +26187,7 @@
       <c r="N75" s="2"/>
       <c r="O75" s="2"/>
       <c r="P75" s="116" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="Q75" s="31">
         <v>10</v>
@@ -26483,38 +26456,38 @@
       <c r="F82" s="5"/>
       <c r="G82" s="4"/>
       <c r="H82" s="172" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I82" s="2"/>
       <c r="J82" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="K82" s="36" t="s">
+        <v>310</v>
+      </c>
+      <c r="L82" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="K82" s="36" t="s">
-        <v>312</v>
-      </c>
-      <c r="L82" s="2" t="s">
-        <v>240</v>
-      </c>
       <c r="M82" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="N82" s="36" t="s">
+        <v>310</v>
+      </c>
+      <c r="O82" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="N82" s="36" t="s">
-        <v>312</v>
-      </c>
-      <c r="O82" s="2" t="s">
-        <v>240</v>
       </c>
       <c r="P82" s="2"/>
       <c r="Q82" s="2"/>
       <c r="R82" s="2"/>
       <c r="S82" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="T82" s="36" t="s">
+        <v>310</v>
+      </c>
+      <c r="U82" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="T82" s="36" t="s">
-        <v>312</v>
-      </c>
-      <c r="U82" s="2" t="s">
-        <v>240</v>
       </c>
       <c r="V82" s="2"/>
       <c r="W82" s="2"/>
@@ -26538,7 +26511,7 @@
       <c r="F83" s="5"/>
       <c r="G83" s="4"/>
       <c r="H83" s="175" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I83" s="2"/>
       <c r="J83" s="173">
@@ -26593,7 +26566,7 @@
       <c r="F84" s="5"/>
       <c r="G84" s="4"/>
       <c r="H84" s="175" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I84" s="2"/>
       <c r="J84" s="172"/>
@@ -26642,7 +26615,7 @@
       <c r="F85" s="5"/>
       <c r="G85" s="4"/>
       <c r="H85" s="175" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I85" s="2"/>
       <c r="J85" s="172"/>
@@ -26691,7 +26664,7 @@
       <c r="F86" s="5"/>
       <c r="G86" s="4"/>
       <c r="H86" s="175" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I86" s="2"/>
       <c r="J86" s="172"/>
@@ -26740,7 +26713,7 @@
       <c r="F87" s="5"/>
       <c r="G87" s="4"/>
       <c r="H87" s="175" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I87" s="2"/>
       <c r="J87" s="172"/>
@@ -26789,7 +26762,7 @@
       <c r="F88" s="5"/>
       <c r="G88" s="4"/>
       <c r="H88" s="175" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I88" s="2"/>
       <c r="J88" s="172"/>
@@ -26838,7 +26811,7 @@
       <c r="F89" s="5"/>
       <c r="G89" s="4"/>
       <c r="H89" s="175" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I89" s="2"/>
       <c r="J89" s="172"/>
@@ -26887,7 +26860,7 @@
       <c r="F90" s="5"/>
       <c r="G90" s="4"/>
       <c r="H90" s="175" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I90" s="2"/>
       <c r="J90" s="172"/>
@@ -27004,7 +26977,7 @@
       <c r="F93" s="5"/>
       <c r="G93" s="4"/>
       <c r="H93" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I93" s="2"/>
       <c r="J93" s="185" t="s">
@@ -27047,42 +27020,42 @@
       <c r="H94" s="2"/>
       <c r="I94" s="2"/>
       <c r="J94" s="100" t="s">
+        <v>250</v>
+      </c>
+      <c r="K94" s="100" t="s">
         <v>251</v>
       </c>
-      <c r="K94" s="100" t="s">
+      <c r="L94" s="100" t="s">
         <v>252</v>
       </c>
-      <c r="L94" s="100" t="s">
+      <c r="M94" s="100" t="s">
         <v>253</v>
-      </c>
-      <c r="M94" s="100" t="s">
-        <v>254</v>
       </c>
       <c r="N94" s="2"/>
       <c r="O94" s="100" t="s">
+        <v>250</v>
+      </c>
+      <c r="P94" s="100" t="s">
         <v>251</v>
       </c>
-      <c r="P94" s="100" t="s">
+      <c r="Q94" s="100" t="s">
         <v>252</v>
       </c>
-      <c r="Q94" s="100" t="s">
+      <c r="R94" s="100" t="s">
         <v>253</v>
-      </c>
-      <c r="R94" s="100" t="s">
-        <v>254</v>
       </c>
       <c r="S94" s="2"/>
       <c r="T94" s="100" t="s">
+        <v>250</v>
+      </c>
+      <c r="U94" s="100" t="s">
         <v>251</v>
       </c>
-      <c r="U94" s="100" t="s">
+      <c r="V94" s="100" t="s">
         <v>252</v>
       </c>
-      <c r="V94" s="100" t="s">
+      <c r="W94" s="100" t="s">
         <v>253</v>
-      </c>
-      <c r="W94" s="100" t="s">
-        <v>254</v>
       </c>
       <c r="X94" s="4"/>
       <c r="Y94" s="16"/>
@@ -27104,7 +27077,7 @@
       <c r="F95" s="5"/>
       <c r="G95" s="4"/>
       <c r="H95" s="175" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I95" s="2"/>
       <c r="J95" s="176">
@@ -27165,7 +27138,7 @@
       <c r="F96" s="5"/>
       <c r="G96" s="4"/>
       <c r="H96" s="175" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I96" s="2"/>
       <c r="J96" s="2"/>
@@ -27218,7 +27191,7 @@
       <c r="F97" s="5"/>
       <c r="G97" s="4"/>
       <c r="H97" s="175" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I97" s="2"/>
       <c r="J97" s="2"/>
@@ -27891,7 +27864,7 @@
       <c r="F116" s="5"/>
       <c r="G116" s="4"/>
       <c r="H116" s="26" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I116" s="31" t="b">
         <v>0</v>
@@ -27901,7 +27874,7 @@
       <c r="L116" s="36"/>
       <c r="M116" s="36"/>
       <c r="N116" s="36" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="O116" s="31" t="b">
         <v>0</v>
@@ -27938,7 +27911,7 @@
       <c r="L117" s="36"/>
       <c r="M117" s="36"/>
       <c r="N117" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="O117" s="31" t="b">
         <v>0</v>
@@ -27969,7 +27942,7 @@
       <c r="F118" s="5"/>
       <c r="G118" s="4"/>
       <c r="H118" s="26" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I118" s="31">
         <v>0</v>
@@ -27979,7 +27952,7 @@
       <c r="L118" s="36"/>
       <c r="M118" s="36"/>
       <c r="N118" s="26" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="O118" s="31">
         <v>0</v>
@@ -28080,10 +28053,10 @@
       <c r="F121" s="5"/>
       <c r="G121" s="4"/>
       <c r="H121" s="64" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I121" s="64" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J121" s="2"/>
       <c r="K121" s="2"/>
@@ -28119,7 +28092,7 @@
       <c r="F122" s="5"/>
       <c r="G122" s="4"/>
       <c r="H122" s="31" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I122" s="31" t="b">
         <v>0</v>
@@ -28158,7 +28131,7 @@
       <c r="F123" s="5"/>
       <c r="G123" s="4"/>
       <c r="H123" s="31" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="I123" s="31" t="b">
         <v>0</v>
@@ -28197,7 +28170,7 @@
       <c r="F124" s="5"/>
       <c r="G124" s="4"/>
       <c r="H124" s="31" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I124" s="31" t="b">
         <v>0</v>
@@ -28236,7 +28209,7 @@
       <c r="F125" s="5"/>
       <c r="G125" s="4"/>
       <c r="H125" s="31" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I125" s="31" t="b">
         <v>0</v>
@@ -28275,7 +28248,7 @@
       <c r="F126" s="5"/>
       <c r="G126" s="4"/>
       <c r="H126" s="31" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I126" s="31" t="b">
         <v>0</v>
@@ -28314,7 +28287,7 @@
       <c r="F127" s="5"/>
       <c r="G127" s="4"/>
       <c r="H127" s="31" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I127" s="31" t="b">
         <v>0</v>
@@ -28353,7 +28326,7 @@
       <c r="F128" s="5"/>
       <c r="G128" s="4"/>
       <c r="H128" s="31" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I128" s="31" t="b">
         <v>0</v>
@@ -28392,7 +28365,7 @@
       <c r="F129" s="5"/>
       <c r="G129" s="4"/>
       <c r="H129" s="31" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I129" s="31" t="b">
         <v>0</v>
@@ -28839,7 +28812,7 @@
       </c>
       <c r="G142" s="13"/>
       <c r="H142" s="8" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="I142" s="7"/>
       <c r="J142" s="7"/>
@@ -28909,7 +28882,7 @@
       <c r="H144" s="29"/>
       <c r="I144" s="29"/>
       <c r="J144" s="65" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="K144" s="65"/>
       <c r="L144" s="65"/>
@@ -29135,13 +29108,13 @@
       <c r="F150" s="5"/>
       <c r="G150" s="4"/>
       <c r="H150" s="64" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="I150" s="31">
         <v>4</v>
       </c>
       <c r="J150" s="183" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="K150" s="2"/>
       <c r="L150" s="2"/>
@@ -29207,7 +29180,7 @@
       <c r="F152" s="5"/>
       <c r="G152" s="4"/>
       <c r="H152" s="64" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="I152" s="2"/>
       <c r="J152" s="2"/>
@@ -29242,7 +29215,7 @@
       <c r="F153" s="5"/>
       <c r="G153" s="4"/>
       <c r="H153" s="184" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="I153" s="2"/>
       <c r="J153" s="31">
@@ -29297,7 +29270,7 @@
       <c r="F154" s="5"/>
       <c r="G154" s="4"/>
       <c r="H154" s="184" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="I154" s="2"/>
       <c r="J154" s="31">

</xml_diff>

<commit_message>
add i_ to rev names and pkl fs inputs and add input to control if t axis is included in generator.
</commit_message>
<xml_diff>
--- a/Structural.xlsx
+++ b/Structural.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\Models\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D939640E-09BB-4FE3-A7DA-57BA1F88758A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{795F1AFB-0B15-4FB9-8D8A-CEDCEA5BCB71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -27,9 +27,6 @@
     <definedName name="a_nyatf_b1">Stock!$L$154:$V$154</definedName>
     <definedName name="dry_groups" localSheetId="0">General!$I$48:$J$48</definedName>
     <definedName name="foo_levels" localSheetId="0">General!$I$50:$K$50</definedName>
-    <definedName name="fs_create" localSheetId="2">StructuralSA!$O$117</definedName>
-    <definedName name="fs_number" localSheetId="2">StructuralSA!$O$118</definedName>
-    <definedName name="fs_use_pkl" localSheetId="2">StructuralSA!$O$116</definedName>
     <definedName name="grain_pools" localSheetId="0">General!$I$44:$J$44</definedName>
     <definedName name="grazing_int" localSheetId="0">General!$I$49:$L$49</definedName>
     <definedName name="i_a0_pos">Stock!$I$43</definedName>
@@ -67,9 +64,13 @@
     <definedName name="i_feedsupply_itn_max">Stock!$I$72</definedName>
     <definedName name="i_fixed_dvp_mask_f1">Stock!$J$314:$L$314</definedName>
     <definedName name="i_fixed_fvp_mask_dams">Stock!$J$312:$L$312</definedName>
+    <definedName name="i_fs_create" localSheetId="2">StructuralSA!$O$117</definedName>
+    <definedName name="i_fs_number" localSheetId="2">StructuralSA!$O$118</definedName>
+    <definedName name="i_fs_use_pkl" localSheetId="2">StructuralSA!$O$116</definedName>
     <definedName name="i_fvp_mask_dams">StructuralSA!$N$43:$O$43</definedName>
     <definedName name="i_fvp_mask_offs">StructuralSA!$J$52:$L$52</definedName>
     <definedName name="i_fvp4_date_i">StructuralSA!$O$45:$O$47</definedName>
+    <definedName name="i_generate_with_t" localSheetId="2">StructuralSA!$R$117</definedName>
     <definedName name="i_i_pos">Stock!$I$50</definedName>
     <definedName name="i_initial_b1">Stock!$L$155:$V$155</definedName>
     <definedName name="i_is_dry_b1">Stock!$L$149:$V$149</definedName>
@@ -113,6 +114,10 @@
     <definedName name="i_p_pos">Stock!$I$55</definedName>
     <definedName name="i_prejoin_offset">Stock!$I$66</definedName>
     <definedName name="i_progeny_w2_len">StructuralSA!$Q$75</definedName>
+    <definedName name="i_rev_create" localSheetId="2">StructuralSA!$I$116</definedName>
+    <definedName name="i_rev_number" localSheetId="2">StructuralSA!$I$118</definedName>
+    <definedName name="i_rev_trait_inc" localSheetId="2">StructuralSA!$I$122:$I$129</definedName>
+    <definedName name="i_rev_trait_name" localSheetId="2">StructuralSA!$H$122:$H$129</definedName>
     <definedName name="i_sim_periods_year">Stock!$I$62</definedName>
     <definedName name="i_transfer_exists_tg1">Stock!$K$119:$N$121</definedName>
     <definedName name="i_w_pos">Stock!$I$56</definedName>
@@ -137,10 +142,6 @@
     <definedName name="pastures_exist" localSheetId="0">General!$I$47:$K$47</definedName>
     <definedName name="phase_len" localSheetId="0">General!$I$52</definedName>
     <definedName name="rdvp_type_r">Stock!$J$318:$L$318</definedName>
-    <definedName name="rev_create" localSheetId="2">StructuralSA!$I$116</definedName>
-    <definedName name="rev_number" localSheetId="2">StructuralSA!$I$118</definedName>
-    <definedName name="rev_trait_inc" localSheetId="2">StructuralSA!$I$122:$I$129</definedName>
-    <definedName name="rev_trait_name" localSheetId="2">StructuralSA!$H$122:$H$129</definedName>
     <definedName name="worker_levels" localSheetId="0">General!$I$42:$K$42</definedName>
     <definedName name="ZA.Gridlines" localSheetId="3">Admin!$L$29</definedName>
     <definedName name="ZA.Headers" localSheetId="3">Admin!$L$30</definedName>
@@ -1569,6 +1570,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="R117" authorId="0" shapeId="0" xr:uid="{C95D9C14-95B2-44CF-9B17-758EFB269999}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Michael Young (21512438):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+When using pkl fs do you want to run the stk generator with t axis. The default is True so that the fs can be different across t axis when using 1n model.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="H118" authorId="0" shapeId="0" xr:uid="{F11FB435-94C6-4D6B-8CF5-C6375FFCCDEC}">
       <text>
         <r>
@@ -1746,7 +1771,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="317">
   <si>
     <t>Controls for this worksheet</t>
   </si>
@@ -2801,6 +2826,9 @@
 29Mar21: Changed to FVP3, 1N for dams, 3N for Offs
 22Mar21: Alter the initial weight &amp; wool spread for the weaners
 1: 1Apr19-Blank worksheet</t>
+  </si>
+  <si>
+    <t>generate with t axis</t>
   </si>
 </sst>
 </file>
@@ -7635,7 +7663,7 @@
   </sheetPr>
   <dimension ref="A1:AE334"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <pane xSplit="9" ySplit="10" topLeftCell="J144" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
@@ -23438,12 +23466,12 @@
   </sheetPr>
   <dimension ref="A1:AB168"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="9" ySplit="10" topLeftCell="J16" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="9" ySplit="10" topLeftCell="J93" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="O118" sqref="O118"/>
+      <selection pane="bottomRight" activeCell="O116" sqref="O116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -27917,8 +27945,12 @@
         <v>0</v>
       </c>
       <c r="P117" s="36"/>
-      <c r="Q117" s="36"/>
-      <c r="R117" s="2"/>
+      <c r="Q117" s="26" t="s">
+        <v>316</v>
+      </c>
+      <c r="R117" s="31" t="b">
+        <v>1</v>
+      </c>
       <c r="S117" s="2"/>
       <c r="T117" s="2"/>
       <c r="U117" s="2"/>

</xml_diff>

<commit_message>
Add range name to control if the r2 feedsupply adjustment is included. No impact on profit. Required for the code changes made 13Jan 6:42am
</commit_message>
<xml_diff>
--- a/Structural.xlsx
+++ b/Structural.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\Models\AFO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8AD8FE7-C7EC-4E20-9BB7-5A66B8D3C21A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C11D069-3629-4432-B62D-917CAA462641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="1095" yWindow="570" windowWidth="27705" windowHeight="15630" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -64,13 +64,13 @@
     <definedName name="i_feedsupply_itn_max">Stock!$I$72</definedName>
     <definedName name="i_fixed_dvp_mask_f1">Stock!$J$314:$L$314</definedName>
     <definedName name="i_fixed_fvp_mask_dams">Stock!$J$312:$L$312</definedName>
-    <definedName name="i_fs_create" localSheetId="2">StructuralSA!$O$117</definedName>
-    <definedName name="i_fs_number" localSheetId="2">StructuralSA!$O$118</definedName>
-    <definedName name="i_fs_use_pkl" localSheetId="2">StructuralSA!$O$116</definedName>
+    <definedName name="i_fs_create" localSheetId="2">StructuralSA!$M$117</definedName>
+    <definedName name="i_fs_number" localSheetId="2">StructuralSA!$M$118</definedName>
+    <definedName name="i_fs_use_pkl" localSheetId="2">StructuralSA!$M$116</definedName>
     <definedName name="i_fvp_mask_dams">StructuralSA!$N$43:$O$43</definedName>
     <definedName name="i_fvp_mask_offs">StructuralSA!$J$52:$L$52</definedName>
     <definedName name="i_fvp4_date_i">StructuralSA!$O$45:$O$47</definedName>
-    <definedName name="i_generate_with_t" localSheetId="2">StructuralSA!$R$117</definedName>
+    <definedName name="i_generate_with_t" localSheetId="2">StructuralSA!$P$117</definedName>
     <definedName name="i_i_pos">Stock!$I$50</definedName>
     <definedName name="i_idx_k" localSheetId="0">General!$M$80:$M$113</definedName>
     <definedName name="i_idx_k1" localSheetId="0">General!$I$80:$I$96</definedName>
@@ -117,6 +117,7 @@
     <definedName name="i_p_pos">Stock!$I$55</definedName>
     <definedName name="i_prejoin_offset">Stock!$I$66</definedName>
     <definedName name="i_progeny_w2_len">StructuralSA!$Q$75</definedName>
+    <definedName name="i_r2adjust_inc">StructuralSA!$U$116</definedName>
     <definedName name="i_rev_create" localSheetId="2">StructuralSA!$I$116</definedName>
     <definedName name="i_rev_number" localSheetId="2">StructuralSA!$I$118</definedName>
     <definedName name="i_rev_trait_inc" localSheetId="2">StructuralSA!$I$122:$I$129</definedName>
@@ -157,7 +158,8 @@
     <definedName name="ZA.WidthCol" localSheetId="3">Admin!$L$26</definedName>
     <definedName name="ZA.ZoomSheet" localSheetId="3">Admin!$O$26</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -165,9 +167,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1436,7 +1436,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Michael Young (21512438):</t>
         </r>
@@ -1445,7 +1445,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 This control allows confinement to occur if it is turned on for the given p6 period (controlled in feedsupply in property inputs)</t>
@@ -1460,7 +1460,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Michael Young (21512438):</t>
         </r>
@@ -1469,7 +1469,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 This control allows confinement to occur if it is turned on for the given p6 period (controlled in feedsupply in property inputs)</t>
@@ -1524,7 +1524,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N116" authorId="0" shapeId="0" xr:uid="{A9138754-B6ED-47ED-AB84-13224D267758}">
+    <comment ref="L116" authorId="0" shapeId="0" xr:uid="{A9138754-B6ED-47ED-AB84-13224D267758}">
       <text>
         <r>
           <rPr>
@@ -1548,7 +1548,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="N117" authorId="0" shapeId="0" xr:uid="{4842D124-AE7E-42FA-B06C-37867218491F}">
+    <comment ref="T116" authorId="1" shapeId="0" xr:uid="{0BE691B8-DC57-483C-A9C2-33F348E1FE81}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>John:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+r2 adjustment is usually included if generating the feed supply from Excel inputs. However, it is usually excluded if using the optimum feedsupply from a pkl file.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L117" authorId="0" shapeId="0" xr:uid="{4842D124-AE7E-42FA-B06C-37867218491F}">
       <text>
         <r>
           <rPr>
@@ -1572,7 +1596,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R117" authorId="0" shapeId="0" xr:uid="{C95D9C14-95B2-44CF-9B17-758EFB269999}">
+    <comment ref="P117" authorId="0" shapeId="0" xr:uid="{C95D9C14-95B2-44CF-9B17-758EFB269999}">
       <text>
         <r>
           <rPr>
@@ -1580,7 +1604,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Michael Young (21512438):</t>
         </r>
@@ -1589,7 +1613,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 When using pkl fs do you want to run the stk generator with t axis. The default is True so that the fs can be different across t axis when using 1n model.</t>
@@ -1620,7 +1644,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N118" authorId="0" shapeId="0" xr:uid="{1D224ECA-F2E2-44DB-A203-7D8A825CE404}">
+    <comment ref="L118" authorId="0" shapeId="0" xr:uid="{1D224ECA-F2E2-44DB-A203-7D8A825CE404}">
       <text>
         <r>
           <rPr>
@@ -1773,7 +1797,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="357">
   <si>
     <t>Controls for this worksheet</t>
   </si>
@@ -2782,24 +2806,6 @@
     <t>Confinement</t>
   </si>
   <si>
-    <t>26Nov21: Add confinement to the nutspread inputs.
-11Jul21: dvp/fvp updates -  to go with node structure (remove season dvp/fvp)
-30Jun21: Change rangename from fev to nv
-24Jun21: Fix the conditional formatting in the Initial LW section.  
-                  Add inputs for the user defined feed pools
-20May21: Add extra N for dams (now 8)
-16May21: Add extra TOL to the extra FVP date
-5May21: Adjust the extra FVP date for TOL[0] (for GEPEP calibration)
-4May21: add random rev
-29Apr21: Added the fixed DVPs to the formula for the number of dam FVPs
-27Apr21: add named ranges to inputs copied from pinp.
-                   Add REV inputs
-                    Split fvp inputs
-25Apr21: Moved inputs from Property.xlsx
-                   Moved FVP &amp; N inputs from Stock
-1: 1Apr19-Created the version control table</t>
-  </si>
-  <si>
     <t>fs_use_pkl</t>
   </si>
   <si>
@@ -2949,6 +2955,28 @@
   <si>
     <t xml:space="preserve">*These shoud match the landuse arrays in universal.xl and property.xl </t>
   </si>
+  <si>
+    <t>Include the i_feedoptions_var_r2p adjustment</t>
+  </si>
+  <si>
+    <t>14Jan22: Add control for r2 adjustments included in the calculations
+26Nov21: Add confinement to the nutspread inputs.
+11Jul21: dvp/fvp updates -  to go with node structure (remove season dvp/fvp)
+30Jun21: Change rangename from fev to nv
+24Jun21: Fix the conditional formatting in the Initial LW section.  
+                  Add inputs for the user defined feed pools
+20May21: Add extra N for dams (now 8)
+16May21: Add extra TOL to the extra FVP date
+5May21: Adjust the extra FVP date for TOL[0] (for GEPEP calibration)
+4May21: add random rev
+29Apr21: Added the fixed DVPs to the formula for the number of dam FVPs
+27Apr21: add named ranges to inputs copied from pinp.
+                   Add REV inputs
+                    Split fvp inputs
+25Apr21: Moved inputs from Property.xlsx
+                   Moved FVP &amp; N inputs from Stock
+1: 1Apr19-Created the version control table</t>
+  </si>
 </sst>
 </file>
 
@@ -2957,7 +2985,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3150,19 +3178,6 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="35">
@@ -4667,6 +4682,21 @@
     <xf numFmtId="0" fontId="22" fillId="8" borderId="25" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="28" xfId="3" applyBorder="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="55" xfId="3" applyBorder="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="56" xfId="3" applyBorder="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="57" xfId="3" applyBorder="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="58" xfId="3" applyBorder="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="38" xfId="12" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -4690,21 +4720,6 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="23" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="28" xfId="3" applyBorder="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="55" xfId="3" applyBorder="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="56" xfId="3" applyBorder="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="57" xfId="3" applyBorder="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="58" xfId="3" applyBorder="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -5358,7 +5373,7 @@
   </sheetPr>
   <dimension ref="A1:AT127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <pane xSplit="9" ySplit="10" topLeftCell="J94" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
@@ -5857,19 +5872,19 @@
       <c r="I13" s="149">
         <v>44371.659649305599</v>
       </c>
-      <c r="J13" s="186" t="s">
+      <c r="J13" s="191" t="s">
         <v>298</v>
       </c>
-      <c r="K13" s="187"/>
-      <c r="L13" s="187"/>
-      <c r="M13" s="187"/>
-      <c r="N13" s="187"/>
-      <c r="O13" s="187"/>
-      <c r="P13" s="187"/>
-      <c r="Q13" s="187"/>
-      <c r="R13" s="187"/>
-      <c r="S13" s="187"/>
-      <c r="T13" s="188"/>
+      <c r="K13" s="192"/>
+      <c r="L13" s="192"/>
+      <c r="M13" s="192"/>
+      <c r="N13" s="192"/>
+      <c r="O13" s="192"/>
+      <c r="P13" s="192"/>
+      <c r="Q13" s="192"/>
+      <c r="R13" s="192"/>
+      <c r="S13" s="192"/>
+      <c r="T13" s="193"/>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
@@ -5896,19 +5911,19 @@
       <c r="I14" s="148">
         <v>44371.660335300898</v>
       </c>
-      <c r="J14" s="189" t="s">
+      <c r="J14" s="194" t="s">
         <v>299</v>
       </c>
-      <c r="K14" s="190"/>
-      <c r="L14" s="190"/>
-      <c r="M14" s="190"/>
-      <c r="N14" s="190"/>
-      <c r="O14" s="190"/>
-      <c r="P14" s="190"/>
-      <c r="Q14" s="190"/>
-      <c r="R14" s="190"/>
-      <c r="S14" s="190"/>
-      <c r="T14" s="190"/>
+      <c r="K14" s="195"/>
+      <c r="L14" s="195"/>
+      <c r="M14" s="195"/>
+      <c r="N14" s="195"/>
+      <c r="O14" s="195"/>
+      <c r="P14" s="195"/>
+      <c r="Q14" s="195"/>
+      <c r="R14" s="195"/>
+      <c r="S14" s="195"/>
+      <c r="T14" s="195"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
@@ -7066,7 +7081,7 @@
       <c r="F47" s="5"/>
       <c r="G47" s="4"/>
       <c r="H47" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I47" s="101" t="b">
         <v>1</v>
@@ -8143,11 +8158,11 @@
       <c r="F77" s="5"/>
       <c r="G77" s="4"/>
       <c r="H77" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I77" s="2"/>
       <c r="J77" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
@@ -8213,16 +8228,16 @@
       <c r="F79" s="5"/>
       <c r="G79" s="4"/>
       <c r="H79" s="2"/>
-      <c r="I79" s="193" t="s">
+      <c r="I79" s="186" t="s">
+        <v>317</v>
+      </c>
+      <c r="J79" s="2"/>
+      <c r="K79" s="186" t="s">
         <v>318</v>
       </c>
-      <c r="J79" s="2"/>
-      <c r="K79" s="193" t="s">
+      <c r="L79" s="2"/>
+      <c r="M79" s="186" t="s">
         <v>319</v>
-      </c>
-      <c r="L79" s="2"/>
-      <c r="M79" s="193" t="s">
-        <v>320</v>
       </c>
       <c r="N79" s="2"/>
       <c r="O79" s="2"/>
@@ -8252,16 +8267,16 @@
       <c r="F80" s="5"/>
       <c r="G80" s="4"/>
       <c r="H80" s="172"/>
-      <c r="I80" s="194" t="s">
+      <c r="I80" s="187" t="s">
+        <v>320</v>
+      </c>
+      <c r="J80" s="190"/>
+      <c r="K80" s="187" t="s">
         <v>321</v>
       </c>
-      <c r="J80" s="197"/>
-      <c r="K80" s="194" t="s">
-        <v>322</v>
-      </c>
-      <c r="L80" s="197"/>
-      <c r="M80" s="194" t="s">
-        <v>322</v>
+      <c r="L80" s="190"/>
+      <c r="M80" s="187" t="s">
+        <v>321</v>
       </c>
       <c r="N80" s="55"/>
       <c r="O80" s="2"/>
@@ -8288,16 +8303,16 @@
       <c r="F81" s="5"/>
       <c r="G81" s="4"/>
       <c r="H81" s="172"/>
-      <c r="I81" s="195" t="s">
+      <c r="I81" s="188" t="s">
+        <v>322</v>
+      </c>
+      <c r="J81" s="190"/>
+      <c r="K81" s="188" t="s">
         <v>323</v>
       </c>
-      <c r="J81" s="197"/>
-      <c r="K81" s="195" t="s">
-        <v>324</v>
-      </c>
-      <c r="L81" s="197"/>
-      <c r="M81" s="195" t="s">
-        <v>324</v>
+      <c r="L81" s="190"/>
+      <c r="M81" s="188" t="s">
+        <v>323</v>
       </c>
       <c r="N81" s="55"/>
       <c r="O81" s="2"/>
@@ -8324,16 +8339,16 @@
       <c r="F82" s="5"/>
       <c r="G82" s="4"/>
       <c r="H82" s="172"/>
-      <c r="I82" s="195" t="s">
+      <c r="I82" s="188" t="s">
+        <v>324</v>
+      </c>
+      <c r="J82" s="190"/>
+      <c r="K82" s="188" t="s">
         <v>325</v>
       </c>
-      <c r="J82" s="197"/>
-      <c r="K82" s="195" t="s">
-        <v>326</v>
-      </c>
-      <c r="L82" s="197"/>
-      <c r="M82" s="195" t="s">
-        <v>321</v>
+      <c r="L82" s="190"/>
+      <c r="M82" s="188" t="s">
+        <v>320</v>
       </c>
       <c r="N82" s="55"/>
       <c r="O82" s="2"/>
@@ -8360,16 +8375,16 @@
       <c r="F83" s="5"/>
       <c r="G83" s="4"/>
       <c r="H83" s="172"/>
-      <c r="I83" s="195" t="s">
+      <c r="I83" s="188" t="s">
+        <v>326</v>
+      </c>
+      <c r="J83" s="190"/>
+      <c r="K83" s="188" t="s">
         <v>327</v>
       </c>
-      <c r="J83" s="197"/>
-      <c r="K83" s="195" t="s">
-        <v>328</v>
-      </c>
-      <c r="L83" s="197"/>
-      <c r="M83" s="195" t="s">
-        <v>323</v>
+      <c r="L83" s="190"/>
+      <c r="M83" s="188" t="s">
+        <v>322</v>
       </c>
       <c r="N83" s="55"/>
       <c r="O83" s="2"/>
@@ -8396,16 +8411,16 @@
       <c r="F84" s="5"/>
       <c r="G84" s="4"/>
       <c r="H84" s="172"/>
-      <c r="I84" s="195" t="s">
+      <c r="I84" s="188" t="s">
+        <v>328</v>
+      </c>
+      <c r="J84" s="190"/>
+      <c r="K84" s="188" t="s">
         <v>329</v>
       </c>
-      <c r="J84" s="197"/>
-      <c r="K84" s="195" t="s">
-        <v>330</v>
-      </c>
-      <c r="L84" s="197"/>
-      <c r="M84" s="195" t="s">
-        <v>325</v>
+      <c r="L84" s="190"/>
+      <c r="M84" s="188" t="s">
+        <v>324</v>
       </c>
       <c r="N84" s="55"/>
       <c r="O84" s="2"/>
@@ -8432,16 +8447,16 @@
       <c r="F85" s="5"/>
       <c r="G85" s="4"/>
       <c r="H85" s="172"/>
-      <c r="I85" s="195" t="s">
+      <c r="I85" s="188" t="s">
+        <v>330</v>
+      </c>
+      <c r="J85" s="190"/>
+      <c r="K85" s="188" t="s">
         <v>331</v>
       </c>
-      <c r="J85" s="197"/>
-      <c r="K85" s="195" t="s">
-        <v>332</v>
-      </c>
-      <c r="L85" s="197"/>
-      <c r="M85" s="195" t="s">
-        <v>327</v>
+      <c r="L85" s="190"/>
+      <c r="M85" s="188" t="s">
+        <v>326</v>
       </c>
       <c r="N85" s="55"/>
       <c r="O85" s="2"/>
@@ -8468,16 +8483,16 @@
       <c r="F86" s="5"/>
       <c r="G86" s="4"/>
       <c r="H86" s="172"/>
-      <c r="I86" s="195" t="s">
+      <c r="I86" s="188" t="s">
+        <v>332</v>
+      </c>
+      <c r="J86" s="190"/>
+      <c r="K86" s="188" t="s">
         <v>333</v>
       </c>
-      <c r="J86" s="197"/>
-      <c r="K86" s="195" t="s">
-        <v>334</v>
-      </c>
-      <c r="L86" s="197"/>
-      <c r="M86" s="195" t="s">
-        <v>329</v>
+      <c r="L86" s="190"/>
+      <c r="M86" s="188" t="s">
+        <v>328</v>
       </c>
       <c r="N86" s="55"/>
       <c r="O86" s="2"/>
@@ -8504,16 +8519,16 @@
       <c r="F87" s="5"/>
       <c r="G87" s="4"/>
       <c r="H87" s="172"/>
-      <c r="I87" s="195" t="s">
+      <c r="I87" s="188" t="s">
+        <v>334</v>
+      </c>
+      <c r="J87" s="190"/>
+      <c r="K87" s="188" t="s">
         <v>335</v>
       </c>
-      <c r="J87" s="197"/>
-      <c r="K87" s="195" t="s">
-        <v>336</v>
-      </c>
-      <c r="L87" s="197"/>
-      <c r="M87" s="195" t="s">
-        <v>328</v>
+      <c r="L87" s="190"/>
+      <c r="M87" s="188" t="s">
+        <v>327</v>
       </c>
       <c r="N87" s="55"/>
       <c r="O87" s="2"/>
@@ -8540,16 +8555,16 @@
       <c r="F88" s="5"/>
       <c r="G88" s="4"/>
       <c r="H88" s="172"/>
-      <c r="I88" s="195" t="s">
+      <c r="I88" s="188" t="s">
+        <v>336</v>
+      </c>
+      <c r="J88" s="190"/>
+      <c r="K88" s="188" t="s">
         <v>337</v>
       </c>
-      <c r="J88" s="197"/>
-      <c r="K88" s="195" t="s">
-        <v>338</v>
-      </c>
-      <c r="L88" s="197"/>
-      <c r="M88" s="195" t="s">
-        <v>330</v>
+      <c r="L88" s="190"/>
+      <c r="M88" s="188" t="s">
+        <v>329</v>
       </c>
       <c r="N88" s="55"/>
       <c r="O88" s="2"/>
@@ -8576,16 +8591,16 @@
       <c r="F89" s="5"/>
       <c r="G89" s="4"/>
       <c r="H89" s="172"/>
-      <c r="I89" s="195" t="s">
+      <c r="I89" s="188" t="s">
+        <v>338</v>
+      </c>
+      <c r="J89" s="190"/>
+      <c r="K89" s="188" t="s">
         <v>339</v>
       </c>
-      <c r="J89" s="197"/>
-      <c r="K89" s="195" t="s">
-        <v>340</v>
-      </c>
-      <c r="L89" s="197"/>
-      <c r="M89" s="195" t="s">
-        <v>332</v>
+      <c r="L89" s="190"/>
+      <c r="M89" s="188" t="s">
+        <v>331</v>
       </c>
       <c r="N89" s="55"/>
       <c r="O89" s="2"/>
@@ -8612,16 +8627,16 @@
       <c r="F90" s="5"/>
       <c r="G90" s="4"/>
       <c r="H90" s="172"/>
-      <c r="I90" s="195" t="s">
+      <c r="I90" s="188" t="s">
+        <v>340</v>
+      </c>
+      <c r="J90" s="190"/>
+      <c r="K90" s="188" t="s">
         <v>341</v>
       </c>
-      <c r="J90" s="197"/>
-      <c r="K90" s="195" t="s">
-        <v>342</v>
-      </c>
-      <c r="L90" s="197"/>
-      <c r="M90" s="195" t="s">
-        <v>331</v>
+      <c r="L90" s="190"/>
+      <c r="M90" s="188" t="s">
+        <v>330</v>
       </c>
       <c r="N90" s="55"/>
       <c r="O90" s="2"/>
@@ -8648,16 +8663,16 @@
       <c r="F91" s="5"/>
       <c r="G91" s="4"/>
       <c r="H91" s="172"/>
-      <c r="I91" s="195" t="s">
+      <c r="I91" s="188" t="s">
+        <v>342</v>
+      </c>
+      <c r="J91" s="190"/>
+      <c r="K91" s="188" t="s">
         <v>343</v>
       </c>
-      <c r="J91" s="197"/>
-      <c r="K91" s="195" t="s">
-        <v>344</v>
-      </c>
-      <c r="L91" s="197"/>
-      <c r="M91" s="195" t="s">
-        <v>333</v>
+      <c r="L91" s="190"/>
+      <c r="M91" s="188" t="s">
+        <v>332</v>
       </c>
       <c r="N91" s="55"/>
       <c r="O91" s="2"/>
@@ -8684,16 +8699,16 @@
       <c r="F92" s="5"/>
       <c r="G92" s="4"/>
       <c r="H92" s="172"/>
-      <c r="I92" s="195" t="s">
+      <c r="I92" s="188" t="s">
+        <v>344</v>
+      </c>
+      <c r="J92" s="190"/>
+      <c r="K92" s="188" t="s">
         <v>345</v>
       </c>
-      <c r="J92" s="197"/>
-      <c r="K92" s="195" t="s">
-        <v>346</v>
-      </c>
-      <c r="L92" s="197"/>
-      <c r="M92" s="195" t="s">
-        <v>326</v>
+      <c r="L92" s="190"/>
+      <c r="M92" s="188" t="s">
+        <v>325</v>
       </c>
       <c r="N92" s="55"/>
       <c r="O92" s="2"/>
@@ -8720,16 +8735,16 @@
       <c r="F93" s="5"/>
       <c r="G93" s="4"/>
       <c r="H93" s="172"/>
-      <c r="I93" s="195" t="s">
+      <c r="I93" s="188" t="s">
+        <v>346</v>
+      </c>
+      <c r="J93" s="190"/>
+      <c r="K93" s="188" t="s">
         <v>347</v>
       </c>
-      <c r="J93" s="197"/>
-      <c r="K93" s="195" t="s">
-        <v>348</v>
-      </c>
-      <c r="L93" s="197"/>
-      <c r="M93" s="195" t="s">
-        <v>335</v>
+      <c r="L93" s="190"/>
+      <c r="M93" s="188" t="s">
+        <v>334</v>
       </c>
       <c r="N93" s="55"/>
       <c r="O93" s="2"/>
@@ -8756,16 +8771,16 @@
       <c r="F94" s="5"/>
       <c r="G94" s="4"/>
       <c r="H94" s="172"/>
-      <c r="I94" s="195" t="s">
+      <c r="I94" s="188" t="s">
+        <v>348</v>
+      </c>
+      <c r="J94" s="190"/>
+      <c r="K94" s="188" t="s">
         <v>349</v>
       </c>
-      <c r="J94" s="197"/>
-      <c r="K94" s="195" t="s">
-        <v>350</v>
-      </c>
-      <c r="L94" s="197"/>
-      <c r="M94" s="195" t="s">
-        <v>337</v>
+      <c r="L94" s="190"/>
+      <c r="M94" s="188" t="s">
+        <v>336</v>
       </c>
       <c r="N94" s="55"/>
       <c r="O94" s="2"/>
@@ -8792,16 +8807,16 @@
       <c r="F95" s="5"/>
       <c r="G95" s="4"/>
       <c r="H95" s="172"/>
-      <c r="I95" s="195" t="s">
+      <c r="I95" s="188" t="s">
+        <v>350</v>
+      </c>
+      <c r="J95" s="190"/>
+      <c r="K95" s="188" t="s">
         <v>351</v>
       </c>
-      <c r="J95" s="197"/>
-      <c r="K95" s="195" t="s">
-        <v>352</v>
-      </c>
-      <c r="L95" s="197"/>
-      <c r="M95" s="195" t="s">
-        <v>339</v>
+      <c r="L95" s="190"/>
+      <c r="M95" s="188" t="s">
+        <v>338</v>
       </c>
       <c r="N95" s="55"/>
       <c r="O95" s="2"/>
@@ -8828,16 +8843,16 @@
       <c r="F96" s="5"/>
       <c r="G96" s="4"/>
       <c r="H96" s="172"/>
-      <c r="I96" s="196" t="s">
+      <c r="I96" s="189" t="s">
+        <v>352</v>
+      </c>
+      <c r="J96" s="190"/>
+      <c r="K96" s="189" t="s">
         <v>353</v>
       </c>
-      <c r="J96" s="197"/>
-      <c r="K96" s="196" t="s">
-        <v>354</v>
-      </c>
-      <c r="L96" s="197"/>
-      <c r="M96" s="195" t="s">
-        <v>341</v>
+      <c r="L96" s="190"/>
+      <c r="M96" s="188" t="s">
+        <v>340</v>
       </c>
       <c r="N96" s="55"/>
       <c r="O96" s="2"/>
@@ -8868,8 +8883,8 @@
       <c r="J97" s="2"/>
       <c r="K97" s="53"/>
       <c r="L97" s="172"/>
-      <c r="M97" s="195" t="s">
-        <v>343</v>
+      <c r="M97" s="188" t="s">
+        <v>342</v>
       </c>
       <c r="N97" s="55"/>
       <c r="O97" s="2"/>
@@ -8900,8 +8915,8 @@
       <c r="J98" s="2"/>
       <c r="K98" s="2"/>
       <c r="L98" s="172"/>
-      <c r="M98" s="195" t="s">
-        <v>334</v>
+      <c r="M98" s="188" t="s">
+        <v>333</v>
       </c>
       <c r="N98" s="55"/>
       <c r="O98" s="2"/>
@@ -8932,8 +8947,8 @@
       <c r="J99" s="2"/>
       <c r="K99" s="2"/>
       <c r="L99" s="172"/>
-      <c r="M99" s="195" t="s">
-        <v>336</v>
+      <c r="M99" s="188" t="s">
+        <v>335</v>
       </c>
       <c r="N99" s="55"/>
       <c r="O99" s="2"/>
@@ -8964,8 +8979,8 @@
       <c r="J100" s="2"/>
       <c r="K100" s="2"/>
       <c r="L100" s="172"/>
-      <c r="M100" s="195" t="s">
-        <v>338</v>
+      <c r="M100" s="188" t="s">
+        <v>337</v>
       </c>
       <c r="N100" s="55"/>
       <c r="O100" s="2"/>
@@ -8996,8 +9011,8 @@
       <c r="J101" s="2"/>
       <c r="K101" s="2"/>
       <c r="L101" s="172"/>
-      <c r="M101" s="195" t="s">
-        <v>340</v>
+      <c r="M101" s="188" t="s">
+        <v>339</v>
       </c>
       <c r="N101" s="55"/>
       <c r="O101" s="2"/>
@@ -9028,8 +9043,8 @@
       <c r="J102" s="2"/>
       <c r="K102" s="2"/>
       <c r="L102" s="172"/>
-      <c r="M102" s="195" t="s">
-        <v>342</v>
+      <c r="M102" s="188" t="s">
+        <v>341</v>
       </c>
       <c r="N102" s="55"/>
       <c r="O102" s="2"/>
@@ -9060,8 +9075,8 @@
       <c r="J103" s="2"/>
       <c r="K103" s="2"/>
       <c r="L103" s="172"/>
-      <c r="M103" s="195" t="s">
-        <v>344</v>
+      <c r="M103" s="188" t="s">
+        <v>343</v>
       </c>
       <c r="N103" s="55"/>
       <c r="O103" s="2"/>
@@ -9092,8 +9107,8 @@
       <c r="J104" s="2"/>
       <c r="K104" s="2"/>
       <c r="L104" s="172"/>
-      <c r="M104" s="195" t="s">
-        <v>346</v>
+      <c r="M104" s="188" t="s">
+        <v>345</v>
       </c>
       <c r="N104" s="55"/>
       <c r="O104" s="2"/>
@@ -9124,8 +9139,8 @@
       <c r="J105" s="2"/>
       <c r="K105" s="2"/>
       <c r="L105" s="172"/>
-      <c r="M105" s="195" t="s">
-        <v>348</v>
+      <c r="M105" s="188" t="s">
+        <v>347</v>
       </c>
       <c r="N105" s="55"/>
       <c r="O105" s="2"/>
@@ -9156,8 +9171,8 @@
       <c r="J106" s="2"/>
       <c r="K106" s="2"/>
       <c r="L106" s="172"/>
-      <c r="M106" s="195" t="s">
-        <v>345</v>
+      <c r="M106" s="188" t="s">
+        <v>344</v>
       </c>
       <c r="N106" s="55"/>
       <c r="O106" s="2"/>
@@ -9188,8 +9203,8 @@
       <c r="J107" s="2"/>
       <c r="K107" s="2"/>
       <c r="L107" s="172"/>
-      <c r="M107" s="195" t="s">
-        <v>347</v>
+      <c r="M107" s="188" t="s">
+        <v>346</v>
       </c>
       <c r="N107" s="55"/>
       <c r="O107" s="2"/>
@@ -9220,8 +9235,8 @@
       <c r="J108" s="2"/>
       <c r="K108" s="2"/>
       <c r="L108" s="172"/>
-      <c r="M108" s="195" t="s">
-        <v>349</v>
+      <c r="M108" s="188" t="s">
+        <v>348</v>
       </c>
       <c r="N108" s="55"/>
       <c r="O108" s="2"/>
@@ -9252,8 +9267,8 @@
       <c r="J109" s="2"/>
       <c r="K109" s="2"/>
       <c r="L109" s="172"/>
-      <c r="M109" s="195" t="s">
-        <v>350</v>
+      <c r="M109" s="188" t="s">
+        <v>349</v>
       </c>
       <c r="N109" s="55"/>
       <c r="O109" s="2"/>
@@ -9287,8 +9302,8 @@
       <c r="J110" s="2"/>
       <c r="K110" s="2"/>
       <c r="L110" s="172"/>
-      <c r="M110" s="195" t="s">
-        <v>352</v>
+      <c r="M110" s="188" t="s">
+        <v>351</v>
       </c>
       <c r="N110" s="55"/>
       <c r="O110" s="2"/>
@@ -9322,8 +9337,8 @@
       <c r="J111" s="2"/>
       <c r="K111" s="2"/>
       <c r="L111" s="172"/>
-      <c r="M111" s="195" t="s">
-        <v>354</v>
+      <c r="M111" s="188" t="s">
+        <v>353</v>
       </c>
       <c r="N111" s="55"/>
       <c r="O111" s="2"/>
@@ -9357,8 +9372,8 @@
       <c r="J112" s="2"/>
       <c r="K112" s="2"/>
       <c r="L112" s="172"/>
-      <c r="M112" s="195" t="s">
-        <v>351</v>
+      <c r="M112" s="188" t="s">
+        <v>350</v>
       </c>
       <c r="N112" s="55"/>
       <c r="O112" s="2"/>
@@ -9392,8 +9407,8 @@
       <c r="J113" s="2"/>
       <c r="K113" s="2"/>
       <c r="L113" s="172"/>
-      <c r="M113" s="196" t="s">
-        <v>353</v>
+      <c r="M113" s="189" t="s">
+        <v>352</v>
       </c>
       <c r="N113" s="55"/>
       <c r="O113" s="2"/>
@@ -10364,19 +10379,19 @@
       <c r="I13" s="149">
         <v>44311.756953009302</v>
       </c>
-      <c r="J13" s="186" t="s">
+      <c r="J13" s="191" t="s">
         <v>305</v>
       </c>
-      <c r="K13" s="187"/>
-      <c r="L13" s="187"/>
-      <c r="M13" s="187"/>
-      <c r="N13" s="187"/>
-      <c r="O13" s="187"/>
-      <c r="P13" s="187"/>
-      <c r="Q13" s="187"/>
-      <c r="R13" s="187"/>
-      <c r="S13" s="187"/>
-      <c r="T13" s="188"/>
+      <c r="K13" s="192"/>
+      <c r="L13" s="192"/>
+      <c r="M13" s="192"/>
+      <c r="N13" s="192"/>
+      <c r="O13" s="192"/>
+      <c r="P13" s="192"/>
+      <c r="Q13" s="192"/>
+      <c r="R13" s="192"/>
+      <c r="S13" s="192"/>
+      <c r="T13" s="193"/>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
@@ -10403,19 +10418,19 @@
       <c r="I14" s="148">
         <v>44355.378988657401</v>
       </c>
-      <c r="J14" s="189" t="s">
-        <v>314</v>
-      </c>
-      <c r="K14" s="190"/>
-      <c r="L14" s="190"/>
-      <c r="M14" s="190"/>
-      <c r="N14" s="190"/>
-      <c r="O14" s="190"/>
-      <c r="P14" s="190"/>
-      <c r="Q14" s="190"/>
-      <c r="R14" s="190"/>
-      <c r="S14" s="190"/>
-      <c r="T14" s="190"/>
+      <c r="J14" s="194" t="s">
+        <v>313</v>
+      </c>
+      <c r="K14" s="195"/>
+      <c r="L14" s="195"/>
+      <c r="M14" s="195"/>
+      <c r="N14" s="195"/>
+      <c r="O14" s="195"/>
+      <c r="P14" s="195"/>
+      <c r="Q14" s="195"/>
+      <c r="R14" s="195"/>
+      <c r="S14" s="195"/>
+      <c r="T14" s="195"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
@@ -25670,12 +25685,12 @@
   </sheetPr>
   <dimension ref="A1:AB168"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="9" ySplit="10" topLeftCell="J93" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="O116" sqref="O116"/>
+      <selection pane="bottomRight" activeCell="U116" sqref="U116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -26169,21 +26184,21 @@
         <v>16</v>
       </c>
       <c r="I13" s="149">
-        <v>44526.640759722199</v>
-      </c>
-      <c r="J13" s="186" t="s">
-        <v>310</v>
-      </c>
-      <c r="K13" s="187"/>
-      <c r="L13" s="187"/>
-      <c r="M13" s="187"/>
-      <c r="N13" s="187"/>
-      <c r="O13" s="187"/>
-      <c r="P13" s="187"/>
-      <c r="Q13" s="187"/>
-      <c r="R13" s="187"/>
-      <c r="S13" s="187"/>
-      <c r="T13" s="188"/>
+        <v>44575.469814583303</v>
+      </c>
+      <c r="J13" s="191" t="s">
+        <v>356</v>
+      </c>
+      <c r="K13" s="192"/>
+      <c r="L13" s="192"/>
+      <c r="M13" s="192"/>
+      <c r="N13" s="192"/>
+      <c r="O13" s="192"/>
+      <c r="P13" s="192"/>
+      <c r="Q13" s="192"/>
+      <c r="R13" s="192"/>
+      <c r="S13" s="192"/>
+      <c r="T13" s="193"/>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
@@ -26210,19 +26225,19 @@
       <c r="I14" s="148">
         <v>44336.775273148101</v>
       </c>
-      <c r="J14" s="189" t="s">
+      <c r="J14" s="194" t="s">
         <v>302</v>
       </c>
-      <c r="K14" s="190"/>
-      <c r="L14" s="190"/>
-      <c r="M14" s="190"/>
-      <c r="N14" s="190"/>
-      <c r="O14" s="190"/>
-      <c r="P14" s="190"/>
-      <c r="Q14" s="190"/>
-      <c r="R14" s="190"/>
-      <c r="S14" s="190"/>
-      <c r="T14" s="190"/>
+      <c r="K14" s="195"/>
+      <c r="L14" s="195"/>
+      <c r="M14" s="195"/>
+      <c r="N14" s="195"/>
+      <c r="O14" s="195"/>
+      <c r="P14" s="195"/>
+      <c r="Q14" s="195"/>
+      <c r="R14" s="195"/>
+      <c r="S14" s="195"/>
+      <c r="T14" s="195"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
@@ -30103,20 +30118,24 @@
       </c>
       <c r="J116" s="36"/>
       <c r="K116" s="36"/>
-      <c r="L116" s="36"/>
-      <c r="M116" s="36"/>
-      <c r="N116" s="36" t="s">
-        <v>311</v>
-      </c>
-      <c r="O116" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="P116" s="36"/>
-      <c r="Q116" s="36"/>
+      <c r="L116" s="36" t="s">
+        <v>310</v>
+      </c>
+      <c r="M116" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="N116" s="36"/>
+      <c r="O116" s="36"/>
+      <c r="P116" s="2"/>
+      <c r="Q116" s="2"/>
       <c r="R116" s="2"/>
       <c r="S116" s="2"/>
-      <c r="T116" s="2"/>
-      <c r="U116" s="2"/>
+      <c r="T116" s="26" t="s">
+        <v>355</v>
+      </c>
+      <c r="U116" s="31" t="b">
+        <v>1</v>
+      </c>
       <c r="V116" s="2"/>
       <c r="W116" s="2"/>
       <c r="X116" s="4"/>
@@ -30140,21 +30159,21 @@
       <c r="I117" s="36"/>
       <c r="J117" s="36"/>
       <c r="K117" s="36"/>
-      <c r="L117" s="36"/>
-      <c r="M117" s="36"/>
-      <c r="N117" s="26" t="s">
-        <v>312</v>
-      </c>
-      <c r="O117" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="P117" s="36"/>
-      <c r="Q117" s="26" t="s">
-        <v>315</v>
-      </c>
-      <c r="R117" s="31" t="b">
-        <v>1</v>
-      </c>
+      <c r="L117" s="26" t="s">
+        <v>311</v>
+      </c>
+      <c r="M117" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="N117" s="36"/>
+      <c r="O117" s="26" t="s">
+        <v>314</v>
+      </c>
+      <c r="P117" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q117" s="2"/>
+      <c r="R117" s="2"/>
       <c r="S117" s="2"/>
       <c r="T117" s="2"/>
       <c r="U117" s="2"/>
@@ -30185,16 +30204,16 @@
       </c>
       <c r="J118" s="36"/>
       <c r="K118" s="36"/>
-      <c r="L118" s="36"/>
-      <c r="M118" s="36"/>
-      <c r="N118" s="26" t="s">
-        <v>313</v>
-      </c>
-      <c r="O118" s="31">
-        <v>0</v>
-      </c>
-      <c r="P118" s="36"/>
-      <c r="Q118" s="36"/>
+      <c r="L118" s="26" t="s">
+        <v>312</v>
+      </c>
+      <c r="M118" s="31">
+        <v>0</v>
+      </c>
+      <c r="N118" s="36"/>
+      <c r="O118" s="36"/>
+      <c r="P118" s="2"/>
+      <c r="Q118" s="2"/>
       <c r="R118" s="2"/>
       <c r="S118" s="2"/>
       <c r="T118" s="2"/>
@@ -32701,23 +32720,23 @@
       <c r="I18" s="31">
         <v>1</v>
       </c>
-      <c r="J18" s="191" t="s">
+      <c r="J18" s="196" t="s">
         <v>22</v>
       </c>
-      <c r="K18" s="191"/>
-      <c r="L18" s="191"/>
-      <c r="M18" s="191"/>
-      <c r="N18" s="191"/>
-      <c r="O18" s="191"/>
-      <c r="P18" s="191"/>
-      <c r="Q18" s="191"/>
-      <c r="R18" s="191"/>
-      <c r="S18" s="191"/>
-      <c r="T18" s="191"/>
-      <c r="U18" s="191"/>
-      <c r="V18" s="191"/>
-      <c r="W18" s="191"/>
-      <c r="X18" s="191"/>
+      <c r="K18" s="196"/>
+      <c r="L18" s="196"/>
+      <c r="M18" s="196"/>
+      <c r="N18" s="196"/>
+      <c r="O18" s="196"/>
+      <c r="P18" s="196"/>
+      <c r="Q18" s="196"/>
+      <c r="R18" s="196"/>
+      <c r="S18" s="196"/>
+      <c r="T18" s="196"/>
+      <c r="U18" s="196"/>
+      <c r="V18" s="196"/>
+      <c r="W18" s="196"/>
+      <c r="X18" s="196"/>
       <c r="Y18" s="2"/>
       <c r="Z18" s="4"/>
       <c r="AA18" s="16"/>
@@ -32812,23 +32831,23 @@
       <c r="I21" s="23">
         <v>1</v>
       </c>
-      <c r="J21" s="189" t="s">
+      <c r="J21" s="194" t="s">
         <v>34</v>
       </c>
-      <c r="K21" s="190"/>
-      <c r="L21" s="190"/>
-      <c r="M21" s="190"/>
-      <c r="N21" s="190"/>
-      <c r="O21" s="190"/>
-      <c r="P21" s="190"/>
-      <c r="Q21" s="190"/>
-      <c r="R21" s="190"/>
-      <c r="S21" s="190"/>
-      <c r="T21" s="190"/>
-      <c r="U21" s="190"/>
-      <c r="V21" s="190"/>
-      <c r="W21" s="190"/>
-      <c r="X21" s="192"/>
+      <c r="K21" s="195"/>
+      <c r="L21" s="195"/>
+      <c r="M21" s="195"/>
+      <c r="N21" s="195"/>
+      <c r="O21" s="195"/>
+      <c r="P21" s="195"/>
+      <c r="Q21" s="195"/>
+      <c r="R21" s="195"/>
+      <c r="S21" s="195"/>
+      <c r="T21" s="195"/>
+      <c r="U21" s="195"/>
+      <c r="V21" s="195"/>
+      <c r="W21" s="195"/>
+      <c r="X21" s="197"/>
       <c r="Y21" s="2"/>
       <c r="Z21" s="4"/>
       <c r="AA21" s="16"/>

</xml_diff>

<commit_message>
Add a d axis to the min age for selling progeny and offspring. Fix error in association between g2 & g3 in Structural.xl No effect on Obj
</commit_message>
<xml_diff>
--- a/Structural.xlsx
+++ b/Structural.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C11D069-3629-4432-B62D-917CAA462641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBB2C94-5B17-4584-9B45-E921D846A809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1095" yWindow="570" windowWidth="27705" windowHeight="15630" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="27705" windowHeight="15630" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -158,8 +158,7 @@
     <definedName name="ZA.WidthCol" localSheetId="3">Admin!$L$26</definedName>
     <definedName name="ZA.ZoomSheet" localSheetId="3">Admin!$O$26</definedName>
   </definedNames>
-  <calcPr calcId="191029" refMode="R1C1"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2785,15 +2784,6 @@
     <t>is DVP</t>
   </si>
   <si>
-    <t>11/Jul/21: dvp/fvp updates 
-27Apr21: Split fvp inputs
-25Apr21: Deleted range names i_w1_len &amp; w3
-9Apr21: Fix formatting (box) around k2 cluster definition.
-30Mar21: Added inputs for % dry and number dams mated
-2: 17Jul20-Added structural inputs table
-1: 1Apr19-Created the version control table</t>
-  </si>
-  <si>
     <t>enterprises</t>
   </si>
   <si>
@@ -2813,24 +2803,6 @@
   </si>
   <si>
     <t>fs_number</t>
-  </si>
-  <si>
-    <t>2Dec21 remove min numbers b1. it wasnt doing anything in the code.
-8Jun21: Change definition of the 'k2 input cluster' to include NM so these animals can be differentially fed.
-                 Add comments about difference between 'k2 input cluster' and 'k2 post processing cluster'
-                 Added comment about including the axis length inputs in the first table
-16May21: Remove heading user defined date
-14Apr21: MRY changes for EV pools and confinement (removed about confinement patterns being included)
-12Apr21: Change back to 3N for analysis
-                  1N for LW profile comparisons
-10Apr21: Altered k2 cluster for scan 0 to allocate all ewes to the 11 slice
-                   Changed inputs for GBAL because it can't be represented in the matrix
-4Apr21: Change to 3FVP with 3N
-2Apr21: Change to 3N for dams &amp; 5FVP
-31Mar21: Change the index for the k2 cluster (for the seasonality model)
-29Mar21: Changed to FVP3, 1N for dams, 3N for Offs
-22Mar21: Alter the initial weight &amp; wool spread for the weaners
-1: 1Apr19-Blank worksheet</t>
   </si>
   <si>
     <t>generate with t axis</t>
@@ -2975,6 +2947,34 @@
                     Split fvp inputs
 25Apr21: Moved inputs from Property.xlsx
                    Moved FVP &amp; N inputs from Stock
+1: 1Apr19-Created the version control table</t>
+  </si>
+  <si>
+    <t>19Jan22: Fix error in i_mask_g1g3 that included True for [BMT,BM]
+2Dec21 remove min numbers b1. it wasnt doing anything in the code.
+8Jun21: Change definition of the 'k2 input cluster' to include NM so these animals can be differentially fed.
+                 Add comments about difference between 'k2 input cluster' and 'k2 post processing cluster'
+                 Added comment about including the axis length inputs in the first table
+16May21: Remove heading user defined date
+14Apr21: MRY changes for EV pools and confinement (removed about confinement patterns being included)
+12Apr21: Change back to 3N for analysis
+                  1N for LW profile comparisons
+10Apr21: Altered k2 cluster for scan 0 to allocate all ewes to the 11 slice
+                   Changed inputs for GBAL because it can't be represented in the matrix
+4Apr21: Change to 3FVP with 3N
+2Apr21: Change to 3N for dams &amp; 5FVP
+31Mar21: Change the index for the k2 cluster (for the seasonality model)
+29Mar21: Changed to FVP3, 1N for dams, 3N for Offs
+22Mar21: Alter the initial weight &amp; wool spread for the weaners
+1: 1Apr19-Blank worksheet</t>
+  </si>
+  <si>
+    <t>11Jul21: dvp/fvp updates 
+27Apr21: Split fvp inputs
+25Apr21: Deleted range names i_w1_len &amp; w3
+9Apr21: Fix formatting (box) around k2 cluster definition.
+30Mar21: Added inputs for % dry and number dams mated
+2: 17Jul20-Added structural inputs table
 1: 1Apr19-Created the version control table</t>
   </si>
 </sst>
@@ -7081,7 +7081,7 @@
       <c r="F47" s="5"/>
       <c r="G47" s="4"/>
       <c r="H47" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I47" s="101" t="b">
         <v>1</v>
@@ -7418,13 +7418,13 @@
       <c r="F56" s="5"/>
       <c r="G56" s="4"/>
       <c r="H56" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="I56" s="101" t="s">
         <v>306</v>
       </c>
-      <c r="I56" s="101" t="s">
+      <c r="J56" s="101" t="s">
         <v>307</v>
-      </c>
-      <c r="J56" s="101" t="s">
-        <v>308</v>
       </c>
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
@@ -8158,11 +8158,11 @@
       <c r="F77" s="5"/>
       <c r="G77" s="4"/>
       <c r="H77" s="2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="I77" s="2"/>
       <c r="J77" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
@@ -8229,15 +8229,15 @@
       <c r="G79" s="4"/>
       <c r="H79" s="2"/>
       <c r="I79" s="186" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="J79" s="2"/>
       <c r="K79" s="186" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="L79" s="2"/>
       <c r="M79" s="186" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="N79" s="2"/>
       <c r="O79" s="2"/>
@@ -8268,15 +8268,15 @@
       <c r="G80" s="4"/>
       <c r="H80" s="172"/>
       <c r="I80" s="187" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="J80" s="190"/>
       <c r="K80" s="187" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="L80" s="190"/>
       <c r="M80" s="187" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="N80" s="55"/>
       <c r="O80" s="2"/>
@@ -8304,15 +8304,15 @@
       <c r="G81" s="4"/>
       <c r="H81" s="172"/>
       <c r="I81" s="188" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="J81" s="190"/>
       <c r="K81" s="188" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="L81" s="190"/>
       <c r="M81" s="188" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="N81" s="55"/>
       <c r="O81" s="2"/>
@@ -8340,15 +8340,15 @@
       <c r="G82" s="4"/>
       <c r="H82" s="172"/>
       <c r="I82" s="188" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="J82" s="190"/>
       <c r="K82" s="188" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="L82" s="190"/>
       <c r="M82" s="188" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="N82" s="55"/>
       <c r="O82" s="2"/>
@@ -8376,15 +8376,15 @@
       <c r="G83" s="4"/>
       <c r="H83" s="172"/>
       <c r="I83" s="188" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="J83" s="190"/>
       <c r="K83" s="188" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="L83" s="190"/>
       <c r="M83" s="188" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="N83" s="55"/>
       <c r="O83" s="2"/>
@@ -8412,15 +8412,15 @@
       <c r="G84" s="4"/>
       <c r="H84" s="172"/>
       <c r="I84" s="188" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="J84" s="190"/>
       <c r="K84" s="188" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="L84" s="190"/>
       <c r="M84" s="188" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="N84" s="55"/>
       <c r="O84" s="2"/>
@@ -8448,15 +8448,15 @@
       <c r="G85" s="4"/>
       <c r="H85" s="172"/>
       <c r="I85" s="188" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="J85" s="190"/>
       <c r="K85" s="188" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="L85" s="190"/>
       <c r="M85" s="188" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="N85" s="55"/>
       <c r="O85" s="2"/>
@@ -8484,15 +8484,15 @@
       <c r="G86" s="4"/>
       <c r="H86" s="172"/>
       <c r="I86" s="188" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="J86" s="190"/>
       <c r="K86" s="188" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="L86" s="190"/>
       <c r="M86" s="188" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="N86" s="55"/>
       <c r="O86" s="2"/>
@@ -8520,15 +8520,15 @@
       <c r="G87" s="4"/>
       <c r="H87" s="172"/>
       <c r="I87" s="188" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="J87" s="190"/>
       <c r="K87" s="188" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="L87" s="190"/>
       <c r="M87" s="188" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="N87" s="55"/>
       <c r="O87" s="2"/>
@@ -8556,15 +8556,15 @@
       <c r="G88" s="4"/>
       <c r="H88" s="172"/>
       <c r="I88" s="188" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="J88" s="190"/>
       <c r="K88" s="188" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="L88" s="190"/>
       <c r="M88" s="188" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="N88" s="55"/>
       <c r="O88" s="2"/>
@@ -8592,15 +8592,15 @@
       <c r="G89" s="4"/>
       <c r="H89" s="172"/>
       <c r="I89" s="188" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="J89" s="190"/>
       <c r="K89" s="188" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="L89" s="190"/>
       <c r="M89" s="188" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="N89" s="55"/>
       <c r="O89" s="2"/>
@@ -8628,15 +8628,15 @@
       <c r="G90" s="4"/>
       <c r="H90" s="172"/>
       <c r="I90" s="188" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="J90" s="190"/>
       <c r="K90" s="188" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="L90" s="190"/>
       <c r="M90" s="188" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="N90" s="55"/>
       <c r="O90" s="2"/>
@@ -8664,15 +8664,15 @@
       <c r="G91" s="4"/>
       <c r="H91" s="172"/>
       <c r="I91" s="188" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="J91" s="190"/>
       <c r="K91" s="188" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="L91" s="190"/>
       <c r="M91" s="188" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="N91" s="55"/>
       <c r="O91" s="2"/>
@@ -8700,15 +8700,15 @@
       <c r="G92" s="4"/>
       <c r="H92" s="172"/>
       <c r="I92" s="188" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="J92" s="190"/>
       <c r="K92" s="188" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="L92" s="190"/>
       <c r="M92" s="188" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="N92" s="55"/>
       <c r="O92" s="2"/>
@@ -8736,15 +8736,15 @@
       <c r="G93" s="4"/>
       <c r="H93" s="172"/>
       <c r="I93" s="188" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="J93" s="190"/>
       <c r="K93" s="188" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="L93" s="190"/>
       <c r="M93" s="188" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="N93" s="55"/>
       <c r="O93" s="2"/>
@@ -8772,15 +8772,15 @@
       <c r="G94" s="4"/>
       <c r="H94" s="172"/>
       <c r="I94" s="188" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="J94" s="190"/>
       <c r="K94" s="188" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="L94" s="190"/>
       <c r="M94" s="188" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="N94" s="55"/>
       <c r="O94" s="2"/>
@@ -8808,15 +8808,15 @@
       <c r="G95" s="4"/>
       <c r="H95" s="172"/>
       <c r="I95" s="188" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="J95" s="190"/>
       <c r="K95" s="188" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="L95" s="190"/>
       <c r="M95" s="188" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="N95" s="55"/>
       <c r="O95" s="2"/>
@@ -8844,15 +8844,15 @@
       <c r="G96" s="4"/>
       <c r="H96" s="172"/>
       <c r="I96" s="189" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="J96" s="190"/>
       <c r="K96" s="189" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="L96" s="190"/>
       <c r="M96" s="188" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="N96" s="55"/>
       <c r="O96" s="2"/>
@@ -8884,7 +8884,7 @@
       <c r="K97" s="53"/>
       <c r="L97" s="172"/>
       <c r="M97" s="188" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="N97" s="55"/>
       <c r="O97" s="2"/>
@@ -8916,7 +8916,7 @@
       <c r="K98" s="2"/>
       <c r="L98" s="172"/>
       <c r="M98" s="188" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="N98" s="55"/>
       <c r="O98" s="2"/>
@@ -8948,7 +8948,7 @@
       <c r="K99" s="2"/>
       <c r="L99" s="172"/>
       <c r="M99" s="188" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="N99" s="55"/>
       <c r="O99" s="2"/>
@@ -8980,7 +8980,7 @@
       <c r="K100" s="2"/>
       <c r="L100" s="172"/>
       <c r="M100" s="188" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="N100" s="55"/>
       <c r="O100" s="2"/>
@@ -9012,7 +9012,7 @@
       <c r="K101" s="2"/>
       <c r="L101" s="172"/>
       <c r="M101" s="188" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="N101" s="55"/>
       <c r="O101" s="2"/>
@@ -9044,7 +9044,7 @@
       <c r="K102" s="2"/>
       <c r="L102" s="172"/>
       <c r="M102" s="188" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="N102" s="55"/>
       <c r="O102" s="2"/>
@@ -9076,7 +9076,7 @@
       <c r="K103" s="2"/>
       <c r="L103" s="172"/>
       <c r="M103" s="188" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="N103" s="55"/>
       <c r="O103" s="2"/>
@@ -9108,7 +9108,7 @@
       <c r="K104" s="2"/>
       <c r="L104" s="172"/>
       <c r="M104" s="188" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="N104" s="55"/>
       <c r="O104" s="2"/>
@@ -9140,7 +9140,7 @@
       <c r="K105" s="2"/>
       <c r="L105" s="172"/>
       <c r="M105" s="188" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="N105" s="55"/>
       <c r="O105" s="2"/>
@@ -9172,7 +9172,7 @@
       <c r="K106" s="2"/>
       <c r="L106" s="172"/>
       <c r="M106" s="188" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="N106" s="55"/>
       <c r="O106" s="2"/>
@@ -9204,7 +9204,7 @@
       <c r="K107" s="2"/>
       <c r="L107" s="172"/>
       <c r="M107" s="188" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="N107" s="55"/>
       <c r="O107" s="2"/>
@@ -9236,7 +9236,7 @@
       <c r="K108" s="2"/>
       <c r="L108" s="172"/>
       <c r="M108" s="188" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="N108" s="55"/>
       <c r="O108" s="2"/>
@@ -9268,7 +9268,7 @@
       <c r="K109" s="2"/>
       <c r="L109" s="172"/>
       <c r="M109" s="188" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="N109" s="55"/>
       <c r="O109" s="2"/>
@@ -9303,7 +9303,7 @@
       <c r="K110" s="2"/>
       <c r="L110" s="172"/>
       <c r="M110" s="188" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="N110" s="55"/>
       <c r="O110" s="2"/>
@@ -9338,7 +9338,7 @@
       <c r="K111" s="2"/>
       <c r="L111" s="172"/>
       <c r="M111" s="188" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="N111" s="55"/>
       <c r="O111" s="2"/>
@@ -9373,7 +9373,7 @@
       <c r="K112" s="2"/>
       <c r="L112" s="172"/>
       <c r="M112" s="188" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="N112" s="55"/>
       <c r="O112" s="2"/>
@@ -9408,7 +9408,7 @@
       <c r="K113" s="2"/>
       <c r="L113" s="172"/>
       <c r="M113" s="189" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="N113" s="55"/>
       <c r="O113" s="2"/>
@@ -9882,8 +9882,8 @@
   </sheetPr>
   <dimension ref="A1:AE334"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <pane xSplit="9" ySplit="10" topLeftCell="J144" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <pane xSplit="9" ySplit="10" topLeftCell="J93" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
@@ -10377,10 +10377,10 @@
         <v>16</v>
       </c>
       <c r="I13" s="149">
-        <v>44311.756953009302</v>
+        <v>44388</v>
       </c>
       <c r="J13" s="191" t="s">
-        <v>305</v>
+        <v>356</v>
       </c>
       <c r="K13" s="192"/>
       <c r="L13" s="192"/>
@@ -10416,10 +10416,10 @@
         <v>17</v>
       </c>
       <c r="I14" s="148">
-        <v>44355.378988657401</v>
+        <v>44580.5012369213</v>
       </c>
       <c r="J14" s="194" t="s">
-        <v>313</v>
+        <v>355</v>
       </c>
       <c r="K14" s="195"/>
       <c r="L14" s="195"/>
@@ -13632,7 +13632,7 @@
         <v>0</v>
       </c>
       <c r="L101" s="31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M101" s="31" t="b">
         <v>0</v>
@@ -25685,8 +25685,8 @@
   </sheetPr>
   <dimension ref="A1:AB168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="9" ySplit="10" topLeftCell="J93" activePane="bottomRight" state="frozen"/>
+    <sheetView topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="9" ySplit="10" topLeftCell="J45" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
@@ -26187,7 +26187,7 @@
         <v>44575.469814583303</v>
       </c>
       <c r="J13" s="191" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="K13" s="192"/>
       <c r="L13" s="192"/>
@@ -28710,7 +28710,7 @@
         <v>237</v>
       </c>
       <c r="K82" s="36" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="L82" s="2" t="s">
         <v>238</v>
@@ -28719,7 +28719,7 @@
         <v>237</v>
       </c>
       <c r="N82" s="36" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="O82" s="2" t="s">
         <v>238</v>
@@ -28731,7 +28731,7 @@
         <v>237</v>
       </c>
       <c r="T82" s="36" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="U82" s="2" t="s">
         <v>238</v>
@@ -30119,7 +30119,7 @@
       <c r="J116" s="36"/>
       <c r="K116" s="36"/>
       <c r="L116" s="36" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="M116" s="31" t="b">
         <v>0</v>
@@ -30131,7 +30131,7 @@
       <c r="R116" s="2"/>
       <c r="S116" s="2"/>
       <c r="T116" s="26" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="U116" s="31" t="b">
         <v>1</v>
@@ -30160,14 +30160,14 @@
       <c r="J117" s="36"/>
       <c r="K117" s="36"/>
       <c r="L117" s="26" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="M117" s="31" t="b">
         <v>0</v>
       </c>
       <c r="N117" s="36"/>
       <c r="O117" s="26" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="P117" s="31" t="b">
         <v>1</v>
@@ -30205,7 +30205,7 @@
       <c r="J118" s="36"/>
       <c r="K118" s="36"/>
       <c r="L118" s="26" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="M118" s="31">
         <v>0</v>

</xml_diff>

<commit_message>
Separate the SAV for the feedsupply pickle number for creating and using
</commit_message>
<xml_diff>
--- a/Structural.xlsx
+++ b/Structural.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBB2C94-5B17-4584-9B45-E921D846A809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4C9DBC-DBFC-4D43-B373-81760A225E28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="27705" windowHeight="15630" tabRatio="678" activeTab="1" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="1095" yWindow="570" windowWidth="27705" windowHeight="15630" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -64,8 +64,9 @@
     <definedName name="i_feedsupply_itn_max">Stock!$I$72</definedName>
     <definedName name="i_fixed_dvp_mask_f1">Stock!$J$314:$L$314</definedName>
     <definedName name="i_fixed_fvp_mask_dams">Stock!$J$312:$L$312</definedName>
-    <definedName name="i_fs_create" localSheetId="2">StructuralSA!$M$117</definedName>
-    <definedName name="i_fs_number" localSheetId="2">StructuralSA!$M$118</definedName>
+    <definedName name="i_fs_create_number" localSheetId="2">StructuralSA!$M$119</definedName>
+    <definedName name="i_fs_create_pkl" localSheetId="2">StructuralSA!$M$118</definedName>
+    <definedName name="i_fs_use_number">StructuralSA!$M$117</definedName>
     <definedName name="i_fs_use_pkl" localSheetId="2">StructuralSA!$M$116</definedName>
     <definedName name="i_fvp_mask_dams">StructuralSA!$N$43:$O$43</definedName>
     <definedName name="i_fvp_mask_offs">StructuralSA!$J$52:$L$52</definedName>
@@ -84,7 +85,7 @@
     <definedName name="i_k5_pos">Stock!$I$53</definedName>
     <definedName name="i_lag_organs">Stock!$I$70</definedName>
     <definedName name="i_lag_wool">Stock!$I$69</definedName>
-    <definedName name="i_len_f">StructuralSA!$I$150</definedName>
+    <definedName name="i_len_f">StructuralSA!$I$151</definedName>
     <definedName name="i_len_l">Stock!$M$160</definedName>
     <definedName name="i_len_m">Stock!$L$160</definedName>
     <definedName name="i_len_s">Stock!$N$160</definedName>
@@ -112,16 +113,16 @@
     <definedName name="i_nut_spread_n0" localSheetId="2">StructuralSA!$J$83</definedName>
     <definedName name="i_nut_spread_n1" localSheetId="2">StructuralSA!$M$83:$M$90</definedName>
     <definedName name="i_nut_spread_n3" localSheetId="2">StructuralSA!$S$83:$S$90</definedName>
-    <definedName name="i_nv_lower_p6">StructuralSA!$J$153:$S$153</definedName>
-    <definedName name="i_nv_upper_p6">StructuralSA!$J$154:$S$154</definedName>
+    <definedName name="i_nv_lower_p6">StructuralSA!$J$154:$S$154</definedName>
+    <definedName name="i_nv_upper_p6">StructuralSA!$J$155:$S$155</definedName>
     <definedName name="i_p_pos">Stock!$I$55</definedName>
     <definedName name="i_prejoin_offset">Stock!$I$66</definedName>
     <definedName name="i_progeny_w2_len">StructuralSA!$Q$75</definedName>
     <definedName name="i_r2adjust_inc">StructuralSA!$U$116</definedName>
     <definedName name="i_rev_create" localSheetId="2">StructuralSA!$I$116</definedName>
     <definedName name="i_rev_number" localSheetId="2">StructuralSA!$I$118</definedName>
-    <definedName name="i_rev_trait_inc" localSheetId="2">StructuralSA!$I$122:$I$129</definedName>
-    <definedName name="i_rev_trait_name" localSheetId="2">StructuralSA!$H$122:$H$129</definedName>
+    <definedName name="i_rev_trait_inc" localSheetId="2">StructuralSA!$I$123:$I$130</definedName>
+    <definedName name="i_rev_trait_name" localSheetId="2">StructuralSA!$H$123:$H$130</definedName>
     <definedName name="i_sim_periods_year">Stock!$I$62</definedName>
     <definedName name="i_transfer_exists_tg1">Stock!$K$119:$N$121</definedName>
     <definedName name="i_w_pos">Stock!$I$56</definedName>
@@ -1543,7 +1544,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Controls if a trial uses the pkl feedsupply or used the excel input feedsupply.</t>
+Controls if a trial uses the pkl feedsupply or uses the excel input feedsupply.</t>
         </r>
       </text>
     </comment>
@@ -1571,7 +1572,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L117" authorId="0" shapeId="0" xr:uid="{4842D124-AE7E-42FA-B06C-37867218491F}">
+    <comment ref="L117" authorId="0" shapeId="0" xr:uid="{3A059F15-AF38-4EF5-95AD-1E84708B7362}">
       <text>
         <r>
           <rPr>
@@ -1591,7 +1592,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-This is to controls if the feedsupply from a given trial is saved (typically this will be False except for a group of trials used to determine optimal fs).</t>
+This number is appended to the std fs pickle filename. This allows multiple fs to be stored &amp; accessed simultaneously.</t>
         </r>
       </text>
     </comment>
@@ -1643,7 +1644,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L118" authorId="0" shapeId="0" xr:uid="{1D224ECA-F2E2-44DB-A203-7D8A825CE404}">
+    <comment ref="L118" authorId="0" shapeId="0" xr:uid="{4842D124-AE7E-42FA-B06C-37867218491F}">
       <text>
         <r>
           <rPr>
@@ -1663,11 +1664,36 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-This number is appended to the std fs pickle file. This is required so multiple fs can be stored similtaneously.</t>
+This is to controls if the feedsupply from a given trial is saved (typically this will be False except for a group of trials used to determine optimal fs).</t>
         </r>
       </text>
     </comment>
-    <comment ref="H121" authorId="0" shapeId="0" xr:uid="{FD0151C6-9F6F-4723-995E-804A9122F39A}">
+    <comment ref="L119" authorId="0" shapeId="0" xr:uid="{FAA22A7D-F2B0-4057-B3F4-C98675457DA8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Young (21512438):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This number is appended to the std fs pickle filename. This allows multiple fs to be stored &amp; accessed simultaneously.
+Separate values for use and create allow the steps in the fs optimisation process to be revistited. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H122" authorId="0" shapeId="0" xr:uid="{FD0151C6-9F6F-4723-995E-804A9122F39A}">
       <text>
         <r>
           <rPr>
@@ -1691,7 +1717,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H126" authorId="0" shapeId="0" xr:uid="{B4758F67-1D7E-4D60-BB06-F13A6FE89F0F}">
+    <comment ref="H127" authorId="0" shapeId="0" xr:uid="{B4758F67-1D7E-4D60-BB06-F13A6FE89F0F}">
       <text>
         <r>
           <rPr>
@@ -1715,7 +1741,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H150" authorId="1" shapeId="0" xr:uid="{B39EFDC6-7ABB-4808-93B1-2819F2755236}">
+    <comment ref="H151" authorId="1" shapeId="0" xr:uid="{B39EFDC6-7ABB-4808-93B1-2819F2755236}">
       <text>
         <r>
           <rPr>
@@ -1739,7 +1765,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H153" authorId="1" shapeId="0" xr:uid="{315CC92D-C01A-4D16-90CA-458397130ECA}">
+    <comment ref="H154" authorId="1" shapeId="0" xr:uid="{315CC92D-C01A-4D16-90CA-458397130ECA}">
       <text>
         <r>
           <rPr>
@@ -1765,7 +1791,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H154" authorId="1" shapeId="0" xr:uid="{24292EB5-78CD-4E29-870F-1743067DEF27}">
+    <comment ref="H155" authorId="1" shapeId="0" xr:uid="{24292EB5-78CD-4E29-870F-1743067DEF27}">
       <text>
         <r>
           <rPr>
@@ -1796,7 +1822,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="358">
   <si>
     <t>Controls for this worksheet</t>
   </si>
@@ -2802,9 +2828,6 @@
     <t>fs_create</t>
   </si>
   <si>
-    <t>fs_number</t>
-  </si>
-  <si>
     <t>generate with t axis</t>
   </si>
   <si>
@@ -2929,25 +2952,6 @@
   </si>
   <si>
     <t>Include the i_feedoptions_var_r2p adjustment</t>
-  </si>
-  <si>
-    <t>14Jan22: Add control for r2 adjustments included in the calculations
-26Nov21: Add confinement to the nutspread inputs.
-11Jul21: dvp/fvp updates -  to go with node structure (remove season dvp/fvp)
-30Jun21: Change rangename from fev to nv
-24Jun21: Fix the conditional formatting in the Initial LW section.  
-                  Add inputs for the user defined feed pools
-20May21: Add extra N for dams (now 8)
-16May21: Add extra TOL to the extra FVP date
-5May21: Adjust the extra FVP date for TOL[0] (for GEPEP calibration)
-4May21: add random rev
-29Apr21: Added the fixed DVPs to the formula for the number of dam FVPs
-27Apr21: add named ranges to inputs copied from pinp.
-                   Add REV inputs
-                    Split fvp inputs
-25Apr21: Moved inputs from Property.xlsx
-                   Moved FVP &amp; N inputs from Stock
-1: 1Apr19-Created the version control table</t>
   </si>
   <si>
     <t>19Jan22: Fix error in i_mask_g1g3 that included True for [BMT,BM]
@@ -2975,6 +2979,32 @@
 9Apr21: Fix formatting (box) around k2 cluster definition.
 30Mar21: Added inputs for % dry and number dams mated
 2: 17Jul20-Added structural inputs table
+1: 1Apr19-Created the version control table</t>
+  </si>
+  <si>
+    <t>fs_create_number</t>
+  </si>
+  <si>
+    <t>fs_use_number</t>
+  </si>
+  <si>
+    <t>17Mar22: Add fs_create_number so that the fs optimisatin steps can be examined
+14Jan22: Add control for r2 adjustments included in the calculations
+26Nov21: Add confinement to the nutspread inputs.
+11Jul21: dvp/fvp updates -  to go with node structure (remove season dvp/fvp)
+30Jun21: Change rangename from fev to nv
+24Jun21: Fix the conditional formatting in the Initial LW section.  
+                  Add inputs for the user defined feed pools
+20May21: Add extra N for dams (now 8)
+16May21: Add extra TOL to the extra FVP date
+5May21: Adjust the extra FVP date for TOL[0] (for GEPEP calibration)
+4May21: add random rev
+29Apr21: Added the fixed DVPs to the formula for the number of dam FVPs
+27Apr21: add named ranges to inputs copied from pinp.
+                   Add REV inputs
+                    Split fvp inputs
+25Apr21: Moved inputs from Property.xlsx
+                   Moved FVP &amp; N inputs from Stock
 1: 1Apr19-Created the version control table</t>
   </si>
 </sst>
@@ -7081,7 +7111,7 @@
       <c r="F47" s="5"/>
       <c r="G47" s="4"/>
       <c r="H47" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I47" s="101" t="b">
         <v>1</v>
@@ -8158,11 +8188,11 @@
       <c r="F77" s="5"/>
       <c r="G77" s="4"/>
       <c r="H77" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="I77" s="2"/>
       <c r="J77" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
@@ -8229,15 +8259,15 @@
       <c r="G79" s="4"/>
       <c r="H79" s="2"/>
       <c r="I79" s="186" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="J79" s="2"/>
       <c r="K79" s="186" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L79" s="2"/>
       <c r="M79" s="186" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="N79" s="2"/>
       <c r="O79" s="2"/>
@@ -8268,15 +8298,15 @@
       <c r="G80" s="4"/>
       <c r="H80" s="172"/>
       <c r="I80" s="187" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="J80" s="190"/>
       <c r="K80" s="187" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="L80" s="190"/>
       <c r="M80" s="187" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="N80" s="55"/>
       <c r="O80" s="2"/>
@@ -8304,15 +8334,15 @@
       <c r="G81" s="4"/>
       <c r="H81" s="172"/>
       <c r="I81" s="188" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="J81" s="190"/>
       <c r="K81" s="188" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="L81" s="190"/>
       <c r="M81" s="188" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="N81" s="55"/>
       <c r="O81" s="2"/>
@@ -8340,15 +8370,15 @@
       <c r="G82" s="4"/>
       <c r="H82" s="172"/>
       <c r="I82" s="188" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="J82" s="190"/>
       <c r="K82" s="188" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="L82" s="190"/>
       <c r="M82" s="188" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="N82" s="55"/>
       <c r="O82" s="2"/>
@@ -8376,15 +8406,15 @@
       <c r="G83" s="4"/>
       <c r="H83" s="172"/>
       <c r="I83" s="188" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J83" s="190"/>
       <c r="K83" s="188" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="L83" s="190"/>
       <c r="M83" s="188" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="N83" s="55"/>
       <c r="O83" s="2"/>
@@ -8412,15 +8442,15 @@
       <c r="G84" s="4"/>
       <c r="H84" s="172"/>
       <c r="I84" s="188" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="J84" s="190"/>
       <c r="K84" s="188" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="L84" s="190"/>
       <c r="M84" s="188" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="N84" s="55"/>
       <c r="O84" s="2"/>
@@ -8448,15 +8478,15 @@
       <c r="G85" s="4"/>
       <c r="H85" s="172"/>
       <c r="I85" s="188" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="J85" s="190"/>
       <c r="K85" s="188" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="L85" s="190"/>
       <c r="M85" s="188" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="N85" s="55"/>
       <c r="O85" s="2"/>
@@ -8484,15 +8514,15 @@
       <c r="G86" s="4"/>
       <c r="H86" s="172"/>
       <c r="I86" s="188" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="J86" s="190"/>
       <c r="K86" s="188" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="L86" s="190"/>
       <c r="M86" s="188" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="N86" s="55"/>
       <c r="O86" s="2"/>
@@ -8520,15 +8550,15 @@
       <c r="G87" s="4"/>
       <c r="H87" s="172"/>
       <c r="I87" s="188" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="J87" s="190"/>
       <c r="K87" s="188" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="L87" s="190"/>
       <c r="M87" s="188" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="N87" s="55"/>
       <c r="O87" s="2"/>
@@ -8556,15 +8586,15 @@
       <c r="G88" s="4"/>
       <c r="H88" s="172"/>
       <c r="I88" s="188" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="J88" s="190"/>
       <c r="K88" s="188" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="L88" s="190"/>
       <c r="M88" s="188" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="N88" s="55"/>
       <c r="O88" s="2"/>
@@ -8592,15 +8622,15 @@
       <c r="G89" s="4"/>
       <c r="H89" s="172"/>
       <c r="I89" s="188" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="J89" s="190"/>
       <c r="K89" s="188" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="L89" s="190"/>
       <c r="M89" s="188" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="N89" s="55"/>
       <c r="O89" s="2"/>
@@ -8628,15 +8658,15 @@
       <c r="G90" s="4"/>
       <c r="H90" s="172"/>
       <c r="I90" s="188" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J90" s="190"/>
       <c r="K90" s="188" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="L90" s="190"/>
       <c r="M90" s="188" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="N90" s="55"/>
       <c r="O90" s="2"/>
@@ -8664,15 +8694,15 @@
       <c r="G91" s="4"/>
       <c r="H91" s="172"/>
       <c r="I91" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="J91" s="190"/>
       <c r="K91" s="188" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="L91" s="190"/>
       <c r="M91" s="188" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="N91" s="55"/>
       <c r="O91" s="2"/>
@@ -8700,15 +8730,15 @@
       <c r="G92" s="4"/>
       <c r="H92" s="172"/>
       <c r="I92" s="188" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="J92" s="190"/>
       <c r="K92" s="188" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="L92" s="190"/>
       <c r="M92" s="188" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N92" s="55"/>
       <c r="O92" s="2"/>
@@ -8736,15 +8766,15 @@
       <c r="G93" s="4"/>
       <c r="H93" s="172"/>
       <c r="I93" s="188" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="J93" s="190"/>
       <c r="K93" s="188" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="L93" s="190"/>
       <c r="M93" s="188" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="N93" s="55"/>
       <c r="O93" s="2"/>
@@ -8772,15 +8802,15 @@
       <c r="G94" s="4"/>
       <c r="H94" s="172"/>
       <c r="I94" s="188" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J94" s="190"/>
       <c r="K94" s="188" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="L94" s="190"/>
       <c r="M94" s="188" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="N94" s="55"/>
       <c r="O94" s="2"/>
@@ -8808,15 +8838,15 @@
       <c r="G95" s="4"/>
       <c r="H95" s="172"/>
       <c r="I95" s="188" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="J95" s="190"/>
       <c r="K95" s="188" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="L95" s="190"/>
       <c r="M95" s="188" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="N95" s="55"/>
       <c r="O95" s="2"/>
@@ -8844,15 +8874,15 @@
       <c r="G96" s="4"/>
       <c r="H96" s="172"/>
       <c r="I96" s="189" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="J96" s="190"/>
       <c r="K96" s="189" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="L96" s="190"/>
       <c r="M96" s="188" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="N96" s="55"/>
       <c r="O96" s="2"/>
@@ -8884,7 +8914,7 @@
       <c r="K97" s="53"/>
       <c r="L97" s="172"/>
       <c r="M97" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="N97" s="55"/>
       <c r="O97" s="2"/>
@@ -8916,7 +8946,7 @@
       <c r="K98" s="2"/>
       <c r="L98" s="172"/>
       <c r="M98" s="188" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="N98" s="55"/>
       <c r="O98" s="2"/>
@@ -8948,7 +8978,7 @@
       <c r="K99" s="2"/>
       <c r="L99" s="172"/>
       <c r="M99" s="188" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="N99" s="55"/>
       <c r="O99" s="2"/>
@@ -8980,7 +9010,7 @@
       <c r="K100" s="2"/>
       <c r="L100" s="172"/>
       <c r="M100" s="188" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N100" s="55"/>
       <c r="O100" s="2"/>
@@ -9012,7 +9042,7 @@
       <c r="K101" s="2"/>
       <c r="L101" s="172"/>
       <c r="M101" s="188" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="N101" s="55"/>
       <c r="O101" s="2"/>
@@ -9044,7 +9074,7 @@
       <c r="K102" s="2"/>
       <c r="L102" s="172"/>
       <c r="M102" s="188" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="N102" s="55"/>
       <c r="O102" s="2"/>
@@ -9076,7 +9106,7 @@
       <c r="K103" s="2"/>
       <c r="L103" s="172"/>
       <c r="M103" s="188" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="N103" s="55"/>
       <c r="O103" s="2"/>
@@ -9108,7 +9138,7 @@
       <c r="K104" s="2"/>
       <c r="L104" s="172"/>
       <c r="M104" s="188" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="N104" s="55"/>
       <c r="O104" s="2"/>
@@ -9140,7 +9170,7 @@
       <c r="K105" s="2"/>
       <c r="L105" s="172"/>
       <c r="M105" s="188" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="N105" s="55"/>
       <c r="O105" s="2"/>
@@ -9172,7 +9202,7 @@
       <c r="K106" s="2"/>
       <c r="L106" s="172"/>
       <c r="M106" s="188" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="N106" s="55"/>
       <c r="O106" s="2"/>
@@ -9204,7 +9234,7 @@
       <c r="K107" s="2"/>
       <c r="L107" s="172"/>
       <c r="M107" s="188" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="N107" s="55"/>
       <c r="O107" s="2"/>
@@ -9236,7 +9266,7 @@
       <c r="K108" s="2"/>
       <c r="L108" s="172"/>
       <c r="M108" s="188" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="N108" s="55"/>
       <c r="O108" s="2"/>
@@ -9268,7 +9298,7 @@
       <c r="K109" s="2"/>
       <c r="L109" s="172"/>
       <c r="M109" s="188" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="N109" s="55"/>
       <c r="O109" s="2"/>
@@ -9303,7 +9333,7 @@
       <c r="K110" s="2"/>
       <c r="L110" s="172"/>
       <c r="M110" s="188" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="N110" s="55"/>
       <c r="O110" s="2"/>
@@ -9338,7 +9368,7 @@
       <c r="K111" s="2"/>
       <c r="L111" s="172"/>
       <c r="M111" s="188" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="N111" s="55"/>
       <c r="O111" s="2"/>
@@ -9373,7 +9403,7 @@
       <c r="K112" s="2"/>
       <c r="L112" s="172"/>
       <c r="M112" s="188" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="N112" s="55"/>
       <c r="O112" s="2"/>
@@ -9408,7 +9438,7 @@
       <c r="K113" s="2"/>
       <c r="L113" s="172"/>
       <c r="M113" s="189" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="N113" s="55"/>
       <c r="O113" s="2"/>
@@ -9882,7 +9912,7 @@
   </sheetPr>
   <dimension ref="A1:AE334"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <pane xSplit="9" ySplit="10" topLeftCell="J93" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
@@ -10380,7 +10410,7 @@
         <v>44388</v>
       </c>
       <c r="J13" s="191" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="K13" s="192"/>
       <c r="L13" s="192"/>
@@ -10419,7 +10449,7 @@
         <v>44580.5012369213</v>
       </c>
       <c r="J14" s="194" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="K14" s="195"/>
       <c r="L14" s="195"/>
@@ -25683,14 +25713,14 @@
   <sheetPr codeName="Sheet3">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AB168"/>
+  <dimension ref="A1:AB169"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="9" ySplit="10" topLeftCell="J45" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="9" ySplit="10" topLeftCell="J102" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="U116" sqref="U116"/>
+      <selection pane="bottomRight" activeCell="M117" sqref="M117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -26184,10 +26214,10 @@
         <v>16</v>
       </c>
       <c r="I13" s="149">
-        <v>44575.469814583303</v>
+        <v>44637.790818518501</v>
       </c>
       <c r="J13" s="191" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="K13" s="192"/>
       <c r="L13" s="192"/>
@@ -29784,7 +29814,7 @@
       <c r="A107" s="1"/>
       <c r="B107" s="33"/>
       <c r="C107" s="73">
-        <f>INT(MAX($C$115:$C$132))+1</f>
+        <f>INT(MAX($C$115:$C$133))+1</f>
         <v>5</v>
       </c>
       <c r="D107" s="3"/>
@@ -30131,7 +30161,7 @@
       <c r="R116" s="2"/>
       <c r="S116" s="2"/>
       <c r="T116" s="26" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="U116" s="31" t="b">
         <v>1</v>
@@ -30160,14 +30190,14 @@
       <c r="J117" s="36"/>
       <c r="K117" s="36"/>
       <c r="L117" s="26" t="s">
-        <v>310</v>
-      </c>
-      <c r="M117" s="31" t="b">
+        <v>356</v>
+      </c>
+      <c r="M117" s="31">
         <v>0</v>
       </c>
       <c r="N117" s="36"/>
       <c r="O117" s="26" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="P117" s="31" t="b">
         <v>1</v>
@@ -30185,7 +30215,7 @@
       <c r="AA117" s="1"/>
       <c r="AB117" s="1"/>
     </row>
-    <row r="118" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="33"/>
       <c r="C118" s="73">
@@ -30205,9 +30235,9 @@
       <c r="J118" s="36"/>
       <c r="K118" s="36"/>
       <c r="L118" s="26" t="s">
-        <v>311</v>
-      </c>
-      <c r="M118" s="31">
+        <v>310</v>
+      </c>
+      <c r="M118" s="31" t="b">
         <v>0</v>
       </c>
       <c r="N118" s="36"/>
@@ -30226,141 +30256,139 @@
       <c r="AA118" s="1"/>
       <c r="AB118" s="1"/>
     </row>
-    <row r="119" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="33"/>
       <c r="C119" s="73">
-        <f>INT($C$108)+3.005</f>
-        <v>4.0049999999999999</v>
+        <f>INT(C$108+3)</f>
+        <v>4</v>
       </c>
       <c r="D119" s="4"/>
-      <c r="E119" s="4"/>
-      <c r="F119" s="4"/>
+      <c r="E119" s="5"/>
+      <c r="F119" s="5"/>
       <c r="G119" s="4"/>
-      <c r="H119" s="83"/>
-      <c r="I119" s="83"/>
-      <c r="J119" s="83"/>
-      <c r="K119" s="83"/>
-      <c r="L119" s="83"/>
-      <c r="M119" s="83"/>
-      <c r="N119" s="83"/>
-      <c r="O119" s="83"/>
-      <c r="P119" s="83"/>
-      <c r="Q119" s="83"/>
-      <c r="R119" s="83"/>
-      <c r="S119" s="83"/>
-      <c r="T119" s="83"/>
-      <c r="U119" s="83"/>
-      <c r="V119" s="83"/>
-      <c r="W119" s="83"/>
-      <c r="X119" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="H119" s="172"/>
+      <c r="I119" s="172"/>
+      <c r="J119" s="172"/>
+      <c r="K119" s="172"/>
+      <c r="L119" s="26" t="s">
+        <v>355</v>
+      </c>
+      <c r="M119" s="31">
+        <v>0</v>
+      </c>
+      <c r="N119" s="172"/>
+      <c r="O119" s="172"/>
+      <c r="P119" s="172"/>
+      <c r="Q119" s="172"/>
+      <c r="R119" s="172"/>
+      <c r="S119" s="2"/>
+      <c r="T119" s="2"/>
+      <c r="U119" s="2"/>
+      <c r="V119" s="2"/>
+      <c r="W119" s="2"/>
+      <c r="X119" s="4"/>
       <c r="Y119" s="16"/>
       <c r="Z119" s="1"/>
       <c r="AA119" s="1"/>
       <c r="AB119" s="1"/>
     </row>
-    <row r="120" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="33"/>
       <c r="C120" s="73">
-        <f>INT($C$108)+2.005</f>
-        <v>3.0049999999999999</v>
-      </c>
-      <c r="D120" s="4" t="s">
-        <v>2</v>
-      </c>
+        <f>INT($C$108)+3.005</f>
+        <v>4.0049999999999999</v>
+      </c>
+      <c r="D120" s="4"/>
       <c r="E120" s="4"/>
       <c r="F120" s="4"/>
       <c r="G120" s="4"/>
-      <c r="H120" s="58"/>
-      <c r="I120" s="58"/>
-      <c r="J120" s="58"/>
-      <c r="K120" s="58"/>
-      <c r="L120" s="58"/>
-      <c r="M120" s="58"/>
-      <c r="N120" s="58"/>
-      <c r="O120" s="58"/>
-      <c r="P120" s="58"/>
-      <c r="Q120" s="58"/>
-      <c r="R120" s="58"/>
-      <c r="S120" s="58"/>
-      <c r="T120" s="58"/>
-      <c r="U120" s="58"/>
-      <c r="V120" s="58"/>
-      <c r="W120" s="58"/>
-      <c r="X120" s="4"/>
+      <c r="H120" s="83"/>
+      <c r="I120" s="83"/>
+      <c r="J120" s="83"/>
+      <c r="K120" s="83"/>
+      <c r="L120" s="83"/>
+      <c r="M120" s="83"/>
+      <c r="N120" s="83"/>
+      <c r="O120" s="83"/>
+      <c r="P120" s="83"/>
+      <c r="Q120" s="83"/>
+      <c r="R120" s="83"/>
+      <c r="S120" s="83"/>
+      <c r="T120" s="83"/>
+      <c r="U120" s="83"/>
+      <c r="V120" s="83"/>
+      <c r="W120" s="83"/>
+      <c r="X120" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="Y120" s="16"/>
       <c r="Z120" s="1"/>
       <c r="AA120" s="1"/>
       <c r="AB120" s="1"/>
     </row>
-    <row r="121" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="33"/>
       <c r="C121" s="73">
-        <f>INT($C$108)+2</f>
-        <v>3</v>
-      </c>
-      <c r="D121" s="4"/>
-      <c r="E121" s="5"/>
-      <c r="F121" s="5"/>
+        <f>INT($C$108)+2.005</f>
+        <v>3.0049999999999999</v>
+      </c>
+      <c r="D121" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E121" s="4"/>
+      <c r="F121" s="4"/>
       <c r="G121" s="4"/>
-      <c r="H121" s="64" t="s">
-        <v>259</v>
-      </c>
-      <c r="I121" s="64" t="s">
-        <v>258</v>
-      </c>
-      <c r="J121" s="2"/>
-      <c r="K121" s="2"/>
-      <c r="L121" s="2"/>
-      <c r="M121" s="2"/>
-      <c r="N121" s="2"/>
-      <c r="O121" s="2"/>
-      <c r="P121" s="2"/>
-      <c r="Q121" s="2"/>
-      <c r="R121" s="2"/>
-      <c r="S121" s="2"/>
-      <c r="T121" s="2"/>
-      <c r="U121" s="2"/>
-      <c r="V121" s="2"/>
-      <c r="W121" s="2"/>
+      <c r="H121" s="58"/>
+      <c r="I121" s="58"/>
+      <c r="J121" s="58"/>
+      <c r="K121" s="58"/>
+      <c r="L121" s="58"/>
+      <c r="M121" s="58"/>
+      <c r="N121" s="58"/>
+      <c r="O121" s="58"/>
+      <c r="P121" s="58"/>
+      <c r="Q121" s="58"/>
+      <c r="R121" s="58"/>
+      <c r="S121" s="58"/>
+      <c r="T121" s="58"/>
+      <c r="U121" s="58"/>
+      <c r="V121" s="58"/>
+      <c r="W121" s="58"/>
       <c r="X121" s="4"/>
       <c r="Y121" s="16"/>
       <c r="Z121" s="1"/>
       <c r="AA121" s="1"/>
       <c r="AB121" s="1"/>
     </row>
-    <row r="122" spans="1:28" outlineLevel="3" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="33"/>
       <c r="C122" s="73">
-        <f>INT($C$108)+3</f>
-        <v>4</v>
+        <f>INT($C$108)+2</f>
+        <v>3</v>
       </c>
       <c r="D122" s="4"/>
-      <c r="E122" s="5">
-        <v>0</v>
-      </c>
+      <c r="E122" s="5"/>
       <c r="F122" s="5"/>
       <c r="G122" s="4"/>
-      <c r="H122" s="31" t="s">
-        <v>260</v>
-      </c>
-      <c r="I122" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="J122" s="172"/>
-      <c r="K122" s="172"/>
-      <c r="L122" s="172"/>
-      <c r="M122" s="172"/>
-      <c r="N122" s="172"/>
-      <c r="O122" s="172"/>
-      <c r="P122" s="172"/>
-      <c r="Q122" s="172"/>
-      <c r="R122" s="172"/>
+      <c r="H122" s="64" t="s">
+        <v>259</v>
+      </c>
+      <c r="I122" s="64" t="s">
+        <v>258</v>
+      </c>
+      <c r="J122" s="2"/>
+      <c r="K122" s="2"/>
+      <c r="L122" s="2"/>
+      <c r="M122" s="2"/>
+      <c r="N122" s="2"/>
+      <c r="O122" s="2"/>
+      <c r="P122" s="2"/>
+      <c r="Q122" s="2"/>
+      <c r="R122" s="2"/>
       <c r="S122" s="2"/>
       <c r="T122" s="2"/>
       <c r="U122" s="2"/>
@@ -30372,7 +30400,7 @@
       <c r="AA122" s="1"/>
       <c r="AB122" s="1"/>
     </row>
-    <row r="123" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:28" outlineLevel="3" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
       <c r="B123" s="33"/>
       <c r="C123" s="73">
@@ -30381,12 +30409,12 @@
       </c>
       <c r="D123" s="4"/>
       <c r="E123" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F123" s="5"/>
       <c r="G123" s="4"/>
       <c r="H123" s="31" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I123" s="31" t="b">
         <v>0</v>
@@ -30420,12 +30448,12 @@
       </c>
       <c r="D124" s="4"/>
       <c r="E124" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F124" s="5"/>
       <c r="G124" s="4"/>
       <c r="H124" s="31" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I124" s="31" t="b">
         <v>0</v>
@@ -30454,17 +30482,17 @@
       <c r="A125" s="1"/>
       <c r="B125" s="33"/>
       <c r="C125" s="73">
-        <f>INT(C$108+3)</f>
+        <f>INT($C$108)+3</f>
         <v>4</v>
       </c>
       <c r="D125" s="4"/>
       <c r="E125" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F125" s="5"/>
       <c r="G125" s="4"/>
       <c r="H125" s="31" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="I125" s="31" t="b">
         <v>0</v>
@@ -30498,12 +30526,12 @@
       </c>
       <c r="D126" s="4"/>
       <c r="E126" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F126" s="5"/>
       <c r="G126" s="4"/>
       <c r="H126" s="31" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I126" s="31" t="b">
         <v>0</v>
@@ -30532,17 +30560,17 @@
       <c r="A127" s="1"/>
       <c r="B127" s="33"/>
       <c r="C127" s="73">
-        <f t="shared" ref="C127:C129" si="4">INT(C$108+3)</f>
+        <f>INT(C$108+3)</f>
         <v>4</v>
       </c>
       <c r="D127" s="4"/>
       <c r="E127" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F127" s="5"/>
       <c r="G127" s="4"/>
       <c r="H127" s="31" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I127" s="31" t="b">
         <v>0</v>
@@ -30571,17 +30599,17 @@
       <c r="A128" s="1"/>
       <c r="B128" s="33"/>
       <c r="C128" s="73">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="C128:C130" si="4">INT(C$108+3)</f>
         <v>4</v>
       </c>
       <c r="D128" s="4"/>
       <c r="E128" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F128" s="5"/>
       <c r="G128" s="4"/>
       <c r="H128" s="31" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="I128" s="31" t="b">
         <v>0</v>
@@ -30615,12 +30643,12 @@
       </c>
       <c r="D129" s="4"/>
       <c r="E129" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F129" s="5"/>
       <c r="G129" s="4"/>
       <c r="H129" s="31" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I129" s="31" t="b">
         <v>0</v>
@@ -30649,15 +30677,21 @@
       <c r="A130" s="1"/>
       <c r="B130" s="33"/>
       <c r="C130" s="73">
-        <f>INT(C$108+3)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="D130" s="4"/>
-      <c r="E130" s="5"/>
+      <c r="E130" s="5">
+        <v>7</v>
+      </c>
       <c r="F130" s="5"/>
       <c r="G130" s="4"/>
-      <c r="H130" s="172"/>
-      <c r="I130" s="172"/>
+      <c r="H130" s="31" t="s">
+        <v>268</v>
+      </c>
+      <c r="I130" s="31" t="b">
+        <v>0</v>
+      </c>
       <c r="J130" s="172"/>
       <c r="K130" s="172"/>
       <c r="L130" s="172"/>
@@ -30711,47 +30745,45 @@
       <c r="AA131" s="1"/>
       <c r="AB131" s="1"/>
     </row>
-    <row r="132" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="33"/>
       <c r="C132" s="73">
-        <f>INT($C$108)+3.005</f>
-        <v>4.0049999999999999</v>
+        <f>INT(C$108+3)</f>
+        <v>4</v>
       </c>
       <c r="D132" s="4"/>
-      <c r="E132" s="4"/>
-      <c r="F132" s="4"/>
+      <c r="E132" s="5"/>
+      <c r="F132" s="5"/>
       <c r="G132" s="4"/>
-      <c r="H132" s="4"/>
-      <c r="I132" s="4"/>
-      <c r="J132" s="4"/>
-      <c r="K132" s="4"/>
-      <c r="L132" s="4"/>
-      <c r="M132" s="4"/>
-      <c r="N132" s="4"/>
-      <c r="O132" s="4"/>
-      <c r="P132" s="4"/>
-      <c r="Q132" s="4"/>
-      <c r="R132" s="4"/>
-      <c r="S132" s="4"/>
-      <c r="T132" s="4"/>
-      <c r="U132" s="4"/>
-      <c r="V132" s="4"/>
-      <c r="W132" s="4"/>
-      <c r="X132" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="H132" s="172"/>
+      <c r="I132" s="172"/>
+      <c r="J132" s="172"/>
+      <c r="K132" s="172"/>
+      <c r="L132" s="172"/>
+      <c r="M132" s="172"/>
+      <c r="N132" s="172"/>
+      <c r="O132" s="172"/>
+      <c r="P132" s="172"/>
+      <c r="Q132" s="172"/>
+      <c r="R132" s="172"/>
+      <c r="S132" s="2"/>
+      <c r="T132" s="2"/>
+      <c r="U132" s="2"/>
+      <c r="V132" s="2"/>
+      <c r="W132" s="2"/>
+      <c r="X132" s="4"/>
       <c r="Y132" s="16"/>
       <c r="Z132" s="1"/>
       <c r="AA132" s="1"/>
       <c r="AB132" s="1"/>
     </row>
-    <row r="133" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" s="33"/>
       <c r="C133" s="73">
-        <f>INT($C$108)+2.005</f>
-        <v>3.0049999999999999</v>
+        <f>INT($C$108)+3.005</f>
+        <v>4.0049999999999999</v>
       </c>
       <c r="D133" s="4"/>
       <c r="E133" s="4"/>
@@ -30773,109 +30805,111 @@
       <c r="U133" s="4"/>
       <c r="V133" s="4"/>
       <c r="W133" s="4"/>
-      <c r="X133" s="4"/>
+      <c r="X133" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="Y133" s="16"/>
       <c r="Z133" s="1"/>
       <c r="AA133" s="1"/>
       <c r="AB133" s="1"/>
     </row>
-    <row r="134" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
-      <c r="B134" s="35"/>
-      <c r="C134" s="76">
-        <f>INT($C$108)+1.005</f>
-        <v>2.0049999999999999</v>
-      </c>
-      <c r="D134" s="17"/>
-      <c r="E134" s="17"/>
-      <c r="F134" s="17"/>
-      <c r="G134" s="17"/>
-      <c r="H134" s="17"/>
-      <c r="I134" s="17"/>
-      <c r="J134" s="17"/>
-      <c r="K134" s="17"/>
-      <c r="L134" s="17"/>
-      <c r="M134" s="17"/>
-      <c r="N134" s="17"/>
-      <c r="O134" s="17"/>
-      <c r="P134" s="17"/>
-      <c r="Q134" s="17"/>
-      <c r="R134" s="17"/>
-      <c r="S134" s="17"/>
-      <c r="T134" s="17"/>
-      <c r="U134" s="17"/>
-      <c r="V134" s="17"/>
-      <c r="W134" s="17"/>
-      <c r="X134" s="17"/>
-      <c r="Y134" s="18" t="s">
-        <v>1</v>
-      </c>
+      <c r="B134" s="33"/>
+      <c r="C134" s="73">
+        <f>INT($C$108)+2.005</f>
+        <v>3.0049999999999999</v>
+      </c>
+      <c r="D134" s="4"/>
+      <c r="E134" s="4"/>
+      <c r="F134" s="4"/>
+      <c r="G134" s="4"/>
+      <c r="H134" s="4"/>
+      <c r="I134" s="4"/>
+      <c r="J134" s="4"/>
+      <c r="K134" s="4"/>
+      <c r="L134" s="4"/>
+      <c r="M134" s="4"/>
+      <c r="N134" s="4"/>
+      <c r="O134" s="4"/>
+      <c r="P134" s="4"/>
+      <c r="Q134" s="4"/>
+      <c r="R134" s="4"/>
+      <c r="S134" s="4"/>
+      <c r="T134" s="4"/>
+      <c r="U134" s="4"/>
+      <c r="V134" s="4"/>
+      <c r="W134" s="4"/>
+      <c r="X134" s="4"/>
+      <c r="Y134" s="16"/>
       <c r="Z134" s="1"/>
       <c r="AA134" s="1"/>
       <c r="AB134" s="1"/>
     </row>
-    <row r="135" spans="1:28" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
-      <c r="B135" s="19"/>
-      <c r="C135" s="77">
-        <f>INT($C$108)+0.005</f>
-        <v>1.0049999999999999</v>
-      </c>
-      <c r="D135" s="19"/>
-      <c r="E135" s="19"/>
-      <c r="F135" s="19"/>
-      <c r="G135" s="19"/>
-      <c r="H135" s="19"/>
-      <c r="I135" s="19"/>
-      <c r="J135" s="19"/>
-      <c r="K135" s="19"/>
-      <c r="L135" s="19"/>
-      <c r="M135" s="19"/>
-      <c r="N135" s="19"/>
-      <c r="O135" s="19"/>
-      <c r="P135" s="19"/>
-      <c r="Q135" s="19"/>
-      <c r="R135" s="19"/>
-      <c r="S135" s="19"/>
-      <c r="T135" s="19"/>
-      <c r="U135" s="19"/>
-      <c r="V135" s="19"/>
-      <c r="W135" s="19"/>
-      <c r="X135" s="19"/>
-      <c r="Y135" s="19"/>
+      <c r="B135" s="35"/>
+      <c r="C135" s="76">
+        <f>INT($C$108)+1.005</f>
+        <v>2.0049999999999999</v>
+      </c>
+      <c r="D135" s="17"/>
+      <c r="E135" s="17"/>
+      <c r="F135" s="17"/>
+      <c r="G135" s="17"/>
+      <c r="H135" s="17"/>
+      <c r="I135" s="17"/>
+      <c r="J135" s="17"/>
+      <c r="K135" s="17"/>
+      <c r="L135" s="17"/>
+      <c r="M135" s="17"/>
+      <c r="N135" s="17"/>
+      <c r="O135" s="17"/>
+      <c r="P135" s="17"/>
+      <c r="Q135" s="17"/>
+      <c r="R135" s="17"/>
+      <c r="S135" s="17"/>
+      <c r="T135" s="17"/>
+      <c r="U135" s="17"/>
+      <c r="V135" s="17"/>
+      <c r="W135" s="17"/>
+      <c r="X135" s="17"/>
+      <c r="Y135" s="18" t="s">
+        <v>1</v>
+      </c>
       <c r="Z135" s="1"/>
       <c r="AA135" s="1"/>
       <c r="AB135" s="1"/>
     </row>
-    <row r="136" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:28" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
-      <c r="B136" s="1"/>
-      <c r="C136" s="73">
-        <f>INT($C$108)+2</f>
-        <v>3</v>
-      </c>
-      <c r="D136" s="1"/>
-      <c r="E136" s="1"/>
-      <c r="F136" s="1"/>
-      <c r="G136" s="1"/>
-      <c r="H136" s="1"/>
-      <c r="I136" s="1"/>
-      <c r="J136" s="1"/>
-      <c r="K136" s="1"/>
-      <c r="L136" s="1"/>
-      <c r="M136" s="1"/>
-      <c r="N136" s="1"/>
-      <c r="O136" s="1"/>
-      <c r="P136" s="1"/>
-      <c r="Q136" s="1"/>
-      <c r="R136" s="1"/>
-      <c r="S136" s="1"/>
-      <c r="T136" s="1"/>
-      <c r="U136" s="1"/>
-      <c r="V136" s="1"/>
-      <c r="W136" s="1"/>
-      <c r="X136" s="1"/>
-      <c r="Y136" s="1"/>
+      <c r="B136" s="19"/>
+      <c r="C136" s="77">
+        <f>INT($C$108)+0.005</f>
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="D136" s="19"/>
+      <c r="E136" s="19"/>
+      <c r="F136" s="19"/>
+      <c r="G136" s="19"/>
+      <c r="H136" s="19"/>
+      <c r="I136" s="19"/>
+      <c r="J136" s="19"/>
+      <c r="K136" s="19"/>
+      <c r="L136" s="19"/>
+      <c r="M136" s="19"/>
+      <c r="N136" s="19"/>
+      <c r="O136" s="19"/>
+      <c r="P136" s="19"/>
+      <c r="Q136" s="19"/>
+      <c r="R136" s="19"/>
+      <c r="S136" s="19"/>
+      <c r="T136" s="19"/>
+      <c r="U136" s="19"/>
+      <c r="V136" s="19"/>
+      <c r="W136" s="19"/>
+      <c r="X136" s="19"/>
+      <c r="Y136" s="19"/>
       <c r="Z136" s="1"/>
       <c r="AA136" s="1"/>
       <c r="AB136" s="1"/>
@@ -30884,7 +30918,7 @@
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="73">
-        <f>INT($C$141)+2</f>
+        <f>INT($C$108)+2</f>
         <v>3</v>
       </c>
       <c r="D137" s="1"/>
@@ -30913,245 +30947,243 @@
       <c r="AA137" s="1"/>
       <c r="AB137" s="1"/>
     </row>
-    <row r="138" spans="1:28" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
-      <c r="B138" s="20"/>
-      <c r="C138" s="74">
-        <f>INT($C$141)+0.005</f>
-        <v>1.0049999999999999</v>
-      </c>
-      <c r="D138" s="20"/>
-      <c r="E138" s="20"/>
-      <c r="F138" s="20"/>
-      <c r="G138" s="20"/>
-      <c r="H138" s="20"/>
-      <c r="I138" s="20"/>
-      <c r="J138" s="20"/>
-      <c r="K138" s="20"/>
-      <c r="L138" s="20"/>
-      <c r="M138" s="20"/>
-      <c r="N138" s="20"/>
-      <c r="O138" s="20"/>
-      <c r="P138" s="20"/>
-      <c r="Q138" s="20"/>
-      <c r="R138" s="20"/>
-      <c r="S138" s="20"/>
-      <c r="T138" s="20"/>
-      <c r="U138" s="20"/>
-      <c r="V138" s="20"/>
-      <c r="W138" s="20"/>
-      <c r="X138" s="20"/>
-      <c r="Y138" s="20"/>
+      <c r="B138" s="1"/>
+      <c r="C138" s="73">
+        <f>INT($C$142)+2</f>
+        <v>3</v>
+      </c>
+      <c r="D138" s="1"/>
+      <c r="E138" s="1"/>
+      <c r="F138" s="1"/>
+      <c r="G138" s="1"/>
+      <c r="H138" s="1"/>
+      <c r="I138" s="1"/>
+      <c r="J138" s="1"/>
+      <c r="K138" s="1"/>
+      <c r="L138" s="1"/>
+      <c r="M138" s="1"/>
+      <c r="N138" s="1"/>
+      <c r="O138" s="1"/>
+      <c r="P138" s="1"/>
+      <c r="Q138" s="1"/>
+      <c r="R138" s="1"/>
+      <c r="S138" s="1"/>
+      <c r="T138" s="1"/>
+      <c r="U138" s="1"/>
+      <c r="V138" s="1"/>
+      <c r="W138" s="1"/>
+      <c r="X138" s="1"/>
+      <c r="Y138" s="1"/>
       <c r="Z138" s="1"/>
       <c r="AA138" s="1"/>
       <c r="AB138" s="1"/>
     </row>
-    <row r="139" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:28" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="1"/>
-      <c r="B139" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="C139" s="75">
-        <f>INT($C$141)+1.005</f>
-        <v>2.0049999999999999</v>
-      </c>
-      <c r="D139" s="14"/>
-      <c r="E139" s="14"/>
-      <c r="F139" s="14"/>
-      <c r="G139" s="14"/>
-      <c r="H139" s="14"/>
-      <c r="I139" s="14"/>
-      <c r="J139" s="14"/>
-      <c r="K139" s="14"/>
-      <c r="L139" s="14"/>
-      <c r="M139" s="14"/>
-      <c r="N139" s="14"/>
-      <c r="O139" s="14"/>
-      <c r="P139" s="14"/>
-      <c r="Q139" s="14"/>
-      <c r="R139" s="14"/>
-      <c r="S139" s="14"/>
-      <c r="T139" s="14"/>
-      <c r="U139" s="14"/>
-      <c r="V139" s="14"/>
-      <c r="W139" s="14"/>
-      <c r="X139" s="14"/>
-      <c r="Y139" s="15"/>
+      <c r="B139" s="20"/>
+      <c r="C139" s="74">
+        <f>INT($C$142)+0.005</f>
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="D139" s="20"/>
+      <c r="E139" s="20"/>
+      <c r="F139" s="20"/>
+      <c r="G139" s="20"/>
+      <c r="H139" s="20"/>
+      <c r="I139" s="20"/>
+      <c r="J139" s="20"/>
+      <c r="K139" s="20"/>
+      <c r="L139" s="20"/>
+      <c r="M139" s="20"/>
+      <c r="N139" s="20"/>
+      <c r="O139" s="20"/>
+      <c r="P139" s="20"/>
+      <c r="Q139" s="20"/>
+      <c r="R139" s="20"/>
+      <c r="S139" s="20"/>
+      <c r="T139" s="20"/>
+      <c r="U139" s="20"/>
+      <c r="V139" s="20"/>
+      <c r="W139" s="20"/>
+      <c r="X139" s="20"/>
+      <c r="Y139" s="20"/>
       <c r="Z139" s="1"/>
       <c r="AA139" s="1"/>
       <c r="AB139" s="1"/>
     </row>
-    <row r="140" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
-      <c r="B140" s="33"/>
-      <c r="C140" s="73">
-        <f>INT(MAX($C$149:$C$157))+1</f>
-        <v>5</v>
-      </c>
-      <c r="D140" s="3"/>
-      <c r="E140" s="3"/>
-      <c r="F140" s="3"/>
-      <c r="G140" s="3"/>
-      <c r="H140" s="27"/>
-      <c r="I140" s="27"/>
-      <c r="J140" s="27"/>
-      <c r="K140" s="27"/>
-      <c r="L140" s="27"/>
-      <c r="M140" s="27"/>
-      <c r="N140" s="27"/>
-      <c r="O140" s="27"/>
-      <c r="P140" s="27"/>
-      <c r="Q140" s="27"/>
-      <c r="R140" s="27"/>
-      <c r="S140" s="27"/>
-      <c r="T140" s="27"/>
-      <c r="U140" s="27"/>
-      <c r="V140" s="27"/>
-      <c r="W140" s="27"/>
-      <c r="X140" s="3"/>
-      <c r="Y140" s="16"/>
+      <c r="B140" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="C140" s="75">
+        <f>INT($C$142)+1.005</f>
+        <v>2.0049999999999999</v>
+      </c>
+      <c r="D140" s="14"/>
+      <c r="E140" s="14"/>
+      <c r="F140" s="14"/>
+      <c r="G140" s="14"/>
+      <c r="H140" s="14"/>
+      <c r="I140" s="14"/>
+      <c r="J140" s="14"/>
+      <c r="K140" s="14"/>
+      <c r="L140" s="14"/>
+      <c r="M140" s="14"/>
+      <c r="N140" s="14"/>
+      <c r="O140" s="14"/>
+      <c r="P140" s="14"/>
+      <c r="Q140" s="14"/>
+      <c r="R140" s="14"/>
+      <c r="S140" s="14"/>
+      <c r="T140" s="14"/>
+      <c r="U140" s="14"/>
+      <c r="V140" s="14"/>
+      <c r="W140" s="14"/>
+      <c r="X140" s="14"/>
+      <c r="Y140" s="15"/>
       <c r="Z140" s="1"/>
       <c r="AA140" s="1"/>
       <c r="AB140" s="1"/>
     </row>
-    <row r="141" spans="1:28" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
       <c r="B141" s="33"/>
       <c r="C141" s="73">
-        <v>1.02</v>
-      </c>
-      <c r="D141" s="21"/>
-      <c r="E141" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="F141" s="25"/>
-      <c r="G141" s="12"/>
-      <c r="H141" s="171" t="str">
-        <f>COUNTIFS($B$1:$B141, "«")&amp;" Feed Pool definitions"</f>
-        <v>5 Feed Pool definitions</v>
-      </c>
-      <c r="I141" s="6"/>
-      <c r="J141" s="6"/>
-      <c r="K141" s="6"/>
-      <c r="L141" s="6"/>
-      <c r="M141" s="6"/>
-      <c r="N141" s="6"/>
-      <c r="O141" s="6"/>
-      <c r="P141" s="6"/>
-      <c r="Q141" s="6"/>
-      <c r="R141" s="6"/>
-      <c r="S141" s="6"/>
-      <c r="T141" s="6"/>
-      <c r="U141" s="6"/>
-      <c r="V141" s="6"/>
-      <c r="W141" s="6"/>
-      <c r="X141" s="10"/>
+        <f>INT(MAX($C$150:$C$158))+1</f>
+        <v>5</v>
+      </c>
+      <c r="D141" s="3"/>
+      <c r="E141" s="3"/>
+      <c r="F141" s="3"/>
+      <c r="G141" s="3"/>
+      <c r="H141" s="27"/>
+      <c r="I141" s="27"/>
+      <c r="J141" s="27"/>
+      <c r="K141" s="27"/>
+      <c r="L141" s="27"/>
+      <c r="M141" s="27"/>
+      <c r="N141" s="27"/>
+      <c r="O141" s="27"/>
+      <c r="P141" s="27"/>
+      <c r="Q141" s="27"/>
+      <c r="R141" s="27"/>
+      <c r="S141" s="27"/>
+      <c r="T141" s="27"/>
+      <c r="U141" s="27"/>
+      <c r="V141" s="27"/>
+      <c r="W141" s="27"/>
+      <c r="X141" s="3"/>
       <c r="Y141" s="16"/>
       <c r="Z141" s="1"/>
       <c r="AA141" s="1"/>
       <c r="AB141" s="1"/>
     </row>
-    <row r="142" spans="1:28" ht="18.75" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:28" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
       <c r="B142" s="33"/>
       <c r="C142" s="73">
-        <f>INT($C$141)+1.02</f>
-        <v>2.02</v>
+        <v>1.02</v>
       </c>
       <c r="D142" s="21"/>
       <c r="E142" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="F142" s="28">
-        <v>1</v>
-      </c>
-      <c r="G142" s="13"/>
-      <c r="H142" s="8" t="s">
-        <v>297</v>
-      </c>
-      <c r="I142" s="7"/>
-      <c r="J142" s="7"/>
-      <c r="K142" s="7"/>
-      <c r="L142" s="7"/>
-      <c r="M142" s="7"/>
-      <c r="N142" s="7"/>
-      <c r="O142" s="7"/>
-      <c r="P142" s="7"/>
-      <c r="Q142" s="7"/>
-      <c r="R142" s="7"/>
-      <c r="S142" s="7"/>
-      <c r="T142" s="7"/>
-      <c r="U142" s="7"/>
-      <c r="V142" s="7"/>
-      <c r="W142" s="7"/>
-      <c r="X142" s="11"/>
+        <v>6</v>
+      </c>
+      <c r="F142" s="25"/>
+      <c r="G142" s="12"/>
+      <c r="H142" s="171" t="str">
+        <f>COUNTIFS($B$1:$B142, "«")&amp;" Feed Pool definitions"</f>
+        <v>5 Feed Pool definitions</v>
+      </c>
+      <c r="I142" s="6"/>
+      <c r="J142" s="6"/>
+      <c r="K142" s="6"/>
+      <c r="L142" s="6"/>
+      <c r="M142" s="6"/>
+      <c r="N142" s="6"/>
+      <c r="O142" s="6"/>
+      <c r="P142" s="6"/>
+      <c r="Q142" s="6"/>
+      <c r="R142" s="6"/>
+      <c r="S142" s="6"/>
+      <c r="T142" s="6"/>
+      <c r="U142" s="6"/>
+      <c r="V142" s="6"/>
+      <c r="W142" s="6"/>
+      <c r="X142" s="10"/>
       <c r="Y142" s="16"/>
       <c r="Z142" s="1"/>
       <c r="AA142" s="1"/>
       <c r="AB142" s="1"/>
     </row>
-    <row r="143" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:28" ht="18.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
       <c r="B143" s="33"/>
       <c r="C143" s="73">
-        <f>INT($C$141)+2.005</f>
-        <v>3.0049999999999999</v>
-      </c>
-      <c r="D143" s="3"/>
-      <c r="E143" s="3"/>
-      <c r="F143" s="3"/>
-      <c r="G143" s="3"/>
-      <c r="H143" s="3"/>
-      <c r="I143" s="3"/>
-      <c r="J143" s="3"/>
-      <c r="K143" s="3"/>
-      <c r="L143" s="3"/>
-      <c r="M143" s="3"/>
-      <c r="N143" s="3"/>
-      <c r="O143" s="3"/>
-      <c r="P143" s="3"/>
-      <c r="Q143" s="3"/>
-      <c r="R143" s="3"/>
-      <c r="S143" s="3"/>
-      <c r="T143" s="3"/>
-      <c r="U143" s="3"/>
-      <c r="V143" s="3"/>
-      <c r="W143" s="3"/>
-      <c r="X143" s="3"/>
+        <f>INT($C$142)+1.02</f>
+        <v>2.02</v>
+      </c>
+      <c r="D143" s="21"/>
+      <c r="E143" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F143" s="28">
+        <v>1</v>
+      </c>
+      <c r="G143" s="13"/>
+      <c r="H143" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="I143" s="7"/>
+      <c r="J143" s="7"/>
+      <c r="K143" s="7"/>
+      <c r="L143" s="7"/>
+      <c r="M143" s="7"/>
+      <c r="N143" s="7"/>
+      <c r="O143" s="7"/>
+      <c r="P143" s="7"/>
+      <c r="Q143" s="7"/>
+      <c r="R143" s="7"/>
+      <c r="S143" s="7"/>
+      <c r="T143" s="7"/>
+      <c r="U143" s="7"/>
+      <c r="V143" s="7"/>
+      <c r="W143" s="7"/>
+      <c r="X143" s="11"/>
       <c r="Y143" s="16"/>
       <c r="Z143" s="1"/>
       <c r="AA143" s="1"/>
       <c r="AB143" s="1"/>
     </row>
-    <row r="144" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
       <c r="B144" s="33"/>
       <c r="C144" s="73">
-        <f>INT($C$141)+2</f>
-        <v>3</v>
+        <f>INT($C$142)+2.005</f>
+        <v>3.0049999999999999</v>
       </c>
       <c r="D144" s="3"/>
-      <c r="E144" s="5"/>
-      <c r="F144" s="5"/>
+      <c r="E144" s="3"/>
+      <c r="F144" s="3"/>
       <c r="G144" s="3"/>
-      <c r="H144" s="29"/>
-      <c r="I144" s="29"/>
-      <c r="J144" s="65" t="s">
-        <v>295</v>
-      </c>
-      <c r="K144" s="65"/>
-      <c r="L144" s="65"/>
-      <c r="M144" s="65"/>
-      <c r="N144" s="65"/>
-      <c r="O144" s="65"/>
-      <c r="P144" s="65"/>
-      <c r="Q144" s="65"/>
-      <c r="R144" s="65"/>
-      <c r="S144" s="65"/>
-      <c r="T144" s="29"/>
-      <c r="U144" s="29"/>
-      <c r="V144" s="29"/>
-      <c r="W144" s="29"/>
+      <c r="H144" s="3"/>
+      <c r="I144" s="3"/>
+      <c r="J144" s="3"/>
+      <c r="K144" s="3"/>
+      <c r="L144" s="3"/>
+      <c r="M144" s="3"/>
+      <c r="N144" s="3"/>
+      <c r="O144" s="3"/>
+      <c r="P144" s="3"/>
+      <c r="Q144" s="3"/>
+      <c r="R144" s="3"/>
+      <c r="S144" s="3"/>
+      <c r="T144" s="3"/>
+      <c r="U144" s="3"/>
+      <c r="V144" s="3"/>
+      <c r="W144" s="3"/>
       <c r="X144" s="3"/>
       <c r="Y144" s="16"/>
       <c r="Z144" s="1"/>
@@ -31162,7 +31194,7 @@
       <c r="A145" s="1"/>
       <c r="B145" s="33"/>
       <c r="C145" s="73">
-        <f>INT($C$141)+2</f>
+        <f>INT($C$142)+2</f>
         <v>3</v>
       </c>
       <c r="D145" s="3"/>
@@ -31171,36 +31203,18 @@
       <c r="G145" s="3"/>
       <c r="H145" s="29"/>
       <c r="I145" s="29"/>
-      <c r="J145" s="29">
-        <v>0</v>
-      </c>
-      <c r="K145" s="29">
-        <v>1</v>
-      </c>
-      <c r="L145" s="29">
-        <v>2</v>
-      </c>
-      <c r="M145" s="29">
-        <v>3</v>
-      </c>
-      <c r="N145" s="29">
-        <v>4</v>
-      </c>
-      <c r="O145" s="29">
-        <v>5</v>
-      </c>
-      <c r="P145" s="29">
-        <v>6</v>
-      </c>
-      <c r="Q145" s="29">
-        <v>7</v>
-      </c>
-      <c r="R145" s="29">
-        <v>8</v>
-      </c>
-      <c r="S145" s="29">
-        <v>9</v>
-      </c>
+      <c r="J145" s="65" t="s">
+        <v>295</v>
+      </c>
+      <c r="K145" s="65"/>
+      <c r="L145" s="65"/>
+      <c r="M145" s="65"/>
+      <c r="N145" s="65"/>
+      <c r="O145" s="65"/>
+      <c r="P145" s="65"/>
+      <c r="Q145" s="65"/>
+      <c r="R145" s="65"/>
+      <c r="S145" s="65"/>
       <c r="T145" s="29"/>
       <c r="U145" s="29"/>
       <c r="V145" s="29"/>
@@ -31211,31 +31225,49 @@
       <c r="AA145" s="1"/>
       <c r="AB145" s="1"/>
     </row>
-    <row r="146" spans="1:28" ht="9.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
-      <c r="B146" s="33" t="s">
-        <v>20</v>
-      </c>
+      <c r="B146" s="33"/>
       <c r="C146" s="73">
-        <f>INT($C$141)+2.01</f>
-        <v>3.01</v>
+        <f>INT($C$142)+2</f>
+        <v>3</v>
       </c>
       <c r="D146" s="3"/>
-      <c r="E146" s="3"/>
-      <c r="F146" s="3"/>
+      <c r="E146" s="5"/>
+      <c r="F146" s="5"/>
       <c r="G146" s="3"/>
       <c r="H146" s="29"/>
       <c r="I146" s="29"/>
-      <c r="J146" s="29"/>
-      <c r="K146" s="29"/>
-      <c r="L146" s="29"/>
-      <c r="M146" s="29"/>
-      <c r="N146" s="29"/>
-      <c r="O146" s="29"/>
-      <c r="P146" s="29"/>
-      <c r="Q146" s="29"/>
-      <c r="R146" s="29"/>
-      <c r="S146" s="29"/>
+      <c r="J146" s="29">
+        <v>0</v>
+      </c>
+      <c r="K146" s="29">
+        <v>1</v>
+      </c>
+      <c r="L146" s="29">
+        <v>2</v>
+      </c>
+      <c r="M146" s="29">
+        <v>3</v>
+      </c>
+      <c r="N146" s="29">
+        <v>4</v>
+      </c>
+      <c r="O146" s="29">
+        <v>5</v>
+      </c>
+      <c r="P146" s="29">
+        <v>6</v>
+      </c>
+      <c r="Q146" s="29">
+        <v>7</v>
+      </c>
+      <c r="R146" s="29">
+        <v>8</v>
+      </c>
+      <c r="S146" s="29">
+        <v>9</v>
+      </c>
       <c r="T146" s="29"/>
       <c r="U146" s="29"/>
       <c r="V146" s="29"/>
@@ -31246,34 +31278,36 @@
       <c r="AA146" s="1"/>
       <c r="AB146" s="1"/>
     </row>
-    <row r="147" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:28" ht="9.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
-      <c r="B147" s="33"/>
+      <c r="B147" s="33" t="s">
+        <v>20</v>
+      </c>
       <c r="C147" s="73">
-        <f>C$140</f>
-        <v>5</v>
-      </c>
-      <c r="D147" s="4"/>
-      <c r="E147" s="5"/>
-      <c r="F147" s="5"/>
-      <c r="G147" s="4"/>
-      <c r="H147" s="5"/>
-      <c r="I147" s="5"/>
-      <c r="J147" s="5"/>
-      <c r="K147" s="5"/>
-      <c r="L147" s="5"/>
-      <c r="M147" s="5"/>
-      <c r="N147" s="5"/>
-      <c r="O147" s="5"/>
-      <c r="P147" s="5"/>
-      <c r="Q147" s="5"/>
-      <c r="R147" s="5"/>
-      <c r="S147" s="5"/>
-      <c r="T147" s="5"/>
-      <c r="U147" s="5"/>
-      <c r="V147" s="5"/>
-      <c r="W147" s="5"/>
-      <c r="X147" s="4"/>
+        <f>INT($C$142)+2.01</f>
+        <v>3.01</v>
+      </c>
+      <c r="D147" s="3"/>
+      <c r="E147" s="3"/>
+      <c r="F147" s="3"/>
+      <c r="G147" s="3"/>
+      <c r="H147" s="29"/>
+      <c r="I147" s="29"/>
+      <c r="J147" s="29"/>
+      <c r="K147" s="29"/>
+      <c r="L147" s="29"/>
+      <c r="M147" s="29"/>
+      <c r="N147" s="29"/>
+      <c r="O147" s="29"/>
+      <c r="P147" s="29"/>
+      <c r="Q147" s="29"/>
+      <c r="R147" s="29"/>
+      <c r="S147" s="29"/>
+      <c r="T147" s="29"/>
+      <c r="U147" s="29"/>
+      <c r="V147" s="29"/>
+      <c r="W147" s="29"/>
+      <c r="X147" s="3"/>
       <c r="Y147" s="16"/>
       <c r="Z147" s="1"/>
       <c r="AA147" s="1"/>
@@ -31281,16 +31315,12 @@
     </row>
     <row r="148" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
-      <c r="B148" s="33" t="s">
-        <v>19</v>
-      </c>
+      <c r="B148" s="33"/>
       <c r="C148" s="73">
-        <f>C$140</f>
+        <f>C$141</f>
         <v>5</v>
       </c>
-      <c r="D148" s="4" t="s">
-        <v>44</v>
-      </c>
+      <c r="D148" s="4"/>
       <c r="E148" s="5"/>
       <c r="F148" s="5"/>
       <c r="G148" s="4"/>
@@ -31316,94 +31346,98 @@
       <c r="AA148" s="1"/>
       <c r="AB148" s="1"/>
     </row>
-    <row r="149" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:28" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
-      <c r="B149" s="33"/>
+      <c r="B149" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="C149" s="73">
-        <f>INT($C$141)+2.005</f>
-        <v>3.0049999999999999</v>
+        <f>C$141</f>
+        <v>5</v>
       </c>
       <c r="D149" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E149" s="4"/>
-      <c r="F149" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="E149" s="5"/>
+      <c r="F149" s="5"/>
       <c r="G149" s="4"/>
-      <c r="H149" s="58"/>
-      <c r="I149" s="58"/>
-      <c r="J149" s="58"/>
-      <c r="K149" s="58"/>
-      <c r="L149" s="58"/>
-      <c r="M149" s="58"/>
-      <c r="N149" s="58"/>
-      <c r="O149" s="58"/>
-      <c r="P149" s="58"/>
-      <c r="Q149" s="58"/>
-      <c r="R149" s="58"/>
-      <c r="S149" s="58"/>
-      <c r="T149" s="58"/>
-      <c r="U149" s="58"/>
-      <c r="V149" s="58"/>
-      <c r="W149" s="58"/>
+      <c r="H149" s="5"/>
+      <c r="I149" s="5"/>
+      <c r="J149" s="5"/>
+      <c r="K149" s="5"/>
+      <c r="L149" s="5"/>
+      <c r="M149" s="5"/>
+      <c r="N149" s="5"/>
+      <c r="O149" s="5"/>
+      <c r="P149" s="5"/>
+      <c r="Q149" s="5"/>
+      <c r="R149" s="5"/>
+      <c r="S149" s="5"/>
+      <c r="T149" s="5"/>
+      <c r="U149" s="5"/>
+      <c r="V149" s="5"/>
+      <c r="W149" s="5"/>
       <c r="X149" s="4"/>
       <c r="Y149" s="16"/>
       <c r="Z149" s="1"/>
       <c r="AA149" s="1"/>
       <c r="AB149" s="1"/>
     </row>
-    <row r="150" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
       <c r="B150" s="33"/>
       <c r="C150" s="73">
-        <f>INT($C$141)+2</f>
-        <v>3</v>
-      </c>
-      <c r="D150" s="4"/>
-      <c r="E150" s="5"/>
-      <c r="F150" s="5"/>
+        <f>INT($C$142)+2.005</f>
+        <v>3.0049999999999999</v>
+      </c>
+      <c r="D150" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E150" s="4"/>
+      <c r="F150" s="4"/>
       <c r="G150" s="4"/>
-      <c r="H150" s="64" t="s">
-        <v>289</v>
-      </c>
-      <c r="I150" s="31">
-        <v>4</v>
-      </c>
-      <c r="J150" s="183" t="s">
-        <v>293</v>
-      </c>
-      <c r="K150" s="2"/>
-      <c r="L150" s="2"/>
-      <c r="M150" s="2"/>
-      <c r="N150" s="2"/>
-      <c r="O150" s="2"/>
-      <c r="P150" s="2"/>
-      <c r="Q150" s="2"/>
-      <c r="R150" s="2"/>
-      <c r="S150" s="2"/>
-      <c r="T150" s="2"/>
-      <c r="U150" s="2"/>
-      <c r="V150" s="2"/>
-      <c r="W150" s="2"/>
+      <c r="H150" s="58"/>
+      <c r="I150" s="58"/>
+      <c r="J150" s="58"/>
+      <c r="K150" s="58"/>
+      <c r="L150" s="58"/>
+      <c r="M150" s="58"/>
+      <c r="N150" s="58"/>
+      <c r="O150" s="58"/>
+      <c r="P150" s="58"/>
+      <c r="Q150" s="58"/>
+      <c r="R150" s="58"/>
+      <c r="S150" s="58"/>
+      <c r="T150" s="58"/>
+      <c r="U150" s="58"/>
+      <c r="V150" s="58"/>
+      <c r="W150" s="58"/>
       <c r="X150" s="4"/>
       <c r="Y150" s="16"/>
       <c r="Z150" s="1"/>
       <c r="AA150" s="1"/>
       <c r="AB150" s="1"/>
     </row>
-    <row r="151" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
       <c r="B151" s="33"/>
       <c r="C151" s="73">
-        <f>INT($C$141)+3</f>
-        <v>4</v>
+        <f>INT($C$142)+2</f>
+        <v>3</v>
       </c>
       <c r="D151" s="4"/>
       <c r="E151" s="5"/>
       <c r="F151" s="5"/>
       <c r="G151" s="4"/>
-      <c r="H151" s="181"/>
-      <c r="I151" s="2"/>
-      <c r="J151" s="2"/>
+      <c r="H151" s="64" t="s">
+        <v>289</v>
+      </c>
+      <c r="I151" s="31">
+        <v>4</v>
+      </c>
+      <c r="J151" s="183" t="s">
+        <v>293</v>
+      </c>
       <c r="K151" s="2"/>
       <c r="L151" s="2"/>
       <c r="M151" s="2"/>
@@ -31423,20 +31457,18 @@
       <c r="AA151" s="1"/>
       <c r="AB151" s="1"/>
     </row>
-    <row r="152" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
       <c r="B152" s="33"/>
       <c r="C152" s="73">
-        <f>INT($C$141)+2</f>
-        <v>3</v>
+        <f>INT($C$142)+3</f>
+        <v>4</v>
       </c>
       <c r="D152" s="4"/>
       <c r="E152" s="5"/>
       <c r="F152" s="5"/>
       <c r="G152" s="4"/>
-      <c r="H152" s="64" t="s">
-        <v>294</v>
-      </c>
+      <c r="H152" s="181"/>
       <c r="I152" s="2"/>
       <c r="J152" s="2"/>
       <c r="K152" s="2"/>
@@ -31458,51 +31490,31 @@
       <c r="AA152" s="1"/>
       <c r="AB152" s="1"/>
     </row>
-    <row r="153" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A153" s="1"/>
       <c r="B153" s="33"/>
       <c r="C153" s="73">
-        <f>INT($C$141)+3</f>
-        <v>4</v>
+        <f>INT($C$142)+2</f>
+        <v>3</v>
       </c>
       <c r="D153" s="4"/>
       <c r="E153" s="5"/>
       <c r="F153" s="5"/>
       <c r="G153" s="4"/>
-      <c r="H153" s="184" t="s">
-        <v>301</v>
+      <c r="H153" s="64" t="s">
+        <v>294</v>
       </c>
       <c r="I153" s="2"/>
-      <c r="J153" s="31">
-        <v>3</v>
-      </c>
-      <c r="K153" s="31">
-        <v>4</v>
-      </c>
-      <c r="L153" s="31">
-        <v>6</v>
-      </c>
-      <c r="M153" s="31">
-        <v>8</v>
-      </c>
-      <c r="N153" s="31">
-        <v>9</v>
-      </c>
-      <c r="O153" s="31">
-        <v>6</v>
-      </c>
-      <c r="P153" s="31">
-        <v>5</v>
-      </c>
-      <c r="Q153" s="31">
-        <v>4</v>
-      </c>
-      <c r="R153" s="31">
-        <v>3.5</v>
-      </c>
-      <c r="S153" s="31">
-        <v>3</v>
-      </c>
+      <c r="J153" s="2"/>
+      <c r="K153" s="2"/>
+      <c r="L153" s="2"/>
+      <c r="M153" s="2"/>
+      <c r="N153" s="2"/>
+      <c r="O153" s="2"/>
+      <c r="P153" s="2"/>
+      <c r="Q153" s="2"/>
+      <c r="R153" s="2"/>
+      <c r="S153" s="2"/>
       <c r="T153" s="2"/>
       <c r="U153" s="2"/>
       <c r="V153" s="2"/>
@@ -31513,11 +31525,11 @@
       <c r="AA153" s="1"/>
       <c r="AB153" s="1"/>
     </row>
-    <row r="154" spans="1:28" outlineLevel="3" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A154" s="1"/>
       <c r="B154" s="33"/>
       <c r="C154" s="73">
-        <f>INT($C$141)+3</f>
+        <f>INT($C$142)+3</f>
         <v>4</v>
       </c>
       <c r="D154" s="4"/>
@@ -31525,38 +31537,38 @@
       <c r="F154" s="5"/>
       <c r="G154" s="4"/>
       <c r="H154" s="184" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="I154" s="2"/>
       <c r="J154" s="31">
-        <v>13.3</v>
+        <v>3</v>
       </c>
       <c r="K154" s="31">
-        <v>13.3</v>
+        <v>4</v>
       </c>
       <c r="L154" s="31">
-        <v>13.3</v>
+        <v>6</v>
       </c>
       <c r="M154" s="31">
-        <v>13.3</v>
+        <v>8</v>
       </c>
       <c r="N154" s="31">
-        <v>13.3</v>
+        <v>9</v>
       </c>
       <c r="O154" s="31">
-        <v>13.3</v>
+        <v>6</v>
       </c>
       <c r="P154" s="31">
-        <v>13.3</v>
+        <v>5</v>
       </c>
       <c r="Q154" s="31">
-        <v>13.3</v>
+        <v>4</v>
       </c>
       <c r="R154" s="31">
-        <v>13.3</v>
+        <v>3.5</v>
       </c>
       <c r="S154" s="31">
-        <v>13.3</v>
+        <v>3</v>
       </c>
       <c r="T154" s="2"/>
       <c r="U154" s="2"/>
@@ -31568,29 +31580,51 @@
       <c r="AA154" s="1"/>
       <c r="AB154" s="1"/>
     </row>
-    <row r="155" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:28" outlineLevel="3" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
       <c r="B155" s="33"/>
       <c r="C155" s="73">
-        <f>INT(C$141+3)</f>
+        <f>INT($C$142)+3</f>
         <v>4</v>
       </c>
       <c r="D155" s="4"/>
       <c r="E155" s="5"/>
       <c r="F155" s="5"/>
       <c r="G155" s="4"/>
-      <c r="H155" s="172"/>
-      <c r="I155" s="172"/>
-      <c r="J155" s="172"/>
-      <c r="K155" s="172"/>
-      <c r="L155" s="172"/>
-      <c r="M155" s="172"/>
-      <c r="N155" s="172"/>
-      <c r="O155" s="172"/>
-      <c r="P155" s="172"/>
-      <c r="Q155" s="172"/>
-      <c r="R155" s="172"/>
-      <c r="S155" s="172"/>
+      <c r="H155" s="184" t="s">
+        <v>296</v>
+      </c>
+      <c r="I155" s="2"/>
+      <c r="J155" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="K155" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="L155" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="M155" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="N155" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="O155" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="P155" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="Q155" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="R155" s="31">
+        <v>13.3</v>
+      </c>
+      <c r="S155" s="31">
+        <v>13.3</v>
+      </c>
       <c r="T155" s="2"/>
       <c r="U155" s="2"/>
       <c r="V155" s="2"/>
@@ -31605,7 +31639,7 @@
       <c r="A156" s="1"/>
       <c r="B156" s="33"/>
       <c r="C156" s="73">
-        <f>INT(C$141+3)</f>
+        <f>INT(C$142+3)</f>
         <v>4</v>
       </c>
       <c r="D156" s="4"/>
@@ -31623,7 +31657,7 @@
       <c r="P156" s="172"/>
       <c r="Q156" s="172"/>
       <c r="R156" s="172"/>
-      <c r="S156" s="2"/>
+      <c r="S156" s="172"/>
       <c r="T156" s="2"/>
       <c r="U156" s="2"/>
       <c r="V156" s="2"/>
@@ -31634,47 +31668,45 @@
       <c r="AA156" s="1"/>
       <c r="AB156" s="1"/>
     </row>
-    <row r="157" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:28" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
       <c r="B157" s="33"/>
       <c r="C157" s="73">
-        <f>INT($C$141)+3.005</f>
-        <v>4.0049999999999999</v>
+        <f>INT(C$142+3)</f>
+        <v>4</v>
       </c>
       <c r="D157" s="4"/>
-      <c r="E157" s="4"/>
-      <c r="F157" s="4"/>
+      <c r="E157" s="5"/>
+      <c r="F157" s="5"/>
       <c r="G157" s="4"/>
-      <c r="H157" s="4"/>
-      <c r="I157" s="4"/>
-      <c r="J157" s="4"/>
-      <c r="K157" s="4"/>
-      <c r="L157" s="4"/>
-      <c r="M157" s="4"/>
-      <c r="N157" s="4"/>
-      <c r="O157" s="4"/>
-      <c r="P157" s="4"/>
-      <c r="Q157" s="4"/>
-      <c r="R157" s="4"/>
-      <c r="S157" s="4"/>
-      <c r="T157" s="4"/>
-      <c r="U157" s="4"/>
-      <c r="V157" s="4"/>
-      <c r="W157" s="4"/>
-      <c r="X157" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="H157" s="172"/>
+      <c r="I157" s="172"/>
+      <c r="J157" s="172"/>
+      <c r="K157" s="172"/>
+      <c r="L157" s="172"/>
+      <c r="M157" s="172"/>
+      <c r="N157" s="172"/>
+      <c r="O157" s="172"/>
+      <c r="P157" s="172"/>
+      <c r="Q157" s="172"/>
+      <c r="R157" s="172"/>
+      <c r="S157" s="2"/>
+      <c r="T157" s="2"/>
+      <c r="U157" s="2"/>
+      <c r="V157" s="2"/>
+      <c r="W157" s="2"/>
+      <c r="X157" s="4"/>
       <c r="Y157" s="16"/>
       <c r="Z157" s="1"/>
       <c r="AA157" s="1"/>
       <c r="AB157" s="1"/>
     </row>
-    <row r="158" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
       <c r="B158" s="33"/>
       <c r="C158" s="73">
-        <f>INT($C$141)+2.005</f>
-        <v>3.0049999999999999</v>
+        <f>INT($C$142)+3.005</f>
+        <v>4.0049999999999999</v>
       </c>
       <c r="D158" s="4"/>
       <c r="E158" s="4"/>
@@ -31696,117 +31728,122 @@
       <c r="U158" s="4"/>
       <c r="V158" s="4"/>
       <c r="W158" s="4"/>
-      <c r="X158" s="4"/>
+      <c r="X158" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="Y158" s="16"/>
       <c r="Z158" s="1"/>
       <c r="AA158" s="1"/>
       <c r="AB158" s="1"/>
     </row>
-    <row r="159" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A159" s="1"/>
-      <c r="B159" s="35"/>
-      <c r="C159" s="76">
-        <f>INT($C$141)+1.005</f>
-        <v>2.0049999999999999</v>
-      </c>
-      <c r="D159" s="17"/>
-      <c r="E159" s="17"/>
-      <c r="F159" s="17"/>
-      <c r="G159" s="17"/>
-      <c r="H159" s="17"/>
-      <c r="I159" s="17"/>
-      <c r="J159" s="17"/>
-      <c r="K159" s="17"/>
-      <c r="L159" s="17"/>
-      <c r="M159" s="17"/>
-      <c r="N159" s="17"/>
-      <c r="O159" s="17"/>
-      <c r="P159" s="17"/>
-      <c r="Q159" s="17"/>
-      <c r="R159" s="17"/>
-      <c r="S159" s="17"/>
-      <c r="T159" s="17"/>
-      <c r="U159" s="17"/>
-      <c r="V159" s="17"/>
-      <c r="W159" s="17"/>
-      <c r="X159" s="17"/>
-      <c r="Y159" s="18" t="s">
-        <v>1</v>
-      </c>
+      <c r="B159" s="33"/>
+      <c r="C159" s="73">
+        <f>INT($C$142)+2.005</f>
+        <v>3.0049999999999999</v>
+      </c>
+      <c r="D159" s="4"/>
+      <c r="E159" s="4"/>
+      <c r="F159" s="4"/>
+      <c r="G159" s="4"/>
+      <c r="H159" s="4"/>
+      <c r="I159" s="4"/>
+      <c r="J159" s="4"/>
+      <c r="K159" s="4"/>
+      <c r="L159" s="4"/>
+      <c r="M159" s="4"/>
+      <c r="N159" s="4"/>
+      <c r="O159" s="4"/>
+      <c r="P159" s="4"/>
+      <c r="Q159" s="4"/>
+      <c r="R159" s="4"/>
+      <c r="S159" s="4"/>
+      <c r="T159" s="4"/>
+      <c r="U159" s="4"/>
+      <c r="V159" s="4"/>
+      <c r="W159" s="4"/>
+      <c r="X159" s="4"/>
+      <c r="Y159" s="16"/>
       <c r="Z159" s="1"/>
       <c r="AA159" s="1"/>
       <c r="AB159" s="1"/>
     </row>
-    <row r="160" spans="1:28" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:28" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
-      <c r="B160" s="19"/>
-      <c r="C160" s="77">
-        <f>INT($C$141)+0.005</f>
-        <v>1.0049999999999999</v>
-      </c>
-      <c r="D160" s="19"/>
-      <c r="E160" s="19"/>
-      <c r="F160" s="19"/>
-      <c r="G160" s="19"/>
-      <c r="H160" s="19"/>
-      <c r="I160" s="19"/>
-      <c r="J160" s="19"/>
-      <c r="K160" s="19"/>
-      <c r="L160" s="19"/>
-      <c r="M160" s="19"/>
-      <c r="N160" s="19"/>
-      <c r="O160" s="19"/>
-      <c r="P160" s="19"/>
-      <c r="Q160" s="19"/>
-      <c r="R160" s="19"/>
-      <c r="S160" s="19"/>
-      <c r="T160" s="19"/>
-      <c r="U160" s="19"/>
-      <c r="V160" s="19"/>
-      <c r="W160" s="19"/>
-      <c r="X160" s="19"/>
-      <c r="Y160" s="19"/>
+      <c r="B160" s="35"/>
+      <c r="C160" s="76">
+        <f>INT($C$142)+1.005</f>
+        <v>2.0049999999999999</v>
+      </c>
+      <c r="D160" s="17"/>
+      <c r="E160" s="17"/>
+      <c r="F160" s="17"/>
+      <c r="G160" s="17"/>
+      <c r="H160" s="17"/>
+      <c r="I160" s="17"/>
+      <c r="J160" s="17"/>
+      <c r="K160" s="17"/>
+      <c r="L160" s="17"/>
+      <c r="M160" s="17"/>
+      <c r="N160" s="17"/>
+      <c r="O160" s="17"/>
+      <c r="P160" s="17"/>
+      <c r="Q160" s="17"/>
+      <c r="R160" s="17"/>
+      <c r="S160" s="17"/>
+      <c r="T160" s="17"/>
+      <c r="U160" s="17"/>
+      <c r="V160" s="17"/>
+      <c r="W160" s="17"/>
+      <c r="X160" s="17"/>
+      <c r="Y160" s="18" t="s">
+        <v>1</v>
+      </c>
       <c r="Z160" s="1"/>
       <c r="AA160" s="1"/>
       <c r="AB160" s="1"/>
     </row>
-    <row r="161" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:28" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="1"/>
-      <c r="B161" s="1"/>
-      <c r="C161" s="73">
-        <f>INT($C$141)+2</f>
-        <v>3</v>
-      </c>
-      <c r="D161" s="1"/>
-      <c r="E161" s="1"/>
-      <c r="F161" s="1"/>
-      <c r="G161" s="1"/>
-      <c r="H161" s="1"/>
-      <c r="I161" s="1"/>
-      <c r="J161" s="1"/>
-      <c r="K161" s="1"/>
-      <c r="L161" s="1"/>
-      <c r="M161" s="1"/>
-      <c r="N161" s="1"/>
-      <c r="O161" s="1"/>
-      <c r="P161" s="1"/>
-      <c r="Q161" s="1"/>
-      <c r="R161" s="1"/>
-      <c r="S161" s="1"/>
-      <c r="T161" s="1"/>
-      <c r="U161" s="1"/>
-      <c r="V161" s="1"/>
-      <c r="W161" s="1"/>
-      <c r="X161" s="1"/>
-      <c r="Y161" s="1"/>
+      <c r="B161" s="19"/>
+      <c r="C161" s="77">
+        <f>INT($C$142)+0.005</f>
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="D161" s="19"/>
+      <c r="E161" s="19"/>
+      <c r="F161" s="19"/>
+      <c r="G161" s="19"/>
+      <c r="H161" s="19"/>
+      <c r="I161" s="19"/>
+      <c r="J161" s="19"/>
+      <c r="K161" s="19"/>
+      <c r="L161" s="19"/>
+      <c r="M161" s="19"/>
+      <c r="N161" s="19"/>
+      <c r="O161" s="19"/>
+      <c r="P161" s="19"/>
+      <c r="Q161" s="19"/>
+      <c r="R161" s="19"/>
+      <c r="S161" s="19"/>
+      <c r="T161" s="19"/>
+      <c r="U161" s="19"/>
+      <c r="V161" s="19"/>
+      <c r="W161" s="19"/>
+      <c r="X161" s="19"/>
+      <c r="Y161" s="19"/>
       <c r="Z161" s="1"/>
       <c r="AA161" s="1"/>
       <c r="AB161" s="1"/>
     </row>
-    <row r="162" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:28" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
-      <c r="C162" s="66"/>
+      <c r="C162" s="73">
+        <f>INT($C$142)+2</f>
+        <v>3</v>
+      </c>
       <c r="D162" s="1"/>
       <c r="E162" s="1"/>
       <c r="F162" s="1"/>
@@ -31984,7 +32021,37 @@
       <c r="AB167" s="1"/>
     </row>
     <row r="168" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C168" s="72" t="s">
+      <c r="A168" s="1"/>
+      <c r="B168" s="1"/>
+      <c r="C168" s="66"/>
+      <c r="D168" s="1"/>
+      <c r="E168" s="1"/>
+      <c r="F168" s="1"/>
+      <c r="G168" s="1"/>
+      <c r="H168" s="1"/>
+      <c r="I168" s="1"/>
+      <c r="J168" s="1"/>
+      <c r="K168" s="1"/>
+      <c r="L168" s="1"/>
+      <c r="M168" s="1"/>
+      <c r="N168" s="1"/>
+      <c r="O168" s="1"/>
+      <c r="P168" s="1"/>
+      <c r="Q168" s="1"/>
+      <c r="R168" s="1"/>
+      <c r="S168" s="1"/>
+      <c r="T168" s="1"/>
+      <c r="U168" s="1"/>
+      <c r="V168" s="1"/>
+      <c r="W168" s="1"/>
+      <c r="X168" s="1"/>
+      <c r="Y168" s="1"/>
+      <c r="Z168" s="1"/>
+      <c r="AA168" s="1"/>
+      <c r="AB168" s="1"/>
+    </row>
+    <row r="169" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="C169" s="72" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Set r2adjust default to FALSE. Set it to TRUE in QuickTest no profit effect
</commit_message>
<xml_diff>
--- a/Structural.xlsx
+++ b/Structural.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4C9DBC-DBFC-4D43-B373-81760A225E28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1EDB48B-187C-4138-B206-542210F7FBB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1095" yWindow="570" windowWidth="27705" windowHeight="15630" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="210" yWindow="495" windowWidth="27705" windowHeight="15630" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -2800,10 +2800,6 @@
     <t>Lowest value</t>
   </si>
   <si>
-    <t>20May21: Make the extra nut_spread_g1 = 0.1
-1Apr19: Blank worksheet</t>
-  </si>
-  <si>
     <t>is FVP</t>
   </si>
   <si>
@@ -3006,6 +3002,11 @@
 25Apr21: Moved inputs from Property.xlsx
                    Moved FVP &amp; N inputs from Stock
 1: 1Apr19-Created the version control table</t>
+  </si>
+  <si>
+    <t>18Mar22: Change the default r2_inc to False now that a pickled feed supply is working.
+20May21: Make the extra nut_spread_g1 = 0.1
+1Apr19: Blank worksheet</t>
   </si>
 </sst>
 </file>
@@ -5404,7 +5405,7 @@
   <dimension ref="A1:AT127"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <pane xSplit="9" ySplit="10" topLeftCell="J94" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="10" topLeftCell="J91" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
@@ -7111,7 +7112,7 @@
       <c r="F47" s="5"/>
       <c r="G47" s="4"/>
       <c r="H47" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="I47" s="101" t="b">
         <v>1</v>
@@ -7448,13 +7449,13 @@
       <c r="F56" s="5"/>
       <c r="G56" s="4"/>
       <c r="H56" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="I56" s="101" t="s">
         <v>305</v>
       </c>
-      <c r="I56" s="101" t="s">
+      <c r="J56" s="101" t="s">
         <v>306</v>
-      </c>
-      <c r="J56" s="101" t="s">
-        <v>307</v>
       </c>
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
@@ -8188,11 +8189,11 @@
       <c r="F77" s="5"/>
       <c r="G77" s="4"/>
       <c r="H77" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I77" s="2"/>
       <c r="J77" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
@@ -8259,15 +8260,15 @@
       <c r="G79" s="4"/>
       <c r="H79" s="2"/>
       <c r="I79" s="186" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="J79" s="2"/>
       <c r="K79" s="186" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L79" s="2"/>
       <c r="M79" s="186" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="N79" s="2"/>
       <c r="O79" s="2"/>
@@ -8298,15 +8299,15 @@
       <c r="G80" s="4"/>
       <c r="H80" s="172"/>
       <c r="I80" s="187" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="J80" s="190"/>
       <c r="K80" s="187" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="L80" s="190"/>
       <c r="M80" s="187" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="N80" s="55"/>
       <c r="O80" s="2"/>
@@ -8334,15 +8335,15 @@
       <c r="G81" s="4"/>
       <c r="H81" s="172"/>
       <c r="I81" s="188" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J81" s="190"/>
       <c r="K81" s="188" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="L81" s="190"/>
       <c r="M81" s="188" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="N81" s="55"/>
       <c r="O81" s="2"/>
@@ -8370,15 +8371,15 @@
       <c r="G82" s="4"/>
       <c r="H82" s="172"/>
       <c r="I82" s="188" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="J82" s="190"/>
       <c r="K82" s="188" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="L82" s="190"/>
       <c r="M82" s="188" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="N82" s="55"/>
       <c r="O82" s="2"/>
@@ -8406,15 +8407,15 @@
       <c r="G83" s="4"/>
       <c r="H83" s="172"/>
       <c r="I83" s="188" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="J83" s="190"/>
       <c r="K83" s="188" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="L83" s="190"/>
       <c r="M83" s="188" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="N83" s="55"/>
       <c r="O83" s="2"/>
@@ -8442,15 +8443,15 @@
       <c r="G84" s="4"/>
       <c r="H84" s="172"/>
       <c r="I84" s="188" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="J84" s="190"/>
       <c r="K84" s="188" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="L84" s="190"/>
       <c r="M84" s="188" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="N84" s="55"/>
       <c r="O84" s="2"/>
@@ -8478,15 +8479,15 @@
       <c r="G85" s="4"/>
       <c r="H85" s="172"/>
       <c r="I85" s="188" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="J85" s="190"/>
       <c r="K85" s="188" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="L85" s="190"/>
       <c r="M85" s="188" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N85" s="55"/>
       <c r="O85" s="2"/>
@@ -8514,15 +8515,15 @@
       <c r="G86" s="4"/>
       <c r="H86" s="172"/>
       <c r="I86" s="188" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="J86" s="190"/>
       <c r="K86" s="188" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="L86" s="190"/>
       <c r="M86" s="188" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="N86" s="55"/>
       <c r="O86" s="2"/>
@@ -8550,15 +8551,15 @@
       <c r="G87" s="4"/>
       <c r="H87" s="172"/>
       <c r="I87" s="188" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="J87" s="190"/>
       <c r="K87" s="188" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L87" s="190"/>
       <c r="M87" s="188" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="N87" s="55"/>
       <c r="O87" s="2"/>
@@ -8586,15 +8587,15 @@
       <c r="G88" s="4"/>
       <c r="H88" s="172"/>
       <c r="I88" s="188" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="J88" s="190"/>
       <c r="K88" s="188" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="L88" s="190"/>
       <c r="M88" s="188" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="N88" s="55"/>
       <c r="O88" s="2"/>
@@ -8622,15 +8623,15 @@
       <c r="G89" s="4"/>
       <c r="H89" s="172"/>
       <c r="I89" s="188" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="J89" s="190"/>
       <c r="K89" s="188" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="L89" s="190"/>
       <c r="M89" s="188" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="N89" s="55"/>
       <c r="O89" s="2"/>
@@ -8658,15 +8659,15 @@
       <c r="G90" s="4"/>
       <c r="H90" s="172"/>
       <c r="I90" s="188" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="J90" s="190"/>
       <c r="K90" s="188" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="L90" s="190"/>
       <c r="M90" s="188" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="N90" s="55"/>
       <c r="O90" s="2"/>
@@ -8694,15 +8695,15 @@
       <c r="G91" s="4"/>
       <c r="H91" s="172"/>
       <c r="I91" s="188" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="J91" s="190"/>
       <c r="K91" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="L91" s="190"/>
       <c r="M91" s="188" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="N91" s="55"/>
       <c r="O91" s="2"/>
@@ -8730,15 +8731,15 @@
       <c r="G92" s="4"/>
       <c r="H92" s="172"/>
       <c r="I92" s="188" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="J92" s="190"/>
       <c r="K92" s="188" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L92" s="190"/>
       <c r="M92" s="188" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="N92" s="55"/>
       <c r="O92" s="2"/>
@@ -8766,15 +8767,15 @@
       <c r="G93" s="4"/>
       <c r="H93" s="172"/>
       <c r="I93" s="188" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="J93" s="190"/>
       <c r="K93" s="188" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="L93" s="190"/>
       <c r="M93" s="188" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="N93" s="55"/>
       <c r="O93" s="2"/>
@@ -8802,15 +8803,15 @@
       <c r="G94" s="4"/>
       <c r="H94" s="172"/>
       <c r="I94" s="188" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="J94" s="190"/>
       <c r="K94" s="188" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="L94" s="190"/>
       <c r="M94" s="188" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="N94" s="55"/>
       <c r="O94" s="2"/>
@@ -8838,15 +8839,15 @@
       <c r="G95" s="4"/>
       <c r="H95" s="172"/>
       <c r="I95" s="188" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J95" s="190"/>
       <c r="K95" s="188" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="L95" s="190"/>
       <c r="M95" s="188" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N95" s="55"/>
       <c r="O95" s="2"/>
@@ -8874,15 +8875,15 @@
       <c r="G96" s="4"/>
       <c r="H96" s="172"/>
       <c r="I96" s="189" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="J96" s="190"/>
       <c r="K96" s="189" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="L96" s="190"/>
       <c r="M96" s="188" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="N96" s="55"/>
       <c r="O96" s="2"/>
@@ -8914,7 +8915,7 @@
       <c r="K97" s="53"/>
       <c r="L97" s="172"/>
       <c r="M97" s="188" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="N97" s="55"/>
       <c r="O97" s="2"/>
@@ -8946,7 +8947,7 @@
       <c r="K98" s="2"/>
       <c r="L98" s="172"/>
       <c r="M98" s="188" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="N98" s="55"/>
       <c r="O98" s="2"/>
@@ -8978,7 +8979,7 @@
       <c r="K99" s="2"/>
       <c r="L99" s="172"/>
       <c r="M99" s="188" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="N99" s="55"/>
       <c r="O99" s="2"/>
@@ -9010,7 +9011,7 @@
       <c r="K100" s="2"/>
       <c r="L100" s="172"/>
       <c r="M100" s="188" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="N100" s="55"/>
       <c r="O100" s="2"/>
@@ -9042,7 +9043,7 @@
       <c r="K101" s="2"/>
       <c r="L101" s="172"/>
       <c r="M101" s="188" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="N101" s="55"/>
       <c r="O101" s="2"/>
@@ -9074,7 +9075,7 @@
       <c r="K102" s="2"/>
       <c r="L102" s="172"/>
       <c r="M102" s="188" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="N102" s="55"/>
       <c r="O102" s="2"/>
@@ -9106,7 +9107,7 @@
       <c r="K103" s="2"/>
       <c r="L103" s="172"/>
       <c r="M103" s="188" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="N103" s="55"/>
       <c r="O103" s="2"/>
@@ -9138,7 +9139,7 @@
       <c r="K104" s="2"/>
       <c r="L104" s="172"/>
       <c r="M104" s="188" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="N104" s="55"/>
       <c r="O104" s="2"/>
@@ -9170,7 +9171,7 @@
       <c r="K105" s="2"/>
       <c r="L105" s="172"/>
       <c r="M105" s="188" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="N105" s="55"/>
       <c r="O105" s="2"/>
@@ -9202,7 +9203,7 @@
       <c r="K106" s="2"/>
       <c r="L106" s="172"/>
       <c r="M106" s="188" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="N106" s="55"/>
       <c r="O106" s="2"/>
@@ -9234,7 +9235,7 @@
       <c r="K107" s="2"/>
       <c r="L107" s="172"/>
       <c r="M107" s="188" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="N107" s="55"/>
       <c r="O107" s="2"/>
@@ -9266,7 +9267,7 @@
       <c r="K108" s="2"/>
       <c r="L108" s="172"/>
       <c r="M108" s="188" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="N108" s="55"/>
       <c r="O108" s="2"/>
@@ -9298,7 +9299,7 @@
       <c r="K109" s="2"/>
       <c r="L109" s="172"/>
       <c r="M109" s="188" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="N109" s="55"/>
       <c r="O109" s="2"/>
@@ -9333,7 +9334,7 @@
       <c r="K110" s="2"/>
       <c r="L110" s="172"/>
       <c r="M110" s="188" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="N110" s="55"/>
       <c r="O110" s="2"/>
@@ -9368,7 +9369,7 @@
       <c r="K111" s="2"/>
       <c r="L111" s="172"/>
       <c r="M111" s="188" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="N111" s="55"/>
       <c r="O111" s="2"/>
@@ -9403,7 +9404,7 @@
       <c r="K112" s="2"/>
       <c r="L112" s="172"/>
       <c r="M112" s="188" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="N112" s="55"/>
       <c r="O112" s="2"/>
@@ -9438,7 +9439,7 @@
       <c r="K113" s="2"/>
       <c r="L113" s="172"/>
       <c r="M113" s="189" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="N113" s="55"/>
       <c r="O113" s="2"/>
@@ -9913,11 +9914,11 @@
   <dimension ref="A1:AE334"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <pane xSplit="9" ySplit="10" topLeftCell="J93" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="10" topLeftCell="J89" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="J14" sqref="J14:T14"/>
+      <selection pane="bottomRight" activeCell="P99" sqref="P99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -10410,7 +10411,7 @@
         <v>44388</v>
       </c>
       <c r="J13" s="191" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="K13" s="192"/>
       <c r="L13" s="192"/>
@@ -10449,7 +10450,7 @@
         <v>44580.5012369213</v>
       </c>
       <c r="J14" s="194" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="K14" s="195"/>
       <c r="L14" s="195"/>
@@ -24949,7 +24950,7 @@
       <c r="F312" s="5"/>
       <c r="G312" s="4"/>
       <c r="H312" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="I312" s="2"/>
       <c r="J312" s="31" t="b">
@@ -25031,7 +25032,7 @@
       <c r="F314" s="5"/>
       <c r="G314" s="4"/>
       <c r="H314" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I314" s="2"/>
       <c r="J314" s="31" t="b">
@@ -25720,7 +25721,7 @@
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="M117" sqref="M117"/>
+      <selection pane="bottomRight" activeCell="J14" sqref="J14:T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -26217,7 +26218,7 @@
         <v>44637.790818518501</v>
       </c>
       <c r="J13" s="191" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="K13" s="192"/>
       <c r="L13" s="192"/>
@@ -26253,10 +26254,10 @@
         <v>17</v>
       </c>
       <c r="I14" s="148">
-        <v>44336.775273148101</v>
+        <v>44638.685893287002</v>
       </c>
       <c r="J14" s="194" t="s">
-        <v>302</v>
+        <v>357</v>
       </c>
       <c r="K14" s="195"/>
       <c r="L14" s="195"/>
@@ -27289,7 +27290,7 @@
       <c r="F43" s="5"/>
       <c r="G43" s="4"/>
       <c r="H43" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
@@ -27328,7 +27329,7 @@
       <c r="F44" s="5"/>
       <c r="G44" s="4"/>
       <c r="H44" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
@@ -28740,7 +28741,7 @@
         <v>237</v>
       </c>
       <c r="K82" s="36" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L82" s="2" t="s">
         <v>238</v>
@@ -28749,7 +28750,7 @@
         <v>237</v>
       </c>
       <c r="N82" s="36" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="O82" s="2" t="s">
         <v>238</v>
@@ -28761,7 +28762,7 @@
         <v>237</v>
       </c>
       <c r="T82" s="36" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="U82" s="2" t="s">
         <v>238</v>
@@ -30149,7 +30150,7 @@
       <c r="J116" s="36"/>
       <c r="K116" s="36"/>
       <c r="L116" s="36" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="M116" s="31" t="b">
         <v>0</v>
@@ -30161,10 +30162,10 @@
       <c r="R116" s="2"/>
       <c r="S116" s="2"/>
       <c r="T116" s="26" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="U116" s="31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V116" s="2"/>
       <c r="W116" s="2"/>
@@ -30190,14 +30191,14 @@
       <c r="J117" s="36"/>
       <c r="K117" s="36"/>
       <c r="L117" s="26" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="M117" s="31">
         <v>0</v>
       </c>
       <c r="N117" s="36"/>
       <c r="O117" s="26" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="P117" s="31" t="b">
         <v>1</v>
@@ -30235,7 +30236,7 @@
       <c r="J118" s="36"/>
       <c r="K118" s="36"/>
       <c r="L118" s="26" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="M118" s="31" t="b">
         <v>0</v>
@@ -30272,7 +30273,7 @@
       <c r="J119" s="172"/>
       <c r="K119" s="172"/>
       <c r="L119" s="26" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="M119" s="31">
         <v>0</v>

</xml_diff>

<commit_message>
Change so that AFO works on day of the year rather than using a date. Most of profit change due to changes to lp and some due to rounding things to nearest week (eg seeding now starts 7 day after brk rather than 10).
</commit_message>
<xml_diff>
--- a/Structural.xlsx
+++ b/Structural.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\Models\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1EDB48B-187C-4138-B206-542210F7FBB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5606E3A4-1A2E-4169-A2A5-10BA2F30A1F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="210" yWindow="495" windowWidth="27705" windowHeight="15630" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
@@ -70,7 +70,7 @@
     <definedName name="i_fs_use_pkl" localSheetId="2">StructuralSA!$M$116</definedName>
     <definedName name="i_fvp_mask_dams">StructuralSA!$N$43:$O$43</definedName>
     <definedName name="i_fvp_mask_offs">StructuralSA!$J$52:$L$52</definedName>
-    <definedName name="i_fvp4_date_i">StructuralSA!$O$45:$O$47</definedName>
+    <definedName name="i_fvp4_date_i">StructuralSA!$P$45:$P$47</definedName>
     <definedName name="i_generate_with_t" localSheetId="2">StructuralSA!$P$117</definedName>
     <definedName name="i_i_pos">Stock!$I$50</definedName>
     <definedName name="i_idx_k" localSheetId="0">General!$M$80:$M$113</definedName>
@@ -167,7 +167,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1181,6 +1183,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="P45" authorId="0" shapeId="0" xr:uid="{61078212-122D-45DD-BD3A-73F56FDE3E1C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Michael Young (21512438):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+DOY</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="O46" authorId="1" shapeId="0" xr:uid="{2C53C2B2-30D1-4DBB-9BCA-B031DE33B441}">
       <text>
         <r>
@@ -3016,7 +3042,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3209,6 +3235,19 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="35">
@@ -4244,7 +4283,7 @@
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="198">
+  <cellXfs count="199">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="25" xfId="3">
@@ -4750,6 +4789,10 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="23" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="25" xfId="9">
+      <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -5405,7 +5448,7 @@
   <dimension ref="A1:AT127"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <pane xSplit="9" ySplit="10" topLeftCell="J91" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="10" topLeftCell="J118" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
@@ -9914,11 +9957,11 @@
   <dimension ref="A1:AE334"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <pane xSplit="9" ySplit="10" topLeftCell="J89" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="10" topLeftCell="J309" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="P99" sqref="P99"/>
+      <selection pane="bottomRight" activeCell="I62" sqref="I62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -25717,11 +25760,11 @@
   <dimension ref="A1:AB169"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="9" ySplit="10" topLeftCell="J102" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="10" topLeftCell="J16" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="J6" sqref="J6"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="J14" sqref="J14:T14"/>
+      <selection pane="bottomRight" activeCell="U45" sqref="U45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -27379,7 +27422,10 @@
       <c r="O45" s="144">
         <v>43748</v>
       </c>
-      <c r="P45" s="2"/>
+      <c r="P45" s="198">
+        <f>MIN(364,INT((O45 - DATE(YEAR(O45),1,1))))</f>
+        <v>282</v>
+      </c>
       <c r="Q45" s="2"/>
       <c r="R45" s="2"/>
       <c r="S45" s="2"/>
@@ -27416,7 +27462,10 @@
       <c r="O46" s="144">
         <v>43826</v>
       </c>
-      <c r="P46" s="2"/>
+      <c r="P46" s="198">
+        <f t="shared" ref="P46:P47" si="2">MIN(364,INT((O46 - DATE(YEAR(O46),1,1))))</f>
+        <v>360</v>
+      </c>
       <c r="Q46" s="2"/>
       <c r="R46" s="2"/>
       <c r="S46" s="2"/>
@@ -27453,7 +27502,10 @@
       <c r="O47" s="144">
         <v>43826</v>
       </c>
-      <c r="P47" s="2"/>
+      <c r="P47" s="198">
+        <f t="shared" si="2"/>
+        <v>360</v>
+      </c>
       <c r="Q47" s="2"/>
       <c r="R47" s="2"/>
       <c r="S47" s="2"/>
@@ -28981,7 +29033,7 @@
       <c r="A87" s="1"/>
       <c r="B87" s="33"/>
       <c r="C87" s="73">
-        <f t="shared" ref="C87:C90" si="2">INT(C$64+3)</f>
+        <f t="shared" ref="C87:C90" si="3">INT(C$64+3)</f>
         <v>4</v>
       </c>
       <c r="D87" s="4"/>
@@ -29030,7 +29082,7 @@
       <c r="A88" s="1"/>
       <c r="B88" s="33"/>
       <c r="C88" s="73">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="D88" s="4"/>
@@ -29079,7 +29131,7 @@
       <c r="A89" s="1"/>
       <c r="B89" s="33"/>
       <c r="C89" s="73">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="D89" s="4"/>
@@ -29128,7 +29180,7 @@
       <c r="A90" s="1"/>
       <c r="B90" s="33"/>
       <c r="C90" s="73">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="D90" s="4"/>
@@ -29345,7 +29397,7 @@
       <c r="A95" s="1"/>
       <c r="B95" s="33"/>
       <c r="C95" s="73">
-        <f t="shared" ref="C95:C98" si="3">INT($C$64)+3</f>
+        <f t="shared" ref="C95:C98" si="4">INT($C$64)+3</f>
         <v>4</v>
       </c>
       <c r="D95" s="4"/>
@@ -29406,7 +29458,7 @@
       <c r="A96" s="1"/>
       <c r="B96" s="33"/>
       <c r="C96" s="73">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="D96" s="4"/>
@@ -29459,7 +29511,7 @@
       <c r="A97" s="1"/>
       <c r="B97" s="33"/>
       <c r="C97" s="73">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="D97" s="4"/>
@@ -29512,7 +29564,7 @@
       <c r="A98" s="1"/>
       <c r="B98" s="33"/>
       <c r="C98" s="73">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="D98" s="4"/>
@@ -30600,7 +30652,7 @@
       <c r="A128" s="1"/>
       <c r="B128" s="33"/>
       <c r="C128" s="73">
-        <f t="shared" ref="C128:C130" si="4">INT(C$108+3)</f>
+        <f t="shared" ref="C128:C130" si="5">INT(C$108+3)</f>
         <v>4</v>
       </c>
       <c r="D128" s="4"/>
@@ -30639,7 +30691,7 @@
       <c r="A129" s="1"/>
       <c r="B129" s="33"/>
       <c r="C129" s="73">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="D129" s="4"/>
@@ -30678,7 +30730,7 @@
       <c r="A130" s="1"/>
       <c r="B130" s="33"/>
       <c r="C130" s="73">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="D130" s="4"/>

</xml_diff>

<commit_message>
create feedbudget report and move default report controls from pinp to sinp. Add sav to include feedbudget report (exp.xl). Add run report control for feedbudget report (exp.xl).
</commit_message>
<xml_diff>
--- a/Structural.xlsx
+++ b/Structural.xlsx
@@ -8,18 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\Models\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5606E3A4-1A2E-4169-A2A5-10BA2F30A1F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52E6C29-7BB9-4732-B3F1-0E7AD5ADBBF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" activeTab="2" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="678" activeTab="3" xr2:uid="{0842FB8C-088A-42F9-B075-24D0619777A0}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="24" r:id="rId1"/>
     <sheet name="Stock" sheetId="12" r:id="rId2"/>
     <sheet name="StructuralSA" sheetId="25" r:id="rId3"/>
-    <sheet name="Admin" sheetId="3" state="hidden" r:id="rId4"/>
+    <sheet name="Report Settings" sheetId="26" r:id="rId4"/>
+    <sheet name="Admin" sheetId="3" state="hidden" r:id="rId5"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
+  </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Admin!$E$13:$Y$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Admin!$E$13:$Y$31</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">General!$E$10:$W$22</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Stock!$E$10:$W$22</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">StructuralSA!$E$10:$W$22</definedName>
@@ -47,12 +53,15 @@
     <definedName name="i_age_max_offs">Stock!$I$64</definedName>
     <definedName name="i_b0_pos">Stock!$I$45</definedName>
     <definedName name="i_b1_pos">Stock!$I$46</definedName>
+    <definedName name="i_break">[1]General!$Z$104:$Z$113</definedName>
+    <definedName name="i_break_date">[2]General!$R$104:$R$113</definedName>
     <definedName name="i_btrt_idx_offs">Stock!$L$268:$Q$268</definedName>
     <definedName name="i_confinement_n0">StructuralSA!$K$83</definedName>
     <definedName name="i_confinement_n1">StructuralSA!$N$83:$N$90</definedName>
     <definedName name="i_confinement_n3">StructuralSA!$T$83:$T$90</definedName>
     <definedName name="i_core_dvp_types_f1" localSheetId="1">Stock!$J$313:$L$313</definedName>
     <definedName name="i_d_pos">Stock!$I$47</definedName>
+    <definedName name="i_date_node_zm">[2]General!$T$104:$V$113</definedName>
     <definedName name="i_density_n0" localSheetId="2">StructuralSA!$L$83</definedName>
     <definedName name="i_density_n1" localSheetId="2">StructuralSA!$O$83:$O$90</definedName>
     <definedName name="i_density_n3" localSheetId="2">StructuralSA!$U$83:$U$90</definedName>
@@ -116,6 +125,7 @@
     <definedName name="i_nv_lower_p6">StructuralSA!$J$154:$S$154</definedName>
     <definedName name="i_nv_upper_p6">StructuralSA!$J$155:$S$155</definedName>
     <definedName name="i_p_pos">Stock!$I$55</definedName>
+    <definedName name="i_pasture_stage_p6z">[2]Annual!$K$20:$T$29</definedName>
     <definedName name="i_prejoin_offset">Stock!$I$66</definedName>
     <definedName name="i_progeny_w2_len">StructuralSA!$Q$75</definedName>
     <definedName name="i_r2adjust_inc">StructuralSA!$U$116</definedName>
@@ -123,7 +133,14 @@
     <definedName name="i_rev_number" localSheetId="2">StructuralSA!$I$118</definedName>
     <definedName name="i_rev_trait_inc" localSheetId="2">StructuralSA!$I$123:$I$130</definedName>
     <definedName name="i_rev_trait_name" localSheetId="2">StructuralSA!$H$123:$H$130</definedName>
+    <definedName name="i_sim_periods_year" localSheetId="3">[2]FeedSupply!$P$28</definedName>
     <definedName name="i_sim_periods_year">Stock!$I$62</definedName>
+    <definedName name="i_store_feedbud" localSheetId="3">'Report Settings'!$Q$18</definedName>
+    <definedName name="i_store_ffcfw_rep">'Report Settings'!$G$18</definedName>
+    <definedName name="i_store_lw_rep">'Report Settings'!$I$18</definedName>
+    <definedName name="i_store_mort" localSheetId="3">'Report Settings'!$O$18</definedName>
+    <definedName name="i_store_nv_rep">'Report Settings'!$K$18</definedName>
+    <definedName name="i_store_on_hand_mort" localSheetId="3">'Report Settings'!$M$18</definedName>
     <definedName name="i_transfer_exists_tg1">Stock!$K$119:$N$121</definedName>
     <definedName name="i_w_pos">Stock!$I$56</definedName>
     <definedName name="i_w_start_len1">StructuralSA!$M$76</definedName>
@@ -148,16 +165,18 @@
     <definedName name="phase_len" localSheetId="0">General!$I$52</definedName>
     <definedName name="rdvp_type_r">Stock!$J$318:$L$318</definedName>
     <definedName name="worker_levels" localSheetId="0">General!$I$42:$K$42</definedName>
-    <definedName name="ZA.Gridlines" localSheetId="3">Admin!$L$29</definedName>
-    <definedName name="ZA.Headers" localSheetId="3">Admin!$L$30</definedName>
-    <definedName name="ZA.HeightRow" localSheetId="3">Admin!$J$26</definedName>
-    <definedName name="ZA.Outline" localSheetId="3">Admin!$C$1:$C$49</definedName>
-    <definedName name="ZA.UserAccess" localSheetId="3">Admin!$L$28</definedName>
-    <definedName name="ZA.UserUnprotect" localSheetId="3">Admin!$L$27</definedName>
-    <definedName name="ZA.VersionData" localSheetId="3">Admin!$I$21</definedName>
-    <definedName name="ZA.VersionStr" localSheetId="3">Admin!$I$18</definedName>
-    <definedName name="ZA.WidthCol" localSheetId="3">Admin!$L$26</definedName>
-    <definedName name="ZA.ZoomSheet" localSheetId="3">Admin!$O$26</definedName>
+    <definedName name="YieldBySoil.i">[3]Rotation!$J$47:$V$59</definedName>
+    <definedName name="YieldBySoil.n">[3]Rotation!$H$47:$H$59</definedName>
+    <definedName name="ZA.Gridlines" localSheetId="4">Admin!$L$29</definedName>
+    <definedName name="ZA.Headers" localSheetId="4">Admin!$L$30</definedName>
+    <definedName name="ZA.HeightRow" localSheetId="4">Admin!$J$26</definedName>
+    <definedName name="ZA.Outline" localSheetId="4">Admin!$C$1:$C$49</definedName>
+    <definedName name="ZA.UserAccess" localSheetId="4">Admin!$L$28</definedName>
+    <definedName name="ZA.UserUnprotect" localSheetId="4">Admin!$L$27</definedName>
+    <definedName name="ZA.VersionData" localSheetId="4">Admin!$I$21</definedName>
+    <definedName name="ZA.VersionStr" localSheetId="4">Admin!$I$18</definedName>
+    <definedName name="ZA.WidthCol" localSheetId="4">Admin!$L$26</definedName>
+    <definedName name="ZA.ZoomSheet" localSheetId="4">Admin!$O$26</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1847,8 +1866,42 @@
 </comments>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>John</author>
+  </authors>
+  <commentList>
+    <comment ref="M16" authorId="0" shapeId="0" xr:uid="{2E84FAC6-A425-42D0-899A-CA98558F543C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>John:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+with mortality weighting</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="370">
   <si>
     <t>Controls for this worksheet</t>
   </si>
@@ -3034,15 +3087,53 @@
 20May21: Make the extra nut_spread_g1 = 0.1
 1Apr19: Blank worksheet</t>
   </si>
+  <si>
+    <t>Control variable to be stored for reporting</t>
+  </si>
+  <si>
+    <t>Some arrays used for reporting are vary big so the default is not to store them. This is the default settings which can be overwritten using sensitivity values</t>
+  </si>
+  <si>
+    <t>FFCFW</t>
+  </si>
+  <si>
+    <t>NV</t>
+  </si>
+  <si>
+    <t>On-hand_p</t>
+  </si>
+  <si>
+    <t>Mort</t>
+  </si>
+  <si>
+    <t>store lw patterns</t>
+  </si>
+  <si>
+    <t>store NV patterns</t>
+  </si>
+  <si>
+    <t>store on hand with p axis</t>
+  </si>
+  <si>
+    <t>store mort with p axis</t>
+  </si>
+  <si>
+    <t>Feed budget</t>
+  </si>
+  <si>
+    <t>store mei with v and o axis</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode=";;;"/>
+    <numFmt numFmtId="166" formatCode="0.00_)"/>
   </numFmts>
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3249,8 +3340,34 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000CC"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="35">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3450,6 +3567,35 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="29"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="27"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFFF"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -4160,7 +4306,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="44">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0">
       <alignment horizontal="centerContinuous" vertical="center"/>
@@ -4282,8 +4428,11 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="39" borderId="51" applyNumberFormat="0" applyBorder="0" applyAlignment="0">
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="199">
+  <cellXfs count="236">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="25" xfId="3">
@@ -4767,6 +4916,10 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="58" xfId="3" applyBorder="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="25" xfId="9">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="38" xfId="12" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -4791,12 +4944,93 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="25" xfId="9">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="21" fillId="37" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="37" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="21" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="37" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="15" fontId="32" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="38" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="21" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="21" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="21" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="21" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="21" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="31" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="39" borderId="0" xfId="44" applyBorder="1" applyAlignment="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="166" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="21" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="21" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="37" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="37" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="37" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="44">
+  <cellStyles count="45">
     <cellStyle name="Accent2" xfId="33" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="41" builtinId="49"/>
     <cellStyle name="Admin" xfId="12" xr:uid="{2B7910BB-6C56-41C3-B52A-A76E890A4DBD}"/>
@@ -4822,6 +5056,7 @@
     <cellStyle name="FormulaControl" xfId="6" xr:uid="{06292D03-2B9E-4759-95AA-9D1BB12152C3}"/>
     <cellStyle name="FormulaControl 2" xfId="34" xr:uid="{AE574CB0-3DD5-4734-9B76-6310F1789C2B}"/>
     <cellStyle name="IndexSelectBackground" xfId="38" xr:uid="{775E2DDA-C7F9-4148-A5AE-E9541B85C9B2}"/>
+    <cellStyle name="InpPy" xfId="44" xr:uid="{3C4B7809-EA6C-4CC9-BC7D-52F51D2B5AD9}"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="InputsToDo" xfId="40" xr:uid="{D103EA41-1C2D-48A0-84CA-D4441B20EAFA}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5143,6 +5378,987 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Home"/>
+      <sheetName val="General"/>
+      <sheetName val="Sup Feed"/>
+      <sheetName val="Crop"/>
+      <sheetName val="CropGrazing"/>
+      <sheetName val="Periods"/>
+      <sheetName val="Labour"/>
+      <sheetName val="Annual"/>
+      <sheetName val="Sheep"/>
+      <sheetName val="FeedSupply"/>
+      <sheetName val="Mach"/>
+      <sheetName val="CropResidue"/>
+      <sheetName val="Finance"/>
+      <sheetName val="MVEnergy"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1">
+        <row r="104">
+          <cell r="Z104">
+            <v>119</v>
+          </cell>
+        </row>
+        <row r="105">
+          <cell r="Z105">
+            <v>105</v>
+          </cell>
+        </row>
+        <row r="106">
+          <cell r="Z106">
+            <v>105</v>
+          </cell>
+        </row>
+        <row r="107">
+          <cell r="Z107">
+            <v>105</v>
+          </cell>
+        </row>
+        <row r="108">
+          <cell r="Z108">
+            <v>105</v>
+          </cell>
+        </row>
+        <row r="109">
+          <cell r="Z109">
+            <v>126</v>
+          </cell>
+        </row>
+        <row r="110">
+          <cell r="Z110">
+            <v>126</v>
+          </cell>
+        </row>
+        <row r="111">
+          <cell r="Z111">
+            <v>147</v>
+          </cell>
+        </row>
+        <row r="112">
+          <cell r="Z112">
+            <v>147</v>
+          </cell>
+        </row>
+        <row r="113">
+          <cell r="Z113">
+            <v>147</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Home"/>
+      <sheetName val="General"/>
+      <sheetName val="Sup Feed"/>
+      <sheetName val="Crop"/>
+      <sheetName val="CropGrazing"/>
+      <sheetName val="Periods"/>
+      <sheetName val="Labour"/>
+      <sheetName val="Annual"/>
+      <sheetName val="Sheep"/>
+      <sheetName val="FeedSupply"/>
+      <sheetName val="Mach"/>
+      <sheetName val="CropResidue"/>
+      <sheetName val="Finance"/>
+      <sheetName val="MVEnergy"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1">
+        <row r="104">
+          <cell r="R104">
+            <v>43595</v>
+          </cell>
+          <cell r="T104">
+            <v>105</v>
+          </cell>
+          <cell r="U104">
+            <v>217</v>
+          </cell>
+          <cell r="V104">
+            <v>287</v>
+          </cell>
+        </row>
+        <row r="105">
+          <cell r="R105">
+            <v>43572</v>
+          </cell>
+          <cell r="T105">
+            <v>105</v>
+          </cell>
+          <cell r="U105">
+            <v>217</v>
+          </cell>
+          <cell r="V105">
+            <v>287</v>
+          </cell>
+        </row>
+        <row r="106">
+          <cell r="R106">
+            <v>43572</v>
+          </cell>
+          <cell r="T106">
+            <v>105</v>
+          </cell>
+          <cell r="U106">
+            <v>217</v>
+          </cell>
+          <cell r="V106">
+            <v>287</v>
+          </cell>
+        </row>
+        <row r="107">
+          <cell r="R107">
+            <v>43572</v>
+          </cell>
+          <cell r="T107">
+            <v>105</v>
+          </cell>
+          <cell r="U107">
+            <v>217</v>
+          </cell>
+          <cell r="V107">
+            <v>287</v>
+          </cell>
+        </row>
+        <row r="108">
+          <cell r="R108">
+            <v>43593</v>
+          </cell>
+          <cell r="T108">
+            <v>105</v>
+          </cell>
+          <cell r="U108">
+            <v>217</v>
+          </cell>
+          <cell r="V108">
+            <v>287</v>
+          </cell>
+        </row>
+        <row r="109">
+          <cell r="R109">
+            <v>43593</v>
+          </cell>
+          <cell r="T109">
+            <v>105</v>
+          </cell>
+          <cell r="U109">
+            <v>217</v>
+          </cell>
+          <cell r="V109">
+            <v>287</v>
+          </cell>
+        </row>
+        <row r="110">
+          <cell r="R110">
+            <v>43593</v>
+          </cell>
+          <cell r="T110">
+            <v>105</v>
+          </cell>
+          <cell r="U110">
+            <v>217</v>
+          </cell>
+          <cell r="V110">
+            <v>287</v>
+          </cell>
+        </row>
+        <row r="111">
+          <cell r="R111">
+            <v>43614</v>
+          </cell>
+          <cell r="T111">
+            <v>105</v>
+          </cell>
+          <cell r="U111">
+            <v>217</v>
+          </cell>
+          <cell r="V111">
+            <v>287</v>
+          </cell>
+        </row>
+        <row r="112">
+          <cell r="R112">
+            <v>43614</v>
+          </cell>
+          <cell r="T112">
+            <v>105</v>
+          </cell>
+          <cell r="U112">
+            <v>217</v>
+          </cell>
+          <cell r="V112">
+            <v>287</v>
+          </cell>
+        </row>
+        <row r="113">
+          <cell r="R113">
+            <v>43614</v>
+          </cell>
+          <cell r="T113">
+            <v>105</v>
+          </cell>
+          <cell r="U113">
+            <v>217</v>
+          </cell>
+          <cell r="V113">
+            <v>287</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7">
+        <row r="20">
+          <cell r="K20">
+            <v>0</v>
+          </cell>
+          <cell r="L20">
+            <v>0</v>
+          </cell>
+          <cell r="M20">
+            <v>0</v>
+          </cell>
+          <cell r="N20">
+            <v>0</v>
+          </cell>
+          <cell r="O20">
+            <v>0</v>
+          </cell>
+          <cell r="P20">
+            <v>0</v>
+          </cell>
+          <cell r="Q20">
+            <v>0</v>
+          </cell>
+          <cell r="R20">
+            <v>0</v>
+          </cell>
+          <cell r="S20">
+            <v>0</v>
+          </cell>
+          <cell r="T20">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="K21">
+            <v>0</v>
+          </cell>
+          <cell r="L21">
+            <v>0</v>
+          </cell>
+          <cell r="M21">
+            <v>0</v>
+          </cell>
+          <cell r="N21">
+            <v>0</v>
+          </cell>
+          <cell r="O21">
+            <v>0</v>
+          </cell>
+          <cell r="P21">
+            <v>0</v>
+          </cell>
+          <cell r="Q21">
+            <v>0</v>
+          </cell>
+          <cell r="R21">
+            <v>0</v>
+          </cell>
+          <cell r="S21">
+            <v>0</v>
+          </cell>
+          <cell r="T21">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="K22">
+            <v>1</v>
+          </cell>
+          <cell r="L22">
+            <v>1</v>
+          </cell>
+          <cell r="M22">
+            <v>1</v>
+          </cell>
+          <cell r="N22">
+            <v>1</v>
+          </cell>
+          <cell r="O22">
+            <v>1</v>
+          </cell>
+          <cell r="P22">
+            <v>1</v>
+          </cell>
+          <cell r="Q22">
+            <v>1</v>
+          </cell>
+          <cell r="R22">
+            <v>1</v>
+          </cell>
+          <cell r="S22">
+            <v>1</v>
+          </cell>
+          <cell r="T22">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="K23">
+            <v>1</v>
+          </cell>
+          <cell r="L23">
+            <v>1</v>
+          </cell>
+          <cell r="M23">
+            <v>1</v>
+          </cell>
+          <cell r="N23">
+            <v>1</v>
+          </cell>
+          <cell r="O23">
+            <v>1</v>
+          </cell>
+          <cell r="P23">
+            <v>1</v>
+          </cell>
+          <cell r="Q23">
+            <v>1</v>
+          </cell>
+          <cell r="R23">
+            <v>1</v>
+          </cell>
+          <cell r="S23">
+            <v>1</v>
+          </cell>
+          <cell r="T23">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="K24">
+            <v>1</v>
+          </cell>
+          <cell r="L24">
+            <v>1</v>
+          </cell>
+          <cell r="M24">
+            <v>1</v>
+          </cell>
+          <cell r="N24">
+            <v>1</v>
+          </cell>
+          <cell r="O24">
+            <v>1</v>
+          </cell>
+          <cell r="P24">
+            <v>1</v>
+          </cell>
+          <cell r="Q24">
+            <v>1</v>
+          </cell>
+          <cell r="R24">
+            <v>1</v>
+          </cell>
+          <cell r="S24">
+            <v>1</v>
+          </cell>
+          <cell r="T24">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="K25">
+            <v>1</v>
+          </cell>
+          <cell r="L25">
+            <v>1</v>
+          </cell>
+          <cell r="M25">
+            <v>1</v>
+          </cell>
+          <cell r="N25">
+            <v>1</v>
+          </cell>
+          <cell r="O25">
+            <v>1</v>
+          </cell>
+          <cell r="P25">
+            <v>1</v>
+          </cell>
+          <cell r="Q25">
+            <v>1</v>
+          </cell>
+          <cell r="R25">
+            <v>1</v>
+          </cell>
+          <cell r="S25">
+            <v>1</v>
+          </cell>
+          <cell r="T25">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="K26">
+            <v>1</v>
+          </cell>
+          <cell r="L26">
+            <v>1</v>
+          </cell>
+          <cell r="M26">
+            <v>1</v>
+          </cell>
+          <cell r="N26">
+            <v>1</v>
+          </cell>
+          <cell r="O26">
+            <v>1</v>
+          </cell>
+          <cell r="P26">
+            <v>1</v>
+          </cell>
+          <cell r="Q26">
+            <v>1</v>
+          </cell>
+          <cell r="R26">
+            <v>1</v>
+          </cell>
+          <cell r="S26">
+            <v>1</v>
+          </cell>
+          <cell r="T26">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="K27">
+            <v>1</v>
+          </cell>
+          <cell r="L27">
+            <v>1</v>
+          </cell>
+          <cell r="M27">
+            <v>1</v>
+          </cell>
+          <cell r="N27">
+            <v>1</v>
+          </cell>
+          <cell r="O27">
+            <v>1</v>
+          </cell>
+          <cell r="P27">
+            <v>1</v>
+          </cell>
+          <cell r="Q27">
+            <v>1</v>
+          </cell>
+          <cell r="R27">
+            <v>1</v>
+          </cell>
+          <cell r="S27">
+            <v>1</v>
+          </cell>
+          <cell r="T27">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="K28">
+            <v>1</v>
+          </cell>
+          <cell r="L28">
+            <v>1</v>
+          </cell>
+          <cell r="M28">
+            <v>1</v>
+          </cell>
+          <cell r="N28">
+            <v>1</v>
+          </cell>
+          <cell r="O28">
+            <v>1</v>
+          </cell>
+          <cell r="P28">
+            <v>1</v>
+          </cell>
+          <cell r="Q28">
+            <v>1</v>
+          </cell>
+          <cell r="R28">
+            <v>1</v>
+          </cell>
+          <cell r="S28">
+            <v>1</v>
+          </cell>
+          <cell r="T28">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="K29">
+            <v>1</v>
+          </cell>
+          <cell r="L29">
+            <v>1</v>
+          </cell>
+          <cell r="M29">
+            <v>1</v>
+          </cell>
+          <cell r="N29">
+            <v>1</v>
+          </cell>
+          <cell r="O29">
+            <v>1</v>
+          </cell>
+          <cell r="P29">
+            <v>1</v>
+          </cell>
+          <cell r="Q29">
+            <v>1</v>
+          </cell>
+          <cell r="R29">
+            <v>1</v>
+          </cell>
+          <cell r="S29">
+            <v>1</v>
+          </cell>
+          <cell r="T29">
+            <v>1</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9">
+        <row r="28">
+          <cell r="P28">
+            <v>52</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Controls"/>
+      <sheetName val="Gloss"/>
+      <sheetName val="MPS"/>
+      <sheetName val="FullRepStd"/>
+      <sheetName val="Names"/>
+      <sheetName val="GenData"/>
+      <sheetName val="Mach"/>
+      <sheetName val="Rotation"/>
+      <sheetName val="FullRep callibration"/>
+      <sheetName val="MRY callibration"/>
+      <sheetName val="Table Fill"/>
+      <sheetName val="Summ-MRY (2)"/>
+      <sheetName val="Sum-MRY"/>
+      <sheetName val="EL-Std"/>
+      <sheetName val="Summ-Std"/>
+      <sheetName val="Sheep"/>
+      <sheetName val="Grazingcrop"/>
+      <sheetName val="LabourSheep"/>
+      <sheetName val="Labour"/>
+      <sheetName val="LabourCrop"/>
+      <sheetName val="Emissions"/>
+      <sheetName val="EmPast1"/>
+      <sheetName val="Annual"/>
+      <sheetName val="Lucerne"/>
+      <sheetName val="TederaP"/>
+      <sheetName val="TederaM"/>
+      <sheetName val="Stubble"/>
+      <sheetName val="ChaffPiles"/>
+      <sheetName val="FodCrop"/>
+      <sheetName val="Saltbush"/>
+      <sheetName val="Sheep$"/>
+      <sheetName val="Luc Structural"/>
+      <sheetName val="LucRotnData"/>
+      <sheetName val="Luc Rotn Inputs"/>
+      <sheetName val="LucFertMPS"/>
+      <sheetName val="Blank"/>
+      <sheetName val="Starter"/>
+      <sheetName val="MinROE"/>
+      <sheetName val="MVEnergy"/>
+      <sheetName val="ExpLib"/>
+      <sheetName val="Chart2"/>
+      <sheetName val="Rep-MVP"/>
+      <sheetName val="RepLib"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7">
+        <row r="48">
+          <cell r="H48" t="str">
+            <v>T</v>
+          </cell>
+          <cell r="J48">
+            <v>0.54</v>
+          </cell>
+          <cell r="K48">
+            <v>0.68</v>
+          </cell>
+          <cell r="L48">
+            <v>0.78</v>
+          </cell>
+          <cell r="M48">
+            <v>1</v>
+          </cell>
+          <cell r="N48">
+            <v>0</v>
+          </cell>
+          <cell r="O48">
+            <v>0</v>
+          </cell>
+          <cell r="P48">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="H49" t="str">
+            <v>R</v>
+          </cell>
+          <cell r="J49">
+            <v>0</v>
+          </cell>
+          <cell r="K49">
+            <v>0</v>
+          </cell>
+          <cell r="L49">
+            <v>0</v>
+          </cell>
+          <cell r="M49">
+            <v>1</v>
+          </cell>
+          <cell r="N49">
+            <v>0</v>
+          </cell>
+          <cell r="O49">
+            <v>0</v>
+          </cell>
+          <cell r="P49">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="H50" t="str">
+            <v>W</v>
+          </cell>
+          <cell r="J50">
+            <v>0.67</v>
+          </cell>
+          <cell r="K50">
+            <v>0.77</v>
+          </cell>
+          <cell r="L50">
+            <v>0.85</v>
+          </cell>
+          <cell r="M50">
+            <v>1</v>
+          </cell>
+          <cell r="N50">
+            <v>0</v>
+          </cell>
+          <cell r="O50">
+            <v>0</v>
+          </cell>
+          <cell r="P50">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="H51" t="str">
+            <v>F</v>
+          </cell>
+          <cell r="J51">
+            <v>0</v>
+          </cell>
+          <cell r="K51">
+            <v>0</v>
+          </cell>
+          <cell r="L51">
+            <v>0</v>
+          </cell>
+          <cell r="M51">
+            <v>0</v>
+          </cell>
+          <cell r="N51">
+            <v>0</v>
+          </cell>
+          <cell r="O51">
+            <v>0</v>
+          </cell>
+          <cell r="P51">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="H52" t="str">
+            <v>O</v>
+          </cell>
+          <cell r="J52">
+            <v>0.7</v>
+          </cell>
+          <cell r="K52">
+            <v>0.8</v>
+          </cell>
+          <cell r="L52">
+            <v>0.87</v>
+          </cell>
+          <cell r="M52">
+            <v>1</v>
+          </cell>
+          <cell r="N52">
+            <v>0</v>
+          </cell>
+          <cell r="O52">
+            <v>0</v>
+          </cell>
+          <cell r="P52">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="53">
+          <cell r="H53" t="str">
+            <v>B</v>
+          </cell>
+          <cell r="J53">
+            <v>0.63</v>
+          </cell>
+          <cell r="K53">
+            <v>0.75</v>
+          </cell>
+          <cell r="L53">
+            <v>0.83</v>
+          </cell>
+          <cell r="M53">
+            <v>1</v>
+          </cell>
+          <cell r="N53">
+            <v>0</v>
+          </cell>
+          <cell r="O53">
+            <v>0</v>
+          </cell>
+          <cell r="P53">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="54">
+          <cell r="H54" t="str">
+            <v>L</v>
+          </cell>
+          <cell r="J54">
+            <v>0</v>
+          </cell>
+          <cell r="K54">
+            <v>0.31</v>
+          </cell>
+          <cell r="L54">
+            <v>0.55000000000000004</v>
+          </cell>
+          <cell r="M54">
+            <v>1</v>
+          </cell>
+          <cell r="N54">
+            <v>0</v>
+          </cell>
+          <cell r="O54">
+            <v>0</v>
+          </cell>
+          <cell r="P54">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="55">
+          <cell r="H55" t="str">
+            <v>H</v>
+          </cell>
+          <cell r="J55">
+            <v>0.86</v>
+          </cell>
+          <cell r="K55">
+            <v>0.9</v>
+          </cell>
+          <cell r="L55">
+            <v>0.94</v>
+          </cell>
+          <cell r="M55">
+            <v>1</v>
+          </cell>
+          <cell r="N55">
+            <v>0</v>
+          </cell>
+          <cell r="O55">
+            <v>0</v>
+          </cell>
+          <cell r="P55">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="56">
+          <cell r="H56" t="str">
+            <v>D</v>
+          </cell>
+          <cell r="J56">
+            <v>0</v>
+          </cell>
+          <cell r="K56">
+            <v>0</v>
+          </cell>
+          <cell r="L56">
+            <v>0</v>
+          </cell>
+          <cell r="M56">
+            <v>0</v>
+          </cell>
+          <cell r="N56">
+            <v>0</v>
+          </cell>
+          <cell r="O56">
+            <v>0</v>
+          </cell>
+          <cell r="P56">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="57">
+          <cell r="H57" t="str">
+            <v>Z</v>
+          </cell>
+          <cell r="J57">
+            <v>0</v>
+          </cell>
+          <cell r="K57">
+            <v>0</v>
+          </cell>
+          <cell r="L57">
+            <v>0</v>
+          </cell>
+          <cell r="M57">
+            <v>0</v>
+          </cell>
+          <cell r="N57">
+            <v>0</v>
+          </cell>
+          <cell r="O57">
+            <v>0</v>
+          </cell>
+          <cell r="P57">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="58">
+          <cell r="H58" t="str">
+            <v>A</v>
+          </cell>
+          <cell r="J58">
+            <v>0</v>
+          </cell>
+          <cell r="K58">
+            <v>0</v>
+          </cell>
+          <cell r="L58">
+            <v>0</v>
+          </cell>
+          <cell r="M58">
+            <v>0</v>
+          </cell>
+          <cell r="N58">
+            <v>0</v>
+          </cell>
+          <cell r="O58">
+            <v>0</v>
+          </cell>
+          <cell r="P58">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
+      <sheetData sheetId="30"/>
+      <sheetData sheetId="31"/>
+      <sheetData sheetId="32"/>
+      <sheetData sheetId="33"/>
+      <sheetData sheetId="34"/>
+      <sheetData sheetId="35"/>
+      <sheetData sheetId="36"/>
+      <sheetData sheetId="37"/>
+      <sheetData sheetId="38"/>
+      <sheetData sheetId="39"/>
+      <sheetData sheetId="40" refreshError="1"/>
+      <sheetData sheetId="41"/>
+      <sheetData sheetId="42"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5946,19 +7162,19 @@
       <c r="I13" s="149">
         <v>44371.659649305599</v>
       </c>
-      <c r="J13" s="191" t="s">
+      <c r="J13" s="192" t="s">
         <v>298</v>
       </c>
-      <c r="K13" s="192"/>
-      <c r="L13" s="192"/>
-      <c r="M13" s="192"/>
-      <c r="N13" s="192"/>
-      <c r="O13" s="192"/>
-      <c r="P13" s="192"/>
-      <c r="Q13" s="192"/>
-      <c r="R13" s="192"/>
-      <c r="S13" s="192"/>
-      <c r="T13" s="193"/>
+      <c r="K13" s="193"/>
+      <c r="L13" s="193"/>
+      <c r="M13" s="193"/>
+      <c r="N13" s="193"/>
+      <c r="O13" s="193"/>
+      <c r="P13" s="193"/>
+      <c r="Q13" s="193"/>
+      <c r="R13" s="193"/>
+      <c r="S13" s="193"/>
+      <c r="T13" s="194"/>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
@@ -5985,19 +7201,19 @@
       <c r="I14" s="148">
         <v>44371.660335300898</v>
       </c>
-      <c r="J14" s="194" t="s">
+      <c r="J14" s="195" t="s">
         <v>299</v>
       </c>
-      <c r="K14" s="195"/>
-      <c r="L14" s="195"/>
-      <c r="M14" s="195"/>
-      <c r="N14" s="195"/>
-      <c r="O14" s="195"/>
-      <c r="P14" s="195"/>
-      <c r="Q14" s="195"/>
-      <c r="R14" s="195"/>
-      <c r="S14" s="195"/>
-      <c r="T14" s="195"/>
+      <c r="K14" s="196"/>
+      <c r="L14" s="196"/>
+      <c r="M14" s="196"/>
+      <c r="N14" s="196"/>
+      <c r="O14" s="196"/>
+      <c r="P14" s="196"/>
+      <c r="Q14" s="196"/>
+      <c r="R14" s="196"/>
+      <c r="S14" s="196"/>
+      <c r="T14" s="196"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
@@ -10453,19 +11669,19 @@
       <c r="I13" s="149">
         <v>44388</v>
       </c>
-      <c r="J13" s="191" t="s">
+      <c r="J13" s="192" t="s">
         <v>353</v>
       </